<commit_message>
FINISH: MVP-template bulk from Excel migration
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,8 +14,10 @@
     <sheet name="families" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="ap_profiles" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="ap_programs" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="ap_subjects" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="rules" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ap_subject_types" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="ap_knowledges" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ap_subjects" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="rules" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="SUBSTAGES_FRECUENCY" hidden="0">DB!$A$2:$A$8</definedName>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -424,6 +426,12 @@
     <t>substagesFrequency</t>
   </si>
   <si>
+    <t>maxSubstageAbbreviation</t>
+  </si>
+  <si>
+    <t>maxSubstageAbbreviationIsOnlyNumbers</t>
+  </si>
+  <si>
     <t>haveKnowledge</t>
   </si>
   <si>
@@ -493,15 +501,15 @@
     <t xml:space="preserve">Substage Frequency</t>
   </si>
   <si>
+    <t xml:space="preserve">Max acronym length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is acronym only numbers?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Have knowlegde areas?</t>
   </si>
   <si>
-    <t xml:space="preserve">Max acronym length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is acronym only numbers?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Only one group per course?</t>
   </si>
   <si>
@@ -533,13 +541,229 @@
   </si>
   <si>
     <t xml:space="preserve">Semester 1|S01, Semester 2|S02</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>credits_program</t>
+  </si>
+  <si>
+    <t>groupVisibility</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is visible in tree?</t>
+  </si>
+  <si>
+    <t>type01</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>type02</t>
+  </si>
+  <si>
+    <t>type03</t>
+  </si>
+  <si>
+    <t>Specific</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>knowArea01</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>SCNC</t>
+  </si>
+  <si>
+    <t>#1B72E8</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/biology_icon_3f80619648.svg</t>
+  </si>
+  <si>
+    <t>knowArea02</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>#E81B4A</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/computer_icon_56ca0c26bc.svg</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>internalId</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>knowledge</t>
+  </si>
+  <si>
+    <t>subjectType</t>
+  </si>
+  <si>
+    <t>teachers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class config</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Credits</t>
+  </si>
+  <si>
+    <t>InternalID</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knowledge Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject Type</t>
+  </si>
+  <si>
+    <t>Teachers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group A|G1A, Group B|G1B</t>
+  </si>
+  <si>
+    <t>#FFEB9C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social sciences I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group A|G2A, Group B|G2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math II</t>
+  </si>
+  <si>
+    <t>#FFC7CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social sciences II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group A|G3A, Group B|G3B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social sciences III</t>
+  </si>
+  <si>
+    <t>#C6EFCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group A|G4A, Group B|G4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social sciences IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports IV</t>
+  </si>
+  <si>
+    <t>#FFCC99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group A|G5A, Group B|G5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social sciences V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -623,6 +847,18 @@
     <font>
       <name val="Calibri"/>
       <b/>
+      <color theme="1"/>
+      <sz val="10.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="10"/>
+      <sz val="10.500000"/>
+      <u/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <color theme="1"/>
       <sz val="10.000000"/>
       <scheme val="minor"/>
@@ -1003,7 +1239,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="125">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1029,14 +1265,20 @@
     <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf fontId="1" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1157,17 +1399,20 @@
     <xf fontId="4" fillId="15" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1175,27 +1420,52 @@
     <xf fontId="1" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1">
+    <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="4" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf fontId="1" fillId="2" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="4" fillId="4" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="16" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -1231,56 +1501,113 @@
     <xf fontId="1" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="12" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="4" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="12" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="12" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="12" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="13" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="13" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="13" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="18" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="18" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="14" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="14" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="4" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="16" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="4" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="13" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="7" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="7" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="16" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="14" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="14" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="14" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1788,6 +2115,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1" tint="0"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1863,6 +2195,1086 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="0"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="14.57421875"/>
+    <col customWidth="1" min="3" max="3" width="10.8515625"/>
+    <col customWidth="1" min="5" max="5" width="13.8515625"/>
+    <col customWidth="1" min="6" max="6" width="10.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" ht="28.5">
+      <c r="A2" s="107" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="108" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="108" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="109" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="110" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="64" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" s="75" t="str">
+        <f>ap_programs!$A$5</f>
+        <v>programB</v>
+      </c>
+      <c r="G3" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="64" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="75" t="str">
+        <f>ap_programs!$A$5</f>
+        <v>programB</v>
+      </c>
+      <c r="G4" s="58">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E3"/>
+    <hyperlink r:id="rId2" ref="E4"/>
+  </hyperlinks>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="0"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="12.8515625"/>
+    <col customWidth="1" min="2" max="2" width="18.421875"/>
+    <col customWidth="1" min="3" max="3" width="12.8515625"/>
+    <col customWidth="1" min="6" max="6" width="10.421875"/>
+    <col customWidth="1" min="7" max="7" width="13.00390625"/>
+    <col customWidth="1" min="8" max="8" width="10.8515625"/>
+    <col customWidth="1" min="9" max="9" width="11.8515625"/>
+    <col customWidth="1" min="10" max="10" width="10.140625"/>
+    <col customWidth="1" min="11" max="11" width="23.28125"/>
+    <col customWidth="1" min="12" max="12" width="3.57421875"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="112" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="112" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="112" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="K1" s="113" t="s">
+        <v>200</v>
+      </c>
+      <c r="L1" s="72"/>
+    </row>
+    <row r="2" ht="28.850000000000001" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="114" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="72"/>
+    </row>
+    <row r="3" ht="31.850000000000001" customHeight="1">
+      <c r="A3" s="107" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="90" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" s="90" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="116" t="s">
+        <v>205</v>
+      </c>
+      <c r="H3" s="117" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="117" t="s">
+        <v>206</v>
+      </c>
+      <c r="J3" s="118" t="s">
+        <v>207</v>
+      </c>
+      <c r="K3" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="L3" s="119"/>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L4&lt;10,"0",""),L4)</f>
+        <v>subject01</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="75" t="str">
+        <f>ap_programs!A4</f>
+        <v>programA</v>
+      </c>
+      <c r="D4" s="58">
+        <v>1</v>
+      </c>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L4&lt;10,"0",""),L4)</f>
+        <v>001</v>
+      </c>
+      <c r="G4" s="120" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" s="121" t="s">
+        <v>211</v>
+      </c>
+      <c r="I4" s="58"/>
+      <c r="J4" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K4" s="123" t="s">
+        <v>212</v>
+      </c>
+      <c r="L4" s="124">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L5&lt;10,"0",""),L5)</f>
+        <v>subject02</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="75" t="str">
+        <f>C4</f>
+        <v>programA</v>
+      </c>
+      <c r="D5" s="58">
+        <v>1</v>
+      </c>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L5&lt;10,"0",""),L5)</f>
+        <v>002</v>
+      </c>
+      <c r="G5" s="120" t="str">
+        <f>G4</f>
+        <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
+      </c>
+      <c r="H5" s="121" t="str">
+        <f>H4</f>
+        <v>#FFEB9C</v>
+      </c>
+      <c r="I5" s="58"/>
+      <c r="J5" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K5" s="123" t="str">
+        <f>K4</f>
+        <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
+      </c>
+      <c r="L5" s="124">
+        <f>L4+1</f>
+        <v>2</v>
+      </c>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L6&lt;10,"0",""),L6)</f>
+        <v>subject03</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="75" t="str">
+        <f>C5</f>
+        <v>programA</v>
+      </c>
+      <c r="D6" s="58">
+        <v>1</v>
+      </c>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L6&lt;10,"0",""),L6)</f>
+        <v>003</v>
+      </c>
+      <c r="G6" s="120" t="str">
+        <f>G5</f>
+        <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
+      </c>
+      <c r="H6" s="121" t="str">
+        <f>H5</f>
+        <v>#FFEB9C</v>
+      </c>
+      <c r="I6" s="58"/>
+      <c r="J6" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K6" s="123" t="str">
+        <f>K5</f>
+        <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
+      </c>
+      <c r="L6" s="124">
+        <f>L5+1</f>
+        <v>3</v>
+      </c>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L7&lt;10,"0",""),L7)</f>
+        <v>subject04</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="75" t="str">
+        <f>C6</f>
+        <v>programA</v>
+      </c>
+      <c r="D7" s="58">
+        <v>1</v>
+      </c>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L7&lt;10,"0",""),L7)</f>
+        <v>004</v>
+      </c>
+      <c r="G7" s="120" t="str">
+        <f>G6</f>
+        <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
+      </c>
+      <c r="H7" s="121" t="str">
+        <f>H6</f>
+        <v>#FFEB9C</v>
+      </c>
+      <c r="I7" s="58"/>
+      <c r="J7" s="122" t="str">
+        <f>ap_subject_types!$A$5</f>
+        <v>type03</v>
+      </c>
+      <c r="K7" s="123" t="str">
+        <f>K6</f>
+        <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
+      </c>
+      <c r="L7" s="124">
+        <f>L6+1</f>
+        <v>4</v>
+      </c>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L8&lt;10,"0",""),L8)</f>
+        <v>subject05</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="75" t="str">
+        <f>C7</f>
+        <v>programA</v>
+      </c>
+      <c r="D8" s="58">
+        <v>2</v>
+      </c>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L8&lt;10,"0",""),L8)</f>
+        <v>005</v>
+      </c>
+      <c r="G8" s="120" t="s">
+        <v>217</v>
+      </c>
+      <c r="H8" s="121" t="str">
+        <f>H7</f>
+        <v>#FFEB9C</v>
+      </c>
+      <c r="I8" s="58"/>
+      <c r="J8" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K8" s="123" t="s">
+        <v>218</v>
+      </c>
+      <c r="L8" s="124">
+        <f>L7+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L9&lt;10,"0",""),L9)</f>
+        <v>subject06</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="75" t="str">
+        <f>C8</f>
+        <v>programA</v>
+      </c>
+      <c r="D9" s="58">
+        <v>2</v>
+      </c>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L9&lt;10,"0",""),L9)</f>
+        <v>006</v>
+      </c>
+      <c r="G9" s="120" t="str">
+        <f>G8</f>
+        <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
+      </c>
+      <c r="H9" s="121" t="s">
+        <v>220</v>
+      </c>
+      <c r="I9" s="58"/>
+      <c r="J9" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K9" s="123" t="str">
+        <f>K8</f>
+        <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
+      </c>
+      <c r="L9" s="124">
+        <f>L8+1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L10&lt;10,"0",""),L10)</f>
+        <v>subject07</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="75" t="str">
+        <f>C9</f>
+        <v>programA</v>
+      </c>
+      <c r="D10" s="58">
+        <v>2</v>
+      </c>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L10&lt;10,"0",""),L10)</f>
+        <v>007</v>
+      </c>
+      <c r="G10" s="120" t="str">
+        <f>G9</f>
+        <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
+      </c>
+      <c r="H10" s="121" t="str">
+        <f>H9</f>
+        <v>#FFC7CE</v>
+      </c>
+      <c r="I10" s="58"/>
+      <c r="J10" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K10" s="123" t="str">
+        <f>K9</f>
+        <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
+      </c>
+      <c r="L10" s="124">
+        <f>L9+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L11&lt;10,"0",""),L11)</f>
+        <v>subject08</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="75" t="str">
+        <f>C10</f>
+        <v>programA</v>
+      </c>
+      <c r="D11" s="58">
+        <v>2</v>
+      </c>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L11&lt;10,"0",""),L11)</f>
+        <v>008</v>
+      </c>
+      <c r="G11" s="120" t="str">
+        <f>G10</f>
+        <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
+      </c>
+      <c r="H11" s="121" t="str">
+        <f>H10</f>
+        <v>#FFC7CE</v>
+      </c>
+      <c r="I11" s="58"/>
+      <c r="J11" s="122" t="str">
+        <f>ap_subject_types!$A$5</f>
+        <v>type03</v>
+      </c>
+      <c r="K11" s="123" t="str">
+        <f>K10</f>
+        <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
+      </c>
+      <c r="L11" s="124">
+        <f>L10+1</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L12&lt;10,"0",""),L12)</f>
+        <v>subject09</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" s="75" t="str">
+        <f>C11</f>
+        <v>programA</v>
+      </c>
+      <c r="D12" s="58">
+        <v>3</v>
+      </c>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L12&lt;10,"0",""),L12)</f>
+        <v>009</v>
+      </c>
+      <c r="G12" s="120" t="s">
+        <v>224</v>
+      </c>
+      <c r="H12" s="121" t="str">
+        <f>H11</f>
+        <v>#FFC7CE</v>
+      </c>
+      <c r="I12" s="58"/>
+      <c r="J12" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K12" s="123" t="s">
+        <v>225</v>
+      </c>
+      <c r="L12" s="124">
+        <f>L11+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1">
+      <c r="A13" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L13&lt;10,"0",""),L13)</f>
+        <v>subject10</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="75" t="str">
+        <f>C12</f>
+        <v>programA</v>
+      </c>
+      <c r="D13" s="58">
+        <v>3</v>
+      </c>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L13&lt;10,"0",""),L13)</f>
+        <v>010</v>
+      </c>
+      <c r="G13" s="120" t="str">
+        <f>G12</f>
+        <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
+      </c>
+      <c r="H13" s="121" t="str">
+        <f>H12</f>
+        <v>#FFC7CE</v>
+      </c>
+      <c r="I13" s="58"/>
+      <c r="J13" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K13" s="123" t="str">
+        <f>K12</f>
+        <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
+      </c>
+      <c r="L13" s="124">
+        <f>L12+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L14&lt;10,"0",""),L14)</f>
+        <v>subject11</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C14" s="75" t="str">
+        <f>C13</f>
+        <v>programA</v>
+      </c>
+      <c r="D14" s="58">
+        <v>3</v>
+      </c>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L14&lt;10,"0",""),L14)</f>
+        <v>011</v>
+      </c>
+      <c r="G14" s="120" t="str">
+        <f>G13</f>
+        <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
+      </c>
+      <c r="H14" s="121" t="s">
+        <v>228</v>
+      </c>
+      <c r="I14" s="58"/>
+      <c r="J14" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K14" s="123" t="str">
+        <f>K13</f>
+        <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
+      </c>
+      <c r="L14" s="124">
+        <f>L13+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" ht="30" customHeight="1">
+      <c r="A15" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L15&lt;10,"0",""),L15)</f>
+        <v>subject12</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="75" t="str">
+        <f>C14</f>
+        <v>programA</v>
+      </c>
+      <c r="D15" s="58">
+        <v>3</v>
+      </c>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L15&lt;10,"0",""),L15)</f>
+        <v>012</v>
+      </c>
+      <c r="G15" s="120" t="str">
+        <f>G14</f>
+        <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
+      </c>
+      <c r="H15" s="121" t="str">
+        <f>H14</f>
+        <v>#C6EFCD</v>
+      </c>
+      <c r="I15" s="58"/>
+      <c r="J15" s="122" t="str">
+        <f>ap_subject_types!$A$5</f>
+        <v>type03</v>
+      </c>
+      <c r="K15" s="123" t="str">
+        <f>K14</f>
+        <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
+      </c>
+      <c r="L15" s="124">
+        <f>L14+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L16&lt;10,"0",""),L16)</f>
+        <v>subject13</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="75" t="str">
+        <f>C15</f>
+        <v>programA</v>
+      </c>
+      <c r="D16" s="58">
+        <v>4</v>
+      </c>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L16&lt;10,"0",""),L16)</f>
+        <v>013</v>
+      </c>
+      <c r="G16" s="120" t="s">
+        <v>231</v>
+      </c>
+      <c r="H16" s="121" t="str">
+        <f>H15</f>
+        <v>#C6EFCD</v>
+      </c>
+      <c r="I16" s="58"/>
+      <c r="J16" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K16" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="L16" s="124">
+        <f>L15+1</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L17&lt;10,"0",""),L17)</f>
+        <v>subject14</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17" s="75" t="str">
+        <f>C16</f>
+        <v>programA</v>
+      </c>
+      <c r="D17" s="58">
+        <v>4</v>
+      </c>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L17&lt;10,"0",""),L17)</f>
+        <v>014</v>
+      </c>
+      <c r="G17" s="120" t="str">
+        <f>G16</f>
+        <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
+      </c>
+      <c r="H17" s="121" t="str">
+        <f>H16</f>
+        <v>#C6EFCD</v>
+      </c>
+      <c r="I17" s="58"/>
+      <c r="J17" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K17" s="123" t="str">
+        <f>K16</f>
+        <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
+      </c>
+      <c r="L17" s="124">
+        <f>L16+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" ht="30" customHeight="1">
+      <c r="A18" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L18&lt;10,"0",""),L18)</f>
+        <v>subject15</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="75" t="str">
+        <f>C17</f>
+        <v>programA</v>
+      </c>
+      <c r="D18" s="58">
+        <v>4</v>
+      </c>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L18&lt;10,"0",""),L18)</f>
+        <v>015</v>
+      </c>
+      <c r="G18" s="120" t="str">
+        <f>G17</f>
+        <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
+      </c>
+      <c r="H18" s="121" t="str">
+        <f>H17</f>
+        <v>#C6EFCD</v>
+      </c>
+      <c r="I18" s="58"/>
+      <c r="J18" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K18" s="123" t="str">
+        <f>K17</f>
+        <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
+      </c>
+      <c r="L18" s="124">
+        <f>L17+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" ht="30" customHeight="1">
+      <c r="A19" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L19&lt;10,"0",""),L19)</f>
+        <v>subject16</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C19" s="75" t="str">
+        <f>C18</f>
+        <v>programA</v>
+      </c>
+      <c r="D19" s="58">
+        <v>4</v>
+      </c>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L19&lt;10,"0",""),L19)</f>
+        <v>016</v>
+      </c>
+      <c r="G19" s="120" t="str">
+        <f>G18</f>
+        <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
+      </c>
+      <c r="H19" s="121" t="s">
+        <v>236</v>
+      </c>
+      <c r="I19" s="58"/>
+      <c r="J19" s="122" t="str">
+        <f>ap_subject_types!$A$5</f>
+        <v>type03</v>
+      </c>
+      <c r="K19" s="123" t="str">
+        <f>K18</f>
+        <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
+      </c>
+      <c r="L19" s="124">
+        <f>L18+1</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" ht="30" customHeight="1">
+      <c r="A20" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L20&lt;10,"0",""),L20)</f>
+        <v>subject17</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C20" s="75" t="str">
+        <f>C19</f>
+        <v>programA</v>
+      </c>
+      <c r="D20" s="58">
+        <v>5</v>
+      </c>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L20&lt;10,"0",""),L20)</f>
+        <v>017</v>
+      </c>
+      <c r="G20" s="120" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" s="121" t="s">
+        <v>236</v>
+      </c>
+      <c r="I20" s="58"/>
+      <c r="J20" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K20" s="123" t="s">
+        <v>239</v>
+      </c>
+      <c r="L20" s="124">
+        <f>L19+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" ht="30" customHeight="1">
+      <c r="A21" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L21&lt;10,"0",""),L21)</f>
+        <v>subject18</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" s="75" t="str">
+        <f>C20</f>
+        <v>programA</v>
+      </c>
+      <c r="D21" s="58">
+        <v>5</v>
+      </c>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L21&lt;10,"0",""),L21)</f>
+        <v>018</v>
+      </c>
+      <c r="G21" s="120" t="str">
+        <f>G20</f>
+        <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
+      </c>
+      <c r="H21" s="121" t="s">
+        <v>236</v>
+      </c>
+      <c r="I21" s="58"/>
+      <c r="J21" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K21" s="123" t="str">
+        <f>K20</f>
+        <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
+      </c>
+      <c r="L21" s="124">
+        <f>L20+1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" ht="30" customHeight="1">
+      <c r="A22" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L22&lt;10,"0",""),L22)</f>
+        <v>subject19</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C22" s="75" t="str">
+        <f>C21</f>
+        <v>programA</v>
+      </c>
+      <c r="D22" s="58">
+        <v>5</v>
+      </c>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L22&lt;10,"0",""),L22)</f>
+        <v>019</v>
+      </c>
+      <c r="G22" s="120" t="str">
+        <f>G21</f>
+        <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
+      </c>
+      <c r="H22" s="121" t="s">
+        <v>236</v>
+      </c>
+      <c r="I22" s="58"/>
+      <c r="J22" s="122" t="str">
+        <f>ap_subject_types!$A$3</f>
+        <v>type01</v>
+      </c>
+      <c r="K22" s="123" t="str">
+        <f>K21</f>
+        <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
+      </c>
+      <c r="L22" s="124">
+        <f>L21+1</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" ht="30" customHeight="1">
+      <c r="A23" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(L23&lt;10,"0",""),L23)</f>
+        <v>subject20</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C23" s="75" t="str">
+        <f>C22</f>
+        <v>programA</v>
+      </c>
+      <c r="D23" s="58">
+        <v>5</v>
+      </c>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58" t="str">
+        <f>_xlfn.CONCAT("0",IF(L23&lt;10,"0",""),L23)</f>
+        <v>020</v>
+      </c>
+      <c r="G23" s="120" t="str">
+        <f>G22</f>
+        <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
+      </c>
+      <c r="H23" s="121" t="s">
+        <v>236</v>
+      </c>
+      <c r="I23" s="58"/>
+      <c r="J23" s="122" t="str">
+        <f>ap_subject_types!$A$5</f>
+        <v>type03</v>
+      </c>
+      <c r="K23" s="123" t="str">
+        <f>K22</f>
+        <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
+      </c>
+      <c r="L23" s="124">
+        <f>L22+1</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="L24" s="72"/>
+    </row>
+    <row r="25" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G2:K2"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
@@ -1910,7 +3322,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" ht="19.850000000000001" customHeight="1">
+    <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -1924,31 +3336,31 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1968,7 +3380,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G2" workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1987,93 +3399,93 @@
     <col customWidth="1" min="22" max="22" width="14.421875"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" ht="14.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="13" customFormat="1" ht="14.25">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="12" t="str">
+      <c r="E1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",E5)</f>
         <v>plugins.users.users</v>
       </c>
-      <c r="F1" s="12" t="str">
+      <c r="F1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",F5)</f>
         <v>plugins.users.user-data</v>
       </c>
-      <c r="G1" s="12" t="str">
+      <c r="G1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",G5)</f>
         <v>plugins.users.centers</v>
       </c>
-      <c r="H1" s="12" t="str">
+      <c r="H1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",H5)</f>
         <v>plugins.users.profiles</v>
       </c>
-      <c r="I1" s="12" t="str">
+      <c r="I1" s="13" t="str">
         <f>_xlfn.CONCAT($I$3,".",I5)</f>
         <v>plugins.dataset.dataset</v>
       </c>
-      <c r="J1" s="12" t="str">
+      <c r="J1" s="13" t="str">
         <f>_xlfn.CONCAT($J$3,".",J5)</f>
         <v>plugins.calendar.calendar</v>
       </c>
-      <c r="K1" s="12" t="str">
+      <c r="K1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",K5)</f>
         <v>plugins.academic-portfolio.portfolio</v>
       </c>
-      <c r="L1" s="12" t="str">
+      <c r="L1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",L5)</f>
         <v>plugins.academic-portfolio.programs</v>
       </c>
-      <c r="M1" s="12" t="str">
+      <c r="M1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",M5)</f>
         <v>plugins.academic-portfolio.profiles</v>
       </c>
-      <c r="N1" s="12" t="str">
+      <c r="N1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",N5)</f>
         <v>plugins.academic-portfolio.subjects</v>
       </c>
-      <c r="O1" s="12" t="str">
+      <c r="O1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",O5)</f>
         <v>plugins.academic-portfolio.tree</v>
       </c>
-      <c r="P1" s="12" t="str">
+      <c r="P1" s="13" t="str">
         <f>_xlfn.CONCAT($P$3,".",P5)</f>
         <v>plugins.families.families</v>
       </c>
-      <c r="Q1" s="13" t="str">
+      <c r="Q1" s="14" t="str">
         <f>_xlfn.CONCAT($P$3,".",Q5)</f>
         <v>plugins.families.config</v>
       </c>
-      <c r="R1" s="13" t="str">
+      <c r="R1" s="14" t="str">
         <f>_xlfn.CONCAT($P$3,".",R5)</f>
         <v>plugins.families.families-basic-info</v>
       </c>
-      <c r="S1" s="13" t="str">
+      <c r="S1" s="14" t="str">
         <f>_xlfn.CONCAT($P$3,".",S5)</f>
         <v>plugins.families.families-custom-info</v>
       </c>
-      <c r="T1" s="13" t="str">
+      <c r="T1" s="14" t="str">
         <f>_xlfn.CONCAT($P$3,".",T5)</f>
         <v>plugins.families.families-guardians-info</v>
       </c>
-      <c r="U1" s="13" t="str">
+      <c r="U1" s="14" t="str">
         <f>_xlfn.CONCAT($P$3,".",U5)</f>
         <v>plugins.families.families-students-info</v>
       </c>
     </row>
-    <row r="2" s="14" customFormat="1" ht="21.350000000000001" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+    <row r="2" s="9" customFormat="1" ht="21.350000000000001" customHeight="1">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="15" t="s">
         <v>27</v>
       </c>
@@ -2214,7 +3626,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" s="46" customFormat="1" ht="19.100000000000001" customHeight="1">
+    <row r="6" s="46" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2279,232 +3691,232 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>69</v>
       </c>
       <c r="D7" s="57"/>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="57" t="s">
+      <c r="H7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="57" t="s">
+      <c r="I7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="57" t="s">
+      <c r="J7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="57" t="s">
+      <c r="K7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="57" t="s">
+      <c r="L7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="M7" s="57" t="s">
+      <c r="M7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="57" t="s">
+      <c r="N7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="O7" s="57" t="s">
+      <c r="O7" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="58" t="s">
+      <c r="P7" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="Q7" s="58" t="s">
+      <c r="Q7" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="R7" s="58"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
-      <c r="U7" s="59"/>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="9" t="s">
+      <c r="R7" s="59"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="60"/>
+    </row>
+    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="57"/>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="57" t="s">
+      <c r="H8" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="57" t="s">
+      <c r="J8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="57" t="s">
+      <c r="K8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="L8" s="57" t="s">
+      <c r="L8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57" t="s">
+      <c r="M8" s="58"/>
+      <c r="N8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="O8" s="57" t="s">
+      <c r="O8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="P8" s="57" t="s">
+      <c r="P8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="Q8" s="57" t="s">
+      <c r="Q8" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="R8" s="58"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="9" t="s">
+      <c r="R8" s="59"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+    </row>
+    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>77</v>
       </c>
       <c r="D9" s="57"/>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="57" t="s">
+      <c r="I9" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="57" t="s">
+      <c r="J9" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="57" t="s">
+      <c r="K9" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="L9" s="57" t="s">
+      <c r="L9" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="M9" s="57"/>
-      <c r="N9" s="57" t="s">
+      <c r="M9" s="58"/>
+      <c r="N9" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="57"/>
-      <c r="P9" s="57" t="s">
+      <c r="O9" s="58"/>
+      <c r="P9" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="Q9" s="57" t="s">
+      <c r="Q9" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="R9" s="60" t="s">
+      <c r="R9" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="S9" s="57" t="s">
+      <c r="S9" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="T9" s="57" t="s">
+      <c r="T9" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="U9" s="57" t="s">
+      <c r="U9" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D10" s="57" t="str">
         <f>A9</f>
         <v>student</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I10" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="57" t="s">
+      <c r="J10" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="57" t="s">
+      <c r="K10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="57" t="s">
+      <c r="L10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57" t="s">
+      <c r="M10" s="58"/>
+      <c r="N10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57" t="s">
+      <c r="O10" s="58"/>
+      <c r="P10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="Q10" s="57" t="s">
+      <c r="Q10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="R10" s="57" t="s">
+      <c r="R10" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="S10" s="57" t="s">
+      <c r="S10" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="T10" s="57" t="s">
+      <c r="T10" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="U10" s="57" t="s">
+      <c r="U10" s="58" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2570,7 +3982,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" ht="22.100000000000001" customHeight="1">
+    <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
@@ -2586,191 +3998,191 @@
       <c r="E2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="63" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="63" t="s">
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="66" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="63" t="s">
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="66" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="66" t="s">
+    <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A5" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="66" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="66" t="s">
+    <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A6" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="D6" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="G6" s="70" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="66" t="s">
+    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="66" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="66" t="s">
+    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="70" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="66" t="s">
+    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A9" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="65" t="s">
+      <c r="G9" s="66" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="69"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="69"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2817,25 +4229,37 @@
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="73" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="63" t="s">
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="9" t="s">
+      <c r="B3" s="74" t="str">
+        <f>profiles!$A$10</f>
+        <v>guardian</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="B4" s="75" t="str">
+        <f>profiles!$A$9</f>
+        <v>student</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" ht="14.25"/>
     <row r="6" ht="14.25"/>
@@ -2864,7 +4288,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="2" max="2" width="58.78125"/>
+    <col customWidth="1" min="2" max="2" width="67.57421875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2876,20 +4300,21 @@
       </c>
     </row>
     <row r="2" ht="24.350000000000001" customHeight="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="9" t="s">
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="74" t="s">
         <v>123</v>
       </c>
+      <c r="C3" s="9"/>
     </row>
     <row r="4"/>
   </sheetData>
@@ -2926,27 +4351,29 @@
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="77" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="74" t="str">
+        <f>profiles!$A$8</f>
+        <v>teacher</v>
+      </c>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>75</v>
+      <c r="B4" s="75" t="str">
+        <f>profiles!$A$9</f>
+        <v>student</v>
       </c>
     </row>
   </sheetData>
@@ -2965,7 +4392,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="Q1" workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="0" topLeftCell="O1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2974,18 +4401,22 @@
     <col customWidth="1" min="1" max="1" width="11.00390625"/>
     <col customWidth="1" min="2" max="2" width="19.140625"/>
     <col customWidth="1" min="3" max="3" width="12.00390625"/>
-    <col customWidth="1" min="5" max="5" width="17.7109375"/>
-    <col customWidth="1" min="6" max="6" width="12.28125"/>
-    <col customWidth="1" min="7" max="7" width="13.00390625"/>
-    <col customWidth="1" min="8" max="11" width="17.00390625"/>
-    <col bestFit="1" min="12" max="12" width="20.8515625"/>
-    <col min="13" max="13" width="20.8515625"/>
-    <col bestFit="1" min="14" max="14" width="22.78125"/>
-    <col customWidth="1" min="15" max="15" width="23.7109375"/>
-    <col customWidth="1" min="16" max="18" width="26.7109375"/>
-    <col customWidth="1" min="19" max="19" width="18.7109375"/>
-    <col bestFit="1" min="20" max="20" width="23.78125"/>
-    <col customWidth="1" min="21" max="21" width="29.8515625"/>
+    <col customWidth="1" min="5" max="5" width="11.140625"/>
+    <col customWidth="1" min="6" max="6" width="9.57421875"/>
+    <col customWidth="1" min="7" max="7" width="9.00390625"/>
+    <col customWidth="1" min="8" max="8" width="11.8515625"/>
+    <col customWidth="1" min="9" max="10" width="17.00390625"/>
+    <col customWidth="1" min="11" max="11" width="12.421875"/>
+    <col customWidth="1" min="12" max="12" width="12.140625"/>
+    <col customWidth="1" min="13" max="13" width="17.00390625"/>
+    <col customWidth="1" min="14" max="14" width="14.8515625"/>
+    <col customWidth="1" min="15" max="15" width="13.00390625"/>
+    <col customWidth="1" min="16" max="18" width="14.7109375"/>
+    <col customWidth="1" min="19" max="19" width="15.8515625"/>
+    <col customWidth="1" min="20" max="20" width="15.28125"/>
+    <col customWidth="1" min="21" max="21" width="12.8515625"/>
+    <col customWidth="1" min="22" max="22" width="14.140625"/>
+    <col customWidth="1" min="23" max="23" width="18.140625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3052,8 +4483,12 @@
       <c r="U1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="V1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
@@ -3068,231 +4503,253 @@
       <c r="AI1" s="5"/>
       <c r="AJ1" s="5"/>
       <c r="AK1" s="5"/>
-    </row>
-    <row r="2" s="14" customFormat="1" ht="23.600000000000001" customHeight="1">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="E2" s="73" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="77" t="s">
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+    </row>
+    <row r="2" s="9" customFormat="1" ht="23.600000000000001" customHeight="1">
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="E2" s="79" t="s">
         <v>144</v>
       </c>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78" t="s">
+      <c r="F2" s="79"/>
+      <c r="G2" s="80" t="s">
         <v>145</v>
       </c>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="81" t="s">
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-    </row>
-    <row r="3" ht="24.350000000000001" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="84" t="s">
+        <v>147</v>
+      </c>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+    </row>
+    <row r="3" ht="34.100000000000001" customHeight="1">
+      <c r="A3" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="90" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="83" t="s">
-        <v>148</v>
-      </c>
-      <c r="F3" s="84" t="s">
-        <v>149</v>
-      </c>
-      <c r="G3" s="85" t="s">
+      <c r="E3" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="H3" s="86" t="s">
+      <c r="F3" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="I3" s="87" t="s">
+      <c r="G3" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="H3" s="95" t="s">
         <v>153</v>
       </c>
-      <c r="K3" s="87" t="s">
+      <c r="I3" s="96" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="88" t="s">
+      <c r="J3" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="M3" s="89" t="s">
+      <c r="K3" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="N3" s="90" t="s">
+      <c r="L3" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="O3" s="91" t="s">
+      <c r="M3" s="96" t="s">
         <v>158</v>
       </c>
-      <c r="P3" s="92" t="s">
+      <c r="N3" s="97" t="s">
         <v>159</v>
       </c>
-      <c r="Q3" s="92" t="s">
-        <v>156</v>
-      </c>
-      <c r="R3" s="92" t="s">
+      <c r="O3" s="98" t="s">
         <v>157</v>
       </c>
-      <c r="S3" s="93" t="s">
-        <v>156</v>
-      </c>
-      <c r="T3" s="94" t="s">
+      <c r="P3" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q3" s="100" t="s">
         <v>160</v>
       </c>
-      <c r="U3" s="95" t="s">
+      <c r="R3" s="101" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" s="14" customFormat="1">
-      <c r="A4" s="96" t="s">
+      <c r="S3" s="101" t="s">
+        <v>157</v>
+      </c>
+      <c r="T3" s="101" t="s">
+        <v>158</v>
+      </c>
+      <c r="U3" s="102" t="s">
+        <v>157</v>
+      </c>
+      <c r="V3" s="103" t="s">
         <v>162</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="W3" s="104" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="98" t="s">
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="98" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="98" t="s">
+      <c r="B4" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="74" t="str">
+        <f>centers!$A$3</f>
+        <v>centerA</v>
+      </c>
+      <c r="E4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97">
+      <c r="F4" s="58">
+        <v>0</v>
+      </c>
+      <c r="G4" s="58">
         <v>5</v>
       </c>
-      <c r="H4" s="97"/>
-      <c r="I4" s="98" t="s">
+      <c r="H4" s="58"/>
+      <c r="I4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="99"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98" t="s">
+      <c r="J4" s="105"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="97"/>
-      <c r="N4" s="98" t="s">
+      <c r="O4" s="58"/>
+      <c r="P4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="98" t="s">
+      <c r="Q4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="97" t="s">
+      <c r="R4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="97">
+      <c r="S4" s="58">
         <v>3</v>
       </c>
-      <c r="R4" s="97" t="s">
+      <c r="T4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="97">
+      <c r="U4" s="58">
+        <v>3</v>
+      </c>
+      <c r="V4" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" s="58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" s="9" customFormat="1" ht="28.5">
+      <c r="A5" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="74" t="str">
+        <f>centers!$A$4</f>
+        <v>centerB</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="58">
+        <v>240</v>
+      </c>
+      <c r="G5" s="58">
         <v>4</v>
       </c>
-      <c r="T4" s="97" t="s">
+      <c r="H5" s="58">
+        <v>60</v>
+      </c>
+      <c r="I5" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="97" t="s">
+      <c r="J5" s="105" t="s">
+        <v>170</v>
+      </c>
+      <c r="K5" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="58">
+        <v>4</v>
+      </c>
+      <c r="M5" s="61" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" s="14" customFormat="1" ht="28.5">
-      <c r="A5" s="96" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="97" t="s">
-        <v>166</v>
-      </c>
-      <c r="C5" s="98" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="98" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="97" t="s">
+      <c r="N5" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="97">
-        <v>240</v>
-      </c>
-      <c r="G5" s="97">
+      <c r="O5" s="58">
         <v>4</v>
       </c>
-      <c r="H5" s="97">
-        <v>60</v>
-      </c>
-      <c r="I5" s="97" t="s">
+      <c r="P5" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="58">
+        <v>3</v>
+      </c>
+      <c r="T5" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="U5" s="58">
+        <v>3</v>
+      </c>
+      <c r="V5" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="99" t="s">
-        <v>168</v>
-      </c>
-      <c r="K5" s="97" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="97">
-        <v>4</v>
-      </c>
-      <c r="N5" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="P5" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="97">
-        <v>3</v>
-      </c>
-      <c r="R5" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="97">
-        <v>4</v>
-      </c>
-      <c r="T5" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="U5" s="97" t="s">
+      <c r="W5" s="58" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="U2:W2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -3301,79 +4758,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00280057-00EE-4C32-AFB3-006400E5004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C20012-0087-4370-A086-00AF00320063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>U4</xm:sqref>
+          <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CC009C-0074-4F64-984D-00E100CF0084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00900010-0065-4553-ABE7-00C5008700D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>U5</xm:sqref>
+          <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009E000A-0083-491D-8E68-008200F30034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B80059-0069-4640-9FFB-007D00C800EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>V4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00CD0065-0061-4059-A05F-008700490055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>V5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00750008-00EA-4FA0-8869-005E00520075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D1008E-0042-45DB-BED4-0038009A009A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00800098-0094-40AC-AB32-003D00040072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003000A3-004B-429E-832B-009700AE009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F3006A-00AD-4F2C-993A-00B500FC0009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>R4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00540040-0075-4ED1-8F54-00A700B90004}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>BOOLEAN_ANSWER</xm:f>
-          </x14:formula1>
-          <xm:sqref>R5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0014006F-0053-4809-B438-000400F100C9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>BOOLEAN_ANSWER</xm:f>
-          </x14:formula1>
-          <xm:sqref>P4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CA0082-00F7-4107-9D9A-009300790080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00350060-001F-4262-A2FB-00CA005F0067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DC00DC-0057-410A-8D23-009800920095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00280060-006F-4D11-A880-00FA003D0046}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F90096-0040-4EC1-BA5A-002900D7001B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000D0037-0028-4FED-BF71-00D400710068}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001B0035-00B9-48DD-BD61-00EF004400F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003A00BB-0004-490E-B403-009700BE008F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004E0056-006B-447E-B646-001400C70086}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B00026-00C5-4B2E-A29D-005100EB0096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FA00D4-0093-4F38-A778-00BE00ED000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EB00D7-00D5-4E2C-87E7-0062006300C9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -3393,15 +4850,133 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="11.421875"/>
+    <col customWidth="1" min="4" max="4" width="10.421875"/>
+    <col customWidth="1" min="5" max="5" width="12.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" ht="28.5">
+      <c r="A2" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="91" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="106" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="106" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="64" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="75" t="str">
+        <f>ap_programs!$A$4</f>
+        <v>programA</v>
+      </c>
+      <c r="D3" s="58">
+        <v>0</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="75" t="str">
+        <f>ap_programs!$A$5</f>
+        <v>programB</v>
+      </c>
+      <c r="D4" s="58">
+        <v>0</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="64" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="75" t="str">
+        <f>ap_programs!$A$4</f>
+        <v>programA</v>
+      </c>
+      <c r="D5" s="58">
+        <v>0</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
+        <x14:dataValidation xr:uid="{0046008B-0027-4D50-B669-00BD0023004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D10051-0023-454F-B6CA-00E2008600EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00A800BD-004C-404B-9ABE-001B00E700FC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATED: MVP-template profiles columns and permissions
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -129,6 +129,15 @@
     <t>plugins.families</t>
   </si>
   <si>
+    <t>plugins.timetable</t>
+  </si>
+  <si>
+    <t>plugins.tasks</t>
+  </si>
+  <si>
+    <t>plugins.curriculum</t>
+  </si>
+  <si>
     <t>Users</t>
   </si>
   <si>
@@ -144,6 +153,15 @@
     <t>Families</t>
   </si>
   <si>
+    <t>Timetable</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Curriculum</t>
+  </si>
+  <si>
     <t>users</t>
   </si>
   <si>
@@ -192,6 +210,24 @@
     <t>families-students-info</t>
   </si>
   <si>
+    <t>timetable</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>library</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>curriculum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Can access to</t>
   </si>
   <si>
@@ -229,6 +265,18 @@
   </si>
   <si>
     <t xml:space="preserve">Students info</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>History</t>
   </si>
   <si>
     <t>admin</t>
@@ -974,7 +1022,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1172,6 +1220,19 @@
     </border>
     <border>
       <left style="thin">
+        <color theme="0" tint="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="0" tint="-0.249977111117893"/>
       </left>
       <right style="thin">
@@ -1239,7 +1300,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="129">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1306,6 +1367,12 @@
     <xf fontId="9" fillId="11" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="6" fillId="8" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="6" fillId="8" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1336,6 +1403,9 @@
     <xf fontId="1" fillId="11" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="1" fillId="8" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="5" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1399,16 +1469,19 @@
     <xf fontId="4" fillId="15" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="4" fillId="13" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1471,10 +1544,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="7" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="1" fillId="8" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="7" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="8" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1483,16 +1553,19 @@
     <xf fontId="1" fillId="8" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="9" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="8" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="17" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="9" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="17" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="17" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="17" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="10" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2222,89 +2295,89 @@
         <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="108" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="108" t="s">
-        <v>183</v>
-      </c>
-      <c r="E2" s="108" t="s">
-        <v>184</v>
-      </c>
-      <c r="F2" s="109" t="s">
-        <v>174</v>
-      </c>
-      <c r="G2" s="110" t="s">
-        <v>151</v>
+      <c r="C2" s="112" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="112" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="112" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" s="113" t="s">
+        <v>190</v>
+      </c>
+      <c r="G2" s="114" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="64" t="s">
-        <v>185</v>
+      <c r="A3" s="68" t="s">
+        <v>201</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="111" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" s="75" t="str">
+        <v>204</v>
+      </c>
+      <c r="E3" s="115" t="s">
+        <v>205</v>
+      </c>
+      <c r="F3" s="79" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G3" s="58">
+      <c r="G3" s="62">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="64" t="s">
-        <v>190</v>
+      <c r="A4" s="68" t="s">
+        <v>206</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>194</v>
-      </c>
-      <c r="F4" s="75" t="str">
+        <v>209</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="79" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="62">
         <v>0</v>
       </c>
     </row>
@@ -2329,6 +2402,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0" zoomScale="100">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A4" ySplit="3"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2353,86 +2427,86 @@
       <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="112" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" s="112" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="112" t="s">
-        <v>196</v>
+      <c r="C1" s="116" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="116" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="116" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="116" t="s">
+        <v>212</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>181</v>
-      </c>
       <c r="I1" s="5" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="K1" s="113" t="s">
-        <v>200</v>
-      </c>
-      <c r="L1" s="72"/>
+        <v>215</v>
+      </c>
+      <c r="K1" s="117" t="s">
+        <v>216</v>
+      </c>
+      <c r="L1" s="76"/>
     </row>
     <row r="2" ht="28.850000000000001" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="114" t="s">
-        <v>201</v>
-      </c>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="72"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="118" t="s">
+        <v>217</v>
+      </c>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="76"/>
     </row>
     <row r="3" ht="31.850000000000001" customHeight="1">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="115" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" s="90" t="s">
-        <v>202</v>
-      </c>
-      <c r="E3" s="90" t="s">
-        <v>203</v>
-      </c>
-      <c r="F3" s="90" t="s">
-        <v>204</v>
-      </c>
-      <c r="G3" s="116" t="s">
-        <v>205</v>
-      </c>
-      <c r="H3" s="117" t="s">
-        <v>183</v>
-      </c>
-      <c r="I3" s="117" t="s">
-        <v>206</v>
-      </c>
-      <c r="J3" s="118" t="s">
-        <v>207</v>
-      </c>
-      <c r="K3" s="109" t="s">
-        <v>208</v>
-      </c>
-      <c r="L3" s="119"/>
+      <c r="C3" s="119" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="94" t="s">
+        <v>219</v>
+      </c>
+      <c r="F3" s="94" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="H3" s="121" t="s">
+        <v>199</v>
+      </c>
+      <c r="I3" s="121" t="s">
+        <v>222</v>
+      </c>
+      <c r="J3" s="122" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="113" t="s">
+        <v>224</v>
+      </c>
+      <c r="L3" s="123"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
@@ -2440,35 +2514,35 @@
         <v>subject01</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="75" t="str">
+        <v>225</v>
+      </c>
+      <c r="C4" s="79" t="str">
         <f>ap_programs!A4</f>
         <v>programA</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="62">
         <v>1</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58" t="str">
+      <c r="E4" s="62"/>
+      <c r="F4" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L4&lt;10,"0",""),L4)</f>
         <v>001</v>
       </c>
-      <c r="G4" s="120" t="s">
-        <v>210</v>
-      </c>
-      <c r="H4" s="121" t="s">
-        <v>211</v>
-      </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="122" t="str">
+      <c r="G4" s="124" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="125" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" s="62"/>
+      <c r="J4" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K4" s="123" t="s">
-        <v>212</v>
-      </c>
-      <c r="L4" s="124">
+      <c r="K4" s="127" t="s">
+        <v>228</v>
+      </c>
+      <c r="L4" s="128">
         <v>1</v>
       </c>
       <c r="M4" s="9"/>
@@ -2479,38 +2553,38 @@
         <v>subject02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="C5" s="75" t="str">
+        <v>229</v>
+      </c>
+      <c r="C5" s="79" t="str">
         <f>C4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="62">
         <v>1</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58" t="str">
+      <c r="E5" s="62"/>
+      <c r="F5" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L5&lt;10,"0",""),L5)</f>
         <v>002</v>
       </c>
-      <c r="G5" s="120" t="str">
+      <c r="G5" s="124" t="str">
         <f>G4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H5" s="121" t="str">
+      <c r="H5" s="125" t="str">
         <f>H4</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="122" t="str">
+      <c r="I5" s="62"/>
+      <c r="J5" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K5" s="123" t="str">
+      <c r="K5" s="127" t="str">
         <f>K4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L5" s="124">
+      <c r="L5" s="128">
         <f>L4+1</f>
         <v>2</v>
       </c>
@@ -2522,38 +2596,38 @@
         <v>subject03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C6" s="75" t="str">
+        <v>230</v>
+      </c>
+      <c r="C6" s="79" t="str">
         <f>C5</f>
         <v>programA</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="62">
         <v>1</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58" t="str">
+      <c r="E6" s="62"/>
+      <c r="F6" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L6&lt;10,"0",""),L6)</f>
         <v>003</v>
       </c>
-      <c r="G6" s="120" t="str">
+      <c r="G6" s="124" t="str">
         <f>G5</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H6" s="121" t="str">
+      <c r="H6" s="125" t="str">
         <f>H5</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="122" t="str">
+      <c r="I6" s="62"/>
+      <c r="J6" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K6" s="123" t="str">
+      <c r="K6" s="127" t="str">
         <f>K5</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L6" s="124">
+      <c r="L6" s="128">
         <f>L5+1</f>
         <v>3</v>
       </c>
@@ -2565,38 +2639,38 @@
         <v>subject04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" s="75" t="str">
+        <v>231</v>
+      </c>
+      <c r="C7" s="79" t="str">
         <f>C6</f>
         <v>programA</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="62">
         <v>1</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58" t="str">
+      <c r="E7" s="62"/>
+      <c r="F7" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L7&lt;10,"0",""),L7)</f>
         <v>004</v>
       </c>
-      <c r="G7" s="120" t="str">
+      <c r="G7" s="124" t="str">
         <f>G6</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H7" s="121" t="str">
+      <c r="H7" s="125" t="str">
         <f>H6</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="122" t="str">
+      <c r="I7" s="62"/>
+      <c r="J7" s="126" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K7" s="123" t="str">
+      <c r="K7" s="127" t="str">
         <f>K6</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L7" s="124">
+      <c r="L7" s="128">
         <f>L6+1</f>
         <v>4</v>
       </c>
@@ -2608,36 +2682,36 @@
         <v>subject05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C8" s="75" t="str">
+        <v>232</v>
+      </c>
+      <c r="C8" s="79" t="str">
         <f>C7</f>
         <v>programA</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="62">
         <v>2</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58" t="str">
+      <c r="E8" s="62"/>
+      <c r="F8" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L8&lt;10,"0",""),L8)</f>
         <v>005</v>
       </c>
-      <c r="G8" s="120" t="s">
-        <v>217</v>
-      </c>
-      <c r="H8" s="121" t="str">
+      <c r="G8" s="124" t="s">
+        <v>233</v>
+      </c>
+      <c r="H8" s="125" t="str">
         <f>H7</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I8" s="58"/>
-      <c r="J8" s="122" t="str">
+      <c r="I8" s="62"/>
+      <c r="J8" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K8" s="123" t="s">
-        <v>218</v>
-      </c>
-      <c r="L8" s="124">
+      <c r="K8" s="127" t="s">
+        <v>234</v>
+      </c>
+      <c r="L8" s="128">
         <f>L7+1</f>
         <v>5</v>
       </c>
@@ -2648,37 +2722,37 @@
         <v>subject06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C9" s="75" t="str">
+        <v>235</v>
+      </c>
+      <c r="C9" s="79" t="str">
         <f>C8</f>
         <v>programA</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="62">
         <v>2</v>
       </c>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58" t="str">
+      <c r="E9" s="62"/>
+      <c r="F9" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L9&lt;10,"0",""),L9)</f>
         <v>006</v>
       </c>
-      <c r="G9" s="120" t="str">
+      <c r="G9" s="124" t="str">
         <f>G8</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H9" s="121" t="s">
-        <v>220</v>
-      </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="122" t="str">
+      <c r="H9" s="125" t="s">
+        <v>236</v>
+      </c>
+      <c r="I9" s="62"/>
+      <c r="J9" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K9" s="123" t="str">
+      <c r="K9" s="127" t="str">
         <f>K8</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L9" s="124">
+      <c r="L9" s="128">
         <f>L8+1</f>
         <v>6</v>
       </c>
@@ -2689,38 +2763,38 @@
         <v>subject07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="C10" s="75" t="str">
+        <v>237</v>
+      </c>
+      <c r="C10" s="79" t="str">
         <f>C9</f>
         <v>programA</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="62">
         <v>2</v>
       </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58" t="str">
+      <c r="E10" s="62"/>
+      <c r="F10" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L10&lt;10,"0",""),L10)</f>
         <v>007</v>
       </c>
-      <c r="G10" s="120" t="str">
+      <c r="G10" s="124" t="str">
         <f>G9</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H10" s="121" t="str">
+      <c r="H10" s="125" t="str">
         <f>H9</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I10" s="58"/>
-      <c r="J10" s="122" t="str">
+      <c r="I10" s="62"/>
+      <c r="J10" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K10" s="123" t="str">
+      <c r="K10" s="127" t="str">
         <f>K9</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L10" s="124">
+      <c r="L10" s="128">
         <f>L9+1</f>
         <v>7</v>
       </c>
@@ -2731,38 +2805,38 @@
         <v>subject08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11" s="75" t="str">
+        <v>238</v>
+      </c>
+      <c r="C11" s="79" t="str">
         <f>C10</f>
         <v>programA</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="62">
         <v>2</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58" t="str">
+      <c r="E11" s="62"/>
+      <c r="F11" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L11&lt;10,"0",""),L11)</f>
         <v>008</v>
       </c>
-      <c r="G11" s="120" t="str">
+      <c r="G11" s="124" t="str">
         <f>G10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H11" s="121" t="str">
+      <c r="H11" s="125" t="str">
         <f>H10</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I11" s="58"/>
-      <c r="J11" s="122" t="str">
+      <c r="I11" s="62"/>
+      <c r="J11" s="126" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K11" s="123" t="str">
+      <c r="K11" s="127" t="str">
         <f>K10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L11" s="124">
+      <c r="L11" s="128">
         <f>L10+1</f>
         <v>8</v>
       </c>
@@ -2773,36 +2847,36 @@
         <v>subject09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C12" s="75" t="str">
+        <v>239</v>
+      </c>
+      <c r="C12" s="79" t="str">
         <f>C11</f>
         <v>programA</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="62">
         <v>3</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58" t="str">
+      <c r="E12" s="62"/>
+      <c r="F12" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L12&lt;10,"0",""),L12)</f>
         <v>009</v>
       </c>
-      <c r="G12" s="120" t="s">
-        <v>224</v>
-      </c>
-      <c r="H12" s="121" t="str">
+      <c r="G12" s="124" t="s">
+        <v>240</v>
+      </c>
+      <c r="H12" s="125" t="str">
         <f>H11</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I12" s="58"/>
-      <c r="J12" s="122" t="str">
+      <c r="I12" s="62"/>
+      <c r="J12" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K12" s="123" t="s">
-        <v>225</v>
-      </c>
-      <c r="L12" s="124">
+      <c r="K12" s="127" t="s">
+        <v>241</v>
+      </c>
+      <c r="L12" s="128">
         <f>L11+1</f>
         <v>9</v>
       </c>
@@ -2813,38 +2887,38 @@
         <v>subject10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="C13" s="75" t="str">
+        <v>242</v>
+      </c>
+      <c r="C13" s="79" t="str">
         <f>C12</f>
         <v>programA</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="62">
         <v>3</v>
       </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58" t="str">
+      <c r="E13" s="62"/>
+      <c r="F13" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L13&lt;10,"0",""),L13)</f>
         <v>010</v>
       </c>
-      <c r="G13" s="120" t="str">
+      <c r="G13" s="124" t="str">
         <f>G12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H13" s="121" t="str">
+      <c r="H13" s="125" t="str">
         <f>H12</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I13" s="58"/>
-      <c r="J13" s="122" t="str">
+      <c r="I13" s="62"/>
+      <c r="J13" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K13" s="123" t="str">
+      <c r="K13" s="127" t="str">
         <f>K12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L13" s="124">
+      <c r="L13" s="128">
         <f>L12+1</f>
         <v>10</v>
       </c>
@@ -2855,37 +2929,37 @@
         <v>subject11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C14" s="75" t="str">
+        <v>243</v>
+      </c>
+      <c r="C14" s="79" t="str">
         <f>C13</f>
         <v>programA</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="62">
         <v>3</v>
       </c>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58" t="str">
+      <c r="E14" s="62"/>
+      <c r="F14" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L14&lt;10,"0",""),L14)</f>
         <v>011</v>
       </c>
-      <c r="G14" s="120" t="str">
+      <c r="G14" s="124" t="str">
         <f>G13</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H14" s="121" t="s">
-        <v>228</v>
-      </c>
-      <c r="I14" s="58"/>
-      <c r="J14" s="122" t="str">
+      <c r="H14" s="125" t="s">
+        <v>244</v>
+      </c>
+      <c r="I14" s="62"/>
+      <c r="J14" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K14" s="123" t="str">
+      <c r="K14" s="127" t="str">
         <f>K13</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L14" s="124">
+      <c r="L14" s="128">
         <f>L13+1</f>
         <v>11</v>
       </c>
@@ -2896,38 +2970,38 @@
         <v>subject12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="C15" s="75" t="str">
+        <v>245</v>
+      </c>
+      <c r="C15" s="79" t="str">
         <f>C14</f>
         <v>programA</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="62">
         <v>3</v>
       </c>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58" t="str">
+      <c r="E15" s="62"/>
+      <c r="F15" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L15&lt;10,"0",""),L15)</f>
         <v>012</v>
       </c>
-      <c r="G15" s="120" t="str">
+      <c r="G15" s="124" t="str">
         <f>G14</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H15" s="121" t="str">
+      <c r="H15" s="125" t="str">
         <f>H14</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I15" s="58"/>
-      <c r="J15" s="122" t="str">
+      <c r="I15" s="62"/>
+      <c r="J15" s="126" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K15" s="123" t="str">
+      <c r="K15" s="127" t="str">
         <f>K14</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L15" s="124">
+      <c r="L15" s="128">
         <f>L14+1</f>
         <v>12</v>
       </c>
@@ -2938,36 +3012,36 @@
         <v>subject13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="C16" s="75" t="str">
+        <v>246</v>
+      </c>
+      <c r="C16" s="79" t="str">
         <f>C15</f>
         <v>programA</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="62">
         <v>4</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58" t="str">
+      <c r="E16" s="62"/>
+      <c r="F16" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L16&lt;10,"0",""),L16)</f>
         <v>013</v>
       </c>
-      <c r="G16" s="120" t="s">
-        <v>231</v>
-      </c>
-      <c r="H16" s="121" t="str">
+      <c r="G16" s="124" t="s">
+        <v>247</v>
+      </c>
+      <c r="H16" s="125" t="str">
         <f>H15</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I16" s="58"/>
-      <c r="J16" s="122" t="str">
+      <c r="I16" s="62"/>
+      <c r="J16" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K16" s="123" t="s">
-        <v>232</v>
-      </c>
-      <c r="L16" s="124">
+      <c r="K16" s="127" t="s">
+        <v>248</v>
+      </c>
+      <c r="L16" s="128">
         <f>L15+1</f>
         <v>13</v>
       </c>
@@ -2978,38 +3052,38 @@
         <v>subject14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="C17" s="75" t="str">
+        <v>249</v>
+      </c>
+      <c r="C17" s="79" t="str">
         <f>C16</f>
         <v>programA</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="62">
         <v>4</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58" t="str">
+      <c r="E17" s="62"/>
+      <c r="F17" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L17&lt;10,"0",""),L17)</f>
         <v>014</v>
       </c>
-      <c r="G17" s="120" t="str">
+      <c r="G17" s="124" t="str">
         <f>G16</f>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H17" s="121" t="str">
+      <c r="H17" s="125" t="str">
         <f>H16</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I17" s="58"/>
-      <c r="J17" s="122" t="str">
+      <c r="I17" s="62"/>
+      <c r="J17" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K17" s="123" t="str">
+      <c r="K17" s="127" t="str">
         <f>K16</f>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L17" s="124">
+      <c r="L17" s="128">
         <f>L16+1</f>
         <v>14</v>
       </c>
@@ -3020,38 +3094,38 @@
         <v>subject15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="75" t="str">
+        <v>250</v>
+      </c>
+      <c r="C18" s="79" t="str">
         <f>C17</f>
         <v>programA</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="62">
         <v>4</v>
       </c>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58" t="str">
+      <c r="E18" s="62"/>
+      <c r="F18" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L18&lt;10,"0",""),L18)</f>
         <v>015</v>
       </c>
-      <c r="G18" s="120" t="str">
+      <c r="G18" s="124" t="str">
         <f>G17</f>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H18" s="121" t="str">
+      <c r="H18" s="125" t="str">
         <f>H17</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I18" s="58"/>
-      <c r="J18" s="122" t="str">
+      <c r="I18" s="62"/>
+      <c r="J18" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K18" s="123" t="str">
+      <c r="K18" s="127" t="str">
         <f>K17</f>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L18" s="124">
+      <c r="L18" s="128">
         <f>L17+1</f>
         <v>15</v>
       </c>
@@ -3062,37 +3136,37 @@
         <v>subject16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C19" s="75" t="str">
+        <v>251</v>
+      </c>
+      <c r="C19" s="79" t="str">
         <f>C18</f>
         <v>programA</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="62">
         <v>4</v>
       </c>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58" t="str">
+      <c r="E19" s="62"/>
+      <c r="F19" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L19&lt;10,"0",""),L19)</f>
         <v>016</v>
       </c>
-      <c r="G19" s="120" t="str">
+      <c r="G19" s="124" t="str">
         <f>G18</f>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H19" s="121" t="s">
-        <v>236</v>
-      </c>
-      <c r="I19" s="58"/>
-      <c r="J19" s="122" t="str">
+      <c r="H19" s="125" t="s">
+        <v>252</v>
+      </c>
+      <c r="I19" s="62"/>
+      <c r="J19" s="126" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K19" s="123" t="str">
+      <c r="K19" s="127" t="str">
         <f>K18</f>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L19" s="124">
+      <c r="L19" s="128">
         <f>L18+1</f>
         <v>16</v>
       </c>
@@ -3103,35 +3177,35 @@
         <v>subject17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C20" s="75" t="str">
+        <v>253</v>
+      </c>
+      <c r="C20" s="79" t="str">
         <f>C19</f>
         <v>programA</v>
       </c>
-      <c r="D20" s="58">
+      <c r="D20" s="62">
         <v>5</v>
       </c>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58" t="str">
+      <c r="E20" s="62"/>
+      <c r="F20" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L20&lt;10,"0",""),L20)</f>
         <v>017</v>
       </c>
-      <c r="G20" s="120" t="s">
-        <v>238</v>
-      </c>
-      <c r="H20" s="121" t="s">
-        <v>236</v>
-      </c>
-      <c r="I20" s="58"/>
-      <c r="J20" s="122" t="str">
+      <c r="G20" s="124" t="s">
+        <v>254</v>
+      </c>
+      <c r="H20" s="125" t="s">
+        <v>252</v>
+      </c>
+      <c r="I20" s="62"/>
+      <c r="J20" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K20" s="123" t="s">
-        <v>239</v>
-      </c>
-      <c r="L20" s="124">
+      <c r="K20" s="127" t="s">
+        <v>255</v>
+      </c>
+      <c r="L20" s="128">
         <f>L19+1</f>
         <v>17</v>
       </c>
@@ -3142,37 +3216,37 @@
         <v>subject18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C21" s="75" t="str">
+        <v>256</v>
+      </c>
+      <c r="C21" s="79" t="str">
         <f>C20</f>
         <v>programA</v>
       </c>
-      <c r="D21" s="58">
+      <c r="D21" s="62">
         <v>5</v>
       </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58" t="str">
+      <c r="E21" s="62"/>
+      <c r="F21" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L21&lt;10,"0",""),L21)</f>
         <v>018</v>
       </c>
-      <c r="G21" s="120" t="str">
+      <c r="G21" s="124" t="str">
         <f>G20</f>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H21" s="121" t="s">
-        <v>236</v>
-      </c>
-      <c r="I21" s="58"/>
-      <c r="J21" s="122" t="str">
+      <c r="H21" s="125" t="s">
+        <v>252</v>
+      </c>
+      <c r="I21" s="62"/>
+      <c r="J21" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K21" s="123" t="str">
+      <c r="K21" s="127" t="str">
         <f>K20</f>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L21" s="124">
+      <c r="L21" s="128">
         <f>L20+1</f>
         <v>18</v>
       </c>
@@ -3183,37 +3257,37 @@
         <v>subject19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="C22" s="75" t="str">
+        <v>257</v>
+      </c>
+      <c r="C22" s="79" t="str">
         <f>C21</f>
         <v>programA</v>
       </c>
-      <c r="D22" s="58">
+      <c r="D22" s="62">
         <v>5</v>
       </c>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58" t="str">
+      <c r="E22" s="62"/>
+      <c r="F22" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L22&lt;10,"0",""),L22)</f>
         <v>019</v>
       </c>
-      <c r="G22" s="120" t="str">
+      <c r="G22" s="124" t="str">
         <f>G21</f>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H22" s="121" t="s">
-        <v>236</v>
-      </c>
-      <c r="I22" s="58"/>
-      <c r="J22" s="122" t="str">
+      <c r="H22" s="125" t="s">
+        <v>252</v>
+      </c>
+      <c r="I22" s="62"/>
+      <c r="J22" s="126" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K22" s="123" t="str">
+      <c r="K22" s="127" t="str">
         <f>K21</f>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L22" s="124">
+      <c r="L22" s="128">
         <f>L21+1</f>
         <v>19</v>
       </c>
@@ -3224,43 +3298,43 @@
         <v>subject20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="C23" s="75" t="str">
+        <v>258</v>
+      </c>
+      <c r="C23" s="79" t="str">
         <f>C22</f>
         <v>programA</v>
       </c>
-      <c r="D23" s="58">
+      <c r="D23" s="62">
         <v>5</v>
       </c>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58" t="str">
+      <c r="E23" s="62"/>
+      <c r="F23" s="62" t="str">
         <f>_xlfn.CONCAT("0",IF(L23&lt;10,"0",""),L23)</f>
         <v>020</v>
       </c>
-      <c r="G23" s="120" t="str">
+      <c r="G23" s="124" t="str">
         <f>G22</f>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H23" s="121" t="s">
-        <v>236</v>
-      </c>
-      <c r="I23" s="58"/>
-      <c r="J23" s="122" t="str">
+      <c r="H23" s="125" t="s">
+        <v>252</v>
+      </c>
+      <c r="I23" s="62"/>
+      <c r="J23" s="126" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K23" s="123" t="str">
+      <c r="K23" s="127" t="str">
         <f>K22</f>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L23" s="124">
+      <c r="L23" s="128">
         <f>L22+1</f>
         <v>20</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="L24" s="72"/>
+      <c r="L24" s="76"/>
     </row>
     <row r="25" ht="14.25"/>
   </sheetData>
@@ -3381,6 +3455,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="B7" xSplit="1" ySplit="6"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3397,6 +3472,7 @@
     <col customWidth="1" min="19" max="19" width="12.140625"/>
     <col customWidth="1" min="20" max="21" width="14.7109375"/>
     <col customWidth="1" min="22" max="22" width="14.421875"/>
+    <col customWidth="1" min="28" max="28" width="15.00390625"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="1" ht="14.25">
@@ -3479,6 +3555,34 @@
       <c r="U1" s="14" t="str">
         <f>_xlfn.CONCAT($P$3,".",U5)</f>
         <v>plugins.families.families-students-info</v>
+      </c>
+      <c r="V1" s="13" t="str">
+        <f>_xlfn.CONCAT($V$3,".",V5)</f>
+        <v>plugins.timetable.config</v>
+      </c>
+      <c r="W1" s="13" t="str">
+        <f>_xlfn.CONCAT($V$3,".",W5)</f>
+        <v>plugins.timetable.timetable</v>
+      </c>
+      <c r="X1" s="13" t="str">
+        <f>_xlfn.CONCAT($X$3,".",X5)</f>
+        <v>plugins.tasks.tasks</v>
+      </c>
+      <c r="Y1" s="13" t="str">
+        <f>_xlfn.CONCAT($X$3,".",Y5)</f>
+        <v>plugins.tasks.library</v>
+      </c>
+      <c r="Z1" s="13" t="str">
+        <f>_xlfn.CONCAT($X$3,".",Z5)</f>
+        <v>plugins.tasks.ongoing</v>
+      </c>
+      <c r="AA1" s="13" t="str">
+        <f>_xlfn.CONCAT($X$3,".",AA5)</f>
+        <v>plugins.tasks.history</v>
+      </c>
+      <c r="AB1" s="13" t="str">
+        <f>_xlfn.CONCAT($AB$3,".",AB5)</f>
+        <v>plugins.curriculum.curriculum</v>
       </c>
     </row>
     <row r="2" s="9" customFormat="1" ht="21.350000000000001" customHeight="1">
@@ -3505,6 +3609,13 @@
       <c r="S2" s="15"/>
       <c r="T2" s="15"/>
       <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
     </row>
     <row r="3" ht="14.25">
       <c r="B3" s="16"/>
@@ -3537,96 +3648,143 @@
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
       <c r="U3" s="25"/>
-    </row>
-    <row r="4" s="26" customFormat="1" ht="19.850000000000001" customHeight="1">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27" t="s">
+      <c r="V3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29" t="s">
+      <c r="W3" s="18"/>
+      <c r="X3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="31" t="s">
+    </row>
+    <row r="4" s="28" customFormat="1" ht="19.850000000000001" customHeight="1">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="33" t="s">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="35"/>
+      <c r="J4" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="30"/>
+      <c r="X4" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="32" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
-      <c r="E5" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="41" t="s">
+      <c r="E5" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="F5" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" s="42" t="s">
+      <c r="G5" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="42" t="s">
+      <c r="H5" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="P5" s="43" t="s">
+      <c r="I5" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="Q5" s="44" t="s">
+      <c r="J5" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="R5" s="44" t="s">
+      <c r="K5" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="S5" s="44" t="s">
+      <c r="L5" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="T5" s="44" t="s">
+      <c r="M5" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="U5" s="45" t="s">
+      <c r="O5" s="45" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" s="46" customFormat="1" ht="19.5" customHeight="1">
+      <c r="P5" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="V5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="W5" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="X5" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y5" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z5" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA5" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB5" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" s="49" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -3636,299 +3794,394 @@
       <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>33</v>
+      <c r="D6" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>36</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="P6" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="R6" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="S6" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="T6" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="U6" s="56" t="s">
-        <v>66</v>
+      <c r="J6" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="N6" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="S6" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="T6" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="U6" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="V6" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="X6" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z6" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA6" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB6" s="60" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="K7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="L7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" s="59" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" s="59" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" s="59"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
+        <v>85</v>
+      </c>
+      <c r="D7" s="61"/>
+      <c r="E7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="O7" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="R7" s="63"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="W7" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="X7" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y7" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z7" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA7" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB7" s="62" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="P8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q8" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="59"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
+        <v>88</v>
+      </c>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="O8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="63"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="W8" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="X8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA8" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB8" s="62" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="L9" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="R9" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="S9" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="T9" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="U9" s="58" t="s">
-        <v>78</v>
+        <v>93</v>
+      </c>
+      <c r="D9" s="61"/>
+      <c r="E9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="M9" s="62"/>
+      <c r="N9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="R9" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="S9" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="T9" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="U9" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="V9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="W9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="X9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y9" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA9" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB9" s="65" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="57" t="str">
+        <v>97</v>
+      </c>
+      <c r="D10" s="61" t="str">
         <f>A9</f>
         <v>student</v>
       </c>
-      <c r="E10" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="K10" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q10" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="R10" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="S10" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="T10" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="U10" s="58" t="s">
-        <v>78</v>
-      </c>
+      <c r="E10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="L10" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q10" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="S10" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="T10" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="U10" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E2:U2"/>
+  <mergeCells count="11">
+    <mergeCell ref="E2:AB2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="K3:O3"/>
     <mergeCell ref="P3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:AA3"/>
     <mergeCell ref="E4:H4"/>
     <mergeCell ref="K4:O4"/>
     <mergeCell ref="P4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:AA4"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -3967,19 +4220,19 @@
         <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
@@ -3990,199 +4243,199 @@
         <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="D4" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A5" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="D5" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="66" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="G5" s="70" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A6" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="D7" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="66" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="67" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="69" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F5" s="58" t="s">
+      <c r="G7" s="70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="66" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="68" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="69" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" s="58" t="s">
+      <c r="G8" s="74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A9" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="75" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="70" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="69" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="66" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="69" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="70" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="67" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="71" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="66" t="s">
-        <v>117</v>
+      <c r="G9" s="70" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="72"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4222,22 +4475,22 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="73" t="s">
-        <v>119</v>
+      <c r="B2" s="77" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="74" t="str">
+      <c r="A3" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="78" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
@@ -4249,9 +4502,9 @@
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="75" t="str">
+        <v>91</v>
+      </c>
+      <c r="B4" s="79" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -4296,23 +4549,23 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" ht="24.350000000000001" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="77" t="s">
-        <v>121</v>
+      <c r="B2" s="81" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="74" t="s">
-        <v>123</v>
+        <v>138</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>139</v>
       </c>
       <c r="C3" s="9"/>
     </row>
@@ -4347,31 +4600,31 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="77" t="s">
-        <v>119</v>
+      <c r="B2" s="81" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="74" t="str">
+      <c r="A3" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="78" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="75" t="str">
+        <v>91</v>
+      </c>
+      <c r="B4" s="79" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -4393,6 +4646,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="O1" workbookViewId="0" zoomScale="100">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="B4" xSplit="1" ySplit="3"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4427,67 +4681,67 @@
         <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
@@ -4507,239 +4761,239 @@
       <c r="AM1" s="5"/>
     </row>
     <row r="2" s="9" customFormat="1" ht="23.600000000000001" customHeight="1">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="E2" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="79"/>
-      <c r="G2" s="80" t="s">
-        <v>145</v>
-      </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="83" t="s">
-        <v>146</v>
-      </c>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="84" t="s">
-        <v>147</v>
-      </c>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="87" t="s">
-        <v>148</v>
-      </c>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="E2" s="83" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="83"/>
+      <c r="G2" s="84" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="88" t="s">
+        <v>163</v>
+      </c>
+      <c r="R2" s="89"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="91" t="s">
+        <v>164</v>
+      </c>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
     </row>
     <row r="3" ht="34.100000000000001" customHeight="1">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="90" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="91" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="92" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="93" t="s">
-        <v>151</v>
-      </c>
-      <c r="G3" s="94" t="s">
-        <v>152</v>
-      </c>
-      <c r="H3" s="95" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="96" t="s">
-        <v>154</v>
-      </c>
-      <c r="J3" s="96" t="s">
-        <v>155</v>
-      </c>
-      <c r="K3" s="96" t="s">
-        <v>156</v>
-      </c>
-      <c r="L3" s="96" t="s">
-        <v>157</v>
-      </c>
-      <c r="M3" s="96" t="s">
-        <v>158</v>
-      </c>
-      <c r="N3" s="97" t="s">
-        <v>159</v>
-      </c>
-      <c r="O3" s="98" t="s">
-        <v>157</v>
-      </c>
-      <c r="P3" s="99" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q3" s="100" t="s">
-        <v>160</v>
-      </c>
-      <c r="R3" s="101" t="s">
-        <v>161</v>
-      </c>
-      <c r="S3" s="101" t="s">
-        <v>157</v>
-      </c>
-      <c r="T3" s="101" t="s">
-        <v>158</v>
-      </c>
-      <c r="U3" s="102" t="s">
-        <v>157</v>
-      </c>
-      <c r="V3" s="103" t="s">
-        <v>162</v>
-      </c>
-      <c r="W3" s="104" t="s">
-        <v>163</v>
+      <c r="C3" s="94" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="98" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="99" t="s">
+        <v>169</v>
+      </c>
+      <c r="I3" s="100" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="100" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" s="100" t="s">
+        <v>172</v>
+      </c>
+      <c r="L3" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="M3" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="O3" s="102" t="s">
+        <v>173</v>
+      </c>
+      <c r="P3" s="103" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q3" s="104" t="s">
+        <v>176</v>
+      </c>
+      <c r="R3" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="S3" s="105" t="s">
+        <v>173</v>
+      </c>
+      <c r="T3" s="105" t="s">
+        <v>174</v>
+      </c>
+      <c r="U3" s="106" t="s">
+        <v>173</v>
+      </c>
+      <c r="V3" s="107" t="s">
+        <v>178</v>
+      </c>
+      <c r="W3" s="108" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="D4" s="74" t="str">
+        <v>182</v>
+      </c>
+      <c r="D4" s="78" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="62">
         <v>0</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="62">
         <v>5</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="61" t="s">
+      <c r="H4" s="62"/>
+      <c r="I4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="105"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61" t="s">
+      <c r="J4" s="109"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="61" t="s">
+      <c r="O4" s="62"/>
+      <c r="P4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="61" t="s">
+      <c r="Q4" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="58" t="s">
+      <c r="R4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="58">
+      <c r="S4" s="62">
         <v>3</v>
       </c>
-      <c r="T4" s="58" t="s">
+      <c r="T4" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="58">
+      <c r="U4" s="62">
         <v>3</v>
       </c>
-      <c r="V4" s="58" t="s">
+      <c r="V4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="58" t="s">
+      <c r="W4" s="62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="28.5">
       <c r="A5" s="10" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" s="74" t="str">
+        <v>185</v>
+      </c>
+      <c r="D5" s="78" t="str">
         <f>centers!$A$4</f>
         <v>centerB</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="62">
         <v>240</v>
       </c>
-      <c r="G5" s="58">
+      <c r="G5" s="62">
         <v>4</v>
       </c>
-      <c r="H5" s="58">
+      <c r="H5" s="62">
         <v>60</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="105" t="s">
-        <v>170</v>
-      </c>
-      <c r="K5" s="58" t="s">
+      <c r="J5" s="109" t="s">
+        <v>186</v>
+      </c>
+      <c r="K5" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="58">
+      <c r="L5" s="62">
         <v>4</v>
       </c>
-      <c r="M5" s="61" t="s">
+      <c r="M5" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="61" t="s">
+      <c r="N5" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="58">
+      <c r="O5" s="62">
         <v>4</v>
       </c>
-      <c r="P5" s="61" t="s">
+      <c r="P5" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="61" t="s">
+      <c r="Q5" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="61" t="s">
+      <c r="R5" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="58">
+      <c r="S5" s="62">
         <v>3</v>
       </c>
-      <c r="T5" s="58" t="s">
+      <c r="T5" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="58">
+      <c r="U5" s="62">
         <v>3</v>
       </c>
-      <c r="V5" s="58" t="s">
+      <c r="V5" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="W5" s="58" t="s">
+      <c r="W5" s="62" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4758,79 +5012,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00C20012-0087-4370-A086-00AF00320063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0004009D-0093-4F2B-BDF5-00C400E60061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00900010-0065-4553-ABE7-00C5008700D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B60057-00F7-402E-8925-008800F400E1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B80059-0069-4640-9FFB-007D00C800EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CE004C-00FB-4B9C-ABBE-004B00C40032}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CD0065-0061-4059-A05F-008700490055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A20025-0099-45AE-B651-004F00C2007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00750008-00EA-4FA0-8869-005E00520075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005D0058-00F6-4C45-BCBD-00C6009F0045}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00800098-0094-40AC-AB32-003D00040072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007F00D1-0090-4CDF-887D-00CC002100EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F3006A-00AD-4F2C-993A-00B500FC0009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F900F3-002D-4225-9AF7-00F9006100CC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>R4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00350060-001F-4262-A2FB-00CA005F0067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007300B6-0001-4D4A-9CFB-0023000B0061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00280060-006F-4D11-A880-00FA003D0046}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007300E0-0087-4E68-A7D2-00E600030071}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000D0037-0028-4FED-BF71-00D400710068}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00660019-002D-4F6C-912F-0077008900A3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003A00BB-0004-490E-B403-009700BE008F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000F003E-00A7-4F7C-A198-006C006C0042}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B00026-00C5-4B2E-A29D-005100EB0096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00360064-0097-4245-BEBF-002400DB005E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EB00D7-00D5-4E2C-87E7-0062006300C9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DF00F3-0082-4759-AE3C-006C00E40081}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -4869,83 +5123,83 @@
         <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="91" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="106" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="106" t="s">
-        <v>175</v>
+      <c r="C2" s="95" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="110" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="110" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="64" t="s">
-        <v>176</v>
+      <c r="A3" s="68" t="s">
+        <v>192</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="75" t="str">
+        <v>193</v>
+      </c>
+      <c r="C3" s="79" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D3" s="58">
+      <c r="D3" s="62">
         <v>0</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="64" t="s">
-        <v>178</v>
+      <c r="A4" s="68" t="s">
+        <v>194</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" s="75" t="str">
+        <v>193</v>
+      </c>
+      <c r="C4" s="79" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="62">
         <v>0</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="64" t="s">
-        <v>179</v>
+      <c r="A5" s="68" t="s">
+        <v>195</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="75" t="str">
+        <v>196</v>
+      </c>
+      <c r="C5" s="79" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="62">
         <v>0</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="62" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4957,19 +5211,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0046008B-0027-4D50-B669-00BD0023004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DD0041-0095-4F26-8E06-008C00D70099}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D10051-0023-454F-B6CA-00E2008600EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003F001F-0041-472C-B338-00DB008E004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A800BD-004C-404B-9ABE-001B00E700FC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009900F6-00C7-4413-8066-00EB00860002}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
MOVED: Tags logic to Leemons common.
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -343,6 +343,9 @@
     <t>genre</t>
   </si>
   <si>
+    <t>birthdate</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -355,6 +358,9 @@
     <t>Genre</t>
   </si>
   <si>
+    <t>Birthdate</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -400,31 +406,31 @@
     <t>student@leemons.io</t>
   </si>
   <si>
+    <t>student@centerB</t>
+  </si>
+  <si>
+    <t>studentA02</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>student+emma@leemons.io</t>
+  </si>
+  <si>
+    <t>studentB01</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>student+lisa@leemons.io</t>
+  </si>
+  <si>
     <t>student@centerA</t>
-  </si>
-  <si>
-    <t>studentA02</t>
-  </si>
-  <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>School</t>
-  </si>
-  <si>
-    <t>student+emma@leemons.io</t>
-  </si>
-  <si>
-    <t>studentB01</t>
-  </si>
-  <si>
-    <t>Lisa</t>
-  </si>
-  <si>
-    <t>student+lisa@leemons.io</t>
-  </si>
-  <si>
-    <t>student@centerB</t>
   </si>
   <si>
     <t>studentB02</t>
@@ -830,6 +836,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="15">
     <font>
       <name val="Calibri"/>
@@ -1319,7 +1328,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="122">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1332,9 +1341,6 @@
     </xf>
     <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1508,16 +1514,13 @@
     <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="160" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1536,6 +1539,10 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -2266,12 +2273,12 @@
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2304,96 +2311,96 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>194</v>
+      <c r="C1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="109" t="s">
-        <v>171</v>
-      </c>
-      <c r="D2" s="109" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="109" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" s="110" t="s">
-        <v>196</v>
-      </c>
-      <c r="G2" s="111" t="s">
+      <c r="C2" s="108" t="s">
         <v>173</v>
       </c>
+      <c r="D2" s="108" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="108" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="G2" s="110" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="E3" s="112" t="s">
+      <c r="C3" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="F3" s="77" t="str">
+      <c r="D3" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="111" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="76" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G3" s="64">
+      <c r="G3" s="63">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="C4" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="F4" s="77" t="str">
+      <c r="D4" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>218</v>
+      </c>
+      <c r="F4" s="76" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="63">
         <v>0</v>
       </c>
     </row>
@@ -2437,920 +2444,920 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="K1" s="113" t="s">
+      <c r="H1" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="L1" s="75"/>
+      <c r="J1" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K1" s="112" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" s="74"/>
     </row>
     <row r="2" ht="28.850000000000001" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="75"/>
+      <c r="L2" s="74"/>
     </row>
     <row r="3" ht="31.850000000000001" customHeight="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="92" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="91" t="s">
-        <v>224</v>
-      </c>
-      <c r="E3" s="91" t="s">
-        <v>225</v>
-      </c>
-      <c r="F3" s="91" t="s">
+      <c r="C3" s="91" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="G3" s="114" t="s">
+      <c r="E3" s="90" t="s">
         <v>227</v>
       </c>
-      <c r="H3" s="115" t="s">
-        <v>205</v>
-      </c>
-      <c r="I3" s="115" t="s">
+      <c r="F3" s="90" t="s">
         <v>228</v>
       </c>
-      <c r="J3" s="116" t="s">
+      <c r="G3" s="113" t="s">
         <v>229</v>
       </c>
-      <c r="K3" s="110" t="s">
+      <c r="H3" s="114" t="s">
+        <v>207</v>
+      </c>
+      <c r="I3" s="114" t="s">
         <v>230</v>
       </c>
-      <c r="L3" s="117"/>
-    </row>
-    <row r="4" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="11" t="str">
+      <c r="J3" s="115" t="s">
+        <v>231</v>
+      </c>
+      <c r="K3" s="109" t="s">
+        <v>232</v>
+      </c>
+      <c r="L3" s="116"/>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="10" t="str">
         <f t="shared" ref="A4:A9" si="0">_xlfn.CONCAT("subject",IF(L4&lt;10,"0",""),L4)</f>
         <v>subject01</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="C4" s="77" t="str">
+      <c r="B4" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="76" t="str">
         <f>ap_programs!A4</f>
         <v>programA</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="63">
         <v>1</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64" t="str">
+      <c r="E4" s="63"/>
+      <c r="F4" s="63" t="str">
         <f t="shared" ref="F4:F9" si="1">_xlfn.CONCAT("0",IF(L4&lt;10,"0",""),L4)</f>
         <v>001</v>
       </c>
-      <c r="G4" s="118" t="s">
-        <v>232</v>
-      </c>
-      <c r="H4" s="119" t="s">
-        <v>233</v>
-      </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="120" t="str">
+      <c r="G4" s="117" t="s">
+        <v>234</v>
+      </c>
+      <c r="H4" s="118" t="s">
+        <v>235</v>
+      </c>
+      <c r="I4" s="63"/>
+      <c r="J4" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K4" s="121" t="s">
-        <v>234</v>
-      </c>
-      <c r="L4" s="122">
+      <c r="K4" s="120" t="s">
+        <v>236</v>
+      </c>
+      <c r="L4" s="121">
         <v>1</v>
       </c>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="11" t="str">
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="10" t="str">
         <f t="shared" si="0"/>
         <v>subject02</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="C5" s="77" t="str">
+      <c r="B5" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="76" t="str">
         <f t="shared" ref="C5:C10" si="2">C4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="63">
         <v>1</v>
       </c>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64" t="str">
+      <c r="E5" s="63"/>
+      <c r="F5" s="63" t="str">
         <f t="shared" si="1"/>
         <v>002</v>
       </c>
-      <c r="G5" s="118" t="str">
+      <c r="G5" s="117" t="str">
         <f t="shared" ref="G5:G10" si="3">G4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H5" s="119" t="str">
+      <c r="H5" s="118" t="str">
         <f t="shared" ref="H5:H10" si="4">H4</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I5" s="64"/>
-      <c r="J5" s="120" t="str">
+      <c r="I5" s="63"/>
+      <c r="J5" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K5" s="121" t="str">
+      <c r="K5" s="120" t="str">
         <f t="shared" ref="K5:K10" si="5">K4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L5" s="122">
+      <c r="L5" s="121">
         <f t="shared" ref="L5:L10" si="6">L4+1</f>
         <v>2</v>
       </c>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="11" t="str">
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="10" t="str">
         <f t="shared" si="0"/>
         <v>subject03</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="C6" s="77" t="str">
+      <c r="B6" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="76" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D6" s="64">
+      <c r="D6" s="63">
         <v>1</v>
       </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64" t="str">
+      <c r="E6" s="63"/>
+      <c r="F6" s="63" t="str">
         <f t="shared" si="1"/>
         <v>003</v>
       </c>
-      <c r="G6" s="118" t="str">
+      <c r="G6" s="117" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H6" s="119" t="str">
+      <c r="H6" s="118" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="120" t="str">
+      <c r="I6" s="63"/>
+      <c r="J6" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K6" s="121" t="str">
+      <c r="K6" s="120" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L6" s="122">
+      <c r="L6" s="121">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="11" t="str">
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" s="9" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="10" t="str">
         <f t="shared" si="0"/>
         <v>subject04</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="77" t="str">
+      <c r="B7" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="76" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="63">
         <v>1</v>
       </c>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64" t="str">
+      <c r="E7" s="63"/>
+      <c r="F7" s="63" t="str">
         <f t="shared" si="1"/>
         <v>004</v>
       </c>
-      <c r="G7" s="118" t="str">
+      <c r="G7" s="117" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H7" s="119" t="str">
+      <c r="H7" s="118" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="120" t="str">
+      <c r="I7" s="63"/>
+      <c r="J7" s="119" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K7" s="121" t="str">
+      <c r="K7" s="120" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L7" s="122">
+      <c r="L7" s="121">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="11" t="str">
+      <c r="A8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>subject05</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="77" t="str">
+      <c r="B8" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="76" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="63">
         <v>2</v>
       </c>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64" t="str">
+      <c r="E8" s="63"/>
+      <c r="F8" s="63" t="str">
         <f t="shared" si="1"/>
         <v>005</v>
       </c>
-      <c r="G8" s="118" t="s">
-        <v>239</v>
-      </c>
-      <c r="H8" s="119" t="str">
+      <c r="G8" s="117" t="s">
+        <v>241</v>
+      </c>
+      <c r="H8" s="118" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="120" t="str">
+      <c r="I8" s="63"/>
+      <c r="J8" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K8" s="121" t="s">
-        <v>240</v>
-      </c>
-      <c r="L8" s="122">
+      <c r="K8" s="120" t="s">
+        <v>242</v>
+      </c>
+      <c r="L8" s="121">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
-      <c r="A9" s="11" t="str">
+      <c r="A9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>subject06</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="C9" s="77" t="str">
+      <c r="B9" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" s="76" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="63">
         <v>2</v>
       </c>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64" t="str">
+      <c r="E9" s="63"/>
+      <c r="F9" s="63" t="str">
         <f t="shared" si="1"/>
         <v>006</v>
       </c>
-      <c r="G9" s="118" t="str">
+      <c r="G9" s="117" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H9" s="119" t="s">
-        <v>242</v>
-      </c>
-      <c r="I9" s="64"/>
-      <c r="J9" s="120" t="str">
+      <c r="H9" s="118" t="s">
+        <v>244</v>
+      </c>
+      <c r="I9" s="63"/>
+      <c r="J9" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K9" s="121" t="str">
+      <c r="K9" s="120" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L9" s="122">
+      <c r="L9" s="121">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
-      <c r="A10" s="11" t="str">
+      <c r="A10" s="10" t="str">
         <f t="shared" ref="A10:A23" si="7">_xlfn.CONCAT("subject",IF(L10&lt;10,"0",""),L10)</f>
         <v>subject07</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="C10" s="77" t="str">
+      <c r="B10" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="76" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="63">
         <v>2</v>
       </c>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64" t="str">
+      <c r="E10" s="63"/>
+      <c r="F10" s="63" t="str">
         <f t="shared" ref="F10:F23" si="8">_xlfn.CONCAT("0",IF(L10&lt;10,"0",""),L10)</f>
         <v>007</v>
       </c>
-      <c r="G10" s="118" t="str">
+      <c r="G10" s="117" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H10" s="119" t="str">
+      <c r="H10" s="118" t="str">
         <f t="shared" si="4"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="I10" s="64"/>
-      <c r="J10" s="120" t="str">
+      <c r="I10" s="63"/>
+      <c r="J10" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K10" s="121" t="str">
+      <c r="K10" s="120" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L10" s="122">
+      <c r="L10" s="121">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
-      <c r="A11" s="11" t="str">
+      <c r="A11" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject08</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="C11" s="77" t="str">
+      <c r="B11" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="76" t="str">
         <f t="shared" ref="C11:C23" si="9">C10</f>
         <v>programA</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="63">
         <v>2</v>
       </c>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64" t="str">
+      <c r="E11" s="63"/>
+      <c r="F11" s="63" t="str">
         <f t="shared" si="8"/>
         <v>008</v>
       </c>
-      <c r="G11" s="118" t="str">
+      <c r="G11" s="117" t="str">
         <f>G10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H11" s="119" t="str">
+      <c r="H11" s="118" t="str">
         <f t="shared" ref="H11:H18" si="10">H10</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I11" s="64"/>
-      <c r="J11" s="120" t="str">
+      <c r="I11" s="63"/>
+      <c r="J11" s="119" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K11" s="121" t="str">
+      <c r="K11" s="120" t="str">
         <f>K10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L11" s="122">
+      <c r="L11" s="121">
         <f t="shared" ref="L11:L23" si="11">L10+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
-      <c r="A12" s="11" t="str">
+      <c r="A12" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject09</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="C12" s="77" t="str">
+      <c r="B12" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="63">
         <v>3</v>
       </c>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64" t="str">
+      <c r="E12" s="63"/>
+      <c r="F12" s="63" t="str">
         <f t="shared" si="8"/>
         <v>009</v>
       </c>
-      <c r="G12" s="118" t="s">
-        <v>246</v>
-      </c>
-      <c r="H12" s="119" t="str">
+      <c r="G12" s="117" t="s">
+        <v>248</v>
+      </c>
+      <c r="H12" s="118" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="I12" s="64"/>
-      <c r="J12" s="120" t="str">
+      <c r="I12" s="63"/>
+      <c r="J12" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K12" s="121" t="s">
-        <v>247</v>
-      </c>
-      <c r="L12" s="122">
+      <c r="K12" s="120" t="s">
+        <v>249</v>
+      </c>
+      <c r="L12" s="121">
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
-      <c r="A13" s="11" t="str">
+      <c r="A13" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject10</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="C13" s="77" t="str">
+      <c r="B13" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="63">
         <v>3</v>
       </c>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64" t="str">
+      <c r="E13" s="63"/>
+      <c r="F13" s="63" t="str">
         <f t="shared" si="8"/>
         <v>010</v>
       </c>
-      <c r="G13" s="118" t="str">
+      <c r="G13" s="117" t="str">
         <f t="shared" ref="G13:G23" si="12">G12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H13" s="119" t="str">
+      <c r="H13" s="118" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="I13" s="64"/>
-      <c r="J13" s="120" t="str">
+      <c r="I13" s="63"/>
+      <c r="J13" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K13" s="121" t="str">
+      <c r="K13" s="120" t="str">
         <f t="shared" ref="K13:K23" si="13">K12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L13" s="122">
+      <c r="L13" s="121">
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1">
-      <c r="A14" s="11" t="str">
+      <c r="A14" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject11</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="C14" s="77" t="str">
+      <c r="B14" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C14" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="63">
         <v>3</v>
       </c>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64" t="str">
+      <c r="E14" s="63"/>
+      <c r="F14" s="63" t="str">
         <f t="shared" si="8"/>
         <v>011</v>
       </c>
-      <c r="G14" s="118" t="str">
+      <c r="G14" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H14" s="119" t="s">
-        <v>250</v>
-      </c>
-      <c r="I14" s="64"/>
-      <c r="J14" s="120" t="str">
+      <c r="H14" s="118" t="s">
+        <v>252</v>
+      </c>
+      <c r="I14" s="63"/>
+      <c r="J14" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K14" s="121" t="str">
+      <c r="K14" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L14" s="122">
+      <c r="L14" s="121">
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="11" t="str">
+      <c r="A15" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject12</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="C15" s="77" t="str">
+      <c r="B15" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="63">
         <v>3</v>
       </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64" t="str">
+      <c r="E15" s="63"/>
+      <c r="F15" s="63" t="str">
         <f t="shared" si="8"/>
         <v>012</v>
       </c>
-      <c r="G15" s="118" t="str">
+      <c r="G15" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H15" s="119" t="str">
+      <c r="H15" s="118" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I15" s="64"/>
-      <c r="J15" s="120" t="str">
+      <c r="I15" s="63"/>
+      <c r="J15" s="119" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K15" s="121" t="str">
+      <c r="K15" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L15" s="122">
+      <c r="L15" s="121">
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="11" t="str">
+      <c r="A16" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject13</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="C16" s="77" t="str">
+      <c r="B16" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="63">
         <v>4</v>
       </c>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64" t="str">
+      <c r="E16" s="63"/>
+      <c r="F16" s="63" t="str">
         <f t="shared" si="8"/>
         <v>013</v>
       </c>
-      <c r="G16" s="118" t="s">
-        <v>253</v>
-      </c>
-      <c r="H16" s="119" t="str">
+      <c r="G16" s="117" t="s">
+        <v>255</v>
+      </c>
+      <c r="H16" s="118" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I16" s="64"/>
-      <c r="J16" s="120" t="str">
+      <c r="I16" s="63"/>
+      <c r="J16" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K16" s="121" t="s">
-        <v>254</v>
-      </c>
-      <c r="L16" s="122">
+      <c r="K16" s="120" t="s">
+        <v>256</v>
+      </c>
+      <c r="L16" s="121">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
     <row r="17" ht="30" customHeight="1">
-      <c r="A17" s="11" t="str">
+      <c r="A17" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject14</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="C17" s="77" t="str">
+      <c r="B17" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C17" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D17" s="64">
+      <c r="D17" s="63">
         <v>4</v>
       </c>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64" t="str">
+      <c r="E17" s="63"/>
+      <c r="F17" s="63" t="str">
         <f t="shared" si="8"/>
         <v>014</v>
       </c>
-      <c r="G17" s="118" t="str">
+      <c r="G17" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H17" s="119" t="str">
+      <c r="H17" s="118" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I17" s="64"/>
-      <c r="J17" s="120" t="str">
+      <c r="I17" s="63"/>
+      <c r="J17" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K17" s="121" t="str">
+      <c r="K17" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L17" s="122">
+      <c r="L17" s="121">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
-      <c r="A18" s="11" t="str">
+      <c r="A18" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject15</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C18" s="77" t="str">
+      <c r="B18" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="63">
         <v>4</v>
       </c>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64" t="str">
+      <c r="E18" s="63"/>
+      <c r="F18" s="63" t="str">
         <f t="shared" si="8"/>
         <v>015</v>
       </c>
-      <c r="G18" s="118" t="str">
+      <c r="G18" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H18" s="119" t="str">
+      <c r="H18" s="118" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I18" s="64"/>
-      <c r="J18" s="120" t="str">
+      <c r="I18" s="63"/>
+      <c r="J18" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K18" s="121" t="str">
+      <c r="K18" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L18" s="122">
+      <c r="L18" s="121">
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1">
-      <c r="A19" s="11" t="str">
+      <c r="A19" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject16</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="C19" s="77" t="str">
+      <c r="B19" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C19" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D19" s="64">
+      <c r="D19" s="63">
         <v>4</v>
       </c>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64" t="str">
+      <c r="E19" s="63"/>
+      <c r="F19" s="63" t="str">
         <f t="shared" si="8"/>
         <v>016</v>
       </c>
-      <c r="G19" s="118" t="str">
+      <c r="G19" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H19" s="119" t="s">
-        <v>258</v>
-      </c>
-      <c r="I19" s="64"/>
-      <c r="J19" s="120" t="str">
+      <c r="H19" s="118" t="s">
+        <v>260</v>
+      </c>
+      <c r="I19" s="63"/>
+      <c r="J19" s="119" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K19" s="121" t="str">
+      <c r="K19" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L19" s="122">
+      <c r="L19" s="121">
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="1">
-      <c r="A20" s="11" t="str">
+      <c r="A20" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject17</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="C20" s="77" t="str">
+      <c r="B20" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="C20" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="63">
         <v>5</v>
       </c>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64" t="str">
+      <c r="E20" s="63"/>
+      <c r="F20" s="63" t="str">
         <f t="shared" si="8"/>
         <v>017</v>
       </c>
-      <c r="G20" s="118" t="s">
+      <c r="G20" s="117" t="s">
+        <v>262</v>
+      </c>
+      <c r="H20" s="118" t="s">
         <v>260</v>
       </c>
-      <c r="H20" s="119" t="s">
-        <v>258</v>
-      </c>
-      <c r="I20" s="64"/>
-      <c r="J20" s="120" t="str">
+      <c r="I20" s="63"/>
+      <c r="J20" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K20" s="121" t="s">
-        <v>261</v>
-      </c>
-      <c r="L20" s="122">
+      <c r="K20" s="120" t="s">
+        <v>263</v>
+      </c>
+      <c r="L20" s="121">
         <f t="shared" si="11"/>
         <v>17</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
-      <c r="A21" s="11" t="str">
+      <c r="A21" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject18</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="C21" s="77" t="str">
+      <c r="B21" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="C21" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D21" s="64">
+      <c r="D21" s="63">
         <v>5</v>
       </c>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64" t="str">
+      <c r="E21" s="63"/>
+      <c r="F21" s="63" t="str">
         <f t="shared" si="8"/>
         <v>018</v>
       </c>
-      <c r="G21" s="118" t="str">
+      <c r="G21" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H21" s="119" t="s">
-        <v>258</v>
-      </c>
-      <c r="I21" s="64"/>
-      <c r="J21" s="120" t="str">
+      <c r="H21" s="118" t="s">
+        <v>260</v>
+      </c>
+      <c r="I21" s="63"/>
+      <c r="J21" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K21" s="121" t="str">
+      <c r="K21" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L21" s="122">
+      <c r="L21" s="121">
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="30" customHeight="1">
-      <c r="A22" s="11" t="str">
+      <c r="A22" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject19</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="C22" s="77" t="str">
+      <c r="B22" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C22" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D22" s="63">
         <v>5</v>
       </c>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64" t="str">
+      <c r="E22" s="63"/>
+      <c r="F22" s="63" t="str">
         <f t="shared" si="8"/>
         <v>019</v>
       </c>
-      <c r="G22" s="118" t="str">
+      <c r="G22" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H22" s="119" t="s">
-        <v>258</v>
-      </c>
-      <c r="I22" s="64"/>
-      <c r="J22" s="120" t="str">
+      <c r="H22" s="118" t="s">
+        <v>260</v>
+      </c>
+      <c r="I22" s="63"/>
+      <c r="J22" s="119" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K22" s="121" t="str">
+      <c r="K22" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L22" s="122">
+      <c r="L22" s="121">
         <f t="shared" si="11"/>
         <v>19</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
-      <c r="A23" s="11" t="str">
+      <c r="A23" s="10" t="str">
         <f t="shared" si="7"/>
         <v>subject20</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="C23" s="77" t="str">
+      <c r="B23" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C23" s="76" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="63">
         <v>5</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64" t="str">
+      <c r="E23" s="63"/>
+      <c r="F23" s="63" t="str">
         <f t="shared" si="8"/>
         <v>020</v>
       </c>
-      <c r="G23" s="118" t="str">
+      <c r="G23" s="117" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H23" s="119" t="s">
-        <v>258</v>
-      </c>
-      <c r="I23" s="64"/>
-      <c r="J23" s="120" t="str">
+      <c r="H23" s="118" t="s">
+        <v>260</v>
+      </c>
+      <c r="I23" s="63"/>
+      <c r="J23" s="119" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K23" s="121" t="str">
+      <c r="K23" s="120" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L23" s="122">
+      <c r="L23" s="121">
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="L24" s="75"/>
+      <c r="L24" s="74"/>
     </row>
     <row r="25" ht="14.25"/>
   </sheetData>
@@ -3399,58 +3406,58 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="11" t="s">
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="11" t="s">
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3492,726 +3499,726 @@
     <col customWidth="1" min="29" max="29" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="1" ht="14.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" s="12" customFormat="1" ht="14.25">
+      <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="13" t="str">
+      <c r="E1" s="12" t="str">
         <f>_xlfn.CONCAT($E$3,".",E5)</f>
         <v>plugins.users.users</v>
       </c>
-      <c r="F1" s="13" t="str">
+      <c r="F1" s="12" t="str">
         <f>_xlfn.CONCAT($E$3,".",F5)</f>
         <v>plugins.users.user-data</v>
       </c>
-      <c r="G1" s="13" t="str">
+      <c r="G1" s="12" t="str">
         <f>_xlfn.CONCAT($E$3,".",G5)</f>
         <v>plugins.users.centers</v>
       </c>
-      <c r="H1" s="13" t="str">
+      <c r="H1" s="12" t="str">
         <f>_xlfn.CONCAT($E$3,".",H5)</f>
         <v>plugins.users.profiles</v>
       </c>
-      <c r="I1" s="13" t="str">
+      <c r="I1" s="12" t="str">
         <f>_xlfn.CONCAT($I$3,".",I5)</f>
         <v>plugins.dataset.dataset</v>
       </c>
-      <c r="J1" s="13" t="str">
+      <c r="J1" s="12" t="str">
         <f>_xlfn.CONCAT($J$3,".",J5)</f>
         <v>plugins.calendar.calendar</v>
       </c>
-      <c r="K1" s="13" t="str">
+      <c r="K1" s="12" t="str">
         <f>_xlfn.CONCAT($K$3,".",K5)</f>
         <v>plugins.academic-portfolio.portfolio</v>
       </c>
-      <c r="L1" s="13" t="str">
+      <c r="L1" s="12" t="str">
         <f>_xlfn.CONCAT($K$3,".",L5)</f>
         <v>plugins.academic-portfolio.programs</v>
       </c>
-      <c r="M1" s="13" t="str">
+      <c r="M1" s="12" t="str">
         <f>_xlfn.CONCAT($K$3,".",M5)</f>
         <v>plugins.academic-portfolio.profiles</v>
       </c>
-      <c r="N1" s="13" t="str">
+      <c r="N1" s="12" t="str">
         <f>_xlfn.CONCAT($K$3,".",N5)</f>
         <v>plugins.academic-portfolio.subjects</v>
       </c>
-      <c r="O1" s="13" t="str">
+      <c r="O1" s="12" t="str">
         <f>_xlfn.CONCAT($K$3,".",O5)</f>
         <v>plugins.academic-portfolio.tree</v>
       </c>
-      <c r="P1" s="13" t="str">
+      <c r="P1" s="12" t="str">
         <f>_xlfn.CONCAT($P$3,".",P5)</f>
         <v>plugins.families.families</v>
       </c>
-      <c r="Q1" s="13" t="str">
+      <c r="Q1" s="12" t="str">
         <f>_xlfn.CONCAT($P$3,".",Q5)</f>
         <v>plugins.families.config</v>
       </c>
-      <c r="R1" s="13" t="str">
+      <c r="R1" s="12" t="str">
         <f>_xlfn.CONCAT($P$3,".",R5)</f>
         <v>plugins.families.families-basic-info</v>
       </c>
-      <c r="S1" s="13" t="str">
+      <c r="S1" s="12" t="str">
         <f>_xlfn.CONCAT($P$3,".",S5)</f>
         <v>plugins.families.families-custom-info</v>
       </c>
-      <c r="T1" s="13" t="str">
+      <c r="T1" s="12" t="str">
         <f>_xlfn.CONCAT($P$3,".",T5)</f>
         <v>plugins.families.families-guardians-info</v>
       </c>
-      <c r="U1" s="13" t="str">
+      <c r="U1" s="12" t="str">
         <f>_xlfn.CONCAT($P$3,".",U5)</f>
         <v>plugins.families.families-students-info</v>
       </c>
-      <c r="V1" s="13" t="str">
+      <c r="V1" s="12" t="str">
         <f>_xlfn.CONCAT($V$3,".",V5)</f>
         <v>plugins.timetable.config</v>
       </c>
-      <c r="W1" s="13" t="str">
+      <c r="W1" s="12" t="str">
         <f>_xlfn.CONCAT($V$3,".",W5)</f>
         <v>plugins.timetable.timetable</v>
       </c>
-      <c r="X1" s="13" t="str">
+      <c r="X1" s="12" t="str">
         <f>_xlfn.CONCAT($X$3,".",X5)</f>
         <v>plugins.tasks.tasks</v>
       </c>
-      <c r="Y1" s="13" t="str">
+      <c r="Y1" s="12" t="str">
         <f>_xlfn.CONCAT($X$3,".",Y5)</f>
         <v>plugins.tasks.library</v>
       </c>
-      <c r="Z1" s="13" t="str">
+      <c r="Z1" s="12" t="str">
         <f>_xlfn.CONCAT($X$3,".",Z5)</f>
         <v>plugins.tasks.ongoing</v>
       </c>
-      <c r="AA1" s="13" t="str">
+      <c r="AA1" s="12" t="str">
         <f>_xlfn.CONCAT($X$3,".",AA5)</f>
         <v>plugins.tasks.history</v>
       </c>
-      <c r="AB1" s="13" t="str">
+      <c r="AB1" s="12" t="str">
         <f>_xlfn.CONCAT($AB$3,".",AB5)</f>
         <v>plugins.curriculum.curriculum</v>
       </c>
-      <c r="AC1" s="13" t="str">
+      <c r="AC1" s="12" t="str">
         <f>_xlfn.CONCAT($AC$3,".",AC5)</f>
         <v>plugins.leebrary.library</v>
       </c>
     </row>
-    <row r="2" s="10" customFormat="1" ht="21.350000000000001" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="14" t="s">
+    <row r="2" s="9" customFormat="1" ht="21.350000000000001" customHeight="1">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22" t="s">
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="16" t="s">
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="17"/>
-      <c r="X3" s="25" t="s">
+      <c r="W3" s="16"/>
+      <c r="X3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="27" t="s">
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AC3" s="20" t="s">
+      <c r="AC3" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" s="28" customFormat="1" ht="19.850000000000001" customHeight="1">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29" t="s">
+    <row r="4" s="27" customFormat="1" ht="19.850000000000001" customHeight="1">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35" t="s">
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="29" t="s">
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="31" t="s">
+      <c r="W4" s="29"/>
+      <c r="X4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="32" t="s">
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="AC4" s="33" t="s">
+      <c r="AC4" s="32" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="39" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="K5" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L5" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="45" t="s">
+      <c r="O5" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="46" t="s">
+      <c r="P5" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="Q5" s="47" t="s">
+      <c r="Q5" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="R5" s="47" t="s">
+      <c r="R5" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="S5" s="47" t="s">
+      <c r="S5" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="T5" s="47" t="s">
+      <c r="T5" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="U5" s="48" t="s">
+      <c r="U5" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="V5" s="39" t="s">
+      <c r="V5" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="W5" s="40" t="s">
+      <c r="W5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="X5" s="42" t="s">
+      <c r="X5" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="Y5" s="42" t="s">
+      <c r="Y5" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="Z5" s="42" t="s">
+      <c r="Z5" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="AA5" s="42" t="s">
+      <c r="AA5" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="AC5" s="49" t="s">
+      <c r="AC5" s="48" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" s="50" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="7" t="s">
+    <row r="6" s="49" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="55" t="s">
+      <c r="J6" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="56" t="s">
+      <c r="K6" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="57" t="s">
+      <c r="L6" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="M6" s="57" t="s">
+      <c r="M6" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="57" t="s">
+      <c r="N6" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="57" t="s">
+      <c r="O6" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="P6" s="58" t="s">
+      <c r="P6" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="59" t="s">
+      <c r="Q6" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="R6" s="59" t="s">
+      <c r="R6" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="S6" s="59" t="s">
+      <c r="S6" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="T6" s="59" t="s">
+      <c r="T6" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="U6" s="60" t="s">
+      <c r="U6" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="V6" s="52" t="s">
+      <c r="V6" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="W6" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="X6" s="54" t="s">
+      <c r="X6" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="Y6" s="54" t="s">
+      <c r="Y6" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="Z6" s="54" t="s">
+      <c r="Z6" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="AA6" s="54" t="s">
+      <c r="AA6" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="AB6" s="61" t="s">
+      <c r="AB6" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="AC6" s="62" t="s">
+      <c r="AC6" s="61" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="11" t="s">
+    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64" t="s">
+      <c r="D7" s="62"/>
+      <c r="E7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="64" t="s">
+      <c r="I7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="64" t="s">
+      <c r="J7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="K7" s="64" t="s">
+      <c r="K7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="64" t="s">
+      <c r="L7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="N7" s="64" t="s">
+      <c r="N7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="O7" s="64" t="s">
+      <c r="O7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="P7" s="65" t="s">
+      <c r="P7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="Q7" s="65" t="s">
+      <c r="Q7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="R7" s="65"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="65"/>
-      <c r="V7" s="65" t="s">
+      <c r="R7" s="64"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="W7" s="65" t="s">
+      <c r="W7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="X7" s="65" t="s">
+      <c r="X7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="Y7" s="65" t="s">
+      <c r="Y7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="Z7" s="65" t="s">
+      <c r="Z7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="65" t="s">
+      <c r="AA7" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="AB7" s="64" t="s">
+      <c r="AB7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="AC7" s="64" t="s">
+      <c r="AC7" s="63" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="11" t="s">
+    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64" t="s">
+      <c r="D8" s="62"/>
+      <c r="E8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="64" t="s">
+      <c r="G8" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="J8" s="64" t="s">
+      <c r="J8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="K8" s="64" t="s">
+      <c r="K8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="L8" s="64" t="s">
+      <c r="L8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64" t="s">
+      <c r="M8" s="63"/>
+      <c r="N8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="O8" s="64" t="s">
+      <c r="O8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="P8" s="64" t="s">
+      <c r="P8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="Q8" s="64" t="s">
+      <c r="Q8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="R8" s="65"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64" t="s">
+      <c r="R8" s="64"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="W8" s="64" t="s">
+      <c r="W8" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="X8" s="64" t="s">
+      <c r="X8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" s="64" t="s">
+      <c r="Y8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="Z8" s="64" t="s">
+      <c r="Z8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="AA8" s="64" t="s">
+      <c r="AA8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="AB8" s="64" t="s">
+      <c r="AB8" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="AC8" s="66" t="s">
+      <c r="AC8" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="11" t="s">
+    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64" t="s">
+      <c r="D9" s="62"/>
+      <c r="E9" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="H9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="J9" s="64" t="s">
+      <c r="J9" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="64" t="s">
+      <c r="K9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="L9" s="64" t="s">
+      <c r="L9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64" t="s">
+      <c r="M9" s="63"/>
+      <c r="N9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64" t="s">
+      <c r="O9" s="63"/>
+      <c r="P9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="Q9" s="64" t="s">
+      <c r="Q9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="R9" s="64" t="s">
+      <c r="R9" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="S9" s="64" t="s">
+      <c r="S9" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="T9" s="64" t="s">
+      <c r="T9" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="U9" s="64" t="s">
+      <c r="U9" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="V9" s="64" t="s">
+      <c r="V9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="W9" s="64" t="s">
+      <c r="W9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="X9" s="64" t="s">
+      <c r="X9" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="Y9" s="64" t="s">
+      <c r="Y9" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="Z9" s="64" t="s">
+      <c r="Z9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="AA9" s="64" t="s">
+      <c r="AA9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="AB9" s="64" t="s">
+      <c r="AB9" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="AC9" s="66" t="s">
+      <c r="AC9" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A10" s="11" t="s">
+    <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="63" t="str">
+      <c r="D10" s="62" t="str">
         <f>A9</f>
         <v>student</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="64" t="s">
+      <c r="G10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="64" t="s">
+      <c r="H10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="64" t="s">
+      <c r="I10" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="J10" s="64" t="s">
+      <c r="J10" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="K10" s="64" t="s">
+      <c r="K10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="L10" s="64" t="s">
+      <c r="L10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64" t="s">
+      <c r="M10" s="63"/>
+      <c r="N10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64" t="s">
+      <c r="O10" s="63"/>
+      <c r="P10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="Q10" s="64" t="s">
+      <c r="Q10" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="R10" s="64" t="s">
+      <c r="R10" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="S10" s="64" t="s">
+      <c r="S10" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="T10" s="64" t="s">
+      <c r="T10" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="U10" s="64" t="s">
+      <c r="U10" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-      <c r="X10" s="64"/>
-      <c r="Y10" s="64"/>
-      <c r="Z10" s="64"/>
-      <c r="AA10" s="64"/>
-      <c r="AB10" s="64"/>
-      <c r="AC10" s="66" t="s">
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="63"/>
+      <c r="Z10" s="63"/>
+      <c r="AA10" s="63"/>
+      <c r="AB10" s="63"/>
+      <c r="AC10" s="63" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4254,272 +4261,302 @@
     <col customWidth="1" min="2" max="2" width="13.140625"/>
     <col customWidth="1" min="3" max="3" width="19.8515625"/>
     <col customWidth="1" min="4" max="4" width="11.00390625"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" width="24.78125"/>
-    <col bestFit="1" min="6" max="6" width="9.140625"/>
-    <col customWidth="1" min="8" max="8" width="36.57421875"/>
+    <col customWidth="1" min="5" max="5" width="12.421875"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" width="24.78125"/>
+    <col bestFit="1" min="7" max="7" width="9.140625"/>
+    <col customWidth="1" min="9" max="9" width="36.57421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="F2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="I2" s="66" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="12" t="s">
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="B3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="70" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" s="64" t="s">
+      <c r="E3" s="67">
+        <v>36526</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="71" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="I3" s="69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="67">
+        <v>34781</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="H4" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A5" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="70" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G4" s="64" t="s">
+      <c r="E5" s="67">
+        <v>39205</v>
+      </c>
+      <c r="F5" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="71" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="72" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="73" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="73" t="s">
+      <c r="I5" s="73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A6" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="67">
+        <v>39156</v>
+      </c>
+      <c r="F6" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="67">
+        <v>42171</v>
+      </c>
+      <c r="F7" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="74" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" s="64" t="s">
+      <c r="E8" s="67">
+        <v>42237</v>
+      </c>
+      <c r="F8" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="71" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="I8" s="73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A9" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="64" t="s">
+      <c r="E9" s="67">
+        <v>27791</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="71" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="73" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="74" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="71" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="72" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="74" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="71" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="74" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="71" t="s">
-        <v>139</v>
+      <c r="I9" s="69" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E3"/>
-    <hyperlink r:id="rId2" ref="E4"/>
-    <hyperlink r:id="rId3" ref="E5"/>
-    <hyperlink r:id="rId4" ref="E7"/>
-    <hyperlink r:id="rId5" ref="E9"/>
+    <hyperlink r:id="rId1" ref="F3"/>
+    <hyperlink r:id="rId2" ref="F4"/>
+    <hyperlink r:id="rId3" ref="F5"/>
+    <hyperlink r:id="rId4" ref="F7"/>
+    <hyperlink r:id="rId5" ref="F9"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -4528,43 +4565,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00B600FA-0097-463C-B503-00FD00A500D7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000A00A4-00CB-473C-829E-002F007F00E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008C00E7-00C8-4EA1-9F02-00E600100080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004500ED-0079-498A-9BBF-009300EF001A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B800BD-00C5-48A6-9F45-000E001B00A0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E200D2-0071-401F-95C1-002C00A20077}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F60005-003F-443D-B0A7-00FB003F003E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006A0050-00C8-4384-8726-00DB00AF00FA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F40051-0044-4C7F-9722-00EE00A8009C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B700E2-0038-4CD3-968E-0024006B000A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A30045-005E-48EF-88BF-002900550009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0047006C-0004-44B1-A32B-005400980021}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003300DF-00CA-48EC-9435-00070079006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000D0037-0023-4F6A-86D0-00B8008E007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -4595,48 +4632,48 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>140</v>
+      <c r="B1" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="76" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="B2" s="75" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="77" t="str">
+      <c r="B3" s="76" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="77" t="str">
+      <c r="B4" s="76" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" ht="14.25"/>
     <row r="6" ht="14.25"/>
@@ -4669,29 +4706,29 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>142</v>
+      <c r="B1" s="5" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="2" ht="24.350000000000001" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="79" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="77" t="s">
+      <c r="B2" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="10"/>
+    </row>
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="9"/>
     </row>
     <row r="4"/>
   </sheetData>
@@ -4720,35 +4757,35 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>140</v>
+      <c r="B1" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="79" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="B2" s="78" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="77" t="str">
+      <c r="B3" s="76" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
     </row>
-    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="11" t="s">
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="77" t="str">
+      <c r="B4" s="76" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -4798,326 +4835,326 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-    </row>
-    <row r="2" s="10" customFormat="1" ht="23.600000000000001" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="E2" s="80" t="s">
+      <c r="V1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="81" t="s">
+      <c r="W1" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="84" t="s">
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+    </row>
+    <row r="2" s="9" customFormat="1" ht="23.600000000000001" customHeight="1">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="E2" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="85" t="s">
+      <c r="F2" s="79"/>
+      <c r="G2" s="80" t="s">
         <v>169</v>
       </c>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="88" t="s">
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="83" t="s">
         <v>170</v>
       </c>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="84" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
     </row>
     <row r="3" ht="34.100000000000001" customHeight="1">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="91" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="92" t="s">
+      <c r="C3" s="90" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="93" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" s="94" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="95" t="s">
+      <c r="E3" s="92" t="s">
         <v>174</v>
       </c>
-      <c r="H3" s="96" t="s">
+      <c r="F3" s="93" t="s">
         <v>175</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="G3" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="J3" s="97" t="s">
+      <c r="H3" s="95" t="s">
         <v>177</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="I3" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="L3" s="97" t="s">
+      <c r="J3" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="M3" s="97" t="s">
+      <c r="K3" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="N3" s="98" t="s">
+      <c r="L3" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="O3" s="99" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" s="100" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q3" s="101" t="s">
+      <c r="M3" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="R3" s="102" t="s">
+      <c r="N3" s="97" t="s">
         <v>183</v>
       </c>
-      <c r="S3" s="102" t="s">
-        <v>179</v>
-      </c>
-      <c r="T3" s="102" t="s">
-        <v>180</v>
-      </c>
-      <c r="U3" s="103" t="s">
-        <v>179</v>
-      </c>
-      <c r="V3" s="104" t="s">
+      <c r="O3" s="98" t="s">
+        <v>181</v>
+      </c>
+      <c r="P3" s="99" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q3" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="W3" s="105" t="s">
+      <c r="R3" s="101" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="S3" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="T3" s="101" t="s">
+        <v>182</v>
+      </c>
+      <c r="U3" s="102" t="s">
+        <v>181</v>
+      </c>
+      <c r="V3" s="103" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="W3" s="104" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="12" t="s">
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="77" t="str">
+      <c r="B4" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="76" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="64">
+      <c r="F4" s="63">
         <v>0</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="63">
         <v>5</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64" t="s">
+      <c r="H4" s="63"/>
+      <c r="I4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="106"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64" t="s">
+      <c r="J4" s="105"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64" t="s">
+      <c r="O4" s="63"/>
+      <c r="P4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="64" t="s">
+      <c r="Q4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="R4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="64">
+      <c r="S4" s="63">
         <v>3</v>
       </c>
-      <c r="T4" s="64" t="s">
+      <c r="T4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="64">
+      <c r="U4" s="63">
         <v>3</v>
       </c>
-      <c r="V4" s="64" t="s">
+      <c r="V4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="64" t="s">
+      <c r="W4" s="63" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" s="10" customFormat="1" ht="28.5">
-      <c r="A5" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" s="12" t="s">
+    <row r="5" s="9" customFormat="1" ht="28.5">
+      <c r="A5" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="77" t="str">
+      <c r="B5" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="76" t="str">
         <f>centers!$A$4</f>
         <v>centerB</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="63">
         <v>240</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="63">
         <v>4</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="63">
         <v>60</v>
       </c>
-      <c r="I5" s="64" t="s">
+      <c r="I5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="106" t="s">
-        <v>192</v>
-      </c>
-      <c r="K5" s="64" t="s">
+      <c r="J5" s="105" t="s">
+        <v>194</v>
+      </c>
+      <c r="K5" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="64">
+      <c r="L5" s="63">
         <v>4</v>
       </c>
-      <c r="M5" s="64" t="s">
+      <c r="M5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="64" t="s">
+      <c r="N5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="64">
+      <c r="O5" s="63">
         <v>4</v>
       </c>
-      <c r="P5" s="64" t="s">
+      <c r="P5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="64" t="s">
+      <c r="Q5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="64" t="s">
+      <c r="R5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="64">
+      <c r="S5" s="63">
         <v>3</v>
       </c>
-      <c r="T5" s="64" t="s">
+      <c r="T5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="64">
+      <c r="U5" s="63">
         <v>3</v>
       </c>
-      <c r="V5" s="64" t="s">
+      <c r="V5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="W5" s="64" t="s">
+      <c r="W5" s="63" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5136,79 +5173,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00FC001B-0057-48C2-9CA0-001800930069}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00760014-00A6-4807-BAFB-0000005C002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F40072-009F-43FB-8410-00F9002E00EA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E200E6-00BB-49AE-9602-00BA00B100FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E100F6-002D-4F26-8F4C-007A00A20057}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F800B7-0065-4C20-B7BB-008E0004000A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005E00A6-00D6-4B41-9999-007E002600F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00860067-00EC-4284-A1B5-00B40087001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00140079-00AF-40D2-8382-0025000C003F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F600B5-001C-4AFB-9763-00A7004700F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002900A0-006B-4BDD-A90C-00A5005F0018}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0075004C-0014-4C24-B6FC-009100350070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00170054-001E-4277-B077-00C600CF00F0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DC00CC-00A2-4E06-A24A-001B00570067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>R4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE003E-00BC-4D4D-BC29-007300D9009B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0094003A-0098-40CE-AE33-003A005700E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CA0098-00AE-429B-A513-00D100D90019}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003500F2-0057-457D-A210-00A600830088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008B0094-0077-43CD-B6D5-00C400A300C8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005B0057-0065-4E71-9906-003700A90047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AE0094-0000-4C4C-B5E5-003A00D60016}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00800010-0080-46BD-82EB-0075008900EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002100F0-00FD-4A2B-9136-00DE007700C7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009200A7-0072-49E8-840F-000B00A60056}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C20049-008A-48F3-96E0-004C003E0072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D30091-006B-4E77-B7E6-003100C100A2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5240,90 +5277,90 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>195</v>
       </c>
+      <c r="D1" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="92" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" s="107" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" s="107" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="C2" s="91" t="s">
         <v>198</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="D2" s="106" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="106" t="s">
         <v>199</v>
       </c>
-      <c r="C3" s="77" t="str">
+    </row>
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="76" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D3" s="64">
+      <c r="D3" s="63">
         <v>0</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="63" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="77" t="str">
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="76" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="63">
         <v>0</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="63" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" s="77" t="str">
+      <c r="A5" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="76" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="63">
         <v>0</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5335,19 +5372,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0055009D-00BD-4911-9A9F-00AA00DA00C6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006300CD-00AF-41EC-9872-00D2004B0006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B400BB-005E-4060-908F-006D00610045}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006800B1-00FB-4464-8CFB-0063006F0027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A40053-00D1-4348-87B0-006B007D002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006A009E-0059-4004-AC54-00D500320006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
ADDDED: Add Family on bulk from MVP
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <definedName name="SUBSTAGES_FRECUENCY" hidden="0">DB!$A$2:$A$8</definedName>
     <definedName name="BOOLEAN_ANSWER" hidden="0">DB!$A$11:$A$12</definedName>
     <definedName name="GENRE_ANSWER" hidden="0">DB!$A$15:$A$16</definedName>
+    <definedName name="GUARDIANS_RELATIONSHIPS" hidden="0">DB!$A$19:$A$23</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="279">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -73,6 +74,24 @@
     <t>Female</t>
   </si>
   <si>
+    <t xml:space="preserve">Marital Status</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Divorced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic partners</t>
+  </si>
+  <si>
+    <t>Cohabitants</t>
+  </si>
+  <si>
+    <t>Separated</t>
+  </si>
+  <si>
     <t>root</t>
   </si>
   <si>
@@ -466,13 +485,31 @@
     <t>relations</t>
   </si>
   <si>
+    <t>maritalStatus</t>
+  </si>
+  <si>
+    <t>emergencyPhoneNumbers</t>
+  </si>
+  <si>
     <t>Relations</t>
   </si>
   <si>
+    <t xml:space="preserve">Guardians relationship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emergency phone numbers</t>
+  </si>
+  <si>
     <t>family01</t>
   </si>
   <si>
+    <t xml:space="preserve">School's family</t>
+  </si>
+  <si>
     <t xml:space="preserve">guardian01|mother@studentA02, guardian01|mother@studentB02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111-222-333@Mom's phone|mother</t>
   </si>
   <si>
     <t>abbreviation</t>
@@ -940,7 +977,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1035,6 +1072,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -1328,7 +1371,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="127">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1341,6 +1384,9 @@
     </xf>
     <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1558,9 +1604,21 @@
     <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf fontId="4" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf fontId="4" fillId="16" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="17" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf fontId="1" fillId="7" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1576,13 +1634,13 @@
     <xf fontId="1" fillId="9" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="17" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="18" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="17" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="18" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="17" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="18" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="10" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1624,10 +1682,10 @@
     <xf fontId="12" fillId="13" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="12" fillId="18" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="19" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="12" fillId="18" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="19" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="14" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2202,7 +2260,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2282,6 +2340,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25"/>
+    <row r="25" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -2311,96 +2401,96 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>196</v>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="108" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="108" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="108" t="s">
-        <v>207</v>
-      </c>
-      <c r="E2" s="108" t="s">
-        <v>208</v>
-      </c>
-      <c r="F2" s="109" t="s">
-        <v>198</v>
-      </c>
-      <c r="G2" s="110" t="s">
-        <v>175</v>
+      <c r="A2" s="112" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="113" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="113" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="113" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="113" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="114" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="115" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E3" s="111" t="s">
-        <v>213</v>
-      </c>
-      <c r="F3" s="76" t="str">
+      <c r="A3" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="116" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="77" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="64">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>218</v>
-      </c>
-      <c r="F4" s="76" t="str">
+      <c r="A4" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="77" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="64">
         <v>0</v>
       </c>
     </row>
@@ -2444,920 +2534,920 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="K1" s="112" t="s">
-        <v>224</v>
-      </c>
-      <c r="L1" s="74"/>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="K1" s="117" t="s">
+        <v>236</v>
+      </c>
+      <c r="L1" s="75"/>
     </row>
     <row r="2" ht="28.850000000000001" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="1" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="74"/>
+      <c r="L2" s="75"/>
     </row>
     <row r="3" ht="31.850000000000001" customHeight="1">
-      <c r="A3" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="108" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="91" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="90" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" s="90" t="s">
-        <v>227</v>
-      </c>
-      <c r="F3" s="90" t="s">
-        <v>228</v>
-      </c>
-      <c r="G3" s="113" t="s">
-        <v>229</v>
-      </c>
-      <c r="H3" s="114" t="s">
-        <v>207</v>
-      </c>
-      <c r="I3" s="114" t="s">
-        <v>230</v>
-      </c>
-      <c r="J3" s="115" t="s">
-        <v>231</v>
-      </c>
-      <c r="K3" s="109" t="s">
-        <v>232</v>
-      </c>
-      <c r="L3" s="116"/>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="10" t="str">
+      <c r="A3" s="112" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="113" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="95" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="95" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" s="95" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="118" t="s">
+        <v>241</v>
+      </c>
+      <c r="H3" s="119" t="s">
+        <v>219</v>
+      </c>
+      <c r="I3" s="119" t="s">
+        <v>242</v>
+      </c>
+      <c r="J3" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="K3" s="114" t="s">
+        <v>244</v>
+      </c>
+      <c r="L3" s="121"/>
+    </row>
+    <row r="4" s="10" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="11" t="str">
         <f t="shared" ref="A4:A9" si="0">_xlfn.CONCAT("subject",IF(L4&lt;10,"0",""),L4)</f>
         <v>subject01</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="C4" s="76" t="str">
+      <c r="B4" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="77" t="str">
         <f>ap_programs!A4</f>
         <v>programA</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="64">
         <v>1</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63" t="str">
+      <c r="E4" s="64"/>
+      <c r="F4" s="64" t="str">
         <f t="shared" ref="F4:F9" si="1">_xlfn.CONCAT("0",IF(L4&lt;10,"0",""),L4)</f>
         <v>001</v>
       </c>
-      <c r="G4" s="117" t="s">
-        <v>234</v>
-      </c>
-      <c r="H4" s="118" t="s">
-        <v>235</v>
-      </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="119" t="str">
+      <c r="G4" s="122" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4" s="123" t="s">
+        <v>247</v>
+      </c>
+      <c r="I4" s="64"/>
+      <c r="J4" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K4" s="120" t="s">
-        <v>236</v>
-      </c>
-      <c r="L4" s="121">
+      <c r="K4" s="125" t="s">
+        <v>248</v>
+      </c>
+      <c r="L4" s="126">
         <v>1</v>
       </c>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="10" t="str">
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" s="10" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="11" t="str">
         <f t="shared" si="0"/>
         <v>subject02</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C5" s="76" t="str">
+      <c r="B5" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="77" t="str">
         <f t="shared" ref="C5:C10" si="2">C4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="64">
         <v>1</v>
       </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63" t="str">
+      <c r="E5" s="64"/>
+      <c r="F5" s="64" t="str">
         <f t="shared" si="1"/>
         <v>002</v>
       </c>
-      <c r="G5" s="117" t="str">
+      <c r="G5" s="122" t="str">
         <f t="shared" ref="G5:G10" si="3">G4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H5" s="118" t="str">
+      <c r="H5" s="123" t="str">
         <f t="shared" ref="H5:H10" si="4">H4</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="119" t="str">
+      <c r="I5" s="64"/>
+      <c r="J5" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K5" s="120" t="str">
+      <c r="K5" s="125" t="str">
         <f t="shared" ref="K5:K10" si="5">K4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L5" s="121">
+      <c r="L5" s="126">
         <f t="shared" ref="L5:L10" si="6">L4+1</f>
         <v>2</v>
       </c>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="10" t="str">
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" s="10" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="11" t="str">
         <f t="shared" si="0"/>
         <v>subject03</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="C6" s="76" t="str">
+      <c r="B6" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="64">
         <v>1</v>
       </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63" t="str">
+      <c r="E6" s="64"/>
+      <c r="F6" s="64" t="str">
         <f t="shared" si="1"/>
         <v>003</v>
       </c>
-      <c r="G6" s="117" t="str">
+      <c r="G6" s="122" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H6" s="118" t="str">
+      <c r="H6" s="123" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="I6" s="63"/>
-      <c r="J6" s="119" t="str">
+      <c r="I6" s="64"/>
+      <c r="J6" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K6" s="120" t="str">
+      <c r="K6" s="125" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L6" s="121">
+      <c r="L6" s="126">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="10" t="str">
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" s="10" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="11" t="str">
         <f t="shared" si="0"/>
         <v>subject04</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C7" s="76" t="str">
+      <c r="B7" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="64">
         <v>1</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63" t="str">
+      <c r="E7" s="64"/>
+      <c r="F7" s="64" t="str">
         <f t="shared" si="1"/>
         <v>004</v>
       </c>
-      <c r="G7" s="117" t="str">
+      <c r="G7" s="122" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H7" s="118" t="str">
+      <c r="H7" s="123" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="119" t="str">
+      <c r="I7" s="64"/>
+      <c r="J7" s="124" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K7" s="120" t="str">
+      <c r="K7" s="125" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L7" s="121">
+      <c r="L7" s="126">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="10" t="str">
+      <c r="A8" s="11" t="str">
         <f t="shared" si="0"/>
         <v>subject05</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C8" s="76" t="str">
+      <c r="B8" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C8" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="64">
         <v>2</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63" t="str">
+      <c r="E8" s="64"/>
+      <c r="F8" s="64" t="str">
         <f t="shared" si="1"/>
         <v>005</v>
       </c>
-      <c r="G8" s="117" t="s">
-        <v>241</v>
-      </c>
-      <c r="H8" s="118" t="str">
+      <c r="G8" s="122" t="s">
+        <v>253</v>
+      </c>
+      <c r="H8" s="123" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="I8" s="63"/>
-      <c r="J8" s="119" t="str">
+      <c r="I8" s="64"/>
+      <c r="J8" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K8" s="120" t="s">
-        <v>242</v>
-      </c>
-      <c r="L8" s="121">
+      <c r="K8" s="125" t="s">
+        <v>254</v>
+      </c>
+      <c r="L8" s="126">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
-      <c r="A9" s="10" t="str">
+      <c r="A9" s="11" t="str">
         <f t="shared" si="0"/>
         <v>subject06</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="C9" s="76" t="str">
+      <c r="B9" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="64">
         <v>2</v>
       </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63" t="str">
+      <c r="E9" s="64"/>
+      <c r="F9" s="64" t="str">
         <f t="shared" si="1"/>
         <v>006</v>
       </c>
-      <c r="G9" s="117" t="str">
+      <c r="G9" s="122" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H9" s="118" t="s">
-        <v>244</v>
-      </c>
-      <c r="I9" s="63"/>
-      <c r="J9" s="119" t="str">
+      <c r="H9" s="123" t="s">
+        <v>256</v>
+      </c>
+      <c r="I9" s="64"/>
+      <c r="J9" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K9" s="120" t="str">
+      <c r="K9" s="125" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L9" s="121">
+      <c r="L9" s="126">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
-      <c r="A10" s="10" t="str">
+      <c r="A10" s="11" t="str">
         <f t="shared" ref="A10:A23" si="7">_xlfn.CONCAT("subject",IF(L10&lt;10,"0",""),L10)</f>
         <v>subject07</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="C10" s="76" t="str">
+      <c r="B10" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="64">
         <v>2</v>
       </c>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63" t="str">
+      <c r="E10" s="64"/>
+      <c r="F10" s="64" t="str">
         <f t="shared" ref="F10:F23" si="8">_xlfn.CONCAT("0",IF(L10&lt;10,"0",""),L10)</f>
         <v>007</v>
       </c>
-      <c r="G10" s="117" t="str">
+      <c r="G10" s="122" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H10" s="118" t="str">
+      <c r="H10" s="123" t="str">
         <f t="shared" si="4"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="I10" s="63"/>
-      <c r="J10" s="119" t="str">
+      <c r="I10" s="64"/>
+      <c r="J10" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K10" s="120" t="str">
+      <c r="K10" s="125" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L10" s="121">
+      <c r="L10" s="126">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
-      <c r="A11" s="10" t="str">
+      <c r="A11" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject08</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C11" s="76" t="str">
+      <c r="B11" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="77" t="str">
         <f t="shared" ref="C11:C23" si="9">C10</f>
         <v>programA</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="64">
         <v>2</v>
       </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63" t="str">
+      <c r="E11" s="64"/>
+      <c r="F11" s="64" t="str">
         <f t="shared" si="8"/>
         <v>008</v>
       </c>
-      <c r="G11" s="117" t="str">
+      <c r="G11" s="122" t="str">
         <f>G10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H11" s="118" t="str">
+      <c r="H11" s="123" t="str">
         <f t="shared" ref="H11:H18" si="10">H10</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I11" s="63"/>
-      <c r="J11" s="119" t="str">
+      <c r="I11" s="64"/>
+      <c r="J11" s="124" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K11" s="120" t="str">
+      <c r="K11" s="125" t="str">
         <f>K10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L11" s="121">
+      <c r="L11" s="126">
         <f t="shared" ref="L11:L23" si="11">L10+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
-      <c r="A12" s="10" t="str">
+      <c r="A12" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject09</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="C12" s="76" t="str">
+      <c r="B12" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="64">
         <v>3</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63" t="str">
+      <c r="E12" s="64"/>
+      <c r="F12" s="64" t="str">
         <f t="shared" si="8"/>
         <v>009</v>
       </c>
-      <c r="G12" s="117" t="s">
-        <v>248</v>
-      </c>
-      <c r="H12" s="118" t="str">
+      <c r="G12" s="122" t="s">
+        <v>260</v>
+      </c>
+      <c r="H12" s="123" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="119" t="str">
+      <c r="I12" s="64"/>
+      <c r="J12" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K12" s="120" t="s">
-        <v>249</v>
-      </c>
-      <c r="L12" s="121">
+      <c r="K12" s="125" t="s">
+        <v>261</v>
+      </c>
+      <c r="L12" s="126">
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
-      <c r="A13" s="10" t="str">
+      <c r="A13" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject10</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="C13" s="76" t="str">
+      <c r="B13" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="64">
         <v>3</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63" t="str">
+      <c r="E13" s="64"/>
+      <c r="F13" s="64" t="str">
         <f t="shared" si="8"/>
         <v>010</v>
       </c>
-      <c r="G13" s="117" t="str">
+      <c r="G13" s="122" t="str">
         <f t="shared" ref="G13:G23" si="12">G12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H13" s="118" t="str">
+      <c r="H13" s="123" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="I13" s="63"/>
-      <c r="J13" s="119" t="str">
+      <c r="I13" s="64"/>
+      <c r="J13" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K13" s="120" t="str">
+      <c r="K13" s="125" t="str">
         <f t="shared" ref="K13:K23" si="13">K12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L13" s="121">
+      <c r="L13" s="126">
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1">
-      <c r="A14" s="10" t="str">
+      <c r="A14" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject11</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="C14" s="76" t="str">
+      <c r="B14" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="64">
         <v>3</v>
       </c>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63" t="str">
+      <c r="E14" s="64"/>
+      <c r="F14" s="64" t="str">
         <f t="shared" si="8"/>
         <v>011</v>
       </c>
-      <c r="G14" s="117" t="str">
+      <c r="G14" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H14" s="118" t="s">
-        <v>252</v>
-      </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="119" t="str">
+      <c r="H14" s="123" t="s">
+        <v>264</v>
+      </c>
+      <c r="I14" s="64"/>
+      <c r="J14" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K14" s="120" t="str">
+      <c r="K14" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L14" s="121">
+      <c r="L14" s="126">
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="10" t="str">
+      <c r="A15" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject12</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="C15" s="76" t="str">
+      <c r="B15" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C15" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="64">
         <v>3</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63" t="str">
+      <c r="E15" s="64"/>
+      <c r="F15" s="64" t="str">
         <f t="shared" si="8"/>
         <v>012</v>
       </c>
-      <c r="G15" s="117" t="str">
+      <c r="G15" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H15" s="118" t="str">
+      <c r="H15" s="123" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="119" t="str">
+      <c r="I15" s="64"/>
+      <c r="J15" s="124" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K15" s="120" t="str">
+      <c r="K15" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L15" s="121">
+      <c r="L15" s="126">
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="10" t="str">
+      <c r="A16" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject13</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="C16" s="76" t="str">
+      <c r="B16" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C16" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D16" s="63">
+      <c r="D16" s="64">
         <v>4</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63" t="str">
+      <c r="E16" s="64"/>
+      <c r="F16" s="64" t="str">
         <f t="shared" si="8"/>
         <v>013</v>
       </c>
-      <c r="G16" s="117" t="s">
-        <v>255</v>
-      </c>
-      <c r="H16" s="118" t="str">
+      <c r="G16" s="122" t="s">
+        <v>267</v>
+      </c>
+      <c r="H16" s="123" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I16" s="63"/>
-      <c r="J16" s="119" t="str">
+      <c r="I16" s="64"/>
+      <c r="J16" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K16" s="120" t="s">
-        <v>256</v>
-      </c>
-      <c r="L16" s="121">
+      <c r="K16" s="125" t="s">
+        <v>268</v>
+      </c>
+      <c r="L16" s="126">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
     <row r="17" ht="30" customHeight="1">
-      <c r="A17" s="10" t="str">
+      <c r="A17" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject14</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C17" s="76" t="str">
+      <c r="B17" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C17" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="64">
         <v>4</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63" t="str">
+      <c r="E17" s="64"/>
+      <c r="F17" s="64" t="str">
         <f t="shared" si="8"/>
         <v>014</v>
       </c>
-      <c r="G17" s="117" t="str">
+      <c r="G17" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H17" s="118" t="str">
+      <c r="H17" s="123" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I17" s="63"/>
-      <c r="J17" s="119" t="str">
+      <c r="I17" s="64"/>
+      <c r="J17" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K17" s="120" t="str">
+      <c r="K17" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L17" s="121">
+      <c r="L17" s="126">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
-      <c r="A18" s="10" t="str">
+      <c r="A18" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject15</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="C18" s="76" t="str">
+      <c r="B18" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="C18" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="64">
         <v>4</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63" t="str">
+      <c r="E18" s="64"/>
+      <c r="F18" s="64" t="str">
         <f t="shared" si="8"/>
         <v>015</v>
       </c>
-      <c r="G18" s="117" t="str">
+      <c r="G18" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H18" s="118" t="str">
+      <c r="H18" s="123" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="I18" s="63"/>
-      <c r="J18" s="119" t="str">
+      <c r="I18" s="64"/>
+      <c r="J18" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K18" s="120" t="str">
+      <c r="K18" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L18" s="121">
+      <c r="L18" s="126">
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1">
-      <c r="A19" s="10" t="str">
+      <c r="A19" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject16</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C19" s="76" t="str">
+      <c r="B19" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="64">
         <v>4</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63" t="str">
+      <c r="E19" s="64"/>
+      <c r="F19" s="64" t="str">
         <f t="shared" si="8"/>
         <v>016</v>
       </c>
-      <c r="G19" s="117" t="str">
+      <c r="G19" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H19" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="119" t="str">
+      <c r="H19" s="123" t="s">
+        <v>272</v>
+      </c>
+      <c r="I19" s="64"/>
+      <c r="J19" s="124" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K19" s="120" t="str">
+      <c r="K19" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L19" s="121">
+      <c r="L19" s="126">
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="1">
-      <c r="A20" s="10" t="str">
+      <c r="A20" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject17</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C20" s="76" t="str">
+      <c r="B20" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D20" s="63">
+      <c r="D20" s="64">
         <v>5</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63" t="str">
+      <c r="E20" s="64"/>
+      <c r="F20" s="64" t="str">
         <f t="shared" si="8"/>
         <v>017</v>
       </c>
-      <c r="G20" s="117" t="s">
-        <v>262</v>
-      </c>
-      <c r="H20" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="I20" s="63"/>
-      <c r="J20" s="119" t="str">
+      <c r="G20" s="122" t="s">
+        <v>274</v>
+      </c>
+      <c r="H20" s="123" t="s">
+        <v>272</v>
+      </c>
+      <c r="I20" s="64"/>
+      <c r="J20" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K20" s="120" t="s">
-        <v>263</v>
-      </c>
-      <c r="L20" s="121">
+      <c r="K20" s="125" t="s">
+        <v>275</v>
+      </c>
+      <c r="L20" s="126">
         <f t="shared" si="11"/>
         <v>17</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
-      <c r="A21" s="10" t="str">
+      <c r="A21" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject18</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="C21" s="76" t="str">
+      <c r="B21" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="C21" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D21" s="63">
+      <c r="D21" s="64">
         <v>5</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63" t="str">
+      <c r="E21" s="64"/>
+      <c r="F21" s="64" t="str">
         <f t="shared" si="8"/>
         <v>018</v>
       </c>
-      <c r="G21" s="117" t="str">
+      <c r="G21" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H21" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="I21" s="63"/>
-      <c r="J21" s="119" t="str">
+      <c r="H21" s="123" t="s">
+        <v>272</v>
+      </c>
+      <c r="I21" s="64"/>
+      <c r="J21" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K21" s="120" t="str">
+      <c r="K21" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L21" s="121">
+      <c r="L21" s="126">
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="30" customHeight="1">
-      <c r="A22" s="10" t="str">
+      <c r="A22" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject19</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="C22" s="76" t="str">
+      <c r="B22" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D22" s="63">
+      <c r="D22" s="64">
         <v>5</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63" t="str">
+      <c r="E22" s="64"/>
+      <c r="F22" s="64" t="str">
         <f t="shared" si="8"/>
         <v>019</v>
       </c>
-      <c r="G22" s="117" t="str">
+      <c r="G22" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H22" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="I22" s="63"/>
-      <c r="J22" s="119" t="str">
+      <c r="H22" s="123" t="s">
+        <v>272</v>
+      </c>
+      <c r="I22" s="64"/>
+      <c r="J22" s="124" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K22" s="120" t="str">
+      <c r="K22" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L22" s="121">
+      <c r="L22" s="126">
         <f t="shared" si="11"/>
         <v>19</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
-      <c r="A23" s="10" t="str">
+      <c r="A23" s="11" t="str">
         <f t="shared" si="7"/>
         <v>subject20</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="C23" s="76" t="str">
+      <c r="B23" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D23" s="63">
+      <c r="D23" s="64">
         <v>5</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63" t="str">
+      <c r="E23" s="64"/>
+      <c r="F23" s="64" t="str">
         <f t="shared" si="8"/>
         <v>020</v>
       </c>
-      <c r="G23" s="117" t="str">
+      <c r="G23" s="122" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H23" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="I23" s="63"/>
-      <c r="J23" s="119" t="str">
+      <c r="H23" s="123" t="s">
+        <v>272</v>
+      </c>
+      <c r="I23" s="64"/>
+      <c r="J23" s="124" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K23" s="120" t="str">
+      <c r="K23" s="125" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L23" s="121">
+      <c r="L23" s="126">
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="L24" s="74"/>
+      <c r="L24" s="75"/>
     </row>
     <row r="25" ht="14.25"/>
   </sheetData>
@@ -3406,59 +3496,59 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>17</v>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="11" t="s">
+    </row>
+    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>25</v>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3499,727 +3589,727 @@
     <col customWidth="1" min="29" max="29" width="17.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" ht="14.25">
-      <c r="A1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="12" t="str">
+    <row r="1" s="13" customFormat="1" ht="14.25">
+      <c r="A1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",E5)</f>
         <v>plugins.users.users</v>
       </c>
-      <c r="F1" s="12" t="str">
+      <c r="F1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",F5)</f>
         <v>plugins.users.user-data</v>
       </c>
-      <c r="G1" s="12" t="str">
+      <c r="G1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",G5)</f>
         <v>plugins.users.centers</v>
       </c>
-      <c r="H1" s="12" t="str">
+      <c r="H1" s="13" t="str">
         <f>_xlfn.CONCAT($E$3,".",H5)</f>
         <v>plugins.users.profiles</v>
       </c>
-      <c r="I1" s="12" t="str">
+      <c r="I1" s="13" t="str">
         <f>_xlfn.CONCAT($I$3,".",I5)</f>
         <v>plugins.dataset.dataset</v>
       </c>
-      <c r="J1" s="12" t="str">
+      <c r="J1" s="13" t="str">
         <f>_xlfn.CONCAT($J$3,".",J5)</f>
         <v>plugins.calendar.calendar</v>
       </c>
-      <c r="K1" s="12" t="str">
+      <c r="K1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",K5)</f>
         <v>plugins.academic-portfolio.portfolio</v>
       </c>
-      <c r="L1" s="12" t="str">
+      <c r="L1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",L5)</f>
         <v>plugins.academic-portfolio.programs</v>
       </c>
-      <c r="M1" s="12" t="str">
+      <c r="M1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",M5)</f>
         <v>plugins.academic-portfolio.profiles</v>
       </c>
-      <c r="N1" s="12" t="str">
+      <c r="N1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",N5)</f>
         <v>plugins.academic-portfolio.subjects</v>
       </c>
-      <c r="O1" s="12" t="str">
+      <c r="O1" s="13" t="str">
         <f>_xlfn.CONCAT($K$3,".",O5)</f>
         <v>plugins.academic-portfolio.tree</v>
       </c>
-      <c r="P1" s="12" t="str">
+      <c r="P1" s="13" t="str">
         <f>_xlfn.CONCAT($P$3,".",P5)</f>
         <v>plugins.families.families</v>
       </c>
-      <c r="Q1" s="12" t="str">
+      <c r="Q1" s="13" t="str">
         <f>_xlfn.CONCAT($P$3,".",Q5)</f>
         <v>plugins.families.config</v>
       </c>
-      <c r="R1" s="12" t="str">
+      <c r="R1" s="13" t="str">
         <f>_xlfn.CONCAT($P$3,".",R5)</f>
         <v>plugins.families.families-basic-info</v>
       </c>
-      <c r="S1" s="12" t="str">
+      <c r="S1" s="13" t="str">
         <f>_xlfn.CONCAT($P$3,".",S5)</f>
         <v>plugins.families.families-custom-info</v>
       </c>
-      <c r="T1" s="12" t="str">
+      <c r="T1" s="13" t="str">
         <f>_xlfn.CONCAT($P$3,".",T5)</f>
         <v>plugins.families.families-guardians-info</v>
       </c>
-      <c r="U1" s="12" t="str">
+      <c r="U1" s="13" t="str">
         <f>_xlfn.CONCAT($P$3,".",U5)</f>
         <v>plugins.families.families-students-info</v>
       </c>
-      <c r="V1" s="12" t="str">
+      <c r="V1" s="13" t="str">
         <f>_xlfn.CONCAT($V$3,".",V5)</f>
         <v>plugins.timetable.config</v>
       </c>
-      <c r="W1" s="12" t="str">
+      <c r="W1" s="13" t="str">
         <f>_xlfn.CONCAT($V$3,".",W5)</f>
         <v>plugins.timetable.timetable</v>
       </c>
-      <c r="X1" s="12" t="str">
+      <c r="X1" s="13" t="str">
         <f>_xlfn.CONCAT($X$3,".",X5)</f>
         <v>plugins.tasks.tasks</v>
       </c>
-      <c r="Y1" s="12" t="str">
+      <c r="Y1" s="13" t="str">
         <f>_xlfn.CONCAT($X$3,".",Y5)</f>
         <v>plugins.tasks.library</v>
       </c>
-      <c r="Z1" s="12" t="str">
+      <c r="Z1" s="13" t="str">
         <f>_xlfn.CONCAT($X$3,".",Z5)</f>
         <v>plugins.tasks.ongoing</v>
       </c>
-      <c r="AA1" s="12" t="str">
+      <c r="AA1" s="13" t="str">
         <f>_xlfn.CONCAT($X$3,".",AA5)</f>
         <v>plugins.tasks.history</v>
       </c>
-      <c r="AB1" s="12" t="str">
+      <c r="AB1" s="13" t="str">
         <f>_xlfn.CONCAT($AB$3,".",AB5)</f>
         <v>plugins.curriculum.curriculum</v>
       </c>
-      <c r="AC1" s="12" t="str">
+      <c r="AC1" s="13" t="str">
         <f>_xlfn.CONCAT($AC$3,".",AC5)</f>
         <v>plugins.leebrary.library</v>
       </c>
     </row>
-    <row r="2" s="9" customFormat="1" ht="21.350000000000001" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
+    <row r="2" s="10" customFormat="1" ht="21.350000000000001" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="W3" s="16"/>
-      <c r="X3" s="24" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="26" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="AC3" s="19" t="s">
+      <c r="J3" s="19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" s="27" customFormat="1" ht="19.850000000000001" customHeight="1">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28" t="s">
+      <c r="K3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30" t="s">
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="W3" s="17"/>
+      <c r="X3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="34" t="s">
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="28" t="s">
+      <c r="AC3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="29"/>
-      <c r="X4" s="30" t="s">
+    </row>
+    <row r="4" s="28" customFormat="1" ht="19.850000000000001" customHeight="1">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="31" t="s">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="AC4" s="32" t="s">
+      <c r="J4" s="32" t="s">
         <v>48</v>
       </c>
+      <c r="K4" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="30"/>
+      <c r="X4" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC4" s="33" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="39" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="R5" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="W5" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="X5" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y5" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z5" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA5" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB5" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC5" s="49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" s="50" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="N6" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="P6" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="40" t="s">
+      <c r="Q6" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="R6" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="S6" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="T6" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="U6" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="V6" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="X6" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="42" t="s">
+      <c r="Y6" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="M5" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="P5" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q5" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="S5" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="T5" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="U5" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="V5" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="W5" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="X5" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y5" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z5" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA5" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB5" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC5" s="48" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" s="49" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="L6" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="M6" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="N6" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="P6" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q6" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="R6" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="S6" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="T6" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="U6" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="V6" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="W6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="X6" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y6" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z6" s="53" t="s">
+      <c r="Z6" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA6" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB6" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="AA6" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB6" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC6" s="61" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="H7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="I7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="J7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="L7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="N7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="O7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="P7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="R7" s="64"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="W7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="X7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA7" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB7" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC7" s="63" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="63" t="s">
+      <c r="AC6" s="62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="63" t="s">
+      <c r="B7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="J8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="K8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="L8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="O8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="P8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="R8" s="64"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="63"/>
-      <c r="U8" s="63"/>
-      <c r="V8" s="63" t="s">
+      <c r="F7" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="W8" s="63" t="s">
+      <c r="G7" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="X8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB8" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC8" s="63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="H7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="O7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="P7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="W7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="X7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA7" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB7" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC7" s="64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="63" t="s">
+      <c r="D8" s="63"/>
+      <c r="E8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="F8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="J9" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="K9" s="63" t="s">
+      <c r="G8" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="I8" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="L9" s="63" t="s">
+      <c r="K8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63" t="s">
+      <c r="L8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63" t="s">
+      <c r="M8" s="64"/>
+      <c r="N8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="Q9" s="63" t="s">
+      <c r="O8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="R9" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="S9" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="T9" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="U9" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="V9" s="63" t="s">
+      <c r="P8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="W9" s="63" t="s">
+      <c r="Q8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="X9" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y9" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z9" s="63" t="s">
+      <c r="R8" s="65"/>
+      <c r="S8" s="64"/>
+      <c r="T8" s="64"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="W8" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="X8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="AA9" s="63" t="s">
+      <c r="Y8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="AB9" s="63" t="s">
+      <c r="Z8" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="AC9" s="63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A10" s="10" t="s">
+      <c r="AA8" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB8" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC8" s="64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A9" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="H9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="J9" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="O9" s="64"/>
+      <c r="P9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="62" t="str">
+      <c r="S9" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="T9" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="U9" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="V9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="W9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="X9" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y9" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB9" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC9" s="64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="63" t="str">
         <f>A9</f>
         <v>student</v>
       </c>
-      <c r="E10" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="63" t="s">
+      <c r="E10" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="63" t="s">
+      <c r="F10" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="K10" s="63" t="s">
+      <c r="G10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="L10" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q10" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="R10" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="S10" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="T10" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="U10" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="V10" s="63"/>
-      <c r="W10" s="63"/>
-      <c r="X10" s="63"/>
-      <c r="Y10" s="63"/>
-      <c r="Z10" s="63"/>
-      <c r="AA10" s="63"/>
-      <c r="AB10" s="63"/>
-      <c r="AC10" s="63" t="s">
-        <v>95</v>
+      <c r="K10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="O10" s="64"/>
+      <c r="P10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="R10" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="S10" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="T10" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="U10" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="V10" s="64"/>
+      <c r="W10" s="64"/>
+      <c r="X10" s="64"/>
+      <c r="Y10" s="64"/>
+      <c r="Z10" s="64"/>
+      <c r="AA10" s="64"/>
+      <c r="AB10" s="64"/>
+      <c r="AC10" s="64" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4268,287 +4358,287 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="67" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="68">
+        <v>36526</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="68">
+        <v>34781</v>
+      </c>
+      <c r="F4" s="69" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A5" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="67">
-        <v>36526</v>
-      </c>
-      <c r="F3" s="68" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="69" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="E5" s="68">
+        <v>39205</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A6" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="68">
+        <v>39156</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="68">
+        <v>42171</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="74" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="67">
-        <v>34781</v>
-      </c>
-      <c r="F4" s="68" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="69" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="70" t="s">
+      <c r="E8" s="68">
+        <v>42237</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="67">
-        <v>39205</v>
-      </c>
-      <c r="F5" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="73" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="70" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="71" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="H8" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="74" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A9" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="67">
-        <v>39156</v>
-      </c>
-      <c r="F6" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="73" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="70" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="71" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="67">
-        <v>42171</v>
-      </c>
-      <c r="F7" s="72" t="s">
-        <v>132</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H7" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="73" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="70" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="67">
-        <v>42237</v>
-      </c>
-      <c r="F8" s="72" t="s">
-        <v>136</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="73" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="67">
+      <c r="E9" s="68">
         <v>27791</v>
       </c>
-      <c r="F9" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H9" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="69" t="s">
-        <v>141</v>
+      <c r="F9" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="70" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4565,43 +4655,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{000A00A4-00CB-473C-829E-002F007F00E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0028004D-00ED-43F5-9E2C-0004000300F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004500ED-0079-498A-9BBF-009300EF001A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005A00EE-006C-47E7-9E79-0037001200FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E200D2-0071-401F-95C1-002C00A20077}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C400A1-004C-4540-AED4-0048000800E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006A0050-00C8-4384-8726-00DB00AF00FA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A00006-0003-48E4-9C8F-00DF006B0063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B700E2-0038-4CD3-968E-0024006B000A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FA00C2-0099-4930-A02C-00ED009E00B8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0047006C-0004-44B1-A32B-005400980021}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004C0076-009D-46B5-89D1-0044008900E4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000D0037-0023-4F6A-86D0-00B8008E007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EE0062-0025-48EE-80A8-00BD002000EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -4632,48 +4722,48 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>142</v>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="76" t="str">
+      <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="77" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="76" t="str">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="77" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" ht="14.25"/>
     <row r="6" ht="14.25"/>
@@ -4702,33 +4792,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="67.57421875"/>
+    <col customWidth="1" min="2" max="2" width="14.8515625"/>
+    <col customWidth="1" min="3" max="3" width="61.140625"/>
+    <col customWidth="1" min="4" max="4" width="21.57421875"/>
+    <col customWidth="1" min="5" max="5" width="33.57421875"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>144</v>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="2" ht="24.350000000000001" customHeight="1">
-      <c r="A2" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="76" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="A2" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="4"/>
   </sheetData>
@@ -4736,6 +4855,18 @@
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
+        <x14:dataValidation xr:uid="{00120081-00BD-4066-B623-002400B60089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4757,35 +4888,35 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>142</v>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="76" t="str">
+      <c r="A2" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="77" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
     </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="76" t="str">
+    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="77" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -4835,326 +4966,326 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="P1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="D1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-    </row>
-    <row r="2" s="9" customFormat="1" ht="23.600000000000001" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="E2" s="79" t="s">
+      <c r="L1" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F2" s="79"/>
-      <c r="G2" s="80" t="s">
+      <c r="M1" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="83" t="s">
+      <c r="N1" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="84" t="s">
+      <c r="O1" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="87" t="s">
+      <c r="P1" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
+      <c r="Q1" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+    </row>
+    <row r="2" s="10" customFormat="1" ht="23.600000000000001" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="E2" s="84" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="89" t="s">
+        <v>183</v>
+      </c>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
     </row>
     <row r="3" ht="34.100000000000001" customHeight="1">
-      <c r="A3" s="89" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="90" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="90" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="92" t="s">
-        <v>174</v>
-      </c>
-      <c r="F3" s="93" t="s">
-        <v>175</v>
-      </c>
-      <c r="G3" s="94" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="95" t="s">
-        <v>177</v>
-      </c>
-      <c r="I3" s="96" t="s">
-        <v>178</v>
-      </c>
-      <c r="J3" s="96" t="s">
-        <v>179</v>
-      </c>
-      <c r="K3" s="96" t="s">
-        <v>180</v>
-      </c>
-      <c r="L3" s="96" t="s">
-        <v>181</v>
-      </c>
-      <c r="M3" s="96" t="s">
-        <v>182</v>
-      </c>
-      <c r="N3" s="97" t="s">
-        <v>183</v>
-      </c>
-      <c r="O3" s="98" t="s">
-        <v>181</v>
-      </c>
-      <c r="P3" s="99" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q3" s="100" t="s">
-        <v>184</v>
-      </c>
-      <c r="R3" s="101" t="s">
+      <c r="A3" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="S3" s="101" t="s">
-        <v>181</v>
-      </c>
-      <c r="T3" s="101" t="s">
-        <v>182</v>
-      </c>
-      <c r="U3" s="102" t="s">
-        <v>181</v>
-      </c>
-      <c r="V3" s="103" t="s">
+      <c r="D3" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="97" t="s">
         <v>186</v>
       </c>
-      <c r="W3" s="104" t="s">
+      <c r="F3" s="98" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="G3" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="H3" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="I3" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="D4" s="76" t="str">
+      <c r="J3" s="101" t="s">
+        <v>191</v>
+      </c>
+      <c r="K3" s="101" t="s">
+        <v>192</v>
+      </c>
+      <c r="L3" s="101" t="s">
+        <v>193</v>
+      </c>
+      <c r="M3" s="101" t="s">
+        <v>194</v>
+      </c>
+      <c r="N3" s="102" t="s">
+        <v>195</v>
+      </c>
+      <c r="O3" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="P3" s="104" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q3" s="105" t="s">
+        <v>196</v>
+      </c>
+      <c r="R3" s="106" t="s">
+        <v>197</v>
+      </c>
+      <c r="S3" s="106" t="s">
+        <v>193</v>
+      </c>
+      <c r="T3" s="106" t="s">
+        <v>194</v>
+      </c>
+      <c r="U3" s="107" t="s">
+        <v>193</v>
+      </c>
+      <c r="V3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="W3" s="109" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="77" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="64">
         <v>0</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="64">
         <v>5</v>
       </c>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63" t="s">
+      <c r="H4" s="64"/>
+      <c r="I4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="105"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63" t="s">
+      <c r="J4" s="110"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63" t="s">
+      <c r="O4" s="64"/>
+      <c r="P4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="63" t="s">
+      <c r="Q4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="63" t="s">
+      <c r="R4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="63">
+      <c r="S4" s="64">
         <v>3</v>
       </c>
-      <c r="T4" s="63" t="s">
+      <c r="T4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="63">
+      <c r="U4" s="64">
         <v>3</v>
       </c>
-      <c r="V4" s="63" t="s">
+      <c r="V4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="63" t="s">
+      <c r="W4" s="64" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" s="9" customFormat="1" ht="28.5">
-      <c r="A5" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="76" t="str">
+    <row r="5" s="10" customFormat="1" ht="28.5">
+      <c r="A5" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="77" t="str">
         <f>centers!$A$4</f>
         <v>centerB</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="63">
+      <c r="F5" s="64">
         <v>240</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="64">
         <v>4</v>
       </c>
-      <c r="H5" s="63">
+      <c r="H5" s="64">
         <v>60</v>
       </c>
-      <c r="I5" s="63" t="s">
+      <c r="I5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="105" t="s">
-        <v>194</v>
-      </c>
-      <c r="K5" s="63" t="s">
+      <c r="J5" s="110" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="63">
+      <c r="L5" s="64">
         <v>4</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="63" t="s">
+      <c r="N5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="63">
+      <c r="O5" s="64">
         <v>4</v>
       </c>
-      <c r="P5" s="63" t="s">
+      <c r="P5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="63" t="s">
+      <c r="Q5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="63" t="s">
+      <c r="R5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="63">
+      <c r="S5" s="64">
         <v>3</v>
       </c>
-      <c r="T5" s="63" t="s">
+      <c r="T5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="63">
+      <c r="U5" s="64">
         <v>3</v>
       </c>
-      <c r="V5" s="63" t="s">
+      <c r="V5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="W5" s="63" t="s">
+      <c r="W5" s="64" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5173,79 +5304,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00760014-00A6-4807-BAFB-0000005C002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00970071-00FD-4B34-BE28-009700D80050}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E200E6-00BB-49AE-9602-00BA00B100FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004F00EA-001D-4C16-831E-007F0072001B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F800B7-0065-4C20-B7BB-008E0004000A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FD0051-00B3-4EB2-BD32-0091006A0063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00860067-00EC-4284-A1B5-00B40087001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D500BE-005F-4F7C-AD47-004E0034004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F600B5-001C-4AFB-9763-00A7004700F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00110048-007B-4467-828B-005400B10084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0075004C-0014-4C24-B6FC-009100350070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0070005F-00A6-4F00-8C3A-0007005F005E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DC00CC-00A2-4E06-A24A-001B00570067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005E0059-00CF-463C-AD24-002F00DD00D3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>R4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0094003A-0098-40CE-AE33-003A005700E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004F0095-0061-4959-A401-005100CD00E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003500F2-0057-457D-A210-00A600830088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C500CB-00B7-48DB-8354-001400630037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005B0057-0065-4E71-9906-003700A90047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0079004A-00EF-4768-BEA8-0061003800B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00800010-0080-46BD-82EB-0075008900EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A600D6-0074-45D0-88B2-0086002600BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009200A7-0072-49E8-840F-000B00A60056}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00130013-0059-405B-B162-00D0003400AD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D30091-006B-4E77-B7E6-003100C100A2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002F00F9-00A8-4CC0-941C-00B90036006E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5277,90 +5408,90 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>197</v>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="89" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="90" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="91" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="106" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="106" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" s="76" t="str">
+      <c r="A2" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="96" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="111" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="111" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="77" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="64">
         <v>0</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="64" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" s="76" t="str">
+    <row r="4" s="10" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="77" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="64">
         <v>0</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="64" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="76" t="str">
+      <c r="A5" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="77" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="64">
         <v>0</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="64" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5372,19 +5503,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{006300CD-00AF-41EC-9872-00D2004B0006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CA001D-00AA-4E7E-BCD8-00160039005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006800B1-00FB-4464-8CFB-0063006F0027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D5005A-0099-4A64-9D76-0009004700F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006A009E-0059-4004-AC54-00D500320006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0041004B-0026-48A6-B90B-009E00DC0092}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
ADDED: Import Families Emergency numbers in MVP Template bulk.
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -4655,43 +4655,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0028004D-00ED-43F5-9E2C-0004000300F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00960023-00C6-4EE4-9B31-00FA002C00BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005A00EE-006C-47E7-9E79-0037001200FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002B00DD-0024-489F-A7CE-002A002200DB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C400A1-004C-4540-AED4-0048000800E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C10083-00FF-4DB5-9AA5-00C80067003B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A00006-0003-48E4-9C8F-00DF006B0063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AE00D2-00E6-414A-A20F-000F0080002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FA00C2-0099-4930-A02C-00ED009E00B8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008C005C-00A2-4D9F-A20A-00E0003700FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004C0076-009D-46B5-89D1-0044008900E4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006A0077-005D-4300-8D36-00A0002C00DE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EE0062-0025-48EE-80A8-00BD002000EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0035009B-0066-4253-AE28-00390067008F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -4858,7 +4858,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00120081-00BD-4066-B623-002400B60089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00720056-00EE-4319-A6C4-008300CB00E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5304,79 +5304,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00970071-00FD-4B34-BE28-009700D80050}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E900D4-00A8-40B4-B779-001D00C90029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004F00EA-001D-4C16-831E-007F0072001B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B800C1-00A2-4288-AE97-0085004D005C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FD0051-00B3-4EB2-BD32-0091006A0063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00270020-00CB-4143-B45F-00A0008A0095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D500BE-005F-4F7C-AD47-004E0034004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EB0027-0096-4957-81D5-0000009E003D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00110048-007B-4467-828B-005400B10084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00290025-0075-43E6-AF73-001400DB00EA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0070005F-00A6-4F00-8C3A-0007005F005E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000F0045-006A-416A-A306-00390010006A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005E0059-00CF-463C-AD24-002F00DD00D3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008100D4-0058-4CCC-A872-005000AC007A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>R4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004F0095-0061-4959-A401-005100CD00E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00880097-00D0-44F3-AB9F-000E00FB008E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C500CB-00B7-48DB-8354-001400630037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DF0061-0035-46AB-B943-0057003900E1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0079004A-00EF-4768-BEA8-0061003800B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B80055-0011-477B-B700-00C1007F0075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A600D6-0074-45D0-88B2-0086002600BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007500E3-00FA-4BE3-9FA6-0006003A00A8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00130013-0059-405B-B162-00D0003400AD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FE0099-0031-4581-B0A6-0054000100E4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002F00F9-00A8-4CC0-941C-00B90036006E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F6002E-00E4-40D6-89C4-00ED00F20019}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5503,19 +5503,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00CA001D-00AA-4E7E-BCD8-00160039005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007A00DA-00BC-4841-9B45-008900D5007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D5005A-0099-4A64-9D76-0009004700F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D8007B-0097-4FB4-B12A-00D900A10076}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0041004B-0026-48A6-B90B-009E00DC0092}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EC004C-00D4-487B-BA10-007900AB00F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Add users to classes.
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="287">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -746,6 +746,9 @@
     <t>course</t>
   </si>
   <si>
+    <t>seats</t>
+  </si>
+  <si>
     <t>internalId</t>
   </si>
   <si>
@@ -765,6 +768,9 @@
   </si>
   <si>
     <t>Course</t>
+  </si>
+  <si>
+    <t>Seats</t>
   </si>
   <si>
     <t>Credits</t>
@@ -2525,7 +2531,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="0" topLeftCell="A1" workbookViewId="0" zoomScale="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A4" ySplit="3"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -2535,13 +2541,13 @@
     <col customWidth="1" min="1" max="1" width="12.8515625"/>
     <col customWidth="1" min="2" max="2" width="18.421875"/>
     <col customWidth="1" min="3" max="3" width="12.8515625"/>
-    <col customWidth="1" min="6" max="6" width="10.421875"/>
-    <col customWidth="1" min="7" max="7" width="13.00390625"/>
-    <col customWidth="1" min="8" max="8" width="10.8515625"/>
-    <col customWidth="1" min="9" max="9" width="11.8515625"/>
-    <col customWidth="1" min="10" max="10" width="10.140625"/>
-    <col customWidth="1" min="11" max="11" width="23.28125"/>
-    <col customWidth="1" min="12" max="12" width="3.57421875"/>
+    <col customWidth="1" min="7" max="7" width="10.421875"/>
+    <col customWidth="1" min="8" max="8" width="13.00390625"/>
+    <col customWidth="1" min="9" max="9" width="10.8515625"/>
+    <col customWidth="1" min="10" max="10" width="11.8515625"/>
+    <col customWidth="1" min="11" max="11" width="10.140625"/>
+    <col customWidth="1" min="12" max="12" width="23.28125"/>
+    <col customWidth="1" min="13" max="13" width="3.57421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -2558,27 +2564,30 @@
         <v>237</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>239</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>240</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="K1" s="115" t="s">
+      <c r="K1" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="L1" s="74"/>
+      <c r="L1" s="115" t="s">
+        <v>243</v>
+      </c>
+      <c r="M1" s="74"/>
     </row>
     <row r="2" ht="28.850000000000001" customHeight="1">
       <c r="A2" s="5"/>
@@ -2587,14 +2596,15 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="H2" s="1"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="1" t="s">
+        <v>244</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="74"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="74"/>
     </row>
     <row r="3" ht="31.850000000000001" customHeight="1">
       <c r="A3" s="110" t="s">
@@ -2607,38 +2617,41 @@
         <v>216</v>
       </c>
       <c r="D3" s="93" t="s">
-        <v>244</v>
-      </c>
-      <c r="E3" s="93" t="s">
         <v>245</v>
       </c>
+      <c r="E3" s="111" t="s">
+        <v>246</v>
+      </c>
       <c r="F3" s="93" t="s">
-        <v>246</v>
-      </c>
-      <c r="G3" s="116" t="s">
         <v>247</v>
       </c>
-      <c r="H3" s="117" t="s">
+      <c r="G3" s="93" t="s">
+        <v>248</v>
+      </c>
+      <c r="H3" s="116" t="s">
+        <v>249</v>
+      </c>
+      <c r="I3" s="117" t="s">
         <v>225</v>
       </c>
-      <c r="I3" s="117" t="s">
-        <v>248</v>
-      </c>
-      <c r="J3" s="118" t="s">
-        <v>249</v>
-      </c>
-      <c r="K3" s="112" t="s">
+      <c r="J3" s="117" t="s">
         <v>250</v>
       </c>
-      <c r="L3" s="119"/>
+      <c r="K3" s="118" t="s">
+        <v>251</v>
+      </c>
+      <c r="L3" s="112" t="s">
+        <v>252</v>
+      </c>
+      <c r="M3" s="119"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
-        <f t="shared" ref="A4:A9" si="0">_xlfn.CONCAT("subject",IF(L4&lt;10,"0",""),L4)</f>
+        <f>_xlfn.CONCAT("subject",IF(M4&lt;10,"0",""),M4)</f>
         <v>subject01</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C4" s="77" t="str">
         <f>ap_programs!A4</f>
@@ -2647,823 +2660,884 @@
       <c r="D4" s="63">
         <v>1</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63" t="str">
-        <f t="shared" ref="F4:F9" si="1">_xlfn.CONCAT("0",IF(L4&lt;10,"0",""),L4)</f>
+      <c r="E4" s="63">
+        <v>20</v>
+      </c>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M4&lt;10,"0",""),M4)</f>
         <v>001</v>
       </c>
-      <c r="G4" s="120" t="s">
-        <v>252</v>
-      </c>
-      <c r="H4" s="121" t="s">
-        <v>253</v>
-      </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="122" t="str">
+      <c r="H4" s="120" t="s">
+        <v>254</v>
+      </c>
+      <c r="I4" s="121" t="s">
+        <v>255</v>
+      </c>
+      <c r="J4" s="63"/>
+      <c r="K4" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K4" s="123" t="s">
-        <v>254</v>
-      </c>
-      <c r="L4" s="124">
+      <c r="L4" s="123" t="s">
+        <v>256</v>
+      </c>
+      <c r="M4" s="124">
         <v>1</v>
       </c>
-      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
     </row>
     <row r="5" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("subject",IF(M5&lt;10,"0",""),M5)</f>
         <v>subject02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C5" s="77" t="str">
-        <f t="shared" ref="C5:C10" si="2">C4</f>
+        <f t="shared" ref="C5:C10" si="0">C4</f>
         <v>programA</v>
       </c>
       <c r="D5" s="63">
         <v>1</v>
       </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63" t="str">
-        <f t="shared" si="1"/>
+      <c r="E5" s="63">
+        <v>20</v>
+      </c>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M5&lt;10,"0",""),M5)</f>
         <v>002</v>
       </c>
-      <c r="G5" s="120" t="str">
-        <f t="shared" ref="G5:G10" si="3">G4</f>
+      <c r="H5" s="120" t="str">
+        <f>H4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H5" s="121" t="str">
-        <f t="shared" ref="H5:H10" si="4">H4</f>
+      <c r="I5" s="121" t="str">
+        <f>I4</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="122" t="str">
+      <c r="J5" s="63"/>
+      <c r="K5" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K5" s="123" t="str">
-        <f t="shared" ref="K5:K10" si="5">K4</f>
+      <c r="L5" s="123" t="str">
+        <f>L4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L5" s="124">
-        <f t="shared" ref="L5:L10" si="6">L4+1</f>
+      <c r="M5" s="124">
+        <f>M4+1</f>
         <v>2</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="6" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(M6&lt;10,"0",""),M6)</f>
+        <v>subject03</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="77" t="str">
         <f t="shared" si="0"/>
-        <v>subject03</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="C6" s="77" t="str">
-        <f t="shared" si="2"/>
         <v>programA</v>
       </c>
       <c r="D6" s="63">
         <v>1</v>
       </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63" t="str">
-        <f t="shared" si="1"/>
+      <c r="E6" s="63">
+        <v>20</v>
+      </c>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M6&lt;10,"0",""),M6)</f>
         <v>003</v>
       </c>
-      <c r="G6" s="120" t="str">
-        <f t="shared" si="3"/>
+      <c r="H6" s="120" t="str">
+        <f>H5</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H6" s="121" t="str">
-        <f t="shared" si="4"/>
+      <c r="I6" s="121" t="str">
+        <f>I5</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I6" s="63"/>
-      <c r="J6" s="122" t="str">
+      <c r="J6" s="63"/>
+      <c r="K6" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K6" s="123" t="str">
-        <f t="shared" si="5"/>
+      <c r="L6" s="123" t="str">
+        <f>L5</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L6" s="124">
-        <f t="shared" si="6"/>
+      <c r="M6" s="124">
+        <f>M5+1</f>
         <v>3</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
     </row>
     <row r="7" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(M7&lt;10,"0",""),M7)</f>
+        <v>subject04</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="77" t="str">
         <f t="shared" si="0"/>
-        <v>subject04</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C7" s="77" t="str">
-        <f t="shared" si="2"/>
         <v>programA</v>
       </c>
       <c r="D7" s="63">
         <v>1</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63" t="str">
-        <f t="shared" si="1"/>
+      <c r="E7" s="63">
+        <v>20</v>
+      </c>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M7&lt;10,"0",""),M7)</f>
         <v>004</v>
       </c>
-      <c r="G7" s="120" t="str">
-        <f t="shared" si="3"/>
+      <c r="H7" s="120" t="str">
+        <f>H6</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="H7" s="121" t="str">
-        <f t="shared" si="4"/>
+      <c r="I7" s="121" t="str">
+        <f>I6</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="122" t="str">
+      <c r="J7" s="63"/>
+      <c r="K7" s="122" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K7" s="123" t="str">
-        <f t="shared" si="5"/>
+      <c r="L7" s="123" t="str">
+        <f>L6</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="L7" s="124">
-        <f t="shared" si="6"/>
+      <c r="M7" s="124">
+        <f>M6+1</f>
         <v>4</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(M8&lt;10,"0",""),M8)</f>
+        <v>subject05</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="77" t="str">
         <f t="shared" si="0"/>
-        <v>subject05</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" s="77" t="str">
-        <f t="shared" si="2"/>
         <v>programA</v>
       </c>
       <c r="D8" s="63">
         <v>2</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63" t="str">
-        <f t="shared" si="1"/>
+      <c r="E8" s="63">
+        <v>20</v>
+      </c>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M8&lt;10,"0",""),M8)</f>
         <v>005</v>
       </c>
-      <c r="G8" s="120" t="s">
-        <v>259</v>
-      </c>
-      <c r="H8" s="121" t="str">
-        <f t="shared" si="4"/>
+      <c r="H8" s="120" t="s">
+        <v>261</v>
+      </c>
+      <c r="I8" s="121" t="str">
+        <f>I7</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="I8" s="63"/>
-      <c r="J8" s="122" t="str">
+      <c r="J8" s="63"/>
+      <c r="K8" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K8" s="123" t="s">
-        <v>260</v>
-      </c>
-      <c r="L8" s="124">
-        <f t="shared" si="6"/>
+      <c r="L8" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="M8" s="124">
+        <f>M7+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(M9&lt;10,"0",""),M9)</f>
+        <v>subject06</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" s="77" t="str">
         <f t="shared" si="0"/>
-        <v>subject06</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="77" t="str">
-        <f t="shared" si="2"/>
         <v>programA</v>
       </c>
       <c r="D9" s="63">
         <v>2</v>
       </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63" t="str">
-        <f t="shared" si="1"/>
+      <c r="E9" s="63">
+        <v>20</v>
+      </c>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M9&lt;10,"0",""),M9)</f>
         <v>006</v>
       </c>
-      <c r="G9" s="120" t="str">
-        <f t="shared" si="3"/>
+      <c r="H9" s="120" t="str">
+        <f>H8</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H9" s="121" t="s">
-        <v>262</v>
-      </c>
-      <c r="I9" s="63"/>
-      <c r="J9" s="122" t="str">
+      <c r="I9" s="121" t="s">
+        <v>264</v>
+      </c>
+      <c r="J9" s="63"/>
+      <c r="K9" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K9" s="123" t="str">
-        <f t="shared" si="5"/>
+      <c r="L9" s="123" t="str">
+        <f>L8</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L9" s="124">
-        <f t="shared" si="6"/>
+      <c r="M9" s="124">
+        <f>M8+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="10" t="str">
-        <f t="shared" ref="A10:A23" si="7">_xlfn.CONCAT("subject",IF(L10&lt;10,"0",""),L10)</f>
+        <f>_xlfn.CONCAT("subject",IF(M10&lt;10,"0",""),M10)</f>
         <v>subject07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C10" s="77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>programA</v>
       </c>
       <c r="D10" s="63">
         <v>2</v>
       </c>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63" t="str">
-        <f t="shared" ref="F10:F23" si="8">_xlfn.CONCAT("0",IF(L10&lt;10,"0",""),L10)</f>
+      <c r="E10" s="63">
+        <v>20</v>
+      </c>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M10&lt;10,"0",""),M10)</f>
         <v>007</v>
       </c>
-      <c r="G10" s="120" t="str">
-        <f t="shared" si="3"/>
+      <c r="H10" s="120" t="str">
+        <f>H9</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H10" s="121" t="str">
-        <f t="shared" si="4"/>
+      <c r="I10" s="121" t="str">
+        <f>I9</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I10" s="63"/>
-      <c r="J10" s="122" t="str">
+      <c r="J10" s="63"/>
+      <c r="K10" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K10" s="123" t="str">
-        <f t="shared" si="5"/>
+      <c r="L10" s="123" t="str">
+        <f>L9</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L10" s="124">
-        <f t="shared" si="6"/>
+      <c r="M10" s="124">
+        <f>M9+1</f>
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M11&lt;10,"0",""),M11)</f>
         <v>subject08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C11" s="77" t="str">
-        <f t="shared" ref="C11:C23" si="9">C10</f>
+        <f t="shared" ref="C11:C23" si="1">C10</f>
         <v>programA</v>
       </c>
       <c r="D11" s="63">
         <v>2</v>
       </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E11" s="63">
+        <v>20</v>
+      </c>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M11&lt;10,"0",""),M11)</f>
         <v>008</v>
       </c>
-      <c r="G11" s="120" t="str">
-        <f>G10</f>
+      <c r="H11" s="120" t="str">
+        <f>H10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="H11" s="121" t="str">
-        <f t="shared" ref="H11:H18" si="10">H10</f>
+      <c r="I11" s="121" t="str">
+        <f>I10</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I11" s="63"/>
-      <c r="J11" s="122" t="str">
+      <c r="J11" s="63"/>
+      <c r="K11" s="122" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K11" s="123" t="str">
-        <f>K10</f>
+      <c r="L11" s="123" t="str">
+        <f>L10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="L11" s="124">
-        <f t="shared" ref="L11:L23" si="11">L10+1</f>
+      <c r="M11" s="124">
+        <f>M10+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
       <c r="A12" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M12&lt;10,"0",""),M12)</f>
         <v>subject09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C12" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D12" s="63">
         <v>3</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E12" s="63">
+        <v>20</v>
+      </c>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M12&lt;10,"0",""),M12)</f>
         <v>009</v>
       </c>
-      <c r="G12" s="120" t="s">
-        <v>266</v>
-      </c>
-      <c r="H12" s="121" t="str">
-        <f t="shared" si="10"/>
+      <c r="H12" s="120" t="s">
+        <v>268</v>
+      </c>
+      <c r="I12" s="121" t="str">
+        <f>I11</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I12" s="63"/>
-      <c r="J12" s="122" t="str">
+      <c r="J12" s="63"/>
+      <c r="K12" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K12" s="123" t="s">
-        <v>267</v>
-      </c>
-      <c r="L12" s="124">
-        <f t="shared" si="11"/>
+      <c r="L12" s="123" t="s">
+        <v>269</v>
+      </c>
+      <c r="M12" s="124">
+        <f>M11+1</f>
         <v>9</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M13&lt;10,"0",""),M13)</f>
         <v>subject10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C13" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D13" s="63">
         <v>3</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E13" s="63">
+        <v>20</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M13&lt;10,"0",""),M13)</f>
         <v>010</v>
       </c>
-      <c r="G13" s="120" t="str">
-        <f t="shared" ref="G13:G23" si="12">G12</f>
+      <c r="H13" s="120" t="str">
+        <f>H12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H13" s="121" t="str">
-        <f t="shared" si="10"/>
+      <c r="I13" s="121" t="str">
+        <f>I12</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="I13" s="63"/>
-      <c r="J13" s="122" t="str">
+      <c r="J13" s="63"/>
+      <c r="K13" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K13" s="123" t="str">
-        <f t="shared" ref="K13:K23" si="13">K12</f>
+      <c r="L13" s="123" t="str">
+        <f>L12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L13" s="124">
-        <f t="shared" si="11"/>
+      <c r="M13" s="124">
+        <f>M12+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M14&lt;10,"0",""),M14)</f>
         <v>subject11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C14" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D14" s="63">
         <v>3</v>
       </c>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E14" s="63">
+        <v>20</v>
+      </c>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M14&lt;10,"0",""),M14)</f>
         <v>011</v>
       </c>
-      <c r="G14" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H14" s="120" t="str">
+        <f>H13</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H14" s="121" t="s">
-        <v>270</v>
-      </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="122" t="str">
+      <c r="I14" s="121" t="s">
+        <v>272</v>
+      </c>
+      <c r="J14" s="63"/>
+      <c r="K14" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K14" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L14" s="123" t="str">
+        <f>L13</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L14" s="124">
-        <f t="shared" si="11"/>
+      <c r="M14" s="124">
+        <f>M13+1</f>
         <v>11</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M15&lt;10,"0",""),M15)</f>
         <v>subject12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C15" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D15" s="63">
         <v>3</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E15" s="63">
+        <v>20</v>
+      </c>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M15&lt;10,"0",""),M15)</f>
         <v>012</v>
       </c>
-      <c r="G15" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H15" s="120" t="str">
+        <f>H14</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="H15" s="121" t="str">
-        <f t="shared" si="10"/>
+      <c r="I15" s="121" t="str">
+        <f>I14</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="122" t="str">
+      <c r="J15" s="63"/>
+      <c r="K15" s="122" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K15" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L15" s="123" t="str">
+        <f>L14</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="L15" s="124">
-        <f t="shared" si="11"/>
+      <c r="M15" s="124">
+        <f>M14+1</f>
         <v>12</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M16&lt;10,"0",""),M16)</f>
         <v>subject13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C16" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D16" s="63">
         <v>4</v>
       </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E16" s="63">
+        <v>20</v>
+      </c>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M16&lt;10,"0",""),M16)</f>
         <v>013</v>
       </c>
-      <c r="G16" s="120" t="s">
-        <v>273</v>
-      </c>
-      <c r="H16" s="121" t="str">
-        <f t="shared" si="10"/>
+      <c r="H16" s="120" t="s">
+        <v>275</v>
+      </c>
+      <c r="I16" s="121" t="str">
+        <f>I15</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I16" s="63"/>
-      <c r="J16" s="122" t="str">
+      <c r="J16" s="63"/>
+      <c r="K16" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K16" s="123" t="s">
-        <v>274</v>
-      </c>
-      <c r="L16" s="124">
-        <f t="shared" si="11"/>
+      <c r="L16" s="123" t="s">
+        <v>276</v>
+      </c>
+      <c r="M16" s="124">
+        <f>M15+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M17&lt;10,"0",""),M17)</f>
         <v>subject14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C17" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D17" s="63">
         <v>4</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E17" s="63">
+        <v>20</v>
+      </c>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M17&lt;10,"0",""),M17)</f>
         <v>014</v>
       </c>
-      <c r="G17" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H17" s="120" t="str">
+        <f>H16</f>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H17" s="121" t="str">
-        <f t="shared" si="10"/>
+      <c r="I17" s="121" t="str">
+        <f>I16</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I17" s="63"/>
-      <c r="J17" s="122" t="str">
+      <c r="J17" s="63"/>
+      <c r="K17" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K17" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L17" s="123" t="str">
+        <f>L16</f>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L17" s="124">
-        <f t="shared" si="11"/>
+      <c r="M17" s="124">
+        <f>M16+1</f>
         <v>14</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M18&lt;10,"0",""),M18)</f>
         <v>subject15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C18" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D18" s="63">
         <v>4</v>
       </c>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E18" s="63">
+        <v>20</v>
+      </c>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M18&lt;10,"0",""),M18)</f>
         <v>015</v>
       </c>
-      <c r="G18" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H18" s="120" t="str">
+        <f>H17</f>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H18" s="121" t="str">
-        <f t="shared" si="10"/>
+      <c r="I18" s="121" t="str">
+        <f>I17</f>
         <v>#C6EFCD</v>
       </c>
-      <c r="I18" s="63"/>
-      <c r="J18" s="122" t="str">
+      <c r="J18" s="63"/>
+      <c r="K18" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K18" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L18" s="123" t="str">
+        <f>L17</f>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L18" s="124">
-        <f t="shared" si="11"/>
+      <c r="M18" s="124">
+        <f>M17+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1">
       <c r="A19" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M19&lt;10,"0",""),M19)</f>
         <v>subject16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C19" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D19" s="63">
         <v>4</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E19" s="63">
+        <v>20</v>
+      </c>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M19&lt;10,"0",""),M19)</f>
         <v>016</v>
       </c>
-      <c r="G19" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H19" s="120" t="str">
+        <f>H18</f>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="H19" s="121" t="s">
-        <v>278</v>
-      </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="122" t="str">
+      <c r="I19" s="121" t="s">
+        <v>280</v>
+      </c>
+      <c r="J19" s="63"/>
+      <c r="K19" s="122" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K19" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L19" s="123" t="str">
+        <f>L18</f>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="L19" s="124">
-        <f t="shared" si="11"/>
+      <c r="M19" s="124">
+        <f>M18+1</f>
         <v>16</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M20&lt;10,"0",""),M20)</f>
         <v>subject17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C20" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D20" s="63">
         <v>5</v>
       </c>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E20" s="63">
+        <v>20</v>
+      </c>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M20&lt;10,"0",""),M20)</f>
         <v>017</v>
       </c>
-      <c r="G20" s="120" t="s">
+      <c r="H20" s="120" t="s">
+        <v>282</v>
+      </c>
+      <c r="I20" s="121" t="s">
         <v>280</v>
       </c>
-      <c r="H20" s="121" t="s">
-        <v>278</v>
-      </c>
-      <c r="I20" s="63"/>
-      <c r="J20" s="122" t="str">
+      <c r="J20" s="63"/>
+      <c r="K20" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K20" s="123" t="s">
-        <v>281</v>
-      </c>
-      <c r="L20" s="124">
-        <f t="shared" si="11"/>
+      <c r="L20" s="123" t="s">
+        <v>283</v>
+      </c>
+      <c r="M20" s="124">
+        <f>M19+1</f>
         <v>17</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
       <c r="A21" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M21&lt;10,"0",""),M21)</f>
         <v>subject18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C21" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D21" s="63">
         <v>5</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E21" s="63">
+        <v>20</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M21&lt;10,"0",""),M21)</f>
         <v>018</v>
       </c>
-      <c r="G21" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H21" s="120" t="str">
+        <f>H20</f>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H21" s="121" t="s">
-        <v>278</v>
-      </c>
-      <c r="I21" s="63"/>
-      <c r="J21" s="122" t="str">
+      <c r="I21" s="121" t="s">
+        <v>280</v>
+      </c>
+      <c r="J21" s="63"/>
+      <c r="K21" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K21" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L21" s="123" t="str">
+        <f>L20</f>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L21" s="124">
-        <f t="shared" si="11"/>
+      <c r="M21" s="124">
+        <f>M20+1</f>
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M22&lt;10,"0",""),M22)</f>
         <v>subject19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C22" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D22" s="63">
         <v>5</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E22" s="63">
+        <v>20</v>
+      </c>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M22&lt;10,"0",""),M22)</f>
         <v>019</v>
       </c>
-      <c r="G22" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H22" s="120" t="str">
+        <f>H21</f>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H22" s="121" t="s">
-        <v>278</v>
-      </c>
-      <c r="I22" s="63"/>
-      <c r="J22" s="122" t="str">
+      <c r="I22" s="121" t="s">
+        <v>280</v>
+      </c>
+      <c r="J22" s="63"/>
+      <c r="K22" s="122" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="K22" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L22" s="123" t="str">
+        <f>L21</f>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L22" s="124">
-        <f t="shared" si="11"/>
+      <c r="M22" s="124">
+        <f>M21+1</f>
         <v>19</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.CONCAT("subject",IF(M23&lt;10,"0",""),M23)</f>
         <v>subject20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C23" s="77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D23" s="63">
         <v>5</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63" t="str">
-        <f t="shared" si="8"/>
+      <c r="E23" s="63">
+        <v>20</v>
+      </c>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(M23&lt;10,"0",""),M23)</f>
         <v>020</v>
       </c>
-      <c r="G23" s="120" t="str">
-        <f t="shared" si="12"/>
+      <c r="H23" s="120" t="str">
+        <f>H22</f>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="H23" s="121" t="s">
-        <v>278</v>
-      </c>
-      <c r="I23" s="63"/>
-      <c r="J23" s="122" t="str">
+      <c r="I23" s="121" t="s">
+        <v>280</v>
+      </c>
+      <c r="J23" s="63"/>
+      <c r="K23" s="122" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="K23" s="123" t="str">
-        <f t="shared" si="13"/>
+      <c r="L23" s="123" t="str">
+        <f>L22</f>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="L23" s="124">
-        <f t="shared" si="11"/>
+      <c r="M23" s="124">
+        <f>M22+1</f>
         <v>20</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="L24" s="74"/>
+      <c r="E24" s="14"/>
+      <c r="M24" s="74"/>
     </row>
     <row r="25" ht="14.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -4697,43 +4771,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00A80097-006C-4A8E-A41D-00E400D100E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000100E4-0000-4B37-88AB-003700320026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F70036-0094-4901-86AE-004D00CF00FC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E10099-0090-4586-8327-00DD00A60003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004C000B-006C-408D-BB7B-00B900760092}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CE00D7-0061-4175-9841-00A7005C0061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E600F7-0052-4766-A6EE-00C5007A00E1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BA00D3-00E1-40A4-9C94-001F0028002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00510039-0034-4FEC-A23A-00BA003A0080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002A0033-00DF-46E1-9536-00AE0011009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004E005B-00A4-47DA-BF5D-0047009B0041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00340056-00BA-4753-BBE5-00C900DD0048}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00270010-00C3-4840-8D19-00CB001B00F5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C100C7-00BA-47B0-A952-000300EE008A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -4900,7 +4974,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00380045-00DF-40D3-ADBD-001A00A1004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DB007B-001D-4AFF-B551-000600AE00BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5346,79 +5420,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{008800EA-003A-458B-9009-0001005C0036}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00710006-0061-4141-97DB-00F60019002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AF004B-0020-42E1-BBE8-0073002E0021}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004C0030-007B-4E38-A648-004600D8001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D100C5-0034-47C7-8B73-005A009400F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006900EF-00EB-495A-9593-004C0021001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A10011-00A3-42ED-A70E-009400F10083}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D500E4-0003-4CE2-9E79-00F900B90039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>V5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000A004B-006A-4DA1-ACAE-00EF00E70004}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000900D5-0096-4887-A6B4-0052004A0095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001F00BE-00DC-4C03-880B-00B300790018}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D100A9-00FD-4992-B033-002E00A80096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C700FE-00D0-45F3-AF8C-003600620031}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001B0086-00CD-4C4E-B757-00F30097009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>R4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C00004-0084-4A29-AAA7-00FC004B00B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AA006B-0003-4837-9681-002C000C009D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003D00FC-0071-4C28-9C95-00F800EB0078}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AB0005-0026-48EB-BBC4-00AE0076004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00200021-00AF-47F5-84E6-008000B90045}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00970040-0096-4822-8C64-00A300F1003D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D4008E-0021-4D20-BE40-006D00C90085}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008B0054-00F9-479A-B4E0-00FF002E0025}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>I5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0047002F-002F-4809-B954-004F00FE00A3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CE0022-00A1-4606-8501-008A006B0001}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007E004D-0083-4EAE-BFEB-000200A4002F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0004003D-0095-4AB0-8C29-00C8009E00F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5545,19 +5619,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{006A006A-0051-42B6-AA56-007A001E00A1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AE00EC-002B-4BE1-8267-003800D700A7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009D00FD-0086-4E39-ABE7-00BB0076001C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BA0057-009B-4900-B582-00C2003800FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00670044-0060-452D-9C0A-0074003C0013}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00990098-006A-414C-9B7F-003900410061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPDATED: MVP template to include AcademicRules grades bulk
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,25 +12,26 @@
     <sheet name="users" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="f_profiles" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="families" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="ap_profiles" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="ap_programs" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="ap_subject_types" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="ap_knowledges" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="ap_subjects" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="rules" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="ar_evaluations" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ap_profiles" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ap_programs" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="ap_subject_types" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ap_knowledges" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="ap_subjects" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="SUBSTAGES_FRECUENCY" hidden="0">DB!$A$2:$A$8</definedName>
     <definedName name="BOOLEAN_ANSWER" hidden="0">DB!$A$11:$A$12</definedName>
     <definedName name="GENRE_ANSWER" hidden="0">DB!$A$15:$A$16</definedName>
     <definedName name="GUARDIANS_RELATIONSHIPS" hidden="0">DB!$A$19:$A$23</definedName>
+    <definedName name="GRADES_TYPES" hidden="0">DB!$A$26:$A$27</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -92,6 +93,15 @@
     <t>Separated</t>
   </si>
   <si>
+    <t xml:space="preserve">Grades types</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
     <t>root</t>
   </si>
   <si>
@@ -560,9 +570,42 @@
     <t xml:space="preserve">111-222-333@Mom's phone|mother</t>
   </si>
   <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>isPercentage</t>
+  </si>
+  <si>
+    <t>scales</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is percentage?</t>
+  </si>
+  <si>
+    <t>Scales</t>
+  </si>
+  <si>
+    <t>gradeA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESO grades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN|1|Insuficiente, IN|2|Insuficiente, IN|3|Insuficiente, IN|4|Insuficiente, SU|5|Suficiente, BI|6|Bien, NT|7|Notable, NT|8|Notable, SB|9|Sobresaliente, SB|10|Sobresaliente</t>
+  </si>
+  <si>
     <t>abbreviation</t>
   </si>
   <si>
+    <t>evaluationSystem</t>
+  </si>
+  <si>
     <t>creditSystem</t>
   </si>
   <si>
@@ -636,6 +679,9 @@
   </si>
   <si>
     <t>Acronym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluation system</t>
   </si>
   <si>
     <t xml:space="preserve">Use credit system?</t>
@@ -1425,7 +1471,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="131">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1612,6 +1658,9 @@
     <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1667,6 +1716,21 @@
     <xf fontId="0" fillId="17" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf fontId="4" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="16" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="7" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1706,6 +1770,9 @@
     <xf fontId="4" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="4" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="12" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1752,12 +1819,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="4" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="4" fillId="16" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="4" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2419,7 +2480,21 @@
       </c>
     </row>
     <row r="24" ht="14.25"/>
-    <row r="25" ht="14.25"/>
+    <row r="25" ht="14.25">
+      <c r="A25" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -2442,6 +2517,145 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col customWidth="1" min="3" max="3" width="11.421875"/>
+    <col customWidth="1" min="4" max="4" width="10.421875"/>
+    <col customWidth="1" min="5" max="5" width="12.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" ht="28.5">
+      <c r="A2" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="117" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="117" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="79" t="str">
+        <f>ap_programs!$A$4</f>
+        <v>programA</v>
+      </c>
+      <c r="D3" s="64">
+        <v>0</v>
+      </c>
+      <c r="E3" s="64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="79" t="str">
+        <f>ap_programs!$A$5</f>
+        <v>programB</v>
+      </c>
+      <c r="D4" s="64">
+        <v>0</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" s="79" t="str">
+        <f>ap_programs!$A$4</f>
+        <v>programA</v>
+      </c>
+      <c r="D5" s="64">
+        <v>0</v>
+      </c>
+      <c r="E5" s="64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
+        <x14:dataValidation xr:uid="{00AB004C-00BF-43AF-B98C-00E10079001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E5002D-005B-480B-97F8-006D0087001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000A001C-0093-46FB-95E9-005C002D0087}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="0"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
     <col customWidth="1" min="1" max="1" width="14.57421875"/>
     <col customWidth="1" min="3" max="3" width="10.8515625"/>
     <col customWidth="1" min="5" max="5" width="13.8515625"/>
@@ -2450,67 +2664,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="112" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="112" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="112" t="s">
-        <v>235</v>
-      </c>
-      <c r="E2" s="112" t="s">
-        <v>236</v>
-      </c>
-      <c r="F2" s="113" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2" s="114" t="s">
-        <v>203</v>
+      <c r="A2" s="118" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="84" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2" s="85" t="s">
+        <v>241</v>
+      </c>
+      <c r="G2" s="119" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="E3" s="115" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="78" t="str">
+        <v>255</v>
+      </c>
+      <c r="E3" s="120" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" s="79" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -2520,21 +2734,21 @@
     </row>
     <row r="4" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="E4" s="70" t="s">
-        <v>246</v>
-      </c>
-      <c r="F4" s="78" t="str">
+        <v>260</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>261</v>
+      </c>
+      <c r="F4" s="79" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -2554,7 +2768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0"/>
@@ -2583,42 +2797,42 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>233</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="L1" s="116" t="s">
-        <v>253</v>
-      </c>
-      <c r="M1" s="75"/>
+        <v>267</v>
+      </c>
+      <c r="L1" s="121" t="s">
+        <v>268</v>
+      </c>
+      <c r="M1" s="76"/>
     </row>
     <row r="2" ht="28.850000000000001" customHeight="1">
       <c r="A2" s="5"/>
@@ -2629,52 +2843,52 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="1" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="75"/>
+      <c r="M2" s="76"/>
     </row>
     <row r="3" ht="31.850000000000001" customHeight="1">
-      <c r="A3" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="112" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="95" t="s">
-        <v>226</v>
-      </c>
-      <c r="D3" s="94" t="s">
-        <v>255</v>
-      </c>
-      <c r="E3" s="112" t="s">
-        <v>256</v>
-      </c>
-      <c r="F3" s="94" t="s">
-        <v>257</v>
-      </c>
-      <c r="G3" s="94" t="s">
-        <v>258</v>
-      </c>
-      <c r="H3" s="117" t="s">
-        <v>259</v>
-      </c>
-      <c r="I3" s="118" t="s">
-        <v>235</v>
-      </c>
-      <c r="J3" s="118" t="s">
-        <v>260</v>
-      </c>
-      <c r="K3" s="119" t="s">
-        <v>261</v>
-      </c>
-      <c r="L3" s="113" t="s">
-        <v>262</v>
-      </c>
-      <c r="M3" s="120"/>
+      <c r="A3" s="118" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="101" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="100" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="100" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" s="100" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="122" t="s">
+        <v>274</v>
+      </c>
+      <c r="I3" s="123" t="s">
+        <v>250</v>
+      </c>
+      <c r="J3" s="123" t="s">
+        <v>275</v>
+      </c>
+      <c r="K3" s="124" t="s">
+        <v>276</v>
+      </c>
+      <c r="L3" s="85" t="s">
+        <v>277</v>
+      </c>
+      <c r="M3" s="125"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
@@ -2682,9 +2896,9 @@
         <v>subject01</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="78" t="str">
+        <v>278</v>
+      </c>
+      <c r="C4" s="79" t="str">
         <f>ap_programs!A4</f>
         <v>programA</v>
       </c>
@@ -2699,21 +2913,21 @@
         <f t="shared" ref="G4:G9" si="1">_xlfn.CONCAT("0",IF(M4&lt;10,"0",""),M4)</f>
         <v>001</v>
       </c>
-      <c r="H4" s="121" t="s">
-        <v>264</v>
-      </c>
-      <c r="I4" s="122" t="s">
-        <v>265</v>
+      <c r="H4" s="126" t="s">
+        <v>279</v>
+      </c>
+      <c r="I4" s="127" t="s">
+        <v>280</v>
       </c>
       <c r="J4" s="64"/>
-      <c r="K4" s="123" t="str">
+      <c r="K4" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L4" s="124" t="s">
-        <v>266</v>
-      </c>
-      <c r="M4" s="125">
+      <c r="L4" s="129" t="s">
+        <v>281</v>
+      </c>
+      <c r="M4" s="130">
         <v>1</v>
       </c>
       <c r="N4" s="9"/>
@@ -2724,9 +2938,9 @@
         <v>subject02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="C5" s="78" t="str">
+        <v>282</v>
+      </c>
+      <c r="C5" s="79" t="str">
         <f t="shared" ref="C5:C10" si="2">C4</f>
         <v>programA</v>
       </c>
@@ -2741,24 +2955,24 @@
         <f t="shared" si="1"/>
         <v>002</v>
       </c>
-      <c r="H5" s="121" t="str">
+      <c r="H5" s="126" t="str">
         <f t="shared" ref="H5:H10" si="3">H4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I5" s="122" t="str">
+      <c r="I5" s="127" t="str">
         <f t="shared" ref="I5:I10" si="4">I4</f>
         <v>#FFEB9C</v>
       </c>
       <c r="J5" s="64"/>
-      <c r="K5" s="123" t="str">
+      <c r="K5" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L5" s="124" t="str">
+      <c r="L5" s="129" t="str">
         <f t="shared" ref="L5:L10" si="5">L4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M5" s="125">
+      <c r="M5" s="130">
         <f t="shared" ref="M5:M10" si="6">M4+1</f>
         <v>2</v>
       </c>
@@ -2770,9 +2984,9 @@
         <v>subject03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="C6" s="78" t="str">
+        <v>283</v>
+      </c>
+      <c r="C6" s="79" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
@@ -2787,24 +3001,24 @@
         <f t="shared" si="1"/>
         <v>003</v>
       </c>
-      <c r="H6" s="121" t="str">
+      <c r="H6" s="126" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I6" s="122" t="str">
+      <c r="I6" s="127" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
       <c r="J6" s="64"/>
-      <c r="K6" s="123" t="str">
+      <c r="K6" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L6" s="124" t="str">
+      <c r="L6" s="129" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M6" s="125">
+      <c r="M6" s="130">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -2816,9 +3030,9 @@
         <v>subject04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C7" s="78" t="str">
+        <v>284</v>
+      </c>
+      <c r="C7" s="79" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
@@ -2833,24 +3047,24 @@
         <f t="shared" si="1"/>
         <v>004</v>
       </c>
-      <c r="H7" s="121" t="str">
+      <c r="H7" s="126" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I7" s="122" t="str">
+      <c r="I7" s="127" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
       <c r="J7" s="64"/>
-      <c r="K7" s="123" t="str">
+      <c r="K7" s="128" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L7" s="124" t="str">
+      <c r="L7" s="129" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M7" s="125">
+      <c r="M7" s="130">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -2862,9 +3076,9 @@
         <v>subject05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C8" s="78" t="str">
+        <v>285</v>
+      </c>
+      <c r="C8" s="79" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
@@ -2879,22 +3093,22 @@
         <f t="shared" si="1"/>
         <v>005</v>
       </c>
-      <c r="H8" s="121" t="s">
-        <v>271</v>
-      </c>
-      <c r="I8" s="122" t="str">
+      <c r="H8" s="126" t="s">
+        <v>286</v>
+      </c>
+      <c r="I8" s="127" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
       <c r="J8" s="64"/>
-      <c r="K8" s="123" t="str">
+      <c r="K8" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L8" s="124" t="s">
-        <v>272</v>
-      </c>
-      <c r="M8" s="125">
+      <c r="L8" s="129" t="s">
+        <v>287</v>
+      </c>
+      <c r="M8" s="130">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -2905,9 +3119,9 @@
         <v>subject06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="78" t="str">
+        <v>288</v>
+      </c>
+      <c r="C9" s="79" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
@@ -2922,23 +3136,23 @@
         <f t="shared" si="1"/>
         <v>006</v>
       </c>
-      <c r="H9" s="121" t="str">
+      <c r="H9" s="126" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I9" s="122" t="s">
-        <v>274</v>
+      <c r="I9" s="127" t="s">
+        <v>289</v>
       </c>
       <c r="J9" s="64"/>
-      <c r="K9" s="123" t="str">
+      <c r="K9" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L9" s="124" t="str">
+      <c r="L9" s="129" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M9" s="125">
+      <c r="M9" s="130">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -2949,9 +3163,9 @@
         <v>subject07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="C10" s="78" t="str">
+        <v>290</v>
+      </c>
+      <c r="C10" s="79" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
@@ -2966,24 +3180,24 @@
         <f t="shared" ref="G10:G23" si="8">_xlfn.CONCAT("0",IF(M10&lt;10,"0",""),M10)</f>
         <v>007</v>
       </c>
-      <c r="H10" s="121" t="str">
+      <c r="H10" s="126" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I10" s="122" t="str">
+      <c r="I10" s="127" t="str">
         <f t="shared" si="4"/>
         <v>#FFC7CE</v>
       </c>
       <c r="J10" s="64"/>
-      <c r="K10" s="123" t="str">
+      <c r="K10" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L10" s="124" t="str">
+      <c r="L10" s="129" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M10" s="125">
+      <c r="M10" s="130">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
@@ -2994,9 +3208,9 @@
         <v>subject08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="C11" s="78" t="str">
+        <v>291</v>
+      </c>
+      <c r="C11" s="79" t="str">
         <f t="shared" ref="C11:C23" si="9">C10</f>
         <v>programA</v>
       </c>
@@ -3011,24 +3225,24 @@
         <f t="shared" si="8"/>
         <v>008</v>
       </c>
-      <c r="H11" s="121" t="str">
+      <c r="H11" s="126" t="str">
         <f>H10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I11" s="122" t="str">
+      <c r="I11" s="127" t="str">
         <f t="shared" ref="I11:I18" si="10">I10</f>
         <v>#FFC7CE</v>
       </c>
       <c r="J11" s="64"/>
-      <c r="K11" s="123" t="str">
+      <c r="K11" s="128" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L11" s="124" t="str">
+      <c r="L11" s="129" t="str">
         <f>L10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M11" s="125">
+      <c r="M11" s="130">
         <f t="shared" ref="M11:M23" si="11">M10+1</f>
         <v>8</v>
       </c>
@@ -3039,9 +3253,9 @@
         <v>subject09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="C12" s="78" t="str">
+        <v>292</v>
+      </c>
+      <c r="C12" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3056,22 +3270,22 @@
         <f t="shared" si="8"/>
         <v>009</v>
       </c>
-      <c r="H12" s="121" t="s">
-        <v>278</v>
-      </c>
-      <c r="I12" s="122" t="str">
+      <c r="H12" s="126" t="s">
+        <v>293</v>
+      </c>
+      <c r="I12" s="127" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
       <c r="J12" s="64"/>
-      <c r="K12" s="123" t="str">
+      <c r="K12" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L12" s="124" t="s">
-        <v>279</v>
-      </c>
-      <c r="M12" s="125">
+      <c r="L12" s="129" t="s">
+        <v>294</v>
+      </c>
+      <c r="M12" s="130">
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
@@ -3082,9 +3296,9 @@
         <v>subject10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="C13" s="78" t="str">
+        <v>295</v>
+      </c>
+      <c r="C13" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3099,24 +3313,24 @@
         <f t="shared" si="8"/>
         <v>010</v>
       </c>
-      <c r="H13" s="121" t="str">
+      <c r="H13" s="126" t="str">
         <f t="shared" ref="H13:H23" si="12">H12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I13" s="122" t="str">
+      <c r="I13" s="127" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
       <c r="J13" s="64"/>
-      <c r="K13" s="123" t="str">
+      <c r="K13" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L13" s="124" t="str">
+      <c r="L13" s="129" t="str">
         <f t="shared" ref="L13:L23" si="13">L12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M13" s="125">
+      <c r="M13" s="130">
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
@@ -3127,9 +3341,9 @@
         <v>subject11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="C14" s="78" t="str">
+        <v>296</v>
+      </c>
+      <c r="C14" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3144,23 +3358,23 @@
         <f t="shared" si="8"/>
         <v>011</v>
       </c>
-      <c r="H14" s="121" t="str">
+      <c r="H14" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I14" s="122" t="s">
-        <v>282</v>
+      <c r="I14" s="127" t="s">
+        <v>297</v>
       </c>
       <c r="J14" s="64"/>
-      <c r="K14" s="123" t="str">
+      <c r="K14" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L14" s="124" t="str">
+      <c r="L14" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M14" s="125">
+      <c r="M14" s="130">
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
@@ -3171,9 +3385,9 @@
         <v>subject12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="C15" s="78" t="str">
+        <v>298</v>
+      </c>
+      <c r="C15" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3188,24 +3402,24 @@
         <f t="shared" si="8"/>
         <v>012</v>
       </c>
-      <c r="H15" s="121" t="str">
+      <c r="H15" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I15" s="122" t="str">
+      <c r="I15" s="127" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J15" s="64"/>
-      <c r="K15" s="123" t="str">
+      <c r="K15" s="128" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L15" s="124" t="str">
+      <c r="L15" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M15" s="125">
+      <c r="M15" s="130">
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
@@ -3216,9 +3430,9 @@
         <v>subject13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="C16" s="78" t="str">
+        <v>299</v>
+      </c>
+      <c r="C16" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3233,22 +3447,22 @@
         <f t="shared" si="8"/>
         <v>013</v>
       </c>
-      <c r="H16" s="121" t="s">
-        <v>285</v>
-      </c>
-      <c r="I16" s="122" t="str">
+      <c r="H16" s="126" t="s">
+        <v>300</v>
+      </c>
+      <c r="I16" s="127" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J16" s="64"/>
-      <c r="K16" s="123" t="str">
+      <c r="K16" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L16" s="124" t="s">
-        <v>286</v>
-      </c>
-      <c r="M16" s="125">
+      <c r="L16" s="129" t="s">
+        <v>301</v>
+      </c>
+      <c r="M16" s="130">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
@@ -3259,9 +3473,9 @@
         <v>subject14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="C17" s="78" t="str">
+        <v>302</v>
+      </c>
+      <c r="C17" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3276,24 +3490,24 @@
         <f t="shared" si="8"/>
         <v>014</v>
       </c>
-      <c r="H17" s="121" t="str">
+      <c r="H17" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I17" s="122" t="str">
+      <c r="I17" s="127" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J17" s="64"/>
-      <c r="K17" s="123" t="str">
+      <c r="K17" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L17" s="124" t="str">
+      <c r="L17" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M17" s="125">
+      <c r="M17" s="130">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
@@ -3304,9 +3518,9 @@
         <v>subject15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="C18" s="78" t="str">
+        <v>303</v>
+      </c>
+      <c r="C18" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3321,24 +3535,24 @@
         <f t="shared" si="8"/>
         <v>015</v>
       </c>
-      <c r="H18" s="121" t="str">
+      <c r="H18" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I18" s="122" t="str">
+      <c r="I18" s="127" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J18" s="64"/>
-      <c r="K18" s="123" t="str">
+      <c r="K18" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L18" s="124" t="str">
+      <c r="L18" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M18" s="125">
+      <c r="M18" s="130">
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
@@ -3349,9 +3563,9 @@
         <v>subject16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="C19" s="78" t="str">
+        <v>304</v>
+      </c>
+      <c r="C19" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3366,23 +3580,23 @@
         <f t="shared" si="8"/>
         <v>016</v>
       </c>
-      <c r="H19" s="121" t="str">
+      <c r="H19" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I19" s="122" t="s">
-        <v>290</v>
+      <c r="I19" s="127" t="s">
+        <v>305</v>
       </c>
       <c r="J19" s="64"/>
-      <c r="K19" s="123" t="str">
+      <c r="K19" s="128" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L19" s="124" t="str">
+      <c r="L19" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M19" s="125">
+      <c r="M19" s="130">
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
@@ -3393,9 +3607,9 @@
         <v>subject17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="C20" s="78" t="str">
+        <v>306</v>
+      </c>
+      <c r="C20" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3410,21 +3624,21 @@
         <f t="shared" si="8"/>
         <v>017</v>
       </c>
-      <c r="H20" s="121" t="s">
-        <v>292</v>
-      </c>
-      <c r="I20" s="122" t="s">
-        <v>290</v>
+      <c r="H20" s="126" t="s">
+        <v>307</v>
+      </c>
+      <c r="I20" s="127" t="s">
+        <v>305</v>
       </c>
       <c r="J20" s="64"/>
-      <c r="K20" s="123" t="str">
+      <c r="K20" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L20" s="124" t="s">
-        <v>293</v>
-      </c>
-      <c r="M20" s="125">
+      <c r="L20" s="129" t="s">
+        <v>308</v>
+      </c>
+      <c r="M20" s="130">
         <f t="shared" si="11"/>
         <v>17</v>
       </c>
@@ -3435,9 +3649,9 @@
         <v>subject18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="C21" s="78" t="str">
+        <v>309</v>
+      </c>
+      <c r="C21" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3452,23 +3666,23 @@
         <f t="shared" si="8"/>
         <v>018</v>
       </c>
-      <c r="H21" s="121" t="str">
+      <c r="H21" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I21" s="122" t="s">
-        <v>290</v>
+      <c r="I21" s="127" t="s">
+        <v>305</v>
       </c>
       <c r="J21" s="64"/>
-      <c r="K21" s="123" t="str">
+      <c r="K21" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L21" s="124" t="str">
+      <c r="L21" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M21" s="125">
+      <c r="M21" s="130">
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
@@ -3479,9 +3693,9 @@
         <v>subject19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="C22" s="78" t="str">
+        <v>310</v>
+      </c>
+      <c r="C22" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3496,23 +3710,23 @@
         <f t="shared" si="8"/>
         <v>019</v>
       </c>
-      <c r="H22" s="121" t="str">
+      <c r="H22" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I22" s="122" t="s">
-        <v>290</v>
+      <c r="I22" s="127" t="s">
+        <v>305</v>
       </c>
       <c r="J22" s="64"/>
-      <c r="K22" s="123" t="str">
+      <c r="K22" s="128" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L22" s="124" t="str">
+      <c r="L22" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M22" s="125">
+      <c r="M22" s="130">
         <f t="shared" si="11"/>
         <v>19</v>
       </c>
@@ -3523,9 +3737,9 @@
         <v>subject20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="C23" s="78" t="str">
+        <v>311</v>
+      </c>
+      <c r="C23" s="79" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
@@ -3540,52 +3754,36 @@
         <f t="shared" si="8"/>
         <v>020</v>
       </c>
-      <c r="H23" s="121" t="str">
+      <c r="H23" s="126" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I23" s="122" t="s">
-        <v>290</v>
+      <c r="I23" s="127" t="s">
+        <v>305</v>
       </c>
       <c r="J23" s="64"/>
-      <c r="K23" s="123" t="str">
+      <c r="K23" s="128" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L23" s="124" t="str">
+      <c r="L23" s="129" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M23" s="125">
+      <c r="M23" s="130">
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" ht="14.25">
       <c r="E24" s="15"/>
-      <c r="M24" s="75"/>
+      <c r="M24" s="76"/>
     </row>
     <row r="25" ht="14.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H2:L2"/>
   </mergeCells>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -3613,58 +3811,58 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3710,16 +3908,16 @@
   <sheetData>
     <row r="1" s="12" customFormat="1" ht="14.25">
       <c r="A1" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E1" s="12" t="str">
         <f>_xlfn.CONCAT($E$3,".",E5)</f>
@@ -3844,7 +4042,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -3880,26 +4078,26 @@
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="18" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
       <c r="P3" s="22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="23"/>
       <c r="R3" s="23"/>
@@ -3907,23 +4105,23 @@
       <c r="T3" s="23"/>
       <c r="U3" s="24"/>
       <c r="V3" s="16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="W3" s="17"/>
       <c r="X3" s="25" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
       <c r="AA3" s="26"/>
       <c r="AB3" s="27" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AC3" s="20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AD3" s="22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AE3" s="23"/>
       <c r="AF3" s="23"/>
@@ -3934,26 +4132,26 @@
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L4" s="34"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
       <c r="O4" s="34"/>
       <c r="P4" s="35" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="36"/>
       <c r="R4" s="36"/>
@@ -3961,23 +4159,23 @@
       <c r="T4" s="36"/>
       <c r="U4" s="37"/>
       <c r="V4" s="29" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="W4" s="30"/>
       <c r="X4" s="31" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Y4" s="38"/>
       <c r="Z4" s="38"/>
       <c r="AA4" s="38"/>
       <c r="AB4" s="32" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AC4" s="33" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AD4" s="35" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AE4" s="36"/>
       <c r="AF4" s="36"/>
@@ -3988,529 +4186,529 @@
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="E5" s="39" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I5" s="42" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J5" s="43" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K5" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="45" t="s">
-        <v>60</v>
-      </c>
       <c r="N5" s="45" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O5" s="45" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="P5" s="46" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="47" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R5" s="47" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="S5" s="47" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="T5" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="U5" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="V5" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="U5" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="V5" s="39" t="s">
-        <v>68</v>
-      </c>
       <c r="W5" s="40" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="X5" s="42" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Y5" s="42" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Z5" s="42" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AA5" s="42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AB5" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC5" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="AC5" s="49" t="s">
-        <v>75</v>
-      </c>
       <c r="AD5" s="46" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AE5" s="47" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AF5" s="47" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AG5" s="47" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" s="50" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I6" s="54" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K6" s="56" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L6" s="57" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M6" s="57" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N6" s="57" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O6" s="57" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="P6" s="58" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="59" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="R6" s="59" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="S6" s="59" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="T6" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="U6" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="V6" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="U6" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="V6" s="52" t="s">
-        <v>91</v>
-      </c>
       <c r="W6" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="X6" s="54" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Y6" s="54" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Z6" s="54" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="AA6" s="54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AB6" s="61" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AC6" s="62" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AD6" s="58" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="AE6" s="59" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AF6" s="59" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AG6" s="59" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D7" s="63"/>
       <c r="E7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="J7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="N7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="P7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Q7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="R7" s="65"/>
       <c r="S7" s="65"/>
       <c r="T7" s="65"/>
       <c r="U7" s="65"/>
       <c r="V7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="W7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="X7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Y7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Z7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AA7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AB7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AC7" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AD7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AE7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AF7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AG7" s="65" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D8" s="63"/>
       <c r="E8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G8" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H8" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I8" s="64" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M8" s="64"/>
       <c r="N8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="P8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Q8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="R8" s="65"/>
       <c r="S8" s="64"/>
       <c r="T8" s="64"/>
       <c r="U8" s="64"/>
       <c r="V8" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="W8" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="X8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Y8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Z8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AA8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AB8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AC8" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AD8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AE8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AF8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AG8" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D9" s="63"/>
       <c r="E9" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F9" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I9" s="64" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J9" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="L9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M9" s="64"/>
       <c r="N9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O9" s="64"/>
       <c r="P9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="Q9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="R9" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="S9" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="T9" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="U9" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="W9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="X9" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Y9" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="Z9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AA9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AB9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AC9" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="AD9" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE9" s="64" t="s">
-        <v>103</v>
+        <v>114</v>
+      </c>
+      <c r="AD9" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE9" s="66" t="s">
+        <v>112</v>
       </c>
       <c r="AF9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AG9" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D10" s="63" t="str">
         <f>A9</f>
         <v>student</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G10" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H10" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I10" s="64" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K10" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="L10" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M10" s="64"/>
       <c r="N10" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O10" s="64"/>
       <c r="P10" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="Q10" s="64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="R10" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="S10" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="T10" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="U10" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V10" s="64"/>
       <c r="W10" s="64"/>
@@ -4520,7 +4718,7 @@
       <c r="AA10" s="64"/>
       <c r="AB10" s="64"/>
       <c r="AC10" s="64" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AD10" s="64"/>
       <c r="AE10" s="64"/>
@@ -4578,315 +4776,315 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="68" t="s">
-        <v>86</v>
+        <v>131</v>
+      </c>
+      <c r="H2" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="69" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="69">
+      <c r="E3" s="70">
         <v>36526</v>
       </c>
-      <c r="F3" s="70" t="s">
-        <v>133</v>
+      <c r="F3" s="71" t="s">
+        <v>136</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H3" s="64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I3" s="64" t="s">
-        <v>135</v>
-      </c>
-      <c r="J3" s="71" t="s">
-        <v>136</v>
+        <v>138</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="69">
+      <c r="E4" s="70">
         <v>34781</v>
       </c>
-      <c r="F4" s="70" t="s">
-        <v>139</v>
+      <c r="F4" s="71" t="s">
+        <v>142</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H4" s="64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>140</v>
-      </c>
-      <c r="J4" s="71" t="s">
-        <v>141</v>
+        <v>143</v>
+      </c>
+      <c r="J4" s="72" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>113</v>
+      <c r="A5" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>116</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="69">
+      <c r="E5" s="70">
         <v>39205</v>
       </c>
-      <c r="F5" s="74" t="s">
-        <v>144</v>
+      <c r="F5" s="75" t="s">
+        <v>147</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H5" s="64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I5" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="71" t="s">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="J5" s="72" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="72" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="73" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>149</v>
+      <c r="A6" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>152</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="69">
+      <c r="E6" s="70">
         <v>39156</v>
       </c>
-      <c r="F6" s="74" t="s">
-        <v>150</v>
+      <c r="F6" s="75" t="s">
+        <v>153</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H6" s="64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I6" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="J6" s="71" t="s">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="J6" s="72" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="72" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>113</v>
+      <c r="A7" s="73" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>116</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="69">
+      <c r="E7" s="70">
         <v>42171</v>
       </c>
-      <c r="F7" s="74" t="s">
-        <v>153</v>
+      <c r="F7" s="75" t="s">
+        <v>156</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H7" s="64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I7" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="J7" s="71" t="s">
-        <v>154</v>
+        <v>148</v>
+      </c>
+      <c r="J7" s="72" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>149</v>
+      <c r="A8" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>152</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="69">
+      <c r="E8" s="70">
         <v>42237</v>
       </c>
-      <c r="F8" s="74" t="s">
+      <c r="F8" s="75" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="64" t="s">
+        <v>148</v>
+      </c>
+      <c r="J8" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="J8" s="71" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>160</v>
+      <c r="A9" s="73" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>163</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="70">
         <v>27791</v>
       </c>
-      <c r="F9" s="74" t="s">
-        <v>161</v>
+      <c r="F9" s="75" t="s">
+        <v>164</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H9" s="64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I9" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="J9" s="71" t="s">
-        <v>163</v>
+        <v>165</v>
+      </c>
+      <c r="J9" s="72" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="75"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="76"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4903,43 +5101,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E20068-00EA-466A-8C14-005A0072003E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D7007E-0067-4AB0-8225-00C700A6002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DC0091-008E-443F-8A0B-00E400FF0030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A40063-0041-47C3-957C-003C00440058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F500AE-0033-491F-AAFF-00B70011004D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0096007B-00E4-4252-A1A7-007D008A00F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00380058-0023-45F5-92E1-004600B80070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00430052-0091-467A-A294-000E0087009C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00370022-0032-48A4-B475-00AE000E0065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0088006F-00C4-4D02-B029-00D700C70094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004E0096-0057-4D3A-930F-002E0018003A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B000CC-002A-4C58-921B-00FD00820020}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004C0034-0067-4D3A-9301-009E00D900F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009900DF-00DE-4202-BAD0-0038001C00D6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -4971,25 +5169,25 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="77" t="s">
-        <v>165</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="78" t="str">
+        <v>118</v>
+      </c>
+      <c r="B3" s="79" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
@@ -5001,9 +5199,9 @@
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="78" t="str">
+        <v>115</v>
+      </c>
+      <c r="B4" s="79" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -5048,53 +5246,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" ht="24.350000000000001" customHeight="1">
-      <c r="A2" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="81" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" s="68" t="s">
-        <v>171</v>
+      <c r="A2" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="78" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="69" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" s="82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="78" t="s">
-        <v>175</v>
+      <c r="E3" s="79" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4"/>
@@ -5106,7 +5304,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00F300FA-0092-4F71-8A30-003E00610031}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BB001D-008E-4D60-88A0-00F8005700ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5119,6 +5317,113 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFB472C4"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="18.7109375"/>
+    <col customWidth="1" min="5" max="5" width="13.7109375"/>
+    <col customWidth="1" min="6" max="6" width="19.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="85" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="84" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" ht="146.25" customHeight="1">
+      <c r="A3" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="79" t="str">
+        <f>centers!$A$3</f>
+        <v>centerA</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
+        <x14:dataValidation xr:uid="{00C800DB-00EC-413B-B7D0-007500A900F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>GRADES_TYPES</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D900DF-00C5-4890-A1FF-00E000E300D4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0"/>
@@ -5137,34 +5442,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="81" t="s">
-        <v>165</v>
+      <c r="A2" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="82" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="78" t="str">
+        <v>109</v>
+      </c>
+      <c r="B3" s="79" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="78" t="str">
+        <v>115</v>
+      </c>
+      <c r="B4" s="79" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -5177,7 +5482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0"/>
@@ -5195,95 +5500,97 @@
     <col customWidth="1" min="1" max="1" width="11.00390625"/>
     <col customWidth="1" min="2" max="2" width="19.140625"/>
     <col customWidth="1" min="3" max="3" width="12.00390625"/>
-    <col customWidth="1" min="5" max="5" width="11.140625"/>
-    <col customWidth="1" min="6" max="6" width="9.57421875"/>
-    <col customWidth="1" min="7" max="7" width="9.00390625"/>
-    <col customWidth="1" min="8" max="8" width="11.8515625"/>
-    <col customWidth="1" min="9" max="10" width="17.00390625"/>
-    <col customWidth="1" min="11" max="11" width="12.421875"/>
-    <col customWidth="1" min="12" max="12" width="12.140625"/>
-    <col customWidth="1" min="13" max="13" width="17.00390625"/>
-    <col customWidth="1" min="14" max="14" width="14.8515625"/>
-    <col customWidth="1" min="15" max="15" width="13.00390625"/>
-    <col customWidth="1" min="16" max="18" width="14.7109375"/>
-    <col customWidth="1" min="19" max="19" width="15.8515625"/>
-    <col customWidth="1" min="20" max="20" width="15.28125"/>
-    <col customWidth="1" min="21" max="21" width="12.8515625"/>
-    <col customWidth="1" min="22" max="22" width="14.140625"/>
-    <col customWidth="1" min="23" max="23" width="18.140625"/>
+    <col customWidth="1" min="5" max="6" width="11.140625"/>
+    <col customWidth="1" min="7" max="7" width="9.57421875"/>
+    <col customWidth="1" min="8" max="8" width="9.00390625"/>
+    <col customWidth="1" min="9" max="9" width="11.8515625"/>
+    <col customWidth="1" min="10" max="11" width="17.00390625"/>
+    <col customWidth="1" min="12" max="12" width="12.421875"/>
+    <col customWidth="1" min="13" max="13" width="12.140625"/>
+    <col customWidth="1" min="14" max="14" width="17.00390625"/>
+    <col customWidth="1" min="15" max="15" width="14.8515625"/>
+    <col customWidth="1" min="16" max="16" width="13.00390625"/>
+    <col customWidth="1" min="17" max="19" width="14.7109375"/>
+    <col customWidth="1" min="20" max="20" width="15.8515625"/>
+    <col customWidth="1" min="21" max="21" width="15.28125"/>
+    <col customWidth="1" min="22" max="22" width="12.8515625"/>
+    <col customWidth="1" min="23" max="23" width="14.140625"/>
+    <col customWidth="1" min="24" max="24" width="18.140625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="X1" s="5"/>
+        <v>208</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>209</v>
+      </c>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
@@ -5299,221 +5606,230 @@
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
       <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
     </row>
     <row r="2" s="9" customFormat="1" ht="23.600000000000001" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
-      <c r="E2" s="83" t="s">
-        <v>196</v>
-      </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="84" t="s">
-        <v>197</v>
-      </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="87" t="s">
-        <v>198</v>
-      </c>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="88" t="s">
-        <v>199</v>
-      </c>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="91" t="s">
-        <v>200</v>
-      </c>
-      <c r="V2" s="92"/>
-      <c r="W2" s="92"/>
+      <c r="F2" s="89" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" s="89"/>
+      <c r="H2" s="90" t="s">
+        <v>211</v>
+      </c>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="93" t="s">
+        <v>212</v>
+      </c>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="94" t="s">
+        <v>213</v>
+      </c>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="97" t="s">
+        <v>214</v>
+      </c>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
     </row>
     <row r="3" ht="34.100000000000001" customHeight="1">
-      <c r="A3" s="93" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="94" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="94" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="95" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="96" t="s">
-        <v>202</v>
-      </c>
-      <c r="F3" s="97" t="s">
-        <v>203</v>
-      </c>
-      <c r="G3" s="98" t="s">
-        <v>204</v>
-      </c>
-      <c r="H3" s="99" t="s">
-        <v>205</v>
-      </c>
-      <c r="I3" s="100" t="s">
-        <v>206</v>
-      </c>
-      <c r="J3" s="100" t="s">
-        <v>207</v>
-      </c>
-      <c r="K3" s="100" t="s">
-        <v>208</v>
-      </c>
-      <c r="L3" s="100" t="s">
-        <v>209</v>
-      </c>
-      <c r="M3" s="100" t="s">
-        <v>210</v>
-      </c>
-      <c r="N3" s="101" t="s">
-        <v>211</v>
-      </c>
-      <c r="O3" s="102" t="s">
-        <v>209</v>
-      </c>
-      <c r="P3" s="103" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q3" s="104" t="s">
-        <v>212</v>
-      </c>
-      <c r="R3" s="105" t="s">
-        <v>213</v>
-      </c>
-      <c r="S3" s="105" t="s">
-        <v>209</v>
-      </c>
-      <c r="T3" s="105" t="s">
-        <v>210</v>
-      </c>
-      <c r="U3" s="106" t="s">
-        <v>209</v>
-      </c>
-      <c r="V3" s="107" t="s">
-        <v>214</v>
-      </c>
-      <c r="W3" s="108" t="s">
+      <c r="A3" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="100" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="100" t="s">
         <v>215</v>
+      </c>
+      <c r="D3" s="101" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="102" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" s="103" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="104" t="s">
+        <v>218</v>
+      </c>
+      <c r="H3" s="105" t="s">
+        <v>219</v>
+      </c>
+      <c r="I3" s="106" t="s">
+        <v>220</v>
+      </c>
+      <c r="J3" s="107" t="s">
+        <v>221</v>
+      </c>
+      <c r="K3" s="107" t="s">
+        <v>222</v>
+      </c>
+      <c r="L3" s="107" t="s">
+        <v>223</v>
+      </c>
+      <c r="M3" s="107" t="s">
+        <v>224</v>
+      </c>
+      <c r="N3" s="107" t="s">
+        <v>225</v>
+      </c>
+      <c r="O3" s="108" t="s">
+        <v>226</v>
+      </c>
+      <c r="P3" s="109" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q3" s="110" t="s">
+        <v>225</v>
+      </c>
+      <c r="R3" s="111" t="s">
+        <v>227</v>
+      </c>
+      <c r="S3" s="112" t="s">
+        <v>228</v>
+      </c>
+      <c r="T3" s="112" t="s">
+        <v>224</v>
+      </c>
+      <c r="U3" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="V3" s="113" t="s">
+        <v>224</v>
+      </c>
+      <c r="W3" s="114" t="s">
+        <v>229</v>
+      </c>
+      <c r="X3" s="115" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D4" s="78" t="str">
+        <v>233</v>
+      </c>
+      <c r="D4" s="63" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="63" t="str">
+        <f>ar_evaluations!A3</f>
+        <v>gradeA</v>
+      </c>
+      <c r="F4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="64">
+      <c r="G4" s="64">
         <v>0</v>
       </c>
-      <c r="G4" s="64">
+      <c r="H4" s="64">
         <v>5</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64" t="s">
+      <c r="I4" s="64"/>
+      <c r="J4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="109"/>
-      <c r="K4" s="64"/>
+      <c r="K4" s="116"/>
       <c r="L4" s="64"/>
       <c r="M4" s="64"/>
-      <c r="N4" s="64" t="s">
+      <c r="N4" s="64"/>
+      <c r="O4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64" t="s">
-        <v>10</v>
-      </c>
+      <c r="P4" s="64"/>
       <c r="Q4" s="64" t="s">
         <v>10</v>
       </c>
       <c r="R4" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="64">
+      <c r="T4" s="64">
         <v>3</v>
       </c>
-      <c r="T4" s="64" t="s">
+      <c r="U4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="64">
+      <c r="V4" s="64">
         <v>3</v>
       </c>
-      <c r="V4" s="64" t="s">
+      <c r="W4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="64" t="s">
+      <c r="X4" s="64" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="28.5">
       <c r="A5" s="10" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="78" t="str">
+        <v>236</v>
+      </c>
+      <c r="D5" s="63" t="str">
         <f>centers!$A$4</f>
         <v>centerB</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="str">
+        <f>ar_evaluations!A3</f>
+        <v>gradeA</v>
+      </c>
+      <c r="F5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="64">
+      <c r="G5" s="64">
         <v>240</v>
       </c>
-      <c r="G5" s="64">
+      <c r="H5" s="64">
         <v>4</v>
       </c>
-      <c r="H5" s="64">
+      <c r="I5" s="64">
         <v>60</v>
       </c>
-      <c r="I5" s="64" t="s">
+      <c r="J5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="109" t="s">
-        <v>222</v>
-      </c>
-      <c r="K5" s="64" t="s">
+      <c r="K5" s="116" t="s">
+        <v>237</v>
+      </c>
+      <c r="L5" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="64">
+      <c r="M5" s="64">
         <v>4</v>
       </c>
-      <c r="M5" s="64" t="s">
+      <c r="N5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="64" t="s">
+      <c r="O5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="64">
+      <c r="P5" s="64">
         <v>4</v>
-      </c>
-      <c r="P5" s="64" t="s">
-        <v>10</v>
       </c>
       <c r="Q5" s="64" t="s">
         <v>10</v>
@@ -5521,29 +5837,32 @@
       <c r="R5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="64">
+      <c r="S5" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="64">
         <v>3</v>
       </c>
-      <c r="T5" s="64" t="s">
+      <c r="U5" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="64">
+      <c r="V5" s="64">
         <v>3</v>
-      </c>
-      <c r="V5" s="64" t="s">
-        <v>9</v>
       </c>
       <c r="W5" s="64" t="s">
         <v>9</v>
       </c>
+      <c r="X5" s="64" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:X2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -5552,222 +5871,83 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00150003-0056-4217-9812-007500FC004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B80010-0035-4C02-B880-00F3008400B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>X4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{007F0079-002F-4480-8FD5-00CC000B00F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>X5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0055008E-00E4-4A13-A09C-00A0007B00E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006B00AE-00C6-4E73-9FA1-0040009800AF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D90011-0088-4538-A3AF-00DA00680068}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AB004E-0031-475E-9D5B-00FD008A0073}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001E00C9-0022-414D-B99F-004300DF0016}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>V4</xm:sqref>
+          <xm:sqref>U4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00760039-00BA-4951-923B-001C008E00EB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0084001E-0000-4F1D-A633-003A00FC005B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>V5</xm:sqref>
+          <xm:sqref>U5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000B0045-00D0-45E4-A095-00FC00160061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B6000F-00FF-484B-A399-007900A0008C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>T4</xm:sqref>
+          <xm:sqref>S4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F8001F-00A4-4BAD-B87B-0007002500E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005F00D2-005F-4A09-8EEF-0050002C0045}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>T5</xm:sqref>
+          <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0057009F-001A-46EF-909D-007D00DE0066}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F00085-00E0-46FD-8672-00DB006F00A9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>R4</xm:sqref>
+          <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009F00B3-0056-4F73-BFF2-00EB0077008E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001D000D-005A-4EF3-8FAB-009B00900063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>E4</xm:sqref>
+          <xm:sqref>J4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FF0033-00EB-454E-8361-006E009A00B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B0007E-00ED-4D5B-A07E-00D2008F0030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
-          <xm:sqref>E5</xm:sqref>
+          <xm:sqref>J5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008600B8-005B-49DB-B53F-006B00F30093}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>BOOLEAN_ANSWER</xm:f>
-          </x14:formula1>
-          <xm:sqref>I4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003B00F7-0068-4C26-B92B-009500A00089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>BOOLEAN_ANSWER</xm:f>
-          </x14:formula1>
-          <xm:sqref>I5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003300F3-0059-4F07-84D3-00C500960012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000100FE-007A-485C-B5C3-00BF004B007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
-          <xm:sqref>K4</xm:sqref>
+          <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004A006D-00AF-4F5A-88ED-00E9007600D0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00760064-00F8-4920-B3C3-00F1008500C0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
-          <xm:sqref>K5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="7" tint="0"/>
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col customWidth="1" min="3" max="3" width="11.421875"/>
-    <col customWidth="1" min="4" max="4" width="10.421875"/>
-    <col customWidth="1" min="5" max="5" width="12.421875"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" ht="28.5">
-      <c r="A2" s="93" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="94" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="95" t="s">
-        <v>226</v>
-      </c>
-      <c r="D2" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="110" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="78" t="str">
-        <f>ap_programs!$A$4</f>
-        <v>programA</v>
-      </c>
-      <c r="D3" s="64">
-        <v>0</v>
-      </c>
-      <c r="E3" s="64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" s="78" t="str">
-        <f>ap_programs!$A$5</f>
-        <v>programB</v>
-      </c>
-      <c r="D4" s="64">
-        <v>0</v>
-      </c>
-      <c r="E4" s="64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="C5" s="78" t="str">
-        <f>ap_programs!$A$4</f>
-        <v>programA</v>
-      </c>
-      <c r="D5" s="64">
-        <v>0</v>
-      </c>
-      <c r="E5" s="64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{008D005A-00C0-403F-81DB-00E20094004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>BOOLEAN_ANSWER</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A60045-0013-44A2-89E7-003500510019}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>BOOLEAN_ANSWER</xm:f>
-          </x14:formula1>
-          <xm:sqref>E4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E8008E-00D2-4E98-B729-009D00E50024}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>BOOLEAN_ANSWER</xm:f>
-          </x14:formula1>
-          <xm:sqref>E5</xm:sqref>
+          <xm:sqref>L5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added minScaleToPromote to mvp template
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="314">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -582,6 +582,9 @@
     <t>scales</t>
   </si>
   <si>
+    <t>minScaleToPromote</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -589,6 +592,9 @@
   </si>
   <si>
     <t>Scales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min scale to promote</t>
   </si>
   <si>
     <t>gradeA</t>
@@ -1471,7 +1477,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="128">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1506,7 +1512,6 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="1" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1658,9 +1663,6 @@
     <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1722,14 +1724,11 @@
     <xf fontId="4" fillId="16" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="7" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2530,83 +2529,83 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="101" t="s">
-        <v>241</v>
-      </c>
-      <c r="D2" s="117" t="s">
-        <v>218</v>
-      </c>
-      <c r="E2" s="117" t="s">
-        <v>242</v>
+      <c r="C2" s="98" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="114" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="114" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="C3" s="79" t="str">
+        <v>246</v>
+      </c>
+      <c r="C3" s="77" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D3" s="64">
+      <c r="D3" s="63">
         <v>0</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="63" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4" s="79" t="str">
+        <v>246</v>
+      </c>
+      <c r="C4" s="77" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="63">
         <v>0</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="63" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="C5" s="79" t="str">
+        <v>249</v>
+      </c>
+      <c r="C5" s="77" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="63">
         <v>0</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2618,19 +2617,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00AB004C-00BF-43AF-B98C-00E10079001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00250057-001B-4EAA-A0EB-0068007A0014}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E5002D-005B-480B-97F8-006D0087001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00990013-0081-4C50-B059-0080006F0068}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000A001C-0093-46FB-95E9-005C002D0087}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002B0047-005A-401A-A35C-004C00210033}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -2670,89 +2669,89 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="84" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="84" t="s">
-        <v>250</v>
-      </c>
-      <c r="E2" s="84" t="s">
-        <v>251</v>
-      </c>
-      <c r="F2" s="85" t="s">
-        <v>241</v>
-      </c>
-      <c r="G2" s="119" t="s">
-        <v>218</v>
+      <c r="C2" s="82" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>243</v>
+      </c>
+      <c r="G2" s="116" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E3" s="120" t="s">
-        <v>256</v>
-      </c>
-      <c r="F3" s="79" t="str">
+        <v>257</v>
+      </c>
+      <c r="E3" s="117" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" s="77" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G3" s="64">
+      <c r="G3" s="63">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="E4" s="71" t="s">
-        <v>261</v>
-      </c>
-      <c r="F4" s="79" t="str">
+        <v>262</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="77" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="63">
         <v>0</v>
       </c>
     </row>
@@ -2803,36 +2802,36 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="L1" s="121" t="s">
-        <v>268</v>
-      </c>
-      <c r="M1" s="76"/>
+        <v>269</v>
+      </c>
+      <c r="L1" s="118" t="s">
+        <v>270</v>
+      </c>
+      <c r="M1" s="74"/>
     </row>
     <row r="2" ht="28.850000000000001" customHeight="1">
       <c r="A2" s="5"/>
@@ -2843,52 +2842,52 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="76"/>
+      <c r="M2" s="74"/>
     </row>
     <row r="3" ht="31.850000000000001" customHeight="1">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="101" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" s="100" t="s">
-        <v>270</v>
-      </c>
-      <c r="E3" s="84" t="s">
-        <v>271</v>
-      </c>
-      <c r="F3" s="100" t="s">
+      <c r="C3" s="98" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="97" t="s">
         <v>272</v>
       </c>
-      <c r="G3" s="100" t="s">
+      <c r="E3" s="82" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="122" t="s">
+      <c r="F3" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="I3" s="123" t="s">
-        <v>250</v>
-      </c>
-      <c r="J3" s="123" t="s">
+      <c r="G3" s="97" t="s">
         <v>275</v>
       </c>
-      <c r="K3" s="124" t="s">
+      <c r="H3" s="119" t="s">
         <v>276</v>
       </c>
-      <c r="L3" s="85" t="s">
+      <c r="I3" s="120" t="s">
+        <v>252</v>
+      </c>
+      <c r="J3" s="120" t="s">
         <v>277</v>
       </c>
-      <c r="M3" s="125"/>
+      <c r="K3" s="121" t="s">
+        <v>278</v>
+      </c>
+      <c r="L3" s="83" t="s">
+        <v>279</v>
+      </c>
+      <c r="M3" s="122"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
@@ -2896,38 +2895,38 @@
         <v>subject01</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>278</v>
-      </c>
-      <c r="C4" s="79" t="str">
+        <v>280</v>
+      </c>
+      <c r="C4" s="77" t="str">
         <f>ap_programs!A4</f>
         <v>programA</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="63">
         <v>1</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="63">
         <v>20</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64" t="str">
+      <c r="F4" s="63"/>
+      <c r="G4" s="63" t="str">
         <f t="shared" ref="G4:G9" si="1">_xlfn.CONCAT("0",IF(M4&lt;10,"0",""),M4)</f>
         <v>001</v>
       </c>
-      <c r="H4" s="126" t="s">
-        <v>279</v>
-      </c>
-      <c r="I4" s="127" t="s">
-        <v>280</v>
-      </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="128" t="str">
+      <c r="H4" s="123" t="s">
+        <v>281</v>
+      </c>
+      <c r="I4" s="124" t="s">
+        <v>282</v>
+      </c>
+      <c r="J4" s="63"/>
+      <c r="K4" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L4" s="129" t="s">
-        <v>281</v>
-      </c>
-      <c r="M4" s="130">
+      <c r="L4" s="126" t="s">
+        <v>283</v>
+      </c>
+      <c r="M4" s="127">
         <v>1</v>
       </c>
       <c r="N4" s="9"/>
@@ -2938,41 +2937,41 @@
         <v>subject02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="C5" s="79" t="str">
+        <v>284</v>
+      </c>
+      <c r="C5" s="77" t="str">
         <f t="shared" ref="C5:C10" si="2">C4</f>
         <v>programA</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="63">
         <v>1</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="63">
         <v>20</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64" t="str">
+      <c r="F5" s="63"/>
+      <c r="G5" s="63" t="str">
         <f t="shared" si="1"/>
         <v>002</v>
       </c>
-      <c r="H5" s="126" t="str">
+      <c r="H5" s="123" t="str">
         <f t="shared" ref="H5:H10" si="3">H4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I5" s="127" t="str">
+      <c r="I5" s="124" t="str">
         <f t="shared" ref="I5:I10" si="4">I4</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="J5" s="64"/>
-      <c r="K5" s="128" t="str">
+      <c r="J5" s="63"/>
+      <c r="K5" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L5" s="129" t="str">
+      <c r="L5" s="126" t="str">
         <f t="shared" ref="L5:L10" si="5">L4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M5" s="130">
+      <c r="M5" s="127">
         <f t="shared" ref="M5:M10" si="6">M4+1</f>
         <v>2</v>
       </c>
@@ -2984,41 +2983,41 @@
         <v>subject03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="C6" s="79" t="str">
+        <v>285</v>
+      </c>
+      <c r="C6" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D6" s="64">
+      <c r="D6" s="63">
         <v>1</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="63">
         <v>20</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64" t="str">
+      <c r="F6" s="63"/>
+      <c r="G6" s="63" t="str">
         <f t="shared" si="1"/>
         <v>003</v>
       </c>
-      <c r="H6" s="126" t="str">
+      <c r="H6" s="123" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I6" s="127" t="str">
+      <c r="I6" s="124" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="J6" s="64"/>
-      <c r="K6" s="128" t="str">
+      <c r="J6" s="63"/>
+      <c r="K6" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L6" s="129" t="str">
+      <c r="L6" s="126" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M6" s="130">
+      <c r="M6" s="127">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -3030,41 +3029,41 @@
         <v>subject04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="C7" s="79" t="str">
+        <v>286</v>
+      </c>
+      <c r="C7" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="63">
         <v>1</v>
       </c>
-      <c r="E7" s="64">
+      <c r="E7" s="63">
         <v>20</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64" t="str">
+      <c r="F7" s="63"/>
+      <c r="G7" s="63" t="str">
         <f t="shared" si="1"/>
         <v>004</v>
       </c>
-      <c r="H7" s="126" t="str">
+      <c r="H7" s="123" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I7" s="127" t="str">
+      <c r="I7" s="124" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="J7" s="64"/>
-      <c r="K7" s="128" t="str">
+      <c r="J7" s="63"/>
+      <c r="K7" s="125" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L7" s="129" t="str">
+      <c r="L7" s="126" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M7" s="130">
+      <c r="M7" s="127">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -3076,39 +3075,39 @@
         <v>subject05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="C8" s="79" t="str">
+        <v>287</v>
+      </c>
+      <c r="C8" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="63">
         <v>2</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="63">
         <v>20</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64" t="str">
+      <c r="F8" s="63"/>
+      <c r="G8" s="63" t="str">
         <f t="shared" si="1"/>
         <v>005</v>
       </c>
-      <c r="H8" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="I8" s="127" t="str">
+      <c r="H8" s="123" t="s">
+        <v>288</v>
+      </c>
+      <c r="I8" s="124" t="str">
         <f t="shared" si="4"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="J8" s="64"/>
-      <c r="K8" s="128" t="str">
+      <c r="J8" s="63"/>
+      <c r="K8" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L8" s="129" t="s">
-        <v>287</v>
-      </c>
-      <c r="M8" s="130">
+      <c r="L8" s="126" t="s">
+        <v>289</v>
+      </c>
+      <c r="M8" s="127">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
@@ -3119,40 +3118,40 @@
         <v>subject06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="C9" s="79" t="str">
+        <v>290</v>
+      </c>
+      <c r="C9" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="63">
         <v>2</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="63">
         <v>20</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64" t="str">
+      <c r="F9" s="63"/>
+      <c r="G9" s="63" t="str">
         <f t="shared" si="1"/>
         <v>006</v>
       </c>
-      <c r="H9" s="126" t="str">
+      <c r="H9" s="123" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I9" s="127" t="s">
-        <v>289</v>
-      </c>
-      <c r="J9" s="64"/>
-      <c r="K9" s="128" t="str">
+      <c r="I9" s="124" t="s">
+        <v>291</v>
+      </c>
+      <c r="J9" s="63"/>
+      <c r="K9" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L9" s="129" t="str">
+      <c r="L9" s="126" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M9" s="130">
+      <c r="M9" s="127">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
@@ -3163,41 +3162,41 @@
         <v>subject07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="C10" s="79" t="str">
+        <v>292</v>
+      </c>
+      <c r="C10" s="77" t="str">
         <f t="shared" si="2"/>
         <v>programA</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="63">
         <v>2</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="63">
         <v>20</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64" t="str">
+      <c r="F10" s="63"/>
+      <c r="G10" s="63" t="str">
         <f t="shared" ref="G10:G23" si="8">_xlfn.CONCAT("0",IF(M10&lt;10,"0",""),M10)</f>
         <v>007</v>
       </c>
-      <c r="H10" s="126" t="str">
+      <c r="H10" s="123" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I10" s="127" t="str">
+      <c r="I10" s="124" t="str">
         <f t="shared" si="4"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="J10" s="64"/>
-      <c r="K10" s="128" t="str">
+      <c r="J10" s="63"/>
+      <c r="K10" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L10" s="129" t="str">
+      <c r="L10" s="126" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M10" s="130">
+      <c r="M10" s="127">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
@@ -3208,41 +3207,41 @@
         <v>subject08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="C11" s="79" t="str">
+        <v>293</v>
+      </c>
+      <c r="C11" s="77" t="str">
         <f t="shared" ref="C11:C23" si="9">C10</f>
         <v>programA</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="63">
         <v>2</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="63">
         <v>20</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64" t="str">
+      <c r="F11" s="63"/>
+      <c r="G11" s="63" t="str">
         <f t="shared" si="8"/>
         <v>008</v>
       </c>
-      <c r="H11" s="126" t="str">
+      <c r="H11" s="123" t="str">
         <f>H10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I11" s="127" t="str">
+      <c r="I11" s="124" t="str">
         <f t="shared" ref="I11:I18" si="10">I10</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="J11" s="64"/>
-      <c r="K11" s="128" t="str">
+      <c r="J11" s="63"/>
+      <c r="K11" s="125" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L11" s="129" t="str">
+      <c r="L11" s="126" t="str">
         <f>L10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M11" s="130">
+      <c r="M11" s="127">
         <f t="shared" ref="M11:M23" si="11">M10+1</f>
         <v>8</v>
       </c>
@@ -3253,39 +3252,39 @@
         <v>subject09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="C12" s="79" t="str">
+        <v>294</v>
+      </c>
+      <c r="C12" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="63">
         <v>3</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="63">
         <v>20</v>
       </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64" t="str">
+      <c r="F12" s="63"/>
+      <c r="G12" s="63" t="str">
         <f t="shared" si="8"/>
         <v>009</v>
       </c>
-      <c r="H12" s="126" t="s">
-        <v>293</v>
-      </c>
-      <c r="I12" s="127" t="str">
+      <c r="H12" s="123" t="s">
+        <v>295</v>
+      </c>
+      <c r="I12" s="124" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="J12" s="64"/>
-      <c r="K12" s="128" t="str">
+      <c r="J12" s="63"/>
+      <c r="K12" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L12" s="129" t="s">
-        <v>294</v>
-      </c>
-      <c r="M12" s="130">
+      <c r="L12" s="126" t="s">
+        <v>296</v>
+      </c>
+      <c r="M12" s="127">
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
@@ -3296,41 +3295,41 @@
         <v>subject10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="C13" s="79" t="str">
+        <v>297</v>
+      </c>
+      <c r="C13" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="63">
         <v>3</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="63">
         <v>20</v>
       </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64" t="str">
+      <c r="F13" s="63"/>
+      <c r="G13" s="63" t="str">
         <f t="shared" si="8"/>
         <v>010</v>
       </c>
-      <c r="H13" s="126" t="str">
+      <c r="H13" s="123" t="str">
         <f t="shared" ref="H13:H23" si="12">H12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I13" s="127" t="str">
+      <c r="I13" s="124" t="str">
         <f t="shared" si="10"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="J13" s="64"/>
-      <c r="K13" s="128" t="str">
+      <c r="J13" s="63"/>
+      <c r="K13" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L13" s="129" t="str">
+      <c r="L13" s="126" t="str">
         <f t="shared" ref="L13:L23" si="13">L12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M13" s="130">
+      <c r="M13" s="127">
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
@@ -3341,40 +3340,40 @@
         <v>subject11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="C14" s="79" t="str">
+        <v>298</v>
+      </c>
+      <c r="C14" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="63">
         <v>3</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="63">
         <v>20</v>
       </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64" t="str">
+      <c r="F14" s="63"/>
+      <c r="G14" s="63" t="str">
         <f t="shared" si="8"/>
         <v>011</v>
       </c>
-      <c r="H14" s="126" t="str">
+      <c r="H14" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I14" s="127" t="s">
-        <v>297</v>
-      </c>
-      <c r="J14" s="64"/>
-      <c r="K14" s="128" t="str">
+      <c r="I14" s="124" t="s">
+        <v>299</v>
+      </c>
+      <c r="J14" s="63"/>
+      <c r="K14" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L14" s="129" t="str">
+      <c r="L14" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M14" s="130">
+      <c r="M14" s="127">
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
@@ -3385,41 +3384,41 @@
         <v>subject12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="79" t="str">
+        <v>300</v>
+      </c>
+      <c r="C15" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="63">
         <v>3</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="63">
         <v>20</v>
       </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64" t="str">
+      <c r="F15" s="63"/>
+      <c r="G15" s="63" t="str">
         <f t="shared" si="8"/>
         <v>012</v>
       </c>
-      <c r="H15" s="126" t="str">
+      <c r="H15" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I15" s="127" t="str">
+      <c r="I15" s="124" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J15" s="64"/>
-      <c r="K15" s="128" t="str">
+      <c r="J15" s="63"/>
+      <c r="K15" s="125" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L15" s="129" t="str">
+      <c r="L15" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M15" s="130">
+      <c r="M15" s="127">
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
@@ -3430,39 +3429,39 @@
         <v>subject13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="C16" s="79" t="str">
+        <v>301</v>
+      </c>
+      <c r="C16" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="63">
         <v>4</v>
       </c>
-      <c r="E16" s="64">
+      <c r="E16" s="63">
         <v>20</v>
       </c>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64" t="str">
+      <c r="F16" s="63"/>
+      <c r="G16" s="63" t="str">
         <f t="shared" si="8"/>
         <v>013</v>
       </c>
-      <c r="H16" s="126" t="s">
-        <v>300</v>
-      </c>
-      <c r="I16" s="127" t="str">
+      <c r="H16" s="123" t="s">
+        <v>302</v>
+      </c>
+      <c r="I16" s="124" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J16" s="64"/>
-      <c r="K16" s="128" t="str">
+      <c r="J16" s="63"/>
+      <c r="K16" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L16" s="129" t="s">
-        <v>301</v>
-      </c>
-      <c r="M16" s="130">
+      <c r="L16" s="126" t="s">
+        <v>303</v>
+      </c>
+      <c r="M16" s="127">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
@@ -3473,41 +3472,41 @@
         <v>subject14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="C17" s="79" t="str">
+        <v>304</v>
+      </c>
+      <c r="C17" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D17" s="64">
+      <c r="D17" s="63">
         <v>4</v>
       </c>
-      <c r="E17" s="64">
+      <c r="E17" s="63">
         <v>20</v>
       </c>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64" t="str">
+      <c r="F17" s="63"/>
+      <c r="G17" s="63" t="str">
         <f t="shared" si="8"/>
         <v>014</v>
       </c>
-      <c r="H17" s="126" t="str">
+      <c r="H17" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I17" s="127" t="str">
+      <c r="I17" s="124" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J17" s="64"/>
-      <c r="K17" s="128" t="str">
+      <c r="J17" s="63"/>
+      <c r="K17" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L17" s="129" t="str">
+      <c r="L17" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M17" s="130">
+      <c r="M17" s="127">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
@@ -3518,41 +3517,41 @@
         <v>subject15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="C18" s="79" t="str">
+        <v>305</v>
+      </c>
+      <c r="C18" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="63">
         <v>4</v>
       </c>
-      <c r="E18" s="64">
+      <c r="E18" s="63">
         <v>20</v>
       </c>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64" t="str">
+      <c r="F18" s="63"/>
+      <c r="G18" s="63" t="str">
         <f t="shared" si="8"/>
         <v>015</v>
       </c>
-      <c r="H18" s="126" t="str">
+      <c r="H18" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I18" s="127" t="str">
+      <c r="I18" s="124" t="str">
         <f t="shared" si="10"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J18" s="64"/>
-      <c r="K18" s="128" t="str">
+      <c r="J18" s="63"/>
+      <c r="K18" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L18" s="129" t="str">
+      <c r="L18" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M18" s="130">
+      <c r="M18" s="127">
         <f t="shared" si="11"/>
         <v>15</v>
       </c>
@@ -3563,40 +3562,40 @@
         <v>subject16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="C19" s="79" t="str">
+        <v>306</v>
+      </c>
+      <c r="C19" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D19" s="64">
+      <c r="D19" s="63">
         <v>4</v>
       </c>
-      <c r="E19" s="64">
+      <c r="E19" s="63">
         <v>20</v>
       </c>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64" t="str">
+      <c r="F19" s="63"/>
+      <c r="G19" s="63" t="str">
         <f t="shared" si="8"/>
         <v>016</v>
       </c>
-      <c r="H19" s="126" t="str">
+      <c r="H19" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I19" s="127" t="s">
-        <v>305</v>
-      </c>
-      <c r="J19" s="64"/>
-      <c r="K19" s="128" t="str">
+      <c r="I19" s="124" t="s">
+        <v>307</v>
+      </c>
+      <c r="J19" s="63"/>
+      <c r="K19" s="125" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L19" s="129" t="str">
+      <c r="L19" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M19" s="130">
+      <c r="M19" s="127">
         <f t="shared" si="11"/>
         <v>16</v>
       </c>
@@ -3607,38 +3606,38 @@
         <v>subject17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="C20" s="79" t="str">
+        <v>308</v>
+      </c>
+      <c r="C20" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="63">
         <v>5</v>
       </c>
-      <c r="E20" s="64">
+      <c r="E20" s="63">
         <v>20</v>
       </c>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64" t="str">
+      <c r="F20" s="63"/>
+      <c r="G20" s="63" t="str">
         <f t="shared" si="8"/>
         <v>017</v>
       </c>
-      <c r="H20" s="126" t="s">
+      <c r="H20" s="123" t="s">
+        <v>309</v>
+      </c>
+      <c r="I20" s="124" t="s">
         <v>307</v>
       </c>
-      <c r="I20" s="127" t="s">
-        <v>305</v>
-      </c>
-      <c r="J20" s="64"/>
-      <c r="K20" s="128" t="str">
+      <c r="J20" s="63"/>
+      <c r="K20" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L20" s="129" t="s">
-        <v>308</v>
-      </c>
-      <c r="M20" s="130">
+      <c r="L20" s="126" t="s">
+        <v>310</v>
+      </c>
+      <c r="M20" s="127">
         <f t="shared" si="11"/>
         <v>17</v>
       </c>
@@ -3649,40 +3648,40 @@
         <v>subject18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>309</v>
-      </c>
-      <c r="C21" s="79" t="str">
+        <v>311</v>
+      </c>
+      <c r="C21" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D21" s="64">
+      <c r="D21" s="63">
         <v>5</v>
       </c>
-      <c r="E21" s="64">
+      <c r="E21" s="63">
         <v>20</v>
       </c>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64" t="str">
+      <c r="F21" s="63"/>
+      <c r="G21" s="63" t="str">
         <f t="shared" si="8"/>
         <v>018</v>
       </c>
-      <c r="H21" s="126" t="str">
+      <c r="H21" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I21" s="127" t="s">
-        <v>305</v>
-      </c>
-      <c r="J21" s="64"/>
-      <c r="K21" s="128" t="str">
+      <c r="I21" s="124" t="s">
+        <v>307</v>
+      </c>
+      <c r="J21" s="63"/>
+      <c r="K21" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L21" s="129" t="str">
+      <c r="L21" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M21" s="130">
+      <c r="M21" s="127">
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
@@ -3693,40 +3692,40 @@
         <v>subject19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="C22" s="79" t="str">
+        <v>312</v>
+      </c>
+      <c r="C22" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D22" s="63">
         <v>5</v>
       </c>
-      <c r="E22" s="64">
+      <c r="E22" s="63">
         <v>20</v>
       </c>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64" t="str">
+      <c r="F22" s="63"/>
+      <c r="G22" s="63" t="str">
         <f t="shared" si="8"/>
         <v>019</v>
       </c>
-      <c r="H22" s="126" t="str">
+      <c r="H22" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I22" s="127" t="s">
-        <v>305</v>
-      </c>
-      <c r="J22" s="64"/>
-      <c r="K22" s="128" t="str">
+      <c r="I22" s="124" t="s">
+        <v>307</v>
+      </c>
+      <c r="J22" s="63"/>
+      <c r="K22" s="125" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L22" s="129" t="str">
+      <c r="L22" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M22" s="130">
+      <c r="M22" s="127">
         <f t="shared" si="11"/>
         <v>19</v>
       </c>
@@ -3737,47 +3736,47 @@
         <v>subject20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="C23" s="79" t="str">
+        <v>313</v>
+      </c>
+      <c r="C23" s="77" t="str">
         <f t="shared" si="9"/>
         <v>programA</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="63">
         <v>5</v>
       </c>
-      <c r="E23" s="64">
+      <c r="E23" s="63">
         <v>20</v>
       </c>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64" t="str">
+      <c r="F23" s="63"/>
+      <c r="G23" s="63" t="str">
         <f t="shared" si="8"/>
         <v>020</v>
       </c>
-      <c r="H23" s="126" t="str">
+      <c r="H23" s="123" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I23" s="127" t="s">
-        <v>305</v>
-      </c>
-      <c r="J23" s="64"/>
-      <c r="K23" s="128" t="str">
+      <c r="I23" s="124" t="s">
+        <v>307</v>
+      </c>
+      <c r="J23" s="63"/>
+      <c r="K23" s="125" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L23" s="129" t="str">
+      <c r="L23" s="126" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M23" s="130">
+      <c r="M23" s="127">
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="E24" s="15"/>
-      <c r="M24" s="76"/>
+      <c r="E24" s="14"/>
+      <c r="M24" s="74"/>
     </row>
     <row r="25" ht="14.25"/>
   </sheetData>
@@ -4023,15 +4022,15 @@
         <f>_xlfn.CONCAT($AD$3,".",AD5)</f>
         <v>plugins.grades.rules</v>
       </c>
-      <c r="AE1" s="13" t="str">
+      <c r="AE1" s="12" t="str">
         <f>_xlfn.CONCAT($AD$3,".",AE5)</f>
         <v>plugins.grades.evaluations</v>
       </c>
-      <c r="AF1" s="13" t="str">
+      <c r="AF1" s="12" t="str">
         <f>_xlfn.CONCAT($AD$3,".",AF5)</f>
         <v>plugins.grades.promotions</v>
       </c>
-      <c r="AG1" s="13" t="str">
+      <c r="AG1" s="12" t="str">
         <f>_xlfn.CONCAT($AD$3,".",AG5)</f>
         <v>plugins.grades.dependencies</v>
       </c>
@@ -4041,239 +4040,239 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22" t="s">
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="16" t="s">
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="W3" s="17"/>
-      <c r="X3" s="25" t="s">
+      <c r="W3" s="16"/>
+      <c r="X3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="27" t="s">
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AC3" s="20" t="s">
+      <c r="AC3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="AD3" s="22" t="s">
+      <c r="AD3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-    </row>
-    <row r="4" s="28" customFormat="1" ht="19.850000000000001" customHeight="1">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29" t="s">
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+    </row>
+    <row r="4" s="27" customFormat="1" ht="19.850000000000001" customHeight="1">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="35" t="s">
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="29" t="s">
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="31" t="s">
+      <c r="W4" s="29"/>
+      <c r="X4" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="32" t="s">
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="AC4" s="33" t="s">
+      <c r="AC4" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="AD4" s="35" t="s">
+      <c r="AD4" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="36"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="39" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="K5" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L5" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="O5" s="45" t="s">
+      <c r="O5" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="P5" s="46" t="s">
+      <c r="P5" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="Q5" s="47" t="s">
+      <c r="Q5" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="R5" s="47" t="s">
+      <c r="R5" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="S5" s="47" t="s">
+      <c r="S5" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="T5" s="47" t="s">
+      <c r="T5" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="U5" s="48" t="s">
+      <c r="U5" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="V5" s="39" t="s">
+      <c r="V5" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="W5" s="40" t="s">
+      <c r="W5" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="X5" s="42" t="s">
+      <c r="X5" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="Y5" s="42" t="s">
+      <c r="Y5" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="Z5" s="42" t="s">
+      <c r="Z5" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="AA5" s="42" t="s">
+      <c r="AA5" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="AC5" s="49" t="s">
+      <c r="AC5" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="AD5" s="46" t="s">
+      <c r="AD5" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="AE5" s="47" t="s">
+      <c r="AE5" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="AF5" s="47" t="s">
+      <c r="AF5" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="AG5" s="47" t="s">
+      <c r="AG5" s="46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" s="50" customFormat="1" ht="19.5" customHeight="1">
+    <row r="6" s="49" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -4283,10 +4282,10 @@
       <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="51" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -4295,82 +4294,82 @@
       <c r="G6" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="55" t="s">
+      <c r="J6" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="56" t="s">
+      <c r="K6" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="57" t="s">
+      <c r="L6" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="M6" s="57" t="s">
+      <c r="M6" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="N6" s="57" t="s">
+      <c r="N6" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="O6" s="57" t="s">
+      <c r="O6" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="P6" s="58" t="s">
+      <c r="P6" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="59" t="s">
+      <c r="Q6" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="R6" s="59" t="s">
+      <c r="R6" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="S6" s="59" t="s">
+      <c r="S6" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="T6" s="59" t="s">
+      <c r="T6" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="U6" s="60" t="s">
+      <c r="U6" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="V6" s="52" t="s">
+      <c r="V6" s="51" t="s">
         <v>94</v>
       </c>
       <c r="W6" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="X6" s="54" t="s">
+      <c r="X6" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="Y6" s="54" t="s">
+      <c r="Y6" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="Z6" s="54" t="s">
+      <c r="Z6" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="AA6" s="54" t="s">
+      <c r="AA6" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AB6" s="61" t="s">
+      <c r="AB6" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="AC6" s="62" t="s">
+      <c r="AC6" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="AD6" s="58" t="s">
+      <c r="AD6" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="AE6" s="59" t="s">
+      <c r="AE6" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="AF6" s="59" t="s">
+      <c r="AF6" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="AG6" s="59" t="s">
+      <c r="AG6" s="58" t="s">
         <v>105</v>
       </c>
     </row>
@@ -4384,84 +4383,84 @@
       <c r="C7" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64" t="s">
+      <c r="D7" s="62"/>
+      <c r="E7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="64" t="s">
+      <c r="I7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="J7" s="64" t="s">
+      <c r="J7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="K7" s="64" t="s">
+      <c r="K7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="L7" s="64" t="s">
+      <c r="L7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="N7" s="64" t="s">
+      <c r="N7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="O7" s="64" t="s">
+      <c r="O7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="P7" s="65" t="s">
+      <c r="P7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="Q7" s="65" t="s">
+      <c r="Q7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="R7" s="65"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="65"/>
-      <c r="V7" s="65" t="s">
+      <c r="R7" s="64"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="W7" s="65" t="s">
+      <c r="W7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="X7" s="65" t="s">
+      <c r="X7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="Y7" s="65" t="s">
+      <c r="Y7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="Z7" s="65" t="s">
+      <c r="Z7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="AA7" s="65" t="s">
+      <c r="AA7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="AB7" s="64" t="s">
+      <c r="AB7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AC7" s="64" t="s">
+      <c r="AC7" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AD7" s="65" t="s">
+      <c r="AD7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="AE7" s="65" t="s">
+      <c r="AE7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="AF7" s="65" t="s">
+      <c r="AF7" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="AG7" s="65" t="s">
+      <c r="AG7" s="64" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4475,82 +4474,82 @@
       <c r="C8" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64" t="s">
+      <c r="D8" s="62"/>
+      <c r="E8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="G8" s="64" t="s">
+      <c r="G8" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="64" t="s">
+      <c r="J8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="64" t="s">
+      <c r="K8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="64" t="s">
+      <c r="L8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64" t="s">
+      <c r="M8" s="63"/>
+      <c r="N8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="O8" s="64" t="s">
+      <c r="O8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="P8" s="64" t="s">
+      <c r="P8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="Q8" s="64" t="s">
+      <c r="Q8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="R8" s="65"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64" t="s">
+      <c r="R8" s="64"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="W8" s="64" t="s">
+      <c r="W8" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="X8" s="64" t="s">
+      <c r="X8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="Y8" s="64" t="s">
+      <c r="Y8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="Z8" s="64" t="s">
+      <c r="Z8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AA8" s="64" t="s">
+      <c r="AA8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AB8" s="64" t="s">
+      <c r="AB8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AC8" s="64" t="s">
+      <c r="AC8" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AD8" s="64" t="s">
+      <c r="AD8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AE8" s="64" t="s">
+      <c r="AE8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AF8" s="64" t="s">
+      <c r="AF8" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AG8" s="64" t="s">
+      <c r="AG8" s="63" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4564,88 +4563,88 @@
       <c r="C9" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64" t="s">
+      <c r="D9" s="62"/>
+      <c r="E9" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="64" t="s">
+      <c r="G9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="H9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="J9" s="64" t="s">
+      <c r="J9" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="K9" s="64" t="s">
+      <c r="K9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="L9" s="64" t="s">
+      <c r="L9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64" t="s">
+      <c r="M9" s="63"/>
+      <c r="N9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64" t="s">
+      <c r="O9" s="63"/>
+      <c r="P9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="Q9" s="64" t="s">
+      <c r="Q9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="R9" s="64" t="s">
+      <c r="R9" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="S9" s="64" t="s">
+      <c r="S9" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="T9" s="64" t="s">
+      <c r="T9" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="U9" s="64" t="s">
+      <c r="U9" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="V9" s="64" t="s">
+      <c r="V9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="W9" s="64" t="s">
+      <c r="W9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="X9" s="64" t="s">
+      <c r="X9" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="Y9" s="64" t="s">
+      <c r="Y9" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="Z9" s="64" t="s">
+      <c r="Z9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AA9" s="64" t="s">
+      <c r="AA9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AB9" s="64" t="s">
+      <c r="AB9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AC9" s="64" t="s">
+      <c r="AC9" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AD9" s="66" t="s">
+      <c r="AD9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AE9" s="66" t="s">
+      <c r="AE9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AF9" s="64" t="s">
+      <c r="AF9" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AG9" s="64" t="s">
+      <c r="AG9" s="63" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4659,71 +4658,71 @@
       <c r="C10" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="63" t="str">
+      <c r="D10" s="62" t="str">
         <f>A9</f>
         <v>student</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="64" t="s">
+      <c r="G10" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="64" t="s">
+      <c r="H10" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="64" t="s">
+      <c r="I10" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="J10" s="64" t="s">
+      <c r="J10" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="K10" s="64" t="s">
+      <c r="K10" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="L10" s="64" t="s">
+      <c r="L10" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64" t="s">
+      <c r="M10" s="63"/>
+      <c r="N10" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64" t="s">
+      <c r="O10" s="63"/>
+      <c r="P10" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="Q10" s="64" t="s">
+      <c r="Q10" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="R10" s="64" t="s">
+      <c r="R10" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="S10" s="64" t="s">
+      <c r="S10" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="T10" s="64" t="s">
+      <c r="T10" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="U10" s="64" t="s">
+      <c r="U10" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-      <c r="X10" s="64"/>
-      <c r="Y10" s="64"/>
-      <c r="Z10" s="64"/>
-      <c r="AA10" s="64"/>
-      <c r="AB10" s="64"/>
-      <c r="AC10" s="64" t="s">
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="63"/>
+      <c r="Z10" s="63"/>
+      <c r="AA10" s="63"/>
+      <c r="AB10" s="63"/>
+      <c r="AC10" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="AD10" s="64"/>
-      <c r="AE10" s="64"/>
-      <c r="AF10" s="64"/>
-      <c r="AG10" s="64"/>
+      <c r="AD10" s="63"/>
+      <c r="AE10" s="63"/>
+      <c r="AF10" s="63"/>
+      <c r="AG10" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -4828,13 +4827,13 @@
       <c r="G2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="67" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4851,22 +4850,22 @@
       <c r="D3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="70">
+      <c r="E3" s="68">
         <v>36526</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="69" t="s">
         <v>136</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="J3" s="70" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4883,208 +4882,208 @@
       <c r="D4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="70">
+      <c r="E4" s="68">
         <v>34781</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="69" t="s">
         <v>142</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="64" t="s">
+      <c r="I4" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="70" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="72" t="s">
         <v>116</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="70">
+      <c r="E5" s="68">
         <v>39205</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="73" t="s">
         <v>147</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="64" t="s">
+      <c r="I5" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="72" t="s">
+      <c r="J5" s="70" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="72" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="72" t="s">
         <v>152</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="68">
         <v>39156</v>
       </c>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="73" t="s">
         <v>153</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="J6" s="72" t="s">
+      <c r="J6" s="70" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="72" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="72" t="s">
         <v>116</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="70">
+      <c r="E7" s="68">
         <v>42171</v>
       </c>
-      <c r="F7" s="75" t="s">
+      <c r="F7" s="73" t="s">
         <v>156</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="64" t="s">
+      <c r="I7" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="J7" s="72" t="s">
+      <c r="J7" s="70" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="72" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="72" t="s">
         <v>152</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="70">
+      <c r="E8" s="68">
         <v>42237</v>
       </c>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="73" t="s">
         <v>160</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="J8" s="72" t="s">
+      <c r="J8" s="70" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="72" t="s">
         <v>163</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="68">
         <v>27791</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="73" t="s">
         <v>164</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="H9" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="J9" s="72" t="s">
+      <c r="J9" s="70" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="76"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="74"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5101,43 +5100,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D7007E-0067-4AB0-8225-00C700A6002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FE0017-0000-430B-AFF1-00E1000800DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A40063-0041-47C3-957C-003C00440058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FF00E0-0045-4FC5-9A6D-001F00AF00BB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0096007B-00E4-4252-A1A7-007D008A00F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00000025-00E4-493C-B072-00B900B100B9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00430052-0091-467A-A294-000E0087009C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0097002B-0050-4D55-8010-003200550034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0088006F-00C4-4D02-B029-00D700C70094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D50096-00F6-4850-AFCE-002400CA00A3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B000CC-002A-4C58-921B-00FD00820020}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00400066-007C-426D-8101-008500040038}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009900DF-00DE-4202-BAD0-0038001C00D6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00140014-0084-4F6C-BF9E-00870058001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -5179,7 +5178,7 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="76" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5187,7 +5186,7 @@
       <c r="A3" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="79" t="str">
+      <c r="B3" s="77" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
@@ -5201,7 +5200,7 @@
       <c r="A4" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="79" t="str">
+      <c r="B4" s="77" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -5262,19 +5261,19 @@
       </c>
     </row>
     <row r="2" ht="24.350000000000001" customHeight="1">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="80" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="67" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5285,13 +5284,13 @@
       <c r="B3" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="77" t="s">
         <v>178</v>
       </c>
     </row>
@@ -5304,7 +5303,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00BB001D-008E-4D60-88A0-00F8005700ED}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002E006C-000A-4DD4-B43C-00460050002F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5333,6 +5332,7 @@
     <col customWidth="1" min="2" max="2" width="18.7109375"/>
     <col customWidth="1" min="5" max="5" width="13.7109375"/>
     <col customWidth="1" min="6" max="6" width="19.421875"/>
+    <col customWidth="1" min="7" max="7" width="25.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -5354,35 +5354,41 @@
       <c r="F1" s="5" t="s">
         <v>182</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="84" t="s">
-        <v>183</v>
-      </c>
-      <c r="E2" s="84" t="s">
+      <c r="D2" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="E2" s="82" t="s">
         <v>185</v>
       </c>
+      <c r="F2" s="82" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" s="82" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="3" ht="146.25" customHeight="1">
-      <c r="A3" s="86" t="s">
-        <v>186</v>
-      </c>
-      <c r="B3" s="87" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="79" t="str">
+      <c r="A3" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="77" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
@@ -5392,8 +5398,11 @@
       <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="88" t="s">
-        <v>188</v>
+      <c r="F3" s="84" t="s">
+        <v>190</v>
+      </c>
+      <c r="G3" s="85">
+        <v>5</v>
       </c>
     </row>
     <row r="4" ht="14.25"/>
@@ -5405,13 +5414,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00C800DB-00EC-413B-B7D0-007500A900F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D900DC-00FA-414A-8478-00BE00A900FF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D900DF-00C5-4890-A1FF-00E000E300D4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009B00F3-005E-449D-B955-0087008C00BB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -5449,10 +5458,10 @@
       </c>
     </row>
     <row r="2" ht="22.100000000000001" customHeight="1">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="80" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5460,7 +5469,7 @@
       <c r="A3" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="79" t="str">
+      <c r="B3" s="77" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
@@ -5469,7 +5478,7 @@
       <c r="A4" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="79" t="str">
+      <c r="B4" s="77" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -5526,70 +5535,70 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
@@ -5612,247 +5621,247 @@
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
-      <c r="F2" s="89" t="s">
-        <v>210</v>
-      </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="90" t="s">
-        <v>211</v>
-      </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="93" t="s">
+      <c r="F2" s="86" t="s">
         <v>212</v>
       </c>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="94" t="s">
+      <c r="G2" s="86"/>
+      <c r="H2" s="87" t="s">
         <v>213</v>
       </c>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="96"/>
-      <c r="V2" s="97" t="s">
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="W2" s="98"/>
-      <c r="X2" s="98"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="91" t="s">
+        <v>215</v>
+      </c>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="94" t="s">
+        <v>216</v>
+      </c>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
     </row>
     <row r="3" ht="34.100000000000001" customHeight="1">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="100" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" s="101" t="s">
+      <c r="C3" s="97" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="102" t="s">
-        <v>216</v>
-      </c>
-      <c r="F3" s="103" t="s">
-        <v>217</v>
-      </c>
-      <c r="G3" s="104" t="s">
+      <c r="E3" s="99" t="s">
         <v>218</v>
       </c>
-      <c r="H3" s="105" t="s">
+      <c r="F3" s="100" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="106" t="s">
+      <c r="G3" s="101" t="s">
         <v>220</v>
       </c>
-      <c r="J3" s="107" t="s">
+      <c r="H3" s="102" t="s">
         <v>221</v>
       </c>
-      <c r="K3" s="107" t="s">
+      <c r="I3" s="103" t="s">
         <v>222</v>
       </c>
-      <c r="L3" s="107" t="s">
+      <c r="J3" s="104" t="s">
         <v>223</v>
       </c>
-      <c r="M3" s="107" t="s">
+      <c r="K3" s="104" t="s">
         <v>224</v>
       </c>
-      <c r="N3" s="107" t="s">
+      <c r="L3" s="104" t="s">
         <v>225</v>
       </c>
-      <c r="O3" s="108" t="s">
+      <c r="M3" s="104" t="s">
         <v>226</v>
       </c>
-      <c r="P3" s="109" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q3" s="110" t="s">
-        <v>225</v>
-      </c>
-      <c r="R3" s="111" t="s">
+      <c r="N3" s="104" t="s">
         <v>227</v>
       </c>
-      <c r="S3" s="112" t="s">
+      <c r="O3" s="105" t="s">
         <v>228</v>
       </c>
-      <c r="T3" s="112" t="s">
-        <v>224</v>
-      </c>
-      <c r="U3" s="112" t="s">
-        <v>225</v>
-      </c>
-      <c r="V3" s="113" t="s">
-        <v>224</v>
-      </c>
-      <c r="W3" s="114" t="s">
+      <c r="P3" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q3" s="107" t="s">
+        <v>227</v>
+      </c>
+      <c r="R3" s="108" t="s">
         <v>229</v>
       </c>
-      <c r="X3" s="115" t="s">
+      <c r="S3" s="109" t="s">
         <v>230</v>
+      </c>
+      <c r="T3" s="109" t="s">
+        <v>226</v>
+      </c>
+      <c r="U3" s="109" t="s">
+        <v>227</v>
+      </c>
+      <c r="V3" s="110" t="s">
+        <v>226</v>
+      </c>
+      <c r="W3" s="111" t="s">
+        <v>231</v>
+      </c>
+      <c r="X3" s="112" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="63" t="str">
+        <v>235</v>
+      </c>
+      <c r="D4" s="62" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
-      <c r="E4" s="63" t="str">
+      <c r="E4" s="62" t="str">
         <f>ar_evaluations!A3</f>
         <v>gradeA</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="63">
         <v>0</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="63">
         <v>5</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64" t="s">
+      <c r="I4" s="63"/>
+      <c r="J4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="116"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64" t="s">
+      <c r="K4" s="113"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64" t="s">
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="R4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="64" t="s">
+      <c r="S4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="64">
+      <c r="T4" s="63">
         <v>3</v>
       </c>
-      <c r="U4" s="64" t="s">
+      <c r="U4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="64">
+      <c r="V4" s="63">
         <v>3</v>
       </c>
-      <c r="W4" s="64" t="s">
+      <c r="W4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="X4" s="64" t="s">
+      <c r="X4" s="63" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="28.5">
       <c r="A5" s="10" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="63" t="str">
+        <v>238</v>
+      </c>
+      <c r="D5" s="62" t="str">
         <f>centers!$A$4</f>
         <v>centerB</v>
       </c>
-      <c r="E5" s="63" t="str">
+      <c r="E5" s="62" t="str">
         <f>ar_evaluations!A3</f>
         <v>gradeA</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="63">
         <v>240</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="63">
         <v>4</v>
       </c>
-      <c r="I5" s="64">
+      <c r="I5" s="63">
         <v>60</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="116" t="s">
-        <v>237</v>
-      </c>
-      <c r="L5" s="64" t="s">
+      <c r="K5" s="113" t="s">
+        <v>239</v>
+      </c>
+      <c r="L5" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="64">
+      <c r="M5" s="63">
         <v>4</v>
       </c>
-      <c r="N5" s="64" t="s">
+      <c r="N5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="64" t="s">
+      <c r="O5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="64">
+      <c r="P5" s="63">
         <v>4</v>
       </c>
-      <c r="Q5" s="64" t="s">
+      <c r="Q5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="64" t="s">
+      <c r="R5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="64" t="s">
+      <c r="S5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="64">
+      <c r="T5" s="63">
         <v>3</v>
       </c>
-      <c r="U5" s="64" t="s">
+      <c r="U5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="64">
+      <c r="V5" s="63">
         <v>3</v>
       </c>
-      <c r="W5" s="64" t="s">
+      <c r="W5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="X5" s="64" t="s">
+      <c r="X5" s="63" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5871,79 +5880,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00B80010-0035-4C02-B880-00F3008400B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001900BD-00B2-42E0-9220-00A90004007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>X4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007F0079-002F-4480-8FD5-00CC000B00F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007A00D8-0034-4100-93F7-00E4004300DA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>X5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0055008E-00E4-4A13-A09C-00A0007B00E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006C00A0-0050-44D5-84CF-00B600C90022}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D90011-0088-4538-A3AF-00DA00680068}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00020058-0085-4FF7-AE1A-005D00DC0061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001E00C9-0022-414D-B99F-004300DF0016}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C7004F-00FA-4156-8001-0074007900E1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>U4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0084001E-0000-4F1D-A633-003A00FC005B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E8005D-0027-4783-A231-006B007F00C8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>U5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B6000F-00FF-484B-A399-007900A0008C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E000E4-0061-4C18-A73A-00FD00E70007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>S4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005F00D2-005F-4A09-8EEF-0050002C0045}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DC0053-0028-460F-8461-002300F300C1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F00085-00E0-46FD-8672-00DB006F00A9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D300BC-008C-4BF0-BCF8-00EE0012006E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001D000D-005A-4EF3-8FAB-009B00900063}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A8004E-00C5-4E63-B8D5-00BA00F600F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>J4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B0007E-00ED-4D5B-A07E-00D2008F0030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C4004B-00AE-44E7-9EF0-00EE0052005F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>J5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000100FE-007A-485C-B5C3-00BF004B007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005D0019-009A-4C6D-AFE9-007E00B900F5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00760064-00F8-4920-B3C3-00F1008500C0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007200DB-0080-48C0-829D-001A00DB0016}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
ADDED: Roles in locales. Asset permissions on Adding new
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -1728,7 +1728,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="7" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2617,19 +2617,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00250057-001B-4EAA-A0EB-0068007A0014}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000A0033-00F7-481D-BE71-007500D600B1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00990013-0081-4C50-B059-0080006F0068}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003200F1-008A-41DE-999E-006F00C20040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002B0047-005A-401A-A35C-004C00210033}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008B00D4-005B-464E-AF7E-0016009E002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -5100,43 +5100,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00FE0017-0000-430B-AFF1-00E1000800DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00080055-0083-4A1A-B551-0011005B000A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FF00E0-0045-4FC5-9A6D-001F00AF00BB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003400A6-00BF-4942-BFDD-0009007D00CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00000025-00E4-493C-B072-00B900B100B9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C30048-005B-4E2F-99A6-00D800070054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0097002B-0050-4D55-8010-003200550034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0057003F-00BC-4EC5-BA30-00F200A800AA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D50096-00F6-4850-AFCE-002400CA00A3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E300B8-0060-4E71-96E3-007600210042}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00400066-007C-426D-8101-008500040038}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003F0078-001F-4669-8D2E-00CD007A0099}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00140014-0084-4F6C-BF9E-00870058001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00640088-007F-47C7-B77A-009A0083004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -5303,7 +5303,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{002E006C-000A-4DD4-B43C-00460050002F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C70097-00A3-4624-9FBE-003600D30092}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5414,13 +5414,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D900DC-00FA-414A-8478-00BE00A900FF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00960021-0048-4591-ADD0-00DD00AC00B9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009B00F3-005E-449D-B955-0087008C00BB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DF0062-00DB-4D9A-832C-009200680068}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -5880,79 +5880,79 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13" disablePrompts="0">
-        <x14:dataValidation xr:uid="{001900BD-00B2-42E0-9220-00A90004007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004D00F8-0066-4D28-BB06-006D005C007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>X4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007A00D8-0034-4100-93F7-00E4004300DA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001200E2-0054-4D79-869D-005F002800D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>X5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006C00A0-0050-44D5-84CF-00B600C90022}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005000F0-00D7-47E1-9E02-0038000700CE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00020058-0085-4FF7-AE1A-005D00DC0061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DC0044-00C5-45F8-93B2-000400190087}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>W5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C7004F-00FA-4156-8001-0074007900E1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BB0075-0018-41AB-8775-00BC00F20002}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>U4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E8005D-0027-4783-A231-006B007F00C8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002F0075-0018-4B8F-83B9-00B90008008C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>U5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E000E4-0061-4C18-A73A-00FD00E70007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00920059-00A5-42AD-AE1E-0083000E00F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>S4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DC0053-0028-460F-8461-002300F300C1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A20005-0067-4D7B-801B-00E5009B007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D300BC-008C-4BF0-BCF8-00EE0012006E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DA000D-003A-41D0-9B56-002C00B60005}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A8004E-00C5-4E63-B8D5-00BA00F600F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000C00D3-00F2-4597-9A77-00AA005B0067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>J4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C4004B-00AE-44E7-9EF0-00EE0052005F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00420027-005C-43B2-AEBF-00380034005B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>J5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005D0019-009A-4C6D-AFE9-007E00B900F5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B70087-0004-4D53-9E54-00D00085007A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
           <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007200DB-0080-48C0-829D-001A00DB0016}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00270043-00DC-4F45-A6C5-007D009000E9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Login refactor for select center.
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -459,7 +459,7 @@
     <t>Admin,Test</t>
   </si>
   <si>
-    <t xml:space="preserve">admin@centerA, admin@centerB, admin@centerC</t>
+    <t xml:space="preserve">admin@centerA, admin@centerB, admin@centerC,student@centerB,teacher@centerA, teacher@centerB</t>
   </si>
   <si>
     <t>teacher01</t>
@@ -1598,7 +1598,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="124">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1806,9 +1806,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="5" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2647,19 +2644,19 @@
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="94" t="s">
         <v>276</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="110" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="110" t="s">
         <v>277</v>
       </c>
     </row>
@@ -2743,7 +2740,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00DD00F4-000F-4E54-8BAD-00B500F500E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E200C8-0059-4422-A9C5-00CF001E00BC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -2799,25 +2796,25 @@
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="78" t="s">
         <v>247</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="F2" s="80" t="s">
+      <c r="F2" s="79" t="s">
         <v>276</v>
       </c>
-      <c r="G2" s="113" t="s">
+      <c r="G2" s="112" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2834,7 +2831,7 @@
       <c r="D3" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="E3" s="114" t="s">
+      <c r="E3" s="113" t="s">
         <v>293</v>
       </c>
       <c r="F3" s="71" t="str">
@@ -2942,7 +2939,7 @@
       <c r="K1" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="L1" s="115" t="s">
+      <c r="L1" s="114" t="s">
         <v>305</v>
       </c>
       <c r="M1" s="14"/>
@@ -2965,43 +2962,43 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" ht="31.75" customHeight="1">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="94" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="93" t="s">
         <v>307</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="78" t="s">
         <v>308</v>
       </c>
-      <c r="F3" s="94" t="s">
+      <c r="F3" s="93" t="s">
         <v>309</v>
       </c>
-      <c r="G3" s="94" t="s">
+      <c r="G3" s="93" t="s">
         <v>310</v>
       </c>
-      <c r="H3" s="116" t="s">
+      <c r="H3" s="115" t="s">
         <v>311</v>
       </c>
-      <c r="I3" s="117" t="s">
+      <c r="I3" s="116" t="s">
         <v>287</v>
       </c>
-      <c r="J3" s="117" t="s">
+      <c r="J3" s="116" t="s">
         <v>312</v>
       </c>
-      <c r="K3" s="118" t="s">
+      <c r="K3" s="117" t="s">
         <v>313</v>
       </c>
-      <c r="L3" s="80" t="s">
+      <c r="L3" s="79" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="119"/>
+      <c r="M3" s="118"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
@@ -3026,21 +3023,21 @@
         <f t="shared" ref="G4:G9" si="2">_xlfn.CONCAT("0",IF(M4&lt;10,"0",""),M4)</f>
         <v>001</v>
       </c>
-      <c r="H4" s="120" t="s">
+      <c r="H4" s="119" t="s">
         <v>316</v>
       </c>
-      <c r="I4" s="121" t="s">
+      <c r="I4" s="120" t="s">
         <v>317</v>
       </c>
       <c r="J4" s="63"/>
-      <c r="K4" s="122" t="str">
+      <c r="K4" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L4" s="123" t="s">
+      <c r="L4" s="122" t="s">
         <v>318</v>
       </c>
-      <c r="M4" s="124">
+      <c r="M4" s="123">
         <v>1</v>
       </c>
     </row>
@@ -3067,24 +3064,24 @@
         <f t="shared" si="2"/>
         <v>002</v>
       </c>
-      <c r="H5" s="120" t="str">
+      <c r="H5" s="119" t="str">
         <f t="shared" ref="H5:H10" si="4">H4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I5" s="121" t="str">
+      <c r="I5" s="120" t="str">
         <f t="shared" ref="I5:I10" si="5">I4</f>
         <v>#FFEB9C</v>
       </c>
       <c r="J5" s="63"/>
-      <c r="K5" s="122" t="str">
+      <c r="K5" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L5" s="123" t="str">
+      <c r="L5" s="122" t="str">
         <f t="shared" ref="L5:L10" si="6">L4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M5" s="124">
+      <c r="M5" s="123">
         <f t="shared" ref="M5:M10" si="7">M4+1</f>
         <v>2</v>
       </c>
@@ -3112,24 +3109,24 @@
         <f t="shared" si="2"/>
         <v>003</v>
       </c>
-      <c r="H6" s="120" t="str">
+      <c r="H6" s="119" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I6" s="121" t="str">
+      <c r="I6" s="120" t="str">
         <f t="shared" si="5"/>
         <v>#FFEB9C</v>
       </c>
       <c r="J6" s="63"/>
-      <c r="K6" s="122" t="str">
+      <c r="K6" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L6" s="123" t="str">
+      <c r="L6" s="122" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M6" s="124">
+      <c r="M6" s="123">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
@@ -3157,24 +3154,24 @@
         <f t="shared" si="2"/>
         <v>004</v>
       </c>
-      <c r="H7" s="120" t="str">
+      <c r="H7" s="119" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I7" s="121" t="str">
+      <c r="I7" s="120" t="str">
         <f t="shared" si="5"/>
         <v>#FFEB9C</v>
       </c>
       <c r="J7" s="63"/>
-      <c r="K7" s="122" t="str">
+      <c r="K7" s="121" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L7" s="123" t="str">
+      <c r="L7" s="122" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M7" s="124">
+      <c r="M7" s="123">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
@@ -3202,22 +3199,22 @@
         <f t="shared" si="2"/>
         <v>005</v>
       </c>
-      <c r="H8" s="120" t="s">
+      <c r="H8" s="119" t="s">
         <v>323</v>
       </c>
-      <c r="I8" s="121" t="str">
+      <c r="I8" s="120" t="str">
         <f t="shared" si="5"/>
         <v>#FFEB9C</v>
       </c>
       <c r="J8" s="63"/>
-      <c r="K8" s="122" t="str">
+      <c r="K8" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L8" s="123" t="s">
+      <c r="L8" s="122" t="s">
         <v>324</v>
       </c>
-      <c r="M8" s="124">
+      <c r="M8" s="123">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
@@ -3245,23 +3242,23 @@
         <f t="shared" si="2"/>
         <v>006</v>
       </c>
-      <c r="H9" s="120" t="str">
+      <c r="H9" s="119" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I9" s="121" t="s">
+      <c r="I9" s="120" t="s">
         <v>326</v>
       </c>
       <c r="J9" s="63"/>
-      <c r="K9" s="122" t="str">
+      <c r="K9" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L9" s="123" t="str">
+      <c r="L9" s="122" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M9" s="124">
+      <c r="M9" s="123">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
@@ -3289,24 +3286,24 @@
         <f t="shared" ref="G10:G24" si="9">_xlfn.CONCAT("0",IF(M10&lt;10,"0",""),M10)</f>
         <v>007</v>
       </c>
-      <c r="H10" s="120" t="str">
+      <c r="H10" s="119" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I10" s="121" t="str">
+      <c r="I10" s="120" t="str">
         <f t="shared" si="5"/>
         <v>#FFC7CE</v>
       </c>
       <c r="J10" s="63"/>
-      <c r="K10" s="122" t="str">
+      <c r="K10" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L10" s="123" t="str">
+      <c r="L10" s="122" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M10" s="124">
+      <c r="M10" s="123">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
@@ -3334,24 +3331,24 @@
         <f t="shared" si="9"/>
         <v>008</v>
       </c>
-      <c r="H11" s="120" t="str">
+      <c r="H11" s="119" t="str">
         <f>H10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I11" s="121" t="str">
+      <c r="I11" s="120" t="str">
         <f t="shared" ref="I11:I18" si="11">I10</f>
         <v>#FFC7CE</v>
       </c>
       <c r="J11" s="63"/>
-      <c r="K11" s="122" t="str">
+      <c r="K11" s="121" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L11" s="123" t="str">
+      <c r="L11" s="122" t="str">
         <f>L10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M11" s="124">
+      <c r="M11" s="123">
         <f t="shared" ref="M11:M24" si="12">M10+1</f>
         <v>8</v>
       </c>
@@ -3379,22 +3376,22 @@
         <f t="shared" si="9"/>
         <v>009</v>
       </c>
-      <c r="H12" s="120" t="s">
+      <c r="H12" s="119" t="s">
         <v>330</v>
       </c>
-      <c r="I12" s="121" t="str">
+      <c r="I12" s="120" t="str">
         <f t="shared" si="11"/>
         <v>#FFC7CE</v>
       </c>
       <c r="J12" s="63"/>
-      <c r="K12" s="122" t="str">
+      <c r="K12" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L12" s="123" t="s">
+      <c r="L12" s="122" t="s">
         <v>331</v>
       </c>
-      <c r="M12" s="124">
+      <c r="M12" s="123">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
@@ -3422,24 +3419,24 @@
         <f t="shared" si="9"/>
         <v>010</v>
       </c>
-      <c r="H13" s="120" t="str">
+      <c r="H13" s="119" t="str">
         <f t="shared" ref="H13:H24" si="13">H12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I13" s="121" t="str">
+      <c r="I13" s="120" t="str">
         <f t="shared" si="11"/>
         <v>#FFC7CE</v>
       </c>
       <c r="J13" s="63"/>
-      <c r="K13" s="122" t="str">
+      <c r="K13" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L13" s="123" t="str">
+      <c r="L13" s="122" t="str">
         <f t="shared" ref="L13:L24" si="14">L12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M13" s="124">
+      <c r="M13" s="123">
         <f t="shared" si="12"/>
         <v>10</v>
       </c>
@@ -3467,23 +3464,23 @@
         <f t="shared" si="9"/>
         <v>011</v>
       </c>
-      <c r="H14" s="120" t="str">
+      <c r="H14" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I14" s="121" t="s">
+      <c r="I14" s="120" t="s">
         <v>334</v>
       </c>
       <c r="J14" s="63"/>
-      <c r="K14" s="122" t="str">
+      <c r="K14" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L14" s="123" t="str">
+      <c r="L14" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M14" s="124">
+      <c r="M14" s="123">
         <f t="shared" si="12"/>
         <v>11</v>
       </c>
@@ -3511,24 +3508,24 @@
         <f t="shared" si="9"/>
         <v>012</v>
       </c>
-      <c r="H15" s="120" t="str">
+      <c r="H15" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I15" s="121" t="str">
+      <c r="I15" s="120" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J15" s="63"/>
-      <c r="K15" s="122" t="str">
+      <c r="K15" s="121" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L15" s="123" t="str">
+      <c r="L15" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M15" s="124">
+      <c r="M15" s="123">
         <f t="shared" si="12"/>
         <v>12</v>
       </c>
@@ -3556,22 +3553,22 @@
         <f t="shared" si="9"/>
         <v>013</v>
       </c>
-      <c r="H16" s="120" t="s">
+      <c r="H16" s="119" t="s">
         <v>337</v>
       </c>
-      <c r="I16" s="121" t="str">
+      <c r="I16" s="120" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J16" s="63"/>
-      <c r="K16" s="122" t="str">
+      <c r="K16" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L16" s="123" t="s">
+      <c r="L16" s="122" t="s">
         <v>338</v>
       </c>
-      <c r="M16" s="124">
+      <c r="M16" s="123">
         <f t="shared" si="12"/>
         <v>13</v>
       </c>
@@ -3599,24 +3596,24 @@
         <f t="shared" si="9"/>
         <v>014</v>
       </c>
-      <c r="H17" s="120" t="str">
+      <c r="H17" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I17" s="121" t="str">
+      <c r="I17" s="120" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J17" s="63"/>
-      <c r="K17" s="122" t="str">
+      <c r="K17" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L17" s="123" t="str">
+      <c r="L17" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M17" s="124">
+      <c r="M17" s="123">
         <f t="shared" si="12"/>
         <v>14</v>
       </c>
@@ -3644,24 +3641,24 @@
         <f t="shared" si="9"/>
         <v>015</v>
       </c>
-      <c r="H18" s="120" t="str">
+      <c r="H18" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I18" s="121" t="str">
+      <c r="I18" s="120" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
       <c r="J18" s="63"/>
-      <c r="K18" s="122" t="str">
+      <c r="K18" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L18" s="123" t="str">
+      <c r="L18" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M18" s="124">
+      <c r="M18" s="123">
         <f t="shared" si="12"/>
         <v>15</v>
       </c>
@@ -3689,23 +3686,23 @@
         <f t="shared" si="9"/>
         <v>016</v>
       </c>
-      <c r="H19" s="120" t="str">
+      <c r="H19" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I19" s="121" t="s">
+      <c r="I19" s="120" t="s">
         <v>342</v>
       </c>
       <c r="J19" s="63"/>
-      <c r="K19" s="122" t="str">
+      <c r="K19" s="121" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L19" s="123" t="str">
+      <c r="L19" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M19" s="124">
+      <c r="M19" s="123">
         <f t="shared" si="12"/>
         <v>16</v>
       </c>
@@ -3733,21 +3730,21 @@
         <f t="shared" si="9"/>
         <v>017</v>
       </c>
-      <c r="H20" s="120" t="s">
+      <c r="H20" s="119" t="s">
         <v>344</v>
       </c>
-      <c r="I20" s="121" t="s">
+      <c r="I20" s="120" t="s">
         <v>342</v>
       </c>
       <c r="J20" s="63"/>
-      <c r="K20" s="122" t="str">
+      <c r="K20" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L20" s="123" t="s">
+      <c r="L20" s="122" t="s">
         <v>345</v>
       </c>
-      <c r="M20" s="124">
+      <c r="M20" s="123">
         <f t="shared" si="12"/>
         <v>17</v>
       </c>
@@ -3775,23 +3772,23 @@
         <f t="shared" si="9"/>
         <v>018</v>
       </c>
-      <c r="H21" s="120" t="str">
+      <c r="H21" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I21" s="121" t="s">
+      <c r="I21" s="120" t="s">
         <v>342</v>
       </c>
       <c r="J21" s="63"/>
-      <c r="K21" s="122" t="str">
+      <c r="K21" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L21" s="123" t="str">
+      <c r="L21" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M21" s="124">
+      <c r="M21" s="123">
         <f t="shared" si="12"/>
         <v>18</v>
       </c>
@@ -3819,23 +3816,23 @@
         <f t="shared" si="9"/>
         <v>019</v>
       </c>
-      <c r="H22" s="120" t="str">
+      <c r="H22" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I22" s="121" t="s">
+      <c r="I22" s="120" t="s">
         <v>342</v>
       </c>
       <c r="J22" s="63"/>
-      <c r="K22" s="122" t="str">
+      <c r="K22" s="121" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L22" s="123" t="str">
+      <c r="L22" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M22" s="124">
+      <c r="M22" s="123">
         <f t="shared" si="12"/>
         <v>19</v>
       </c>
@@ -3863,21 +3860,21 @@
         <f t="shared" si="9"/>
         <v>001</v>
       </c>
-      <c r="H23" s="120" t="s">
+      <c r="H23" s="119" t="s">
         <v>349</v>
       </c>
-      <c r="I23" s="121" t="s">
+      <c r="I23" s="120" t="s">
         <v>350</v>
       </c>
       <c r="J23" s="63"/>
-      <c r="K23" s="122" t="str">
+      <c r="K23" s="121" t="str">
         <f>ap_subject_types!$A$6</f>
         <v>type04</v>
       </c>
-      <c r="L23" s="123" t="s">
+      <c r="L23" s="122" t="s">
         <v>351</v>
       </c>
-      <c r="M23" s="124">
+      <c r="M23" s="123">
         <v>1</v>
       </c>
     </row>
@@ -3904,23 +3901,23 @@
         <f t="shared" si="9"/>
         <v>002</v>
       </c>
-      <c r="H24" s="120" t="str">
+      <c r="H24" s="119" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">2ºA|2ºA, 2ºB|2ºB</v>
       </c>
-      <c r="I24" s="121" t="s">
+      <c r="I24" s="120" t="s">
         <v>353</v>
       </c>
       <c r="J24" s="63"/>
-      <c r="K24" s="122" t="str">
+      <c r="K24" s="121" t="str">
         <f>ap_subject_types!$A$6</f>
         <v>type04</v>
       </c>
-      <c r="L24" s="123" t="str">
+      <c r="L24" s="122" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@2ºA, teacher01|main@2ºB</v>
       </c>
-      <c r="M24" s="124">
+      <c r="M24" s="123">
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
@@ -5082,7 +5079,7 @@
       <c r="I5" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J5" s="71" t="s">
+      <c r="J5" s="70" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5279,7 +5276,7 @@
       </c>
     </row>
     <row r="12" s="14" customFormat="1">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="10" t="s">
         <v>179</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -5311,7 +5308,7 @@
       </c>
     </row>
     <row r="13" s="14" customFormat="1">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="10" t="s">
         <v>183</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -5343,7 +5340,7 @@
       </c>
     </row>
     <row r="14" s="14" customFormat="1">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="10" t="s">
         <v>187</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -5375,7 +5372,7 @@
       </c>
     </row>
     <row r="15" s="14" customFormat="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="10" t="s">
         <v>191</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -5427,7 +5424,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00DF0011-00C4-4DAC-8936-0003004200CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00930025-0041-4827-80E9-00F100810047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -5469,7 +5466,7 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="73" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5537,16 +5534,16 @@
       </c>
     </row>
     <row r="2" ht="24.25" customHeight="1">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="73" t="s">
         <v>201</v>
       </c>
       <c r="E2" s="67" t="s">
@@ -5563,7 +5560,7 @@
       <c r="C3" s="71" t="s">
         <v>205</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="77" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="71" t="s">
@@ -5578,7 +5575,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00EF00C7-00DE-41B2-85DF-0097002A005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00730039-002A-483B-82A6-00D300DE0098}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5634,25 +5631,25 @@
       </c>
     </row>
     <row r="2" ht="16">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="78" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="78" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="78" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5673,10 +5670,10 @@
       <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="80" t="s">
         <v>218</v>
       </c>
-      <c r="G3" s="82">
+      <c r="G3" s="81">
         <v>5</v>
       </c>
     </row>
@@ -5697,10 +5694,10 @@
       <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="80" t="s">
         <v>218</v>
       </c>
-      <c r="G4" s="82">
+      <c r="G4" s="81">
         <v>5</v>
       </c>
     </row>
@@ -5712,13 +5709,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00540080-0021-4711-8567-00DB00340041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F700D7-00CB-4060-BE33-00DD00BC0037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E0009E-00BA-4DF8-BAE3-002700E10015}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A900FF-00CF-4DF6-A121-006900A4004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -5756,10 +5753,10 @@
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="76" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5915,107 +5912,107 @@
       <c r="AN1" s="5"/>
     </row>
     <row r="2" s="9" customFormat="1" ht="23.5" customHeight="1">
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="82" t="s">
         <v>242</v>
       </c>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84" t="s">
+      <c r="G2" s="82"/>
+      <c r="H2" s="83" t="s">
         <v>243</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="87" t="s">
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="88" t="s">
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="87" t="s">
         <v>245</v>
       </c>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="91" t="s">
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="89"/>
+      <c r="V2" s="90" t="s">
         <v>246</v>
       </c>
-      <c r="W2" s="92"/>
-      <c r="X2" s="92"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="91"/>
     </row>
     <row r="3" ht="34" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="93" t="s">
         <v>247</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="G3" s="98" t="s">
+      <c r="G3" s="97" t="s">
         <v>250</v>
       </c>
-      <c r="H3" s="99" t="s">
+      <c r="H3" s="98" t="s">
         <v>251</v>
       </c>
-      <c r="I3" s="100" t="s">
+      <c r="I3" s="99" t="s">
         <v>252</v>
       </c>
-      <c r="J3" s="101" t="s">
+      <c r="J3" s="100" t="s">
         <v>253</v>
       </c>
-      <c r="K3" s="101" t="s">
+      <c r="K3" s="100" t="s">
         <v>254</v>
       </c>
-      <c r="L3" s="101" t="s">
+      <c r="L3" s="100" t="s">
         <v>255</v>
       </c>
-      <c r="M3" s="101" t="s">
+      <c r="M3" s="100" t="s">
         <v>256</v>
       </c>
-      <c r="N3" s="101" t="s">
+      <c r="N3" s="100" t="s">
         <v>257</v>
       </c>
-      <c r="O3" s="102" t="s">
+      <c r="O3" s="101" t="s">
         <v>258</v>
       </c>
-      <c r="P3" s="103" t="s">
+      <c r="P3" s="102" t="s">
         <v>256</v>
       </c>
-      <c r="Q3" s="104" t="s">
+      <c r="Q3" s="103" t="s">
         <v>257</v>
       </c>
-      <c r="R3" s="105" t="s">
+      <c r="R3" s="104" t="s">
         <v>259</v>
       </c>
-      <c r="S3" s="106" t="s">
+      <c r="S3" s="105" t="s">
         <v>260</v>
       </c>
-      <c r="T3" s="106" t="s">
+      <c r="T3" s="105" t="s">
         <v>256</v>
       </c>
-      <c r="U3" s="106" t="s">
+      <c r="U3" s="105" t="s">
         <v>257</v>
       </c>
-      <c r="V3" s="107" t="s">
+      <c r="V3" s="106" t="s">
         <v>256</v>
       </c>
-      <c r="W3" s="108" t="s">
+      <c r="W3" s="107" t="s">
         <v>261</v>
       </c>
-      <c r="X3" s="109" t="s">
+      <c r="X3" s="108" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6050,7 +6047,7 @@
       <c r="J4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="110"/>
+      <c r="K4" s="109"/>
       <c r="L4" s="63"/>
       <c r="M4" s="63"/>
       <c r="N4" s="63"/>
@@ -6116,7 +6113,7 @@
       <c r="J5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="110" t="s">
+      <c r="K5" s="109" t="s">
         <v>269</v>
       </c>
       <c r="L5" s="63" t="s">
@@ -6190,7 +6187,7 @@
       <c r="J6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="110" t="s">
+      <c r="K6" s="109" t="s">
         <v>272</v>
       </c>
       <c r="L6" s="63" t="s">
@@ -6246,13 +6243,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00CF00B3-00BD-4795-8B4D-000B007C001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007A0006-004B-4ECA-BE3B-0047009400FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>J4:J6 F4:F6 S4 U4:U6 W4:X6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00BA005A-00AD-436E-B0FB-0008000A00DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00910010-0084-4272-87E8-00CF007D00EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
MIGRATED: Task setup page to new VerticalStepper
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ap_subject_types" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="ap_knowledges" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="ap_subjects" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="t_profiles" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="BOOLEAN_ANSWER">DB!$A$11:$A$12</definedName>
@@ -1802,13 +1803,13 @@
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="5" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="2" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2667,7 +2668,7 @@
       <c r="B3" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="71" t="str">
+      <c r="C3" s="70" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
@@ -2685,7 +2686,7 @@
       <c r="B4" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="71" t="str">
+      <c r="C4" s="70" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -2703,7 +2704,7 @@
       <c r="B5" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="C5" s="71" t="str">
+      <c r="C5" s="70" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
@@ -2721,7 +2722,7 @@
       <c r="B6" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="71" t="str">
+      <c r="C6" s="70" t="str">
         <f>ap_programs!$A$6</f>
         <v>programC</v>
       </c>
@@ -2740,7 +2741,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E200C8-0059-4422-A9C5-00CF001E00BC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AD009E-008C-4D2D-861F-00E40005008C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -2834,7 +2835,7 @@
       <c r="E3" s="113" t="s">
         <v>293</v>
       </c>
-      <c r="F3" s="71" t="str">
+      <c r="F3" s="70" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -2858,7 +2859,7 @@
       <c r="E4" s="69" t="s">
         <v>298</v>
       </c>
-      <c r="F4" s="71" t="str">
+      <c r="F4" s="70" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -3008,7 +3009,7 @@
       <c r="B4" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="C4" s="71" t="str">
+      <c r="C4" s="70" t="str">
         <f>ap_programs!A4</f>
         <v>programA</v>
       </c>
@@ -3049,7 +3050,7 @@
       <c r="B5" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="C5" s="71" t="str">
+      <c r="C5" s="70" t="str">
         <f t="shared" ref="C5:C10" si="3">C4</f>
         <v>programA</v>
       </c>
@@ -3094,7 +3095,7 @@
       <c r="B6" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="C6" s="71" t="str">
+      <c r="C6" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3139,7 +3140,7 @@
       <c r="B7" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="C7" s="71" t="str">
+      <c r="C7" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3184,7 +3185,7 @@
       <c r="B8" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="C8" s="71" t="str">
+      <c r="C8" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3227,7 +3228,7 @@
       <c r="B9" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="C9" s="71" t="str">
+      <c r="C9" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3271,7 +3272,7 @@
       <c r="B10" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C10" s="71" t="str">
+      <c r="C10" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3316,7 +3317,7 @@
       <c r="B11" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="C11" s="71" t="str">
+      <c r="C11" s="70" t="str">
         <f t="shared" ref="C11:C24" si="10">C10</f>
         <v>programA</v>
       </c>
@@ -3361,7 +3362,7 @@
       <c r="B12" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="C12" s="71" t="str">
+      <c r="C12" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3404,7 +3405,7 @@
       <c r="B13" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="C13" s="71" t="str">
+      <c r="C13" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3449,7 +3450,7 @@
       <c r="B14" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="C14" s="71" t="str">
+      <c r="C14" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3493,7 +3494,7 @@
       <c r="B15" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="C15" s="71" t="str">
+      <c r="C15" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3538,7 +3539,7 @@
       <c r="B16" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="C16" s="71" t="str">
+      <c r="C16" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3581,7 +3582,7 @@
       <c r="B17" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="C17" s="71" t="str">
+      <c r="C17" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3626,7 +3627,7 @@
       <c r="B18" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="C18" s="71" t="str">
+      <c r="C18" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3671,7 +3672,7 @@
       <c r="B19" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="C19" s="71" t="str">
+      <c r="C19" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3715,7 +3716,7 @@
       <c r="B20" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="C20" s="71" t="str">
+      <c r="C20" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3757,7 +3758,7 @@
       <c r="B21" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="C21" s="71" t="str">
+      <c r="C21" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3801,7 +3802,7 @@
       <c r="B22" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="C22" s="71" t="str">
+      <c r="C22" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3845,7 +3846,7 @@
       <c r="B23" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="C23" s="71" t="str">
+      <c r="C23" s="70" t="str">
         <f>ap_programs!A6</f>
         <v>programC</v>
       </c>
@@ -3886,7 +3887,7 @@
       <c r="B24" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="C24" s="71" t="str">
+      <c r="C24" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programC</v>
       </c>
@@ -3929,6 +3930,65 @@
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="14.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" ht="21.75" customHeight="1">
+      <c r="A2" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="70" t="str">
+        <f>profiles!$A$8</f>
+        <v>teacher</v>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="70" t="str">
+        <f>profiles!$A$9</f>
+        <v>student</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -5111,7 +5171,7 @@
       <c r="I6" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J6" s="71" t="s">
+      <c r="J6" s="70" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5143,7 +5203,7 @@
       <c r="I7" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J7" s="71" t="s">
+      <c r="J7" s="70" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5175,7 +5235,7 @@
       <c r="I8" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J8" s="71" t="s">
+      <c r="J8" s="70" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5207,7 +5267,7 @@
       <c r="I9" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="J9" s="71" t="s">
+      <c r="J9" s="70" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5227,7 +5287,7 @@
       <c r="E10" s="68">
         <v>38718</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="71" t="s">
         <v>173</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -5239,7 +5299,7 @@
       <c r="I10" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J10" s="71" t="s">
+      <c r="J10" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5259,7 +5319,7 @@
       <c r="E11" s="68">
         <v>38749</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="71" t="s">
         <v>178</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -5271,7 +5331,7 @@
       <c r="I11" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J11" s="71" t="s">
+      <c r="J11" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5291,7 +5351,7 @@
       <c r="E12" s="68">
         <v>38777</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="71" t="s">
         <v>182</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -5303,7 +5363,7 @@
       <c r="I12" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J12" s="71" t="s">
+      <c r="J12" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5323,7 +5383,7 @@
       <c r="E13" s="68">
         <v>38808</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="71" t="s">
         <v>186</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -5335,7 +5395,7 @@
       <c r="I13" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J13" s="71" t="s">
+      <c r="J13" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5355,7 +5415,7 @@
       <c r="E14" s="68">
         <v>38838</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="71" t="s">
         <v>190</v>
       </c>
       <c r="G14" s="11" t="s">
@@ -5367,7 +5427,7 @@
       <c r="I14" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J14" s="71" t="s">
+      <c r="J14" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5387,7 +5447,7 @@
       <c r="E15" s="68">
         <v>38869</v>
       </c>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="71" t="s">
         <v>194</v>
       </c>
       <c r="G15" s="11" t="s">
@@ -5399,7 +5459,7 @@
       <c r="I15" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J15" s="71" t="s">
+      <c r="J15" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5424,7 +5484,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00930025-0041-4827-80E9-00F100810047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005400B5-003F-48E6-A533-0082008B00D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -5466,7 +5526,7 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5474,16 +5534,16 @@
       <c r="A3" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="70" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="71" t="str">
+      <c r="B4" s="70" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -5543,7 +5603,7 @@
       <c r="C2" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="72" t="s">
         <v>201</v>
       </c>
       <c r="E2" s="67" t="s">
@@ -5557,13 +5617,13 @@
       <c r="B3" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="70" t="s">
         <v>205</v>
       </c>
       <c r="D3" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="70" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5575,7 +5635,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00730039-002A-483B-82A6-00D300DE0098}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A90089-00F9-4BA2-8B38-0098000C0086}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5660,7 +5720,7 @@
       <c r="B3" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="71" t="str">
+      <c r="C3" s="70" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
@@ -5684,7 +5744,7 @@
       <c r="B4" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="71" t="str">
+      <c r="C4" s="70" t="str">
         <f>centers!$A$5</f>
         <v>centerC</v>
       </c>
@@ -5709,13 +5769,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00F700D7-00CB-4060-BE33-00DD00BC0037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000500B0-005C-47AD-984E-00A000A90066}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A900FF-00CF-4DF6-A121-006900A4004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00220015-0070-4689-BA77-00ED00E900A2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -5764,7 +5824,7 @@
       <c r="A3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="70" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
@@ -5773,7 +5833,7 @@
       <c r="A4" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="71" t="str">
+      <c r="B4" s="70" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -6243,13 +6303,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007A0006-004B-4ECA-BE3B-0047009400FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B1004A-003F-4944-88D3-00DA005E0026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>J4:J6 F4:F6 S4 U4:U6 W4:X6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00910010-0084-4272-87E8-00CF007D00EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CD007F-007B-40F4-9B3E-002B0051007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Added images to sujects and classes
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -936,6 +936,9 @@
     <t>seats</t>
   </si>
   <si>
+    <t>creator</t>
+  </si>
+  <si>
     <t>internalId</t>
   </si>
   <si>
@@ -961,6 +964,9 @@
   </si>
   <si>
     <t>Credits</t>
+  </si>
+  <si>
+    <t>Creator</t>
   </si>
   <si>
     <t>InternalID</t>
@@ -1598,7 +1604,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1797,9 +1803,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2644,19 +2647,19 @@
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="93" t="s">
         <v>276</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="109" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="109" t="s">
         <v>277</v>
       </c>
     </row>
@@ -2667,7 +2670,7 @@
       <c r="B3" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="71" t="str">
+      <c r="C3" s="70" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
@@ -2685,7 +2688,7 @@
       <c r="B4" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="71" t="str">
+      <c r="C4" s="70" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -2703,7 +2706,7 @@
       <c r="B5" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="C5" s="71" t="str">
+      <c r="C5" s="70" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
@@ -2721,7 +2724,7 @@
       <c r="B6" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="71" t="str">
+      <c r="C6" s="70" t="str">
         <f>ap_programs!$A$6</f>
         <v>programC</v>
       </c>
@@ -2740,7 +2743,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E200C8-0059-4422-A9C5-00CF001E00BC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AB0053-00CD-4E33-AD8D-00ED00A600D0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -2796,25 +2799,25 @@
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="77" t="s">
         <v>287</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="77" t="s">
         <v>288</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="G2" s="112" t="s">
+      <c r="G2" s="111" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2831,10 +2834,10 @@
       <c r="D3" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="112" t="s">
         <v>293</v>
       </c>
-      <c r="F3" s="71" t="str">
+      <c r="F3" s="70" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -2858,7 +2861,7 @@
       <c r="E4" s="69" t="s">
         <v>298</v>
       </c>
-      <c r="F4" s="71" t="str">
+      <c r="F4" s="70" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -2896,13 +2899,13 @@
     <col customWidth="1" min="1" max="1" width="12.83203125"/>
     <col customWidth="1" min="2" max="2" width="31.421875"/>
     <col customWidth="1" min="3" max="3" width="12.83203125"/>
-    <col customWidth="1" min="7" max="7" width="10.5"/>
-    <col customWidth="1" min="8" max="8" width="13"/>
-    <col customWidth="1" min="9" max="9" width="10.83203125"/>
-    <col customWidth="1" min="10" max="10" width="11.83203125"/>
-    <col customWidth="1" min="11" max="11" width="10.1640625"/>
-    <col customWidth="1" min="12" max="12" width="23.33203125"/>
-    <col customWidth="1" min="13" max="13" width="3.5"/>
+    <col customWidth="1" min="8" max="8" width="10.5"/>
+    <col customWidth="1" min="9" max="9" width="13"/>
+    <col customWidth="1" min="10" max="10" width="10.83203125"/>
+    <col customWidth="1" min="11" max="11" width="11.83203125"/>
+    <col customWidth="1" min="12" max="12" width="10.1640625"/>
+    <col customWidth="1" min="13" max="13" width="23.33203125"/>
+    <col customWidth="1" min="14" max="14" width="3.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2931,18 +2934,21 @@
         <v>302</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>303</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="L1" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="M1" s="14"/>
+      <c r="M1" s="113" t="s">
+        <v>306</v>
+      </c>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" ht="28.75" customHeight="1">
       <c r="A2" s="5"/>
@@ -2952,63 +2958,67 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I2" s="1"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="1" t="s">
+        <v>307</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="14"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" ht="31.75" customHeight="1">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="93" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="93" t="s">
-        <v>307</v>
-      </c>
-      <c r="E3" s="78" t="s">
+      <c r="D3" s="92" t="s">
         <v>308</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="E3" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="F3" s="92" t="s">
         <v>310</v>
       </c>
-      <c r="H3" s="115" t="s">
+      <c r="G3" s="92" t="s">
         <v>311</v>
       </c>
-      <c r="I3" s="116" t="s">
+      <c r="H3" s="92" t="s">
+        <v>312</v>
+      </c>
+      <c r="I3" s="114" t="s">
+        <v>313</v>
+      </c>
+      <c r="J3" s="115" t="s">
         <v>287</v>
       </c>
-      <c r="J3" s="116" t="s">
-        <v>312</v>
-      </c>
-      <c r="K3" s="117" t="s">
-        <v>313</v>
-      </c>
-      <c r="L3" s="79" t="s">
+      <c r="K3" s="115" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="118"/>
+      <c r="L3" s="116" t="s">
+        <v>315</v>
+      </c>
+      <c r="M3" s="78" t="s">
+        <v>316</v>
+      </c>
+      <c r="N3" s="117"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
-        <f t="shared" ref="A4:A9" si="1">_xlfn.CONCAT("subject",IF(M4&lt;10,"0",""),M4)</f>
+        <f t="shared" ref="A4:A9" si="1">_xlfn.CONCAT("subject",IF(N4&lt;10,"0",""),N4)</f>
         <v>subject01</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="71" t="str">
+        <v>317</v>
+      </c>
+      <c r="C4" s="70" t="str">
         <f>ap_programs!A4</f>
         <v>programA</v>
       </c>
@@ -3019,25 +3029,28 @@
         <v>20</v>
       </c>
       <c r="F4" s="63"/>
-      <c r="G4" s="63" t="str">
-        <f t="shared" ref="G4:G9" si="2">_xlfn.CONCAT("0",IF(M4&lt;10,"0",""),M4)</f>
+      <c r="G4" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="63" t="str">
+        <f t="shared" ref="H4:H9" si="2">_xlfn.CONCAT("0",IF(N4&lt;10,"0",""),N4)</f>
         <v>001</v>
       </c>
-      <c r="H4" s="119" t="s">
-        <v>316</v>
-      </c>
-      <c r="I4" s="120" t="s">
-        <v>317</v>
-      </c>
-      <c r="J4" s="63"/>
-      <c r="K4" s="121" t="str">
+      <c r="I4" s="118" t="s">
+        <v>318</v>
+      </c>
+      <c r="J4" s="119" t="s">
+        <v>319</v>
+      </c>
+      <c r="K4" s="63"/>
+      <c r="L4" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L4" s="122" t="s">
-        <v>318</v>
-      </c>
-      <c r="M4" s="123">
+      <c r="M4" s="121" t="s">
+        <v>320</v>
+      </c>
+      <c r="N4" s="122">
         <v>1</v>
       </c>
     </row>
@@ -3047,9 +3060,9 @@
         <v>subject02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="C5" s="71" t="str">
+        <v>321</v>
+      </c>
+      <c r="C5" s="70" t="str">
         <f t="shared" ref="C5:C10" si="3">C4</f>
         <v>programA</v>
       </c>
@@ -3060,29 +3073,32 @@
         <v>20</v>
       </c>
       <c r="F5" s="63"/>
-      <c r="G5" s="63" t="str">
+      <c r="G5" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="63" t="str">
         <f t="shared" si="2"/>
         <v>002</v>
       </c>
-      <c r="H5" s="119" t="str">
-        <f t="shared" ref="H5:H10" si="4">H4</f>
+      <c r="I5" s="118" t="str">
+        <f t="shared" ref="I5:I10" si="4">I4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I5" s="120" t="str">
-        <f t="shared" ref="I5:I10" si="5">I4</f>
+      <c r="J5" s="119" t="str">
+        <f t="shared" ref="J5:J10" si="5">J4</f>
         <v>#FFEB9C</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="121" t="str">
+      <c r="K5" s="63"/>
+      <c r="L5" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L5" s="122" t="str">
-        <f t="shared" ref="L5:L10" si="6">L4</f>
+      <c r="M5" s="121" t="str">
+        <f t="shared" ref="M5:M10" si="6">M4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M5" s="123">
-        <f t="shared" ref="M5:M10" si="7">M4+1</f>
+      <c r="N5" s="122">
+        <f t="shared" ref="N5:N10" si="7">N4+1</f>
         <v>2</v>
       </c>
     </row>
@@ -3092,9 +3108,9 @@
         <v>subject03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="C6" s="71" t="str">
+        <v>322</v>
+      </c>
+      <c r="C6" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3105,28 +3121,31 @@
         <v>20</v>
       </c>
       <c r="F6" s="63"/>
-      <c r="G6" s="63" t="str">
+      <c r="G6" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="63" t="str">
         <f t="shared" si="2"/>
         <v>003</v>
       </c>
-      <c r="H6" s="119" t="str">
+      <c r="I6" s="118" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I6" s="120" t="str">
+      <c r="J6" s="119" t="str">
         <f t="shared" si="5"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="J6" s="63"/>
-      <c r="K6" s="121" t="str">
+      <c r="K6" s="63"/>
+      <c r="L6" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L6" s="122" t="str">
+      <c r="M6" s="121" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M6" s="123">
+      <c r="N6" s="122">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
@@ -3137,9 +3156,9 @@
         <v>subject04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="C7" s="71" t="str">
+        <v>323</v>
+      </c>
+      <c r="C7" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3150,28 +3169,31 @@
         <v>20</v>
       </c>
       <c r="F7" s="63"/>
-      <c r="G7" s="63" t="str">
+      <c r="G7" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="63" t="str">
         <f t="shared" si="2"/>
         <v>004</v>
       </c>
-      <c r="H7" s="119" t="str">
+      <c r="I7" s="118" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="I7" s="120" t="str">
+      <c r="J7" s="119" t="str">
         <f t="shared" si="5"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="J7" s="63"/>
-      <c r="K7" s="121" t="str">
+      <c r="K7" s="63"/>
+      <c r="L7" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L7" s="122" t="str">
+      <c r="M7" s="121" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="M7" s="123">
+      <c r="N7" s="122">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
@@ -3182,9 +3204,9 @@
         <v>subject05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>322</v>
-      </c>
-      <c r="C8" s="71" t="str">
+        <v>324</v>
+      </c>
+      <c r="C8" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3195,26 +3217,29 @@
         <v>20</v>
       </c>
       <c r="F8" s="63"/>
-      <c r="G8" s="63" t="str">
+      <c r="G8" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="63" t="str">
         <f t="shared" si="2"/>
         <v>005</v>
       </c>
-      <c r="H8" s="119" t="s">
-        <v>323</v>
-      </c>
-      <c r="I8" s="120" t="str">
+      <c r="I8" s="118" t="s">
+        <v>325</v>
+      </c>
+      <c r="J8" s="119" t="str">
         <f t="shared" si="5"/>
         <v>#FFEB9C</v>
       </c>
-      <c r="J8" s="63"/>
-      <c r="K8" s="121" t="str">
+      <c r="K8" s="63"/>
+      <c r="L8" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L8" s="122" t="s">
-        <v>324</v>
-      </c>
-      <c r="M8" s="123">
+      <c r="M8" s="121" t="s">
+        <v>326</v>
+      </c>
+      <c r="N8" s="122">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
@@ -3225,9 +3250,9 @@
         <v>subject06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="C9" s="71" t="str">
+        <v>327</v>
+      </c>
+      <c r="C9" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3238,40 +3263,43 @@
         <v>20</v>
       </c>
       <c r="F9" s="63"/>
-      <c r="G9" s="63" t="str">
+      <c r="G9" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H9" s="63" t="str">
         <f t="shared" si="2"/>
         <v>006</v>
       </c>
-      <c r="H9" s="119" t="str">
+      <c r="I9" s="118" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I9" s="120" t="s">
-        <v>326</v>
-      </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="121" t="str">
+      <c r="J9" s="119" t="s">
+        <v>328</v>
+      </c>
+      <c r="K9" s="63"/>
+      <c r="L9" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L9" s="122" t="str">
+      <c r="M9" s="121" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M9" s="123">
+      <c r="N9" s="122">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="10" t="str">
-        <f t="shared" ref="A10:A22" si="8">_xlfn.CONCAT("subject",IF(M10&lt;10,"0",""),M10)</f>
+        <f t="shared" ref="A10:A22" si="8">_xlfn.CONCAT("subject",IF(N10&lt;10,"0",""),N10)</f>
         <v>subject07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="C10" s="71" t="str">
+        <v>329</v>
+      </c>
+      <c r="C10" s="70" t="str">
         <f t="shared" si="3"/>
         <v>programA</v>
       </c>
@@ -3282,28 +3310,31 @@
         <v>20</v>
       </c>
       <c r="F10" s="63"/>
-      <c r="G10" s="63" t="str">
-        <f t="shared" ref="G10:G24" si="9">_xlfn.CONCAT("0",IF(M10&lt;10,"0",""),M10)</f>
+      <c r="G10" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="63" t="str">
+        <f t="shared" ref="H10:H24" si="9">_xlfn.CONCAT("0",IF(N10&lt;10,"0",""),N10)</f>
         <v>007</v>
       </c>
-      <c r="H10" s="119" t="str">
+      <c r="I10" s="118" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I10" s="120" t="str">
+      <c r="J10" s="119" t="str">
         <f t="shared" si="5"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="J10" s="63"/>
-      <c r="K10" s="121" t="str">
+      <c r="K10" s="63"/>
+      <c r="L10" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L10" s="122" t="str">
+      <c r="M10" s="121" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M10" s="123">
+      <c r="N10" s="122">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
@@ -3314,9 +3345,9 @@
         <v>subject08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="C11" s="71" t="str">
+        <v>330</v>
+      </c>
+      <c r="C11" s="70" t="str">
         <f t="shared" ref="C11:C24" si="10">C10</f>
         <v>programA</v>
       </c>
@@ -3327,29 +3358,32 @@
         <v>20</v>
       </c>
       <c r="F11" s="63"/>
-      <c r="G11" s="63" t="str">
+      <c r="G11" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="63" t="str">
         <f t="shared" si="9"/>
         <v>008</v>
       </c>
-      <c r="H11" s="119" t="str">
-        <f>H10</f>
+      <c r="I11" s="118" t="str">
+        <f>I10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="I11" s="120" t="str">
-        <f t="shared" ref="I11:I18" si="11">I10</f>
+      <c r="J11" s="119" t="str">
+        <f t="shared" ref="J11:J18" si="11">J10</f>
         <v>#FFC7CE</v>
       </c>
-      <c r="J11" s="63"/>
-      <c r="K11" s="121" t="str">
+      <c r="K11" s="63"/>
+      <c r="L11" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L11" s="122" t="str">
-        <f>L10</f>
+      <c r="M11" s="121" t="str">
+        <f>M10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="M11" s="123">
-        <f t="shared" ref="M11:M24" si="12">M10+1</f>
+      <c r="N11" s="122">
+        <f t="shared" ref="N11:N24" si="12">N10+1</f>
         <v>8</v>
       </c>
     </row>
@@ -3359,9 +3393,9 @@
         <v>subject09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>329</v>
-      </c>
-      <c r="C12" s="71" t="str">
+        <v>331</v>
+      </c>
+      <c r="C12" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3372,26 +3406,29 @@
         <v>20</v>
       </c>
       <c r="F12" s="63"/>
-      <c r="G12" s="63" t="str">
+      <c r="G12" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" s="63" t="str">
         <f t="shared" si="9"/>
         <v>009</v>
       </c>
-      <c r="H12" s="119" t="s">
-        <v>330</v>
-      </c>
-      <c r="I12" s="120" t="str">
+      <c r="I12" s="118" t="s">
+        <v>332</v>
+      </c>
+      <c r="J12" s="119" t="str">
         <f t="shared" si="11"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="J12" s="63"/>
-      <c r="K12" s="121" t="str">
+      <c r="K12" s="63"/>
+      <c r="L12" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L12" s="122" t="s">
-        <v>331</v>
-      </c>
-      <c r="M12" s="123">
+      <c r="M12" s="121" t="s">
+        <v>333</v>
+      </c>
+      <c r="N12" s="122">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
@@ -3402,9 +3439,9 @@
         <v>subject10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>332</v>
-      </c>
-      <c r="C13" s="71" t="str">
+        <v>334</v>
+      </c>
+      <c r="C13" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3415,28 +3452,31 @@
         <v>20</v>
       </c>
       <c r="F13" s="63"/>
-      <c r="G13" s="63" t="str">
+      <c r="G13" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="63" t="str">
         <f t="shared" si="9"/>
         <v>010</v>
       </c>
-      <c r="H13" s="119" t="str">
-        <f t="shared" ref="H13:H24" si="13">H12</f>
+      <c r="I13" s="118" t="str">
+        <f t="shared" ref="I13:I24" si="13">I12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I13" s="120" t="str">
+      <c r="J13" s="119" t="str">
         <f t="shared" si="11"/>
         <v>#FFC7CE</v>
       </c>
-      <c r="J13" s="63"/>
-      <c r="K13" s="121" t="str">
+      <c r="K13" s="63"/>
+      <c r="L13" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L13" s="122" t="str">
-        <f t="shared" ref="L13:L24" si="14">L12</f>
+      <c r="M13" s="121" t="str">
+        <f t="shared" ref="M13:M24" si="14">M12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M13" s="123">
+      <c r="N13" s="122">
         <f t="shared" si="12"/>
         <v>10</v>
       </c>
@@ -3447,9 +3487,9 @@
         <v>subject11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="C14" s="71" t="str">
+        <v>335</v>
+      </c>
+      <c r="C14" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3460,27 +3500,30 @@
         <v>20</v>
       </c>
       <c r="F14" s="63"/>
-      <c r="G14" s="63" t="str">
+      <c r="G14" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H14" s="63" t="str">
         <f t="shared" si="9"/>
         <v>011</v>
       </c>
-      <c r="H14" s="119" t="str">
+      <c r="I14" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I14" s="120" t="s">
-        <v>334</v>
-      </c>
-      <c r="J14" s="63"/>
-      <c r="K14" s="121" t="str">
+      <c r="J14" s="119" t="s">
+        <v>336</v>
+      </c>
+      <c r="K14" s="63"/>
+      <c r="L14" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L14" s="122" t="str">
+      <c r="M14" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M14" s="123">
+      <c r="N14" s="122">
         <f t="shared" si="12"/>
         <v>11</v>
       </c>
@@ -3491,9 +3534,9 @@
         <v>subject12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="C15" s="71" t="str">
+        <v>337</v>
+      </c>
+      <c r="C15" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3504,28 +3547,31 @@
         <v>20</v>
       </c>
       <c r="F15" s="63"/>
-      <c r="G15" s="63" t="str">
+      <c r="G15" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="63" t="str">
         <f t="shared" si="9"/>
         <v>012</v>
       </c>
-      <c r="H15" s="119" t="str">
+      <c r="I15" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="I15" s="120" t="str">
+      <c r="J15" s="119" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J15" s="63"/>
-      <c r="K15" s="121" t="str">
+      <c r="K15" s="63"/>
+      <c r="L15" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L15" s="122" t="str">
+      <c r="M15" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="M15" s="123">
+      <c r="N15" s="122">
         <f t="shared" si="12"/>
         <v>12</v>
       </c>
@@ -3536,9 +3582,9 @@
         <v>subject13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="C16" s="71" t="str">
+        <v>338</v>
+      </c>
+      <c r="C16" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3549,26 +3595,29 @@
         <v>20</v>
       </c>
       <c r="F16" s="63"/>
-      <c r="G16" s="63" t="str">
+      <c r="G16" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" s="63" t="str">
         <f t="shared" si="9"/>
         <v>013</v>
       </c>
-      <c r="H16" s="119" t="s">
-        <v>337</v>
-      </c>
-      <c r="I16" s="120" t="str">
+      <c r="I16" s="118" t="s">
+        <v>339</v>
+      </c>
+      <c r="J16" s="119" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J16" s="63"/>
-      <c r="K16" s="121" t="str">
+      <c r="K16" s="63"/>
+      <c r="L16" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L16" s="122" t="s">
-        <v>338</v>
-      </c>
-      <c r="M16" s="123">
+      <c r="M16" s="121" t="s">
+        <v>340</v>
+      </c>
+      <c r="N16" s="122">
         <f t="shared" si="12"/>
         <v>13</v>
       </c>
@@ -3579,9 +3628,9 @@
         <v>subject14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="C17" s="71" t="str">
+        <v>341</v>
+      </c>
+      <c r="C17" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3592,28 +3641,31 @@
         <v>20</v>
       </c>
       <c r="F17" s="63"/>
-      <c r="G17" s="63" t="str">
+      <c r="G17" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H17" s="63" t="str">
         <f t="shared" si="9"/>
         <v>014</v>
       </c>
-      <c r="H17" s="119" t="str">
+      <c r="I17" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I17" s="120" t="str">
+      <c r="J17" s="119" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J17" s="63"/>
-      <c r="K17" s="121" t="str">
+      <c r="K17" s="63"/>
+      <c r="L17" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L17" s="122" t="str">
+      <c r="M17" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M17" s="123">
+      <c r="N17" s="122">
         <f t="shared" si="12"/>
         <v>14</v>
       </c>
@@ -3624,9 +3676,9 @@
         <v>subject15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="C18" s="71" t="str">
+        <v>342</v>
+      </c>
+      <c r="C18" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3637,28 +3689,31 @@
         <v>20</v>
       </c>
       <c r="F18" s="63"/>
-      <c r="G18" s="63" t="str">
+      <c r="G18" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H18" s="63" t="str">
         <f t="shared" si="9"/>
         <v>015</v>
       </c>
-      <c r="H18" s="119" t="str">
+      <c r="I18" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I18" s="120" t="str">
+      <c r="J18" s="119" t="str">
         <f t="shared" si="11"/>
         <v>#C6EFCD</v>
       </c>
-      <c r="J18" s="63"/>
-      <c r="K18" s="121" t="str">
+      <c r="K18" s="63"/>
+      <c r="L18" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L18" s="122" t="str">
+      <c r="M18" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M18" s="123">
+      <c r="N18" s="122">
         <f t="shared" si="12"/>
         <v>15</v>
       </c>
@@ -3669,9 +3724,9 @@
         <v>subject16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="C19" s="71" t="str">
+        <v>343</v>
+      </c>
+      <c r="C19" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3682,27 +3737,30 @@
         <v>20</v>
       </c>
       <c r="F19" s="63"/>
-      <c r="G19" s="63" t="str">
+      <c r="G19" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H19" s="63" t="str">
         <f t="shared" si="9"/>
         <v>016</v>
       </c>
-      <c r="H19" s="119" t="str">
+      <c r="I19" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="I19" s="120" t="s">
-        <v>342</v>
-      </c>
-      <c r="J19" s="63"/>
-      <c r="K19" s="121" t="str">
+      <c r="J19" s="119" t="s">
+        <v>344</v>
+      </c>
+      <c r="K19" s="63"/>
+      <c r="L19" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="L19" s="122" t="str">
+      <c r="M19" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="M19" s="123">
+      <c r="N19" s="122">
         <f t="shared" si="12"/>
         <v>16</v>
       </c>
@@ -3713,9 +3771,9 @@
         <v>subject17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="C20" s="71" t="str">
+        <v>345</v>
+      </c>
+      <c r="C20" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3726,25 +3784,28 @@
         <v>20</v>
       </c>
       <c r="F20" s="63"/>
-      <c r="G20" s="63" t="str">
+      <c r="G20" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" s="63" t="str">
         <f t="shared" si="9"/>
         <v>017</v>
       </c>
-      <c r="H20" s="119" t="s">
+      <c r="I20" s="118" t="s">
+        <v>346</v>
+      </c>
+      <c r="J20" s="119" t="s">
         <v>344</v>
       </c>
-      <c r="I20" s="120" t="s">
-        <v>342</v>
-      </c>
-      <c r="J20" s="63"/>
-      <c r="K20" s="121" t="str">
+      <c r="K20" s="63"/>
+      <c r="L20" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L20" s="122" t="s">
-        <v>345</v>
-      </c>
-      <c r="M20" s="123">
+      <c r="M20" s="121" t="s">
+        <v>347</v>
+      </c>
+      <c r="N20" s="122">
         <f t="shared" si="12"/>
         <v>17</v>
       </c>
@@ -3755,9 +3816,9 @@
         <v>subject18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C21" s="71" t="str">
+        <v>348</v>
+      </c>
+      <c r="C21" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3768,27 +3829,30 @@
         <v>20</v>
       </c>
       <c r="F21" s="63"/>
-      <c r="G21" s="63" t="str">
+      <c r="G21" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="63" t="str">
         <f t="shared" si="9"/>
         <v>018</v>
       </c>
-      <c r="H21" s="119" t="str">
+      <c r="I21" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I21" s="120" t="s">
-        <v>342</v>
-      </c>
-      <c r="J21" s="63"/>
-      <c r="K21" s="121" t="str">
+      <c r="J21" s="119" t="s">
+        <v>344</v>
+      </c>
+      <c r="K21" s="63"/>
+      <c r="L21" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L21" s="122" t="str">
+      <c r="M21" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M21" s="123">
+      <c r="N21" s="122">
         <f t="shared" si="12"/>
         <v>18</v>
       </c>
@@ -3799,9 +3863,9 @@
         <v>subject19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C22" s="71" t="str">
+        <v>349</v>
+      </c>
+      <c r="C22" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programA</v>
       </c>
@@ -3812,40 +3876,43 @@
         <v>20</v>
       </c>
       <c r="F22" s="63"/>
-      <c r="G22" s="63" t="str">
+      <c r="G22" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="63" t="str">
         <f t="shared" si="9"/>
         <v>019</v>
       </c>
-      <c r="H22" s="119" t="str">
+      <c r="I22" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="I22" s="120" t="s">
-        <v>342</v>
-      </c>
-      <c r="J22" s="63"/>
-      <c r="K22" s="121" t="str">
+      <c r="J22" s="119" t="s">
+        <v>344</v>
+      </c>
+      <c r="K22" s="63"/>
+      <c r="L22" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="L22" s="122" t="str">
+      <c r="M22" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="M22" s="123">
+      <c r="N22" s="122">
         <f t="shared" si="12"/>
         <v>19</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="10" t="str">
-        <f t="shared" ref="A23:A24" si="15">_xlfn.CONCAT("asignatura",IF(M23&lt;10,"0",""),M23)</f>
+        <f t="shared" ref="A23:A24" si="15">_xlfn.CONCAT("asignatura",IF(N23&lt;10,"0",""),N23)</f>
         <v>asignatura01</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>348</v>
-      </c>
-      <c r="C23" s="71" t="str">
+        <v>350</v>
+      </c>
+      <c r="C23" s="70" t="str">
         <f>ap_programs!A6</f>
         <v>programC</v>
       </c>
@@ -3856,25 +3923,28 @@
         <v>20</v>
       </c>
       <c r="F23" s="63"/>
-      <c r="G23" s="63" t="str">
+      <c r="G23" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H23" s="63" t="str">
         <f t="shared" si="9"/>
         <v>001</v>
       </c>
-      <c r="H23" s="119" t="s">
-        <v>349</v>
-      </c>
-      <c r="I23" s="120" t="s">
-        <v>350</v>
-      </c>
-      <c r="J23" s="63"/>
-      <c r="K23" s="121" t="str">
+      <c r="I23" s="118" t="s">
+        <v>351</v>
+      </c>
+      <c r="J23" s="119" t="s">
+        <v>352</v>
+      </c>
+      <c r="K23" s="63"/>
+      <c r="L23" s="120" t="str">
         <f>ap_subject_types!$A$6</f>
         <v>type04</v>
       </c>
-      <c r="L23" s="122" t="s">
-        <v>351</v>
-      </c>
-      <c r="M23" s="123">
+      <c r="M23" s="121" t="s">
+        <v>353</v>
+      </c>
+      <c r="N23" s="122">
         <v>1</v>
       </c>
     </row>
@@ -3884,9 +3954,9 @@
         <v>asignatura02</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="C24" s="71" t="str">
+        <v>354</v>
+      </c>
+      <c r="C24" s="70" t="str">
         <f t="shared" si="10"/>
         <v>programC</v>
       </c>
@@ -3897,34 +3967,37 @@
         <v>20</v>
       </c>
       <c r="F24" s="63"/>
-      <c r="G24" s="63" t="str">
+      <c r="G24" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H24" s="63" t="str">
         <f t="shared" si="9"/>
         <v>002</v>
       </c>
-      <c r="H24" s="119" t="str">
+      <c r="I24" s="118" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">2ºA|2ºA, 2ºB|2ºB</v>
       </c>
-      <c r="I24" s="120" t="s">
-        <v>353</v>
-      </c>
-      <c r="J24" s="63"/>
-      <c r="K24" s="121" t="str">
+      <c r="J24" s="119" t="s">
+        <v>355</v>
+      </c>
+      <c r="K24" s="63"/>
+      <c r="L24" s="120" t="str">
         <f>ap_subject_types!$A$6</f>
         <v>type04</v>
       </c>
-      <c r="L24" s="122" t="str">
+      <c r="M24" s="121" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">teacher01|main@2ºA, teacher01|main@2ºB</v>
       </c>
-      <c r="M24" s="123">
+      <c r="N24" s="122">
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I2:M2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -5111,7 +5184,7 @@
       <c r="I6" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J6" s="71" t="s">
+      <c r="J6" s="70" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5143,7 +5216,7 @@
       <c r="I7" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J7" s="71" t="s">
+      <c r="J7" s="70" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5175,7 +5248,7 @@
       <c r="I8" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J8" s="71" t="s">
+      <c r="J8" s="70" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5207,7 +5280,7 @@
       <c r="I9" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="J9" s="71" t="s">
+      <c r="J9" s="70" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5227,7 +5300,7 @@
       <c r="E10" s="68">
         <v>38718</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="71" t="s">
         <v>173</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -5239,7 +5312,7 @@
       <c r="I10" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J10" s="71" t="s">
+      <c r="J10" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5259,7 +5332,7 @@
       <c r="E11" s="68">
         <v>38749</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="71" t="s">
         <v>178</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -5271,7 +5344,7 @@
       <c r="I11" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J11" s="71" t="s">
+      <c r="J11" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5291,7 +5364,7 @@
       <c r="E12" s="68">
         <v>38777</v>
       </c>
-      <c r="F12" s="72" t="s">
+      <c r="F12" s="71" t="s">
         <v>182</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -5303,7 +5376,7 @@
       <c r="I12" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J12" s="71" t="s">
+      <c r="J12" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5323,7 +5396,7 @@
       <c r="E13" s="68">
         <v>38808</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="71" t="s">
         <v>186</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -5335,7 +5408,7 @@
       <c r="I13" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J13" s="71" t="s">
+      <c r="J13" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5355,7 +5428,7 @@
       <c r="E14" s="68">
         <v>38838</v>
       </c>
-      <c r="F14" s="72" t="s">
+      <c r="F14" s="71" t="s">
         <v>190</v>
       </c>
       <c r="G14" s="11" t="s">
@@ -5367,7 +5440,7 @@
       <c r="I14" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J14" s="71" t="s">
+      <c r="J14" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5387,7 +5460,7 @@
       <c r="E15" s="68">
         <v>38869</v>
       </c>
-      <c r="F15" s="72" t="s">
+      <c r="F15" s="71" t="s">
         <v>194</v>
       </c>
       <c r="G15" s="11" t="s">
@@ -5399,7 +5472,7 @@
       <c r="I15" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="J15" s="71" t="s">
+      <c r="J15" s="70" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5424,7 +5497,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00930025-0041-4827-80E9-00F100810047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0010008A-002F-4BF6-BB6F-003E005A00F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -5466,7 +5539,7 @@
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5474,7 +5547,7 @@
       <c r="A3" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="70" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
@@ -5483,7 +5556,7 @@
       <c r="A4" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="71" t="str">
+      <c r="B4" s="70" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -5534,16 +5607,16 @@
       </c>
     </row>
     <row r="2" ht="24.25" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="75" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="72" t="s">
         <v>201</v>
       </c>
       <c r="E2" s="67" t="s">
@@ -5557,13 +5630,13 @@
       <c r="B3" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="70" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5575,7 +5648,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00730039-002A-483B-82A6-00D300DE0098}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00520059-00A6-4A17-AE84-0008000600DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5631,25 +5704,25 @@
       </c>
     </row>
     <row r="2" ht="16">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="77" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="77" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="G2" s="78" t="s">
+      <c r="G2" s="77" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5660,7 +5733,7 @@
       <c r="B3" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="71" t="str">
+      <c r="C3" s="70" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
@@ -5670,10 +5743,10 @@
       <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="G3" s="81">
+      <c r="G3" s="80">
         <v>5</v>
       </c>
     </row>
@@ -5684,7 +5757,7 @@
       <c r="B4" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="71" t="str">
+      <c r="C4" s="70" t="str">
         <f>centers!$A$5</f>
         <v>centerC</v>
       </c>
@@ -5694,10 +5767,10 @@
       <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="F4" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="G4" s="81">
+      <c r="G4" s="80">
         <v>5</v>
       </c>
     </row>
@@ -5709,13 +5782,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00F700D7-00CB-4060-BE33-00DD00BC0037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A000DB-00FC-437F-A1D1-00AC00410009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A900FF-00CF-4DF6-A121-006900A4004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005D001C-008B-47E5-83AD-007F0029009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -5753,10 +5826,10 @@
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="75" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5764,7 +5837,7 @@
       <c r="A3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="71" t="str">
+      <c r="B3" s="70" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
@@ -5773,7 +5846,7 @@
       <c r="A4" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="71" t="str">
+      <c r="B4" s="70" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -5912,107 +5985,107 @@
       <c r="AN1" s="5"/>
     </row>
     <row r="2" s="9" customFormat="1" ht="23.5" customHeight="1">
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="81" t="s">
         <v>242</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="83" t="s">
+      <c r="G2" s="81"/>
+      <c r="H2" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="86" t="s">
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="87" t="s">
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="86" t="s">
         <v>245</v>
       </c>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="90" t="s">
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="89" t="s">
         <v>246</v>
       </c>
-      <c r="W2" s="91"/>
-      <c r="X2" s="91"/>
+      <c r="W2" s="90"/>
+      <c r="X2" s="90"/>
     </row>
     <row r="3" ht="34" customHeight="1">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="92" t="s">
         <v>247</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="94" t="s">
         <v>248</v>
       </c>
-      <c r="F3" s="96" t="s">
+      <c r="F3" s="95" t="s">
         <v>249</v>
       </c>
-      <c r="G3" s="97" t="s">
+      <c r="G3" s="96" t="s">
         <v>250</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="97" t="s">
         <v>251</v>
       </c>
-      <c r="I3" s="99" t="s">
+      <c r="I3" s="98" t="s">
         <v>252</v>
       </c>
-      <c r="J3" s="100" t="s">
+      <c r="J3" s="99" t="s">
         <v>253</v>
       </c>
-      <c r="K3" s="100" t="s">
+      <c r="K3" s="99" t="s">
         <v>254</v>
       </c>
-      <c r="L3" s="100" t="s">
+      <c r="L3" s="99" t="s">
         <v>255</v>
       </c>
-      <c r="M3" s="100" t="s">
+      <c r="M3" s="99" t="s">
         <v>256</v>
       </c>
-      <c r="N3" s="100" t="s">
+      <c r="N3" s="99" t="s">
         <v>257</v>
       </c>
-      <c r="O3" s="101" t="s">
+      <c r="O3" s="100" t="s">
         <v>258</v>
       </c>
-      <c r="P3" s="102" t="s">
+      <c r="P3" s="101" t="s">
         <v>256</v>
       </c>
-      <c r="Q3" s="103" t="s">
+      <c r="Q3" s="102" t="s">
         <v>257</v>
       </c>
-      <c r="R3" s="104" t="s">
+      <c r="R3" s="103" t="s">
         <v>259</v>
       </c>
-      <c r="S3" s="105" t="s">
+      <c r="S3" s="104" t="s">
         <v>260</v>
       </c>
-      <c r="T3" s="105" t="s">
+      <c r="T3" s="104" t="s">
         <v>256</v>
       </c>
-      <c r="U3" s="105" t="s">
+      <c r="U3" s="104" t="s">
         <v>257</v>
       </c>
-      <c r="V3" s="106" t="s">
+      <c r="V3" s="105" t="s">
         <v>256</v>
       </c>
-      <c r="W3" s="107" t="s">
+      <c r="W3" s="106" t="s">
         <v>261</v>
       </c>
-      <c r="X3" s="108" t="s">
+      <c r="X3" s="107" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6047,7 +6120,7 @@
       <c r="J4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="109"/>
+      <c r="K4" s="108"/>
       <c r="L4" s="63"/>
       <c r="M4" s="63"/>
       <c r="N4" s="63"/>
@@ -6113,7 +6186,7 @@
       <c r="J5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="109" t="s">
+      <c r="K5" s="108" t="s">
         <v>269</v>
       </c>
       <c r="L5" s="63" t="s">
@@ -6187,7 +6260,7 @@
       <c r="J6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="109" t="s">
+      <c r="K6" s="108" t="s">
         <v>272</v>
       </c>
       <c r="L6" s="63" t="s">
@@ -6243,13 +6316,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007A0006-004B-4ECA-BE3B-0047009400FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AB0038-0056-4290-9B23-00E800E400BC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>J4:J6 F4:F6 S4 U4:U6 W4:X6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00910010-0084-4272-87E8-00CF007D00EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00120069-0084-44F2-9CF9-00DC00BB0020}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPDATE: MVP Template now add students to classes
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="360">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -958,6 +958,9 @@
     <t>teachers</t>
   </si>
   <si>
+    <t>students</t>
+  </si>
+  <si>
     <t xml:space="preserve">Class config</t>
   </si>
   <si>
@@ -985,6 +988,9 @@
     <t>Teachers</t>
   </si>
   <si>
+    <t>Students</t>
+  </si>
+  <si>
     <t xml:space="preserve">Language I</t>
   </si>
   <si>
@@ -997,6 +1003,9 @@
     <t xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</t>
   </si>
   <si>
+    <t xml:space="preserve">studentB01@G1A, studentB02@G1A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Math I</t>
   </si>
   <si>
@@ -1094,6 +1103,9 @@
   </si>
   <si>
     <t xml:space="preserve">teacher01|main@2ºA, teacher01|main@2ºB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">studentC01@2ºA, studentC02@2ºA, studentC03@2ºA, studentC04@2ºB, studentC05@2ºB, studentC06@2ºB</t>
   </si>
   <si>
     <t xml:space="preserve">Lengua Castellana y Literatura</t>
@@ -1921,9 +1933,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="5" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1967,6 +1976,9 @@
     </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2660,10 +2672,10 @@
       <c r="C2" s="93" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="109" t="s">
         <v>252</v>
       </c>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="109" t="s">
         <v>279</v>
       </c>
     </row>
@@ -2747,7 +2759,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007000BE-00CB-47A3-889B-001100A300C0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009100C1-00B2-404B-AD13-0059008D003B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -2803,7 +2815,7 @@
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="110" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="77" t="s">
@@ -2821,7 +2833,7 @@
       <c r="F2" s="78" t="s">
         <v>278</v>
       </c>
-      <c r="G2" s="112" t="s">
+      <c r="G2" s="111" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2838,7 +2850,7 @@
       <c r="D3" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="112" t="s">
         <v>295</v>
       </c>
       <c r="F3" s="70" t="str">
@@ -2893,7 +2905,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A1" workbookViewId="0" zoomScale="160">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0" zoomScale="160">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A4" ySplit="3"/>
       <selection activeCell="L23" activeCellId="0" sqref="L23"/>
     </sheetView>
@@ -2909,7 +2921,8 @@
     <col customWidth="1" min="11" max="11" width="11.83203125"/>
     <col customWidth="1" min="12" max="12" width="10.1640625"/>
     <col customWidth="1" min="13" max="13" width="23.33203125"/>
-    <col customWidth="1" min="14" max="14" width="3.5"/>
+    <col customWidth="1" min="14" max="14" width="55.140625"/>
+    <col customWidth="1" min="15" max="15" width="3.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2949,10 +2962,13 @@
       <c r="L1" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="M1" s="114" t="s">
+      <c r="M1" s="113" t="s">
         <v>307</v>
       </c>
-      <c r="N1" s="14"/>
+      <c r="N1" s="113" t="s">
+        <v>308</v>
+      </c>
+      <c r="O1" s="14"/>
     </row>
     <row r="2" ht="28.75" customHeight="1">
       <c r="A2" s="5"/>
@@ -2964,16 +2980,17 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="14"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" ht="31.75" customHeight="1">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="110" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="77" t="s">
@@ -2983,44 +3000,47 @@
         <v>278</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E3" s="77" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F3" s="92" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G3" s="92" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H3" s="92" t="s">
-        <v>312</v>
-      </c>
-      <c r="I3" s="115" t="s">
         <v>313</v>
       </c>
-      <c r="J3" s="116" t="s">
+      <c r="I3" s="114" t="s">
+        <v>314</v>
+      </c>
+      <c r="J3" s="115" t="s">
         <v>289</v>
       </c>
-      <c r="K3" s="116" t="s">
-        <v>314</v>
-      </c>
-      <c r="L3" s="117" t="s">
+      <c r="K3" s="115" t="s">
         <v>315</v>
       </c>
+      <c r="L3" s="116" t="s">
+        <v>316</v>
+      </c>
       <c r="M3" s="78" t="s">
-        <v>316</v>
-      </c>
-      <c r="N3" s="118"/>
+        <v>317</v>
+      </c>
+      <c r="N3" s="78" t="s">
+        <v>318</v>
+      </c>
+      <c r="O3" s="117"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
-        <f t="shared" ref="A4:A9" si="1">_xlfn.CONCAT("subject",IF(N4&lt;10,"0",""),N4)</f>
+        <f>_xlfn.CONCAT("subject",IF(O4&lt;10,"0",""),O4)</f>
         <v>subject01</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C4" s="70" t="str">
         <f>ap_programs!A4</f>
@@ -3037,37 +3057,40 @@
       </c>
       <c r="G4" s="63"/>
       <c r="H4" s="63" t="str">
-        <f t="shared" ref="H4:H9" si="2">_xlfn.CONCAT("0",IF(N4&lt;10,"0",""),N4)</f>
+        <f>_xlfn.CONCAT("0",IF(O4&lt;10,"0",""),O4)</f>
         <v>001</v>
       </c>
-      <c r="I4" s="119" t="s">
-        <v>318</v>
-      </c>
-      <c r="J4" s="120" t="s">
-        <v>319</v>
+      <c r="I4" s="118" t="s">
+        <v>320</v>
+      </c>
+      <c r="J4" s="119" t="s">
+        <v>321</v>
       </c>
       <c r="K4" s="63"/>
-      <c r="L4" s="121" t="str">
+      <c r="L4" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M4" s="122" t="s">
-        <v>320</v>
-      </c>
-      <c r="N4" s="123">
+      <c r="M4" s="121" t="s">
+        <v>322</v>
+      </c>
+      <c r="N4" s="121" t="s">
+        <v>323</v>
+      </c>
+      <c r="O4" s="122">
         <v>1</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="10" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("subject",IF(O5&lt;10,"0",""),O5)</f>
         <v>subject02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C5" s="70" t="str">
-        <f t="shared" ref="C5:C10" si="3">C4</f>
+        <f t="shared" ref="C5:C10" si="1">C4</f>
         <v>programA</v>
       </c>
       <c r="D5" s="63">
@@ -3081,41 +3104,45 @@
       </c>
       <c r="G5" s="63"/>
       <c r="H5" s="63" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("0",IF(O5&lt;10,"0",""),O5)</f>
         <v>002</v>
       </c>
-      <c r="I5" s="119" t="str">
-        <f t="shared" ref="I5:I10" si="4">I4</f>
+      <c r="I5" s="118" t="str">
+        <f t="shared" ref="I5:I10" si="2">I4</f>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="J5" s="120" t="str">
-        <f t="shared" ref="J5:J10" si="5">J4</f>
+      <c r="J5" s="119" t="str">
+        <f t="shared" ref="J5:J10" si="3">J4</f>
         <v>#FFEB9C</v>
       </c>
       <c r="K5" s="63"/>
-      <c r="L5" s="121" t="str">
+      <c r="L5" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M5" s="122" t="str">
-        <f t="shared" ref="M5:M10" si="6">M4</f>
+      <c r="M5" s="121" t="str">
+        <f t="shared" ref="M5:M10" si="4">M4</f>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="N5" s="123">
-        <f t="shared" ref="N5:N10" si="7">N4+1</f>
+      <c r="N5" s="121" t="str">
+        <f>N4</f>
+        <v xml:space="preserve">studentB01@G1A, studentB02@G1A</v>
+      </c>
+      <c r="O5" s="122">
+        <f>O4+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(O6&lt;10,"0",""),O6)</f>
+        <v>subject03</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" s="70" t="str">
         <f t="shared" si="1"/>
-        <v>subject03</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>322</v>
-      </c>
-      <c r="C6" s="70" t="str">
-        <f t="shared" si="3"/>
         <v>programA</v>
       </c>
       <c r="D6" s="63">
@@ -3129,41 +3156,45 @@
       </c>
       <c r="G6" s="63"/>
       <c r="H6" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(O6&lt;10,"0",""),O6)</f>
+        <v>003</v>
+      </c>
+      <c r="I6" s="118" t="str">
         <f t="shared" si="2"/>
-        <v>003</v>
-      </c>
-      <c r="I6" s="119" t="str">
-        <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="J6" s="120" t="str">
-        <f t="shared" si="5"/>
+      <c r="J6" s="119" t="str">
+        <f t="shared" si="3"/>
         <v>#FFEB9C</v>
       </c>
       <c r="K6" s="63"/>
-      <c r="L6" s="121" t="str">
+      <c r="L6" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M6" s="122" t="str">
-        <f t="shared" si="6"/>
+      <c r="M6" s="121" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="N6" s="123">
-        <f t="shared" si="7"/>
+      <c r="N6" s="121" t="str">
+        <f>N5</f>
+        <v xml:space="preserve">studentB01@G1A, studentB02@G1A</v>
+      </c>
+      <c r="O6" s="122">
+        <f>O5+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(O7&lt;10,"0",""),O7)</f>
+        <v>subject04</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" s="70" t="str">
         <f t="shared" si="1"/>
-        <v>subject04</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="C7" s="70" t="str">
-        <f t="shared" si="3"/>
         <v>programA</v>
       </c>
       <c r="D7" s="63">
@@ -3177,41 +3208,45 @@
       </c>
       <c r="G7" s="63"/>
       <c r="H7" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(O7&lt;10,"0",""),O7)</f>
+        <v>004</v>
+      </c>
+      <c r="I7" s="118" t="str">
         <f t="shared" si="2"/>
-        <v>004</v>
-      </c>
-      <c r="I7" s="119" t="str">
-        <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G1A, Group B|G1B</v>
       </c>
-      <c r="J7" s="120" t="str">
-        <f t="shared" si="5"/>
+      <c r="J7" s="119" t="str">
+        <f t="shared" si="3"/>
         <v>#FFEB9C</v>
       </c>
       <c r="K7" s="63"/>
-      <c r="L7" s="121" t="str">
+      <c r="L7" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="M7" s="122" t="str">
-        <f t="shared" si="6"/>
+      <c r="M7" s="121" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">teacher01|main@G1A, teacher01|main@G1B</v>
       </c>
-      <c r="N7" s="123">
-        <f t="shared" si="7"/>
+      <c r="N7" s="121" t="str">
+        <f>N6</f>
+        <v xml:space="preserve">studentB01@G1A, studentB02@G1A</v>
+      </c>
+      <c r="O7" s="122">
+        <f>O6+1</f>
         <v>4</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(O8&lt;10,"0",""),O8)</f>
+        <v>subject05</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="C8" s="70" t="str">
         <f t="shared" si="1"/>
-        <v>subject05</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="C8" s="70" t="str">
-        <f t="shared" si="3"/>
         <v>programA</v>
       </c>
       <c r="D8" s="63">
@@ -3225,39 +3260,40 @@
       </c>
       <c r="G8" s="63"/>
       <c r="H8" s="63" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT("0",IF(O8&lt;10,"0",""),O8)</f>
         <v>005</v>
       </c>
-      <c r="I8" s="119" t="s">
-        <v>325</v>
-      </c>
-      <c r="J8" s="120" t="str">
-        <f t="shared" si="5"/>
+      <c r="I8" s="118" t="s">
+        <v>328</v>
+      </c>
+      <c r="J8" s="119" t="str">
+        <f t="shared" si="3"/>
         <v>#FFEB9C</v>
       </c>
       <c r="K8" s="63"/>
-      <c r="L8" s="121" t="str">
+      <c r="L8" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M8" s="122" t="s">
-        <v>326</v>
-      </c>
-      <c r="N8" s="123">
-        <f t="shared" si="7"/>
+      <c r="M8" s="121" t="s">
+        <v>329</v>
+      </c>
+      <c r="N8" s="121"/>
+      <c r="O8" s="122">
+        <f>O7+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="10" t="str">
+        <f>_xlfn.CONCAT("subject",IF(O9&lt;10,"0",""),O9)</f>
+        <v>subject06</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" s="70" t="str">
         <f t="shared" si="1"/>
-        <v>subject06</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="C9" s="70" t="str">
-        <f t="shared" si="3"/>
         <v>programA</v>
       </c>
       <c r="D9" s="63">
@@ -3271,40 +3307,41 @@
       </c>
       <c r="G9" s="63"/>
       <c r="H9" s="63" t="str">
+        <f>_xlfn.CONCAT("0",IF(O9&lt;10,"0",""),O9)</f>
+        <v>006</v>
+      </c>
+      <c r="I9" s="118" t="str">
         <f t="shared" si="2"/>
-        <v>006</v>
-      </c>
-      <c r="I9" s="119" t="str">
-        <f t="shared" si="4"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="J9" s="120" t="s">
-        <v>328</v>
+      <c r="J9" s="119" t="s">
+        <v>331</v>
       </c>
       <c r="K9" s="63"/>
-      <c r="L9" s="121" t="str">
+      <c r="L9" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M9" s="122" t="str">
-        <f t="shared" si="6"/>
+      <c r="M9" s="121" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="N9" s="123">
-        <f t="shared" si="7"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="122">
+        <f>O8+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="10" t="str">
-        <f t="shared" ref="A10:A22" si="8">_xlfn.CONCAT("subject",IF(N10&lt;10,"0",""),N10)</f>
+        <f>_xlfn.CONCAT("subject",IF(O10&lt;10,"0",""),O10)</f>
         <v>subject07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C10" s="70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>programA</v>
       </c>
       <c r="D10" s="63">
@@ -3318,41 +3355,42 @@
       </c>
       <c r="G10" s="63"/>
       <c r="H10" s="63" t="str">
-        <f t="shared" ref="H10:H24" si="9">_xlfn.CONCAT("0",IF(N10&lt;10,"0",""),N10)</f>
+        <f>_xlfn.CONCAT("0",IF(O10&lt;10,"0",""),O10)</f>
         <v>007</v>
       </c>
-      <c r="I10" s="119" t="str">
-        <f t="shared" si="4"/>
+      <c r="I10" s="118" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="J10" s="120" t="str">
-        <f t="shared" si="5"/>
+      <c r="J10" s="119" t="str">
+        <f t="shared" si="3"/>
         <v>#FFC7CE</v>
       </c>
       <c r="K10" s="63"/>
-      <c r="L10" s="121" t="str">
+      <c r="L10" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M10" s="122" t="str">
-        <f t="shared" si="6"/>
+      <c r="M10" s="121" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="N10" s="123">
-        <f t="shared" si="7"/>
+      <c r="N10" s="121"/>
+      <c r="O10" s="122">
+        <f>O9+1</f>
         <v>7</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O11&lt;10,"0",""),O11)</f>
         <v>subject08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C11" s="70" t="str">
-        <f t="shared" ref="C11:C24" si="10">C10</f>
+        <f t="shared" ref="C11:C24" si="5">C10</f>
         <v>programA</v>
       </c>
       <c r="D11" s="63">
@@ -3366,41 +3404,42 @@
       </c>
       <c r="G11" s="63"/>
       <c r="H11" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O11&lt;10,"0",""),O11)</f>
         <v>008</v>
       </c>
-      <c r="I11" s="119" t="str">
+      <c r="I11" s="118" t="str">
         <f>I10</f>
         <v xml:space="preserve">Group A|G2A, Group B|G2B</v>
       </c>
-      <c r="J11" s="120" t="str">
-        <f t="shared" ref="J11:J18" si="11">J10</f>
+      <c r="J11" s="119" t="str">
+        <f t="shared" ref="J11:J18" si="6">J10</f>
         <v>#FFC7CE</v>
       </c>
       <c r="K11" s="63"/>
-      <c r="L11" s="121" t="str">
+      <c r="L11" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="M11" s="122" t="str">
+      <c r="M11" s="121" t="str">
         <f>M10</f>
         <v xml:space="preserve">teacher01|main@G2A, teacher01|main@G2B</v>
       </c>
-      <c r="N11" s="123">
-        <f t="shared" ref="N11:N24" si="12">N10+1</f>
+      <c r="N11" s="121"/>
+      <c r="O11" s="122">
+        <f>O10+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
       <c r="A12" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O12&lt;10,"0",""),O12)</f>
         <v>subject09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C12" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D12" s="63">
@@ -3414,39 +3453,40 @@
       </c>
       <c r="G12" s="63"/>
       <c r="H12" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O12&lt;10,"0",""),O12)</f>
         <v>009</v>
       </c>
-      <c r="I12" s="119" t="s">
-        <v>332</v>
-      </c>
-      <c r="J12" s="120" t="str">
-        <f t="shared" si="11"/>
+      <c r="I12" s="118" t="s">
+        <v>335</v>
+      </c>
+      <c r="J12" s="119" t="str">
+        <f t="shared" si="6"/>
         <v>#FFC7CE</v>
       </c>
       <c r="K12" s="63"/>
-      <c r="L12" s="121" t="str">
+      <c r="L12" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M12" s="122" t="s">
-        <v>333</v>
-      </c>
-      <c r="N12" s="123">
-        <f t="shared" si="12"/>
+      <c r="M12" s="121" t="s">
+        <v>336</v>
+      </c>
+      <c r="N12" s="121"/>
+      <c r="O12" s="122">
+        <f>O11+1</f>
         <v>9</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O13&lt;10,"0",""),O13)</f>
         <v>subject10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C13" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D13" s="63">
@@ -3460,41 +3500,42 @@
       </c>
       <c r="G13" s="63"/>
       <c r="H13" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O13&lt;10,"0",""),O13)</f>
         <v>010</v>
       </c>
-      <c r="I13" s="119" t="str">
-        <f t="shared" ref="I13:I24" si="13">I12</f>
+      <c r="I13" s="118" t="str">
+        <f t="shared" ref="I13:I24" si="7">I12</f>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="J13" s="120" t="str">
-        <f t="shared" si="11"/>
+      <c r="J13" s="119" t="str">
+        <f t="shared" si="6"/>
         <v>#FFC7CE</v>
       </c>
       <c r="K13" s="63"/>
-      <c r="L13" s="121" t="str">
+      <c r="L13" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M13" s="122" t="str">
-        <f t="shared" ref="M13:M24" si="14">M12</f>
+      <c r="M13" s="121" t="str">
+        <f t="shared" ref="M13:M24" si="8">M12</f>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="N13" s="123">
-        <f t="shared" si="12"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="122">
+        <f>O12+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O14&lt;10,"0",""),O14)</f>
         <v>subject11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C14" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D14" s="63">
@@ -3508,40 +3549,41 @@
       </c>
       <c r="G14" s="63"/>
       <c r="H14" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O14&lt;10,"0",""),O14)</f>
         <v>011</v>
       </c>
-      <c r="I14" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I14" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="J14" s="120" t="s">
-        <v>336</v>
+      <c r="J14" s="119" t="s">
+        <v>339</v>
       </c>
       <c r="K14" s="63"/>
-      <c r="L14" s="121" t="str">
+      <c r="L14" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M14" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M14" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="N14" s="123">
-        <f t="shared" si="12"/>
+      <c r="N14" s="121"/>
+      <c r="O14" s="122">
+        <f>O13+1</f>
         <v>11</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O15&lt;10,"0",""),O15)</f>
         <v>subject12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="C15" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D15" s="63">
@@ -3555,41 +3597,42 @@
       </c>
       <c r="G15" s="63"/>
       <c r="H15" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O15&lt;10,"0",""),O15)</f>
         <v>012</v>
       </c>
-      <c r="I15" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I15" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">Group A|G3A, Group B|G3B</v>
       </c>
-      <c r="J15" s="120" t="str">
-        <f t="shared" si="11"/>
+      <c r="J15" s="119" t="str">
+        <f t="shared" si="6"/>
         <v>#C6EFCD</v>
       </c>
       <c r="K15" s="63"/>
-      <c r="L15" s="121" t="str">
+      <c r="L15" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="M15" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M15" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@G3A, teacher01|main@G3B</v>
       </c>
-      <c r="N15" s="123">
-        <f t="shared" si="12"/>
+      <c r="N15" s="121"/>
+      <c r="O15" s="122">
+        <f>O14+1</f>
         <v>12</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O16&lt;10,"0",""),O16)</f>
         <v>subject13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C16" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D16" s="63">
@@ -3603,39 +3646,40 @@
       </c>
       <c r="G16" s="63"/>
       <c r="H16" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O16&lt;10,"0",""),O16)</f>
         <v>013</v>
       </c>
-      <c r="I16" s="119" t="s">
-        <v>339</v>
-      </c>
-      <c r="J16" s="120" t="str">
-        <f t="shared" si="11"/>
+      <c r="I16" s="118" t="s">
+        <v>342</v>
+      </c>
+      <c r="J16" s="119" t="str">
+        <f t="shared" si="6"/>
         <v>#C6EFCD</v>
       </c>
       <c r="K16" s="63"/>
-      <c r="L16" s="121" t="str">
+      <c r="L16" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M16" s="122" t="s">
-        <v>340</v>
-      </c>
-      <c r="N16" s="123">
-        <f t="shared" si="12"/>
+      <c r="M16" s="121" t="s">
+        <v>343</v>
+      </c>
+      <c r="N16" s="121"/>
+      <c r="O16" s="122">
+        <f>O15+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O17&lt;10,"0",""),O17)</f>
         <v>subject14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C17" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D17" s="63">
@@ -3649,41 +3693,42 @@
       </c>
       <c r="G17" s="63"/>
       <c r="H17" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O17&lt;10,"0",""),O17)</f>
         <v>014</v>
       </c>
-      <c r="I17" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I17" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="J17" s="120" t="str">
-        <f t="shared" si="11"/>
+      <c r="J17" s="119" t="str">
+        <f t="shared" si="6"/>
         <v>#C6EFCD</v>
       </c>
       <c r="K17" s="63"/>
-      <c r="L17" s="121" t="str">
+      <c r="L17" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M17" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M17" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="N17" s="123">
-        <f t="shared" si="12"/>
+      <c r="N17" s="121"/>
+      <c r="O17" s="122">
+        <f>O16+1</f>
         <v>14</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O18&lt;10,"0",""),O18)</f>
         <v>subject15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C18" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D18" s="63">
@@ -3697,41 +3742,42 @@
       </c>
       <c r="G18" s="63"/>
       <c r="H18" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O18&lt;10,"0",""),O18)</f>
         <v>015</v>
       </c>
-      <c r="I18" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I18" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="J18" s="120" t="str">
-        <f t="shared" si="11"/>
+      <c r="J18" s="119" t="str">
+        <f t="shared" si="6"/>
         <v>#C6EFCD</v>
       </c>
       <c r="K18" s="63"/>
-      <c r="L18" s="121" t="str">
+      <c r="L18" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M18" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M18" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="N18" s="123">
-        <f t="shared" si="12"/>
+      <c r="N18" s="121"/>
+      <c r="O18" s="122">
+        <f>O17+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1">
       <c r="A19" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O19&lt;10,"0",""),O19)</f>
         <v>subject16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C19" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D19" s="63">
@@ -3745,40 +3791,41 @@
       </c>
       <c r="G19" s="63"/>
       <c r="H19" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O19&lt;10,"0",""),O19)</f>
         <v>016</v>
       </c>
-      <c r="I19" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I19" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">Group A|G4A, Group B|G4B</v>
       </c>
-      <c r="J19" s="120" t="s">
-        <v>344</v>
+      <c r="J19" s="119" t="s">
+        <v>347</v>
       </c>
       <c r="K19" s="63"/>
-      <c r="L19" s="121" t="str">
+      <c r="L19" s="120" t="str">
         <f>ap_subject_types!$A$5</f>
         <v>type03</v>
       </c>
-      <c r="M19" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M19" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@G4A, teacher01|main@G4B</v>
       </c>
-      <c r="N19" s="123">
-        <f t="shared" si="12"/>
+      <c r="N19" s="121"/>
+      <c r="O19" s="122">
+        <f>O18+1</f>
         <v>16</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O20&lt;10,"0",""),O20)</f>
         <v>subject17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C20" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D20" s="63">
@@ -3792,38 +3839,39 @@
       </c>
       <c r="G20" s="63"/>
       <c r="H20" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O20&lt;10,"0",""),O20)</f>
         <v>017</v>
       </c>
-      <c r="I20" s="119" t="s">
-        <v>346</v>
-      </c>
-      <c r="J20" s="120" t="s">
-        <v>344</v>
+      <c r="I20" s="118" t="s">
+        <v>349</v>
+      </c>
+      <c r="J20" s="119" t="s">
+        <v>347</v>
       </c>
       <c r="K20" s="63"/>
-      <c r="L20" s="121" t="str">
+      <c r="L20" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M20" s="122" t="s">
-        <v>347</v>
-      </c>
-      <c r="N20" s="123">
-        <f t="shared" si="12"/>
+      <c r="M20" s="121" t="s">
+        <v>350</v>
+      </c>
+      <c r="N20" s="121"/>
+      <c r="O20" s="122">
+        <f>O19+1</f>
         <v>17</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
       <c r="A21" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O21&lt;10,"0",""),O21)</f>
         <v>subject18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C21" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D21" s="63">
@@ -3837,40 +3885,41 @@
       </c>
       <c r="G21" s="63"/>
       <c r="H21" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O21&lt;10,"0",""),O21)</f>
         <v>018</v>
       </c>
-      <c r="I21" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I21" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="J21" s="120" t="s">
-        <v>344</v>
+      <c r="J21" s="119" t="s">
+        <v>347</v>
       </c>
       <c r="K21" s="63"/>
-      <c r="L21" s="121" t="str">
+      <c r="L21" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M21" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M21" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="N21" s="123">
-        <f t="shared" si="12"/>
+      <c r="N21" s="121"/>
+      <c r="O21" s="122">
+        <f>O20+1</f>
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT("subject",IF(O22&lt;10,"0",""),O22)</f>
         <v>subject19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C22" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programA</v>
       </c>
       <c r="D22" s="63">
@@ -3884,37 +3933,38 @@
       </c>
       <c r="G22" s="63"/>
       <c r="H22" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O22&lt;10,"0",""),O22)</f>
         <v>019</v>
       </c>
-      <c r="I22" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I22" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">Group A|G5A, Group B|G5B</v>
       </c>
-      <c r="J22" s="120" t="s">
-        <v>344</v>
+      <c r="J22" s="119" t="s">
+        <v>347</v>
       </c>
       <c r="K22" s="63"/>
-      <c r="L22" s="121" t="str">
+      <c r="L22" s="120" t="str">
         <f>ap_subject_types!$A$3</f>
         <v>type01</v>
       </c>
-      <c r="M22" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M22" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@G5A, teacher01|main@G5B</v>
       </c>
-      <c r="N22" s="123">
-        <f t="shared" si="12"/>
+      <c r="N22" s="121"/>
+      <c r="O22" s="122">
+        <f>O21+1</f>
         <v>19</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="10" t="str">
-        <f t="shared" ref="A23:A24" si="15">_xlfn.CONCAT("asignatura",IF(N23&lt;10,"0",""),N23)</f>
+        <f>_xlfn.CONCAT("asignatura",IF(O23&lt;10,"0",""),O23)</f>
         <v>asignatura01</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="C23" s="70" t="str">
         <f>ap_programs!A6</f>
@@ -3931,37 +3981,40 @@
       </c>
       <c r="G23" s="63"/>
       <c r="H23" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O23&lt;10,"0",""),O23)</f>
         <v>001</v>
       </c>
-      <c r="I23" s="119" t="s">
-        <v>351</v>
-      </c>
-      <c r="J23" s="120" t="s">
-        <v>352</v>
+      <c r="I23" s="118" t="s">
+        <v>354</v>
+      </c>
+      <c r="J23" s="119" t="s">
+        <v>355</v>
       </c>
       <c r="K23" s="63"/>
-      <c r="L23" s="121" t="str">
+      <c r="L23" s="120" t="str">
         <f>ap_subject_types!$A$6</f>
         <v>type04</v>
       </c>
-      <c r="M23" s="122" t="s">
-        <v>353</v>
-      </c>
-      <c r="N23" s="123">
+      <c r="M23" s="121" t="s">
+        <v>356</v>
+      </c>
+      <c r="N23" s="121" t="s">
+        <v>357</v>
+      </c>
+      <c r="O23" s="122">
         <v>1</v>
       </c>
     </row>
-    <row r="24" ht="27">
+    <row r="24" ht="28.5">
       <c r="A24" s="10" t="str">
-        <f t="shared" si="15"/>
+        <f>_xlfn.CONCAT("asignatura",IF(O24&lt;10,"0",""),O24)</f>
         <v>asignatura02</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C24" s="70" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>programC</v>
       </c>
       <c r="D24" s="63">
@@ -3975,27 +4028,31 @@
       </c>
       <c r="G24" s="63"/>
       <c r="H24" s="63" t="str">
-        <f t="shared" si="9"/>
+        <f>_xlfn.CONCAT("0",IF(O24&lt;10,"0",""),O24)</f>
         <v>002</v>
       </c>
-      <c r="I24" s="119" t="str">
-        <f t="shared" si="13"/>
+      <c r="I24" s="118" t="str">
+        <f t="shared" si="7"/>
         <v xml:space="preserve">2ºA|2ºA, 2ºB|2ºB</v>
       </c>
-      <c r="J24" s="120" t="s">
-        <v>355</v>
+      <c r="J24" s="119" t="s">
+        <v>359</v>
       </c>
       <c r="K24" s="63"/>
-      <c r="L24" s="121" t="str">
+      <c r="L24" s="120" t="str">
         <f>ap_subject_types!$A$6</f>
         <v>type04</v>
       </c>
-      <c r="M24" s="122" t="str">
-        <f t="shared" si="14"/>
+      <c r="M24" s="121" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">teacher01|main@2ºA, teacher01|main@2ºB</v>
       </c>
-      <c r="N24" s="123">
-        <f t="shared" si="12"/>
+      <c r="N24" s="123" t="str">
+        <f>N23</f>
+        <v xml:space="preserve">studentC01@2ºA, studentC02@2ºA, studentC03@2ºA, studentC04@2ºB, studentC05@2ºB, studentC06@2ºB</v>
+      </c>
+      <c r="O24" s="122">
+        <f>O23+1</f>
         <v>2</v>
       </c>
     </row>
@@ -5350,7 +5407,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>170</v>
       </c>
@@ -5382,7 +5439,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="19.5" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>175</v>
       </c>
@@ -5414,7 +5471,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" s="14" customFormat="1">
+    <row r="12" s="14" customFormat="1" ht="19.5" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>179</v>
       </c>
@@ -5446,7 +5503,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" s="14" customFormat="1">
+    <row r="13" s="14" customFormat="1" ht="19.5" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>183</v>
       </c>
@@ -5478,7 +5535,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" s="14" customFormat="1">
+    <row r="14" s="14" customFormat="1" ht="19.5" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>187</v>
       </c>
@@ -5510,7 +5567,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" s="14" customFormat="1">
+    <row r="15" s="14" customFormat="1" ht="19.5" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>191</v>
       </c>
@@ -5563,7 +5620,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0029005A-0079-47C7-B86C-004200A000E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D400AB-0022-445E-8965-0036008000A4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -5714,7 +5771,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0049009A-009C-47F6-B83E-00FF0084007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00080041-00F0-4985-B2FD-00D700AD009F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -5848,13 +5905,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{003100FE-00DB-4799-B572-001700D10015}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006A0034-001D-4EE7-AC9C-009300110025}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0047006C-004D-4B39-9FA2-003F001D000D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E9004C-00B5-44E2-96B0-004D006F00E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -6168,7 +6225,7 @@
       <c r="B4" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="11" t="s">
         <v>136</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -6195,7 +6252,7 @@
       <c r="K4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="109"/>
+      <c r="L4" s="108"/>
       <c r="M4" s="63"/>
       <c r="N4" s="63"/>
       <c r="O4" s="63"/>
@@ -6235,7 +6292,7 @@
       <c r="B5" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="11" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -6264,7 +6321,7 @@
       <c r="K5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="109" t="s">
+      <c r="L5" s="108" t="s">
         <v>271</v>
       </c>
       <c r="M5" s="63" t="s">
@@ -6314,7 +6371,7 @@
       <c r="B6" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="11" t="s">
         <v>136</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -6341,7 +6398,7 @@
       <c r="K6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="109" t="s">
+      <c r="L6" s="108" t="s">
         <v>274</v>
       </c>
       <c r="M6" s="63" t="s">
@@ -6397,13 +6454,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{006B00F9-006B-4044-9E39-007D00F600EB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004900E4-00C9-42E5-8F3F-0055007B0003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K6 G4:G6 T4 V4:V6 X4:Y6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00510083-0002-47C4-AA7F-00E600780043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003600B4-0023-4287-AD21-0037006900FF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPDATED: UploadImage optimize image before upload from file UPDATED: now pass locale to CardWrapper
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="11"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="494">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -1225,6 +1225,394 @@
   </si>
   <si>
     <t xml:space="preserve">asignatura01, asignatura02</t>
+  </si>
+  <si>
+    <t>qbank</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>general_imagen</t>
+  </si>
+  <si>
+    <t>answers</t>
+  </si>
+  <si>
+    <t>answer_images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Answer</t>
+  </si>
+  <si>
+    <t>Feedback_escrito</t>
+  </si>
+  <si>
+    <t>Feedback_imagen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question Bank</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with images</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Image</t>
+  </si>
+  <si>
+    <t>Answers</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback escrito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback imagen</t>
+  </si>
+  <si>
+    <t>mono</t>
+  </si>
+  <si>
+    <t>elementary</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, continentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿En qué continente vive más gente?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia. |América. |Europa. |África.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Sí. En 2021 la población en Asia era de 4.600 millones de habitantes.
+|2@No. En 2021 la población en América era de 1.029 millones de habitantes.
+|3@No. En 2018 la población en Europa era de 746,4 millones de habitantes.
+|4@No. En 2021 la población en África era de 1.320 millones de habitantes.</t>
+  </si>
+  <si>
+    <t>intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, vocabulario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es la POBLACIÓN?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es el número de habitantes que vive en un país.
+|Es el número de habitantes por Km2 en un territorio determinado.
+|Es el número de personas que llegan a un territorio en un año determinado.
+|Es el número de habitantes que vive en un territorio determinado y en un momento determinado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Es importante recalcar que la población cambia dependiendo del LUGAR y del TIEMPO. En esta respuesta faltaría decir en qué tiempo (por ejemplo en qué año).
+|2@No. El número de habitantes por km2 hace referencia a la DENSIDAD DE POBLACIÓN.
+|3@No. El número de personas que salen y entran de un país hace que aumente o disminuya el número de habitantes en ese teritorio. Pero NO definen qué es la población.
+|4@Sí. Es importante recalcar SIEMPRE de qué territorio se está hablando. Y también de qué momento determinado (suele detallarse en años). Por ejemplo: la población española en 2021.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, países</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cita los tres países que más población tienen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perú, España y China.
+|Alemania, india y Rusia.
+|China, India y Estados Unidos.
+|Chile, Estados Unidos y China.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Perú: 33 millones de habitantes; España: 47 millones de habitantes.
+|2@Alemania: 83 millones de habitantes; Rusia 145 millones de habitantes.
+|3@China: 1.413 millones de habitantes; India: 1.400 millones de habitantes; Estados Unidos: 329 millones de habitantes.
+|4@Chile: 19 millones de habitantes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es la DENSIDAD DE POBLACIÓN?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es el número de personas recién llegadas a un territorio nuevo cada año.
+|Es el número de habitantes por Km2 en un territorio determinado y en un momento determinado.
+|Es el número de habitantes por Km2 en un territorio determinado.
+|Es el número de habitantes que vive en un territorio determinado y en un momento determinado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No, el número de personas que llegan a un país está relaconado con las tasas de inmigración.
+|2@También se la llama POBLACIÓN RELATIVA, para dferenciarla de la población absoluta (número total de habitantes en un territorio y en un momento determinados, sin tener en cuenta su extensión).
+|3@Falta especificar también que es en un tiempo determinado, porque cada año cambia el núnero de habitantes de un territorio, y por lo tanto cambia también su densidad de población.
+|4@No, eso es la población ABSOLUTA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, España</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cita las dos provincias españolas con MAYOR DENSIDAD DE POBLACIÓN.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madrid y Barcelona.
+|Madrid y Cataluña.
+|Huesca y Madrid.
+|Barcelona y Cáceres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Madrid: 844 hab/km2; Barcelona: 729 hab/km2
+|2@Cataluña no es una provincia, es una Comunidad Autónoma.
+|3@Huesca: 14 hab/km2
+|4@Cáceres: 20 hab/km2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es la TASA DE NATALIDAD?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es el número de niñas y niños que nacen en un país y en un año determinado.
+|Es la relación que existe entre el número de nacimientos y la cantidad total de la población en un período de tiempo. Se mide en tantos por mil (‰)
+|Es el número de nacimientos que hay en un territorio determinado y en un momento determinado sin tener en cuenta el número de niños que mueren antes de cumplir un año.
+|Es la relación que existe entre el número de nacimientos y la cantidad total de la población en un período de tiempo. Se mide en tantos por ciento (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No, ese es el número total de nacimientos que ha habido, pero la tasa de natalidad relaciona ese número con el número total de habitantes que hay.
+|2@Sí. La tasa se calcula multiplicando por 1000 el número de nacimientos y dividiendo el resultado entre la población total. Por ejemplo, en un país de 300 habitantes nacen 6 niños.  (6 x 1000) / 300 = 20. La tasa de natalidad es del 20‰
+|3@Esta respuesta está muuy alejada de la respuesta correcta.
+|4@La definición es correcta, pero la tasa de natalidad se mide en tantos por mil (‰)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es la TASA DE FERTILIDAD?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es el número de nacimientos con vida por cada 1000 mujeres en un territorio y un año determinado.
+|Es la relación que existe entre el número de nacimientos y la cantidad total de la población en un período de tiempo. Se mide en tantos por mil (‰)
+|Es el número de nacimientos con vida por cada 1000 mujeres de edades comprendidas entre los 15 y los 49 años, en un territorio y un año determinado.
+|Es el número de nacimientos con vida por cada 1000 mujeres de edades comprendidas entre los 25 y los 45 años, en un territorio y un año determinado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No, la tasa de fertilidad tiene en cuenta qué mujeres están en edad de tener hijos y cuáles no. Por eso se tiene en cuenta sólo a las mujeres entre 15 y 49 años.
+|2@No. Eso es la tasa de natalidad.
+|3@Sí, y se mide en tantos por mil (‰)
+|4@No, la tasa de fertilidad tiene en cuenta qué mujeres están en edad de tener hijos y cuáles no. Por eso se tiene en cuenta sólo a las mujeres entre 15 y 49 años.</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indica cuál de los siguientes países tiene una TASA DE NATALIDAD muy BAJA.</t>
+  </si>
+  <si>
+    <t>1@https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Niger_67ff7ecf20.png|2@https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Italia_69f8c90a1f.png|3@https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Bolivia_9880c08bfb.png|4@https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/mongolia_82e9e2e35e.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Níger: 45 ‰.
+|2@Italia: 7‰
+|3@Bolivia: 21‰
+|4@Mongolia: 23‰</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observa el siguiente mapa que refleja la densidad de población en los diferentes países del mundo, y responde: ¿Cuál de las siguientes opciones cita países con alta densidad de población?</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/densidad_mundo_df44ce83b6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistán, Japón y Corea del Sur.
+|Bélgica, Sudán e India.
+|Reino Unido, Alemania y Mongolia
+|Italia, Canadá y China.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Sí, en el mapa los tres países aparecen con un color oscuro, lo que indica que su densidad de población es elevada. Pakistán: 276 hab./km2. Japón: 334 hab./km2. Corea del Sur: 515 hab./km2
+|2@No. Sudán aparece en el mapa coloreado con un color claro, lo que indica que tiene baja densidad de población.
+|3@No. Mongolia aparece en el mapa coloreado con un color claro, lo que indica que tiene baja densidad de población.
+|4@No. Canadá aparece en el mapa coloreado con un color claro, lo que indica que tiene baja densidad de población.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es el CRECIMIENTO NATURAL O VEGETATIVO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es lo que suelen crecer las personas en un país, es decir, el número de años que suele vivir. Es lo mismo que la esperanza de vida.
+|Es la diferencia entre la tasa de natalidad y la tasa de mortalidad. Siempre es un número positivo.
+|Es la diferencia entre la tasa de natalidad y la tasa de mortalidad. Siempre es un número negativo.
+|Es la diferencia entre la tasa de natalidad y la tasa de mortalidad. Puede ser positivo, negativo o cero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No, son dos conceptos muy diferentes.
+|2@No es cierto que siempre sea un número positivo. Si hay más muertes que nacimientos, el número es negativo.
+|3@No es cierto que siempre sea un número negativo. Si hay más nacimeintos que muertes, el número es positivo.
+|4@Sí, se calcula restando la tasa de mortalidad a la de natalidad: Crecimiento vegetativo = tasa de natalidad - tasa de mortalidad. Si el resultado es positivo, se dice que el crecimiento es positivo, y si el resultado es negativo, se dice que el crecimiento es negativo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es una PIRÁMIDE DE POBLACIÓN?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es un gráfico que representa la estructura de una población por edad en un lugar y momento determinados.
+|Es un gráfico que representa la estructura de una población por sexo en un lugar y momento determinados.
+|Es un gráfico que representa la estructura de una población por edad y sexo en un lugar y momento determinados.
+|Es un gráfico que representa la estructura de una población por edad y sexo en un lugar determinado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No. También nos indica la estructura de la población por sexo.
+|2@No. También nos indica la estructura de la población por edad.
+|3@Sí. La gráfica nos da información sobre la natalidad, la mortalidad y la esperanza de vida de la población.
+|4@No. También es necesario determinar el momento determinado (suele determinarse en años).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿En qué consiste el neomalthusianismo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los neomalthsianos creen que la población crece mucho más rápidamente que los recursos de la Tierra y creen que se debe frenar el crecimiento demográfico para que no se agoten los recursos.
+|Los neomalthusianos creen que el crecimiento de la población es positivo porque es una fuente de riqueza y de progreso. Creen que los recursos son abundantes e ilimitados gracias al desarrollo tecnológico y la mejora del rendimiento en la producción.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Sí, el neomalthusianismo se apoya la tesis que ya en el siglo XVII proclamaba Malthus, prediciendo que la pblación iba a crecer mucho más rápido que los recursos.
+|2@No. Esa tesis pertenece a los poblacionistas, no a los neomalthusianos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, análisis de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observa la siguiente pirámide de población y responde: ¿La TASA DE NATALIDAD es alta o baja?</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/piramide_poblacion_a59b798d04.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alta.
+|Baja.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2@Se observa que el porcentaje de habitantes (hombres y mujeres) menores de 20 años es bastante menor que en la edad adulta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observa la siguiente pirámide de población y responde: ¿Qué sexo tiene más esperanza de vida, los hombres o las mujeres?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las mujeres.
+|Los hombres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@Se observa que en las barras superiores (que indican las personas vivas en esos rangos de edad, las barras de la derecha (que hacen referencia a las mujeres) son más largas, lo que quiere decir que hay más mujeres vivas en esa edad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, inmigración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Cómo se calcula el CRECIMIENTO REAL de la población en un país?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restando el saldo migratorio al crecimiento natural (crecimiento real = crecimiento natural - saldo migratorio).
+|Sumando el crecimiento natural y el saldo migratorio (crecimiento real = crecimiento natural + saldo migratorio).
+|Es lo mismo que el crecimiento natural.
+|Es lo mismo que el saldo migratorio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No. No se debe realizar una resta sino una suma.
+|2@Sí. Para calcularlo es necesario saber la natalidad, la mortalidad, el número de personas que han emigrado y el número de peronas que han inmigrado.
+|3@No. El crecimiento real es la consecuencia de los efectos del crecimiento natural o vegetativo más los efectos de los movimientos migratorios.
+|4@No. El crecimiento real es la consecuencia de los efectos del crecimiento natural o vegetativo más los efectos de los movimientos migratorios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué factores influyen en que un país tenga BAJAS tasas de natalidad?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La salud reproductiva, la inversión económica que se realiza en los hijos, la planificación familiar y la integración de la mujer en el mundo laboral.
+|La salud reproductiva, la inversión económica que se realiza en los hijos, la ausencia de métodos anticonceptivos y la integración de la mujer en el mundo laboral.
+|La mortalidad infantil, la inversión económica que se realiza en los hijos, la planificación familiar y la integración de la mujer en el mundo laboral.
+|La mortalidad infantil, el trabajo infantil, la ausencia de métodos anticonceptivos y la ausencia de la mujer en el mundo laboral.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2@La ausencia de métodos anticonceptivos provoca más embarazos, lo nque aumenta las tasas de natalidad.
+|3@La mortalidad infantil provoca que haya más natalidad, porque las familias tienen muchos hijos sabiendo que algunos morirán de bebés.
+|4@Todos estos factores favorecen que haya unas ALTAS tasas de natalidad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es una persona inmigrante?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una persona que sale de un país huyendo de una guerra.
+|Una persona que llega a un país huyendo de una guerra.
+|Una persona que llega a un territorio y se instala a vivir en él.
+|Una persona que llega a un país buscando trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No, cuando hablamos de personas que SALEN de un país hablamos de EMIGRANTES.
+|2@No. Son muchas las causas que hacen que una persona llegue a un país, no sólo el huir de una guerra.
+|3@Sí, generalmente asociamos la palabra inmigrante a personas extranjeras que llegan y se instalan en un país (inmigrantes internacionales), pero también podemos hablar de territorios administrrativos más pequeños dentro de un mismo país. Una persona que dentro de un mismo país cambia de residencia y se instala en otra región también es inmigrante, pero inmigrante nacional.
+|4@No. Lo que determina que esa persona sea inmigrante no es el objetivo (como buscar trabajo) sino que viene de otro lugar y se instala a vivir en este.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué es el SALDO MIGRATORIO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es la suma de la inmigración y la emigración en un determinado lugar y en un determinado periodo de tiempo (normalmente, un año)
+|Es la diferencia que existe entre la población de un país y el número de personas que salen de él (emigrantes) en un año determinado.
+|Es la diferencia que existe entre la población de un país y el número de personas que llegan a él (inmigrantes) en un año determinado.
+|Es la diferencia que existe entre la inmigración y la emigración en un determinado lugar y en un determinado periodo de tiempo (normalmente, un año)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No. Es la diferencia. NO se debe sumar, sino que se debe restar. (saldo migratorio = nº inmigrantes - nº emigrantes).
+|2@No. El número de habitantes del país no influye. Sólo se debe restar el número emigrantes al número de inmigrantes.
+|3@No. El número de habitantes del país no influye. Sólo se debe restar el número emigrantes al número de inmigrantes.
+|4@Sí, se resta el número de emigrantes al número de inmigrantes (saldo migratorio = nº inmigrantes - nº emigrantes). Si el resultado es positivo, hablamos de un saldo migratorio positivo, y si el resulytado es negativo hablamos de un sado migratorio negativo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Qué dice la Declaración Universal de los Derechos Humanos sobre la inmigración?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dentro de un Estado, toda persona tiene derecho a circular libremente pero no a elegir su lugar de residencia. Si se trata de inmigración internacional (entre Estados), toda persona tiene derecho a buscar asilo, y a disfrutar de él, en cualquier país si se encuentra en situación de persecución.
+|Dentro de un Estado, toda persona tiene derecho a circular libremente y a elegir su residencia. Si se trata de inmigración internacional (entre Estados), toda persona tiene derecho a buscar asilo, y a disfrutar de él, en cualquier país.
+|Dentro de un Estado, toda persona tiene derecho a circular libremente y a elegir su residencia. Si se trata de inmigración internacional (entre Estados), toda persona tiene derecho a buscar asilo, y a disfrutar de él, en cualquier país si su país se encuentra en guerra.
+|Dentro de un Estado, toda persona tiene derecho a circular libremente y a elegir su residencia. Si se trata de inmigración internacional (entre Estados), toda persona tiene derecho a buscar asilo, y a disfrutar de él, en cualquier país si se encuentra en situación de persecución.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@No. Dentro de un Estado toda persona tiene derecho a elegir su lugar de residencia (Artículo 13 de la Declaración Universal de los Derechos Humanos).
+|2@No. Según el Artículo 14 de la Declaración Universal de los Derechos Humanos, toda persona tiene derecho a disfrutar de asilo en cualquier país SI SE ENCUENTRA EN SITUACIÓN DE PERSECUCIÓN EN EL SUYO.
+|3@No. Según el Artículo 14 de la Declaración Universal de los Derechos Humanos, toda persona tiene derecho a disfrutar de asilo en cualquier país SI SE ENCUENTRA EN SITUACIÓN DE PERSECUCIÓN EN EL SUYO. Pero esta persecución no tiene por qué ser una guerra. Existen otras muchas formas de persecución (por razones politicas, religiosas, de condición sexual, etc.).
+|4@Sí, los Artículos 13 y 14 de la Declaración Universal de los Derechos Humanos centran su atención este punto.</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el siguiente mapa se muestra la densidad de población en 2018 en España por provincias. ¿Sabes los nombres de las provincias marcadas con densidad de población muy baja?</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Densidad_2018_7d243fae08.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cáceres.
+|Zamora.
+|Ávila.
+|Soria.
+|Cuenca.</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Densidad_2018_solucion_477dd169a1.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1622,7 @@
   <numFmts count="1">
     <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -1344,6 +1732,13 @@
     <font>
       <name val="Calibri"/>
       <color rgb="FF292B2C"/>
+      <sz val="10.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <i/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <sz val="10.000000"/>
       <scheme val="minor"/>
     </font>
@@ -1464,7 +1859,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1749,12 +2144,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="155">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2137,23 +2560,73 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="16" fillId="0" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="5" fillId="16" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="5" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="5" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="11" fillId="0" borderId="26" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="11" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2934,7 +3407,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{005600DD-000E-44ED-95B1-000C00E5003A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001200C3-002F-4F7D-BBA1-00D8004C0054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -3210,9 +3683,8 @@
       </c>
       <c r="L4" s="125"/>
       <c r="M4" s="64"/>
-      <c r="N4" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N4" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O4" s="126" t="s">
         <v>348</v>
@@ -3262,9 +3734,8 @@
       </c>
       <c r="L5" s="128"/>
       <c r="M5" s="64"/>
-      <c r="N5" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N5" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O5" s="126" t="s">
         <v>353</v>
@@ -3317,9 +3788,8 @@
       </c>
       <c r="L6" s="128"/>
       <c r="M6" s="64"/>
-      <c r="N6" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N6" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O6" s="126" t="s">
         <v>353</v>
@@ -3372,9 +3842,8 @@
       </c>
       <c r="L7" s="128"/>
       <c r="M7" s="64"/>
-      <c r="N7" s="63" t="str">
-        <f>ap_subject_types!$A$5</f>
-        <v>type03</v>
+      <c r="N7" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O7" s="126" t="s">
         <v>348</v>
@@ -3427,9 +3896,8 @@
       </c>
       <c r="L8" s="128"/>
       <c r="M8" s="64"/>
-      <c r="N8" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N8" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O8" s="126" t="s">
         <v>348</v>
@@ -3481,9 +3949,8 @@
       </c>
       <c r="L9" s="129"/>
       <c r="M9" s="64"/>
-      <c r="N9" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N9" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O9" s="126" t="s">
         <v>348</v>
@@ -3535,9 +4002,8 @@
       </c>
       <c r="L10" s="130"/>
       <c r="M10" s="64"/>
-      <c r="N10" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N10" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O10" s="126" t="s">
         <v>348</v>
@@ -3589,9 +4055,8 @@
       </c>
       <c r="L11" s="128"/>
       <c r="M11" s="64"/>
-      <c r="N11" s="63" t="str">
-        <f>ap_subject_types!$A$5</f>
-        <v>type03</v>
+      <c r="N11" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O11" s="126" t="s">
         <v>348</v>
@@ -3643,9 +4108,8 @@
       </c>
       <c r="L12" s="128"/>
       <c r="M12" s="64"/>
-      <c r="N12" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N12" s="63" t="s">
+        <v>319</v>
       </c>
       <c r="O12" s="126" t="s">
         <v>353</v>
@@ -3697,9 +4161,8 @@
       </c>
       <c r="L13" s="128"/>
       <c r="M13" s="64"/>
-      <c r="N13" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N13" s="63" t="s">
+        <v>319</v>
       </c>
       <c r="O13" s="126" t="s">
         <v>348</v>
@@ -3751,9 +4214,8 @@
       </c>
       <c r="L14" s="128"/>
       <c r="M14" s="64"/>
-      <c r="N14" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N14" s="63" t="s">
+        <v>319</v>
       </c>
       <c r="O14" s="126" t="s">
         <v>348</v>
@@ -3805,9 +4267,8 @@
       </c>
       <c r="L15" s="131"/>
       <c r="M15" s="64"/>
-      <c r="N15" s="63" t="str">
-        <f>ap_subject_types!$A$5</f>
-        <v>type03</v>
+      <c r="N15" s="63" t="s">
+        <v>319</v>
       </c>
       <c r="O15" s="126" t="s">
         <v>348</v>
@@ -3859,9 +4320,8 @@
       </c>
       <c r="L16" s="128"/>
       <c r="M16" s="64"/>
-      <c r="N16" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N16" s="63" t="s">
+        <v>319</v>
       </c>
       <c r="O16" s="126" t="s">
         <v>348</v>
@@ -3913,9 +4373,8 @@
       </c>
       <c r="L17" s="128"/>
       <c r="M17" s="64"/>
-      <c r="N17" s="63" t="str">
-        <f>ap_subject_types!$A$3</f>
-        <v>type01</v>
+      <c r="N17" s="63" t="s">
+        <v>318</v>
       </c>
       <c r="O17" s="126" t="s">
         <v>353</v>
@@ -4019,7 +4478,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4067,33 +4526,33 @@
       </c>
     </row>
     <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="79" t="str">
+      <c r="C2" s="7" t="str">
         <f>PROPER(C1)</f>
         <v>Tagline</v>
       </c>
-      <c r="D2" s="79" t="str">
+      <c r="D2" s="7" t="str">
         <f>PROPER(D1)</f>
         <v>Description</v>
       </c>
-      <c r="E2" s="79" t="str">
+      <c r="E2" s="7" t="str">
         <f>PROPER(E1)</f>
         <v>Color</v>
       </c>
-      <c r="F2" s="79" t="str">
+      <c r="F2" s="7" t="str">
         <f>PROPER(F1)</f>
         <v>Cover</v>
       </c>
-      <c r="G2" s="79" t="str">
+      <c r="G2" s="7" t="str">
         <f>PROPER(G1)</f>
         <v>Tags</v>
       </c>
-      <c r="H2" s="132" t="str">
+      <c r="H2" s="51" t="str">
         <f>PROPER(H1)</f>
         <v>Creator</v>
       </c>
@@ -4101,42 +4560,42 @@
         <f>PROPER(I1)</f>
         <v>Program</v>
       </c>
-      <c r="J2" s="133" t="str">
+      <c r="J2" s="132" t="str">
         <f>PROPER(J1)</f>
         <v>Subjects</v>
       </c>
     </row>
     <row r="3" ht="34.5" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="133" t="s">
         <v>389</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="134" t="s">
         <v>390</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="134" t="s">
         <v>391</v>
       </c>
-      <c r="D3" s="134" t="s">
+      <c r="D3" s="135" t="s">
         <v>392</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="134" t="s">
         <v>393</v>
       </c>
-      <c r="F3" s="135" t="s">
+      <c r="F3" s="136" t="s">
         <v>394</v>
       </c>
-      <c r="G3" s="134" t="s">
+      <c r="G3" s="135" t="s">
         <v>395</v>
       </c>
-      <c r="H3" s="136" t="str">
+      <c r="H3" s="137" t="str">
         <f>users!A4</f>
         <v>teacher01</v>
       </c>
-      <c r="I3" s="63" t="str">
+      <c r="I3" s="138" t="str">
         <f>ap_programs!A5</f>
         <v>programB</v>
       </c>
-      <c r="J3" s="137" t="s">
+      <c r="J3" s="139" t="s">
         <v>396</v>
       </c>
     </row>
@@ -4163,11 +4622,968 @@
   </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="11.8515625"/>
+    <col customWidth="1" min="2" max="2" width="15.8515625"/>
+    <col customWidth="1" min="3" max="3" width="10.00390625"/>
+    <col bestFit="1" min="4" max="4" width="8.50390625"/>
+    <col bestFit="1" min="5" max="5" style="140" width="17.3515625"/>
+    <col bestFit="1" min="6" max="6" width="11.28125"/>
+    <col customWidth="1" min="7" max="7" width="15.57421875"/>
+    <col customWidth="1" min="8" max="8" width="69.57421875"/>
+    <col bestFit="1" min="9" max="9" style="141" width="13.8515625"/>
+    <col customWidth="1" min="10" max="10" width="73.140625"/>
+    <col bestFit="1" min="11" max="11" style="141" width="15.2109375"/>
+    <col bestFit="1" min="12" max="12" width="9.921875"/>
+    <col customWidth="1" min="13" max="13" width="114.28125"/>
+    <col customWidth="1" min="14" max="14" style="141" width="23.8515625"/>
+    <col bestFit="1" min="15" max="15" width="2.78125"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="127" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="127" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1" s="127" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1" s="127" t="s">
+        <v>398</v>
+      </c>
+      <c r="E1" s="127" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="127" t="s">
+        <v>400</v>
+      </c>
+      <c r="G1" s="142" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="127" t="s">
+        <v>401</v>
+      </c>
+      <c r="I1" s="127" t="s">
+        <v>402</v>
+      </c>
+      <c r="J1" s="127" t="s">
+        <v>403</v>
+      </c>
+      <c r="K1" s="127" t="s">
+        <v>404</v>
+      </c>
+      <c r="L1" s="127" t="s">
+        <v>405</v>
+      </c>
+      <c r="M1" s="127" t="s">
+        <v>406</v>
+      </c>
+      <c r="N1" s="127" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" ht="28.5">
+      <c r="A2" s="116" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>408</v>
+      </c>
+      <c r="C2" s="97" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="97" t="s">
+        <v>409</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="G2" s="115" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="143" t="s">
+        <v>412</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="J2" s="115" t="s">
+        <v>414</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="L2" s="97" t="s">
+        <v>405</v>
+      </c>
+      <c r="M2" s="115" t="s">
+        <v>416</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" ht="114">
+      <c r="A3" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O3&lt;10,"0",""),O3)</f>
+        <v>q01</v>
+      </c>
+      <c r="B3" s="145" t="str">
+        <f>te_qbanks!A3</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C3" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140" t="s">
+        <v>419</v>
+      </c>
+      <c r="F3" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G3" s="146" t="s">
+        <v>421</v>
+      </c>
+      <c r="H3" s="147" t="s">
+        <v>422</v>
+      </c>
+      <c r="I3" s="140"/>
+      <c r="J3" s="147" t="s">
+        <v>423</v>
+      </c>
+      <c r="K3" s="141"/>
+      <c r="L3" s="140">
+        <v>1</v>
+      </c>
+      <c r="M3" s="147" t="s">
+        <v>424</v>
+      </c>
+      <c r="N3" s="140"/>
+      <c r="O3" s="148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="199.5">
+      <c r="A4" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O4&lt;10,"0",""),O4)</f>
+        <v>q02</v>
+      </c>
+      <c r="B4" s="137" t="str">
+        <f>B3</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C4" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F4" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G4" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H4" s="147" t="s">
+        <v>427</v>
+      </c>
+      <c r="I4" s="140"/>
+      <c r="J4" s="147" t="s">
+        <v>428</v>
+      </c>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140">
+        <v>4</v>
+      </c>
+      <c r="M4" s="147" t="s">
+        <v>429</v>
+      </c>
+      <c r="N4" s="140"/>
+      <c r="O4" s="148">
+        <f>O3+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" ht="114">
+      <c r="A5" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O5&lt;10,"0",""),O5)</f>
+        <v>q03</v>
+      </c>
+      <c r="B5" s="137" t="str">
+        <f>B4</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C5" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F5" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G5" s="146" t="s">
+        <v>430</v>
+      </c>
+      <c r="H5" s="147" t="s">
+        <v>431</v>
+      </c>
+      <c r="I5" s="140"/>
+      <c r="J5" s="147" t="s">
+        <v>432</v>
+      </c>
+      <c r="K5" s="140"/>
+      <c r="L5" s="140">
+        <v>3</v>
+      </c>
+      <c r="M5" s="147" t="s">
+        <v>433</v>
+      </c>
+      <c r="N5" s="140"/>
+      <c r="O5" s="148">
+        <f>O4+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="156.75">
+      <c r="A6" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O6&lt;10,"0",""),O6)</f>
+        <v>q04</v>
+      </c>
+      <c r="B6" s="137" t="str">
+        <f>B5</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C6" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F6" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G6" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H6" s="147" t="s">
+        <v>434</v>
+      </c>
+      <c r="I6" s="140"/>
+      <c r="J6" s="147" t="s">
+        <v>435</v>
+      </c>
+      <c r="K6" s="140"/>
+      <c r="L6" s="140">
+        <v>2</v>
+      </c>
+      <c r="M6" s="147" t="s">
+        <v>436</v>
+      </c>
+      <c r="N6" s="140"/>
+      <c r="O6" s="148">
+        <f>O5+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" ht="71.25">
+      <c r="A7" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O7&lt;10,"0",""),O7)</f>
+        <v>q05</v>
+      </c>
+      <c r="B7" s="137" t="str">
+        <f>B6</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C7" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F7" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G7" s="146" t="s">
+        <v>437</v>
+      </c>
+      <c r="H7" s="147" t="s">
+        <v>438</v>
+      </c>
+      <c r="I7" s="140"/>
+      <c r="J7" s="147" t="s">
+        <v>439</v>
+      </c>
+      <c r="K7" s="140"/>
+      <c r="L7" s="140">
+        <v>1</v>
+      </c>
+      <c r="M7" s="147" t="s">
+        <v>440</v>
+      </c>
+      <c r="N7" s="140"/>
+      <c r="O7" s="148">
+        <f>O6+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" ht="242.25">
+      <c r="A8" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O8&lt;10,"0",""),O8)</f>
+        <v>q06</v>
+      </c>
+      <c r="B8" s="137" t="str">
+        <f>B7</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C8" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D8" s="140"/>
+      <c r="E8" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F8" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G8" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H8" s="147" t="s">
+        <v>441</v>
+      </c>
+      <c r="I8" s="141"/>
+      <c r="J8" s="147" t="s">
+        <v>442</v>
+      </c>
+      <c r="K8" s="140"/>
+      <c r="L8" s="140">
+        <v>2</v>
+      </c>
+      <c r="M8" s="147" t="s">
+        <v>443</v>
+      </c>
+      <c r="N8" s="149"/>
+      <c r="O8" s="148">
+        <f>O7+1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" ht="242.25">
+      <c r="A9" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O9&lt;10,"0",""),O9)</f>
+        <v>q07</v>
+      </c>
+      <c r="B9" s="137" t="str">
+        <f>B8</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C9" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9" s="140"/>
+      <c r="E9" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F9" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G9" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H9" s="147" t="s">
+        <v>444</v>
+      </c>
+      <c r="I9" s="141"/>
+      <c r="J9" s="147" t="s">
+        <v>445</v>
+      </c>
+      <c r="K9" s="140"/>
+      <c r="L9" s="140">
+        <v>3</v>
+      </c>
+      <c r="M9" s="147" t="s">
+        <v>446</v>
+      </c>
+      <c r="N9" s="140"/>
+      <c r="O9" s="148">
+        <f>O8+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" ht="356.25">
+      <c r="A10" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O10&lt;10,"0",""),O10)</f>
+        <v>q08</v>
+      </c>
+      <c r="B10" s="137" t="str">
+        <f>B9</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C10" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140" t="s">
+        <v>419</v>
+      </c>
+      <c r="F10" s="140" t="s">
+        <v>447</v>
+      </c>
+      <c r="G10" s="146" t="s">
+        <v>430</v>
+      </c>
+      <c r="H10" s="147" t="s">
+        <v>448</v>
+      </c>
+      <c r="I10" s="140"/>
+      <c r="J10" s="140"/>
+      <c r="K10" s="150" t="s">
+        <v>449</v>
+      </c>
+      <c r="L10" s="140">
+        <v>2</v>
+      </c>
+      <c r="M10" s="147" t="s">
+        <v>450</v>
+      </c>
+      <c r="N10" s="140"/>
+      <c r="O10" s="148">
+        <f>O9+1</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" ht="185.25">
+      <c r="A11" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O11&lt;10,"0",""),O11)</f>
+        <v>q09</v>
+      </c>
+      <c r="B11" s="137" t="str">
+        <f>B10</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C11" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140" t="s">
+        <v>419</v>
+      </c>
+      <c r="F11" s="140" t="s">
+        <v>447</v>
+      </c>
+      <c r="G11" s="146" t="s">
+        <v>430</v>
+      </c>
+      <c r="H11" s="147" t="s">
+        <v>451</v>
+      </c>
+      <c r="I11" s="150" t="s">
+        <v>452</v>
+      </c>
+      <c r="J11" s="147" t="s">
+        <v>453</v>
+      </c>
+      <c r="K11" s="140"/>
+      <c r="L11" s="140">
+        <v>1</v>
+      </c>
+      <c r="M11" s="147" t="s">
+        <v>454</v>
+      </c>
+      <c r="N11" s="140"/>
+      <c r="O11" s="148">
+        <f>O10+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="185.25">
+      <c r="A12" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O12&lt;10,"0",""),O12)</f>
+        <v>q10</v>
+      </c>
+      <c r="B12" s="137" t="str">
+        <f>B11</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C12" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D12" s="140"/>
+      <c r="E12" s="140" t="s">
+        <v>455</v>
+      </c>
+      <c r="F12" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G12" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H12" s="147" t="s">
+        <v>456</v>
+      </c>
+      <c r="I12" s="140"/>
+      <c r="J12" s="151" t="s">
+        <v>457</v>
+      </c>
+      <c r="K12" s="140"/>
+      <c r="L12" s="140">
+        <v>4</v>
+      </c>
+      <c r="M12" s="147" t="s">
+        <v>458</v>
+      </c>
+      <c r="N12" s="140"/>
+      <c r="O12" s="148">
+        <f>O11+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" ht="185.25">
+      <c r="A13" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O13&lt;10,"0",""),O13)</f>
+        <v>q11</v>
+      </c>
+      <c r="B13" s="137" t="str">
+        <f>B12</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C13" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D13" s="140"/>
+      <c r="E13" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F13" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G13" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H13" s="147" t="s">
+        <v>459</v>
+      </c>
+      <c r="I13" s="140"/>
+      <c r="J13" s="147" t="s">
+        <v>460</v>
+      </c>
+      <c r="K13" s="140"/>
+      <c r="L13" s="140">
+        <v>3</v>
+      </c>
+      <c r="M13" s="147" t="s">
+        <v>461</v>
+      </c>
+      <c r="N13" s="140"/>
+      <c r="O13" s="148">
+        <f>O12+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" ht="185.25">
+      <c r="A14" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O14&lt;10,"0",""),O14)</f>
+        <v>q12</v>
+      </c>
+      <c r="B14" s="137" t="str">
+        <f>B13</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C14" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D14" s="140"/>
+      <c r="E14" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F14" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G14" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H14" s="147" t="s">
+        <v>462</v>
+      </c>
+      <c r="I14" s="140"/>
+      <c r="J14" s="147" t="s">
+        <v>463</v>
+      </c>
+      <c r="K14" s="140"/>
+      <c r="L14" s="140">
+        <v>1</v>
+      </c>
+      <c r="M14" s="147" t="s">
+        <v>464</v>
+      </c>
+      <c r="N14" s="140"/>
+      <c r="O14" s="148">
+        <f>O13+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" ht="114">
+      <c r="A15" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O15&lt;10,"0",""),O15)</f>
+        <v>q13</v>
+      </c>
+      <c r="B15" s="137" t="str">
+        <f>B14</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C15" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F15" s="140" t="s">
+        <v>447</v>
+      </c>
+      <c r="G15" s="146" t="s">
+        <v>465</v>
+      </c>
+      <c r="H15" s="147" t="s">
+        <v>466</v>
+      </c>
+      <c r="I15" s="140" t="s">
+        <v>467</v>
+      </c>
+      <c r="J15" s="147" t="s">
+        <v>468</v>
+      </c>
+      <c r="K15" s="141"/>
+      <c r="L15" s="140">
+        <v>2</v>
+      </c>
+      <c r="M15" s="147" t="s">
+        <v>469</v>
+      </c>
+      <c r="N15" s="140"/>
+      <c r="O15" s="148">
+        <f>O14+1</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" ht="114">
+      <c r="A16" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O16&lt;10,"0",""),O16)</f>
+        <v>q14</v>
+      </c>
+      <c r="B16" s="137" t="str">
+        <f>B15</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C16" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F16" s="140" t="s">
+        <v>447</v>
+      </c>
+      <c r="G16" s="146" t="s">
+        <v>465</v>
+      </c>
+      <c r="H16" s="147" t="s">
+        <v>470</v>
+      </c>
+      <c r="I16" s="140" t="s">
+        <v>467</v>
+      </c>
+      <c r="J16" s="147" t="s">
+        <v>471</v>
+      </c>
+      <c r="K16" s="141"/>
+      <c r="L16" s="140">
+        <v>1</v>
+      </c>
+      <c r="M16" s="147" t="s">
+        <v>472</v>
+      </c>
+      <c r="N16" s="149"/>
+      <c r="O16" s="148">
+        <f>O15+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" ht="142.5">
+      <c r="A17" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O17&lt;10,"0",""),O17)</f>
+        <v>q15</v>
+      </c>
+      <c r="B17" s="137" t="str">
+        <f>B16</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C17" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F17" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G17" s="146" t="s">
+        <v>473</v>
+      </c>
+      <c r="H17" s="147" t="s">
+        <v>474</v>
+      </c>
+      <c r="I17" s="141"/>
+      <c r="J17" s="147" t="s">
+        <v>475</v>
+      </c>
+      <c r="K17" s="141"/>
+      <c r="L17" s="140">
+        <v>2</v>
+      </c>
+      <c r="M17" s="147" t="s">
+        <v>476</v>
+      </c>
+      <c r="N17" s="149"/>
+      <c r="O17" s="148">
+        <f>O16+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="242.25">
+      <c r="A18" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O18&lt;10,"0",""),O18)</f>
+        <v>q16</v>
+      </c>
+      <c r="B18" s="137" t="str">
+        <f>B17</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C18" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F18" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G18" s="146" t="s">
+        <v>465</v>
+      </c>
+      <c r="H18" s="147" t="s">
+        <v>477</v>
+      </c>
+      <c r="I18" s="141"/>
+      <c r="J18" s="147" t="s">
+        <v>478</v>
+      </c>
+      <c r="K18" s="141"/>
+      <c r="L18" s="140">
+        <v>1</v>
+      </c>
+      <c r="M18" s="147" t="s">
+        <v>479</v>
+      </c>
+      <c r="N18" s="149"/>
+      <c r="O18" s="148">
+        <f>O17+1</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" ht="213.75">
+      <c r="A19" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O19&lt;10,"0",""),O19)</f>
+        <v>q17</v>
+      </c>
+      <c r="B19" s="137" t="str">
+        <f>B18</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C19" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F19" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G19" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H19" s="147" t="s">
+        <v>480</v>
+      </c>
+      <c r="I19" s="141"/>
+      <c r="J19" s="147" t="s">
+        <v>481</v>
+      </c>
+      <c r="K19" s="141"/>
+      <c r="L19" s="140">
+        <v>3</v>
+      </c>
+      <c r="M19" s="147" t="s">
+        <v>482</v>
+      </c>
+      <c r="N19" s="149"/>
+      <c r="O19" s="148">
+        <f>O18+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" ht="242.25">
+      <c r="A20" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O20&lt;10,"0",""),O20)</f>
+        <v>q18</v>
+      </c>
+      <c r="B20" s="137" t="str">
+        <f>B19</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C20" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="140" t="s">
+        <v>425</v>
+      </c>
+      <c r="F20" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G20" s="146" t="s">
+        <v>426</v>
+      </c>
+      <c r="H20" s="147" t="s">
+        <v>483</v>
+      </c>
+      <c r="I20" s="141"/>
+      <c r="J20" s="147" t="s">
+        <v>484</v>
+      </c>
+      <c r="K20" s="141"/>
+      <c r="L20" s="140">
+        <v>4</v>
+      </c>
+      <c r="M20" s="147" t="s">
+        <v>485</v>
+      </c>
+      <c r="N20" s="149"/>
+      <c r="O20" s="148">
+        <f>O19+1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" ht="409.5">
+      <c r="A21" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O21&lt;10,"0",""),O21)</f>
+        <v>q19</v>
+      </c>
+      <c r="B21" s="137" t="str">
+        <f>B20</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C21" s="140" t="s">
+        <v>418</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="140" t="s">
+        <v>455</v>
+      </c>
+      <c r="F21" s="140" t="s">
+        <v>420</v>
+      </c>
+      <c r="G21" s="146" t="s">
+        <v>473</v>
+      </c>
+      <c r="H21" s="147" t="s">
+        <v>486</v>
+      </c>
+      <c r="I21" s="140"/>
+      <c r="J21" s="147" t="s">
+        <v>487</v>
+      </c>
+      <c r="K21" s="140"/>
+      <c r="L21" s="140">
+        <v>4</v>
+      </c>
+      <c r="M21" s="147" t="s">
+        <v>488</v>
+      </c>
+      <c r="N21" s="140"/>
+      <c r="O21" s="148">
+        <f>O20+1</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" ht="114">
+      <c r="A22" s="144" t="str">
+        <f>_xlfn.CONCAT("q",IF(O22&lt;10,"0",""),O22)</f>
+        <v>q20</v>
+      </c>
+      <c r="B22" s="137" t="str">
+        <f>B21</f>
+        <v>qbank01</v>
+      </c>
+      <c r="C22" s="140" t="s">
+        <v>489</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="140" t="s">
+        <v>419</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="151" t="s">
+        <v>437</v>
+      </c>
+      <c r="H22" s="147" t="s">
+        <v>490</v>
+      </c>
+      <c r="I22" s="150" t="s">
+        <v>491</v>
+      </c>
+      <c r="J22" s="147" t="s">
+        <v>492</v>
+      </c>
+      <c r="K22" s="141"/>
+      <c r="L22" s="152"/>
+      <c r="M22" s="153"/>
+      <c r="N22" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="O22" s="154">
+        <f>O21+1</f>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="K10"/>
+    <hyperlink r:id="rId2" ref="I11"/>
+    <hyperlink r:id="rId3" ref="I15"/>
+    <hyperlink r:id="rId3" ref="I16"/>
+    <hyperlink r:id="rId4" ref="I22"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -5976,37 +7392,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00630038-0029-457B-B2A4-007500FD005E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AF007E-00DA-4E9A-B27A-009900AD00EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005000D3-0095-4312-BEEF-004900EC00E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F500E5-0002-48E3-8D4D-000E008100EA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EE00E3-0095-4A80-8ED4-0062001A000E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00480018-00FB-448F-A6FD-00B1005E0080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EE00FD-00BE-4539-BF1B-000A0068006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009B0085-0071-4DA6-AFD8-00EF003000F9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F300A6-00B0-449A-976D-005C002500F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009500AA-00CC-41BF-89B7-00B800A200F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004D00C2-006B-43C2-8CAE-00D7009600B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009A00EB-00D9-4920-A541-00830031000F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -6157,7 +7573,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{008D00CC-005C-4806-904C-0097004E0018}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000B005F-00AE-43F4-94EF-003500EC0019}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -6291,13 +7707,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{005E00DC-000D-47EB-BC06-00BF002C009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00420035-00EF-4AD7-B1C8-00CF003A00C1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007E0052-00E5-466C-9680-00F300C30007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A5000E-0092-41A4-9F92-00E100410086}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -6764,13 +8180,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{009A006D-00E9-4C75-9249-0056003B00F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008F004D-009E-4330-BB9E-00E2009E002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0077002A-003F-4C03-9C8D-005D00A90021}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009F00E8-00B0-442A-892A-00CB00AC0089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPGRADE: Bubbles version to support ActivityCountdown deps
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="489">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -1197,25 +1197,19 @@
     <t>qbank01</t>
   </si>
   <si>
-    <t xml:space="preserve">Mi primer question bank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Cuánto sabes de los qbanks?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Echa un vistazo a las preguntas, y mira cuánto sabes de los qbanks de leemons.</t>
+    <t xml:space="preserve">Demografía 2ºESO</t>
   </si>
   <si>
     <t>#fabada</t>
   </si>
   <si>
-    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/piramide_togo_6b24d983b2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">primer, qbank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asignatura01, asignatura02</t>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/population_d147987780.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, preguntas, eso</t>
+  </si>
+  <si>
+    <t>asignatura02</t>
   </si>
   <si>
     <t>qbank</t>
@@ -2168,7 +2162,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="164">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2582,10 +2576,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="11" fillId="0" borderId="26" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3419,7 +3419,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00870018-006B-4F91-8763-00DE009C0019}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00030072-004B-4021-97AA-0059004E009A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -4490,15 +4490,15 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="33.8515625"/>
-    <col customWidth="1" min="3" max="3" width="28.8515625"/>
-    <col customWidth="1" min="4" max="4" width="36.00390625"/>
+    <col customWidth="1" min="2" max="2" width="25.00390625"/>
+    <col customWidth="1" min="3" max="3" width="16.00390625"/>
+    <col customWidth="1" min="4" max="4" width="22.28125"/>
     <col customWidth="1" min="6" max="6" width="21.00390625"/>
     <col customWidth="1" min="7" max="8" width="14.140625"/>
     <col customWidth="1" min="9" max="9" width="12.7109375"/>
@@ -4584,31 +4584,27 @@
       <c r="B3" s="141" t="s">
         <v>387</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="142" t="s">
         <v>388</v>
       </c>
-      <c r="D3" s="142" t="s">
+      <c r="F3" s="144" t="s">
         <v>389</v>
       </c>
-      <c r="E3" s="141" t="s">
+      <c r="G3" s="145" t="s">
         <v>390</v>
       </c>
-      <c r="F3" s="143" t="s">
-        <v>391</v>
-      </c>
-      <c r="G3" s="142" t="s">
-        <v>392</v>
-      </c>
-      <c r="H3" s="144" t="str">
+      <c r="H3" s="146" t="str">
         <f>users!A4</f>
         <v>teacher01</v>
       </c>
-      <c r="I3" s="145" t="str">
+      <c r="I3" s="147" t="str">
         <f>ap_programs!A5</f>
         <v>programB</v>
       </c>
-      <c r="J3" s="146" t="s">
-        <v>393</v>
+      <c r="J3" s="148" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="4"/>
@@ -4644,16 +4640,16 @@
     <col customWidth="1" min="2" max="2" width="15.8515625"/>
     <col customWidth="1" min="3" max="3" width="10.00390625"/>
     <col bestFit="1" min="4" max="4" width="8.50390625"/>
-    <col bestFit="1" min="5" max="5" style="147" width="17.3515625"/>
+    <col bestFit="1" min="5" max="5" style="149" width="17.3515625"/>
     <col bestFit="1" min="6" max="6" width="11.28125"/>
     <col customWidth="1" min="7" max="7" width="15.57421875"/>
     <col customWidth="1" min="8" max="8" width="69.57421875"/>
-    <col bestFit="1" min="9" max="9" style="148" width="13.8515625"/>
+    <col bestFit="1" min="9" max="9" style="150" width="13.8515625"/>
     <col customWidth="1" min="10" max="10" width="73.140625"/>
-    <col bestFit="1" min="11" max="11" style="148" width="15.2109375"/>
+    <col bestFit="1" min="11" max="11" style="150" width="15.2109375"/>
     <col bestFit="1" min="12" max="12" width="9.921875"/>
     <col customWidth="1" min="13" max="13" width="114.28125"/>
-    <col customWidth="1" min="14" max="14" style="148" width="23.8515625"/>
+    <col customWidth="1" min="14" max="14" style="150" width="23.8515625"/>
     <col bestFit="1" min="15" max="15" width="2.78125"/>
   </cols>
   <sheetData>
@@ -4662,43 +4658,43 @@
         <v>23</v>
       </c>
       <c r="B1" s="134" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C1" s="134" t="s">
         <v>243</v>
       </c>
       <c r="D1" s="134" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1" s="134" t="s">
+        <v>394</v>
+      </c>
+      <c r="F1" s="134" t="s">
         <v>395</v>
       </c>
-      <c r="E1" s="134" t="s">
+      <c r="G1" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="134" t="s">
         <v>396</v>
       </c>
-      <c r="F1" s="134" t="s">
+      <c r="I1" s="134" t="s">
         <v>397</v>
       </c>
-      <c r="G1" s="149" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="134" t="s">
+      <c r="J1" s="134" t="s">
         <v>398</v>
       </c>
-      <c r="I1" s="134" t="s">
+      <c r="K1" s="134" t="s">
         <v>399</v>
       </c>
-      <c r="J1" s="134" t="s">
+      <c r="L1" s="134" t="s">
         <v>400</v>
       </c>
-      <c r="K1" s="134" t="s">
+      <c r="M1" s="134" t="s">
         <v>401</v>
       </c>
-      <c r="L1" s="134" t="s">
+      <c r="N1" s="134" t="s">
         <v>402</v>
-      </c>
-      <c r="M1" s="134" t="s">
-        <v>403</v>
-      </c>
-      <c r="N1" s="134" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -4706,884 +4702,884 @@
         <v>27</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C2" s="104" t="s">
         <v>247</v>
       </c>
       <c r="D2" s="104" t="s">
+        <v>404</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>406</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>408</v>
       </c>
       <c r="G2" s="122" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="150" t="s">
+      <c r="H2" s="152" t="s">
+        <v>407</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="J2" s="122" t="s">
         <v>409</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="J2" s="122" t="s">
+      <c r="L2" s="104" t="s">
+        <v>400</v>
+      </c>
+      <c r="M2" s="122" t="s">
         <v>411</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="L2" s="104" t="s">
-        <v>402</v>
-      </c>
-      <c r="M2" s="122" t="s">
-        <v>413</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="3" ht="114">
-      <c r="A3" s="151" t="str">
+      <c r="A3" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O3&lt;10,"0",""),O3)</f>
         <v>q01</v>
       </c>
-      <c r="B3" s="152" t="str">
+      <c r="B3" s="154" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="F3" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147" t="s">
+      <c r="G3" s="155" t="s">
         <v>416</v>
       </c>
-      <c r="F3" s="147" t="s">
+      <c r="H3" s="156" t="s">
         <v>417</v>
       </c>
-      <c r="G3" s="153" t="s">
+      <c r="I3" s="149"/>
+      <c r="J3" s="156" t="s">
         <v>418</v>
       </c>
-      <c r="H3" s="154" t="s">
+      <c r="K3" s="150"/>
+      <c r="L3" s="149">
+        <v>1</v>
+      </c>
+      <c r="M3" s="156" t="s">
         <v>419</v>
       </c>
-      <c r="I3" s="147"/>
-      <c r="J3" s="154" t="s">
-        <v>420</v>
-      </c>
-      <c r="K3" s="148"/>
-      <c r="L3" s="147">
+      <c r="N3" s="149"/>
+      <c r="O3" s="157">
         <v>1</v>
       </c>
-      <c r="M3" s="154" t="s">
-        <v>421</v>
-      </c>
-      <c r="N3" s="147"/>
-      <c r="O3" s="155">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" ht="199.5">
-      <c r="A4" s="151" t="str">
+      <c r="A4" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O4&lt;10,"0",""),O4)</f>
         <v>q02</v>
       </c>
-      <c r="B4" s="144" t="str">
+      <c r="B4" s="146" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F4" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147" t="s">
+      <c r="G4" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H4" s="156" t="s">
         <v>422</v>
       </c>
-      <c r="F4" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G4" s="153" t="s">
+      <c r="I4" s="149"/>
+      <c r="J4" s="156" t="s">
         <v>423</v>
       </c>
-      <c r="H4" s="154" t="s">
+      <c r="K4" s="149"/>
+      <c r="L4" s="149">
+        <v>4</v>
+      </c>
+      <c r="M4" s="156" t="s">
         <v>424</v>
       </c>
-      <c r="I4" s="147"/>
-      <c r="J4" s="154" t="s">
-        <v>425</v>
-      </c>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147">
-        <v>4</v>
-      </c>
-      <c r="M4" s="154" t="s">
-        <v>426</v>
-      </c>
-      <c r="N4" s="147"/>
-      <c r="O4" s="155">
+      <c r="N4" s="149"/>
+      <c r="O4" s="157">
         <f>O3+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="114">
-      <c r="A5" s="151" t="str">
+      <c r="A5" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O5&lt;10,"0",""),O5)</f>
         <v>q03</v>
       </c>
-      <c r="B5" s="144" t="str">
+      <c r="B5" s="146" t="str">
         <f>B4</f>
         <v>qbank01</v>
       </c>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F5" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F5" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G5" s="153" t="s">
+      <c r="G5" s="155" t="s">
+        <v>425</v>
+      </c>
+      <c r="H5" s="156" t="s">
+        <v>426</v>
+      </c>
+      <c r="I5" s="149"/>
+      <c r="J5" s="156" t="s">
         <v>427</v>
       </c>
-      <c r="H5" s="154" t="s">
+      <c r="K5" s="149"/>
+      <c r="L5" s="149">
+        <v>3</v>
+      </c>
+      <c r="M5" s="156" t="s">
         <v>428</v>
       </c>
-      <c r="I5" s="147"/>
-      <c r="J5" s="154" t="s">
-        <v>429</v>
-      </c>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147">
-        <v>3</v>
-      </c>
-      <c r="M5" s="154" t="s">
-        <v>430</v>
-      </c>
-      <c r="N5" s="147"/>
-      <c r="O5" s="155">
+      <c r="N5" s="149"/>
+      <c r="O5" s="157">
         <f>O4+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="156.75">
-      <c r="A6" s="151" t="str">
+      <c r="A6" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O6&lt;10,"0",""),O6)</f>
         <v>q04</v>
       </c>
-      <c r="B6" s="144" t="str">
+      <c r="B6" s="146" t="str">
         <f>B5</f>
         <v>qbank01</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F6" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D6" s="147"/>
-      <c r="E6" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F6" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G6" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H6" s="154" t="s">
+      <c r="G6" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H6" s="156" t="s">
+        <v>429</v>
+      </c>
+      <c r="I6" s="149"/>
+      <c r="J6" s="156" t="s">
+        <v>430</v>
+      </c>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149">
+        <v>2</v>
+      </c>
+      <c r="M6" s="156" t="s">
         <v>431</v>
       </c>
-      <c r="I6" s="147"/>
-      <c r="J6" s="154" t="s">
-        <v>432</v>
-      </c>
-      <c r="K6" s="147"/>
-      <c r="L6" s="147">
-        <v>2</v>
-      </c>
-      <c r="M6" s="154" t="s">
-        <v>433</v>
-      </c>
-      <c r="N6" s="147"/>
-      <c r="O6" s="155">
+      <c r="N6" s="149"/>
+      <c r="O6" s="157">
         <f>O5+1</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="71.25">
-      <c r="A7" s="151" t="str">
+      <c r="A7" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O7&lt;10,"0",""),O7)</f>
         <v>q05</v>
       </c>
-      <c r="B7" s="144" t="str">
+      <c r="B7" s="146" t="str">
         <f>B6</f>
         <v>qbank01</v>
       </c>
-      <c r="C7" s="147" t="s">
+      <c r="C7" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D7" s="149"/>
+      <c r="E7" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F7" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F7" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G7" s="153" t="s">
+      <c r="G7" s="155" t="s">
+        <v>432</v>
+      </c>
+      <c r="H7" s="156" t="s">
+        <v>433</v>
+      </c>
+      <c r="I7" s="149"/>
+      <c r="J7" s="156" t="s">
         <v>434</v>
       </c>
-      <c r="H7" s="154" t="s">
+      <c r="K7" s="149"/>
+      <c r="L7" s="149">
+        <v>1</v>
+      </c>
+      <c r="M7" s="156" t="s">
         <v>435</v>
       </c>
-      <c r="I7" s="147"/>
-      <c r="J7" s="154" t="s">
-        <v>436</v>
-      </c>
-      <c r="K7" s="147"/>
-      <c r="L7" s="147">
-        <v>1</v>
-      </c>
-      <c r="M7" s="154" t="s">
-        <v>437</v>
-      </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="155">
+      <c r="N7" s="149"/>
+      <c r="O7" s="157">
         <f>O6+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="242.25">
-      <c r="A8" s="151" t="str">
+      <c r="A8" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O8&lt;10,"0",""),O8)</f>
         <v>q06</v>
       </c>
-      <c r="B8" s="144" t="str">
+      <c r="B8" s="146" t="str">
         <f>B7</f>
         <v>qbank01</v>
       </c>
-      <c r="C8" s="147" t="s">
+      <c r="C8" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D8" s="149"/>
+      <c r="E8" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F8" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D8" s="147"/>
-      <c r="E8" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F8" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G8" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H8" s="154" t="s">
+      <c r="G8" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H8" s="156" t="s">
+        <v>436</v>
+      </c>
+      <c r="I8" s="150"/>
+      <c r="J8" s="156" t="s">
+        <v>437</v>
+      </c>
+      <c r="K8" s="149"/>
+      <c r="L8" s="149">
+        <v>2</v>
+      </c>
+      <c r="M8" s="156" t="s">
         <v>438</v>
       </c>
-      <c r="I8" s="148"/>
-      <c r="J8" s="154" t="s">
-        <v>439</v>
-      </c>
-      <c r="K8" s="147"/>
-      <c r="L8" s="147">
-        <v>2</v>
-      </c>
-      <c r="M8" s="154" t="s">
-        <v>440</v>
-      </c>
-      <c r="N8" s="156"/>
-      <c r="O8" s="155">
+      <c r="N8" s="158"/>
+      <c r="O8" s="157">
         <f>O7+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="242.25">
-      <c r="A9" s="151" t="str">
+      <c r="A9" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O9&lt;10,"0",""),O9)</f>
         <v>q07</v>
       </c>
-      <c r="B9" s="144" t="str">
+      <c r="B9" s="146" t="str">
         <f>B8</f>
         <v>qbank01</v>
       </c>
-      <c r="C9" s="147" t="s">
+      <c r="C9" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D9" s="149"/>
+      <c r="E9" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F9" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D9" s="147"/>
-      <c r="E9" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F9" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G9" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H9" s="154" t="s">
+      <c r="G9" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H9" s="156" t="s">
+        <v>439</v>
+      </c>
+      <c r="I9" s="150"/>
+      <c r="J9" s="156" t="s">
+        <v>440</v>
+      </c>
+      <c r="K9" s="149"/>
+      <c r="L9" s="149">
+        <v>3</v>
+      </c>
+      <c r="M9" s="156" t="s">
         <v>441</v>
       </c>
-      <c r="I9" s="148"/>
-      <c r="J9" s="154" t="s">
-        <v>442</v>
-      </c>
-      <c r="K9" s="147"/>
-      <c r="L9" s="147">
-        <v>3</v>
-      </c>
-      <c r="M9" s="154" t="s">
-        <v>443</v>
-      </c>
-      <c r="N9" s="147"/>
-      <c r="O9" s="155">
+      <c r="N9" s="149"/>
+      <c r="O9" s="157">
         <f>O8+1</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="356.25">
-      <c r="A10" s="151" t="str">
+      <c r="A10" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O10&lt;10,"0",""),O10)</f>
         <v>q08</v>
       </c>
-      <c r="B10" s="144" t="str">
+      <c r="B10" s="146" t="str">
         <f>B9</f>
         <v>qbank01</v>
       </c>
-      <c r="C10" s="147" t="s">
-        <v>415</v>
-      </c>
-      <c r="D10" s="147"/>
-      <c r="E10" s="147" t="s">
-        <v>416</v>
-      </c>
-      <c r="F10" s="147" t="s">
+      <c r="C10" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D10" s="149"/>
+      <c r="E10" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="F10" s="149" t="s">
+        <v>442</v>
+      </c>
+      <c r="G10" s="155" t="s">
+        <v>425</v>
+      </c>
+      <c r="H10" s="156" t="s">
+        <v>443</v>
+      </c>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="159" t="s">
         <v>444</v>
       </c>
-      <c r="G10" s="153" t="s">
-        <v>427</v>
-      </c>
-      <c r="H10" s="154" t="s">
+      <c r="L10" s="149">
+        <v>2</v>
+      </c>
+      <c r="M10" s="156" t="s">
         <v>445</v>
       </c>
-      <c r="I10" s="147"/>
-      <c r="J10" s="147"/>
-      <c r="K10" s="157" t="s">
-        <v>446</v>
-      </c>
-      <c r="L10" s="147">
-        <v>2</v>
-      </c>
-      <c r="M10" s="154" t="s">
-        <v>447</v>
-      </c>
-      <c r="N10" s="147"/>
-      <c r="O10" s="155">
+      <c r="N10" s="149"/>
+      <c r="O10" s="157">
         <f>O9+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="11" ht="185.25">
-      <c r="A11" s="151" t="str">
+      <c r="A11" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O11&lt;10,"0",""),O11)</f>
         <v>q09</v>
       </c>
-      <c r="B11" s="144" t="str">
+      <c r="B11" s="146" t="str">
         <f>B10</f>
         <v>qbank01</v>
       </c>
-      <c r="C11" s="147" t="s">
-        <v>415</v>
-      </c>
-      <c r="D11" s="147"/>
-      <c r="E11" s="147" t="s">
-        <v>416</v>
-      </c>
-      <c r="F11" s="147" t="s">
-        <v>444</v>
-      </c>
-      <c r="G11" s="153" t="s">
-        <v>427</v>
-      </c>
-      <c r="H11" s="154" t="s">
+      <c r="C11" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D11" s="149"/>
+      <c r="E11" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="F11" s="149" t="s">
+        <v>442</v>
+      </c>
+      <c r="G11" s="155" t="s">
+        <v>425</v>
+      </c>
+      <c r="H11" s="156" t="s">
+        <v>446</v>
+      </c>
+      <c r="I11" s="159" t="s">
+        <v>447</v>
+      </c>
+      <c r="J11" s="156" t="s">
         <v>448</v>
       </c>
-      <c r="I11" s="157" t="s">
+      <c r="K11" s="149"/>
+      <c r="L11" s="149">
+        <v>1</v>
+      </c>
+      <c r="M11" s="156" t="s">
         <v>449</v>
       </c>
-      <c r="J11" s="154" t="s">
-        <v>450</v>
-      </c>
-      <c r="K11" s="147"/>
-      <c r="L11" s="147">
-        <v>1</v>
-      </c>
-      <c r="M11" s="154" t="s">
-        <v>451</v>
-      </c>
-      <c r="N11" s="147"/>
-      <c r="O11" s="155">
+      <c r="N11" s="149"/>
+      <c r="O11" s="157">
         <f>O10+1</f>
         <v>9</v>
       </c>
     </row>
     <row r="12" ht="185.25">
-      <c r="A12" s="151" t="str">
+      <c r="A12" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O12&lt;10,"0",""),O12)</f>
         <v>q10</v>
       </c>
-      <c r="B12" s="144" t="str">
+      <c r="B12" s="146" t="str">
         <f>B11</f>
         <v>qbank01</v>
       </c>
-      <c r="C12" s="147" t="s">
+      <c r="C12" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D12" s="149"/>
+      <c r="E12" s="149" t="s">
+        <v>450</v>
+      </c>
+      <c r="F12" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D12" s="147"/>
-      <c r="E12" s="147" t="s">
+      <c r="G12" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H12" s="156" t="s">
+        <v>451</v>
+      </c>
+      <c r="I12" s="149"/>
+      <c r="J12" s="160" t="s">
         <v>452</v>
       </c>
-      <c r="F12" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G12" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H12" s="154" t="s">
+      <c r="K12" s="149"/>
+      <c r="L12" s="149">
+        <v>4</v>
+      </c>
+      <c r="M12" s="156" t="s">
         <v>453</v>
       </c>
-      <c r="I12" s="147"/>
-      <c r="J12" s="158" t="s">
-        <v>454</v>
-      </c>
-      <c r="K12" s="147"/>
-      <c r="L12" s="147">
-        <v>4</v>
-      </c>
-      <c r="M12" s="154" t="s">
-        <v>455</v>
-      </c>
-      <c r="N12" s="147"/>
-      <c r="O12" s="155">
+      <c r="N12" s="149"/>
+      <c r="O12" s="157">
         <f>O11+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="185.25">
-      <c r="A13" s="151" t="str">
+      <c r="A13" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O13&lt;10,"0",""),O13)</f>
         <v>q11</v>
       </c>
-      <c r="B13" s="144" t="str">
+      <c r="B13" s="146" t="str">
         <f>B12</f>
         <v>qbank01</v>
       </c>
-      <c r="C13" s="147" t="s">
+      <c r="C13" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D13" s="149"/>
+      <c r="E13" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F13" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D13" s="147"/>
-      <c r="E13" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F13" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G13" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H13" s="154" t="s">
+      <c r="G13" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H13" s="156" t="s">
+        <v>454</v>
+      </c>
+      <c r="I13" s="149"/>
+      <c r="J13" s="156" t="s">
+        <v>455</v>
+      </c>
+      <c r="K13" s="149"/>
+      <c r="L13" s="149">
+        <v>3</v>
+      </c>
+      <c r="M13" s="156" t="s">
         <v>456</v>
       </c>
-      <c r="I13" s="147"/>
-      <c r="J13" s="154" t="s">
-        <v>457</v>
-      </c>
-      <c r="K13" s="147"/>
-      <c r="L13" s="147">
-        <v>3</v>
-      </c>
-      <c r="M13" s="154" t="s">
-        <v>458</v>
-      </c>
-      <c r="N13" s="147"/>
-      <c r="O13" s="155">
+      <c r="N13" s="149"/>
+      <c r="O13" s="157">
         <f>O12+1</f>
         <v>11</v>
       </c>
     </row>
     <row r="14" ht="185.25">
-      <c r="A14" s="151" t="str">
+      <c r="A14" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O14&lt;10,"0",""),O14)</f>
         <v>q12</v>
       </c>
-      <c r="B14" s="144" t="str">
+      <c r="B14" s="146" t="str">
         <f>B13</f>
         <v>qbank01</v>
       </c>
-      <c r="C14" s="147" t="s">
+      <c r="C14" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D14" s="149"/>
+      <c r="E14" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F14" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D14" s="147"/>
-      <c r="E14" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F14" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G14" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H14" s="154" t="s">
+      <c r="G14" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H14" s="156" t="s">
+        <v>457</v>
+      </c>
+      <c r="I14" s="149"/>
+      <c r="J14" s="156" t="s">
+        <v>458</v>
+      </c>
+      <c r="K14" s="149"/>
+      <c r="L14" s="149">
+        <v>1</v>
+      </c>
+      <c r="M14" s="156" t="s">
         <v>459</v>
       </c>
-      <c r="I14" s="147"/>
-      <c r="J14" s="154" t="s">
-        <v>460</v>
-      </c>
-      <c r="K14" s="147"/>
-      <c r="L14" s="147">
-        <v>1</v>
-      </c>
-      <c r="M14" s="154" t="s">
-        <v>461</v>
-      </c>
-      <c r="N14" s="147"/>
-      <c r="O14" s="155">
+      <c r="N14" s="149"/>
+      <c r="O14" s="157">
         <f>O13+1</f>
         <v>12</v>
       </c>
     </row>
     <row r="15" ht="114">
-      <c r="A15" s="151" t="str">
+      <c r="A15" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O15&lt;10,"0",""),O15)</f>
         <v>q13</v>
       </c>
-      <c r="B15" s="144" t="str">
+      <c r="B15" s="146" t="str">
         <f>B14</f>
         <v>qbank01</v>
       </c>
-      <c r="C15" s="147" t="s">
-        <v>415</v>
+      <c r="C15" s="149" t="s">
+        <v>413</v>
       </c>
       <c r="D15" s="18"/>
-      <c r="E15" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F15" s="147" t="s">
-        <v>444</v>
-      </c>
-      <c r="G15" s="153" t="s">
+      <c r="E15" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F15" s="149" t="s">
+        <v>442</v>
+      </c>
+      <c r="G15" s="155" t="s">
+        <v>460</v>
+      </c>
+      <c r="H15" s="156" t="s">
+        <v>461</v>
+      </c>
+      <c r="I15" s="149" t="s">
         <v>462</v>
       </c>
-      <c r="H15" s="154" t="s">
+      <c r="J15" s="156" t="s">
         <v>463</v>
       </c>
-      <c r="I15" s="147" t="s">
+      <c r="K15" s="150"/>
+      <c r="L15" s="149">
+        <v>2</v>
+      </c>
+      <c r="M15" s="156" t="s">
         <v>464</v>
       </c>
-      <c r="J15" s="154" t="s">
-        <v>465</v>
-      </c>
-      <c r="K15" s="148"/>
-      <c r="L15" s="147">
-        <v>2</v>
-      </c>
-      <c r="M15" s="154" t="s">
-        <v>466</v>
-      </c>
-      <c r="N15" s="147"/>
-      <c r="O15" s="155">
+      <c r="N15" s="149"/>
+      <c r="O15" s="157">
         <f>O14+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="16" ht="114">
-      <c r="A16" s="151" t="str">
+      <c r="A16" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O16&lt;10,"0",""),O16)</f>
         <v>q14</v>
       </c>
-      <c r="B16" s="144" t="str">
+      <c r="B16" s="146" t="str">
         <f>B15</f>
         <v>qbank01</v>
       </c>
-      <c r="C16" s="147" t="s">
-        <v>415</v>
+      <c r="C16" s="149" t="s">
+        <v>413</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F16" s="147" t="s">
-        <v>444</v>
-      </c>
-      <c r="G16" s="153" t="s">
+      <c r="E16" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F16" s="149" t="s">
+        <v>442</v>
+      </c>
+      <c r="G16" s="155" t="s">
+        <v>460</v>
+      </c>
+      <c r="H16" s="156" t="s">
+        <v>465</v>
+      </c>
+      <c r="I16" s="149" t="s">
         <v>462</v>
       </c>
-      <c r="H16" s="154" t="s">
+      <c r="J16" s="156" t="s">
+        <v>466</v>
+      </c>
+      <c r="K16" s="150"/>
+      <c r="L16" s="149">
+        <v>1</v>
+      </c>
+      <c r="M16" s="156" t="s">
         <v>467</v>
       </c>
-      <c r="I16" s="147" t="s">
-        <v>464</v>
-      </c>
-      <c r="J16" s="154" t="s">
-        <v>468</v>
-      </c>
-      <c r="K16" s="148"/>
-      <c r="L16" s="147">
-        <v>1</v>
-      </c>
-      <c r="M16" s="154" t="s">
-        <v>469</v>
-      </c>
-      <c r="N16" s="156"/>
-      <c r="O16" s="155">
+      <c r="N16" s="158"/>
+      <c r="O16" s="157">
         <f>O15+1</f>
         <v>14</v>
       </c>
     </row>
     <row r="17" ht="142.5">
-      <c r="A17" s="151" t="str">
+      <c r="A17" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O17&lt;10,"0",""),O17)</f>
         <v>q15</v>
       </c>
-      <c r="B17" s="144" t="str">
+      <c r="B17" s="146" t="str">
         <f>B16</f>
         <v>qbank01</v>
       </c>
-      <c r="C17" s="147" t="s">
+      <c r="C17" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F17" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F17" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G17" s="153" t="s">
+      <c r="G17" s="155" t="s">
+        <v>468</v>
+      </c>
+      <c r="H17" s="156" t="s">
+        <v>469</v>
+      </c>
+      <c r="I17" s="150"/>
+      <c r="J17" s="156" t="s">
         <v>470</v>
       </c>
-      <c r="H17" s="154" t="s">
+      <c r="K17" s="150"/>
+      <c r="L17" s="149">
+        <v>2</v>
+      </c>
+      <c r="M17" s="156" t="s">
         <v>471</v>
       </c>
-      <c r="I17" s="148"/>
-      <c r="J17" s="154" t="s">
-        <v>472</v>
-      </c>
-      <c r="K17" s="148"/>
-      <c r="L17" s="147">
-        <v>2</v>
-      </c>
-      <c r="M17" s="154" t="s">
-        <v>473</v>
-      </c>
-      <c r="N17" s="156"/>
-      <c r="O17" s="155">
+      <c r="N17" s="158"/>
+      <c r="O17" s="157">
         <f>O16+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="242.25">
-      <c r="A18" s="151" t="str">
+      <c r="A18" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O18&lt;10,"0",""),O18)</f>
         <v>q16</v>
       </c>
-      <c r="B18" s="144" t="str">
+      <c r="B18" s="146" t="str">
         <f>B17</f>
         <v>qbank01</v>
       </c>
-      <c r="C18" s="147" t="s">
+      <c r="C18" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F18" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F18" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G18" s="153" t="s">
-        <v>462</v>
-      </c>
-      <c r="H18" s="154" t="s">
+      <c r="G18" s="155" t="s">
+        <v>460</v>
+      </c>
+      <c r="H18" s="156" t="s">
+        <v>472</v>
+      </c>
+      <c r="I18" s="150"/>
+      <c r="J18" s="156" t="s">
+        <v>473</v>
+      </c>
+      <c r="K18" s="150"/>
+      <c r="L18" s="149">
+        <v>1</v>
+      </c>
+      <c r="M18" s="156" t="s">
         <v>474</v>
       </c>
-      <c r="I18" s="148"/>
-      <c r="J18" s="154" t="s">
-        <v>475</v>
-      </c>
-      <c r="K18" s="148"/>
-      <c r="L18" s="147">
-        <v>1</v>
-      </c>
-      <c r="M18" s="154" t="s">
-        <v>476</v>
-      </c>
-      <c r="N18" s="156"/>
-      <c r="O18" s="155">
+      <c r="N18" s="158"/>
+      <c r="O18" s="157">
         <f>O17+1</f>
         <v>16</v>
       </c>
     </row>
     <row r="19" ht="213.75">
-      <c r="A19" s="151" t="str">
+      <c r="A19" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O19&lt;10,"0",""),O19)</f>
         <v>q17</v>
       </c>
-      <c r="B19" s="144" t="str">
+      <c r="B19" s="146" t="str">
         <f>B18</f>
         <v>qbank01</v>
       </c>
-      <c r="C19" s="147" t="s">
+      <c r="C19" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F19" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F19" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G19" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H19" s="154" t="s">
+      <c r="G19" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H19" s="156" t="s">
+        <v>475</v>
+      </c>
+      <c r="I19" s="150"/>
+      <c r="J19" s="156" t="s">
+        <v>476</v>
+      </c>
+      <c r="K19" s="150"/>
+      <c r="L19" s="149">
+        <v>3</v>
+      </c>
+      <c r="M19" s="156" t="s">
         <v>477</v>
       </c>
-      <c r="I19" s="148"/>
-      <c r="J19" s="154" t="s">
-        <v>478</v>
-      </c>
-      <c r="K19" s="148"/>
-      <c r="L19" s="147">
-        <v>3</v>
-      </c>
-      <c r="M19" s="154" t="s">
-        <v>479</v>
-      </c>
-      <c r="N19" s="156"/>
-      <c r="O19" s="155">
+      <c r="N19" s="158"/>
+      <c r="O19" s="157">
         <f>O18+1</f>
         <v>17</v>
       </c>
     </row>
     <row r="20" ht="242.25">
-      <c r="A20" s="151" t="str">
+      <c r="A20" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O20&lt;10,"0",""),O20)</f>
         <v>q18</v>
       </c>
-      <c r="B20" s="144" t="str">
+      <c r="B20" s="146" t="str">
         <f>B19</f>
         <v>qbank01</v>
       </c>
-      <c r="C20" s="147" t="s">
+      <c r="C20" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="149" t="s">
+        <v>420</v>
+      </c>
+      <c r="F20" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="147" t="s">
-        <v>422</v>
-      </c>
-      <c r="F20" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G20" s="153" t="s">
-        <v>423</v>
-      </c>
-      <c r="H20" s="154" t="s">
+      <c r="G20" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="H20" s="156" t="s">
+        <v>478</v>
+      </c>
+      <c r="I20" s="150"/>
+      <c r="J20" s="156" t="s">
+        <v>479</v>
+      </c>
+      <c r="K20" s="150"/>
+      <c r="L20" s="149">
+        <v>4</v>
+      </c>
+      <c r="M20" s="156" t="s">
         <v>480</v>
       </c>
-      <c r="I20" s="148"/>
-      <c r="J20" s="154" t="s">
-        <v>481</v>
-      </c>
-      <c r="K20" s="148"/>
-      <c r="L20" s="147">
-        <v>4</v>
-      </c>
-      <c r="M20" s="154" t="s">
-        <v>482</v>
-      </c>
-      <c r="N20" s="156"/>
-      <c r="O20" s="155">
+      <c r="N20" s="158"/>
+      <c r="O20" s="157">
         <f>O19+1</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" ht="409.5">
-      <c r="A21" s="151" t="str">
+      <c r="A21" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O21&lt;10,"0",""),O21)</f>
         <v>q19</v>
       </c>
-      <c r="B21" s="144" t="str">
+      <c r="B21" s="146" t="str">
         <f>B20</f>
         <v>qbank01</v>
       </c>
-      <c r="C21" s="147" t="s">
+      <c r="C21" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="149" t="s">
+        <v>450</v>
+      </c>
+      <c r="F21" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="147" t="s">
-        <v>452</v>
-      </c>
-      <c r="F21" s="147" t="s">
-        <v>417</v>
-      </c>
-      <c r="G21" s="153" t="s">
-        <v>470</v>
-      </c>
-      <c r="H21" s="154" t="s">
+      <c r="G21" s="155" t="s">
+        <v>468</v>
+      </c>
+      <c r="H21" s="156" t="s">
+        <v>481</v>
+      </c>
+      <c r="I21" s="149"/>
+      <c r="J21" s="156" t="s">
+        <v>482</v>
+      </c>
+      <c r="K21" s="149"/>
+      <c r="L21" s="149">
+        <v>4</v>
+      </c>
+      <c r="M21" s="156" t="s">
         <v>483</v>
       </c>
-      <c r="I21" s="147"/>
-      <c r="J21" s="154" t="s">
-        <v>484</v>
-      </c>
-      <c r="K21" s="147"/>
-      <c r="L21" s="147">
-        <v>4</v>
-      </c>
-      <c r="M21" s="154" t="s">
-        <v>485</v>
-      </c>
-      <c r="N21" s="147"/>
-      <c r="O21" s="155">
+      <c r="N21" s="149"/>
+      <c r="O21" s="157">
         <f>O20+1</f>
         <v>19</v>
       </c>
     </row>
     <row r="22" ht="114">
-      <c r="A22" s="151" t="str">
+      <c r="A22" s="153" t="str">
         <f>_xlfn.CONCAT("q",IF(O22&lt;10,"0",""),O22)</f>
         <v>q20</v>
       </c>
-      <c r="B22" s="144" t="str">
+      <c r="B22" s="146" t="str">
         <f>B21</f>
         <v>qbank01</v>
       </c>
-      <c r="C22" s="147" t="s">
+      <c r="C22" s="149" t="s">
+        <v>484</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="160" t="s">
+        <v>432</v>
+      </c>
+      <c r="H22" s="156" t="s">
+        <v>485</v>
+      </c>
+      <c r="I22" s="159" t="s">
         <v>486</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="147" t="s">
-        <v>416</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="158" t="s">
-        <v>434</v>
-      </c>
-      <c r="H22" s="154" t="s">
+      <c r="J22" s="156" t="s">
         <v>487</v>
       </c>
-      <c r="I22" s="157" t="s">
+      <c r="K22" s="150"/>
+      <c r="L22" s="161"/>
+      <c r="M22" s="162"/>
+      <c r="N22" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="J22" s="154" t="s">
-        <v>489</v>
-      </c>
-      <c r="K22" s="148"/>
-      <c r="L22" s="159"/>
-      <c r="M22" s="160"/>
-      <c r="N22" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="O22" s="161">
+      <c r="O22" s="163">
         <f>O21+1</f>
         <v>20</v>
       </c>
@@ -7369,37 +7365,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00750062-0011-49DA-979F-00E200D1003D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D5002A-0096-489B-A8E8-00CF004E0075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D40032-005B-4D2F-BC26-00FC000C00B9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002F00E1-007C-4DBC-9F9C-0054009D00D9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0068006C-004F-4179-A4F8-00F7006800EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0001004A-006F-4416-AF5E-00500028007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009000EF-00C0-4B32-A829-00E8006400CE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005200B9-0089-4FA0-BEE1-007500CE0029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B100B7-0041-46B2-870B-002A00CF008E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FE0017-00C8-48B4-8EF2-00360007003C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0006003D-008D-4E5D-9BFD-002200CE0058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00360050-0007-4B30-BB42-000F00480032}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -7550,7 +7546,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007700C5-005A-4899-B553-00C90016005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005700B2-0038-4755-9684-007B00F200DE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -7684,13 +7680,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00650091-0027-472E-91FE-00B8005E00F1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00480074-0028-4278-836E-00EC00D20008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F60066-00F3-4717-97D3-00CC00B800CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CA0025-00FE-47F5-9F2D-004100CD0010}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -8157,13 +8153,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00CC0068-0063-4AD8-BD69-0068001D00BD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006F006E-00C4-4D48-9776-00FD00D20038}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00110085-00A5-4BA4-A310-0028001000EB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001F003C-0045-4389-B6FD-00F100F9005C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPDATED: Library Empty states components
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="13"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="488">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -454,9 +454,6 @@
   </si>
   <si>
     <t>admin01</t>
-  </si>
-  <si>
-    <t>Administrator</t>
   </si>
   <si>
     <t>Leemons</t>
@@ -3313,13 +3310,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -3330,21 +3327,21 @@
         <v>28</v>
       </c>
       <c r="C2" s="105" t="s">
+        <v>308</v>
+      </c>
+      <c r="D2" s="122" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="122" t="s">
         <v>309</v>
-      </c>
-      <c r="D2" s="122" t="s">
-        <v>287</v>
-      </c>
-      <c r="E2" s="122" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>311</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>312</v>
       </c>
       <c r="C3" s="85" t="str">
         <f>ap_programs!$A$4</f>
@@ -3359,10 +3356,10 @@
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>313</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="C4" s="85" t="str">
         <f>ap_programs!$A$4</f>
@@ -3377,10 +3374,10 @@
     </row>
     <row r="5" ht="19.5" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C5" s="85" t="str">
         <f>ap_programs!$A$5</f>
@@ -3395,10 +3392,10 @@
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C6" s="85" t="str">
         <f>ap_programs!$A$5</f>
@@ -3419,7 +3416,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00030072-004B-4021-97AA-0059004E009A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CC00A9-0034-4E0E-87F5-002D009300AF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -3459,19 +3456,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>318</v>
-      </c>
       <c r="F1" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>306</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -3482,19 +3479,19 @@
         <v>28</v>
       </c>
       <c r="C2" s="90" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D2" s="90" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="90" t="s">
         <v>319</v>
       </c>
-      <c r="E2" s="90" t="s">
-        <v>320</v>
-      </c>
       <c r="F2" s="91" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G2" s="124" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" ht="14.25"/>
@@ -3543,46 +3540,46 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="125" t="s">
         <v>327</v>
       </c>
-      <c r="O1" s="125" t="s">
+      <c r="P1" s="125" t="s">
         <v>328</v>
-      </c>
-      <c r="P1" s="125" t="s">
-        <v>329</v>
       </c>
       <c r="Q1" s="18"/>
     </row>
@@ -3596,7 +3593,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -3615,46 +3612,46 @@
         <v>28</v>
       </c>
       <c r="C3" s="106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D3" s="104" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="90" t="s">
         <v>331</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="F3" s="104" t="s">
         <v>332</v>
       </c>
-      <c r="F3" s="104" t="s">
+      <c r="G3" s="104" t="s">
         <v>333</v>
       </c>
-      <c r="G3" s="104" t="s">
+      <c r="H3" s="126" t="s">
+        <v>283</v>
+      </c>
+      <c r="I3" s="127" t="s">
         <v>334</v>
       </c>
-      <c r="H3" s="126" t="s">
-        <v>284</v>
-      </c>
-      <c r="I3" s="127" t="s">
+      <c r="J3" s="127" t="s">
+        <v>318</v>
+      </c>
+      <c r="K3" s="127" t="s">
         <v>335</v>
       </c>
-      <c r="J3" s="127" t="s">
+      <c r="L3" s="127" t="s">
         <v>319</v>
       </c>
-      <c r="K3" s="127" t="s">
+      <c r="M3" s="127" t="s">
         <v>336</v>
       </c>
-      <c r="L3" s="127" t="s">
-        <v>320</v>
-      </c>
-      <c r="M3" s="127" t="s">
+      <c r="N3" s="126" t="s">
         <v>337</v>
       </c>
-      <c r="N3" s="126" t="s">
+      <c r="O3" s="91" t="s">
         <v>338</v>
       </c>
-      <c r="O3" s="91" t="s">
+      <c r="P3" s="91" t="s">
         <v>339</v>
-      </c>
-      <c r="P3" s="91" t="s">
-        <v>340</v>
       </c>
       <c r="Q3" s="128"/>
     </row>
@@ -3664,7 +3661,7 @@
         <v>asignatura01</v>
       </c>
       <c r="B4" s="129" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C4" s="66" t="str">
         <f>ap_programs!A5</f>
@@ -3685,24 +3682,24 @@
         <v>139</v>
       </c>
       <c r="I4" s="130" t="s">
+        <v>341</v>
+      </c>
+      <c r="J4" s="131" t="s">
         <v>342</v>
       </c>
-      <c r="J4" s="131" t="s">
+      <c r="K4" s="132" t="s">
         <v>343</v>
-      </c>
-      <c r="K4" s="132" t="s">
-        <v>344</v>
       </c>
       <c r="L4" s="132"/>
       <c r="M4" s="67"/>
       <c r="N4" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O4" s="133" t="s">
+        <v>344</v>
+      </c>
+      <c r="P4" s="133" t="s">
         <v>345</v>
-      </c>
-      <c r="P4" s="133" t="s">
-        <v>346</v>
       </c>
       <c r="Q4" s="134">
         <v>1</v>
@@ -3714,7 +3711,7 @@
         <v>asignatura02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C5" s="66" t="str">
         <f>C4</f>
@@ -3739,18 +3736,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J5" s="131" t="s">
+        <v>347</v>
+      </c>
+      <c r="K5" s="135" t="s">
         <v>348</v>
-      </c>
-      <c r="K5" s="135" t="s">
-        <v>349</v>
       </c>
       <c r="L5" s="135"/>
       <c r="M5" s="67"/>
       <c r="N5" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O5" s="133" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P5" s="133" t="str">
         <f>P4</f>
@@ -3768,7 +3765,7 @@
         <v>asignatura03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C6" s="66" t="str">
         <f>C5</f>
@@ -3793,18 +3790,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J6" s="131" t="s">
+        <v>351</v>
+      </c>
+      <c r="K6" s="135" t="s">
         <v>352</v>
-      </c>
-      <c r="K6" s="135" t="s">
-        <v>353</v>
       </c>
       <c r="L6" s="135"/>
       <c r="M6" s="67"/>
       <c r="N6" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O6" s="133" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P6" s="133" t="str">
         <f>P5</f>
@@ -3822,7 +3819,7 @@
         <v>asignatura04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C7" s="66" t="str">
         <f>C6</f>
@@ -3847,18 +3844,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J7" s="131" t="s">
+        <v>354</v>
+      </c>
+      <c r="K7" s="135" t="s">
         <v>355</v>
-      </c>
-      <c r="K7" s="135" t="s">
-        <v>356</v>
       </c>
       <c r="L7" s="135"/>
       <c r="M7" s="67"/>
       <c r="N7" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O7" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P7" s="133" t="str">
         <f>P6</f>
@@ -3876,7 +3873,7 @@
         <v>asignatura05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C8" s="66" t="str">
         <f>C7</f>
@@ -3901,18 +3898,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J8" s="131" t="s">
+        <v>357</v>
+      </c>
+      <c r="K8" s="135" t="s">
         <v>358</v>
-      </c>
-      <c r="K8" s="135" t="s">
-        <v>359</v>
       </c>
       <c r="L8" s="135"/>
       <c r="M8" s="67"/>
       <c r="N8" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O8" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P8" s="133" t="str">
         <f>P7</f>
@@ -3929,7 +3926,7 @@
         <v>asignatura06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C9" s="66" t="str">
         <f>C8</f>
@@ -3954,18 +3951,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J9" s="131" t="s">
+        <v>360</v>
+      </c>
+      <c r="K9" s="136" t="s">
         <v>361</v>
-      </c>
-      <c r="K9" s="136" t="s">
-        <v>362</v>
       </c>
       <c r="L9" s="136"/>
       <c r="M9" s="67"/>
       <c r="N9" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O9" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P9" s="133" t="str">
         <f>P8</f>
@@ -3982,7 +3979,7 @@
         <v>asignatura07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C10" s="66" t="str">
         <f>C9</f>
@@ -4007,18 +4004,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J10" s="131" t="s">
+        <v>363</v>
+      </c>
+      <c r="K10" s="137" t="s">
         <v>364</v>
-      </c>
-      <c r="K10" s="137" t="s">
-        <v>365</v>
       </c>
       <c r="L10" s="137"/>
       <c r="M10" s="67"/>
       <c r="N10" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O10" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P10" s="133" t="str">
         <f>P9</f>
@@ -4035,7 +4032,7 @@
         <v>asignatura08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C11" s="66" t="str">
         <f>C10</f>
@@ -4060,18 +4057,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J11" s="131" t="s">
+        <v>366</v>
+      </c>
+      <c r="K11" s="135" t="s">
         <v>367</v>
-      </c>
-      <c r="K11" s="135" t="s">
-        <v>368</v>
       </c>
       <c r="L11" s="135"/>
       <c r="M11" s="67"/>
       <c r="N11" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O11" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P11" s="133" t="str">
         <f>P10</f>
@@ -4088,7 +4085,7 @@
         <v>asignatura09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C12" s="66" t="str">
         <f>C11</f>
@@ -4113,18 +4110,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J12" s="131" t="s">
+        <v>369</v>
+      </c>
+      <c r="K12" s="135" t="s">
         <v>370</v>
-      </c>
-      <c r="K12" s="135" t="s">
-        <v>371</v>
       </c>
       <c r="L12" s="135"/>
       <c r="M12" s="67"/>
       <c r="N12" s="66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O12" s="133" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P12" s="133" t="str">
         <f>P11</f>
@@ -4141,7 +4138,7 @@
         <v>asignatura10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C13" s="66" t="str">
         <f>C12</f>
@@ -4166,18 +4163,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J13" s="131" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K13" s="135" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L13" s="135"/>
       <c r="M13" s="67"/>
       <c r="N13" s="66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O13" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P13" s="133" t="str">
         <f>P12</f>
@@ -4194,7 +4191,7 @@
         <v>asignatura11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C14" s="66" t="str">
         <f>C13</f>
@@ -4219,18 +4216,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J14" s="131" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K14" s="135" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L14" s="135"/>
       <c r="M14" s="67"/>
       <c r="N14" s="66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O14" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P14" s="133" t="str">
         <f>P13</f>
@@ -4247,7 +4244,7 @@
         <v>asignatura12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C15" s="66" t="str">
         <f>C14</f>
@@ -4272,18 +4269,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J15" s="131" t="s">
+        <v>376</v>
+      </c>
+      <c r="K15" s="138" t="s">
         <v>377</v>
-      </c>
-      <c r="K15" s="138" t="s">
-        <v>378</v>
       </c>
       <c r="L15" s="138"/>
       <c r="M15" s="67"/>
       <c r="N15" s="66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O15" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P15" s="133" t="str">
         <f>P14</f>
@@ -4300,7 +4297,7 @@
         <v>asignatura13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C16" s="66" t="str">
         <f>C15</f>
@@ -4325,18 +4322,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J16" s="131" t="s">
+        <v>379</v>
+      </c>
+      <c r="K16" s="135" t="s">
         <v>380</v>
-      </c>
-      <c r="K16" s="135" t="s">
-        <v>381</v>
       </c>
       <c r="L16" s="135"/>
       <c r="M16" s="67"/>
       <c r="N16" s="66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O16" s="133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P16" s="133" t="str">
         <f>P15</f>
@@ -4353,7 +4350,7 @@
         <v>asignatura14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C17" s="66" t="str">
         <f>C16</f>
@@ -4378,18 +4375,18 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J17" s="131" t="s">
+        <v>382</v>
+      </c>
+      <c r="K17" s="135" t="s">
         <v>383</v>
-      </c>
-      <c r="K17" s="135" t="s">
-        <v>384</v>
       </c>
       <c r="L17" s="135"/>
       <c r="M17" s="67"/>
       <c r="N17" s="66" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O17" s="133" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P17" s="133" t="str">
         <f>P16</f>
@@ -4445,7 +4442,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" ht="21.75" customHeight="1">
@@ -4453,7 +4450,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="88" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
@@ -4490,7 +4487,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4513,13 +4510,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>130</v>
@@ -4528,10 +4525,10 @@
         <v>131</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>73</v>
@@ -4579,21 +4576,21 @@
     </row>
     <row r="3" ht="34.5" customHeight="1">
       <c r="A3" s="140" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" s="141" t="s">
         <v>386</v>
-      </c>
-      <c r="B3" s="141" t="s">
-        <v>387</v>
       </c>
       <c r="C3" s="142"/>
       <c r="D3" s="143"/>
       <c r="E3" s="142" t="s">
+        <v>387</v>
+      </c>
+      <c r="F3" s="144" t="s">
         <v>388</v>
       </c>
-      <c r="F3" s="144" t="s">
+      <c r="G3" s="145" t="s">
         <v>389</v>
-      </c>
-      <c r="G3" s="145" t="s">
-        <v>390</v>
       </c>
       <c r="H3" s="146" t="str">
         <f>users!A4</f>
@@ -4604,7 +4601,7 @@
         <v>programB</v>
       </c>
       <c r="J3" s="148" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4"/>
@@ -4658,43 +4655,43 @@
         <v>23</v>
       </c>
       <c r="B1" s="134" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" s="134" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1" s="134" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="134" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="134" t="s">
+      <c r="E1" s="134" t="s">
         <v>393</v>
       </c>
-      <c r="E1" s="134" t="s">
+      <c r="F1" s="134" t="s">
         <v>394</v>
-      </c>
-      <c r="F1" s="134" t="s">
-        <v>395</v>
       </c>
       <c r="G1" s="151" t="s">
         <v>131</v>
       </c>
       <c r="H1" s="134" t="s">
+        <v>395</v>
+      </c>
+      <c r="I1" s="134" t="s">
         <v>396</v>
       </c>
-      <c r="I1" s="134" t="s">
+      <c r="J1" s="134" t="s">
         <v>397</v>
       </c>
-      <c r="J1" s="134" t="s">
+      <c r="K1" s="134" t="s">
         <v>398</v>
       </c>
-      <c r="K1" s="134" t="s">
+      <c r="L1" s="134" t="s">
         <v>399</v>
       </c>
-      <c r="L1" s="134" t="s">
+      <c r="M1" s="134" t="s">
         <v>400</v>
       </c>
-      <c r="M1" s="134" t="s">
+      <c r="N1" s="134" t="s">
         <v>401</v>
-      </c>
-      <c r="N1" s="134" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -4702,43 +4699,43 @@
         <v>27</v>
       </c>
       <c r="B2" s="54" t="s">
+        <v>402</v>
+      </c>
+      <c r="C2" s="104" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="104" t="s">
         <v>403</v>
       </c>
-      <c r="C2" s="104" t="s">
-        <v>247</v>
-      </c>
-      <c r="D2" s="104" t="s">
+      <c r="E2" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>405</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>406</v>
       </c>
       <c r="G2" s="122" t="s">
         <v>138</v>
       </c>
       <c r="H2" s="152" t="s">
+        <v>406</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="122" t="s">
         <v>408</v>
       </c>
-      <c r="J2" s="122" t="s">
+      <c r="K2" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="104" t="s">
+        <v>399</v>
+      </c>
+      <c r="M2" s="122" t="s">
         <v>410</v>
       </c>
-      <c r="L2" s="104" t="s">
-        <v>400</v>
-      </c>
-      <c r="M2" s="122" t="s">
+      <c r="N2" s="7" t="s">
         <v>411</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="3" ht="114">
@@ -4751,31 +4748,31 @@
         <v>qbank01</v>
       </c>
       <c r="C3" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D3" s="149"/>
       <c r="E3" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="F3" s="149" t="s">
         <v>414</v>
       </c>
-      <c r="F3" s="149" t="s">
+      <c r="G3" s="155" t="s">
         <v>415</v>
       </c>
-      <c r="G3" s="155" t="s">
+      <c r="H3" s="156" t="s">
         <v>416</v>
-      </c>
-      <c r="H3" s="156" t="s">
-        <v>417</v>
       </c>
       <c r="I3" s="149"/>
       <c r="J3" s="156" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K3" s="150"/>
       <c r="L3" s="149">
         <v>1</v>
       </c>
       <c r="M3" s="156" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="N3" s="149"/>
       <c r="O3" s="157">
@@ -4792,31 +4789,31 @@
         <v>qbank01</v>
       </c>
       <c r="C4" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D4" s="149"/>
       <c r="E4" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F4" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G4" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F4" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G4" s="155" t="s">
+      <c r="H4" s="156" t="s">
         <v>421</v>
-      </c>
-      <c r="H4" s="156" t="s">
-        <v>422</v>
       </c>
       <c r="I4" s="149"/>
       <c r="J4" s="156" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K4" s="149"/>
       <c r="L4" s="149">
         <v>4</v>
       </c>
       <c r="M4" s="156" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N4" s="149"/>
       <c r="O4" s="157">
@@ -4834,31 +4831,31 @@
         <v>qbank01</v>
       </c>
       <c r="C5" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D5" s="149"/>
       <c r="E5" s="149" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F5" s="149" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G5" s="155" t="s">
+        <v>424</v>
+      </c>
+      <c r="H5" s="156" t="s">
         <v>425</v>
-      </c>
-      <c r="H5" s="156" t="s">
-        <v>426</v>
       </c>
       <c r="I5" s="149"/>
       <c r="J5" s="156" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K5" s="149"/>
       <c r="L5" s="149">
         <v>3</v>
       </c>
       <c r="M5" s="156" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="N5" s="149"/>
       <c r="O5" s="157">
@@ -4876,31 +4873,31 @@
         <v>qbank01</v>
       </c>
       <c r="C6" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D6" s="149"/>
       <c r="E6" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F6" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G6" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F6" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G6" s="155" t="s">
-        <v>421</v>
-      </c>
       <c r="H6" s="156" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I6" s="149"/>
       <c r="J6" s="156" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K6" s="149"/>
       <c r="L6" s="149">
         <v>2</v>
       </c>
       <c r="M6" s="156" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="N6" s="149"/>
       <c r="O6" s="157">
@@ -4918,31 +4915,31 @@
         <v>qbank01</v>
       </c>
       <c r="C7" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D7" s="149"/>
       <c r="E7" s="149" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F7" s="149" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G7" s="155" t="s">
+        <v>431</v>
+      </c>
+      <c r="H7" s="156" t="s">
         <v>432</v>
-      </c>
-      <c r="H7" s="156" t="s">
-        <v>433</v>
       </c>
       <c r="I7" s="149"/>
       <c r="J7" s="156" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K7" s="149"/>
       <c r="L7" s="149">
         <v>1</v>
       </c>
       <c r="M7" s="156" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N7" s="149"/>
       <c r="O7" s="157">
@@ -4960,31 +4957,31 @@
         <v>qbank01</v>
       </c>
       <c r="C8" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D8" s="149"/>
       <c r="E8" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F8" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G8" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F8" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G8" s="155" t="s">
-        <v>421</v>
-      </c>
       <c r="H8" s="156" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I8" s="150"/>
       <c r="J8" s="156" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K8" s="149"/>
       <c r="L8" s="149">
         <v>2</v>
       </c>
       <c r="M8" s="156" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N8" s="158"/>
       <c r="O8" s="157">
@@ -5002,31 +4999,31 @@
         <v>qbank01</v>
       </c>
       <c r="C9" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D9" s="149"/>
       <c r="E9" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F9" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G9" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F9" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G9" s="155" t="s">
-        <v>421</v>
-      </c>
       <c r="H9" s="156" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I9" s="150"/>
       <c r="J9" s="156" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K9" s="149"/>
       <c r="L9" s="149">
         <v>3</v>
       </c>
       <c r="M9" s="156" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N9" s="149"/>
       <c r="O9" s="157">
@@ -5044,31 +5041,31 @@
         <v>qbank01</v>
       </c>
       <c r="C10" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D10" s="149"/>
       <c r="E10" s="149" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F10" s="149" t="s">
+        <v>441</v>
+      </c>
+      <c r="G10" s="155" t="s">
+        <v>424</v>
+      </c>
+      <c r="H10" s="156" t="s">
         <v>442</v>
-      </c>
-      <c r="G10" s="155" t="s">
-        <v>425</v>
-      </c>
-      <c r="H10" s="156" t="s">
-        <v>443</v>
       </c>
       <c r="I10" s="149"/>
       <c r="J10" s="149"/>
       <c r="K10" s="159" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L10" s="149">
         <v>2</v>
       </c>
       <c r="M10" s="156" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="N10" s="149"/>
       <c r="O10" s="157">
@@ -5086,33 +5083,33 @@
         <v>qbank01</v>
       </c>
       <c r="C11" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D11" s="149"/>
       <c r="E11" s="149" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F11" s="149" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G11" s="155" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H11" s="156" t="s">
+        <v>445</v>
+      </c>
+      <c r="I11" s="159" t="s">
         <v>446</v>
       </c>
-      <c r="I11" s="159" t="s">
+      <c r="J11" s="156" t="s">
         <v>447</v>
-      </c>
-      <c r="J11" s="156" t="s">
-        <v>448</v>
       </c>
       <c r="K11" s="149"/>
       <c r="L11" s="149">
         <v>1</v>
       </c>
       <c r="M11" s="156" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N11" s="149"/>
       <c r="O11" s="157">
@@ -5130,31 +5127,31 @@
         <v>qbank01</v>
       </c>
       <c r="C12" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D12" s="149"/>
       <c r="E12" s="149" t="s">
+        <v>449</v>
+      </c>
+      <c r="F12" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G12" s="155" t="s">
+        <v>420</v>
+      </c>
+      <c r="H12" s="156" t="s">
         <v>450</v>
-      </c>
-      <c r="F12" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G12" s="155" t="s">
-        <v>421</v>
-      </c>
-      <c r="H12" s="156" t="s">
-        <v>451</v>
       </c>
       <c r="I12" s="149"/>
       <c r="J12" s="160" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K12" s="149"/>
       <c r="L12" s="149">
         <v>4</v>
       </c>
       <c r="M12" s="156" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N12" s="149"/>
       <c r="O12" s="157">
@@ -5172,31 +5169,31 @@
         <v>qbank01</v>
       </c>
       <c r="C13" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D13" s="149"/>
       <c r="E13" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F13" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G13" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F13" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G13" s="155" t="s">
-        <v>421</v>
-      </c>
       <c r="H13" s="156" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I13" s="149"/>
       <c r="J13" s="156" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K13" s="149"/>
       <c r="L13" s="149">
         <v>3</v>
       </c>
       <c r="M13" s="156" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N13" s="149"/>
       <c r="O13" s="157">
@@ -5214,31 +5211,31 @@
         <v>qbank01</v>
       </c>
       <c r="C14" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D14" s="149"/>
       <c r="E14" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F14" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G14" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F14" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G14" s="155" t="s">
-        <v>421</v>
-      </c>
       <c r="H14" s="156" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I14" s="149"/>
       <c r="J14" s="156" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K14" s="149"/>
       <c r="L14" s="149">
         <v>1</v>
       </c>
       <c r="M14" s="156" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="N14" s="149"/>
       <c r="O14" s="157">
@@ -5256,33 +5253,33 @@
         <v>qbank01</v>
       </c>
       <c r="C15" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="149" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F15" s="149" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G15" s="155" t="s">
+        <v>459</v>
+      </c>
+      <c r="H15" s="156" t="s">
         <v>460</v>
       </c>
-      <c r="H15" s="156" t="s">
+      <c r="I15" s="149" t="s">
         <v>461</v>
       </c>
-      <c r="I15" s="149" t="s">
+      <c r="J15" s="156" t="s">
         <v>462</v>
-      </c>
-      <c r="J15" s="156" t="s">
-        <v>463</v>
       </c>
       <c r="K15" s="150"/>
       <c r="L15" s="149">
         <v>2</v>
       </c>
       <c r="M15" s="156" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N15" s="149"/>
       <c r="O15" s="157">
@@ -5300,33 +5297,33 @@
         <v>qbank01</v>
       </c>
       <c r="C16" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="149" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F16" s="149" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G16" s="155" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H16" s="156" t="s">
+        <v>464</v>
+      </c>
+      <c r="I16" s="149" t="s">
+        <v>461</v>
+      </c>
+      <c r="J16" s="156" t="s">
         <v>465</v>
-      </c>
-      <c r="I16" s="149" t="s">
-        <v>462</v>
-      </c>
-      <c r="J16" s="156" t="s">
-        <v>466</v>
       </c>
       <c r="K16" s="150"/>
       <c r="L16" s="149">
         <v>1</v>
       </c>
       <c r="M16" s="156" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="N16" s="158"/>
       <c r="O16" s="157">
@@ -5344,31 +5341,31 @@
         <v>qbank01</v>
       </c>
       <c r="C17" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="149" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F17" s="149" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G17" s="155" t="s">
+        <v>467</v>
+      </c>
+      <c r="H17" s="156" t="s">
         <v>468</v>
-      </c>
-      <c r="H17" s="156" t="s">
-        <v>469</v>
       </c>
       <c r="I17" s="150"/>
       <c r="J17" s="156" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K17" s="150"/>
       <c r="L17" s="149">
         <v>2</v>
       </c>
       <c r="M17" s="156" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="N17" s="158"/>
       <c r="O17" s="157">
@@ -5386,31 +5383,31 @@
         <v>qbank01</v>
       </c>
       <c r="C18" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="149" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F18" s="149" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G18" s="155" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H18" s="156" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I18" s="150"/>
       <c r="J18" s="156" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K18" s="150"/>
       <c r="L18" s="149">
         <v>1</v>
       </c>
       <c r="M18" s="156" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N18" s="158"/>
       <c r="O18" s="157">
@@ -5428,31 +5425,31 @@
         <v>qbank01</v>
       </c>
       <c r="C19" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F19" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G19" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F19" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G19" s="155" t="s">
-        <v>421</v>
-      </c>
       <c r="H19" s="156" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I19" s="150"/>
       <c r="J19" s="156" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K19" s="150"/>
       <c r="L19" s="149">
         <v>3</v>
       </c>
       <c r="M19" s="156" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="N19" s="158"/>
       <c r="O19" s="157">
@@ -5470,31 +5467,31 @@
         <v>qbank01</v>
       </c>
       <c r="C20" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="149" t="s">
+        <v>419</v>
+      </c>
+      <c r="F20" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="G20" s="155" t="s">
         <v>420</v>
       </c>
-      <c r="F20" s="149" t="s">
-        <v>415</v>
-      </c>
-      <c r="G20" s="155" t="s">
-        <v>421</v>
-      </c>
       <c r="H20" s="156" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I20" s="150"/>
       <c r="J20" s="156" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K20" s="150"/>
       <c r="L20" s="149">
         <v>4</v>
       </c>
       <c r="M20" s="156" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="N20" s="158"/>
       <c r="O20" s="157">
@@ -5512,31 +5509,31 @@
         <v>qbank01</v>
       </c>
       <c r="C21" s="149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="149" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F21" s="149" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G21" s="155" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H21" s="156" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I21" s="149"/>
       <c r="J21" s="156" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K21" s="149"/>
       <c r="L21" s="149">
         <v>4</v>
       </c>
       <c r="M21" s="156" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N21" s="149"/>
       <c r="O21" s="157">
@@ -5554,30 +5551,30 @@
         <v>qbank01</v>
       </c>
       <c r="C22" s="149" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="149" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="160" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H22" s="156" t="s">
+        <v>484</v>
+      </c>
+      <c r="I22" s="159" t="s">
         <v>485</v>
       </c>
-      <c r="I22" s="159" t="s">
+      <c r="J22" s="156" t="s">
         <v>486</v>
-      </c>
-      <c r="J22" s="156" t="s">
-        <v>487</v>
       </c>
       <c r="K22" s="150"/>
       <c r="L22" s="161"/>
       <c r="M22" s="162"/>
       <c r="N22" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O22" s="163">
         <f>O21+1</f>
@@ -5788,27 +5785,27 @@
         <v>plugins.academic-portfolio.tree</v>
       </c>
       <c r="P1" s="16" t="str">
-        <f t="shared" ref="P1:U1" si="0">_xlfn.CONCAT($P$3,".",P5)</f>
+        <f>_xlfn.CONCAT($P$3,".",P5)</f>
         <v>plugins.families.families</v>
       </c>
       <c r="Q1" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT($P$3,".",Q5)</f>
         <v>plugins.families.config</v>
       </c>
       <c r="R1" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT($P$3,".",R5)</f>
         <v>plugins.families.families-basic-info</v>
       </c>
       <c r="S1" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT($P$3,".",S5)</f>
         <v>plugins.families.families-custom-info</v>
       </c>
       <c r="T1" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT($P$3,".",T5)</f>
         <v>plugins.families.families-guardians-info</v>
       </c>
       <c r="U1" s="16" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT($P$3,".",U5)</f>
         <v>plugins.families.families-students-info</v>
       </c>
       <c r="V1" s="16" t="str">
@@ -6410,8 +6407,8 @@
         <v>121</v>
       </c>
       <c r="D9" s="66"/>
-      <c r="E9" s="67" t="s">
-        <v>110</v>
+      <c r="E9" s="70" t="s">
+        <v>116</v>
       </c>
       <c r="F9" s="67" t="s">
         <v>110</v>
@@ -6419,9 +6416,7 @@
       <c r="G9" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="H9" s="67" t="s">
-        <v>116</v>
-      </c>
+      <c r="H9" s="67"/>
       <c r="I9" s="67" t="s">
         <v>117</v>
       </c>
@@ -6500,8 +6495,8 @@
         <f>A9</f>
         <v>student</v>
       </c>
-      <c r="E10" s="67" t="s">
-        <v>110</v>
+      <c r="E10" s="70" t="s">
+        <v>116</v>
       </c>
       <c r="F10" s="67" t="s">
         <v>110</v>
@@ -6509,9 +6504,7 @@
       <c r="G10" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="H10" s="67" t="s">
-        <v>116</v>
-      </c>
+      <c r="H10" s="67"/>
       <c r="I10" s="67" t="s">
         <v>117</v>
       </c>
@@ -6591,7 +6584,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="180" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="180" workbookViewId="0">
       <selection activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -6684,11 +6677,11 @@
       <c r="A3" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>12</v>
@@ -6697,31 +6690,31 @@
         <v>36526</v>
       </c>
       <c r="F3" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="H3" s="70" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="67"/>
       <c r="J3" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" s="76" t="s">
         <v>144</v>
-      </c>
-      <c r="K3" s="76" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>12</v>
@@ -6730,10 +6723,10 @@
         <v>27670</v>
       </c>
       <c r="F4" s="75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H4" s="70" t="str">
         <f>H3</f>
@@ -6741,21 +6734,21 @@
       </c>
       <c r="I4" s="67"/>
       <c r="J4" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" s="76" t="s">
         <v>150</v>
-      </c>
-      <c r="K4" s="76" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>153</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
@@ -6764,34 +6757,34 @@
         <v>27518</v>
       </c>
       <c r="F5" s="77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H5" s="70" t="str">
         <f>H4</f>
         <v>es</v>
       </c>
       <c r="I5" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="J5" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="J5" s="70" t="s">
+      <c r="K5" s="78" t="s">
         <v>156</v>
-      </c>
-      <c r="K5" s="78" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>159</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>160</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -6800,10 +6793,10 @@
         <v>34447</v>
       </c>
       <c r="F6" s="80" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="81" t="str">
         <f>H5</f>
@@ -6811,21 +6804,21 @@
       </c>
       <c r="I6" s="82"/>
       <c r="J6" s="81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K6" s="76" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A7" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
@@ -6834,33 +6827,33 @@
         <v>27791</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" s="70" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" s="67" t="s">
         <v>167</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="K7" s="78" t="s">
         <v>168</v>
-      </c>
-      <c r="K7" s="78" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>12</v>
@@ -6869,34 +6862,34 @@
         <v>39571</v>
       </c>
       <c r="F8" s="77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" s="70" t="str">
         <f>H6</f>
         <v>es</v>
       </c>
       <c r="I8" s="67" t="s">
+        <v>173</v>
+      </c>
+      <c r="J8" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="J8" s="70" t="s">
+      <c r="K8" s="78" t="s">
         <v>175</v>
-      </c>
-      <c r="K8" s="78" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
@@ -6905,35 +6898,35 @@
         <v>39572</v>
       </c>
       <c r="F9" s="75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" s="70" t="str">
         <f>H8</f>
         <v>es</v>
       </c>
       <c r="I9" s="67" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J9" s="67" t="str">
         <f>J8</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K9" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>183</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>184</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>13</v>
@@ -6942,35 +6935,35 @@
         <v>39573</v>
       </c>
       <c r="F10" s="75" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H10" s="70" t="str">
         <f>H9</f>
         <v>es</v>
       </c>
       <c r="I10" s="67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J10" s="67" t="str">
         <f>J9</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K10" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A11" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>188</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>189</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>12</v>
@@ -6979,35 +6972,35 @@
         <v>39208</v>
       </c>
       <c r="F11" s="75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="70" t="str">
         <f>H10</f>
         <v>es</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J11" s="67" t="str">
         <f>J10</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K11" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A12" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>193</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>13</v>
@@ -7016,35 +7009,35 @@
         <v>39575</v>
       </c>
       <c r="F12" s="77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H12" s="70" t="str">
         <f>H11</f>
         <v>es</v>
       </c>
       <c r="I12" s="67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J12" s="67" t="str">
         <f>J11</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K12" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>13</v>
@@ -7053,35 +7046,35 @@
         <v>39576</v>
       </c>
       <c r="F13" s="77" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H13" s="70" t="str">
         <f>H12</f>
         <v>es</v>
       </c>
       <c r="I13" s="67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J13" s="67" t="str">
         <f>J12</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K13" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>204</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>12</v>
@@ -7090,35 +7083,35 @@
         <v>39577</v>
       </c>
       <c r="F14" s="77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H14" s="70" t="str">
         <f>H13</f>
         <v>es</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J14" s="67" t="str">
         <f>J13</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K14" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A15" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>208</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>209</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>13</v>
@@ -7127,35 +7120,35 @@
         <v>39578</v>
       </c>
       <c r="F15" s="77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" s="70" t="str">
         <f>H14</f>
         <v>es</v>
       </c>
       <c r="I15" s="67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J15" s="67" t="str">
         <f>J14</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K15" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A16" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>12</v>
@@ -7164,35 +7157,35 @@
         <v>39579</v>
       </c>
       <c r="F16" s="77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" s="70" t="str">
         <f>H15</f>
         <v>es</v>
       </c>
       <c r="I16" s="67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J16" s="67" t="str">
         <f>J15</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K16" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>218</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>219</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>12</v>
@@ -7201,35 +7194,35 @@
         <v>39580</v>
       </c>
       <c r="F17" s="77" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" s="70" t="str">
         <f>H16</f>
         <v>es</v>
       </c>
       <c r="I17" s="67" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J17" s="67" t="str">
         <f>J16</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K17" s="78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>222</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>223</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -7238,10 +7231,10 @@
         <v>39575</v>
       </c>
       <c r="F18" s="83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" s="81" t="str">
         <f>H17</f>
@@ -7253,18 +7246,18 @@
         <v>Estudiante,Test</v>
       </c>
       <c r="K18" s="76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>198</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>199</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -7273,10 +7266,10 @@
         <v>39576</v>
       </c>
       <c r="F19" s="83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H19" s="81" t="str">
         <f>H18</f>
@@ -7288,18 +7281,18 @@
         <v>Estudiante,Test</v>
       </c>
       <c r="K19" s="76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>203</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>204</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>12</v>
@@ -7308,10 +7301,10 @@
         <v>39577</v>
       </c>
       <c r="F20" s="83" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H20" s="81" t="str">
         <f>H19</f>
@@ -7323,7 +7316,7 @@
         <v>Estudiante,Test</v>
       </c>
       <c r="K20" s="76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" ht="14.25"/>
@@ -7365,37 +7358,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D5002A-0096-489B-A8E8-00CF004E0075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0009007D-0029-4B26-BD68-00D700B80028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002F00E1-007C-4DBC-9F9C-0054009D00D9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0043001B-0046-4020-A628-00DA007B0055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0001004A-006F-4416-AF5E-00500028007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00200016-0038-4BC7-9B63-0029000F0020}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005200B9-0089-4FA0-BEE1-007500CE0029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A100FB-00E7-4B3C-96B4-004A00E8005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE0017-00C8-48B4-8EF2-00360007003C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002400AB-0074-445A-8B6B-00C300C700E0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00360050-0007-4B30-BB42-000F00480032}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00100063-00A0-4E3B-9DFB-00C4001600A6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -7430,7 +7423,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
@@ -7438,7 +7431,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="84" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
@@ -7495,13 +7488,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" ht="24.25" customHeight="1">
@@ -7512,30 +7505,30 @@
         <v>28</v>
       </c>
       <c r="C2" s="88" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="84" t="s">
         <v>235</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="E2" s="73" t="s">
         <v>236</v>
-      </c>
-      <c r="E2" s="73" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="76" t="s">
         <v>239</v>
-      </c>
-      <c r="C3" s="76" t="s">
-        <v>240</v>
       </c>
       <c r="D3" s="89" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="85" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -7546,7 +7539,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{005700B2-0038-4755-9684-007B00F200DE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F5008B-00D2-4541-818D-007C00DF00D0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -7586,19 +7579,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="2" ht="24.75" customHeight="1">
@@ -7612,24 +7605,24 @@
         <v>93</v>
       </c>
       <c r="D2" s="90" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="90" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="90" t="s">
+      <c r="F2" s="90" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="G2" s="90" t="s">
         <v>249</v>
-      </c>
-      <c r="G2" s="90" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3" ht="146.25" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>252</v>
       </c>
       <c r="C3" s="85" t="str">
         <f>centers!$A$3</f>
@@ -7642,7 +7635,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G3" s="67">
         <v>5</v>
@@ -7650,10 +7643,10 @@
     </row>
     <row r="4" s="18" customFormat="1" ht="146.25" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>255</v>
       </c>
       <c r="C4" s="85" t="str">
         <f>centers!$A$4</f>
@@ -7666,7 +7659,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G4" s="67">
         <v>5</v>
@@ -7680,13 +7673,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00480074-0028-4278-836E-00EC00D20008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C60015-00E0-429F-B02C-003300CF00EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CA0025-00FE-47F5-9F2D-004100CD0010}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005C008C-00DE-4AA0-A1FC-00F400E4009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7720,7 +7713,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
@@ -7728,7 +7721,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="88" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
@@ -7801,73 +7794,73 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>277</v>
       </c>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
@@ -7889,11 +7882,11 @@
     <row r="2" s="9" customFormat="1" ht="23.5" customHeight="1">
       <c r="C2" s="9"/>
       <c r="G2" s="93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H2" s="93"/>
       <c r="I2" s="94" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J2" s="95"/>
       <c r="K2" s="95"/>
@@ -7902,18 +7895,18 @@
       <c r="N2" s="95"/>
       <c r="O2" s="96"/>
       <c r="P2" s="97" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q2" s="97"/>
       <c r="R2" s="97"/>
       <c r="S2" s="98" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="T2" s="99"/>
       <c r="U2" s="99"/>
       <c r="V2" s="100"/>
       <c r="W2" s="101" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="X2" s="102"/>
       <c r="Y2" s="102"/>
@@ -7926,84 +7919,84 @@
         <v>28</v>
       </c>
       <c r="C3" s="90" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="105" t="s">
         <v>283</v>
-      </c>
-      <c r="D3" s="105" t="s">
-        <v>284</v>
       </c>
       <c r="E3" s="105" t="s">
         <v>93</v>
       </c>
       <c r="F3" s="106" t="s">
+        <v>284</v>
+      </c>
+      <c r="G3" s="107" t="s">
         <v>285</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="H3" s="108" t="s">
         <v>286</v>
       </c>
-      <c r="H3" s="108" t="s">
+      <c r="I3" s="109" t="s">
         <v>287</v>
       </c>
-      <c r="I3" s="109" t="s">
+      <c r="J3" s="110" t="s">
         <v>288</v>
       </c>
-      <c r="J3" s="110" t="s">
+      <c r="K3" s="111" t="s">
         <v>289</v>
       </c>
-      <c r="K3" s="111" t="s">
+      <c r="L3" s="111" t="s">
         <v>290</v>
       </c>
-      <c r="L3" s="111" t="s">
+      <c r="M3" s="111" t="s">
         <v>291</v>
       </c>
-      <c r="M3" s="111" t="s">
+      <c r="N3" s="111" t="s">
         <v>292</v>
       </c>
-      <c r="N3" s="111" t="s">
+      <c r="O3" s="111" t="s">
         <v>293</v>
       </c>
-      <c r="O3" s="111" t="s">
+      <c r="P3" s="112" t="s">
         <v>294</v>
       </c>
-      <c r="P3" s="112" t="s">
+      <c r="Q3" s="113" t="s">
+        <v>292</v>
+      </c>
+      <c r="R3" s="114" t="s">
+        <v>293</v>
+      </c>
+      <c r="S3" s="115" t="s">
         <v>295</v>
       </c>
-      <c r="Q3" s="113" t="s">
+      <c r="T3" s="116" t="s">
+        <v>296</v>
+      </c>
+      <c r="U3" s="116" t="s">
+        <v>292</v>
+      </c>
+      <c r="V3" s="116" t="s">
         <v>293</v>
       </c>
-      <c r="R3" s="114" t="s">
-        <v>294</v>
-      </c>
-      <c r="S3" s="115" t="s">
-        <v>296</v>
-      </c>
-      <c r="T3" s="116" t="s">
+      <c r="W3" s="117" t="s">
+        <v>292</v>
+      </c>
+      <c r="X3" s="118" t="s">
         <v>297</v>
       </c>
-      <c r="U3" s="116" t="s">
-        <v>293</v>
-      </c>
-      <c r="V3" s="116" t="s">
-        <v>294</v>
-      </c>
-      <c r="W3" s="117" t="s">
-        <v>293</v>
-      </c>
-      <c r="X3" s="118" t="s">
+      <c r="Y3" s="119" t="s">
         <v>298</v>
-      </c>
-      <c r="Y3" s="119" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>301</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>302</v>
       </c>
       <c r="D4" s="120" t="s">
         <v>139</v>
@@ -8064,13 +8057,13 @@
     </row>
     <row r="5" s="9" customFormat="1" ht="46.5" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>304</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D5" s="120" t="s">
         <v>139</v>
@@ -8097,7 +8090,7 @@
         <v>10</v>
       </c>
       <c r="L5" s="121" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M5" s="67" t="s">
         <v>4</v>
@@ -8153,13 +8146,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{006F006E-00C4-4D48-9776-00FD00D20038}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001000A5-00D9-452B-A7AA-004E000F0011}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001F003C-0045-4389-B6FD-00F100F9005C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002E00FE-0047-4FE8-B848-00D9009A00DA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPDATED: Some excel data
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="490">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -456,7 +456,7 @@
     <t>admin01</t>
   </si>
   <si>
-    <t>Leemons</t>
+    <t>Estefanía</t>
   </si>
   <si>
     <t>admin@leemons.io</t>
@@ -465,6 +465,9 @@
     <t>testing</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/estefania_admin_abdb21ea4f.jpg</t>
+  </si>
+  <si>
     <t>Admin,Test</t>
   </si>
   <si>
@@ -483,6 +486,9 @@
     <t>teacher@leemons.io</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/willy_teacher_6b95ec70a2.png</t>
+  </si>
+  <si>
     <t>Profesor,Test</t>
   </si>
   <si>
@@ -537,7 +543,7 @@
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Nicole_guardian_f753e6763e.png</t>
   </si>
   <si>
-    <t>Guardian,Test</t>
+    <t>Tutora,Test</t>
   </si>
   <si>
     <t>guardian@centerB</t>
@@ -2159,7 +2165,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="165">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2380,6 +2386,9 @@
     </xf>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3310,40 +3319,40 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="105" t="s">
-        <v>308</v>
-      </c>
-      <c r="D2" s="122" t="s">
-        <v>286</v>
-      </c>
-      <c r="E2" s="122" t="s">
-        <v>309</v>
+      <c r="C2" s="106" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" s="123" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" s="123" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="C3" s="85" t="str">
+        <v>313</v>
+      </c>
+      <c r="C3" s="86" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
@@ -3356,12 +3365,12 @@
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C4" s="85" t="str">
+        <v>315</v>
+      </c>
+      <c r="C4" s="86" t="str">
         <f>ap_programs!$A$4</f>
         <v>programA</v>
       </c>
@@ -3374,12 +3383,12 @@
     </row>
     <row r="5" ht="19.5" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="C5" s="85" t="str">
+        <v>313</v>
+      </c>
+      <c r="C5" s="86" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -3392,12 +3401,12 @@
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C6" s="85" t="str">
+      <c r="C6" s="86" t="str">
         <f>ap_programs!$A$5</f>
         <v>programB</v>
       </c>
@@ -3416,7 +3425,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00CC00A9-0034-4E0E-87F5-002D009300AF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001900C1-007D-44A7-9A53-002A00330035}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -3456,42 +3465,42 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="90" t="s">
-        <v>282</v>
-      </c>
-      <c r="D2" s="90" t="s">
-        <v>318</v>
-      </c>
-      <c r="E2" s="90" t="s">
-        <v>319</v>
-      </c>
-      <c r="F2" s="91" t="s">
-        <v>308</v>
-      </c>
-      <c r="G2" s="124" t="s">
-        <v>286</v>
+      <c r="C2" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" s="91" t="s">
+        <v>320</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="92" t="s">
+        <v>310</v>
+      </c>
+      <c r="G2" s="125" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="3" ht="14.25"/>
@@ -3540,46 +3549,46 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="O1" s="125" t="s">
-        <v>327</v>
-      </c>
-      <c r="P1" s="125" t="s">
         <v>328</v>
+      </c>
+      <c r="O1" s="126" t="s">
+        <v>329</v>
+      </c>
+      <c r="P1" s="126" t="s">
+        <v>330</v>
       </c>
       <c r="Q1" s="18"/>
     </row>
@@ -3593,7 +3602,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -3605,63 +3614,63 @@
       <c r="Q2" s="18"/>
     </row>
     <row r="3" ht="31.75" customHeight="1">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="106" t="s">
-        <v>308</v>
-      </c>
-      <c r="D3" s="104" t="s">
-        <v>330</v>
-      </c>
-      <c r="E3" s="90" t="s">
-        <v>331</v>
-      </c>
-      <c r="F3" s="104" t="s">
+      <c r="C3" s="107" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="105" t="s">
         <v>332</v>
       </c>
-      <c r="G3" s="104" t="s">
+      <c r="E3" s="91" t="s">
         <v>333</v>
       </c>
-      <c r="H3" s="126" t="s">
-        <v>283</v>
-      </c>
-      <c r="I3" s="127" t="s">
+      <c r="F3" s="105" t="s">
         <v>334</v>
       </c>
-      <c r="J3" s="127" t="s">
-        <v>318</v>
-      </c>
-      <c r="K3" s="127" t="s">
+      <c r="G3" s="105" t="s">
         <v>335</v>
       </c>
-      <c r="L3" s="127" t="s">
-        <v>319</v>
-      </c>
-      <c r="M3" s="127" t="s">
+      <c r="H3" s="127" t="s">
+        <v>285</v>
+      </c>
+      <c r="I3" s="128" t="s">
         <v>336</v>
       </c>
-      <c r="N3" s="126" t="s">
+      <c r="J3" s="128" t="s">
+        <v>320</v>
+      </c>
+      <c r="K3" s="128" t="s">
         <v>337</v>
       </c>
-      <c r="O3" s="91" t="s">
+      <c r="L3" s="128" t="s">
+        <v>321</v>
+      </c>
+      <c r="M3" s="128" t="s">
         <v>338</v>
       </c>
-      <c r="P3" s="91" t="s">
+      <c r="N3" s="127" t="s">
         <v>339</v>
       </c>
-      <c r="Q3" s="128"/>
+      <c r="O3" s="92" t="s">
+        <v>340</v>
+      </c>
+      <c r="P3" s="92" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q3" s="129"/>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="str">
         <f>_xlfn.CONCAT("asignatura",IF(Q4&lt;10,"0",""),Q4)</f>
         <v>asignatura01</v>
       </c>
-      <c r="B4" s="129" t="s">
-        <v>340</v>
+      <c r="B4" s="130" t="s">
+        <v>342</v>
       </c>
       <c r="C4" s="66" t="str">
         <f>ap_programs!A5</f>
@@ -3681,27 +3690,27 @@
       <c r="H4" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I4" s="130" t="s">
-        <v>341</v>
-      </c>
-      <c r="J4" s="131" t="s">
-        <v>342</v>
-      </c>
-      <c r="K4" s="132" t="s">
+      <c r="I4" s="131" t="s">
         <v>343</v>
       </c>
-      <c r="L4" s="132"/>
+      <c r="J4" s="132" t="s">
+        <v>344</v>
+      </c>
+      <c r="K4" s="133" t="s">
+        <v>345</v>
+      </c>
+      <c r="L4" s="133"/>
       <c r="M4" s="67"/>
       <c r="N4" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O4" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P4" s="133" t="s">
-        <v>345</v>
-      </c>
-      <c r="Q4" s="134">
+        <v>316</v>
+      </c>
+      <c r="O4" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P4" s="134" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q4" s="135">
         <v>1</v>
       </c>
     </row>
@@ -3711,7 +3720,7 @@
         <v>asignatura02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C5" s="66" t="str">
         <f>C4</f>
@@ -3731,29 +3740,29 @@
       <c r="H5" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I5" s="130" t="str">
+      <c r="I5" s="131" t="str">
         <f>I4</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J5" s="131" t="s">
-        <v>347</v>
-      </c>
-      <c r="K5" s="135" t="s">
-        <v>348</v>
-      </c>
-      <c r="L5" s="135"/>
+      <c r="J5" s="132" t="s">
+        <v>349</v>
+      </c>
+      <c r="K5" s="136" t="s">
+        <v>350</v>
+      </c>
+      <c r="L5" s="136"/>
       <c r="M5" s="67"/>
       <c r="N5" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O5" s="133" t="s">
-        <v>349</v>
-      </c>
-      <c r="P5" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O5" s="134" t="s">
+        <v>351</v>
+      </c>
+      <c r="P5" s="134" t="str">
         <f>P4</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q5" s="134">
+      <c r="Q5" s="135">
         <f>Q4+1</f>
         <v>2</v>
       </c>
@@ -3765,7 +3774,7 @@
         <v>asignatura03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C6" s="66" t="str">
         <f>C5</f>
@@ -3785,29 +3794,29 @@
       <c r="H6" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I6" s="130" t="str">
+      <c r="I6" s="131" t="str">
         <f>I5</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J6" s="131" t="s">
-        <v>351</v>
-      </c>
-      <c r="K6" s="135" t="s">
-        <v>352</v>
-      </c>
-      <c r="L6" s="135"/>
+      <c r="J6" s="132" t="s">
+        <v>353</v>
+      </c>
+      <c r="K6" s="136" t="s">
+        <v>354</v>
+      </c>
+      <c r="L6" s="136"/>
       <c r="M6" s="67"/>
       <c r="N6" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O6" s="133" t="s">
-        <v>349</v>
-      </c>
-      <c r="P6" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O6" s="134" t="s">
+        <v>351</v>
+      </c>
+      <c r="P6" s="134" t="str">
         <f>P5</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q6" s="134">
+      <c r="Q6" s="135">
         <f>Q5+1</f>
         <v>3</v>
       </c>
@@ -3819,7 +3828,7 @@
         <v>asignatura04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C7" s="66" t="str">
         <f>C6</f>
@@ -3839,29 +3848,29 @@
       <c r="H7" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I7" s="130" t="str">
+      <c r="I7" s="131" t="str">
         <f>I6</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J7" s="131" t="s">
-        <v>354</v>
-      </c>
-      <c r="K7" s="135" t="s">
-        <v>355</v>
-      </c>
-      <c r="L7" s="135"/>
+      <c r="J7" s="132" t="s">
+        <v>356</v>
+      </c>
+      <c r="K7" s="136" t="s">
+        <v>357</v>
+      </c>
+      <c r="L7" s="136"/>
       <c r="M7" s="67"/>
       <c r="N7" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O7" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P7" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O7" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P7" s="134" t="str">
         <f>P6</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q7" s="134">
+      <c r="Q7" s="135">
         <f>Q6+1</f>
         <v>4</v>
       </c>
@@ -3873,7 +3882,7 @@
         <v>asignatura05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C8" s="66" t="str">
         <f>C7</f>
@@ -3893,29 +3902,29 @@
       <c r="H8" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="130" t="str">
+      <c r="I8" s="131" t="str">
         <f>I7</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J8" s="131" t="s">
-        <v>357</v>
-      </c>
-      <c r="K8" s="135" t="s">
-        <v>358</v>
-      </c>
-      <c r="L8" s="135"/>
+      <c r="J8" s="132" t="s">
+        <v>359</v>
+      </c>
+      <c r="K8" s="136" t="s">
+        <v>360</v>
+      </c>
+      <c r="L8" s="136"/>
       <c r="M8" s="67"/>
       <c r="N8" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O8" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P8" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O8" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P8" s="134" t="str">
         <f>P7</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q8" s="134">
+      <c r="Q8" s="135">
         <f>Q7+1</f>
         <v>5</v>
       </c>
@@ -3926,7 +3935,7 @@
         <v>asignatura06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C9" s="66" t="str">
         <f>C8</f>
@@ -3946,29 +3955,29 @@
       <c r="H9" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I9" s="130" t="str">
+      <c r="I9" s="131" t="str">
         <f>I8</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J9" s="131" t="s">
-        <v>360</v>
-      </c>
-      <c r="K9" s="136" t="s">
-        <v>361</v>
-      </c>
-      <c r="L9" s="136"/>
+      <c r="J9" s="132" t="s">
+        <v>362</v>
+      </c>
+      <c r="K9" s="137" t="s">
+        <v>363</v>
+      </c>
+      <c r="L9" s="137"/>
       <c r="M9" s="67"/>
       <c r="N9" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O9" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P9" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O9" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P9" s="134" t="str">
         <f>P8</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q9" s="134">
+      <c r="Q9" s="135">
         <f>Q8+1</f>
         <v>6</v>
       </c>
@@ -3979,7 +3988,7 @@
         <v>asignatura07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C10" s="66" t="str">
         <f>C9</f>
@@ -3999,29 +4008,29 @@
       <c r="H10" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I10" s="130" t="str">
+      <c r="I10" s="131" t="str">
         <f>I9</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J10" s="131" t="s">
-        <v>363</v>
-      </c>
-      <c r="K10" s="137" t="s">
-        <v>364</v>
-      </c>
-      <c r="L10" s="137"/>
+      <c r="J10" s="132" t="s">
+        <v>365</v>
+      </c>
+      <c r="K10" s="138" t="s">
+        <v>366</v>
+      </c>
+      <c r="L10" s="138"/>
       <c r="M10" s="67"/>
       <c r="N10" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O10" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P10" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O10" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P10" s="134" t="str">
         <f>P9</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q10" s="134">
+      <c r="Q10" s="135">
         <f>Q9+1</f>
         <v>7</v>
       </c>
@@ -4032,7 +4041,7 @@
         <v>asignatura08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C11" s="66" t="str">
         <f>C10</f>
@@ -4052,29 +4061,29 @@
       <c r="H11" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I11" s="130" t="str">
+      <c r="I11" s="131" t="str">
         <f>I10</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J11" s="131" t="s">
-        <v>366</v>
-      </c>
-      <c r="K11" s="135" t="s">
-        <v>367</v>
-      </c>
-      <c r="L11" s="135"/>
+      <c r="J11" s="132" t="s">
+        <v>368</v>
+      </c>
+      <c r="K11" s="136" t="s">
+        <v>369</v>
+      </c>
+      <c r="L11" s="136"/>
       <c r="M11" s="67"/>
       <c r="N11" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O11" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P11" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O11" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P11" s="134" t="str">
         <f>P10</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q11" s="134">
+      <c r="Q11" s="135">
         <f>Q10+1</f>
         <v>8</v>
       </c>
@@ -4085,7 +4094,7 @@
         <v>asignatura09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C12" s="66" t="str">
         <f>C11</f>
@@ -4105,29 +4114,29 @@
       <c r="H12" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I12" s="130" t="str">
+      <c r="I12" s="131" t="str">
         <f>I11</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J12" s="131" t="s">
-        <v>369</v>
-      </c>
-      <c r="K12" s="135" t="s">
-        <v>370</v>
-      </c>
-      <c r="L12" s="135"/>
+      <c r="J12" s="132" t="s">
+        <v>371</v>
+      </c>
+      <c r="K12" s="136" t="s">
+        <v>372</v>
+      </c>
+      <c r="L12" s="136"/>
       <c r="M12" s="67"/>
       <c r="N12" s="66" t="s">
-        <v>315</v>
-      </c>
-      <c r="O12" s="133" t="s">
-        <v>349</v>
-      </c>
-      <c r="P12" s="133" t="str">
+        <v>317</v>
+      </c>
+      <c r="O12" s="134" t="s">
+        <v>351</v>
+      </c>
+      <c r="P12" s="134" t="str">
         <f>P11</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q12" s="134">
+      <c r="Q12" s="135">
         <f>Q11+1</f>
         <v>9</v>
       </c>
@@ -4138,7 +4147,7 @@
         <v>asignatura10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C13" s="66" t="str">
         <f>C12</f>
@@ -4158,29 +4167,29 @@
       <c r="H13" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="130" t="str">
+      <c r="I13" s="131" t="str">
         <f>I12</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J13" s="131" t="s">
-        <v>372</v>
-      </c>
-      <c r="K13" s="135" t="s">
-        <v>352</v>
-      </c>
-      <c r="L13" s="135"/>
+      <c r="J13" s="132" t="s">
+        <v>374</v>
+      </c>
+      <c r="K13" s="136" t="s">
+        <v>354</v>
+      </c>
+      <c r="L13" s="136"/>
       <c r="M13" s="67"/>
       <c r="N13" s="66" t="s">
-        <v>315</v>
-      </c>
-      <c r="O13" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P13" s="133" t="str">
+        <v>317</v>
+      </c>
+      <c r="O13" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P13" s="134" t="str">
         <f>P12</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q13" s="134">
+      <c r="Q13" s="135">
         <f>Q12+1</f>
         <v>10</v>
       </c>
@@ -4191,7 +4200,7 @@
         <v>asignatura11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C14" s="66" t="str">
         <f>C13</f>
@@ -4211,29 +4220,29 @@
       <c r="H14" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I14" s="130" t="str">
+      <c r="I14" s="131" t="str">
         <f>I13</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J14" s="131" t="s">
-        <v>374</v>
-      </c>
-      <c r="K14" s="135" t="s">
-        <v>355</v>
-      </c>
-      <c r="L14" s="135"/>
+      <c r="J14" s="132" t="s">
+        <v>376</v>
+      </c>
+      <c r="K14" s="136" t="s">
+        <v>357</v>
+      </c>
+      <c r="L14" s="136"/>
       <c r="M14" s="67"/>
       <c r="N14" s="66" t="s">
-        <v>315</v>
-      </c>
-      <c r="O14" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P14" s="133" t="str">
+        <v>317</v>
+      </c>
+      <c r="O14" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P14" s="134" t="str">
         <f>P13</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q14" s="134">
+      <c r="Q14" s="135">
         <f>Q13+1</f>
         <v>11</v>
       </c>
@@ -4244,7 +4253,7 @@
         <v>asignatura12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C15" s="66" t="str">
         <f>C14</f>
@@ -4264,29 +4273,29 @@
       <c r="H15" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I15" s="130" t="str">
+      <c r="I15" s="131" t="str">
         <f>I14</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J15" s="131" t="s">
-        <v>376</v>
-      </c>
-      <c r="K15" s="138" t="s">
-        <v>377</v>
-      </c>
-      <c r="L15" s="138"/>
+      <c r="J15" s="132" t="s">
+        <v>378</v>
+      </c>
+      <c r="K15" s="139" t="s">
+        <v>379</v>
+      </c>
+      <c r="L15" s="139"/>
       <c r="M15" s="67"/>
       <c r="N15" s="66" t="s">
-        <v>315</v>
-      </c>
-      <c r="O15" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P15" s="133" t="str">
+        <v>317</v>
+      </c>
+      <c r="O15" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P15" s="134" t="str">
         <f>P14</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q15" s="134">
+      <c r="Q15" s="135">
         <f>Q14+1</f>
         <v>12</v>
       </c>
@@ -4297,7 +4306,7 @@
         <v>asignatura13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C16" s="66" t="str">
         <f>C15</f>
@@ -4317,29 +4326,29 @@
       <c r="H16" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I16" s="130" t="str">
+      <c r="I16" s="131" t="str">
         <f>I15</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J16" s="131" t="s">
-        <v>379</v>
-      </c>
-      <c r="K16" s="135" t="s">
-        <v>380</v>
-      </c>
-      <c r="L16" s="135"/>
+      <c r="J16" s="132" t="s">
+        <v>381</v>
+      </c>
+      <c r="K16" s="136" t="s">
+        <v>382</v>
+      </c>
+      <c r="L16" s="136"/>
       <c r="M16" s="67"/>
       <c r="N16" s="66" t="s">
-        <v>315</v>
-      </c>
-      <c r="O16" s="133" t="s">
-        <v>344</v>
-      </c>
-      <c r="P16" s="133" t="str">
+        <v>317</v>
+      </c>
+      <c r="O16" s="134" t="s">
+        <v>346</v>
+      </c>
+      <c r="P16" s="134" t="str">
         <f>P15</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q16" s="134">
+      <c r="Q16" s="135">
         <f>Q15+1</f>
         <v>13</v>
       </c>
@@ -4350,7 +4359,7 @@
         <v>asignatura14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C17" s="66" t="str">
         <f>C16</f>
@@ -4370,29 +4379,29 @@
       <c r="H17" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="I17" s="130" t="str">
+      <c r="I17" s="131" t="str">
         <f>I16</f>
         <v>2ºA|2ºA</v>
       </c>
-      <c r="J17" s="131" t="s">
-        <v>382</v>
-      </c>
-      <c r="K17" s="135" t="s">
-        <v>383</v>
-      </c>
-      <c r="L17" s="135"/>
+      <c r="J17" s="132" t="s">
+        <v>384</v>
+      </c>
+      <c r="K17" s="136" t="s">
+        <v>385</v>
+      </c>
+      <c r="L17" s="136"/>
       <c r="M17" s="67"/>
       <c r="N17" s="66" t="s">
-        <v>314</v>
-      </c>
-      <c r="O17" s="133" t="s">
-        <v>349</v>
-      </c>
-      <c r="P17" s="133" t="str">
+        <v>316</v>
+      </c>
+      <c r="O17" s="134" t="s">
+        <v>351</v>
+      </c>
+      <c r="P17" s="134" t="str">
         <f>P16</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q17" s="134">
+      <c r="Q17" s="135">
         <f>Q16+1</f>
         <v>14</v>
       </c>
@@ -4442,22 +4451,22 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" ht="21.75" customHeight="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="88" t="s">
-        <v>230</v>
+      <c r="B2" s="89" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="85" t="str">
+      <c r="B3" s="86" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
@@ -4466,7 +4475,7 @@
       <c r="A4" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="85" t="str">
+      <c r="B4" s="86" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -4510,13 +4519,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>130</v>
@@ -4525,10 +4534,10 @@
         <v>131</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>73</v>
@@ -4569,39 +4578,39 @@
         <f>PROPER(I1)</f>
         <v>Program</v>
       </c>
-      <c r="J2" s="139" t="str">
+      <c r="J2" s="140" t="str">
         <f>PROPER(J1)</f>
         <v>Subjects</v>
       </c>
     </row>
     <row r="3" ht="34.5" customHeight="1">
-      <c r="A3" s="140" t="s">
-        <v>385</v>
-      </c>
-      <c r="B3" s="141" t="s">
-        <v>386</v>
-      </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="142" t="s">
+      <c r="A3" s="141" t="s">
         <v>387</v>
       </c>
-      <c r="F3" s="144" t="s">
+      <c r="B3" s="142" t="s">
         <v>388</v>
       </c>
-      <c r="G3" s="145" t="s">
+      <c r="C3" s="143"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="143" t="s">
         <v>389</v>
       </c>
-      <c r="H3" s="146" t="str">
+      <c r="F3" s="145" t="s">
+        <v>390</v>
+      </c>
+      <c r="G3" s="146" t="s">
+        <v>391</v>
+      </c>
+      <c r="H3" s="147" t="str">
         <f>users!A4</f>
         <v>teacher01</v>
       </c>
-      <c r="I3" s="147" t="str">
+      <c r="I3" s="148" t="str">
         <f>ap_programs!A5</f>
         <v>programB</v>
       </c>
-      <c r="J3" s="148" t="s">
-        <v>390</v>
+      <c r="J3" s="149" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="4"/>
@@ -4637,946 +4646,946 @@
     <col customWidth="1" min="2" max="2" width="15.8515625"/>
     <col customWidth="1" min="3" max="3" width="10.00390625"/>
     <col bestFit="1" min="4" max="4" width="8.50390625"/>
-    <col bestFit="1" min="5" max="5" style="149" width="17.3515625"/>
+    <col bestFit="1" min="5" max="5" style="150" width="17.3515625"/>
     <col bestFit="1" min="6" max="6" width="11.28125"/>
     <col customWidth="1" min="7" max="7" width="15.57421875"/>
     <col customWidth="1" min="8" max="8" width="69.57421875"/>
-    <col bestFit="1" min="9" max="9" style="150" width="13.8515625"/>
+    <col bestFit="1" min="9" max="9" style="151" width="13.8515625"/>
     <col customWidth="1" min="10" max="10" width="73.140625"/>
-    <col bestFit="1" min="11" max="11" style="150" width="15.2109375"/>
+    <col bestFit="1" min="11" max="11" style="151" width="15.2109375"/>
     <col bestFit="1" min="12" max="12" width="9.921875"/>
     <col customWidth="1" min="13" max="13" width="114.28125"/>
-    <col customWidth="1" min="14" max="14" style="150" width="23.8515625"/>
+    <col customWidth="1" min="14" max="14" style="151" width="23.8515625"/>
     <col bestFit="1" min="15" max="15" width="2.78125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="134" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="134" t="s">
-        <v>242</v>
-      </c>
-      <c r="D1" s="134" t="s">
-        <v>392</v>
-      </c>
-      <c r="E1" s="134" t="s">
+      <c r="B1" s="135" t="s">
         <v>393</v>
       </c>
-      <c r="F1" s="134" t="s">
+      <c r="C1" s="135" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="135" t="s">
         <v>394</v>
       </c>
-      <c r="G1" s="151" t="s">
+      <c r="E1" s="135" t="s">
+        <v>395</v>
+      </c>
+      <c r="F1" s="135" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1" s="152" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="134" t="s">
-        <v>395</v>
-      </c>
-      <c r="I1" s="134" t="s">
-        <v>396</v>
-      </c>
-      <c r="J1" s="134" t="s">
+      <c r="H1" s="135" t="s">
         <v>397</v>
       </c>
-      <c r="K1" s="134" t="s">
+      <c r="I1" s="135" t="s">
         <v>398</v>
       </c>
-      <c r="L1" s="134" t="s">
+      <c r="J1" s="135" t="s">
         <v>399</v>
       </c>
-      <c r="M1" s="134" t="s">
+      <c r="K1" s="135" t="s">
         <v>400</v>
       </c>
-      <c r="N1" s="134" t="s">
+      <c r="L1" s="135" t="s">
         <v>401</v>
       </c>
+      <c r="M1" s="135" t="s">
+        <v>402</v>
+      </c>
+      <c r="N1" s="135" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="2" ht="28.5">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="124" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>402</v>
-      </c>
-      <c r="C2" s="104" t="s">
-        <v>246</v>
-      </c>
-      <c r="D2" s="104" t="s">
-        <v>403</v>
+        <v>404</v>
+      </c>
+      <c r="C2" s="105" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2" s="105" t="s">
+        <v>405</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="G2" s="122" t="s">
+        <v>407</v>
+      </c>
+      <c r="G2" s="123" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="152" t="s">
-        <v>406</v>
+      <c r="H2" s="153" t="s">
+        <v>408</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="J2" s="122" t="s">
-        <v>408</v>
+        <v>409</v>
+      </c>
+      <c r="J2" s="123" t="s">
+        <v>410</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="L2" s="104" t="s">
-        <v>399</v>
-      </c>
-      <c r="M2" s="122" t="s">
-        <v>410</v>
+        <v>411</v>
+      </c>
+      <c r="L2" s="105" t="s">
+        <v>401</v>
+      </c>
+      <c r="M2" s="123" t="s">
+        <v>412</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" ht="114">
-      <c r="A3" s="153" t="str">
+      <c r="A3" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O3&lt;10,"0",""),O3)</f>
         <v>q01</v>
       </c>
-      <c r="B3" s="154" t="str">
+      <c r="B3" s="155" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
-      <c r="C3" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D3" s="149"/>
-      <c r="E3" s="149" t="s">
-        <v>413</v>
-      </c>
-      <c r="F3" s="149" t="s">
+      <c r="C3" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G3" s="155" t="s">
+      <c r="D3" s="150"/>
+      <c r="E3" s="150" t="s">
         <v>415</v>
       </c>
-      <c r="H3" s="156" t="s">
+      <c r="F3" s="150" t="s">
         <v>416</v>
       </c>
-      <c r="I3" s="149"/>
-      <c r="J3" s="156" t="s">
+      <c r="G3" s="156" t="s">
         <v>417</v>
       </c>
-      <c r="K3" s="150"/>
-      <c r="L3" s="149">
+      <c r="H3" s="157" t="s">
+        <v>418</v>
+      </c>
+      <c r="I3" s="150"/>
+      <c r="J3" s="157" t="s">
+        <v>419</v>
+      </c>
+      <c r="K3" s="151"/>
+      <c r="L3" s="150">
         <v>1</v>
       </c>
-      <c r="M3" s="156" t="s">
-        <v>418</v>
-      </c>
-      <c r="N3" s="149"/>
-      <c r="O3" s="157">
+      <c r="M3" s="157" t="s">
+        <v>420</v>
+      </c>
+      <c r="N3" s="150"/>
+      <c r="O3" s="158">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="199.5">
-      <c r="A4" s="153" t="str">
+      <c r="A4" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O4&lt;10,"0",""),O4)</f>
         <v>q02</v>
       </c>
-      <c r="B4" s="146" t="str">
+      <c r="B4" s="147" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
-      <c r="C4" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D4" s="149"/>
-      <c r="E4" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F4" s="149" t="s">
+      <c r="C4" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G4" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H4" s="156" t="s">
+      <c r="D4" s="150"/>
+      <c r="E4" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="I4" s="149"/>
-      <c r="J4" s="156" t="s">
+      <c r="F4" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G4" s="156" t="s">
         <v>422</v>
       </c>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149">
+      <c r="H4" s="157" t="s">
+        <v>423</v>
+      </c>
+      <c r="I4" s="150"/>
+      <c r="J4" s="157" t="s">
+        <v>424</v>
+      </c>
+      <c r="K4" s="150"/>
+      <c r="L4" s="150">
         <v>4</v>
       </c>
-      <c r="M4" s="156" t="s">
-        <v>423</v>
-      </c>
-      <c r="N4" s="149"/>
-      <c r="O4" s="157">
+      <c r="M4" s="157" t="s">
+        <v>425</v>
+      </c>
+      <c r="N4" s="150"/>
+      <c r="O4" s="158">
         <f>O3+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="114">
-      <c r="A5" s="153" t="str">
+      <c r="A5" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O5&lt;10,"0",""),O5)</f>
         <v>q03</v>
       </c>
-      <c r="B5" s="146" t="str">
+      <c r="B5" s="147" t="str">
         <f>B4</f>
         <v>qbank01</v>
       </c>
-      <c r="C5" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F5" s="149" t="s">
+      <c r="C5" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G5" s="155" t="s">
-        <v>424</v>
-      </c>
-      <c r="H5" s="156" t="s">
-        <v>425</v>
-      </c>
-      <c r="I5" s="149"/>
-      <c r="J5" s="156" t="s">
+      <c r="D5" s="150"/>
+      <c r="E5" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F5" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G5" s="156" t="s">
         <v>426</v>
       </c>
-      <c r="K5" s="149"/>
-      <c r="L5" s="149">
+      <c r="H5" s="157" t="s">
+        <v>427</v>
+      </c>
+      <c r="I5" s="150"/>
+      <c r="J5" s="157" t="s">
+        <v>428</v>
+      </c>
+      <c r="K5" s="150"/>
+      <c r="L5" s="150">
         <v>3</v>
       </c>
-      <c r="M5" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="N5" s="149"/>
-      <c r="O5" s="157">
+      <c r="M5" s="157" t="s">
+        <v>429</v>
+      </c>
+      <c r="N5" s="150"/>
+      <c r="O5" s="158">
         <f>O4+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="156.75">
-      <c r="A6" s="153" t="str">
+      <c r="A6" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O6&lt;10,"0",""),O6)</f>
         <v>q04</v>
       </c>
-      <c r="B6" s="146" t="str">
+      <c r="B6" s="147" t="str">
         <f>B5</f>
         <v>qbank01</v>
       </c>
-      <c r="C6" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D6" s="149"/>
-      <c r="E6" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F6" s="149" t="s">
+      <c r="C6" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G6" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H6" s="156" t="s">
-        <v>428</v>
-      </c>
-      <c r="I6" s="149"/>
-      <c r="J6" s="156" t="s">
-        <v>429</v>
-      </c>
-      <c r="K6" s="149"/>
-      <c r="L6" s="149">
+      <c r="D6" s="150"/>
+      <c r="E6" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F6" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G6" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H6" s="157" t="s">
+        <v>430</v>
+      </c>
+      <c r="I6" s="150"/>
+      <c r="J6" s="157" t="s">
+        <v>431</v>
+      </c>
+      <c r="K6" s="150"/>
+      <c r="L6" s="150">
         <v>2</v>
       </c>
-      <c r="M6" s="156" t="s">
-        <v>430</v>
-      </c>
-      <c r="N6" s="149"/>
-      <c r="O6" s="157">
+      <c r="M6" s="157" t="s">
+        <v>432</v>
+      </c>
+      <c r="N6" s="150"/>
+      <c r="O6" s="158">
         <f>O5+1</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="71.25">
-      <c r="A7" s="153" t="str">
+      <c r="A7" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O7&lt;10,"0",""),O7)</f>
         <v>q05</v>
       </c>
-      <c r="B7" s="146" t="str">
+      <c r="B7" s="147" t="str">
         <f>B6</f>
         <v>qbank01</v>
       </c>
-      <c r="C7" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D7" s="149"/>
-      <c r="E7" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F7" s="149" t="s">
+      <c r="C7" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G7" s="155" t="s">
-        <v>431</v>
-      </c>
-      <c r="H7" s="156" t="s">
-        <v>432</v>
-      </c>
-      <c r="I7" s="149"/>
-      <c r="J7" s="156" t="s">
+      <c r="D7" s="150"/>
+      <c r="E7" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F7" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G7" s="156" t="s">
         <v>433</v>
       </c>
-      <c r="K7" s="149"/>
-      <c r="L7" s="149">
+      <c r="H7" s="157" t="s">
+        <v>434</v>
+      </c>
+      <c r="I7" s="150"/>
+      <c r="J7" s="157" t="s">
+        <v>435</v>
+      </c>
+      <c r="K7" s="150"/>
+      <c r="L7" s="150">
         <v>1</v>
       </c>
-      <c r="M7" s="156" t="s">
-        <v>434</v>
-      </c>
-      <c r="N7" s="149"/>
-      <c r="O7" s="157">
+      <c r="M7" s="157" t="s">
+        <v>436</v>
+      </c>
+      <c r="N7" s="150"/>
+      <c r="O7" s="158">
         <f>O6+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="242.25">
-      <c r="A8" s="153" t="str">
+      <c r="A8" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O8&lt;10,"0",""),O8)</f>
         <v>q06</v>
       </c>
-      <c r="B8" s="146" t="str">
+      <c r="B8" s="147" t="str">
         <f>B7</f>
         <v>qbank01</v>
       </c>
-      <c r="C8" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D8" s="149"/>
-      <c r="E8" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F8" s="149" t="s">
+      <c r="C8" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G8" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H8" s="156" t="s">
-        <v>435</v>
-      </c>
-      <c r="I8" s="150"/>
-      <c r="J8" s="156" t="s">
-        <v>436</v>
-      </c>
-      <c r="K8" s="149"/>
-      <c r="L8" s="149">
+      <c r="D8" s="150"/>
+      <c r="E8" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F8" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G8" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H8" s="157" t="s">
+        <v>437</v>
+      </c>
+      <c r="I8" s="151"/>
+      <c r="J8" s="157" t="s">
+        <v>438</v>
+      </c>
+      <c r="K8" s="150"/>
+      <c r="L8" s="150">
         <v>2</v>
       </c>
-      <c r="M8" s="156" t="s">
-        <v>437</v>
-      </c>
-      <c r="N8" s="158"/>
-      <c r="O8" s="157">
+      <c r="M8" s="157" t="s">
+        <v>439</v>
+      </c>
+      <c r="N8" s="159"/>
+      <c r="O8" s="158">
         <f>O7+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="242.25">
-      <c r="A9" s="153" t="str">
+      <c r="A9" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O9&lt;10,"0",""),O9)</f>
         <v>q07</v>
       </c>
-      <c r="B9" s="146" t="str">
+      <c r="B9" s="147" t="str">
         <f>B8</f>
         <v>qbank01</v>
       </c>
-      <c r="C9" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D9" s="149"/>
-      <c r="E9" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F9" s="149" t="s">
+      <c r="C9" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G9" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H9" s="156" t="s">
-        <v>438</v>
-      </c>
-      <c r="I9" s="150"/>
-      <c r="J9" s="156" t="s">
-        <v>439</v>
-      </c>
-      <c r="K9" s="149"/>
-      <c r="L9" s="149">
+      <c r="D9" s="150"/>
+      <c r="E9" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F9" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G9" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H9" s="157" t="s">
+        <v>440</v>
+      </c>
+      <c r="I9" s="151"/>
+      <c r="J9" s="157" t="s">
+        <v>441</v>
+      </c>
+      <c r="K9" s="150"/>
+      <c r="L9" s="150">
         <v>3</v>
       </c>
-      <c r="M9" s="156" t="s">
-        <v>440</v>
-      </c>
-      <c r="N9" s="149"/>
-      <c r="O9" s="157">
+      <c r="M9" s="157" t="s">
+        <v>442</v>
+      </c>
+      <c r="N9" s="150"/>
+      <c r="O9" s="158">
         <f>O8+1</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="356.25">
-      <c r="A10" s="153" t="str">
+      <c r="A10" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O10&lt;10,"0",""),O10)</f>
         <v>q08</v>
       </c>
-      <c r="B10" s="146" t="str">
+      <c r="B10" s="147" t="str">
         <f>B9</f>
         <v>qbank01</v>
       </c>
-      <c r="C10" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D10" s="149"/>
-      <c r="E10" s="149" t="s">
-        <v>413</v>
-      </c>
-      <c r="F10" s="149" t="s">
-        <v>441</v>
-      </c>
-      <c r="G10" s="155" t="s">
-        <v>424</v>
-      </c>
-      <c r="H10" s="156" t="s">
-        <v>442</v>
-      </c>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
-      <c r="K10" s="159" t="s">
+      <c r="C10" s="150" t="s">
+        <v>414</v>
+      </c>
+      <c r="D10" s="150"/>
+      <c r="E10" s="150" t="s">
+        <v>415</v>
+      </c>
+      <c r="F10" s="150" t="s">
         <v>443</v>
       </c>
-      <c r="L10" s="149">
+      <c r="G10" s="156" t="s">
+        <v>426</v>
+      </c>
+      <c r="H10" s="157" t="s">
+        <v>444</v>
+      </c>
+      <c r="I10" s="150"/>
+      <c r="J10" s="150"/>
+      <c r="K10" s="160" t="s">
+        <v>445</v>
+      </c>
+      <c r="L10" s="150">
         <v>2</v>
       </c>
-      <c r="M10" s="156" t="s">
-        <v>444</v>
-      </c>
-      <c r="N10" s="149"/>
-      <c r="O10" s="157">
+      <c r="M10" s="157" t="s">
+        <v>446</v>
+      </c>
+      <c r="N10" s="150"/>
+      <c r="O10" s="158">
         <f>O9+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="11" ht="185.25">
-      <c r="A11" s="153" t="str">
+      <c r="A11" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O11&lt;10,"0",""),O11)</f>
         <v>q09</v>
       </c>
-      <c r="B11" s="146" t="str">
+      <c r="B11" s="147" t="str">
         <f>B10</f>
         <v>qbank01</v>
       </c>
-      <c r="C11" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D11" s="149"/>
-      <c r="E11" s="149" t="s">
-        <v>413</v>
-      </c>
-      <c r="F11" s="149" t="s">
-        <v>441</v>
-      </c>
-      <c r="G11" s="155" t="s">
-        <v>424</v>
-      </c>
-      <c r="H11" s="156" t="s">
-        <v>445</v>
-      </c>
-      <c r="I11" s="159" t="s">
-        <v>446</v>
-      </c>
-      <c r="J11" s="156" t="s">
+      <c r="C11" s="150" t="s">
+        <v>414</v>
+      </c>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150" t="s">
+        <v>415</v>
+      </c>
+      <c r="F11" s="150" t="s">
+        <v>443</v>
+      </c>
+      <c r="G11" s="156" t="s">
+        <v>426</v>
+      </c>
+      <c r="H11" s="157" t="s">
         <v>447</v>
       </c>
-      <c r="K11" s="149"/>
-      <c r="L11" s="149">
+      <c r="I11" s="160" t="s">
+        <v>448</v>
+      </c>
+      <c r="J11" s="157" t="s">
+        <v>449</v>
+      </c>
+      <c r="K11" s="150"/>
+      <c r="L11" s="150">
         <v>1</v>
       </c>
-      <c r="M11" s="156" t="s">
-        <v>448</v>
-      </c>
-      <c r="N11" s="149"/>
-      <c r="O11" s="157">
+      <c r="M11" s="157" t="s">
+        <v>450</v>
+      </c>
+      <c r="N11" s="150"/>
+      <c r="O11" s="158">
         <f>O10+1</f>
         <v>9</v>
       </c>
     </row>
     <row r="12" ht="185.25">
-      <c r="A12" s="153" t="str">
+      <c r="A12" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O12&lt;10,"0",""),O12)</f>
         <v>q10</v>
       </c>
-      <c r="B12" s="146" t="str">
+      <c r="B12" s="147" t="str">
         <f>B11</f>
         <v>qbank01</v>
       </c>
-      <c r="C12" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D12" s="149"/>
-      <c r="E12" s="149" t="s">
-        <v>449</v>
-      </c>
-      <c r="F12" s="149" t="s">
+      <c r="C12" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G12" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H12" s="156" t="s">
-        <v>450</v>
-      </c>
-      <c r="I12" s="149"/>
-      <c r="J12" s="160" t="s">
+      <c r="D12" s="150"/>
+      <c r="E12" s="150" t="s">
         <v>451</v>
       </c>
-      <c r="K12" s="149"/>
-      <c r="L12" s="149">
+      <c r="F12" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G12" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H12" s="157" t="s">
+        <v>452</v>
+      </c>
+      <c r="I12" s="150"/>
+      <c r="J12" s="161" t="s">
+        <v>453</v>
+      </c>
+      <c r="K12" s="150"/>
+      <c r="L12" s="150">
         <v>4</v>
       </c>
-      <c r="M12" s="156" t="s">
-        <v>452</v>
-      </c>
-      <c r="N12" s="149"/>
-      <c r="O12" s="157">
+      <c r="M12" s="157" t="s">
+        <v>454</v>
+      </c>
+      <c r="N12" s="150"/>
+      <c r="O12" s="158">
         <f>O11+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="185.25">
-      <c r="A13" s="153" t="str">
+      <c r="A13" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O13&lt;10,"0",""),O13)</f>
         <v>q11</v>
       </c>
-      <c r="B13" s="146" t="str">
+      <c r="B13" s="147" t="str">
         <f>B12</f>
         <v>qbank01</v>
       </c>
-      <c r="C13" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D13" s="149"/>
-      <c r="E13" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F13" s="149" t="s">
+      <c r="C13" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G13" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H13" s="156" t="s">
-        <v>453</v>
-      </c>
-      <c r="I13" s="149"/>
-      <c r="J13" s="156" t="s">
-        <v>454</v>
-      </c>
-      <c r="K13" s="149"/>
-      <c r="L13" s="149">
+      <c r="D13" s="150"/>
+      <c r="E13" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F13" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G13" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H13" s="157" t="s">
+        <v>455</v>
+      </c>
+      <c r="I13" s="150"/>
+      <c r="J13" s="157" t="s">
+        <v>456</v>
+      </c>
+      <c r="K13" s="150"/>
+      <c r="L13" s="150">
         <v>3</v>
       </c>
-      <c r="M13" s="156" t="s">
-        <v>455</v>
-      </c>
-      <c r="N13" s="149"/>
-      <c r="O13" s="157">
+      <c r="M13" s="157" t="s">
+        <v>457</v>
+      </c>
+      <c r="N13" s="150"/>
+      <c r="O13" s="158">
         <f>O12+1</f>
         <v>11</v>
       </c>
     </row>
     <row r="14" ht="185.25">
-      <c r="A14" s="153" t="str">
+      <c r="A14" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O14&lt;10,"0",""),O14)</f>
         <v>q12</v>
       </c>
-      <c r="B14" s="146" t="str">
+      <c r="B14" s="147" t="str">
         <f>B13</f>
         <v>qbank01</v>
       </c>
-      <c r="C14" s="149" t="s">
-        <v>412</v>
-      </c>
-      <c r="D14" s="149"/>
-      <c r="E14" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F14" s="149" t="s">
+      <c r="C14" s="150" t="s">
         <v>414</v>
       </c>
-      <c r="G14" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H14" s="156" t="s">
-        <v>456</v>
-      </c>
-      <c r="I14" s="149"/>
-      <c r="J14" s="156" t="s">
-        <v>457</v>
-      </c>
-      <c r="K14" s="149"/>
-      <c r="L14" s="149">
+      <c r="D14" s="150"/>
+      <c r="E14" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F14" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G14" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H14" s="157" t="s">
+        <v>458</v>
+      </c>
+      <c r="I14" s="150"/>
+      <c r="J14" s="157" t="s">
+        <v>459</v>
+      </c>
+      <c r="K14" s="150"/>
+      <c r="L14" s="150">
         <v>1</v>
       </c>
-      <c r="M14" s="156" t="s">
-        <v>458</v>
-      </c>
-      <c r="N14" s="149"/>
-      <c r="O14" s="157">
+      <c r="M14" s="157" t="s">
+        <v>460</v>
+      </c>
+      <c r="N14" s="150"/>
+      <c r="O14" s="158">
         <f>O13+1</f>
         <v>12</v>
       </c>
     </row>
     <row r="15" ht="114">
-      <c r="A15" s="153" t="str">
+      <c r="A15" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O15&lt;10,"0",""),O15)</f>
         <v>q13</v>
       </c>
-      <c r="B15" s="146" t="str">
+      <c r="B15" s="147" t="str">
         <f>B14</f>
         <v>qbank01</v>
       </c>
-      <c r="C15" s="149" t="s">
-        <v>412</v>
+      <c r="C15" s="150" t="s">
+        <v>414</v>
       </c>
       <c r="D15" s="18"/>
-      <c r="E15" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F15" s="149" t="s">
-        <v>441</v>
-      </c>
-      <c r="G15" s="155" t="s">
-        <v>459</v>
-      </c>
-      <c r="H15" s="156" t="s">
-        <v>460</v>
-      </c>
-      <c r="I15" s="149" t="s">
+      <c r="E15" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F15" s="150" t="s">
+        <v>443</v>
+      </c>
+      <c r="G15" s="156" t="s">
         <v>461</v>
       </c>
-      <c r="J15" s="156" t="s">
+      <c r="H15" s="157" t="s">
         <v>462</v>
       </c>
-      <c r="K15" s="150"/>
-      <c r="L15" s="149">
+      <c r="I15" s="150" t="s">
+        <v>463</v>
+      </c>
+      <c r="J15" s="157" t="s">
+        <v>464</v>
+      </c>
+      <c r="K15" s="151"/>
+      <c r="L15" s="150">
         <v>2</v>
       </c>
-      <c r="M15" s="156" t="s">
-        <v>463</v>
-      </c>
-      <c r="N15" s="149"/>
-      <c r="O15" s="157">
+      <c r="M15" s="157" t="s">
+        <v>465</v>
+      </c>
+      <c r="N15" s="150"/>
+      <c r="O15" s="158">
         <f>O14+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="16" ht="114">
-      <c r="A16" s="153" t="str">
+      <c r="A16" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O16&lt;10,"0",""),O16)</f>
         <v>q14</v>
       </c>
-      <c r="B16" s="146" t="str">
+      <c r="B16" s="147" t="str">
         <f>B15</f>
         <v>qbank01</v>
       </c>
-      <c r="C16" s="149" t="s">
-        <v>412</v>
+      <c r="C16" s="150" t="s">
+        <v>414</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F16" s="149" t="s">
-        <v>441</v>
-      </c>
-      <c r="G16" s="155" t="s">
-        <v>459</v>
-      </c>
-      <c r="H16" s="156" t="s">
-        <v>464</v>
-      </c>
-      <c r="I16" s="149" t="s">
+      <c r="E16" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F16" s="150" t="s">
+        <v>443</v>
+      </c>
+      <c r="G16" s="156" t="s">
         <v>461</v>
       </c>
-      <c r="J16" s="156" t="s">
-        <v>465</v>
-      </c>
-      <c r="K16" s="150"/>
-      <c r="L16" s="149">
+      <c r="H16" s="157" t="s">
+        <v>466</v>
+      </c>
+      <c r="I16" s="150" t="s">
+        <v>463</v>
+      </c>
+      <c r="J16" s="157" t="s">
+        <v>467</v>
+      </c>
+      <c r="K16" s="151"/>
+      <c r="L16" s="150">
         <v>1</v>
       </c>
-      <c r="M16" s="156" t="s">
-        <v>466</v>
-      </c>
-      <c r="N16" s="158"/>
-      <c r="O16" s="157">
+      <c r="M16" s="157" t="s">
+        <v>468</v>
+      </c>
+      <c r="N16" s="159"/>
+      <c r="O16" s="158">
         <f>O15+1</f>
         <v>14</v>
       </c>
     </row>
     <row r="17" ht="142.5">
-      <c r="A17" s="153" t="str">
+      <c r="A17" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O17&lt;10,"0",""),O17)</f>
         <v>q15</v>
       </c>
-      <c r="B17" s="146" t="str">
+      <c r="B17" s="147" t="str">
         <f>B16</f>
         <v>qbank01</v>
       </c>
-      <c r="C17" s="149" t="s">
-        <v>412</v>
+      <c r="C17" s="150" t="s">
+        <v>414</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F17" s="149" t="s">
-        <v>414</v>
-      </c>
-      <c r="G17" s="155" t="s">
-        <v>467</v>
-      </c>
-      <c r="H17" s="156" t="s">
-        <v>468</v>
-      </c>
-      <c r="I17" s="150"/>
-      <c r="J17" s="156" t="s">
+      <c r="E17" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F17" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G17" s="156" t="s">
         <v>469</v>
       </c>
-      <c r="K17" s="150"/>
-      <c r="L17" s="149">
+      <c r="H17" s="157" t="s">
+        <v>470</v>
+      </c>
+      <c r="I17" s="151"/>
+      <c r="J17" s="157" t="s">
+        <v>471</v>
+      </c>
+      <c r="K17" s="151"/>
+      <c r="L17" s="150">
         <v>2</v>
       </c>
-      <c r="M17" s="156" t="s">
-        <v>470</v>
-      </c>
-      <c r="N17" s="158"/>
-      <c r="O17" s="157">
+      <c r="M17" s="157" t="s">
+        <v>472</v>
+      </c>
+      <c r="N17" s="159"/>
+      <c r="O17" s="158">
         <f>O16+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="242.25">
-      <c r="A18" s="153" t="str">
+      <c r="A18" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O18&lt;10,"0",""),O18)</f>
         <v>q16</v>
       </c>
-      <c r="B18" s="146" t="str">
+      <c r="B18" s="147" t="str">
         <f>B17</f>
         <v>qbank01</v>
       </c>
-      <c r="C18" s="149" t="s">
-        <v>412</v>
+      <c r="C18" s="150" t="s">
+        <v>414</v>
       </c>
       <c r="D18" s="18"/>
-      <c r="E18" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F18" s="149" t="s">
-        <v>414</v>
-      </c>
-      <c r="G18" s="155" t="s">
-        <v>459</v>
-      </c>
-      <c r="H18" s="156" t="s">
-        <v>471</v>
-      </c>
-      <c r="I18" s="150"/>
-      <c r="J18" s="156" t="s">
-        <v>472</v>
-      </c>
-      <c r="K18" s="150"/>
-      <c r="L18" s="149">
+      <c r="E18" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F18" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G18" s="156" t="s">
+        <v>461</v>
+      </c>
+      <c r="H18" s="157" t="s">
+        <v>473</v>
+      </c>
+      <c r="I18" s="151"/>
+      <c r="J18" s="157" t="s">
+        <v>474</v>
+      </c>
+      <c r="K18" s="151"/>
+      <c r="L18" s="150">
         <v>1</v>
       </c>
-      <c r="M18" s="156" t="s">
-        <v>473</v>
-      </c>
-      <c r="N18" s="158"/>
-      <c r="O18" s="157">
+      <c r="M18" s="157" t="s">
+        <v>475</v>
+      </c>
+      <c r="N18" s="159"/>
+      <c r="O18" s="158">
         <f>O17+1</f>
         <v>16</v>
       </c>
     </row>
     <row r="19" ht="213.75">
-      <c r="A19" s="153" t="str">
+      <c r="A19" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O19&lt;10,"0",""),O19)</f>
         <v>q17</v>
       </c>
-      <c r="B19" s="146" t="str">
+      <c r="B19" s="147" t="str">
         <f>B18</f>
         <v>qbank01</v>
       </c>
-      <c r="C19" s="149" t="s">
-        <v>412</v>
+      <c r="C19" s="150" t="s">
+        <v>414</v>
       </c>
       <c r="D19" s="18"/>
-      <c r="E19" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F19" s="149" t="s">
-        <v>414</v>
-      </c>
-      <c r="G19" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H19" s="156" t="s">
-        <v>474</v>
-      </c>
-      <c r="I19" s="150"/>
-      <c r="J19" s="156" t="s">
-        <v>475</v>
-      </c>
-      <c r="K19" s="150"/>
-      <c r="L19" s="149">
+      <c r="E19" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F19" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G19" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H19" s="157" t="s">
+        <v>476</v>
+      </c>
+      <c r="I19" s="151"/>
+      <c r="J19" s="157" t="s">
+        <v>477</v>
+      </c>
+      <c r="K19" s="151"/>
+      <c r="L19" s="150">
         <v>3</v>
       </c>
-      <c r="M19" s="156" t="s">
-        <v>476</v>
-      </c>
-      <c r="N19" s="158"/>
-      <c r="O19" s="157">
+      <c r="M19" s="157" t="s">
+        <v>478</v>
+      </c>
+      <c r="N19" s="159"/>
+      <c r="O19" s="158">
         <f>O18+1</f>
         <v>17</v>
       </c>
     </row>
     <row r="20" ht="242.25">
-      <c r="A20" s="153" t="str">
+      <c r="A20" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O20&lt;10,"0",""),O20)</f>
         <v>q18</v>
       </c>
-      <c r="B20" s="146" t="str">
+      <c r="B20" s="147" t="str">
         <f>B19</f>
         <v>qbank01</v>
       </c>
-      <c r="C20" s="149" t="s">
-        <v>412</v>
+      <c r="C20" s="150" t="s">
+        <v>414</v>
       </c>
       <c r="D20" s="18"/>
-      <c r="E20" s="149" t="s">
-        <v>419</v>
-      </c>
-      <c r="F20" s="149" t="s">
-        <v>414</v>
-      </c>
-      <c r="G20" s="155" t="s">
-        <v>420</v>
-      </c>
-      <c r="H20" s="156" t="s">
-        <v>477</v>
-      </c>
-      <c r="I20" s="150"/>
-      <c r="J20" s="156" t="s">
-        <v>478</v>
-      </c>
-      <c r="K20" s="150"/>
-      <c r="L20" s="149">
+      <c r="E20" s="150" t="s">
+        <v>421</v>
+      </c>
+      <c r="F20" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G20" s="156" t="s">
+        <v>422</v>
+      </c>
+      <c r="H20" s="157" t="s">
+        <v>479</v>
+      </c>
+      <c r="I20" s="151"/>
+      <c r="J20" s="157" t="s">
+        <v>480</v>
+      </c>
+      <c r="K20" s="151"/>
+      <c r="L20" s="150">
         <v>4</v>
       </c>
-      <c r="M20" s="156" t="s">
-        <v>479</v>
-      </c>
-      <c r="N20" s="158"/>
-      <c r="O20" s="157">
+      <c r="M20" s="157" t="s">
+        <v>481</v>
+      </c>
+      <c r="N20" s="159"/>
+      <c r="O20" s="158">
         <f>O19+1</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" ht="409.5">
-      <c r="A21" s="153" t="str">
+      <c r="A21" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O21&lt;10,"0",""),O21)</f>
         <v>q19</v>
       </c>
-      <c r="B21" s="146" t="str">
+      <c r="B21" s="147" t="str">
         <f>B20</f>
         <v>qbank01</v>
       </c>
-      <c r="C21" s="149" t="s">
-        <v>412</v>
+      <c r="C21" s="150" t="s">
+        <v>414</v>
       </c>
       <c r="D21" s="18"/>
-      <c r="E21" s="149" t="s">
-        <v>449</v>
-      </c>
-      <c r="F21" s="149" t="s">
-        <v>414</v>
-      </c>
-      <c r="G21" s="155" t="s">
-        <v>467</v>
-      </c>
-      <c r="H21" s="156" t="s">
-        <v>480</v>
-      </c>
-      <c r="I21" s="149"/>
-      <c r="J21" s="156" t="s">
-        <v>481</v>
-      </c>
-      <c r="K21" s="149"/>
-      <c r="L21" s="149">
+      <c r="E21" s="150" t="s">
+        <v>451</v>
+      </c>
+      <c r="F21" s="150" t="s">
+        <v>416</v>
+      </c>
+      <c r="G21" s="156" t="s">
+        <v>469</v>
+      </c>
+      <c r="H21" s="157" t="s">
+        <v>482</v>
+      </c>
+      <c r="I21" s="150"/>
+      <c r="J21" s="157" t="s">
+        <v>483</v>
+      </c>
+      <c r="K21" s="150"/>
+      <c r="L21" s="150">
         <v>4</v>
       </c>
-      <c r="M21" s="156" t="s">
-        <v>482</v>
-      </c>
-      <c r="N21" s="149"/>
-      <c r="O21" s="157">
+      <c r="M21" s="157" t="s">
+        <v>484</v>
+      </c>
+      <c r="N21" s="150"/>
+      <c r="O21" s="158">
         <f>O20+1</f>
         <v>19</v>
       </c>
     </row>
     <row r="22" ht="114">
-      <c r="A22" s="153" t="str">
+      <c r="A22" s="154" t="str">
         <f>_xlfn.CONCAT("q",IF(O22&lt;10,"0",""),O22)</f>
         <v>q20</v>
       </c>
-      <c r="B22" s="146" t="str">
+      <c r="B22" s="147" t="str">
         <f>B21</f>
         <v>qbank01</v>
       </c>
-      <c r="C22" s="149" t="s">
-        <v>483</v>
+      <c r="C22" s="150" t="s">
+        <v>485</v>
       </c>
       <c r="D22" s="18"/>
-      <c r="E22" s="149" t="s">
-        <v>413</v>
+      <c r="E22" s="150" t="s">
+        <v>415</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="160" t="s">
-        <v>431</v>
-      </c>
-      <c r="H22" s="156" t="s">
-        <v>484</v>
-      </c>
-      <c r="I22" s="159" t="s">
-        <v>485</v>
-      </c>
-      <c r="J22" s="156" t="s">
+      <c r="G22" s="161" t="s">
+        <v>433</v>
+      </c>
+      <c r="H22" s="157" t="s">
         <v>486</v>
       </c>
-      <c r="K22" s="150"/>
-      <c r="L22" s="161"/>
-      <c r="M22" s="162"/>
+      <c r="I22" s="160" t="s">
+        <v>487</v>
+      </c>
+      <c r="J22" s="157" t="s">
+        <v>488</v>
+      </c>
+      <c r="K22" s="151"/>
+      <c r="L22" s="162"/>
+      <c r="M22" s="163"/>
       <c r="N22" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="O22" s="163">
+        <v>489</v>
+      </c>
+      <c r="O22" s="164">
         <f>O21+1</f>
         <v>20</v>
       </c>
@@ -5660,7 +5669,7 @@
       <c r="A4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -6678,10 +6687,10 @@
         <v>139</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>140</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>12</v>
@@ -6698,23 +6707,25 @@
       <c r="H3" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="67"/>
+      <c r="I3" s="67" t="s">
+        <v>143</v>
+      </c>
       <c r="J3" s="67" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K3" s="76" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>12</v>
@@ -6723,7 +6734,7 @@
         <v>27670</v>
       </c>
       <c r="F4" s="75" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>142</v>
@@ -6732,23 +6743,25 @@
         <f>H3</f>
         <v>es</v>
       </c>
-      <c r="I4" s="67"/>
+      <c r="I4" s="77" t="s">
+        <v>150</v>
+      </c>
       <c r="J4" s="70" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K4" s="76" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
@@ -6756,8 +6769,8 @@
       <c r="E5" s="74">
         <v>27518</v>
       </c>
-      <c r="F5" s="77" t="s">
-        <v>153</v>
+      <c r="F5" s="78" t="s">
+        <v>155</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>142</v>
@@ -6767,58 +6780,58 @@
         <v>es</v>
       </c>
       <c r="I5" s="67" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J5" s="70" t="s">
-        <v>155</v>
-      </c>
-      <c r="K5" s="78" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="79">
+      <c r="E6" s="80">
         <v>34447</v>
       </c>
-      <c r="F6" s="80" t="s">
-        <v>160</v>
+      <c r="F6" s="81" t="s">
+        <v>162</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="H6" s="81" t="str">
+      <c r="H6" s="82" t="str">
         <f>H5</f>
         <v>es</v>
       </c>
-      <c r="I6" s="82"/>
-      <c r="J6" s="81" t="s">
-        <v>155</v>
+      <c r="I6" s="83"/>
+      <c r="J6" s="82" t="s">
+        <v>157</v>
       </c>
       <c r="K6" s="76" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
@@ -6827,7 +6840,7 @@
         <v>27791</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>142</v>
@@ -6836,24 +6849,24 @@
         <v>34</v>
       </c>
       <c r="I7" s="67" t="s">
-        <v>166</v>
-      </c>
-      <c r="J7" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="K7" s="78" t="s">
         <v>168</v>
+      </c>
+      <c r="J7" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="79" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>12</v>
@@ -6861,8 +6874,8 @@
       <c r="E8" s="74">
         <v>39571</v>
       </c>
-      <c r="F8" s="77" t="s">
-        <v>172</v>
+      <c r="F8" s="78" t="s">
+        <v>174</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>142</v>
@@ -6872,24 +6885,24 @@
         <v>es</v>
       </c>
       <c r="I8" s="67" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J8" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="K8" s="78" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="K8" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
@@ -6898,7 +6911,7 @@
         <v>39572</v>
       </c>
       <c r="F9" s="75" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>142</v>
@@ -6908,25 +6921,25 @@
         <v>es</v>
       </c>
       <c r="I9" s="67" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J9" s="67" t="str">
         <f>J8</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K9" s="78" t="s">
-        <v>175</v>
+      <c r="K9" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>13</v>
@@ -6935,7 +6948,7 @@
         <v>39573</v>
       </c>
       <c r="F10" s="75" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>142</v>
@@ -6945,25 +6958,25 @@
         <v>es</v>
       </c>
       <c r="I10" s="67" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="J10" s="67" t="str">
         <f>J9</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K10" s="78" t="s">
-        <v>175</v>
+      <c r="K10" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="11" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>12</v>
@@ -6972,7 +6985,7 @@
         <v>39208</v>
       </c>
       <c r="F11" s="75" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>142</v>
@@ -6982,25 +6995,25 @@
         <v>es</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J11" s="67" t="str">
         <f>J10</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K11" s="78" t="s">
-        <v>175</v>
+      <c r="K11" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="12" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>13</v>
@@ -7008,8 +7021,8 @@
       <c r="E12" s="74">
         <v>39575</v>
       </c>
-      <c r="F12" s="77" t="s">
-        <v>194</v>
+      <c r="F12" s="78" t="s">
+        <v>196</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>142</v>
@@ -7019,25 +7032,25 @@
         <v>es</v>
       </c>
       <c r="I12" s="67" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J12" s="67" t="str">
         <f>J11</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K12" s="78" t="s">
-        <v>175</v>
+      <c r="K12" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>13</v>
@@ -7045,8 +7058,8 @@
       <c r="E13" s="74">
         <v>39576</v>
       </c>
-      <c r="F13" s="77" t="s">
-        <v>199</v>
+      <c r="F13" s="78" t="s">
+        <v>201</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>142</v>
@@ -7056,25 +7069,25 @@
         <v>es</v>
       </c>
       <c r="I13" s="67" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J13" s="67" t="str">
         <f>J12</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K13" s="78" t="s">
-        <v>175</v>
+      <c r="K13" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>12</v>
@@ -7082,8 +7095,8 @@
       <c r="E14" s="74">
         <v>39577</v>
       </c>
-      <c r="F14" s="77" t="s">
-        <v>204</v>
+      <c r="F14" s="78" t="s">
+        <v>206</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>142</v>
@@ -7093,25 +7106,25 @@
         <v>es</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="J14" s="67" t="str">
         <f>J13</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K14" s="78" t="s">
-        <v>175</v>
+      <c r="K14" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="15" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>13</v>
@@ -7119,8 +7132,8 @@
       <c r="E15" s="74">
         <v>39578</v>
       </c>
-      <c r="F15" s="77" t="s">
-        <v>209</v>
+      <c r="F15" s="78" t="s">
+        <v>211</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>142</v>
@@ -7130,25 +7143,25 @@
         <v>es</v>
       </c>
       <c r="I15" s="67" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J15" s="67" t="str">
         <f>J14</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K15" s="78" t="s">
-        <v>175</v>
+      <c r="K15" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="16" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>12</v>
@@ -7156,8 +7169,8 @@
       <c r="E16" s="74">
         <v>39579</v>
       </c>
-      <c r="F16" s="77" t="s">
-        <v>214</v>
+      <c r="F16" s="78" t="s">
+        <v>216</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>142</v>
@@ -7167,25 +7180,25 @@
         <v>es</v>
       </c>
       <c r="I16" s="67" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J16" s="67" t="str">
         <f>J15</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K16" s="78" t="s">
-        <v>175</v>
+      <c r="K16" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="17" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>12</v>
@@ -7193,8 +7206,8 @@
       <c r="E17" s="74">
         <v>39580</v>
       </c>
-      <c r="F17" s="77" t="s">
-        <v>219</v>
+      <c r="F17" s="78" t="s">
+        <v>221</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>142</v>
@@ -7204,119 +7217,119 @@
         <v>es</v>
       </c>
       <c r="I17" s="67" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="J17" s="67" t="str">
         <f>J16</f>
         <v>Estudiante,Test</v>
       </c>
-      <c r="K17" s="78" t="s">
-        <v>175</v>
+      <c r="K17" s="79" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="13" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="79">
+      <c r="E18" s="80">
         <v>39575</v>
       </c>
-      <c r="F18" s="83" t="s">
-        <v>223</v>
+      <c r="F18" s="84" t="s">
+        <v>225</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="H18" s="81" t="str">
+      <c r="H18" s="82" t="str">
         <f>H17</f>
         <v>es</v>
       </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82" t="str">
+      <c r="I18" s="83"/>
+      <c r="J18" s="83" t="str">
         <f>J17</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K18" s="76" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="79">
+      <c r="E19" s="80">
         <v>39576</v>
       </c>
-      <c r="F19" s="83" t="s">
-        <v>226</v>
+      <c r="F19" s="84" t="s">
+        <v>228</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="H19" s="81" t="str">
+      <c r="H19" s="82" t="str">
         <f>H18</f>
         <v>es</v>
       </c>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82" t="str">
+      <c r="I19" s="83"/>
+      <c r="J19" s="83" t="str">
         <f>J18</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K19" s="76" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="13" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="80">
         <v>39577</v>
       </c>
-      <c r="F20" s="83" t="s">
-        <v>228</v>
+      <c r="F20" s="84" t="s">
+        <v>230</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="H20" s="81" t="str">
+      <c r="H20" s="82" t="str">
         <f>H19</f>
         <v>es</v>
       </c>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82" t="str">
+      <c r="I20" s="83"/>
+      <c r="J20" s="83" t="str">
         <f>J19</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K20" s="76" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" ht="14.25"/>
@@ -7324,32 +7337,33 @@
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F3"/>
     <hyperlink r:id="rId2" ref="F4"/>
-    <hyperlink r:id="rId3" ref="F5"/>
-    <hyperlink r:id="rId4" ref="K5"/>
+    <hyperlink r:id="rId3" ref="I4"/>
+    <hyperlink r:id="rId4" ref="F5"/>
+    <hyperlink r:id="rId5" ref="K5"/>
     <hyperlink r:id="rId2" ref="F6"/>
-    <hyperlink r:id="rId5" ref="F7"/>
-    <hyperlink r:id="rId6" ref="K7"/>
-    <hyperlink r:id="rId7" ref="F8"/>
-    <hyperlink r:id="rId8" ref="K8"/>
-    <hyperlink r:id="rId8" ref="K9"/>
-    <hyperlink r:id="rId9" ref="F10"/>
-    <hyperlink r:id="rId8" ref="K10"/>
-    <hyperlink r:id="rId8" ref="K11"/>
-    <hyperlink r:id="rId10" ref="F12"/>
-    <hyperlink r:id="rId8" ref="K12"/>
-    <hyperlink r:id="rId11" ref="F13"/>
-    <hyperlink r:id="rId8" ref="K13"/>
-    <hyperlink r:id="rId12" ref="F14"/>
-    <hyperlink r:id="rId8" ref="K14"/>
-    <hyperlink r:id="rId13" ref="F15"/>
-    <hyperlink r:id="rId8" ref="K15"/>
-    <hyperlink r:id="rId14" ref="F16"/>
-    <hyperlink r:id="rId8" ref="K16"/>
-    <hyperlink r:id="rId15" ref="F17"/>
-    <hyperlink r:id="rId8" ref="K17"/>
-    <hyperlink r:id="rId10" ref="F18"/>
-    <hyperlink r:id="rId11" ref="F19"/>
-    <hyperlink r:id="rId12" ref="F20"/>
+    <hyperlink r:id="rId6" ref="F7"/>
+    <hyperlink r:id="rId7" ref="K7"/>
+    <hyperlink r:id="rId8" ref="F8"/>
+    <hyperlink r:id="rId9" ref="K8"/>
+    <hyperlink r:id="rId9" ref="K9"/>
+    <hyperlink r:id="rId10" ref="F10"/>
+    <hyperlink r:id="rId9" ref="K10"/>
+    <hyperlink r:id="rId9" ref="K11"/>
+    <hyperlink r:id="rId11" ref="F12"/>
+    <hyperlink r:id="rId9" ref="K12"/>
+    <hyperlink r:id="rId12" ref="F13"/>
+    <hyperlink r:id="rId9" ref="K13"/>
+    <hyperlink r:id="rId13" ref="F14"/>
+    <hyperlink r:id="rId9" ref="K14"/>
+    <hyperlink r:id="rId14" ref="F15"/>
+    <hyperlink r:id="rId9" ref="K15"/>
+    <hyperlink r:id="rId15" ref="F16"/>
+    <hyperlink r:id="rId9" ref="K16"/>
+    <hyperlink r:id="rId16" ref="F17"/>
+    <hyperlink r:id="rId9" ref="K17"/>
+    <hyperlink r:id="rId11" ref="F18"/>
+    <hyperlink r:id="rId12" ref="F19"/>
+    <hyperlink r:id="rId13" ref="F20"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -7358,37 +7372,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0009007D-0029-4B26-BD68-00D700B80028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D30096-001B-443B-9B86-0023003C0073}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0043001B-0046-4020-A628-00DA007B0055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AC00C4-0040-42E1-A565-00DF00E600FC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00200016-0038-4BC7-9B63-0029000F0020}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0098005F-002E-4EDD-BDB5-00E3001700DB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A100FB-00E7-4B3C-96B4-004A00E8005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0025005D-0089-4204-ABF3-00D700F3003C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002400AB-0074-445A-8B6B-00C300C700E0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00340095-002A-41FE-97CE-00E300640053}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00100063-00A0-4E3B-9DFB-00C4001600A6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E60057-0099-49CE-8C14-0098004F00D7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -7423,22 +7437,22 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="84" t="s">
-        <v>230</v>
+      <c r="B2" s="85" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="85" t="str">
+      <c r="B3" s="86" t="str">
         <f>profiles!$A$10</f>
         <v>guardian</v>
       </c>
@@ -7447,7 +7461,7 @@
       <c r="A4" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="85" t="str">
+      <c r="B4" s="86" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -7488,47 +7502,47 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" ht="24.25" customHeight="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="88" t="s">
-        <v>234</v>
-      </c>
-      <c r="D2" s="84" t="s">
-        <v>235</v>
+      <c r="C2" s="89" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="85" t="s">
+        <v>237</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>239</v>
-      </c>
-      <c r="D3" s="89" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="85" t="s">
-        <v>240</v>
+      <c r="E3" s="86" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -7539,7 +7553,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00F5008B-00D2-4541-818D-007C00DF00D0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A2008E-0036-439F-B565-00310010001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -7579,52 +7593,52 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" ht="24.75" customHeight="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="90" t="s">
-        <v>246</v>
-      </c>
-      <c r="E2" s="90" t="s">
-        <v>247</v>
-      </c>
-      <c r="F2" s="90" t="s">
+      <c r="D2" s="91" t="s">
         <v>248</v>
       </c>
-      <c r="G2" s="90" t="s">
+      <c r="E2" s="91" t="s">
         <v>249</v>
+      </c>
+      <c r="F2" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" s="91" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="3" ht="146.25" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="85" t="str">
+        <v>253</v>
+      </c>
+      <c r="C3" s="86" t="str">
         <f>centers!$A$3</f>
         <v>centerA</v>
       </c>
@@ -7634,8 +7648,8 @@
       <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="92" t="s">
-        <v>252</v>
+      <c r="F3" s="93" t="s">
+        <v>254</v>
       </c>
       <c r="G3" s="67">
         <v>5</v>
@@ -7643,12 +7657,12 @@
     </row>
     <row r="4" s="18" customFormat="1" ht="146.25" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="C4" s="85" t="str">
+        <v>256</v>
+      </c>
+      <c r="C4" s="86" t="str">
         <f>centers!$A$4</f>
         <v>centerB</v>
       </c>
@@ -7658,8 +7672,8 @@
       <c r="E4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="92" t="s">
-        <v>252</v>
+      <c r="F4" s="93" t="s">
+        <v>254</v>
       </c>
       <c r="G4" s="67">
         <v>5</v>
@@ -7673,13 +7687,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00C60015-00E0-429F-B02C-003300CF00EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00310097-000A-41C6-9CBB-0052007A0073}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005C008C-00DE-4AA0-A1FC-00F400E4009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D6009D-0073-4218-830C-008100A00036}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7713,22 +7727,22 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="88" t="s">
-        <v>230</v>
+      <c r="B2" s="89" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="85" t="str">
+      <c r="B3" s="86" t="str">
         <f>profiles!$A$8</f>
         <v>teacher</v>
       </c>
@@ -7737,7 +7751,7 @@
       <c r="A4" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="85" t="str">
+      <c r="B4" s="86" t="str">
         <f>profiles!$A$9</f>
         <v>student</v>
       </c>
@@ -7794,73 +7808,73 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
@@ -7881,124 +7895,124 @@
     </row>
     <row r="2" s="9" customFormat="1" ht="23.5" customHeight="1">
       <c r="C2" s="9"/>
-      <c r="G2" s="93" t="s">
-        <v>277</v>
-      </c>
-      <c r="H2" s="93"/>
-      <c r="I2" s="94" t="s">
-        <v>278</v>
-      </c>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="97" t="s">
+      <c r="G2" s="94" t="s">
         <v>279</v>
       </c>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="98" t="s">
+      <c r="H2" s="94"/>
+      <c r="I2" s="95" t="s">
         <v>280</v>
       </c>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="100"/>
-      <c r="W2" s="101" t="s">
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="98" t="s">
         <v>281</v>
       </c>
-      <c r="X2" s="102"/>
-      <c r="Y2" s="102"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="99" t="s">
+        <v>282</v>
+      </c>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
+      <c r="V2" s="101"/>
+      <c r="W2" s="102" t="s">
+        <v>283</v>
+      </c>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
     </row>
     <row r="3" ht="34" customHeight="1">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="90" t="s">
-        <v>282</v>
-      </c>
-      <c r="D3" s="105" t="s">
-        <v>283</v>
-      </c>
-      <c r="E3" s="105" t="s">
+      <c r="C3" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="106" t="s">
+        <v>285</v>
+      </c>
+      <c r="E3" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="106" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" s="107" t="s">
-        <v>285</v>
-      </c>
-      <c r="H3" s="108" t="s">
+      <c r="F3" s="107" t="s">
         <v>286</v>
       </c>
-      <c r="I3" s="109" t="s">
+      <c r="G3" s="108" t="s">
         <v>287</v>
       </c>
-      <c r="J3" s="110" t="s">
+      <c r="H3" s="109" t="s">
         <v>288</v>
       </c>
-      <c r="K3" s="111" t="s">
+      <c r="I3" s="110" t="s">
         <v>289</v>
       </c>
-      <c r="L3" s="111" t="s">
+      <c r="J3" s="111" t="s">
         <v>290</v>
       </c>
-      <c r="M3" s="111" t="s">
+      <c r="K3" s="112" t="s">
         <v>291</v>
       </c>
-      <c r="N3" s="111" t="s">
+      <c r="L3" s="112" t="s">
         <v>292</v>
       </c>
-      <c r="O3" s="111" t="s">
+      <c r="M3" s="112" t="s">
         <v>293</v>
       </c>
-      <c r="P3" s="112" t="s">
+      <c r="N3" s="112" t="s">
         <v>294</v>
       </c>
-      <c r="Q3" s="113" t="s">
-        <v>292</v>
-      </c>
-      <c r="R3" s="114" t="s">
-        <v>293</v>
-      </c>
-      <c r="S3" s="115" t="s">
+      <c r="O3" s="112" t="s">
         <v>295</v>
       </c>
-      <c r="T3" s="116" t="s">
+      <c r="P3" s="113" t="s">
         <v>296</v>
       </c>
-      <c r="U3" s="116" t="s">
-        <v>292</v>
-      </c>
-      <c r="V3" s="116" t="s">
-        <v>293</v>
-      </c>
-      <c r="W3" s="117" t="s">
-        <v>292</v>
-      </c>
-      <c r="X3" s="118" t="s">
+      <c r="Q3" s="114" t="s">
+        <v>294</v>
+      </c>
+      <c r="R3" s="115" t="s">
+        <v>295</v>
+      </c>
+      <c r="S3" s="116" t="s">
         <v>297</v>
       </c>
-      <c r="Y3" s="119" t="s">
+      <c r="T3" s="117" t="s">
         <v>298</v>
+      </c>
+      <c r="U3" s="117" t="s">
+        <v>294</v>
+      </c>
+      <c r="V3" s="117" t="s">
+        <v>295</v>
+      </c>
+      <c r="W3" s="118" t="s">
+        <v>294</v>
+      </c>
+      <c r="X3" s="119" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y3" s="120" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="D4" s="120" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="121" t="s">
         <v>139</v>
       </c>
       <c r="E4" s="66" t="str">
@@ -8022,7 +8036,7 @@
       <c r="K4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="92"/>
+      <c r="L4" s="93"/>
       <c r="M4" s="67"/>
       <c r="N4" s="67"/>
       <c r="O4" s="67"/>
@@ -8057,15 +8071,15 @@
     </row>
     <row r="5" s="9" customFormat="1" ht="46.5" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="D5" s="120" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="121" t="s">
         <v>139</v>
       </c>
       <c r="E5" s="66" t="str">
@@ -8089,8 +8103,8 @@
       <c r="K5" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="121" t="s">
-        <v>304</v>
+      <c r="L5" s="122" t="s">
+        <v>306</v>
       </c>
       <c r="M5" s="67" t="s">
         <v>4</v>
@@ -8146,13 +8160,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{001000A5-00D9-452B-A7AA-004E000F0011}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006F00D1-00B0-462C-A4DA-004300B50007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002E00FE-0047-4FE8-B848-00D9009A00DA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D600D1-00D1-4296-B743-0042004F0066}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPDATED: Added  "autocomplete" to every form in plugins
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="495">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -198,6 +198,9 @@
     <t>plugins.tests</t>
   </si>
   <si>
+    <t>plugins.assignables</t>
+  </si>
+  <si>
     <t>Users</t>
   </si>
   <si>
@@ -231,6 +234,9 @@
     <t>Tests</t>
   </si>
   <si>
+    <t>Activities</t>
+  </si>
+  <si>
     <t>users</t>
   </si>
   <si>
@@ -309,6 +315,15 @@
     <t>questionsBanks</t>
   </si>
   <si>
+    <t>activities</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
     <t xml:space="preserve">Can access to</t>
   </si>
   <si>
@@ -375,6 +390,9 @@
     <t xml:space="preserve">Profile for platform administrators</t>
   </si>
   <si>
+    <t>view</t>
+  </si>
+  <si>
     <t>teacher</t>
   </si>
   <si>
@@ -382,9 +400,6 @@
   </si>
   <si>
     <t xml:space="preserve">Profile for teachers</t>
-  </si>
-  <si>
-    <t>view</t>
   </si>
   <si>
     <t>create</t>
@@ -3319,13 +3334,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -3336,21 +3351,21 @@
         <v>28</v>
       </c>
       <c r="C2" s="106" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D2" s="123" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="E2" s="123" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C3" s="86" t="str">
         <f>ap_programs!$A$4</f>
@@ -3365,10 +3380,10 @@
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C4" s="86" t="str">
         <f>ap_programs!$A$4</f>
@@ -3383,10 +3398,10 @@
     </row>
     <row r="5" ht="19.5" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C5" s="86" t="str">
         <f>ap_programs!$A$5</f>
@@ -3401,10 +3416,10 @@
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C6" s="86" t="str">
         <f>ap_programs!$A$5</f>
@@ -3425,7 +3440,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00BC0093-00C2-449A-9573-008000CB00C2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002E0064-0004-4F26-AAD2-001F00D70022}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -3465,19 +3480,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -3488,19 +3503,19 @@
         <v>28</v>
       </c>
       <c r="C2" s="91" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D2" s="91" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="F2" s="92" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="G2" s="125" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" ht="14.25"/>
@@ -3549,46 +3564,46 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>319</v>
-      </c>
       <c r="M1" s="5" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="O1" s="126" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="P1" s="126" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="Q1" s="18"/>
     </row>
@@ -3602,7 +3617,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="1" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -3621,46 +3636,46 @@
         <v>28</v>
       </c>
       <c r="C3" s="107" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D3" s="105" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="E3" s="91" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="F3" s="105" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="G3" s="105" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="H3" s="127" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="I3" s="128" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="J3" s="128" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="K3" s="128" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="L3" s="128" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="M3" s="128" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="N3" s="127" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="O3" s="92" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="P3" s="92" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="Q3" s="129"/>
     </row>
@@ -3670,7 +3685,7 @@
         <v>asignatura01</v>
       </c>
       <c r="B4" s="130" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C4" s="66" t="str">
         <f>ap_programs!A5</f>
@@ -3688,27 +3703,27 @@
         <v>001</v>
       </c>
       <c r="H4" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I4" s="131" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="J4" s="132" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="K4" s="133" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="L4" s="133"/>
       <c r="M4" s="67"/>
       <c r="N4" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O4" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P4" s="134" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="Q4" s="135">
         <v>1</v>
@@ -3720,7 +3735,7 @@
         <v>asignatura02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="C5" s="66" t="str">
         <f>C4</f>
@@ -3738,25 +3753,25 @@
         <v>002</v>
       </c>
       <c r="H5" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I5" s="131" t="str">
         <f>I4</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J5" s="132" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="K5" s="136" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="L5" s="136"/>
       <c r="M5" s="67"/>
       <c r="N5" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O5" s="134" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="P5" s="134" t="str">
         <f>P4</f>
@@ -3774,7 +3789,7 @@
         <v>asignatura03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="C6" s="66" t="str">
         <f>C5</f>
@@ -3792,25 +3807,25 @@
         <v>003</v>
       </c>
       <c r="H6" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I6" s="131" t="str">
         <f>I5</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J6" s="132" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="K6" s="136" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="L6" s="136"/>
       <c r="M6" s="67"/>
       <c r="N6" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O6" s="134" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="P6" s="134" t="str">
         <f>P5</f>
@@ -3828,7 +3843,7 @@
         <v>asignatura04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="C7" s="66" t="str">
         <f>C6</f>
@@ -3846,25 +3861,25 @@
         <v>004</v>
       </c>
       <c r="H7" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I7" s="131" t="str">
         <f>I6</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J7" s="132" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="K7" s="136" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="L7" s="136"/>
       <c r="M7" s="67"/>
       <c r="N7" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O7" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P7" s="134" t="str">
         <f>P6</f>
@@ -3882,7 +3897,7 @@
         <v>asignatura05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="C8" s="66" t="str">
         <f>C7</f>
@@ -3900,25 +3915,25 @@
         <v>005</v>
       </c>
       <c r="H8" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I8" s="131" t="str">
         <f>I7</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J8" s="132" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="K8" s="136" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="L8" s="136"/>
       <c r="M8" s="67"/>
       <c r="N8" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O8" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P8" s="134" t="str">
         <f>P7</f>
@@ -3935,7 +3950,7 @@
         <v>asignatura06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="C9" s="66" t="str">
         <f>C8</f>
@@ -3953,25 +3968,25 @@
         <v>006</v>
       </c>
       <c r="H9" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I9" s="131" t="str">
         <f>I8</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J9" s="132" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="K9" s="137" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="L9" s="137"/>
       <c r="M9" s="67"/>
       <c r="N9" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O9" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P9" s="134" t="str">
         <f>P8</f>
@@ -3988,7 +4003,7 @@
         <v>asignatura07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="C10" s="66" t="str">
         <f>C9</f>
@@ -4006,25 +4021,25 @@
         <v>007</v>
       </c>
       <c r="H10" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I10" s="131" t="str">
         <f>I9</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J10" s="132" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="K10" s="138" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="L10" s="138"/>
       <c r="M10" s="67"/>
       <c r="N10" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O10" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P10" s="134" t="str">
         <f>P9</f>
@@ -4041,7 +4056,7 @@
         <v>asignatura08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="C11" s="66" t="str">
         <f>C10</f>
@@ -4059,25 +4074,25 @@
         <v>008</v>
       </c>
       <c r="H11" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I11" s="131" t="str">
         <f>I10</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J11" s="132" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="K11" s="136" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="L11" s="136"/>
       <c r="M11" s="67"/>
       <c r="N11" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O11" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P11" s="134" t="str">
         <f>P10</f>
@@ -4094,7 +4109,7 @@
         <v>asignatura09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="C12" s="66" t="str">
         <f>C11</f>
@@ -4112,25 +4127,25 @@
         <v>009</v>
       </c>
       <c r="H12" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I12" s="131" t="str">
         <f>I11</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J12" s="132" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="K12" s="136" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="L12" s="136"/>
       <c r="M12" s="67"/>
       <c r="N12" s="66" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="O12" s="134" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="P12" s="134" t="str">
         <f>P11</f>
@@ -4147,7 +4162,7 @@
         <v>asignatura10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="C13" s="66" t="str">
         <f>C12</f>
@@ -4165,25 +4180,25 @@
         <v>010</v>
       </c>
       <c r="H13" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I13" s="131" t="str">
         <f>I12</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J13" s="132" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="K13" s="136" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="L13" s="136"/>
       <c r="M13" s="67"/>
       <c r="N13" s="66" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="O13" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P13" s="134" t="str">
         <f>P12</f>
@@ -4200,7 +4215,7 @@
         <v>asignatura11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C14" s="66" t="str">
         <f>C13</f>
@@ -4218,25 +4233,25 @@
         <v>011</v>
       </c>
       <c r="H14" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I14" s="131" t="str">
         <f>I13</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J14" s="132" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="K14" s="136" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="L14" s="136"/>
       <c r="M14" s="67"/>
       <c r="N14" s="66" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="O14" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P14" s="134" t="str">
         <f>P13</f>
@@ -4253,7 +4268,7 @@
         <v>asignatura12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="C15" s="66" t="str">
         <f>C14</f>
@@ -4271,25 +4286,25 @@
         <v>012</v>
       </c>
       <c r="H15" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I15" s="131" t="str">
         <f>I14</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J15" s="132" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="K15" s="139" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="L15" s="139"/>
       <c r="M15" s="67"/>
       <c r="N15" s="66" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="O15" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P15" s="134" t="str">
         <f>P14</f>
@@ -4306,7 +4321,7 @@
         <v>asignatura13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="C16" s="66" t="str">
         <f>C15</f>
@@ -4324,25 +4339,25 @@
         <v>013</v>
       </c>
       <c r="H16" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I16" s="131" t="str">
         <f>I15</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J16" s="132" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="K16" s="136" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="L16" s="136"/>
       <c r="M16" s="67"/>
       <c r="N16" s="66" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="O16" s="134" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="P16" s="134" t="str">
         <f>P15</f>
@@ -4359,7 +4374,7 @@
         <v>asignatura14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="C17" s="66" t="str">
         <f>C16</f>
@@ -4377,25 +4392,25 @@
         <v>014</v>
       </c>
       <c r="H17" s="66" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I17" s="131" t="str">
         <f>I16</f>
         <v>2ºA|2ºA</v>
       </c>
       <c r="J17" s="132" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="K17" s="136" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="L17" s="136"/>
       <c r="M17" s="67"/>
       <c r="N17" s="66" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="O17" s="134" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="P17" s="134" t="str">
         <f>P16</f>
@@ -4451,7 +4466,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" ht="21.75" customHeight="1">
@@ -4459,12 +4474,12 @@
         <v>27</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B3" s="86" t="str">
         <f>profiles!$A$8</f>
@@ -4473,7 +4488,7 @@
     </row>
     <row r="4" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B4" s="86" t="str">
         <f>profiles!$A$9</f>
@@ -4519,28 +4534,28 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" ht="24" customHeight="1">
@@ -4585,21 +4600,21 @@
     </row>
     <row r="3" ht="34.5" customHeight="1">
       <c r="A3" s="141" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B3" s="142" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="C3" s="143"/>
       <c r="D3" s="144"/>
       <c r="E3" s="143" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="F3" s="145" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="G3" s="146" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="H3" s="147" t="str">
         <f>users!A4</f>
@@ -4610,7 +4625,7 @@
         <v>programB</v>
       </c>
       <c r="J3" s="149" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4"/>
@@ -4664,43 +4679,43 @@
         <v>23</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="C1" s="135" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D1" s="135" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="E1" s="135" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="F1" s="135" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="G1" s="152" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H1" s="135" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="I1" s="135" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="J1" s="135" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="K1" s="135" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="L1" s="135" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="M1" s="135" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="N1" s="135" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -4708,43 +4723,43 @@
         <v>27</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="C2" s="105" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="D2" s="105" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="G2" s="123" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="153" t="s">
+        <v>413</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="J2" s="123" t="s">
+        <v>415</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="L2" s="105" t="s">
         <v>406</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="G2" s="123" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2" s="153" t="s">
-        <v>408</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="J2" s="123" t="s">
-        <v>410</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="L2" s="105" t="s">
-        <v>401</v>
-      </c>
       <c r="M2" s="123" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" ht="114">
@@ -4757,31 +4772,31 @@
         <v>qbank01</v>
       </c>
       <c r="C3" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D3" s="150"/>
       <c r="E3" s="150" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F3" s="150" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G3" s="156" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="H3" s="157" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="I3" s="150"/>
       <c r="J3" s="157" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="K3" s="151"/>
       <c r="L3" s="150">
         <v>1</v>
       </c>
       <c r="M3" s="157" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="N3" s="150"/>
       <c r="O3" s="158">
@@ -4798,31 +4813,31 @@
         <v>qbank01</v>
       </c>
       <c r="C4" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D4" s="150"/>
       <c r="E4" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F4" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F4" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G4" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H4" s="157" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="I4" s="150"/>
       <c r="J4" s="157" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="K4" s="150"/>
       <c r="L4" s="150">
         <v>4</v>
       </c>
       <c r="M4" s="157" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="N4" s="150"/>
       <c r="O4" s="158">
@@ -4840,31 +4855,31 @@
         <v>qbank01</v>
       </c>
       <c r="C5" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D5" s="150"/>
       <c r="E5" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F5" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F5" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G5" s="156" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="H5" s="157" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="I5" s="150"/>
       <c r="J5" s="157" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="K5" s="150"/>
       <c r="L5" s="150">
         <v>3</v>
       </c>
       <c r="M5" s="157" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="N5" s="150"/>
       <c r="O5" s="158">
@@ -4882,31 +4897,31 @@
         <v>qbank01</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D6" s="150"/>
       <c r="E6" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F6" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F6" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G6" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H6" s="157" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="I6" s="150"/>
       <c r="J6" s="157" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="K6" s="150"/>
       <c r="L6" s="150">
         <v>2</v>
       </c>
       <c r="M6" s="157" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="N6" s="150"/>
       <c r="O6" s="158">
@@ -4924,31 +4939,31 @@
         <v>qbank01</v>
       </c>
       <c r="C7" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D7" s="150"/>
       <c r="E7" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F7" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F7" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G7" s="156" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="H7" s="157" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="I7" s="150"/>
       <c r="J7" s="157" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="K7" s="150"/>
       <c r="L7" s="150">
         <v>1</v>
       </c>
       <c r="M7" s="157" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="N7" s="150"/>
       <c r="O7" s="158">
@@ -4966,31 +4981,31 @@
         <v>qbank01</v>
       </c>
       <c r="C8" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D8" s="150"/>
       <c r="E8" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F8" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F8" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G8" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H8" s="157" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="I8" s="151"/>
       <c r="J8" s="157" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="K8" s="150"/>
       <c r="L8" s="150">
         <v>2</v>
       </c>
       <c r="M8" s="157" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="N8" s="159"/>
       <c r="O8" s="158">
@@ -5008,31 +5023,31 @@
         <v>qbank01</v>
       </c>
       <c r="C9" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D9" s="150"/>
       <c r="E9" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F9" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F9" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G9" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H9" s="157" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="I9" s="151"/>
       <c r="J9" s="157" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="K9" s="150"/>
       <c r="L9" s="150">
         <v>3</v>
       </c>
       <c r="M9" s="157" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="N9" s="150"/>
       <c r="O9" s="158">
@@ -5050,31 +5065,31 @@
         <v>qbank01</v>
       </c>
       <c r="C10" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D10" s="150"/>
       <c r="E10" s="150" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F10" s="150" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="G10" s="156" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="H10" s="157" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="I10" s="150"/>
       <c r="J10" s="150"/>
       <c r="K10" s="160" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="L10" s="150">
         <v>2</v>
       </c>
       <c r="M10" s="157" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="N10" s="150"/>
       <c r="O10" s="158">
@@ -5092,33 +5107,33 @@
         <v>qbank01</v>
       </c>
       <c r="C11" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D11" s="150"/>
       <c r="E11" s="150" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F11" s="150" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="G11" s="156" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="H11" s="157" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="I11" s="160" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="J11" s="157" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="K11" s="150"/>
       <c r="L11" s="150">
         <v>1</v>
       </c>
       <c r="M11" s="157" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="N11" s="150"/>
       <c r="O11" s="158">
@@ -5136,31 +5151,31 @@
         <v>qbank01</v>
       </c>
       <c r="C12" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D12" s="150"/>
       <c r="E12" s="150" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="F12" s="150" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G12" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H12" s="157" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="I12" s="150"/>
       <c r="J12" s="161" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="K12" s="150"/>
       <c r="L12" s="150">
         <v>4</v>
       </c>
       <c r="M12" s="157" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="N12" s="150"/>
       <c r="O12" s="158">
@@ -5178,31 +5193,31 @@
         <v>qbank01</v>
       </c>
       <c r="C13" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D13" s="150"/>
       <c r="E13" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F13" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F13" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G13" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H13" s="157" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="I13" s="150"/>
       <c r="J13" s="157" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="K13" s="150"/>
       <c r="L13" s="150">
         <v>3</v>
       </c>
       <c r="M13" s="157" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="N13" s="150"/>
       <c r="O13" s="158">
@@ -5220,31 +5235,31 @@
         <v>qbank01</v>
       </c>
       <c r="C14" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D14" s="150"/>
       <c r="E14" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F14" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F14" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G14" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H14" s="157" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="I14" s="150"/>
       <c r="J14" s="157" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="K14" s="150"/>
       <c r="L14" s="150">
         <v>1</v>
       </c>
       <c r="M14" s="157" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="N14" s="150"/>
       <c r="O14" s="158">
@@ -5262,33 +5277,33 @@
         <v>qbank01</v>
       </c>
       <c r="C15" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="150" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="F15" s="150" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="G15" s="156" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="H15" s="157" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="I15" s="150" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="J15" s="157" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="K15" s="151"/>
       <c r="L15" s="150">
         <v>2</v>
       </c>
       <c r="M15" s="157" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="N15" s="150"/>
       <c r="O15" s="158">
@@ -5306,33 +5321,33 @@
         <v>qbank01</v>
       </c>
       <c r="C16" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="150" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="F16" s="150" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="G16" s="156" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="H16" s="157" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="I16" s="150" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="J16" s="157" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="K16" s="151"/>
       <c r="L16" s="150">
         <v>1</v>
       </c>
       <c r="M16" s="157" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="N16" s="159"/>
       <c r="O16" s="158">
@@ -5350,31 +5365,31 @@
         <v>qbank01</v>
       </c>
       <c r="C17" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F17" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F17" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G17" s="156" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="H17" s="157" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="I17" s="151"/>
       <c r="J17" s="157" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="K17" s="151"/>
       <c r="L17" s="150">
         <v>2</v>
       </c>
       <c r="M17" s="157" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="N17" s="159"/>
       <c r="O17" s="158">
@@ -5392,31 +5407,31 @@
         <v>qbank01</v>
       </c>
       <c r="C18" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F18" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F18" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G18" s="156" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="H18" s="157" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="I18" s="151"/>
       <c r="J18" s="157" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="K18" s="151"/>
       <c r="L18" s="150">
         <v>1</v>
       </c>
       <c r="M18" s="157" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="N18" s="159"/>
       <c r="O18" s="158">
@@ -5434,31 +5449,31 @@
         <v>qbank01</v>
       </c>
       <c r="C19" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F19" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F19" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G19" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H19" s="157" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="I19" s="151"/>
       <c r="J19" s="157" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="K19" s="151"/>
       <c r="L19" s="150">
         <v>3</v>
       </c>
       <c r="M19" s="157" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="N19" s="159"/>
       <c r="O19" s="158">
@@ -5476,31 +5491,31 @@
         <v>qbank01</v>
       </c>
       <c r="C20" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="150" t="s">
+        <v>426</v>
+      </c>
+      <c r="F20" s="150" t="s">
         <v>421</v>
       </c>
-      <c r="F20" s="150" t="s">
-        <v>416</v>
-      </c>
       <c r="G20" s="156" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H20" s="157" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="I20" s="151"/>
       <c r="J20" s="157" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="K20" s="151"/>
       <c r="L20" s="150">
         <v>4</v>
       </c>
       <c r="M20" s="157" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="N20" s="159"/>
       <c r="O20" s="158">
@@ -5518,31 +5533,31 @@
         <v>qbank01</v>
       </c>
       <c r="C21" s="150" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="150" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="F21" s="150" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G21" s="156" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="H21" s="157" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="I21" s="150"/>
       <c r="J21" s="157" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="K21" s="150"/>
       <c r="L21" s="150">
         <v>4</v>
       </c>
       <c r="M21" s="157" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="N21" s="150"/>
       <c r="O21" s="158">
@@ -5560,30 +5575,30 @@
         <v>qbank01</v>
       </c>
       <c r="C22" s="150" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="150" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="161" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="H22" s="157" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="I22" s="160" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="J22" s="157" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="K22" s="151"/>
       <c r="L22" s="162"/>
       <c r="M22" s="163"/>
       <c r="N22" s="9" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="O22" s="164">
         <f>O21+1</f>
@@ -5869,8 +5884,18 @@
         <f>_xlfn.CONCAT($AG$3,".",AH5)</f>
         <v>plugins.tests.questionsBanks</v>
       </c>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
+      <c r="AI1" s="16" t="str">
+        <f>_xlfn.CONCAT($AI$3,".",AI5)</f>
+        <v>plugins.assignables.activities</v>
+      </c>
+      <c r="AJ1" s="16" t="str">
+        <f>_xlfn.CONCAT($AI$3,".",AJ5)</f>
+        <v>plugins.assignables.ongoing</v>
+      </c>
+      <c r="AK1" s="16" t="str">
+        <f>_xlfn.CONCAT($AI$3,".",AK5)</f>
+        <v>plugins.assignables.history</v>
+      </c>
     </row>
     <row r="2" s="9" customFormat="1" ht="21.25" customHeight="1">
       <c r="E2" s="17" t="s">
@@ -5905,6 +5930,9 @@
       <c r="AF2" s="17"/>
       <c r="AG2" s="17"/>
       <c r="AH2" s="17"/>
+      <c r="AI2" s="17"/>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17"/>
     </row>
     <row r="3">
       <c r="B3" s="18"/>
@@ -5962,29 +5990,34 @@
         <v>53</v>
       </c>
       <c r="AH3" s="20"/>
+      <c r="AI3" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ3" s="29"/>
+      <c r="AK3" s="29"/>
     </row>
     <row r="4" s="31" customFormat="1" ht="19.75" customHeight="1">
       <c r="E4" s="32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
       <c r="I4" s="34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L4" s="37"/>
       <c r="M4" s="37"/>
       <c r="N4" s="37"/>
       <c r="O4" s="37"/>
       <c r="P4" s="38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="39"/>
       <c r="R4" s="39"/>
@@ -5992,124 +6025,138 @@
       <c r="T4" s="39"/>
       <c r="U4" s="40"/>
       <c r="V4" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W4" s="33"/>
       <c r="X4" s="34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y4" s="41"/>
       <c r="Z4" s="41"/>
       <c r="AA4" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AB4" s="36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AC4" s="38" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AD4" s="39"/>
       <c r="AE4" s="39"/>
       <c r="AF4" s="39"/>
       <c r="AG4" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AH4" s="33"/>
+      <c r="AI4" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ4" s="41"/>
+      <c r="AK4" s="41"/>
     </row>
     <row r="5">
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="42" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J5" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5" s="48" t="s">
-        <v>68</v>
-      </c>
       <c r="N5" s="48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O5" s="48" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P5" s="49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Q5" s="50" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="R5" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="S5" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="U5" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="V5" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="T5" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="U5" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="V5" s="42" t="s">
-        <v>76</v>
-      </c>
       <c r="W5" s="43" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="X5" s="45" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y5" s="45" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Z5" s="45" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AA5" s="46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AB5" s="52" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="AC5" s="49" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AD5" s="50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AE5" s="50" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AF5" s="50" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AG5" s="42" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AH5" s="43" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="AI5" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ5" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK5" s="45" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" s="53" customFormat="1" ht="19.5" customHeight="1">
@@ -6123,312 +6170,339 @@
         <v>29</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="H6" s="56" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="I6" s="57" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J6" s="58" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K6" s="59" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L6" s="60" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="M6" s="60" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="N6" s="60" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="O6" s="60" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="P6" s="61" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="62" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="R6" s="62" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S6" s="62" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="T6" s="62" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="U6" s="63" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="V6" s="55" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="X6" s="57" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y6" s="57" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z6" s="57" t="str">
         <f>PROPER(Z5)</f>
         <v>Profiles</v>
       </c>
       <c r="AA6" s="64" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="AB6" s="65" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AC6" s="61" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="AD6" s="62" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="AE6" s="62" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="AF6" s="62" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AG6" s="55" t="str">
         <f>PROPER(AG5)</f>
         <v>Tests</v>
       </c>
       <c r="AH6" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI6" s="53"/>
+        <v>114</v>
+      </c>
+      <c r="AI6" s="57" t="str">
+        <f>PROPER(AI5)</f>
+        <v>Activities</v>
+      </c>
+      <c r="AJ6" s="57" t="str">
+        <f>PROPER(AJ5)</f>
+        <v>Ongoing</v>
+      </c>
+      <c r="AK6" s="57" t="str">
+        <f>PROPER(AK5)</f>
+        <v>History</v>
+      </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D7" s="66"/>
       <c r="E7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="I7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="J7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="L7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="M7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="N7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="O7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="R7" s="68"/>
       <c r="S7" s="68"/>
       <c r="T7" s="68"/>
       <c r="U7" s="68"/>
       <c r="V7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="W7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="X7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Y7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Z7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AA7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AB7" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AC7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AD7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AE7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AF7" s="68" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AG7" s="69" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AH7" s="69" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI7" s="9"/>
+        <v>115</v>
+      </c>
+      <c r="AI7" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ7" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK7" s="67" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D8" s="66"/>
       <c r="E8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F8" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G8" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H8" s="67"/>
       <c r="I8" s="67" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="J8" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="L8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="M8" s="67"/>
       <c r="N8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="O8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="P8" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Q8" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="R8" s="68"/>
       <c r="S8" s="67"/>
       <c r="T8" s="67"/>
       <c r="U8" s="67"/>
       <c r="V8" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="W8" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="X8" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Y8" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="Z8" s="67"/>
       <c r="AA8" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AB8" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC8" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="AC8" s="70" t="s">
-        <v>116</v>
-      </c>
       <c r="AD8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AE8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AF8" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AG8" s="70" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AH8" s="70" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI8" s="9"/>
+        <v>115</v>
+      </c>
+      <c r="AI8" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ8" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK8" s="67" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F9" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H9" s="67"/>
       <c r="I9" s="67" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="J9" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K9" s="67"/>
       <c r="L9" s="67"/>
@@ -6436,87 +6510,95 @@
       <c r="N9" s="67"/>
       <c r="O9" s="67"/>
       <c r="P9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Q9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="R9" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="S9" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="T9" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="U9" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="V9" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="S9" s="67" t="s">
+      <c r="W9" s="67" t="s">
         <v>118</v>
-      </c>
-      <c r="T9" s="67" t="s">
-        <v>118</v>
-      </c>
-      <c r="U9" s="67" t="s">
-        <v>118</v>
-      </c>
-      <c r="V9" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="W9" s="67" t="s">
-        <v>116</v>
       </c>
       <c r="X9" s="67"/>
       <c r="Y9" s="67"/>
       <c r="Z9" s="67"/>
       <c r="AA9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AB9" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC9" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="AC9" s="67" t="s">
-        <v>116</v>
-      </c>
       <c r="AD9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AE9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AF9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AG9" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AH9" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="AI9" s="9"/>
+        <v>118</v>
+      </c>
+      <c r="AI9" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ9" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK9" s="67" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D10" s="66" t="str">
         <f>A9</f>
         <v>student</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F10" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G10" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H10" s="67"/>
       <c r="I10" s="67" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="J10" s="67" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K10" s="67"/>
       <c r="L10" s="67"/>
@@ -6524,22 +6606,22 @@
       <c r="N10" s="67"/>
       <c r="O10" s="67"/>
       <c r="P10" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Q10" s="67" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="R10" s="67" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="S10" s="67" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="T10" s="67" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="U10" s="67" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="V10" s="67"/>
       <c r="W10" s="67"/>
@@ -6548,7 +6630,7 @@
       <c r="Z10" s="67"/>
       <c r="AA10" s="67"/>
       <c r="AB10" s="67" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AC10" s="67"/>
       <c r="AD10" s="67"/>
@@ -6556,11 +6638,13 @@
       <c r="AF10" s="67"/>
       <c r="AG10" s="67"/>
       <c r="AH10" s="67"/>
-      <c r="AI10" s="9"/>
+      <c r="AI10" s="67"/>
+      <c r="AJ10" s="67"/>
+      <c r="AK10" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E2:AH2"/>
+  <mergeCells count="17">
+    <mergeCell ref="E2:AK2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="K3:O3"/>
     <mergeCell ref="P3:U3"/>
@@ -6568,6 +6652,7 @@
     <mergeCell ref="X3:Z3"/>
     <mergeCell ref="AC3:AF3"/>
     <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AI3:AK3"/>
     <mergeCell ref="E4:H4"/>
     <mergeCell ref="K4:O4"/>
     <mergeCell ref="P4:U4"/>
@@ -6575,6 +6660,7 @@
     <mergeCell ref="X4:Z4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI4:AK4"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -6618,31 +6704,31 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
@@ -6653,42 +6739,42 @@
         <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H2" s="71" t="s">
         <v>30</v>
       </c>
       <c r="I2" s="71" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="J2" s="72" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="K2" s="73" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>12</v>
@@ -6697,33 +6783,33 @@
         <v>36526</v>
       </c>
       <c r="F3" s="75" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H3" s="70" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="67" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="J3" s="67" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="K3" s="76" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>12</v>
@@ -6732,34 +6818,34 @@
         <v>27670</v>
       </c>
       <c r="F4" s="75" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H4" s="70" t="str">
         <f>H3</f>
         <v>es</v>
       </c>
       <c r="I4" s="77" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="J4" s="70" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="K4" s="76" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
@@ -6768,34 +6854,34 @@
         <v>27518</v>
       </c>
       <c r="F5" s="78" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H5" s="70" t="str">
         <f>H4</f>
         <v>es</v>
       </c>
       <c r="I5" s="67" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="J5" s="70" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K5" s="79" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -6804,10 +6890,10 @@
         <v>34447</v>
       </c>
       <c r="F6" s="81" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H6" s="82" t="str">
         <f>H5</f>
@@ -6815,21 +6901,21 @@
       </c>
       <c r="I6" s="83"/>
       <c r="J6" s="82" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="K6" s="76" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
@@ -6838,33 +6924,33 @@
         <v>27791</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H7" s="70" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="67" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="J7" s="70" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="K7" s="79" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>12</v>
@@ -6873,34 +6959,34 @@
         <v>39571</v>
       </c>
       <c r="F8" s="78" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H8" s="70" t="str">
         <f>H6</f>
         <v>es</v>
       </c>
       <c r="I8" s="67" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="J8" s="70" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="K8" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
@@ -6909,35 +6995,35 @@
         <v>39572</v>
       </c>
       <c r="F9" s="75" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H9" s="70" t="str">
         <f>H8</f>
         <v>es</v>
       </c>
       <c r="I9" s="67" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="J9" s="67" t="str">
         <f>J8</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K9" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>13</v>
@@ -6946,35 +7032,35 @@
         <v>39573</v>
       </c>
       <c r="F10" s="75" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H10" s="70" t="str">
         <f>H9</f>
         <v>es</v>
       </c>
       <c r="I10" s="67" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="J10" s="67" t="str">
         <f>J9</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K10" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>12</v>
@@ -6983,35 +7069,35 @@
         <v>39208</v>
       </c>
       <c r="F11" s="75" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H11" s="70" t="str">
         <f>H10</f>
         <v>es</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="J11" s="67" t="str">
         <f>J10</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K11" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>13</v>
@@ -7020,35 +7106,35 @@
         <v>39575</v>
       </c>
       <c r="F12" s="78" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H12" s="70" t="str">
         <f>H11</f>
         <v>es</v>
       </c>
       <c r="I12" s="67" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J12" s="67" t="str">
         <f>J11</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K12" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>13</v>
@@ -7057,35 +7143,35 @@
         <v>39576</v>
       </c>
       <c r="F13" s="78" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H13" s="70" t="str">
         <f>H12</f>
         <v>es</v>
       </c>
       <c r="I13" s="67" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="J13" s="67" t="str">
         <f>J12</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K13" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>12</v>
@@ -7094,35 +7180,35 @@
         <v>39577</v>
       </c>
       <c r="F14" s="78" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H14" s="70" t="str">
         <f>H13</f>
         <v>es</v>
       </c>
       <c r="I14" s="67" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="J14" s="67" t="str">
         <f>J13</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K14" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>13</v>
@@ -7131,35 +7217,35 @@
         <v>39578</v>
       </c>
       <c r="F15" s="78" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H15" s="70" t="str">
         <f>H14</f>
         <v>es</v>
       </c>
       <c r="I15" s="67" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="J15" s="67" t="str">
         <f>J14</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K15" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>12</v>
@@ -7168,35 +7254,35 @@
         <v>39579</v>
       </c>
       <c r="F16" s="78" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H16" s="70" t="str">
         <f>H15</f>
         <v>es</v>
       </c>
       <c r="I16" s="67" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="J16" s="67" t="str">
         <f>J15</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K16" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" s="18" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>12</v>
@@ -7205,35 +7291,35 @@
         <v>39580</v>
       </c>
       <c r="F17" s="78" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H17" s="70" t="str">
         <f>H16</f>
         <v>es</v>
       </c>
       <c r="I17" s="67" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="J17" s="67" t="str">
         <f>J16</f>
         <v>Estudiante,Test</v>
       </c>
       <c r="K17" s="79" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="13" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>13</v>
@@ -7242,10 +7328,10 @@
         <v>39575</v>
       </c>
       <c r="F18" s="84" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H18" s="82" t="str">
         <f>H17</f>
@@ -7257,18 +7343,18 @@
         <v>Estudiante,Test</v>
       </c>
       <c r="K18" s="76" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>13</v>
@@ -7277,10 +7363,10 @@
         <v>39576</v>
       </c>
       <c r="F19" s="84" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H19" s="82" t="str">
         <f>H18</f>
@@ -7292,18 +7378,18 @@
         <v>Estudiante,Test</v>
       </c>
       <c r="K19" s="76" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="13" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>12</v>
@@ -7312,10 +7398,10 @@
         <v>39577</v>
       </c>
       <c r="F20" s="84" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H20" s="82" t="str">
         <f>H19</f>
@@ -7327,7 +7413,7 @@
         <v>Estudiante,Test</v>
       </c>
       <c r="K20" s="76" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" ht="14.25"/>
@@ -7370,37 +7456,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0076005C-007C-4698-8253-0009006A0049}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EE00CE-003C-4677-93EC-009800000064}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00190052-00BB-477D-A034-007D003F0057}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000A007C-00E8-417B-AF7B-0036003100C4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A9006C-0099-444A-B27A-000B0054005D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B70082-00BF-439A-B584-00AD00B90075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00210036-0012-4871-898A-00FB00DB000C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001A001A-00E4-4357-9C12-0010003000B4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E1008C-0045-47D7-ABD6-00B300D00040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001A002D-00D6-4A23-98B6-00A500FD002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001200C6-0078-431C-80A5-0080006900C5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0088005F-00B7-476D-B065-009100E5006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -7435,7 +7521,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
@@ -7443,12 +7529,12 @@
         <v>27</v>
       </c>
       <c r="B2" s="85" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B3" s="86" t="str">
         <f>profiles!$A$10</f>
@@ -7457,7 +7543,7 @@
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B4" s="86" t="str">
         <f>profiles!$A$9</f>
@@ -7500,13 +7586,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" ht="24.25" customHeight="1">
@@ -7517,30 +7603,30 @@
         <v>28</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D2" s="85" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="E2" s="73" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D3" s="90" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="86" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -7551,7 +7637,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00F900C7-00CB-4230-A5FE-0017009E00A0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E70085-0037-49FC-B39C-008500310008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -7591,19 +7677,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" ht="24.75" customHeight="1">
@@ -7614,27 +7700,27 @@
         <v>28</v>
       </c>
       <c r="C2" s="92" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D2" s="91" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F2" s="91" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="G2" s="91" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" ht="146.25" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C3" s="86" t="str">
         <f>centers!$A$3</f>
@@ -7647,7 +7733,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="G3" s="67">
         <v>5</v>
@@ -7655,10 +7741,10 @@
     </row>
     <row r="4" s="18" customFormat="1" ht="146.25" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C4" s="86" t="str">
         <f>centers!$A$4</f>
@@ -7671,7 +7757,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="93" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="G4" s="67">
         <v>5</v>
@@ -7685,13 +7771,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00260038-0030-4927-849D-00F300AE0075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00460063-00A0-46B3-BF32-0054004A00CF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E000C3-0090-4201-881E-000800F700DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009F007E-00C0-4928-B826-00DF00F0007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7725,7 +7811,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" ht="22" customHeight="1">
@@ -7733,12 +7819,12 @@
         <v>27</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B3" s="86" t="str">
         <f>profiles!$A$8</f>
@@ -7747,7 +7833,7 @@
     </row>
     <row r="4" s="9" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B4" s="86" t="str">
         <f>profiles!$A$9</f>
@@ -7806,73 +7892,73 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
@@ -7894,11 +7980,11 @@
     <row r="2" s="9" customFormat="1" ht="23.5" customHeight="1">
       <c r="C2" s="9"/>
       <c r="G2" s="94" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="95" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="J2" s="96"/>
       <c r="K2" s="96"/>
@@ -7907,18 +7993,18 @@
       <c r="N2" s="96"/>
       <c r="O2" s="97"/>
       <c r="P2" s="98" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="Q2" s="98"/>
       <c r="R2" s="98"/>
       <c r="S2" s="99" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="T2" s="100"/>
       <c r="U2" s="100"/>
       <c r="V2" s="101"/>
       <c r="W2" s="102" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="X2" s="103"/>
       <c r="Y2" s="103"/>
@@ -7931,87 +8017,87 @@
         <v>28</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D3" s="106" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E3" s="106" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F3" s="107" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="G3" s="108" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="H3" s="109" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="I3" s="110" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="J3" s="111" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="K3" s="112" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="L3" s="112" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="M3" s="112" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="N3" s="112" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="O3" s="112" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="P3" s="113" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="Q3" s="114" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="R3" s="115" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="S3" s="116" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="T3" s="117" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U3" s="117" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="V3" s="117" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="W3" s="118" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="X3" s="119" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="Y3" s="120" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="D4" s="121" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E4" s="66" t="str">
         <f>centers!$A$3</f>
@@ -8069,16 +8155,16 @@
     </row>
     <row r="5" s="9" customFormat="1" ht="46.5" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="D5" s="121" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E5" s="66" t="str">
         <f>centers!$A$4</f>
@@ -8102,7 +8188,7 @@
         <v>10</v>
       </c>
       <c r="L5" s="122" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="M5" s="67" t="s">
         <v>4</v>
@@ -8158,13 +8244,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D5001F-0050-43EE-BD31-008A0057007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DF00F7-0013-4399-AEC1-001B00290012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A4004B-00DE-4D10-BB0A-00F6008700D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001A00DC-0089-4289-8755-0088006A0009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
CHANGED: Excel AR_Evaluations to numeric
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="505">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -813,7 +813,7 @@
     <t xml:space="preserve">Reglas primaria</t>
   </si>
   <si>
-    <t xml:space="preserve">IN|1|Insuficiente, IN|2|Insuficiente, IN|3|Insuficiente, IN|4|Insuficiente, SU|5|Suficiente, BI|6|Bien, NT|7|Notable, NT|8|Notable, SB|9|Sobresaliente, SB|10|Sobresaliente</t>
+    <t xml:space="preserve">1|Insuficiente, 2|Insuficiente, 3|Insuficiente, 4|Insuficiente, 5|Suficiente, 6|Bien, 7|Notable, 8|Notable, 9|Sobresaliente, 10|Sobresaliente</t>
   </si>
   <si>
     <t>gradeB</t>
@@ -1083,12 +1083,15 @@
     <t>2ºA|2ºA</t>
   </si>
   <si>
-    <t>#4290f5</t>
+    <t>#B462F2</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/FQ_2_36a510dc62.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Fisica_y_quimica_B462_F2_1e50644b43.svg</t>
+  </si>
+  <si>
     <t>teacher02|main@2ºA</t>
   </si>
   <si>
@@ -1098,33 +1101,42 @@
     <t xml:space="preserve">Geografía e Historia</t>
   </si>
   <si>
-    <t>#f56c42</t>
+    <t>#1BB184</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/GH_6_cb0f8c51e8.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Geografia_e_Historia_1_BB_184_344ecf5269.svg</t>
+  </si>
+  <si>
     <t>teacher01|main@2ºA</t>
   </si>
   <si>
     <t xml:space="preserve">Lengua castellana y literatura</t>
   </si>
   <si>
-    <t>#f56c43</t>
+    <t>#DC5571</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/LEN_1_c91a1ba005.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Lengua_castellana_y_literatura_DC_5571_38293fa0f0.svg</t>
+  </si>
+  <si>
     <t>Matemáticas</t>
   </si>
   <si>
-    <t>#f56c44</t>
+    <t>#4F96FF</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/MAT_1_f1b208dde4.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Matematicas_4_F96_FF_8ff138d73c.svg</t>
+  </si>
+  <si>
     <t>Inglés</t>
   </si>
   <si>
@@ -1137,30 +1149,39 @@
     <t xml:space="preserve">Educación física</t>
   </si>
   <si>
-    <t>#f56c46</t>
+    <t>#7449F4</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/EF_4_7d44c52842.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Educacion_fisica_7449_F4_f1ebca85a0.svg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Educación plástica, visual y audiovisual</t>
   </si>
   <si>
-    <t>#f56c47</t>
+    <t>#E36B2B</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/epv_3_84d7510eaf.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Educacion_plastica_visual_y_audiovisual_E36_B2_B_3a37e3ce5e.svg</t>
+  </si>
+  <si>
     <t>Música</t>
   </si>
   <si>
-    <t>#f56c48</t>
+    <t>#E8C642</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/MUS_3_faa4332fac.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Musica_E8_C642_00ae04b699.svg</t>
+  </si>
+  <si>
     <t>Francés</t>
   </si>
   <si>
@@ -1173,40 +1194,49 @@
     <t xml:space="preserve">Recuperación de lengua</t>
   </si>
   <si>
-    <t>#f56c50</t>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Recuperacion_de_lengua_DC_5571_fbf841c98c.svg</t>
   </si>
   <si>
     <t xml:space="preserve">Recuperación de matemáticas</t>
   </si>
   <si>
-    <t>#f56c51</t>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/recuperacion_mates_4_F96_FF_7c216d0f8d.svg</t>
   </si>
   <si>
     <t xml:space="preserve">Valores éticos</t>
   </si>
   <si>
-    <t>#f56c52</t>
+    <t>#08829C</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/ETICA_2_cf3d161bde.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Valores_eticos_08829_C_d545e11280.svg</t>
+  </si>
+  <si>
     <t>Religión</t>
   </si>
   <si>
-    <t>#f56c53</t>
+    <t>#5B6577</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/REL_1_4b9c2c7ec6.jpeg</t>
   </si>
   <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Religion_5_B6577_98b0dcd33a.svg</t>
+  </si>
+  <si>
     <t>Tutoría</t>
   </si>
   <si>
-    <t>#f56c54</t>
+    <t>#81CD06</t>
   </si>
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/TUTORIA_2_b91df6d313.jpeg</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/Tutoria_81_CD_06_3d0192414d.svg</t>
   </si>
   <si>
     <t>tagline</t>
@@ -1625,7 +1655,7 @@
   <numFmts count="1">
     <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -1724,6 +1754,12 @@
       <color indexed="64"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="10"/>
+      <sz val="10.000000"/>
+      <u/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1862,7 +1898,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -2137,6 +2173,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2180,7 +2231,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="169">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2573,6 +2624,9 @@
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf fontId="11" fillId="0" borderId="25" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf fontId="13" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2582,39 +2636,48 @@
     <xf fontId="13" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="15" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf fontId="15" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="15" fillId="0" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="16" fillId="0" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="11" fillId="0" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="16" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf fontId="15" fillId="0" borderId="25" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="16" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="17" fillId="0" borderId="26" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="5" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="11" fillId="0" borderId="26" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="11" fillId="0" borderId="27" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -2630,7 +2693,7 @@
     <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -2639,7 +2702,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -2657,7 +2720,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -3440,7 +3503,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{002E0064-0004-4F26-AAD2-001F00D70022}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002400C7-0006-4052-BADB-007400F80064}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -3714,18 +3777,20 @@
       <c r="K4" s="133" t="s">
         <v>350</v>
       </c>
-      <c r="L4" s="133"/>
+      <c r="L4" s="134" t="s">
+        <v>351</v>
+      </c>
       <c r="M4" s="67"/>
       <c r="N4" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O4" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P4" s="134" t="s">
+      <c r="O4" s="135" t="s">
         <v>352</v>
       </c>
-      <c r="Q4" s="135">
+      <c r="P4" s="135" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q4" s="136">
         <v>1</v>
       </c>
     </row>
@@ -3735,7 +3800,7 @@
         <v>asignatura02</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C5" s="66" t="str">
         <f>C4</f>
@@ -3760,24 +3825,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J5" s="132" t="s">
-        <v>354</v>
-      </c>
-      <c r="K5" s="136" t="s">
         <v>355</v>
       </c>
-      <c r="L5" s="136"/>
+      <c r="K5" s="137" t="s">
+        <v>356</v>
+      </c>
+      <c r="L5" s="138" t="s">
+        <v>357</v>
+      </c>
       <c r="M5" s="67"/>
       <c r="N5" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O5" s="134" t="s">
-        <v>356</v>
-      </c>
-      <c r="P5" s="134" t="str">
+      <c r="O5" s="135" t="s">
+        <v>358</v>
+      </c>
+      <c r="P5" s="135" t="str">
         <f>P4</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q5" s="135">
+      <c r="Q5" s="136">
         <f>Q4+1</f>
         <v>2</v>
       </c>
@@ -3789,7 +3856,7 @@
         <v>asignatura03</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C6" s="66" t="str">
         <f>C5</f>
@@ -3814,24 +3881,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J6" s="132" t="s">
-        <v>358</v>
-      </c>
-      <c r="K6" s="136" t="s">
-        <v>359</v>
-      </c>
-      <c r="L6" s="136"/>
+        <v>360</v>
+      </c>
+      <c r="K6" s="137" t="s">
+        <v>361</v>
+      </c>
+      <c r="L6" s="138" t="s">
+        <v>362</v>
+      </c>
       <c r="M6" s="67"/>
       <c r="N6" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O6" s="134" t="s">
-        <v>356</v>
-      </c>
-      <c r="P6" s="134" t="str">
+      <c r="O6" s="135" t="s">
+        <v>358</v>
+      </c>
+      <c r="P6" s="135" t="str">
         <f>P5</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q6" s="135">
+      <c r="Q6" s="136">
         <f>Q5+1</f>
         <v>3</v>
       </c>
@@ -3843,7 +3912,7 @@
         <v>asignatura04</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C7" s="66" t="str">
         <f>C6</f>
@@ -3868,24 +3937,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J7" s="132" t="s">
-        <v>361</v>
-      </c>
-      <c r="K7" s="136" t="s">
-        <v>362</v>
-      </c>
-      <c r="L7" s="136"/>
+        <v>364</v>
+      </c>
+      <c r="K7" s="137" t="s">
+        <v>365</v>
+      </c>
+      <c r="L7" s="139" t="s">
+        <v>366</v>
+      </c>
       <c r="M7" s="67"/>
       <c r="N7" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O7" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P7" s="134" t="str">
+      <c r="O7" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P7" s="135" t="str">
         <f>P6</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q7" s="135">
+      <c r="Q7" s="136">
         <f>Q6+1</f>
         <v>4</v>
       </c>
@@ -3897,7 +3968,7 @@
         <v>asignatura05</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="C8" s="66" t="str">
         <f>C7</f>
@@ -3922,24 +3993,24 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J8" s="132" t="s">
-        <v>364</v>
-      </c>
-      <c r="K8" s="136" t="s">
-        <v>365</v>
-      </c>
-      <c r="L8" s="136"/>
+        <v>368</v>
+      </c>
+      <c r="K8" s="137" t="s">
+        <v>369</v>
+      </c>
+      <c r="L8" s="138"/>
       <c r="M8" s="67"/>
       <c r="N8" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O8" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P8" s="134" t="str">
+      <c r="O8" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P8" s="135" t="str">
         <f>P7</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q8" s="135">
+      <c r="Q8" s="136">
         <f>Q7+1</f>
         <v>5</v>
       </c>
@@ -3950,7 +4021,7 @@
         <v>asignatura06</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C9" s="66" t="str">
         <f>C8</f>
@@ -3975,24 +4046,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J9" s="132" t="s">
-        <v>367</v>
-      </c>
-      <c r="K9" s="137" t="s">
-        <v>368</v>
-      </c>
-      <c r="L9" s="137"/>
+        <v>371</v>
+      </c>
+      <c r="K9" s="140" t="s">
+        <v>372</v>
+      </c>
+      <c r="L9" s="141" t="s">
+        <v>373</v>
+      </c>
       <c r="M9" s="67"/>
       <c r="N9" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O9" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P9" s="134" t="str">
+      <c r="O9" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P9" s="135" t="str">
         <f>P8</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q9" s="135">
+      <c r="Q9" s="136">
         <f>Q8+1</f>
         <v>6</v>
       </c>
@@ -4003,7 +4076,7 @@
         <v>asignatura07</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="C10" s="66" t="str">
         <f>C9</f>
@@ -4028,24 +4101,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J10" s="132" t="s">
-        <v>370</v>
-      </c>
-      <c r="K10" s="138" t="s">
-        <v>371</v>
-      </c>
-      <c r="L10" s="138"/>
+        <v>375</v>
+      </c>
+      <c r="K10" s="142" t="s">
+        <v>376</v>
+      </c>
+      <c r="L10" s="141" t="s">
+        <v>377</v>
+      </c>
       <c r="M10" s="67"/>
       <c r="N10" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O10" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P10" s="134" t="str">
+      <c r="O10" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P10" s="135" t="str">
         <f>P9</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q10" s="135">
+      <c r="Q10" s="136">
         <f>Q9+1</f>
         <v>7</v>
       </c>
@@ -4056,7 +4131,7 @@
         <v>asignatura08</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C11" s="66" t="str">
         <f>C10</f>
@@ -4081,24 +4156,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J11" s="132" t="s">
-        <v>373</v>
-      </c>
-      <c r="K11" s="136" t="s">
-        <v>374</v>
-      </c>
-      <c r="L11" s="136"/>
+        <v>379</v>
+      </c>
+      <c r="K11" s="137" t="s">
+        <v>380</v>
+      </c>
+      <c r="L11" s="138" t="s">
+        <v>381</v>
+      </c>
       <c r="M11" s="67"/>
       <c r="N11" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O11" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P11" s="134" t="str">
+      <c r="O11" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P11" s="135" t="str">
         <f>P10</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q11" s="135">
+      <c r="Q11" s="136">
         <f>Q10+1</f>
         <v>8</v>
       </c>
@@ -4109,7 +4186,7 @@
         <v>asignatura09</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="C12" s="66" t="str">
         <f>C11</f>
@@ -4134,24 +4211,24 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J12" s="132" t="s">
-        <v>376</v>
-      </c>
-      <c r="K12" s="136" t="s">
-        <v>377</v>
-      </c>
-      <c r="L12" s="136"/>
+        <v>383</v>
+      </c>
+      <c r="K12" s="137" t="s">
+        <v>384</v>
+      </c>
+      <c r="L12" s="138"/>
       <c r="M12" s="67"/>
       <c r="N12" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="O12" s="134" t="s">
-        <v>356</v>
-      </c>
-      <c r="P12" s="134" t="str">
+      <c r="O12" s="135" t="s">
+        <v>358</v>
+      </c>
+      <c r="P12" s="135" t="str">
         <f>P11</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q12" s="135">
+      <c r="Q12" s="136">
         <f>Q11+1</f>
         <v>9</v>
       </c>
@@ -4162,7 +4239,7 @@
         <v>asignatura10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="C13" s="66" t="str">
         <f>C12</f>
@@ -4187,24 +4264,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J13" s="132" t="s">
-        <v>379</v>
-      </c>
-      <c r="K13" s="136" t="s">
-        <v>359</v>
-      </c>
-      <c r="L13" s="136"/>
+        <v>360</v>
+      </c>
+      <c r="K13" s="137" t="s">
+        <v>361</v>
+      </c>
+      <c r="L13" s="138" t="s">
+        <v>386</v>
+      </c>
       <c r="M13" s="67"/>
       <c r="N13" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="O13" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P13" s="134" t="str">
+      <c r="O13" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P13" s="135" t="str">
         <f>P12</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q13" s="135">
+      <c r="Q13" s="136">
         <f>Q12+1</f>
         <v>10</v>
       </c>
@@ -4215,7 +4294,7 @@
         <v>asignatura11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C14" s="66" t="str">
         <f>C13</f>
@@ -4240,24 +4319,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J14" s="132" t="s">
-        <v>381</v>
-      </c>
-      <c r="K14" s="136" t="s">
-        <v>362</v>
-      </c>
-      <c r="L14" s="136"/>
+        <v>364</v>
+      </c>
+      <c r="K14" s="137" t="s">
+        <v>365</v>
+      </c>
+      <c r="L14" s="138" t="s">
+        <v>388</v>
+      </c>
       <c r="M14" s="67"/>
       <c r="N14" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="O14" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P14" s="134" t="str">
+      <c r="O14" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P14" s="135" t="str">
         <f>P13</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q14" s="135">
+      <c r="Q14" s="136">
         <f>Q13+1</f>
         <v>11</v>
       </c>
@@ -4268,7 +4349,7 @@
         <v>asignatura12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="C15" s="66" t="str">
         <f>C14</f>
@@ -4293,24 +4374,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J15" s="132" t="s">
-        <v>383</v>
-      </c>
-      <c r="K15" s="139" t="s">
-        <v>384</v>
-      </c>
-      <c r="L15" s="139"/>
+        <v>390</v>
+      </c>
+      <c r="K15" s="143" t="s">
+        <v>391</v>
+      </c>
+      <c r="L15" s="138" t="s">
+        <v>392</v>
+      </c>
       <c r="M15" s="67"/>
       <c r="N15" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="O15" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P15" s="134" t="str">
+      <c r="O15" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P15" s="135" t="str">
         <f>P14</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q15" s="135">
+      <c r="Q15" s="136">
         <f>Q14+1</f>
         <v>12</v>
       </c>
@@ -4321,7 +4404,7 @@
         <v>asignatura13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="C16" s="66" t="str">
         <f>C15</f>
@@ -4346,24 +4429,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J16" s="132" t="s">
-        <v>386</v>
-      </c>
-      <c r="K16" s="136" t="s">
-        <v>387</v>
-      </c>
-      <c r="L16" s="136"/>
+        <v>394</v>
+      </c>
+      <c r="K16" s="137" t="s">
+        <v>395</v>
+      </c>
+      <c r="L16" s="138" t="s">
+        <v>396</v>
+      </c>
       <c r="M16" s="67"/>
       <c r="N16" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="O16" s="134" t="s">
-        <v>351</v>
-      </c>
-      <c r="P16" s="134" t="str">
+      <c r="O16" s="135" t="s">
+        <v>352</v>
+      </c>
+      <c r="P16" s="135" t="str">
         <f>P15</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q16" s="135">
+      <c r="Q16" s="136">
         <f>Q15+1</f>
         <v>13</v>
       </c>
@@ -4374,7 +4459,7 @@
         <v>asignatura14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="C17" s="66" t="str">
         <f>C16</f>
@@ -4399,24 +4484,26 @@
         <v>2ºA|2ºA</v>
       </c>
       <c r="J17" s="132" t="s">
-        <v>389</v>
-      </c>
-      <c r="K17" s="136" t="s">
-        <v>390</v>
-      </c>
-      <c r="L17" s="136"/>
+        <v>398</v>
+      </c>
+      <c r="K17" s="137" t="s">
+        <v>399</v>
+      </c>
+      <c r="L17" s="138" t="s">
+        <v>400</v>
+      </c>
       <c r="M17" s="67"/>
       <c r="N17" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="O17" s="134" t="s">
-        <v>356</v>
-      </c>
-      <c r="P17" s="134" t="str">
+      <c r="O17" s="135" t="s">
+        <v>358</v>
+      </c>
+      <c r="P17" s="135" t="str">
         <f>P16</f>
         <v xml:space="preserve">studentB01@2ºA, studentB02@2ºA, studentB03@2ºA, studentB04@2ºA, studentB05@2ºA, studentB06@2ºA, studentB07@2ºA, studentB08@2ºA, studentB09@2ºA, studentB10@2ºA</v>
       </c>
-      <c r="Q17" s="135">
+      <c r="Q17" s="136">
         <f>Q16+1</f>
         <v>14</v>
       </c>
@@ -4434,8 +4521,20 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="K4"/>
-    <hyperlink r:id="rId2" ref="K9"/>
-    <hyperlink r:id="rId3" ref="K10"/>
+    <hyperlink r:id="rId2" ref="L4" tooltip=""/>
+    <hyperlink r:id="rId3" ref="L5"/>
+    <hyperlink r:id="rId4" ref="L6"/>
+    <hyperlink r:id="rId5" ref="L7" tooltip=""/>
+    <hyperlink r:id="rId6" ref="K9"/>
+    <hyperlink r:id="rId7" ref="L9"/>
+    <hyperlink r:id="rId8" ref="K10"/>
+    <hyperlink r:id="rId9" ref="L10"/>
+    <hyperlink r:id="rId10" ref="L11"/>
+    <hyperlink r:id="rId11" ref="L13"/>
+    <hyperlink r:id="rId12" ref="L14"/>
+    <hyperlink r:id="rId13" ref="L15"/>
+    <hyperlink r:id="rId14" ref="L16"/>
+    <hyperlink r:id="rId15" ref="L17"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -4534,7 +4633,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>25</v>
@@ -4593,39 +4692,39 @@
         <f>PROPER(I1)</f>
         <v>Program</v>
       </c>
-      <c r="J2" s="140" t="str">
+      <c r="J2" s="144" t="str">
         <f>PROPER(J1)</f>
         <v>Subjects</v>
       </c>
     </row>
     <row r="3" ht="34.5" customHeight="1">
-      <c r="A3" s="141" t="s">
-        <v>392</v>
-      </c>
-      <c r="B3" s="142" t="s">
-        <v>393</v>
-      </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="143" t="s">
-        <v>394</v>
-      </c>
-      <c r="F3" s="145" t="s">
-        <v>395</v>
-      </c>
-      <c r="G3" s="146" t="s">
-        <v>396</v>
-      </c>
-      <c r="H3" s="147" t="str">
+      <c r="A3" s="145" t="s">
+        <v>402</v>
+      </c>
+      <c r="B3" s="146" t="s">
+        <v>403</v>
+      </c>
+      <c r="C3" s="147"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="147" t="s">
+        <v>404</v>
+      </c>
+      <c r="F3" s="149" t="s">
+        <v>405</v>
+      </c>
+      <c r="G3" s="150" t="s">
+        <v>406</v>
+      </c>
+      <c r="H3" s="151" t="str">
         <f>users!A4</f>
         <v>teacher01</v>
       </c>
-      <c r="I3" s="148" t="str">
+      <c r="I3" s="152" t="str">
         <f>ap_programs!A5</f>
         <v>programB</v>
       </c>
-      <c r="J3" s="149" t="s">
-        <v>397</v>
+      <c r="J3" s="153" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="4"/>
@@ -4661,61 +4760,61 @@
     <col customWidth="1" min="2" max="2" width="15.8515625"/>
     <col customWidth="1" min="3" max="3" width="10.00390625"/>
     <col bestFit="1" min="4" max="4" width="8.50390625"/>
-    <col bestFit="1" min="5" max="5" style="150" width="17.3515625"/>
+    <col bestFit="1" min="5" max="5" style="154" width="17.3515625"/>
     <col bestFit="1" min="6" max="6" width="11.28125"/>
     <col customWidth="1" min="7" max="7" width="15.57421875"/>
     <col customWidth="1" min="8" max="8" width="69.57421875"/>
-    <col bestFit="1" min="9" max="9" style="151" width="13.8515625"/>
+    <col bestFit="1" min="9" max="9" style="155" width="13.8515625"/>
     <col customWidth="1" min="10" max="10" width="73.140625"/>
-    <col bestFit="1" min="11" max="11" style="151" width="15.2109375"/>
+    <col bestFit="1" min="11" max="11" style="155" width="15.2109375"/>
     <col bestFit="1" min="12" max="12" width="9.921875"/>
     <col customWidth="1" min="13" max="13" width="114.28125"/>
-    <col customWidth="1" min="14" max="14" style="151" width="23.8515625"/>
+    <col customWidth="1" min="14" max="14" style="155" width="23.8515625"/>
     <col bestFit="1" min="15" max="15" width="2.78125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="135" t="s">
-        <v>398</v>
-      </c>
-      <c r="C1" s="135" t="s">
+      <c r="B1" s="136" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1" s="136" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="135" t="s">
-        <v>399</v>
-      </c>
-      <c r="E1" s="135" t="s">
-        <v>400</v>
-      </c>
-      <c r="F1" s="135" t="s">
-        <v>401</v>
-      </c>
-      <c r="G1" s="152" t="s">
+      <c r="D1" s="136" t="s">
+        <v>409</v>
+      </c>
+      <c r="E1" s="136" t="s">
+        <v>410</v>
+      </c>
+      <c r="F1" s="136" t="s">
+        <v>411</v>
+      </c>
+      <c r="G1" s="156" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="135" t="s">
-        <v>402</v>
-      </c>
-      <c r="I1" s="135" t="s">
-        <v>403</v>
-      </c>
-      <c r="J1" s="135" t="s">
-        <v>404</v>
-      </c>
-      <c r="K1" s="135" t="s">
-        <v>405</v>
-      </c>
-      <c r="L1" s="135" t="s">
-        <v>406</v>
-      </c>
-      <c r="M1" s="135" t="s">
-        <v>407</v>
-      </c>
-      <c r="N1" s="135" t="s">
-        <v>408</v>
+      <c r="H1" s="136" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" s="136" t="s">
+        <v>413</v>
+      </c>
+      <c r="J1" s="136" t="s">
+        <v>414</v>
+      </c>
+      <c r="K1" s="136" t="s">
+        <v>415</v>
+      </c>
+      <c r="L1" s="136" t="s">
+        <v>416</v>
+      </c>
+      <c r="M1" s="136" t="s">
+        <v>417</v>
+      </c>
+      <c r="N1" s="136" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -4723,884 +4822,884 @@
         <v>27</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C2" s="105" t="s">
         <v>253</v>
       </c>
       <c r="D2" s="105" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="G2" s="123" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="153" t="s">
-        <v>413</v>
+      <c r="H2" s="157" t="s">
+        <v>423</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="J2" s="123" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="K2" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="L2" s="105" t="s">
         <v>416</v>
       </c>
-      <c r="L2" s="105" t="s">
-        <v>406</v>
-      </c>
       <c r="M2" s="123" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" ht="114">
-      <c r="A3" s="154" t="str">
+      <c r="A3" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O3&lt;10,"0",""),O3)</f>
         <v>q01</v>
       </c>
-      <c r="B3" s="155" t="str">
+      <c r="B3" s="159" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
-      <c r="C3" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150" t="s">
-        <v>420</v>
-      </c>
-      <c r="F3" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G3" s="156" t="s">
-        <v>422</v>
-      </c>
-      <c r="H3" s="157" t="s">
-        <v>423</v>
-      </c>
-      <c r="I3" s="150"/>
-      <c r="J3" s="157" t="s">
-        <v>424</v>
-      </c>
-      <c r="K3" s="151"/>
-      <c r="L3" s="150">
+      <c r="C3" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154" t="s">
+        <v>430</v>
+      </c>
+      <c r="F3" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G3" s="160" t="s">
+        <v>432</v>
+      </c>
+      <c r="H3" s="161" t="s">
+        <v>433</v>
+      </c>
+      <c r="I3" s="154"/>
+      <c r="J3" s="161" t="s">
+        <v>434</v>
+      </c>
+      <c r="K3" s="155"/>
+      <c r="L3" s="154">
         <v>1</v>
       </c>
-      <c r="M3" s="157" t="s">
-        <v>425</v>
-      </c>
-      <c r="N3" s="150"/>
-      <c r="O3" s="158">
+      <c r="M3" s="161" t="s">
+        <v>435</v>
+      </c>
+      <c r="N3" s="154"/>
+      <c r="O3" s="162">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="199.5">
-      <c r="A4" s="154" t="str">
+      <c r="A4" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O4&lt;10,"0",""),O4)</f>
         <v>q02</v>
       </c>
-      <c r="B4" s="147" t="str">
+      <c r="B4" s="151" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
-      <c r="C4" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F4" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G4" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H4" s="157" t="s">
-        <v>428</v>
-      </c>
-      <c r="I4" s="150"/>
-      <c r="J4" s="157" t="s">
+      <c r="C4" s="154" t="s">
         <v>429</v>
       </c>
-      <c r="K4" s="150"/>
-      <c r="L4" s="150">
+      <c r="D4" s="154"/>
+      <c r="E4" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F4" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G4" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H4" s="161" t="s">
+        <v>438</v>
+      </c>
+      <c r="I4" s="154"/>
+      <c r="J4" s="161" t="s">
+        <v>439</v>
+      </c>
+      <c r="K4" s="154"/>
+      <c r="L4" s="154">
         <v>4</v>
       </c>
-      <c r="M4" s="157" t="s">
-        <v>430</v>
-      </c>
-      <c r="N4" s="150"/>
-      <c r="O4" s="158">
+      <c r="M4" s="161" t="s">
+        <v>440</v>
+      </c>
+      <c r="N4" s="154"/>
+      <c r="O4" s="162">
         <f>O3+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="114">
-      <c r="A5" s="154" t="str">
+      <c r="A5" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O5&lt;10,"0",""),O5)</f>
         <v>q03</v>
       </c>
-      <c r="B5" s="147" t="str">
+      <c r="B5" s="151" t="str">
         <f>B4</f>
         <v>qbank01</v>
       </c>
-      <c r="C5" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D5" s="150"/>
-      <c r="E5" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F5" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G5" s="156" t="s">
+      <c r="C5" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F5" s="154" t="s">
         <v>431</v>
       </c>
-      <c r="H5" s="157" t="s">
-        <v>432</v>
-      </c>
-      <c r="I5" s="150"/>
-      <c r="J5" s="157" t="s">
-        <v>433</v>
-      </c>
-      <c r="K5" s="150"/>
-      <c r="L5" s="150">
+      <c r="G5" s="160" t="s">
+        <v>441</v>
+      </c>
+      <c r="H5" s="161" t="s">
+        <v>442</v>
+      </c>
+      <c r="I5" s="154"/>
+      <c r="J5" s="161" t="s">
+        <v>443</v>
+      </c>
+      <c r="K5" s="154"/>
+      <c r="L5" s="154">
         <v>3</v>
       </c>
-      <c r="M5" s="157" t="s">
-        <v>434</v>
-      </c>
-      <c r="N5" s="150"/>
-      <c r="O5" s="158">
+      <c r="M5" s="161" t="s">
+        <v>444</v>
+      </c>
+      <c r="N5" s="154"/>
+      <c r="O5" s="162">
         <f>O4+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="156.75">
-      <c r="A6" s="154" t="str">
+      <c r="A6" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O6&lt;10,"0",""),O6)</f>
         <v>q04</v>
       </c>
-      <c r="B6" s="147" t="str">
+      <c r="B6" s="151" t="str">
         <f>B5</f>
         <v>qbank01</v>
       </c>
-      <c r="C6" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D6" s="150"/>
-      <c r="E6" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F6" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G6" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H6" s="157" t="s">
-        <v>435</v>
-      </c>
-      <c r="I6" s="150"/>
-      <c r="J6" s="157" t="s">
+      <c r="C6" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154" t="s">
         <v>436</v>
       </c>
-      <c r="K6" s="150"/>
-      <c r="L6" s="150">
+      <c r="F6" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G6" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H6" s="161" t="s">
+        <v>445</v>
+      </c>
+      <c r="I6" s="154"/>
+      <c r="J6" s="161" t="s">
+        <v>446</v>
+      </c>
+      <c r="K6" s="154"/>
+      <c r="L6" s="154">
         <v>2</v>
       </c>
-      <c r="M6" s="157" t="s">
-        <v>437</v>
-      </c>
-      <c r="N6" s="150"/>
-      <c r="O6" s="158">
+      <c r="M6" s="161" t="s">
+        <v>447</v>
+      </c>
+      <c r="N6" s="154"/>
+      <c r="O6" s="162">
         <f>O5+1</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="71.25">
-      <c r="A7" s="154" t="str">
+      <c r="A7" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O7&lt;10,"0",""),O7)</f>
         <v>q05</v>
       </c>
-      <c r="B7" s="147" t="str">
+      <c r="B7" s="151" t="str">
         <f>B6</f>
         <v>qbank01</v>
       </c>
-      <c r="C7" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D7" s="150"/>
-      <c r="E7" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F7" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G7" s="156" t="s">
-        <v>438</v>
-      </c>
-      <c r="H7" s="157" t="s">
-        <v>439</v>
-      </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="157" t="s">
-        <v>440</v>
-      </c>
-      <c r="K7" s="150"/>
-      <c r="L7" s="150">
+      <c r="C7" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D7" s="154"/>
+      <c r="E7" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F7" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G7" s="160" t="s">
+        <v>448</v>
+      </c>
+      <c r="H7" s="161" t="s">
+        <v>449</v>
+      </c>
+      <c r="I7" s="154"/>
+      <c r="J7" s="161" t="s">
+        <v>450</v>
+      </c>
+      <c r="K7" s="154"/>
+      <c r="L7" s="154">
         <v>1</v>
       </c>
-      <c r="M7" s="157" t="s">
-        <v>441</v>
-      </c>
-      <c r="N7" s="150"/>
-      <c r="O7" s="158">
+      <c r="M7" s="161" t="s">
+        <v>451</v>
+      </c>
+      <c r="N7" s="154"/>
+      <c r="O7" s="162">
         <f>O6+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="242.25">
-      <c r="A8" s="154" t="str">
+      <c r="A8" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O8&lt;10,"0",""),O8)</f>
         <v>q06</v>
       </c>
-      <c r="B8" s="147" t="str">
+      <c r="B8" s="151" t="str">
         <f>B7</f>
         <v>qbank01</v>
       </c>
-      <c r="C8" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D8" s="150"/>
-      <c r="E8" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F8" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G8" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H8" s="157" t="s">
-        <v>442</v>
-      </c>
-      <c r="I8" s="151"/>
-      <c r="J8" s="157" t="s">
-        <v>443</v>
-      </c>
-      <c r="K8" s="150"/>
-      <c r="L8" s="150">
+      <c r="C8" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D8" s="154"/>
+      <c r="E8" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F8" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G8" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H8" s="161" t="s">
+        <v>452</v>
+      </c>
+      <c r="I8" s="155"/>
+      <c r="J8" s="161" t="s">
+        <v>453</v>
+      </c>
+      <c r="K8" s="154"/>
+      <c r="L8" s="154">
         <v>2</v>
       </c>
-      <c r="M8" s="157" t="s">
-        <v>444</v>
-      </c>
-      <c r="N8" s="159"/>
-      <c r="O8" s="158">
+      <c r="M8" s="161" t="s">
+        <v>454</v>
+      </c>
+      <c r="N8" s="163"/>
+      <c r="O8" s="162">
         <f>O7+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="242.25">
-      <c r="A9" s="154" t="str">
+      <c r="A9" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O9&lt;10,"0",""),O9)</f>
         <v>q07</v>
       </c>
-      <c r="B9" s="147" t="str">
+      <c r="B9" s="151" t="str">
         <f>B8</f>
         <v>qbank01</v>
       </c>
-      <c r="C9" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D9" s="150"/>
-      <c r="E9" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F9" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G9" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H9" s="157" t="s">
-        <v>445</v>
-      </c>
-      <c r="I9" s="151"/>
-      <c r="J9" s="157" t="s">
-        <v>446</v>
-      </c>
-      <c r="K9" s="150"/>
-      <c r="L9" s="150">
+      <c r="C9" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F9" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G9" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H9" s="161" t="s">
+        <v>455</v>
+      </c>
+      <c r="I9" s="155"/>
+      <c r="J9" s="161" t="s">
+        <v>456</v>
+      </c>
+      <c r="K9" s="154"/>
+      <c r="L9" s="154">
         <v>3</v>
       </c>
-      <c r="M9" s="157" t="s">
-        <v>447</v>
-      </c>
-      <c r="N9" s="150"/>
-      <c r="O9" s="158">
+      <c r="M9" s="161" t="s">
+        <v>457</v>
+      </c>
+      <c r="N9" s="154"/>
+      <c r="O9" s="162">
         <f>O8+1</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="356.25">
-      <c r="A10" s="154" t="str">
+      <c r="A10" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O10&lt;10,"0",""),O10)</f>
         <v>q08</v>
       </c>
-      <c r="B10" s="147" t="str">
+      <c r="B10" s="151" t="str">
         <f>B9</f>
         <v>qbank01</v>
       </c>
-      <c r="C10" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D10" s="150"/>
-      <c r="E10" s="150" t="s">
-        <v>420</v>
-      </c>
-      <c r="F10" s="150" t="s">
-        <v>448</v>
-      </c>
-      <c r="G10" s="156" t="s">
-        <v>431</v>
-      </c>
-      <c r="H10" s="157" t="s">
-        <v>449</v>
-      </c>
-      <c r="I10" s="150"/>
-      <c r="J10" s="150"/>
-      <c r="K10" s="160" t="s">
-        <v>450</v>
-      </c>
-      <c r="L10" s="150">
+      <c r="C10" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D10" s="154"/>
+      <c r="E10" s="154" t="s">
+        <v>430</v>
+      </c>
+      <c r="F10" s="154" t="s">
+        <v>458</v>
+      </c>
+      <c r="G10" s="160" t="s">
+        <v>441</v>
+      </c>
+      <c r="H10" s="161" t="s">
+        <v>459</v>
+      </c>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="164" t="s">
+        <v>460</v>
+      </c>
+      <c r="L10" s="154">
         <v>2</v>
       </c>
-      <c r="M10" s="157" t="s">
-        <v>451</v>
-      </c>
-      <c r="N10" s="150"/>
-      <c r="O10" s="158">
+      <c r="M10" s="161" t="s">
+        <v>461</v>
+      </c>
+      <c r="N10" s="154"/>
+      <c r="O10" s="162">
         <f>O9+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="11" ht="185.25">
-      <c r="A11" s="154" t="str">
+      <c r="A11" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O11&lt;10,"0",""),O11)</f>
         <v>q09</v>
       </c>
-      <c r="B11" s="147" t="str">
+      <c r="B11" s="151" t="str">
         <f>B10</f>
         <v>qbank01</v>
       </c>
-      <c r="C11" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150" t="s">
-        <v>420</v>
-      </c>
-      <c r="F11" s="150" t="s">
-        <v>448</v>
-      </c>
-      <c r="G11" s="156" t="s">
-        <v>431</v>
-      </c>
-      <c r="H11" s="157" t="s">
-        <v>452</v>
-      </c>
-      <c r="I11" s="160" t="s">
-        <v>453</v>
-      </c>
-      <c r="J11" s="157" t="s">
-        <v>454</v>
-      </c>
-      <c r="K11" s="150"/>
-      <c r="L11" s="150">
+      <c r="C11" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D11" s="154"/>
+      <c r="E11" s="154" t="s">
+        <v>430</v>
+      </c>
+      <c r="F11" s="154" t="s">
+        <v>458</v>
+      </c>
+      <c r="G11" s="160" t="s">
+        <v>441</v>
+      </c>
+      <c r="H11" s="161" t="s">
+        <v>462</v>
+      </c>
+      <c r="I11" s="164" t="s">
+        <v>463</v>
+      </c>
+      <c r="J11" s="161" t="s">
+        <v>464</v>
+      </c>
+      <c r="K11" s="154"/>
+      <c r="L11" s="154">
         <v>1</v>
       </c>
-      <c r="M11" s="157" t="s">
-        <v>455</v>
-      </c>
-      <c r="N11" s="150"/>
-      <c r="O11" s="158">
+      <c r="M11" s="161" t="s">
+        <v>465</v>
+      </c>
+      <c r="N11" s="154"/>
+      <c r="O11" s="162">
         <f>O10+1</f>
         <v>9</v>
       </c>
     </row>
     <row r="12" ht="185.25">
-      <c r="A12" s="154" t="str">
+      <c r="A12" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O12&lt;10,"0",""),O12)</f>
         <v>q10</v>
       </c>
-      <c r="B12" s="147" t="str">
+      <c r="B12" s="151" t="str">
         <f>B11</f>
         <v>qbank01</v>
       </c>
-      <c r="C12" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D12" s="150"/>
-      <c r="E12" s="150" t="s">
-        <v>456</v>
-      </c>
-      <c r="F12" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G12" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H12" s="157" t="s">
-        <v>457</v>
-      </c>
-      <c r="I12" s="150"/>
-      <c r="J12" s="161" t="s">
-        <v>458</v>
-      </c>
-      <c r="K12" s="150"/>
-      <c r="L12" s="150">
+      <c r="C12" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D12" s="154"/>
+      <c r="E12" s="154" t="s">
+        <v>466</v>
+      </c>
+      <c r="F12" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G12" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H12" s="161" t="s">
+        <v>467</v>
+      </c>
+      <c r="I12" s="154"/>
+      <c r="J12" s="165" t="s">
+        <v>468</v>
+      </c>
+      <c r="K12" s="154"/>
+      <c r="L12" s="154">
         <v>4</v>
       </c>
-      <c r="M12" s="157" t="s">
-        <v>459</v>
-      </c>
-      <c r="N12" s="150"/>
-      <c r="O12" s="158">
+      <c r="M12" s="161" t="s">
+        <v>469</v>
+      </c>
+      <c r="N12" s="154"/>
+      <c r="O12" s="162">
         <f>O11+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="185.25">
-      <c r="A13" s="154" t="str">
+      <c r="A13" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O13&lt;10,"0",""),O13)</f>
         <v>q11</v>
       </c>
-      <c r="B13" s="147" t="str">
+      <c r="B13" s="151" t="str">
         <f>B12</f>
         <v>qbank01</v>
       </c>
-      <c r="C13" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D13" s="150"/>
-      <c r="E13" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F13" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G13" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H13" s="157" t="s">
-        <v>460</v>
-      </c>
-      <c r="I13" s="150"/>
-      <c r="J13" s="157" t="s">
-        <v>461</v>
-      </c>
-      <c r="K13" s="150"/>
-      <c r="L13" s="150">
+      <c r="C13" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D13" s="154"/>
+      <c r="E13" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F13" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G13" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H13" s="161" t="s">
+        <v>470</v>
+      </c>
+      <c r="I13" s="154"/>
+      <c r="J13" s="161" t="s">
+        <v>471</v>
+      </c>
+      <c r="K13" s="154"/>
+      <c r="L13" s="154">
         <v>3</v>
       </c>
-      <c r="M13" s="157" t="s">
-        <v>462</v>
-      </c>
-      <c r="N13" s="150"/>
-      <c r="O13" s="158">
+      <c r="M13" s="161" t="s">
+        <v>472</v>
+      </c>
+      <c r="N13" s="154"/>
+      <c r="O13" s="162">
         <f>O12+1</f>
         <v>11</v>
       </c>
     </row>
     <row r="14" ht="185.25">
-      <c r="A14" s="154" t="str">
+      <c r="A14" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O14&lt;10,"0",""),O14)</f>
         <v>q12</v>
       </c>
-      <c r="B14" s="147" t="str">
+      <c r="B14" s="151" t="str">
         <f>B13</f>
         <v>qbank01</v>
       </c>
-      <c r="C14" s="150" t="s">
-        <v>419</v>
-      </c>
-      <c r="D14" s="150"/>
-      <c r="E14" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F14" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G14" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H14" s="157" t="s">
-        <v>463</v>
-      </c>
-      <c r="I14" s="150"/>
-      <c r="J14" s="157" t="s">
-        <v>464</v>
-      </c>
-      <c r="K14" s="150"/>
-      <c r="L14" s="150">
+      <c r="C14" s="154" t="s">
+        <v>429</v>
+      </c>
+      <c r="D14" s="154"/>
+      <c r="E14" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F14" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G14" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H14" s="161" t="s">
+        <v>473</v>
+      </c>
+      <c r="I14" s="154"/>
+      <c r="J14" s="161" t="s">
+        <v>474</v>
+      </c>
+      <c r="K14" s="154"/>
+      <c r="L14" s="154">
         <v>1</v>
       </c>
-      <c r="M14" s="157" t="s">
-        <v>465</v>
-      </c>
-      <c r="N14" s="150"/>
-      <c r="O14" s="158">
+      <c r="M14" s="161" t="s">
+        <v>475</v>
+      </c>
+      <c r="N14" s="154"/>
+      <c r="O14" s="162">
         <f>O13+1</f>
         <v>12</v>
       </c>
     </row>
     <row r="15" ht="114">
-      <c r="A15" s="154" t="str">
+      <c r="A15" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O15&lt;10,"0",""),O15)</f>
         <v>q13</v>
       </c>
-      <c r="B15" s="147" t="str">
+      <c r="B15" s="151" t="str">
         <f>B14</f>
         <v>qbank01</v>
       </c>
-      <c r="C15" s="150" t="s">
-        <v>419</v>
+      <c r="C15" s="154" t="s">
+        <v>429</v>
       </c>
       <c r="D15" s="18"/>
-      <c r="E15" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F15" s="150" t="s">
-        <v>448</v>
-      </c>
-      <c r="G15" s="156" t="s">
-        <v>466</v>
-      </c>
-      <c r="H15" s="157" t="s">
-        <v>467</v>
-      </c>
-      <c r="I15" s="150" t="s">
-        <v>468</v>
-      </c>
-      <c r="J15" s="157" t="s">
-        <v>469</v>
-      </c>
-      <c r="K15" s="151"/>
-      <c r="L15" s="150">
+      <c r="E15" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F15" s="154" t="s">
+        <v>458</v>
+      </c>
+      <c r="G15" s="160" t="s">
+        <v>476</v>
+      </c>
+      <c r="H15" s="161" t="s">
+        <v>477</v>
+      </c>
+      <c r="I15" s="154" t="s">
+        <v>478</v>
+      </c>
+      <c r="J15" s="161" t="s">
+        <v>479</v>
+      </c>
+      <c r="K15" s="155"/>
+      <c r="L15" s="154">
         <v>2</v>
       </c>
-      <c r="M15" s="157" t="s">
-        <v>470</v>
-      </c>
-      <c r="N15" s="150"/>
-      <c r="O15" s="158">
+      <c r="M15" s="161" t="s">
+        <v>480</v>
+      </c>
+      <c r="N15" s="154"/>
+      <c r="O15" s="162">
         <f>O14+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="16" ht="114">
-      <c r="A16" s="154" t="str">
+      <c r="A16" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O16&lt;10,"0",""),O16)</f>
         <v>q14</v>
       </c>
-      <c r="B16" s="147" t="str">
+      <c r="B16" s="151" t="str">
         <f>B15</f>
         <v>qbank01</v>
       </c>
-      <c r="C16" s="150" t="s">
-        <v>419</v>
+      <c r="C16" s="154" t="s">
+        <v>429</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F16" s="150" t="s">
-        <v>448</v>
-      </c>
-      <c r="G16" s="156" t="s">
-        <v>466</v>
-      </c>
-      <c r="H16" s="157" t="s">
-        <v>471</v>
-      </c>
-      <c r="I16" s="150" t="s">
-        <v>468</v>
-      </c>
-      <c r="J16" s="157" t="s">
-        <v>472</v>
-      </c>
-      <c r="K16" s="151"/>
-      <c r="L16" s="150">
+      <c r="E16" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F16" s="154" t="s">
+        <v>458</v>
+      </c>
+      <c r="G16" s="160" t="s">
+        <v>476</v>
+      </c>
+      <c r="H16" s="161" t="s">
+        <v>481</v>
+      </c>
+      <c r="I16" s="154" t="s">
+        <v>478</v>
+      </c>
+      <c r="J16" s="161" t="s">
+        <v>482</v>
+      </c>
+      <c r="K16" s="155"/>
+      <c r="L16" s="154">
         <v>1</v>
       </c>
-      <c r="M16" s="157" t="s">
-        <v>473</v>
-      </c>
-      <c r="N16" s="159"/>
-      <c r="O16" s="158">
+      <c r="M16" s="161" t="s">
+        <v>483</v>
+      </c>
+      <c r="N16" s="163"/>
+      <c r="O16" s="162">
         <f>O15+1</f>
         <v>14</v>
       </c>
     </row>
     <row r="17" ht="142.5">
-      <c r="A17" s="154" t="str">
+      <c r="A17" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O17&lt;10,"0",""),O17)</f>
         <v>q15</v>
       </c>
-      <c r="B17" s="147" t="str">
+      <c r="B17" s="151" t="str">
         <f>B16</f>
         <v>qbank01</v>
       </c>
-      <c r="C17" s="150" t="s">
-        <v>419</v>
+      <c r="C17" s="154" t="s">
+        <v>429</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F17" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G17" s="156" t="s">
-        <v>474</v>
-      </c>
-      <c r="H17" s="157" t="s">
-        <v>475</v>
-      </c>
-      <c r="I17" s="151"/>
-      <c r="J17" s="157" t="s">
-        <v>476</v>
-      </c>
-      <c r="K17" s="151"/>
-      <c r="L17" s="150">
+      <c r="E17" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F17" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G17" s="160" t="s">
+        <v>484</v>
+      </c>
+      <c r="H17" s="161" t="s">
+        <v>485</v>
+      </c>
+      <c r="I17" s="155"/>
+      <c r="J17" s="161" t="s">
+        <v>486</v>
+      </c>
+      <c r="K17" s="155"/>
+      <c r="L17" s="154">
         <v>2</v>
       </c>
-      <c r="M17" s="157" t="s">
-        <v>477</v>
-      </c>
-      <c r="N17" s="159"/>
-      <c r="O17" s="158">
+      <c r="M17" s="161" t="s">
+        <v>487</v>
+      </c>
+      <c r="N17" s="163"/>
+      <c r="O17" s="162">
         <f>O16+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="242.25">
-      <c r="A18" s="154" t="str">
+      <c r="A18" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O18&lt;10,"0",""),O18)</f>
         <v>q16</v>
       </c>
-      <c r="B18" s="147" t="str">
+      <c r="B18" s="151" t="str">
         <f>B17</f>
         <v>qbank01</v>
       </c>
-      <c r="C18" s="150" t="s">
-        <v>419</v>
+      <c r="C18" s="154" t="s">
+        <v>429</v>
       </c>
       <c r="D18" s="18"/>
-      <c r="E18" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F18" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G18" s="156" t="s">
-        <v>466</v>
-      </c>
-      <c r="H18" s="157" t="s">
-        <v>478</v>
-      </c>
-      <c r="I18" s="151"/>
-      <c r="J18" s="157" t="s">
-        <v>479</v>
-      </c>
-      <c r="K18" s="151"/>
-      <c r="L18" s="150">
+      <c r="E18" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F18" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G18" s="160" t="s">
+        <v>476</v>
+      </c>
+      <c r="H18" s="161" t="s">
+        <v>488</v>
+      </c>
+      <c r="I18" s="155"/>
+      <c r="J18" s="161" t="s">
+        <v>489</v>
+      </c>
+      <c r="K18" s="155"/>
+      <c r="L18" s="154">
         <v>1</v>
       </c>
-      <c r="M18" s="157" t="s">
-        <v>480</v>
-      </c>
-      <c r="N18" s="159"/>
-      <c r="O18" s="158">
+      <c r="M18" s="161" t="s">
+        <v>490</v>
+      </c>
+      <c r="N18" s="163"/>
+      <c r="O18" s="162">
         <f>O17+1</f>
         <v>16</v>
       </c>
     </row>
     <row r="19" ht="213.75">
-      <c r="A19" s="154" t="str">
+      <c r="A19" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O19&lt;10,"0",""),O19)</f>
         <v>q17</v>
       </c>
-      <c r="B19" s="147" t="str">
+      <c r="B19" s="151" t="str">
         <f>B18</f>
         <v>qbank01</v>
       </c>
-      <c r="C19" s="150" t="s">
-        <v>419</v>
+      <c r="C19" s="154" t="s">
+        <v>429</v>
       </c>
       <c r="D19" s="18"/>
-      <c r="E19" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F19" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G19" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H19" s="157" t="s">
-        <v>481</v>
-      </c>
-      <c r="I19" s="151"/>
-      <c r="J19" s="157" t="s">
-        <v>482</v>
-      </c>
-      <c r="K19" s="151"/>
-      <c r="L19" s="150">
+      <c r="E19" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F19" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G19" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H19" s="161" t="s">
+        <v>491</v>
+      </c>
+      <c r="I19" s="155"/>
+      <c r="J19" s="161" t="s">
+        <v>492</v>
+      </c>
+      <c r="K19" s="155"/>
+      <c r="L19" s="154">
         <v>3</v>
       </c>
-      <c r="M19" s="157" t="s">
-        <v>483</v>
-      </c>
-      <c r="N19" s="159"/>
-      <c r="O19" s="158">
+      <c r="M19" s="161" t="s">
+        <v>493</v>
+      </c>
+      <c r="N19" s="163"/>
+      <c r="O19" s="162">
         <f>O18+1</f>
         <v>17</v>
       </c>
     </row>
     <row r="20" ht="242.25">
-      <c r="A20" s="154" t="str">
+      <c r="A20" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O20&lt;10,"0",""),O20)</f>
         <v>q18</v>
       </c>
-      <c r="B20" s="147" t="str">
+      <c r="B20" s="151" t="str">
         <f>B19</f>
         <v>qbank01</v>
       </c>
-      <c r="C20" s="150" t="s">
-        <v>419</v>
+      <c r="C20" s="154" t="s">
+        <v>429</v>
       </c>
       <c r="D20" s="18"/>
-      <c r="E20" s="150" t="s">
-        <v>426</v>
-      </c>
-      <c r="F20" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G20" s="156" t="s">
-        <v>427</v>
-      </c>
-      <c r="H20" s="157" t="s">
-        <v>484</v>
-      </c>
-      <c r="I20" s="151"/>
-      <c r="J20" s="157" t="s">
-        <v>485</v>
-      </c>
-      <c r="K20" s="151"/>
-      <c r="L20" s="150">
+      <c r="E20" s="154" t="s">
+        <v>436</v>
+      </c>
+      <c r="F20" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G20" s="160" t="s">
+        <v>437</v>
+      </c>
+      <c r="H20" s="161" t="s">
+        <v>494</v>
+      </c>
+      <c r="I20" s="155"/>
+      <c r="J20" s="161" t="s">
+        <v>495</v>
+      </c>
+      <c r="K20" s="155"/>
+      <c r="L20" s="154">
         <v>4</v>
       </c>
-      <c r="M20" s="157" t="s">
-        <v>486</v>
-      </c>
-      <c r="N20" s="159"/>
-      <c r="O20" s="158">
+      <c r="M20" s="161" t="s">
+        <v>496</v>
+      </c>
+      <c r="N20" s="163"/>
+      <c r="O20" s="162">
         <f>O19+1</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" ht="409.5">
-      <c r="A21" s="154" t="str">
+      <c r="A21" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O21&lt;10,"0",""),O21)</f>
         <v>q19</v>
       </c>
-      <c r="B21" s="147" t="str">
+      <c r="B21" s="151" t="str">
         <f>B20</f>
         <v>qbank01</v>
       </c>
-      <c r="C21" s="150" t="s">
-        <v>419</v>
+      <c r="C21" s="154" t="s">
+        <v>429</v>
       </c>
       <c r="D21" s="18"/>
-      <c r="E21" s="150" t="s">
-        <v>456</v>
-      </c>
-      <c r="F21" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="G21" s="156" t="s">
-        <v>474</v>
-      </c>
-      <c r="H21" s="157" t="s">
-        <v>487</v>
-      </c>
-      <c r="I21" s="150"/>
-      <c r="J21" s="157" t="s">
-        <v>488</v>
-      </c>
-      <c r="K21" s="150"/>
-      <c r="L21" s="150">
+      <c r="E21" s="154" t="s">
+        <v>466</v>
+      </c>
+      <c r="F21" s="154" t="s">
+        <v>431</v>
+      </c>
+      <c r="G21" s="160" t="s">
+        <v>484</v>
+      </c>
+      <c r="H21" s="161" t="s">
+        <v>497</v>
+      </c>
+      <c r="I21" s="154"/>
+      <c r="J21" s="161" t="s">
+        <v>498</v>
+      </c>
+      <c r="K21" s="154"/>
+      <c r="L21" s="154">
         <v>4</v>
       </c>
-      <c r="M21" s="157" t="s">
-        <v>489</v>
-      </c>
-      <c r="N21" s="150"/>
-      <c r="O21" s="158">
+      <c r="M21" s="161" t="s">
+        <v>499</v>
+      </c>
+      <c r="N21" s="154"/>
+      <c r="O21" s="162">
         <f>O20+1</f>
         <v>19</v>
       </c>
     </row>
     <row r="22" ht="114">
-      <c r="A22" s="154" t="str">
+      <c r="A22" s="158" t="str">
         <f>_xlfn.CONCAT("q",IF(O22&lt;10,"0",""),O22)</f>
         <v>q20</v>
       </c>
-      <c r="B22" s="147" t="str">
+      <c r="B22" s="151" t="str">
         <f>B21</f>
         <v>qbank01</v>
       </c>
-      <c r="C22" s="150" t="s">
-        <v>490</v>
+      <c r="C22" s="154" t="s">
+        <v>500</v>
       </c>
       <c r="D22" s="18"/>
-      <c r="E22" s="150" t="s">
-        <v>420</v>
+      <c r="E22" s="154" t="s">
+        <v>430</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="161" t="s">
-        <v>438</v>
-      </c>
-      <c r="H22" s="157" t="s">
-        <v>491</v>
-      </c>
-      <c r="I22" s="160" t="s">
-        <v>492</v>
-      </c>
-      <c r="J22" s="157" t="s">
-        <v>493</v>
-      </c>
-      <c r="K22" s="151"/>
-      <c r="L22" s="162"/>
-      <c r="M22" s="163"/>
+      <c r="G22" s="165" t="s">
+        <v>448</v>
+      </c>
+      <c r="H22" s="161" t="s">
+        <v>501</v>
+      </c>
+      <c r="I22" s="164" t="s">
+        <v>502</v>
+      </c>
+      <c r="J22" s="161" t="s">
+        <v>503</v>
+      </c>
+      <c r="K22" s="155"/>
+      <c r="L22" s="166"/>
+      <c r="M22" s="167"/>
       <c r="N22" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="O22" s="164">
+        <v>504</v>
+      </c>
+      <c r="O22" s="168">
         <f>O21+1</f>
         <v>20</v>
       </c>
@@ -6327,10 +6426,18 @@
       <c r="Q7" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="R7" s="68"/>
-      <c r="S7" s="68"/>
-      <c r="T7" s="68"/>
-      <c r="U7" s="68"/>
+      <c r="R7" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="S7" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="T7" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="U7" s="68" t="s">
+        <v>115</v>
+      </c>
       <c r="V7" s="68" t="s">
         <v>115</v>
       </c>
@@ -6420,11 +6527,11 @@
       <c r="O8" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="P8" s="67" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q8" s="67" t="s">
-        <v>115</v>
+      <c r="P8" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q8" s="70" t="s">
+        <v>118</v>
       </c>
       <c r="R8" s="68"/>
       <c r="S8" s="67"/>
@@ -7456,37 +7563,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00EE00CE-003C-4677-93EC-009800000064}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0083007F-00C2-41D1-8B94-00B400940039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000A007C-00E8-417B-AF7B-0036003100C4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A3005E-0046-4DEF-94F8-00AF00F000B8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B70082-00BF-439A-B584-00AD00B90075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FA008A-000E-4FCE-8AD2-004500530035}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001A001A-00E4-4357-9C12-0010003000B4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F300EB-002F-4026-B579-000500DB006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001A002D-00D6-4A23-98B6-00A500FD002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005C000B-0064-48E6-BA80-002000E000A2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0088005F-00B7-476D-B065-009100E5006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A4009F-008A-4A72-818D-006A0050005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -7637,7 +7744,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E70085-0037-49FC-B39C-008500310008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000500BE-004A-4C84-8127-001700AE00E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -7665,7 +7772,7 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="18.6640625"/>
     <col customWidth="1" min="5" max="5" width="13.6640625"/>
-    <col customWidth="1" min="6" max="6" width="19.5"/>
+    <col customWidth="1" min="6" max="6" width="16.00390625"/>
     <col customWidth="1" min="7" max="7" width="25.1640625"/>
   </cols>
   <sheetData>
@@ -7727,7 +7834,7 @@
         <v>centerA</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>10</v>
@@ -7751,7 +7858,7 @@
         <v>centerB</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>10</v>
@@ -7771,13 +7878,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00460063-00A0-46B3-BF32-0054004A00CF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008200E0-00DF-457B-8D98-00DF007800B1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009F007E-00C0-4928-B826-00DF00F0007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007200BA-0092-4023-B869-00D80004001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -8244,13 +8351,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00DF00F7-0013-4399-AEC1-001B00290012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003E0055-00E6-4F44-BE24-006700E2001B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001A00DC-0089-4289-8755-0088006A0009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0096006A-002A-4027-A95E-002C00640048}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
INIT: MVP-Template questions parser
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="794">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -2183,7 +2183,7 @@
     <t>level</t>
   </si>
   <si>
-    <t>images</t>
+    <t>with_images</t>
   </si>
   <si>
     <t>question</t>
@@ -2198,34 +2198,37 @@
     <t>answer_images</t>
   </si>
   <si>
+    <t>answer_correct</t>
+  </si>
+  <si>
+    <t>answer_feedback</t>
+  </si>
+  <si>
+    <t>answer_feedback_image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question Bank</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with images</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Image</t>
+  </si>
+  <si>
+    <t>Answers</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
     <t xml:space="preserve">Right Answer</t>
-  </si>
-  <si>
-    <t>Feedback_escrito</t>
-  </si>
-  <si>
-    <t>Feedback_imagen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question Bank</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with images</t>
-  </si>
-  <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General Image</t>
-  </si>
-  <si>
-    <t>Answers</t>
-  </si>
-  <si>
-    <t>Images</t>
   </si>
   <si>
     <t xml:space="preserve">Feedback escrito</t>
@@ -2828,7 +2831,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -3165,25 +3168,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="190">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3660,43 +3650,41 @@
     <xf fontId="12" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="12" fillId="4" borderId="29" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="12" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="12" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="12" fillId="4" borderId="29" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="12" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="5" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="12" fillId="5" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="0" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="0" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="13" fillId="0" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="11" fillId="0" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="12" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -3709,29 +3697,31 @@
     <xf fontId="5" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="30" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="12" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="12" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="12" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf fontId="12" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf fontId="16" fillId="0" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf fontId="12" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="12" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="12" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4839,13 +4829,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{005A00E9-0038-49FA-A9FC-001F003000C5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006B002F-00EC-4042-9D42-002A00F40040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003600B8-00C5-4AEF-AF01-00FF009E00DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003C009A-00EE-42FB-96DA-002A00AA0007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -4990,7 +4980,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00560001-0076-4639-8A92-00F100A000F1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D100A0-008A-4BC0-8F92-0017001B0046}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -6161,7 +6151,7 @@
     <col customWidth="1" min="10" max="10" style="153" width="11.140625"/>
     <col customWidth="1" min="11" max="13" style="151" width="25.140625"/>
     <col customWidth="1" min="14" max="14" style="151" width="41.421875"/>
-    <col customWidth="1" min="15" max="15" style="151" width="53.00390625"/>
+    <col customWidth="1" min="15" max="15" style="151" width="66.57421875"/>
     <col customWidth="1" min="16" max="16" style="153" width="11.7109375"/>
     <col bestFit="1" customWidth="1" min="17" max="17" style="153" width="17.203125"/>
     <col customWidth="1" min="18" max="18" style="153" width="8.140625"/>
@@ -6174,8 +6164,8 @@
     <col customWidth="1" min="25" max="25" width="32.00390625"/>
     <col customWidth="1" min="26" max="26" width="59.8515625"/>
     <col customWidth="1" min="27" max="27" width="40.00390625"/>
-    <col customWidth="1" min="28" max="28" width="39.57421875"/>
-    <col customWidth="1" min="29" max="29" width="40.7109375"/>
+    <col customWidth="1" min="28" max="28" width="51.140625"/>
+    <col customWidth="1" min="29" max="29" width="52.28125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6357,7 +6347,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="3" s="151" customFormat="1" ht="202.5">
+    <row r="3" s="151" customFormat="1" ht="162">
       <c r="A3" s="160" t="s">
         <v>608</v>
       </c>
@@ -6376,17 +6366,17 @@
       <c r="F3" s="161" t="s">
         <v>284</v>
       </c>
-      <c r="G3" s="162" t="s">
+      <c r="G3" s="161" t="s">
         <v>613</v>
       </c>
-      <c r="H3" s="163" t="str">
+      <c r="H3" s="162" t="str">
         <f>users!A4</f>
         <v>teacher01</v>
       </c>
-      <c r="I3" s="164" t="s">
+      <c r="I3" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="165" t="s">
+      <c r="J3" s="164" t="s">
         <v>486</v>
       </c>
       <c r="K3" s="143" t="s">
@@ -6445,7 +6435,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="4" s="151" customFormat="1" ht="283.5">
+    <row r="4" s="151" customFormat="1" ht="243">
       <c r="A4" s="160" t="s">
         <v>628</v>
       </c>
@@ -6464,17 +6454,17 @@
       <c r="F4" s="161" t="s">
         <v>633</v>
       </c>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="161" t="s">
         <v>634</v>
       </c>
-      <c r="H4" s="163" t="str">
+      <c r="H4" s="162" t="str">
         <f>H3</f>
         <v>teacher01</v>
       </c>
-      <c r="I4" s="164" t="s">
+      <c r="I4" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="165" t="s">
+      <c r="J4" s="164" t="s">
         <v>486</v>
       </c>
       <c r="K4" s="143" t="s">
@@ -6552,17 +6542,17 @@
       <c r="F5" s="161" t="s">
         <v>651</v>
       </c>
-      <c r="G5" s="162" t="s">
+      <c r="G5" s="165" t="s">
         <v>652</v>
       </c>
-      <c r="H5" s="163" t="str">
+      <c r="H5" s="162" t="str">
         <f>H4</f>
         <v>teacher01</v>
       </c>
-      <c r="I5" s="164" t="s">
+      <c r="I5" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="165" t="s">
+      <c r="J5" s="164" t="s">
         <v>486</v>
       </c>
       <c r="K5" s="143" t="s">
@@ -6615,7 +6605,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="6" s="151" customFormat="1" ht="67.5">
+    <row r="6" s="151" customFormat="1" ht="94.5">
       <c r="A6" s="160" t="s">
         <v>660</v>
       </c>
@@ -6634,17 +6624,17 @@
       <c r="F6" s="161" t="s">
         <v>665</v>
       </c>
-      <c r="G6" s="162" t="s">
+      <c r="G6" s="161" t="s">
         <v>666</v>
       </c>
-      <c r="H6" s="163" t="str">
+      <c r="H6" s="162" t="str">
         <f>H5</f>
         <v>teacher01</v>
       </c>
-      <c r="I6" s="164" t="s">
+      <c r="I6" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="165" t="s">
+      <c r="J6" s="164" t="s">
         <v>486</v>
       </c>
       <c r="K6" s="143" t="s">
@@ -6689,7 +6679,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="7" s="151" customFormat="1" ht="108">
+    <row r="7" s="151" customFormat="1" ht="94.5">
       <c r="A7" s="160" t="s">
         <v>673</v>
       </c>
@@ -6708,17 +6698,17 @@
       <c r="F7" s="161" t="s">
         <v>678</v>
       </c>
-      <c r="G7" s="162" t="s">
+      <c r="G7" s="161" t="s">
         <v>679</v>
       </c>
-      <c r="H7" s="163" t="str">
+      <c r="H7" s="162" t="str">
         <f>H6</f>
         <v>teacher01</v>
       </c>
-      <c r="I7" s="164" t="s">
+      <c r="I7" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="165" t="s">
+      <c r="J7" s="164" t="s">
         <v>486</v>
       </c>
       <c r="K7" s="143" t="s">
@@ -6769,7 +6759,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="8" s="151" customFormat="1" ht="67.5">
+    <row r="8" s="151" customFormat="1" ht="108">
       <c r="A8" s="160" t="s">
         <v>685</v>
       </c>
@@ -6788,17 +6778,17 @@
       <c r="F8" s="161" t="s">
         <v>690</v>
       </c>
-      <c r="G8" s="162" t="s">
+      <c r="G8" s="161" t="s">
         <v>691</v>
       </c>
-      <c r="H8" s="163" t="str">
+      <c r="H8" s="162" t="str">
         <f>H7</f>
         <v>teacher01</v>
       </c>
-      <c r="I8" s="164" t="s">
+      <c r="I8" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="165" t="s">
+      <c r="J8" s="164" t="s">
         <v>486</v>
       </c>
       <c r="K8" s="143" t="s">
@@ -6867,7 +6857,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6954,11 +6944,11 @@
         <v>Subjects</v>
       </c>
     </row>
-    <row r="3" ht="34.5" customHeight="1">
-      <c r="A3" s="167" t="s">
+    <row r="3" s="167" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A3" s="168" t="s">
         <v>696</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="169" t="s">
         <v>697</v>
       </c>
       <c r="C3" s="169"/>
@@ -6969,10 +6959,10 @@
       <c r="F3" s="171" t="s">
         <v>373</v>
       </c>
-      <c r="G3" s="172" t="s">
+      <c r="G3" s="170" t="s">
         <v>699</v>
       </c>
-      <c r="H3" s="163" t="str">
+      <c r="H3" s="172" t="str">
         <f>users!A4</f>
         <v>teacher01</v>
       </c>
@@ -7006,7 +6996,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -7109,13 +7099,13 @@
         <v>718</v>
       </c>
       <c r="L2" s="112" t="s">
-        <v>709</v>
+        <v>719</v>
       </c>
       <c r="M2" s="130" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="3" ht="114">
@@ -7123,39 +7113,39 @@
         <f>_xlfn.CONCAT("q",IF(O3&lt;10,"0",""),O3)</f>
         <v>q01</v>
       </c>
-      <c r="B3" s="180" t="str">
+      <c r="B3" s="164" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
-      <c r="C3" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175" t="s">
+      <c r="C3" s="88" t="s">
         <v>722</v>
       </c>
-      <c r="F3" s="175" t="s">
+      <c r="D3" s="88"/>
+      <c r="E3" s="88" t="s">
         <v>723</v>
       </c>
-      <c r="G3" s="153" t="s">
+      <c r="F3" s="88" t="s">
         <v>724</v>
       </c>
+      <c r="G3" s="180" t="s">
+        <v>725</v>
+      </c>
       <c r="H3" s="181" t="s">
-        <v>725</v>
-      </c>
-      <c r="I3" s="175"/>
+        <v>726</v>
+      </c>
+      <c r="I3" s="88"/>
       <c r="J3" s="181" t="s">
-        <v>726</v>
-      </c>
-      <c r="K3" s="176"/>
-      <c r="L3" s="175">
+        <v>727</v>
+      </c>
+      <c r="K3" s="182"/>
+      <c r="L3" s="88">
         <v>1</v>
       </c>
       <c r="M3" s="181" t="s">
-        <v>727</v>
-      </c>
-      <c r="N3" s="175"/>
-      <c r="O3" s="182">
+        <v>728</v>
+      </c>
+      <c r="N3" s="88"/>
+      <c r="O3" s="183">
         <v>1</v>
       </c>
     </row>
@@ -7164,39 +7154,39 @@
         <f>_xlfn.CONCAT("q",IF(O4&lt;10,"0",""),O4)</f>
         <v>q02</v>
       </c>
-      <c r="B4" s="163" t="str">
+      <c r="B4" s="164" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
-      <c r="C4" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D4" s="175"/>
-      <c r="E4" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F4" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G4" s="153" t="s">
+      <c r="C4" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F4" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G4" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H4" s="181" t="s">
-        <v>730</v>
-      </c>
-      <c r="I4" s="175"/>
+        <v>731</v>
+      </c>
+      <c r="I4" s="88"/>
       <c r="J4" s="181" t="s">
-        <v>731</v>
-      </c>
-      <c r="K4" s="175"/>
-      <c r="L4" s="175">
+        <v>732</v>
+      </c>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88">
         <v>4</v>
       </c>
       <c r="M4" s="181" t="s">
-        <v>732</v>
-      </c>
-      <c r="N4" s="175"/>
-      <c r="O4" s="182">
+        <v>733</v>
+      </c>
+      <c r="N4" s="88"/>
+      <c r="O4" s="183">
         <f>O3+1</f>
         <v>2</v>
       </c>
@@ -7206,39 +7196,39 @@
         <f>_xlfn.CONCAT("q",IF(O5&lt;10,"0",""),O5)</f>
         <v>q03</v>
       </c>
-      <c r="B5" s="163" t="str">
+      <c r="B5" s="164" t="str">
         <f>B4</f>
         <v>qbank01</v>
       </c>
-      <c r="C5" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D5" s="175"/>
-      <c r="E5" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F5" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G5" s="153" t="s">
-        <v>733</v>
+      <c r="C5" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88" t="s">
+        <v>729</v>
+      </c>
+      <c r="F5" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G5" s="180" t="s">
+        <v>734</v>
       </c>
       <c r="H5" s="181" t="s">
-        <v>734</v>
-      </c>
-      <c r="I5" s="175"/>
+        <v>735</v>
+      </c>
+      <c r="I5" s="88"/>
       <c r="J5" s="181" t="s">
-        <v>735</v>
-      </c>
-      <c r="K5" s="175"/>
-      <c r="L5" s="175">
+        <v>736</v>
+      </c>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88">
         <v>3</v>
       </c>
       <c r="M5" s="181" t="s">
-        <v>736</v>
-      </c>
-      <c r="N5" s="175"/>
-      <c r="O5" s="182">
+        <v>737</v>
+      </c>
+      <c r="N5" s="88"/>
+      <c r="O5" s="183">
         <f>O4+1</f>
         <v>3</v>
       </c>
@@ -7248,39 +7238,39 @@
         <f>_xlfn.CONCAT("q",IF(O6&lt;10,"0",""),O6)</f>
         <v>q04</v>
       </c>
-      <c r="B6" s="163" t="str">
+      <c r="B6" s="164" t="str">
         <f>B5</f>
         <v>qbank01</v>
       </c>
-      <c r="C6" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D6" s="175"/>
-      <c r="E6" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F6" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G6" s="153" t="s">
+      <c r="C6" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F6" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G6" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H6" s="181" t="s">
-        <v>737</v>
-      </c>
-      <c r="I6" s="175"/>
+        <v>738</v>
+      </c>
+      <c r="I6" s="88"/>
       <c r="J6" s="181" t="s">
-        <v>738</v>
-      </c>
-      <c r="K6" s="175"/>
-      <c r="L6" s="175">
+        <v>739</v>
+      </c>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88">
         <v>2</v>
       </c>
       <c r="M6" s="181" t="s">
-        <v>739</v>
-      </c>
-      <c r="N6" s="175"/>
-      <c r="O6" s="182">
+        <v>740</v>
+      </c>
+      <c r="N6" s="88"/>
+      <c r="O6" s="183">
         <f>O5+1</f>
         <v>4</v>
       </c>
@@ -7290,39 +7280,39 @@
         <f>_xlfn.CONCAT("q",IF(O7&lt;10,"0",""),O7)</f>
         <v>q05</v>
       </c>
-      <c r="B7" s="163" t="str">
+      <c r="B7" s="164" t="str">
         <f>B6</f>
         <v>qbank01</v>
       </c>
-      <c r="C7" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F7" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G7" s="153" t="s">
-        <v>740</v>
+      <c r="C7" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88" t="s">
+        <v>729</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G7" s="180" t="s">
+        <v>741</v>
       </c>
       <c r="H7" s="181" t="s">
-        <v>741</v>
-      </c>
-      <c r="I7" s="175"/>
+        <v>742</v>
+      </c>
+      <c r="I7" s="88"/>
       <c r="J7" s="181" t="s">
-        <v>742</v>
-      </c>
-      <c r="K7" s="175"/>
-      <c r="L7" s="175">
+        <v>743</v>
+      </c>
+      <c r="K7" s="88"/>
+      <c r="L7" s="88">
         <v>1</v>
       </c>
       <c r="M7" s="181" t="s">
-        <v>743</v>
-      </c>
-      <c r="N7" s="175"/>
-      <c r="O7" s="182">
+        <v>744</v>
+      </c>
+      <c r="N7" s="88"/>
+      <c r="O7" s="183">
         <f>O6+1</f>
         <v>5</v>
       </c>
@@ -7332,39 +7322,39 @@
         <f>_xlfn.CONCAT("q",IF(O8&lt;10,"0",""),O8)</f>
         <v>q06</v>
       </c>
-      <c r="B8" s="163" t="str">
+      <c r="B8" s="164" t="str">
         <f>B7</f>
         <v>qbank01</v>
       </c>
-      <c r="C8" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D8" s="175"/>
-      <c r="E8" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F8" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G8" s="153" t="s">
+      <c r="C8" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F8" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G8" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H8" s="181" t="s">
-        <v>744</v>
-      </c>
-      <c r="I8" s="176"/>
+        <v>745</v>
+      </c>
+      <c r="I8" s="182"/>
       <c r="J8" s="181" t="s">
-        <v>745</v>
-      </c>
-      <c r="K8" s="175"/>
-      <c r="L8" s="175">
+        <v>746</v>
+      </c>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88">
         <v>2</v>
       </c>
       <c r="M8" s="181" t="s">
-        <v>746</v>
-      </c>
-      <c r="N8" s="183"/>
-      <c r="O8" s="182">
+        <v>747</v>
+      </c>
+      <c r="N8" s="184"/>
+      <c r="O8" s="183">
         <f>O7+1</f>
         <v>6</v>
       </c>
@@ -7374,39 +7364,39 @@
         <f>_xlfn.CONCAT("q",IF(O9&lt;10,"0",""),O9)</f>
         <v>q07</v>
       </c>
-      <c r="B9" s="163" t="str">
+      <c r="B9" s="164" t="str">
         <f>B8</f>
         <v>qbank01</v>
       </c>
-      <c r="C9" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D9" s="175"/>
-      <c r="E9" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F9" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G9" s="153" t="s">
+      <c r="C9" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F9" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G9" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H9" s="181" t="s">
-        <v>747</v>
-      </c>
-      <c r="I9" s="176"/>
+        <v>748</v>
+      </c>
+      <c r="I9" s="182"/>
       <c r="J9" s="181" t="s">
-        <v>748</v>
-      </c>
-      <c r="K9" s="175"/>
-      <c r="L9" s="175">
+        <v>749</v>
+      </c>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88">
         <v>3</v>
       </c>
       <c r="M9" s="181" t="s">
-        <v>749</v>
-      </c>
-      <c r="N9" s="175"/>
-      <c r="O9" s="182">
+        <v>750</v>
+      </c>
+      <c r="N9" s="88"/>
+      <c r="O9" s="183">
         <f>O8+1</f>
         <v>7</v>
       </c>
@@ -7416,39 +7406,39 @@
         <f>_xlfn.CONCAT("q",IF(O10&lt;10,"0",""),O10)</f>
         <v>q08</v>
       </c>
-      <c r="B10" s="163" t="str">
+      <c r="B10" s="164" t="str">
         <f>B9</f>
         <v>qbank01</v>
       </c>
-      <c r="C10" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D10" s="175"/>
-      <c r="E10" s="175" t="s">
+      <c r="C10" s="88" t="s">
         <v>722</v>
       </c>
-      <c r="F10" s="175" t="s">
-        <v>750</v>
-      </c>
-      <c r="G10" s="153" t="s">
-        <v>733</v>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88" t="s">
+        <v>723</v>
+      </c>
+      <c r="F10" s="88" t="s">
+        <v>751</v>
+      </c>
+      <c r="G10" s="180" t="s">
+        <v>734</v>
       </c>
       <c r="H10" s="181" t="s">
-        <v>751</v>
-      </c>
-      <c r="I10" s="175"/>
-      <c r="J10" s="175"/>
-      <c r="K10" s="184" t="s">
         <v>752</v>
       </c>
-      <c r="L10" s="175">
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="185" t="s">
+        <v>753</v>
+      </c>
+      <c r="L10" s="88">
         <v>2</v>
       </c>
       <c r="M10" s="181" t="s">
-        <v>753</v>
-      </c>
-      <c r="N10" s="175"/>
-      <c r="O10" s="182">
+        <v>754</v>
+      </c>
+      <c r="N10" s="88"/>
+      <c r="O10" s="183">
         <f>O9+1</f>
         <v>8</v>
       </c>
@@ -7458,41 +7448,41 @@
         <f>_xlfn.CONCAT("q",IF(O11&lt;10,"0",""),O11)</f>
         <v>q09</v>
       </c>
-      <c r="B11" s="163" t="str">
+      <c r="B11" s="164" t="str">
         <f>B10</f>
         <v>qbank01</v>
       </c>
-      <c r="C11" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D11" s="175"/>
-      <c r="E11" s="175" t="s">
+      <c r="C11" s="88" t="s">
         <v>722</v>
       </c>
-      <c r="F11" s="175" t="s">
-        <v>750</v>
-      </c>
-      <c r="G11" s="153" t="s">
-        <v>733</v>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88" t="s">
+        <v>723</v>
+      </c>
+      <c r="F11" s="88" t="s">
+        <v>751</v>
+      </c>
+      <c r="G11" s="180" t="s">
+        <v>734</v>
       </c>
       <c r="H11" s="181" t="s">
-        <v>754</v>
-      </c>
-      <c r="I11" s="184" t="s">
+        <v>755</v>
+      </c>
+      <c r="I11" s="185" t="s">
         <v>312</v>
       </c>
       <c r="J11" s="181" t="s">
-        <v>755</v>
-      </c>
-      <c r="K11" s="175"/>
-      <c r="L11" s="175">
+        <v>756</v>
+      </c>
+      <c r="K11" s="88"/>
+      <c r="L11" s="88">
         <v>1</v>
       </c>
       <c r="M11" s="181" t="s">
-        <v>756</v>
-      </c>
-      <c r="N11" s="175"/>
-      <c r="O11" s="182">
+        <v>757</v>
+      </c>
+      <c r="N11" s="88"/>
+      <c r="O11" s="183">
         <f>O10+1</f>
         <v>9</v>
       </c>
@@ -7502,39 +7492,39 @@
         <f>_xlfn.CONCAT("q",IF(O12&lt;10,"0",""),O12)</f>
         <v>q10</v>
       </c>
-      <c r="B12" s="163" t="str">
+      <c r="B12" s="164" t="str">
         <f>B11</f>
         <v>qbank01</v>
       </c>
-      <c r="C12" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D12" s="175"/>
-      <c r="E12" s="175" t="s">
-        <v>757</v>
-      </c>
-      <c r="F12" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G12" s="153" t="s">
-        <v>729</v>
+      <c r="C12" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88" t="s">
+        <v>758</v>
+      </c>
+      <c r="F12" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G12" s="180" t="s">
+        <v>730</v>
       </c>
       <c r="H12" s="181" t="s">
-        <v>758</v>
-      </c>
-      <c r="I12" s="175"/>
-      <c r="J12" s="151" t="s">
         <v>759</v>
       </c>
-      <c r="K12" s="175"/>
-      <c r="L12" s="175">
+      <c r="I12" s="88"/>
+      <c r="J12" s="186" t="s">
+        <v>760</v>
+      </c>
+      <c r="K12" s="88"/>
+      <c r="L12" s="88">
         <v>4</v>
       </c>
       <c r="M12" s="181" t="s">
-        <v>760</v>
-      </c>
-      <c r="N12" s="175"/>
-      <c r="O12" s="182">
+        <v>761</v>
+      </c>
+      <c r="N12" s="88"/>
+      <c r="O12" s="183">
         <f>O11+1</f>
         <v>10</v>
       </c>
@@ -7544,39 +7534,39 @@
         <f>_xlfn.CONCAT("q",IF(O13&lt;10,"0",""),O13)</f>
         <v>q11</v>
       </c>
-      <c r="B13" s="163" t="str">
+      <c r="B13" s="164" t="str">
         <f>B12</f>
         <v>qbank01</v>
       </c>
-      <c r="C13" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D13" s="175"/>
-      <c r="E13" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F13" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G13" s="153" t="s">
+      <c r="C13" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F13" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G13" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H13" s="181" t="s">
-        <v>761</v>
-      </c>
-      <c r="I13" s="175"/>
+        <v>762</v>
+      </c>
+      <c r="I13" s="88"/>
       <c r="J13" s="181" t="s">
-        <v>762</v>
-      </c>
-      <c r="K13" s="175"/>
-      <c r="L13" s="175">
+        <v>763</v>
+      </c>
+      <c r="K13" s="88"/>
+      <c r="L13" s="88">
         <v>3</v>
       </c>
       <c r="M13" s="181" t="s">
-        <v>763</v>
-      </c>
-      <c r="N13" s="175"/>
-      <c r="O13" s="182">
+        <v>764</v>
+      </c>
+      <c r="N13" s="88"/>
+      <c r="O13" s="183">
         <f>O12+1</f>
         <v>11</v>
       </c>
@@ -7586,39 +7576,39 @@
         <f>_xlfn.CONCAT("q",IF(O14&lt;10,"0",""),O14)</f>
         <v>q12</v>
       </c>
-      <c r="B14" s="163" t="str">
+      <c r="B14" s="164" t="str">
         <f>B13</f>
         <v>qbank01</v>
       </c>
-      <c r="C14" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D14" s="175"/>
-      <c r="E14" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F14" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G14" s="153" t="s">
+      <c r="C14" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F14" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G14" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H14" s="181" t="s">
-        <v>764</v>
-      </c>
-      <c r="I14" s="175"/>
+        <v>765</v>
+      </c>
+      <c r="I14" s="88"/>
       <c r="J14" s="181" t="s">
-        <v>765</v>
-      </c>
-      <c r="K14" s="175"/>
-      <c r="L14" s="175">
+        <v>766</v>
+      </c>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88">
         <v>1</v>
       </c>
       <c r="M14" s="181" t="s">
-        <v>766</v>
-      </c>
-      <c r="N14" s="175"/>
-      <c r="O14" s="182">
+        <v>767</v>
+      </c>
+      <c r="N14" s="88"/>
+      <c r="O14" s="183">
         <f>O13+1</f>
         <v>12</v>
       </c>
@@ -7628,41 +7618,41 @@
         <f>_xlfn.CONCAT("q",IF(O15&lt;10,"0",""),O15)</f>
         <v>q13</v>
       </c>
-      <c r="B15" s="163" t="str">
+      <c r="B15" s="164" t="str">
         <f>B14</f>
         <v>qbank01</v>
       </c>
-      <c r="C15" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F15" s="175" t="s">
-        <v>750</v>
-      </c>
-      <c r="G15" s="153" t="s">
-        <v>767</v>
+      <c r="C15" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D15" s="187"/>
+      <c r="E15" s="88" t="s">
+        <v>729</v>
+      </c>
+      <c r="F15" s="88" t="s">
+        <v>751</v>
+      </c>
+      <c r="G15" s="180" t="s">
+        <v>768</v>
       </c>
       <c r="H15" s="181" t="s">
-        <v>768</v>
-      </c>
-      <c r="I15" s="175" t="s">
+        <v>769</v>
+      </c>
+      <c r="I15" s="88" t="s">
         <v>338</v>
       </c>
       <c r="J15" s="181" t="s">
-        <v>769</v>
-      </c>
-      <c r="K15" s="176"/>
-      <c r="L15" s="175">
+        <v>770</v>
+      </c>
+      <c r="K15" s="182"/>
+      <c r="L15" s="88">
         <v>2</v>
       </c>
       <c r="M15" s="181" t="s">
-        <v>770</v>
-      </c>
-      <c r="N15" s="175"/>
-      <c r="O15" s="182">
+        <v>771</v>
+      </c>
+      <c r="N15" s="88"/>
+      <c r="O15" s="183">
         <f>O14+1</f>
         <v>13</v>
       </c>
@@ -7672,41 +7662,41 @@
         <f>_xlfn.CONCAT("q",IF(O16&lt;10,"0",""),O16)</f>
         <v>q14</v>
       </c>
-      <c r="B16" s="163" t="str">
+      <c r="B16" s="164" t="str">
         <f>B15</f>
         <v>qbank01</v>
       </c>
-      <c r="C16" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F16" s="175" t="s">
-        <v>750</v>
-      </c>
-      <c r="G16" s="153" t="s">
-        <v>767</v>
+      <c r="C16" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D16" s="187"/>
+      <c r="E16" s="88" t="s">
+        <v>729</v>
+      </c>
+      <c r="F16" s="88" t="s">
+        <v>751</v>
+      </c>
+      <c r="G16" s="180" t="s">
+        <v>768</v>
       </c>
       <c r="H16" s="181" t="s">
-        <v>771</v>
-      </c>
-      <c r="I16" s="175" t="s">
+        <v>772</v>
+      </c>
+      <c r="I16" s="88" t="s">
         <v>338</v>
       </c>
       <c r="J16" s="181" t="s">
-        <v>772</v>
-      </c>
-      <c r="K16" s="176"/>
-      <c r="L16" s="175">
+        <v>773</v>
+      </c>
+      <c r="K16" s="182"/>
+      <c r="L16" s="88">
         <v>1</v>
       </c>
       <c r="M16" s="181" t="s">
-        <v>773</v>
-      </c>
-      <c r="N16" s="183"/>
-      <c r="O16" s="182">
+        <v>774</v>
+      </c>
+      <c r="N16" s="184"/>
+      <c r="O16" s="183">
         <f>O15+1</f>
         <v>14</v>
       </c>
@@ -7716,39 +7706,39 @@
         <f>_xlfn.CONCAT("q",IF(O17&lt;10,"0",""),O17)</f>
         <v>q15</v>
       </c>
-      <c r="B17" s="163" t="str">
+      <c r="B17" s="164" t="str">
         <f>B16</f>
         <v>qbank01</v>
       </c>
-      <c r="C17" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F17" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G17" s="153" t="s">
-        <v>774</v>
+      <c r="C17" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D17" s="187"/>
+      <c r="E17" s="88" t="s">
+        <v>729</v>
+      </c>
+      <c r="F17" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G17" s="180" t="s">
+        <v>775</v>
       </c>
       <c r="H17" s="181" t="s">
-        <v>775</v>
-      </c>
-      <c r="I17" s="176"/>
+        <v>776</v>
+      </c>
+      <c r="I17" s="182"/>
       <c r="J17" s="181" t="s">
-        <v>776</v>
-      </c>
-      <c r="K17" s="176"/>
-      <c r="L17" s="175">
+        <v>777</v>
+      </c>
+      <c r="K17" s="182"/>
+      <c r="L17" s="88">
         <v>2</v>
       </c>
       <c r="M17" s="181" t="s">
-        <v>777</v>
-      </c>
-      <c r="N17" s="183"/>
-      <c r="O17" s="182">
+        <v>778</v>
+      </c>
+      <c r="N17" s="184"/>
+      <c r="O17" s="183">
         <f>O16+1</f>
         <v>15</v>
       </c>
@@ -7758,39 +7748,39 @@
         <f>_xlfn.CONCAT("q",IF(O18&lt;10,"0",""),O18)</f>
         <v>q16</v>
       </c>
-      <c r="B18" s="163" t="str">
+      <c r="B18" s="164" t="str">
         <f>B17</f>
         <v>qbank01</v>
       </c>
-      <c r="C18" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F18" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G18" s="153" t="s">
-        <v>767</v>
+      <c r="C18" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D18" s="187"/>
+      <c r="E18" s="88" t="s">
+        <v>729</v>
+      </c>
+      <c r="F18" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G18" s="180" t="s">
+        <v>768</v>
       </c>
       <c r="H18" s="181" t="s">
-        <v>778</v>
-      </c>
-      <c r="I18" s="176"/>
+        <v>779</v>
+      </c>
+      <c r="I18" s="182"/>
       <c r="J18" s="181" t="s">
-        <v>779</v>
-      </c>
-      <c r="K18" s="176"/>
-      <c r="L18" s="175">
+        <v>780</v>
+      </c>
+      <c r="K18" s="182"/>
+      <c r="L18" s="88">
         <v>1</v>
       </c>
       <c r="M18" s="181" t="s">
-        <v>780</v>
-      </c>
-      <c r="N18" s="183"/>
-      <c r="O18" s="182">
+        <v>781</v>
+      </c>
+      <c r="N18" s="184"/>
+      <c r="O18" s="183">
         <f>O17+1</f>
         <v>16</v>
       </c>
@@ -7800,39 +7790,39 @@
         <f>_xlfn.CONCAT("q",IF(O19&lt;10,"0",""),O19)</f>
         <v>q17</v>
       </c>
-      <c r="B19" s="163" t="str">
+      <c r="B19" s="164" t="str">
         <f>B18</f>
         <v>qbank01</v>
       </c>
-      <c r="C19" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F19" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G19" s="153" t="s">
+      <c r="C19" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D19" s="187"/>
+      <c r="E19" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F19" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G19" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H19" s="181" t="s">
-        <v>781</v>
-      </c>
-      <c r="I19" s="176"/>
+        <v>782</v>
+      </c>
+      <c r="I19" s="182"/>
       <c r="J19" s="181" t="s">
-        <v>782</v>
-      </c>
-      <c r="K19" s="176"/>
-      <c r="L19" s="175">
+        <v>783</v>
+      </c>
+      <c r="K19" s="182"/>
+      <c r="L19" s="88">
         <v>3</v>
       </c>
       <c r="M19" s="181" t="s">
-        <v>783</v>
-      </c>
-      <c r="N19" s="183"/>
-      <c r="O19" s="182">
+        <v>784</v>
+      </c>
+      <c r="N19" s="184"/>
+      <c r="O19" s="183">
         <f>O18+1</f>
         <v>17</v>
       </c>
@@ -7842,39 +7832,39 @@
         <f>_xlfn.CONCAT("q",IF(O20&lt;10,"0",""),O20)</f>
         <v>q18</v>
       </c>
-      <c r="B20" s="163" t="str">
+      <c r="B20" s="164" t="str">
         <f>B19</f>
         <v>qbank01</v>
       </c>
-      <c r="C20" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="175" t="s">
-        <v>728</v>
-      </c>
-      <c r="F20" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G20" s="153" t="s">
+      <c r="C20" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D20" s="187"/>
+      <c r="E20" s="88" t="s">
         <v>729</v>
       </c>
+      <c r="F20" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G20" s="180" t="s">
+        <v>730</v>
+      </c>
       <c r="H20" s="181" t="s">
-        <v>784</v>
-      </c>
-      <c r="I20" s="176"/>
+        <v>785</v>
+      </c>
+      <c r="I20" s="182"/>
       <c r="J20" s="181" t="s">
-        <v>785</v>
-      </c>
-      <c r="K20" s="176"/>
-      <c r="L20" s="175">
+        <v>786</v>
+      </c>
+      <c r="K20" s="182"/>
+      <c r="L20" s="88">
         <v>4</v>
       </c>
       <c r="M20" s="181" t="s">
-        <v>786</v>
-      </c>
-      <c r="N20" s="183"/>
-      <c r="O20" s="182">
+        <v>787</v>
+      </c>
+      <c r="N20" s="184"/>
+      <c r="O20" s="183">
         <f>O19+1</f>
         <v>18</v>
       </c>
@@ -7884,39 +7874,39 @@
         <f>_xlfn.CONCAT("q",IF(O21&lt;10,"0",""),O21)</f>
         <v>q19</v>
       </c>
-      <c r="B21" s="163" t="str">
+      <c r="B21" s="164" t="str">
         <f>B20</f>
         <v>qbank01</v>
       </c>
-      <c r="C21" s="175" t="s">
-        <v>721</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="175" t="s">
-        <v>757</v>
-      </c>
-      <c r="F21" s="175" t="s">
-        <v>723</v>
-      </c>
-      <c r="G21" s="153" t="s">
-        <v>774</v>
+      <c r="C21" s="88" t="s">
+        <v>722</v>
+      </c>
+      <c r="D21" s="187"/>
+      <c r="E21" s="88" t="s">
+        <v>758</v>
+      </c>
+      <c r="F21" s="88" t="s">
+        <v>724</v>
+      </c>
+      <c r="G21" s="180" t="s">
+        <v>775</v>
       </c>
       <c r="H21" s="181" t="s">
-        <v>787</v>
-      </c>
-      <c r="I21" s="175"/>
+        <v>788</v>
+      </c>
+      <c r="I21" s="88"/>
       <c r="J21" s="181" t="s">
-        <v>788</v>
-      </c>
-      <c r="K21" s="175"/>
-      <c r="L21" s="175">
+        <v>789</v>
+      </c>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88">
         <v>4</v>
       </c>
       <c r="M21" s="181" t="s">
-        <v>789</v>
-      </c>
-      <c r="N21" s="175"/>
-      <c r="O21" s="182">
+        <v>790</v>
+      </c>
+      <c r="N21" s="88"/>
+      <c r="O21" s="183">
         <f>O20+1</f>
         <v>19</v>
       </c>
@@ -7926,37 +7916,37 @@
         <f>_xlfn.CONCAT("q",IF(O22&lt;10,"0",""),O22)</f>
         <v>q20</v>
       </c>
-      <c r="B22" s="163" t="str">
+      <c r="B22" s="164" t="str">
         <f>B21</f>
         <v>qbank01</v>
       </c>
-      <c r="C22" s="175" t="s">
-        <v>790</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="175" t="s">
-        <v>722</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="151" t="s">
-        <v>740</v>
+      <c r="C22" s="88" t="s">
+        <v>791</v>
+      </c>
+      <c r="D22" s="187"/>
+      <c r="E22" s="88" t="s">
+        <v>723</v>
+      </c>
+      <c r="F22" s="89"/>
+      <c r="G22" s="186" t="s">
+        <v>741</v>
       </c>
       <c r="H22" s="181" t="s">
-        <v>791</v>
-      </c>
-      <c r="I22" s="184" t="s">
+        <v>792</v>
+      </c>
+      <c r="I22" s="185" t="s">
         <v>315</v>
       </c>
       <c r="J22" s="181" t="s">
-        <v>792</v>
-      </c>
-      <c r="K22" s="176"/>
-      <c r="L22" s="185"/>
-      <c r="M22" s="186"/>
-      <c r="N22" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="K22" s="182"/>
+      <c r="L22" s="188"/>
+      <c r="M22" s="144"/>
+      <c r="N22" s="89" t="s">
         <v>392</v>
       </c>
-      <c r="O22" s="187">
+      <c r="O22" s="189">
         <f>O21+1</f>
         <v>20</v>
       </c>
@@ -9820,37 +9810,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D00035-001A-4EC3-A4FB-00B800E6006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002A0027-0071-4BD4-A583-005B00070058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003F00CE-005A-4ABD-A888-000D0064006E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FE00A8-000F-4085-9A26-007F00060072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CD0075-001F-4357-9FEA-0041004C00D4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FE0006-00CF-482E-B97B-00C800FC000E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005B00E1-0020-4F5C-A0F9-004B00E600B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006500A1-0034-4427-889D-00EA004900BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005000F8-0029-42AB-9B2D-00580064004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AC00D5-00D3-47FF-AB55-00A6005900D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0012009F-00E9-44CD-B76E-00E1004A0069}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001200BB-004C-4DBA-B0B3-00E9002500AC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -11058,31 +11048,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007800FC-009F-4E96-BAF9-00FC00720013}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0046004C-00E4-475C-9C18-008B008800BE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DD0089-00E3-4A62-87F4-008800ED0050}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00650021-0049-40D2-BEB4-00B3007C00AA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F700FF-004A-4735-81C9-00BA004600FD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003800F2-00C5-47C1-BE1C-004800E20088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E20035-00C4-4378-9C9A-00EE00D50056}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000500A1-00D9-47F8-80BC-00A400A40099}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C40001-0070-4E4A-A9C3-00D7006C0090}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006F0097-00E0-4698-94BD-005A00A70075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -11233,7 +11223,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00800025-0006-44AE-BE5A-00A4006000B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0007008B-0009-43DB-B118-009200900060}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -11367,13 +11357,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00E0009A-007C-4352-99B9-00E1003400B4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0030001F-008E-44CA-BB85-00B20018004E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004300E9-0004-4BF0-BEEB-00E300A500D3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003900FB-0006-4BF5-8F35-0040004500BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
FINISHED: Mvp-template qbanks and questions bulk load
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="14"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="796">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -2183,28 +2183,31 @@
     <t>level</t>
   </si>
   <si>
-    <t>with_images</t>
+    <t>withImages</t>
   </si>
   <si>
     <t>question</t>
   </si>
   <si>
-    <t>general_imagen</t>
+    <t>questionImage</t>
   </si>
   <si>
     <t>answers</t>
   </si>
   <si>
-    <t>answer_images</t>
+    <t>answers_images</t>
   </si>
   <si>
     <t>answer_correct</t>
   </si>
   <si>
-    <t>answer_feedback</t>
-  </si>
-  <si>
-    <t>answer_feedback_image</t>
+    <t>answers_feedback</t>
+  </si>
+  <si>
+    <t>clues</t>
+  </si>
+  <si>
+    <t>answers_feedback_image</t>
   </si>
   <si>
     <t xml:space="preserve">Question Bank</t>
@@ -2237,7 +2240,7 @@
     <t xml:space="preserve">Feedback imagen</t>
   </si>
   <si>
-    <t>mono</t>
+    <t>mono-response</t>
   </si>
   <si>
     <t>elementary</t>
@@ -2543,11 +2546,14 @@
     <t xml:space="preserve">En el siguiente mapa se muestra la densidad de población en 2018 en España por provincias. ¿Sabes los nombres de las provincias marcadas con densidad de población muy baja?</t>
   </si>
   <si>
-    <t xml:space="preserve">Cáceres.
-|Zamora.
-|Ávila.
-|Soria.
-|Cuenca.</t>
+    <t xml:space="preserve">Cáceres
+|Zamora
+|Ávila@
+|Soria
+|Cuenca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para llegar a pie a Santiago de Compostela te cansas menos si sales desde Zamora.</t>
   </si>
 </sst>
 </file>
@@ -3173,7 +3179,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3693,6 +3699,9 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="5" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4829,13 +4838,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{006B002F-00EC-4042-9D42-002A00F40040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FB00CA-00BB-41F6-9D76-004A00CE0058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003C009A-00EE-42FB-96DA-002A00AA0007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003A0025-0010-43EE-B516-0003008200BB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -4980,7 +4989,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00D100A0-008A-4BC0-8F92-0017001B0046}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000D0045-00E8-4312-AA9D-009E00510054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7005,7 +7014,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="11.8515625"/>
     <col customWidth="1" min="2" max="2" width="15.8515625"/>
-    <col customWidth="1" min="3" max="3" width="10.00390625"/>
+    <col customWidth="1" min="3" max="3" width="14.00390625"/>
     <col bestFit="1" min="4" max="4" width="8.50390625"/>
     <col bestFit="1" min="5" max="5" style="175" width="17.3515625"/>
     <col bestFit="1" min="6" max="6" width="11.28125"/>
@@ -7016,8 +7025,9 @@
     <col bestFit="1" min="11" max="11" style="176" width="15.2109375"/>
     <col bestFit="1" min="12" max="12" width="9.921875"/>
     <col customWidth="1" min="13" max="13" width="114.28125"/>
-    <col customWidth="1" min="14" max="14" style="176" width="23.8515625"/>
-    <col bestFit="1" min="15" max="15" width="2.78125"/>
+    <col customWidth="1" min="14" max="14" width="16.57421875"/>
+    <col customWidth="1" min="15" max="15" style="176" width="23.8515625"/>
+    <col bestFit="1" min="16" max="16" width="2.78125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -7042,7 +7052,7 @@
       <c r="G1" s="177" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="178" t="s">
         <v>705</v>
       </c>
       <c r="I1" s="86" t="s">
@@ -7062,6 +7072,9 @@
       </c>
       <c r="N1" s="86" t="s">
         <v>711</v>
+      </c>
+      <c r="O1" s="86" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -7069,7 +7082,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C2" s="112" t="s">
         <v>430</v>
@@ -7078,39 +7091,40 @@
         <v>256</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G2" s="130" t="s">
         <v>155</v>
       </c>
-      <c r="H2" s="178" t="s">
-        <v>715</v>
+      <c r="H2" s="179" t="s">
+        <v>716</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="J2" s="130" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="L2" s="112" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="M2" s="130" t="s">
-        <v>720</v>
-      </c>
-      <c r="N2" s="7" t="s">
         <v>721</v>
       </c>
+      <c r="N2" s="130"/>
+      <c r="O2" s="7" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="3" ht="114">
-      <c r="A3" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O3&lt;10,"0",""),O3)</f>
+      <c r="A3" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P3&lt;10,"0",""),P3)</f>
         <v>q01</v>
       </c>
       <c r="B3" s="164" t="str">
@@ -7118,40 +7132,41 @@
         <v>qbank01</v>
       </c>
       <c r="C3" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D3" s="88"/>
       <c r="E3" s="88" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F3" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G3" s="180" t="s">
         <v>725</v>
       </c>
-      <c r="H3" s="181" t="s">
+      <c r="G3" s="181" t="s">
         <v>726</v>
       </c>
+      <c r="H3" s="182" t="s">
+        <v>727</v>
+      </c>
       <c r="I3" s="88"/>
-      <c r="J3" s="181" t="s">
-        <v>727</v>
-      </c>
-      <c r="K3" s="182"/>
+      <c r="J3" s="182" t="s">
+        <v>728</v>
+      </c>
+      <c r="K3" s="183"/>
       <c r="L3" s="88">
         <v>1</v>
       </c>
-      <c r="M3" s="181" t="s">
-        <v>728</v>
-      </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="183">
+      <c r="M3" s="182" t="s">
+        <v>729</v>
+      </c>
+      <c r="N3" s="182"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="184">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="199.5">
-      <c r="A4" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O4&lt;10,"0",""),O4)</f>
+      <c r="A4" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P4&lt;10,"0",""),P4)</f>
         <v>q02</v>
       </c>
       <c r="B4" s="164" t="str">
@@ -7159,41 +7174,42 @@
         <v>qbank01</v>
       </c>
       <c r="C4" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F4" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G4" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H4" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G4" s="181" t="s">
         <v>731</v>
       </c>
+      <c r="H4" s="182" t="s">
+        <v>732</v>
+      </c>
       <c r="I4" s="88"/>
-      <c r="J4" s="181" t="s">
-        <v>732</v>
+      <c r="J4" s="182" t="s">
+        <v>733</v>
       </c>
       <c r="K4" s="88"/>
       <c r="L4" s="88">
         <v>4</v>
       </c>
-      <c r="M4" s="181" t="s">
-        <v>733</v>
-      </c>
-      <c r="N4" s="88"/>
-      <c r="O4" s="183">
-        <f>O3+1</f>
+      <c r="M4" s="182" t="s">
+        <v>734</v>
+      </c>
+      <c r="N4" s="182"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="184">
+        <f>P3+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="114">
-      <c r="A5" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O5&lt;10,"0",""),O5)</f>
+      <c r="A5" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P5&lt;10,"0",""),P5)</f>
         <v>q03</v>
       </c>
       <c r="B5" s="164" t="str">
@@ -7201,41 +7217,42 @@
         <v>qbank01</v>
       </c>
       <c r="C5" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D5" s="88"/>
       <c r="E5" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F5" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G5" s="180" t="s">
-        <v>734</v>
-      </c>
-      <c r="H5" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G5" s="181" t="s">
         <v>735</v>
       </c>
+      <c r="H5" s="182" t="s">
+        <v>736</v>
+      </c>
       <c r="I5" s="88"/>
-      <c r="J5" s="181" t="s">
-        <v>736</v>
+      <c r="J5" s="182" t="s">
+        <v>737</v>
       </c>
       <c r="K5" s="88"/>
       <c r="L5" s="88">
         <v>3</v>
       </c>
-      <c r="M5" s="181" t="s">
-        <v>737</v>
-      </c>
-      <c r="N5" s="88"/>
-      <c r="O5" s="183">
-        <f>O4+1</f>
+      <c r="M5" s="182" t="s">
+        <v>738</v>
+      </c>
+      <c r="N5" s="182"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="184">
+        <f>P4+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="156.75">
-      <c r="A6" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O6&lt;10,"0",""),O6)</f>
+      <c r="A6" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P6&lt;10,"0",""),P6)</f>
         <v>q04</v>
       </c>
       <c r="B6" s="164" t="str">
@@ -7243,41 +7260,42 @@
         <v>qbank01</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D6" s="88"/>
       <c r="E6" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F6" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G6" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H6" s="181" t="s">
-        <v>738</v>
+        <v>725</v>
+      </c>
+      <c r="G6" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H6" s="182" t="s">
+        <v>739</v>
       </c>
       <c r="I6" s="88"/>
-      <c r="J6" s="181" t="s">
-        <v>739</v>
+      <c r="J6" s="182" t="s">
+        <v>740</v>
       </c>
       <c r="K6" s="88"/>
       <c r="L6" s="88">
         <v>2</v>
       </c>
-      <c r="M6" s="181" t="s">
-        <v>740</v>
-      </c>
-      <c r="N6" s="88"/>
-      <c r="O6" s="183">
-        <f>O5+1</f>
+      <c r="M6" s="182" t="s">
+        <v>741</v>
+      </c>
+      <c r="N6" s="182"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="184">
+        <f>P5+1</f>
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="71.25">
-      <c r="A7" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O7&lt;10,"0",""),O7)</f>
+      <c r="A7" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P7&lt;10,"0",""),P7)</f>
         <v>q05</v>
       </c>
       <c r="B7" s="164" t="str">
@@ -7285,41 +7303,42 @@
         <v>qbank01</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D7" s="88"/>
       <c r="E7" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F7" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G7" s="180" t="s">
-        <v>741</v>
-      </c>
-      <c r="H7" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G7" s="181" t="s">
         <v>742</v>
       </c>
+      <c r="H7" s="182" t="s">
+        <v>743</v>
+      </c>
       <c r="I7" s="88"/>
-      <c r="J7" s="181" t="s">
-        <v>743</v>
+      <c r="J7" s="182" t="s">
+        <v>744</v>
       </c>
       <c r="K7" s="88"/>
       <c r="L7" s="88">
         <v>1</v>
       </c>
-      <c r="M7" s="181" t="s">
-        <v>744</v>
-      </c>
-      <c r="N7" s="88"/>
-      <c r="O7" s="183">
-        <f>O6+1</f>
+      <c r="M7" s="182" t="s">
+        <v>745</v>
+      </c>
+      <c r="N7" s="182"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="184">
+        <f>P6+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="242.25">
-      <c r="A8" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O8&lt;10,"0",""),O8)</f>
+      <c r="A8" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P8&lt;10,"0",""),P8)</f>
         <v>q06</v>
       </c>
       <c r="B8" s="164" t="str">
@@ -7327,41 +7346,42 @@
         <v>qbank01</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D8" s="88"/>
       <c r="E8" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F8" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G8" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H8" s="181" t="s">
-        <v>745</v>
-      </c>
-      <c r="I8" s="182"/>
-      <c r="J8" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G8" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H8" s="182" t="s">
         <v>746</v>
+      </c>
+      <c r="I8" s="183"/>
+      <c r="J8" s="182" t="s">
+        <v>747</v>
       </c>
       <c r="K8" s="88"/>
       <c r="L8" s="88">
         <v>2</v>
       </c>
-      <c r="M8" s="181" t="s">
-        <v>747</v>
-      </c>
-      <c r="N8" s="184"/>
-      <c r="O8" s="183">
-        <f>O7+1</f>
+      <c r="M8" s="182" t="s">
+        <v>748</v>
+      </c>
+      <c r="N8" s="182"/>
+      <c r="O8" s="185"/>
+      <c r="P8" s="184">
+        <f>P7+1</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="242.25">
-      <c r="A9" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O9&lt;10,"0",""),O9)</f>
+      <c r="A9" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P9&lt;10,"0",""),P9)</f>
         <v>q07</v>
       </c>
       <c r="B9" s="164" t="str">
@@ -7369,41 +7389,42 @@
         <v>qbank01</v>
       </c>
       <c r="C9" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D9" s="88"/>
       <c r="E9" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F9" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G9" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H9" s="181" t="s">
-        <v>748</v>
-      </c>
-      <c r="I9" s="182"/>
-      <c r="J9" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G9" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H9" s="182" t="s">
         <v>749</v>
+      </c>
+      <c r="I9" s="183"/>
+      <c r="J9" s="182" t="s">
+        <v>750</v>
       </c>
       <c r="K9" s="88"/>
       <c r="L9" s="88">
         <v>3</v>
       </c>
-      <c r="M9" s="181" t="s">
-        <v>750</v>
-      </c>
-      <c r="N9" s="88"/>
-      <c r="O9" s="183">
-        <f>O8+1</f>
+      <c r="M9" s="182" t="s">
+        <v>751</v>
+      </c>
+      <c r="N9" s="182"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="184">
+        <f>P8+1</f>
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="356.25">
-      <c r="A10" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O10&lt;10,"0",""),O10)</f>
+      <c r="A10" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P10&lt;10,"0",""),P10)</f>
         <v>q08</v>
       </c>
       <c r="B10" s="164" t="str">
@@ -7411,41 +7432,42 @@
         <v>qbank01</v>
       </c>
       <c r="C10" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D10" s="88"/>
       <c r="E10" s="88" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F10" s="88" t="s">
-        <v>751</v>
-      </c>
-      <c r="G10" s="180" t="s">
-        <v>734</v>
-      </c>
-      <c r="H10" s="181" t="s">
         <v>752</v>
+      </c>
+      <c r="G10" s="181" t="s">
+        <v>735</v>
+      </c>
+      <c r="H10" s="182" t="s">
+        <v>753</v>
       </c>
       <c r="I10" s="88"/>
       <c r="J10" s="88"/>
-      <c r="K10" s="185" t="s">
-        <v>753</v>
+      <c r="K10" s="186" t="s">
+        <v>754</v>
       </c>
       <c r="L10" s="88">
         <v>2</v>
       </c>
-      <c r="M10" s="181" t="s">
-        <v>754</v>
-      </c>
-      <c r="N10" s="88"/>
-      <c r="O10" s="183">
-        <f>O9+1</f>
+      <c r="M10" s="182" t="s">
+        <v>755</v>
+      </c>
+      <c r="N10" s="182"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="184">
+        <f>P9+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="11" ht="185.25">
-      <c r="A11" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O11&lt;10,"0",""),O11)</f>
+      <c r="A11" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P11&lt;10,"0",""),P11)</f>
         <v>q09</v>
       </c>
       <c r="B11" s="164" t="str">
@@ -7453,43 +7475,44 @@
         <v>qbank01</v>
       </c>
       <c r="C11" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D11" s="88"/>
       <c r="E11" s="88" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F11" s="88" t="s">
-        <v>751</v>
-      </c>
-      <c r="G11" s="180" t="s">
-        <v>734</v>
-      </c>
-      <c r="H11" s="181" t="s">
-        <v>755</v>
-      </c>
-      <c r="I11" s="185" t="s">
+        <v>725</v>
+      </c>
+      <c r="G11" s="181" t="s">
+        <v>735</v>
+      </c>
+      <c r="H11" s="182" t="s">
+        <v>756</v>
+      </c>
+      <c r="I11" s="186" t="s">
         <v>312</v>
       </c>
-      <c r="J11" s="181" t="s">
-        <v>756</v>
+      <c r="J11" s="182" t="s">
+        <v>757</v>
       </c>
       <c r="K11" s="88"/>
       <c r="L11" s="88">
         <v>1</v>
       </c>
-      <c r="M11" s="181" t="s">
-        <v>757</v>
-      </c>
-      <c r="N11" s="88"/>
-      <c r="O11" s="183">
-        <f>O10+1</f>
+      <c r="M11" s="182" t="s">
+        <v>758</v>
+      </c>
+      <c r="N11" s="182"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="184">
+        <f>P10+1</f>
         <v>9</v>
       </c>
     </row>
     <row r="12" ht="185.25">
-      <c r="A12" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O12&lt;10,"0",""),O12)</f>
+      <c r="A12" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P12&lt;10,"0",""),P12)</f>
         <v>q10</v>
       </c>
       <c r="B12" s="164" t="str">
@@ -7497,41 +7520,42 @@
         <v>qbank01</v>
       </c>
       <c r="C12" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D12" s="88"/>
       <c r="E12" s="88" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F12" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G12" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H12" s="181" t="s">
-        <v>759</v>
+        <v>725</v>
+      </c>
+      <c r="G12" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H12" s="182" t="s">
+        <v>760</v>
       </c>
       <c r="I12" s="88"/>
-      <c r="J12" s="186" t="s">
-        <v>760</v>
+      <c r="J12" s="187" t="s">
+        <v>761</v>
       </c>
       <c r="K12" s="88"/>
       <c r="L12" s="88">
         <v>4</v>
       </c>
-      <c r="M12" s="181" t="s">
-        <v>761</v>
-      </c>
-      <c r="N12" s="88"/>
-      <c r="O12" s="183">
-        <f>O11+1</f>
+      <c r="M12" s="182" t="s">
+        <v>762</v>
+      </c>
+      <c r="N12" s="182"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="184">
+        <f>P11+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="185.25">
-      <c r="A13" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O13&lt;10,"0",""),O13)</f>
+      <c r="A13" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P13&lt;10,"0",""),P13)</f>
         <v>q11</v>
       </c>
       <c r="B13" s="164" t="str">
@@ -7539,41 +7563,42 @@
         <v>qbank01</v>
       </c>
       <c r="C13" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D13" s="88"/>
       <c r="E13" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F13" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G13" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H13" s="181" t="s">
-        <v>762</v>
+        <v>725</v>
+      </c>
+      <c r="G13" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H13" s="182" t="s">
+        <v>763</v>
       </c>
       <c r="I13" s="88"/>
-      <c r="J13" s="181" t="s">
-        <v>763</v>
+      <c r="J13" s="182" t="s">
+        <v>764</v>
       </c>
       <c r="K13" s="88"/>
       <c r="L13" s="88">
         <v>3</v>
       </c>
-      <c r="M13" s="181" t="s">
-        <v>764</v>
-      </c>
-      <c r="N13" s="88"/>
-      <c r="O13" s="183">
-        <f>O12+1</f>
+      <c r="M13" s="182" t="s">
+        <v>765</v>
+      </c>
+      <c r="N13" s="182"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="184">
+        <f>P12+1</f>
         <v>11</v>
       </c>
     </row>
     <row r="14" ht="185.25">
-      <c r="A14" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O14&lt;10,"0",""),O14)</f>
+      <c r="A14" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P14&lt;10,"0",""),P14)</f>
         <v>q12</v>
       </c>
       <c r="B14" s="164" t="str">
@@ -7581,41 +7606,42 @@
         <v>qbank01</v>
       </c>
       <c r="C14" s="88" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D14" s="88"/>
       <c r="E14" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F14" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G14" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H14" s="181" t="s">
-        <v>765</v>
+        <v>725</v>
+      </c>
+      <c r="G14" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H14" s="182" t="s">
+        <v>766</v>
       </c>
       <c r="I14" s="88"/>
-      <c r="J14" s="181" t="s">
-        <v>766</v>
+      <c r="J14" s="182" t="s">
+        <v>767</v>
       </c>
       <c r="K14" s="88"/>
       <c r="L14" s="88">
         <v>1</v>
       </c>
-      <c r="M14" s="181" t="s">
-        <v>767</v>
-      </c>
-      <c r="N14" s="88"/>
-      <c r="O14" s="183">
-        <f>O13+1</f>
+      <c r="M14" s="182" t="s">
+        <v>768</v>
+      </c>
+      <c r="N14" s="182"/>
+      <c r="O14" s="88"/>
+      <c r="P14" s="184">
+        <f>P13+1</f>
         <v>12</v>
       </c>
     </row>
     <row r="15" ht="114">
-      <c r="A15" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O15&lt;10,"0",""),O15)</f>
+      <c r="A15" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P15&lt;10,"0",""),P15)</f>
         <v>q13</v>
       </c>
       <c r="B15" s="164" t="str">
@@ -7623,43 +7649,44 @@
         <v>qbank01</v>
       </c>
       <c r="C15" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="D15" s="187"/>
+        <v>723</v>
+      </c>
+      <c r="D15" s="188"/>
       <c r="E15" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F15" s="88" t="s">
-        <v>751</v>
-      </c>
-      <c r="G15" s="180" t="s">
-        <v>768</v>
-      </c>
-      <c r="H15" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G15" s="181" t="s">
         <v>769</v>
+      </c>
+      <c r="H15" s="182" t="s">
+        <v>770</v>
       </c>
       <c r="I15" s="88" t="s">
         <v>338</v>
       </c>
-      <c r="J15" s="181" t="s">
-        <v>770</v>
-      </c>
-      <c r="K15" s="182"/>
+      <c r="J15" s="182" t="s">
+        <v>771</v>
+      </c>
+      <c r="K15" s="183"/>
       <c r="L15" s="88">
         <v>2</v>
       </c>
-      <c r="M15" s="181" t="s">
-        <v>771</v>
-      </c>
-      <c r="N15" s="88"/>
-      <c r="O15" s="183">
-        <f>O14+1</f>
+      <c r="M15" s="182" t="s">
+        <v>772</v>
+      </c>
+      <c r="N15" s="182"/>
+      <c r="O15" s="88"/>
+      <c r="P15" s="184">
+        <f>P14+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="16" ht="114">
-      <c r="A16" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O16&lt;10,"0",""),O16)</f>
+      <c r="A16" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P16&lt;10,"0",""),P16)</f>
         <v>q14</v>
       </c>
       <c r="B16" s="164" t="str">
@@ -7667,43 +7694,44 @@
         <v>qbank01</v>
       </c>
       <c r="C16" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="D16" s="187"/>
+        <v>723</v>
+      </c>
+      <c r="D16" s="188"/>
       <c r="E16" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F16" s="88" t="s">
-        <v>751</v>
-      </c>
-      <c r="G16" s="180" t="s">
-        <v>768</v>
-      </c>
-      <c r="H16" s="181" t="s">
-        <v>772</v>
+        <v>725</v>
+      </c>
+      <c r="G16" s="181" t="s">
+        <v>769</v>
+      </c>
+      <c r="H16" s="182" t="s">
+        <v>773</v>
       </c>
       <c r="I16" s="88" t="s">
         <v>338</v>
       </c>
-      <c r="J16" s="181" t="s">
-        <v>773</v>
-      </c>
-      <c r="K16" s="182"/>
+      <c r="J16" s="182" t="s">
+        <v>774</v>
+      </c>
+      <c r="K16" s="183"/>
       <c r="L16" s="88">
         <v>1</v>
       </c>
-      <c r="M16" s="181" t="s">
-        <v>774</v>
-      </c>
-      <c r="N16" s="184"/>
-      <c r="O16" s="183">
-        <f>O15+1</f>
+      <c r="M16" s="182" t="s">
+        <v>775</v>
+      </c>
+      <c r="N16" s="182"/>
+      <c r="O16" s="185"/>
+      <c r="P16" s="184">
+        <f>P15+1</f>
         <v>14</v>
       </c>
     </row>
     <row r="17" ht="142.5">
-      <c r="A17" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O17&lt;10,"0",""),O17)</f>
+      <c r="A17" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P17&lt;10,"0",""),P17)</f>
         <v>q15</v>
       </c>
       <c r="B17" s="164" t="str">
@@ -7711,41 +7739,42 @@
         <v>qbank01</v>
       </c>
       <c r="C17" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="D17" s="187"/>
+        <v>723</v>
+      </c>
+      <c r="D17" s="188"/>
       <c r="E17" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F17" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G17" s="180" t="s">
-        <v>775</v>
-      </c>
-      <c r="H17" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G17" s="181" t="s">
         <v>776</v>
       </c>
-      <c r="I17" s="182"/>
-      <c r="J17" s="181" t="s">
+      <c r="H17" s="182" t="s">
         <v>777</v>
       </c>
-      <c r="K17" s="182"/>
+      <c r="I17" s="183"/>
+      <c r="J17" s="182" t="s">
+        <v>778</v>
+      </c>
+      <c r="K17" s="183"/>
       <c r="L17" s="88">
         <v>2</v>
       </c>
-      <c r="M17" s="181" t="s">
-        <v>778</v>
-      </c>
-      <c r="N17" s="184"/>
-      <c r="O17" s="183">
-        <f>O16+1</f>
+      <c r="M17" s="182" t="s">
+        <v>779</v>
+      </c>
+      <c r="N17" s="182"/>
+      <c r="O17" s="185"/>
+      <c r="P17" s="184">
+        <f>P16+1</f>
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="242.25">
-      <c r="A18" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O18&lt;10,"0",""),O18)</f>
+      <c r="A18" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P18&lt;10,"0",""),P18)</f>
         <v>q16</v>
       </c>
       <c r="B18" s="164" t="str">
@@ -7753,41 +7782,42 @@
         <v>qbank01</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="D18" s="187"/>
+        <v>723</v>
+      </c>
+      <c r="D18" s="188"/>
       <c r="E18" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F18" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G18" s="180" t="s">
-        <v>768</v>
-      </c>
-      <c r="H18" s="181" t="s">
-        <v>779</v>
-      </c>
-      <c r="I18" s="182"/>
-      <c r="J18" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G18" s="181" t="s">
+        <v>769</v>
+      </c>
+      <c r="H18" s="182" t="s">
         <v>780</v>
       </c>
-      <c r="K18" s="182"/>
+      <c r="I18" s="183"/>
+      <c r="J18" s="182" t="s">
+        <v>781</v>
+      </c>
+      <c r="K18" s="183"/>
       <c r="L18" s="88">
         <v>1</v>
       </c>
-      <c r="M18" s="181" t="s">
-        <v>781</v>
-      </c>
-      <c r="N18" s="184"/>
-      <c r="O18" s="183">
-        <f>O17+1</f>
+      <c r="M18" s="182" t="s">
+        <v>782</v>
+      </c>
+      <c r="N18" s="182"/>
+      <c r="O18" s="185"/>
+      <c r="P18" s="184">
+        <f>P17+1</f>
         <v>16</v>
       </c>
     </row>
     <row r="19" ht="213.75">
-      <c r="A19" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O19&lt;10,"0",""),O19)</f>
+      <c r="A19" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P19&lt;10,"0",""),P19)</f>
         <v>q17</v>
       </c>
       <c r="B19" s="164" t="str">
@@ -7795,41 +7825,42 @@
         <v>qbank01</v>
       </c>
       <c r="C19" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="D19" s="187"/>
+        <v>723</v>
+      </c>
+      <c r="D19" s="188"/>
       <c r="E19" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F19" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G19" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H19" s="181" t="s">
-        <v>782</v>
-      </c>
-      <c r="I19" s="182"/>
-      <c r="J19" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G19" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H19" s="182" t="s">
         <v>783</v>
       </c>
-      <c r="K19" s="182"/>
+      <c r="I19" s="183"/>
+      <c r="J19" s="182" t="s">
+        <v>784</v>
+      </c>
+      <c r="K19" s="183"/>
       <c r="L19" s="88">
         <v>3</v>
       </c>
-      <c r="M19" s="181" t="s">
-        <v>784</v>
-      </c>
-      <c r="N19" s="184"/>
-      <c r="O19" s="183">
-        <f>O18+1</f>
+      <c r="M19" s="182" t="s">
+        <v>785</v>
+      </c>
+      <c r="N19" s="182"/>
+      <c r="O19" s="185"/>
+      <c r="P19" s="184">
+        <f>P18+1</f>
         <v>17</v>
       </c>
     </row>
     <row r="20" ht="242.25">
-      <c r="A20" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O20&lt;10,"0",""),O20)</f>
+      <c r="A20" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P20&lt;10,"0",""),P20)</f>
         <v>q18</v>
       </c>
       <c r="B20" s="164" t="str">
@@ -7837,41 +7868,42 @@
         <v>qbank01</v>
       </c>
       <c r="C20" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="D20" s="187"/>
+        <v>723</v>
+      </c>
+      <c r="D20" s="188"/>
       <c r="E20" s="88" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F20" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G20" s="180" t="s">
-        <v>730</v>
-      </c>
-      <c r="H20" s="181" t="s">
-        <v>785</v>
-      </c>
-      <c r="I20" s="182"/>
-      <c r="J20" s="181" t="s">
+        <v>725</v>
+      </c>
+      <c r="G20" s="181" t="s">
+        <v>731</v>
+      </c>
+      <c r="H20" s="182" t="s">
         <v>786</v>
       </c>
-      <c r="K20" s="182"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="182" t="s">
+        <v>787</v>
+      </c>
+      <c r="K20" s="183"/>
       <c r="L20" s="88">
         <v>4</v>
       </c>
-      <c r="M20" s="181" t="s">
-        <v>787</v>
-      </c>
-      <c r="N20" s="184"/>
-      <c r="O20" s="183">
-        <f>O19+1</f>
+      <c r="M20" s="182" t="s">
+        <v>788</v>
+      </c>
+      <c r="N20" s="182"/>
+      <c r="O20" s="185"/>
+      <c r="P20" s="184">
+        <f>P19+1</f>
         <v>18</v>
       </c>
     </row>
     <row r="21" ht="409.5">
-      <c r="A21" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O21&lt;10,"0",""),O21)</f>
+      <c r="A21" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P21&lt;10,"0",""),P21)</f>
         <v>q19</v>
       </c>
       <c r="B21" s="164" t="str">
@@ -7879,41 +7911,42 @@
         <v>qbank01</v>
       </c>
       <c r="C21" s="88" t="s">
-        <v>722</v>
-      </c>
-      <c r="D21" s="187"/>
+        <v>723</v>
+      </c>
+      <c r="D21" s="188"/>
       <c r="E21" s="88" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F21" s="88" t="s">
-        <v>724</v>
-      </c>
-      <c r="G21" s="180" t="s">
-        <v>775</v>
-      </c>
-      <c r="H21" s="181" t="s">
-        <v>788</v>
+        <v>725</v>
+      </c>
+      <c r="G21" s="181" t="s">
+        <v>776</v>
+      </c>
+      <c r="H21" s="182" t="s">
+        <v>789</v>
       </c>
       <c r="I21" s="88"/>
-      <c r="J21" s="181" t="s">
-        <v>789</v>
+      <c r="J21" s="182" t="s">
+        <v>790</v>
       </c>
       <c r="K21" s="88"/>
       <c r="L21" s="88">
         <v>4</v>
       </c>
-      <c r="M21" s="181" t="s">
-        <v>790</v>
-      </c>
-      <c r="N21" s="88"/>
-      <c r="O21" s="183">
-        <f>O20+1</f>
+      <c r="M21" s="182" t="s">
+        <v>791</v>
+      </c>
+      <c r="N21" s="182"/>
+      <c r="O21" s="88"/>
+      <c r="P21" s="184">
+        <f>P20+1</f>
         <v>19</v>
       </c>
     </row>
     <row r="22" ht="114">
-      <c r="A22" s="179" t="str">
-        <f>_xlfn.CONCAT("q",IF(O22&lt;10,"0",""),O22)</f>
+      <c r="A22" s="180" t="str">
+        <f>_xlfn.CONCAT("q",IF(P22&lt;10,"0",""),P22)</f>
         <v>q20</v>
       </c>
       <c r="B22" s="164" t="str">
@@ -7921,33 +7954,36 @@
         <v>qbank01</v>
       </c>
       <c r="C22" s="88" t="s">
-        <v>791</v>
-      </c>
-      <c r="D22" s="187"/>
+        <v>792</v>
+      </c>
+      <c r="D22" s="188"/>
       <c r="E22" s="88" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F22" s="89"/>
-      <c r="G22" s="186" t="s">
-        <v>741</v>
-      </c>
-      <c r="H22" s="181" t="s">
-        <v>792</v>
-      </c>
-      <c r="I22" s="185" t="s">
+      <c r="G22" s="187" t="s">
+        <v>742</v>
+      </c>
+      <c r="H22" s="182" t="s">
+        <v>793</v>
+      </c>
+      <c r="I22" s="186" t="s">
         <v>315</v>
       </c>
-      <c r="J22" s="181" t="s">
-        <v>793</v>
-      </c>
-      <c r="K22" s="182"/>
-      <c r="L22" s="188"/>
+      <c r="J22" s="182" t="s">
+        <v>794</v>
+      </c>
+      <c r="K22" s="183"/>
+      <c r="L22" s="189"/>
       <c r="M22" s="144"/>
-      <c r="N22" s="89" t="s">
+      <c r="N22" s="144" t="s">
+        <v>795</v>
+      </c>
+      <c r="O22" s="89" t="s">
         <v>392</v>
       </c>
-      <c r="O22" s="189">
-        <f>O21+1</f>
+      <c r="P22" s="190">
+        <f>P21+1</f>
         <v>20</v>
       </c>
     </row>
@@ -8797,8 +8833,8 @@
         <v>127</v>
       </c>
       <c r="Z8" s="67"/>
-      <c r="AA8" s="67" t="s">
-        <v>127</v>
+      <c r="AA8" s="70" t="s">
+        <v>130</v>
       </c>
       <c r="AB8" s="67" t="s">
         <v>135</v>
@@ -9810,37 +9846,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{002A0027-0071-4BD4-A583-005B00070058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CD0068-0039-4B55-9539-00C00016002F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE00A8-000F-4085-9A26-007F00060072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0060000C-00EF-47DD-80EC-00EC004E007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE0006-00CF-482E-B97B-00C800FC000E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A90044-00AC-4E76-BA5D-003000230055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006500A1-0034-4427-889D-00EA004900BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001F005A-007E-400E-AE41-0047009900D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AC00D5-00D3-47FF-AB55-00A6005900D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D0009D-00A7-4297-BC47-0015000F0053}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001200BB-004C-4DBA-B0B3-00E9002500AC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00780067-006E-4A2D-AB2D-008B00230072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -11048,31 +11084,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0046004C-00E4-475C-9C18-008B008800BE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0002002E-005C-401D-88B0-00F3004A00E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00650021-0049-40D2-BEB4-00B3007C00AA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000400BC-00CF-414D-982B-00F9001F003D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003800F2-00C5-47C1-BE1C-004800E20088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D0003D-0074-4250-8494-001B00440025}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000500A1-00D9-47F8-80BC-00A400A40099}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0018008B-00DE-40EB-B466-00850050002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006F0097-00E0-4698-94BD-005A00A70075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00620031-0046-42AB-B9A0-00E20034004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -11223,7 +11259,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0007008B-0009-43DB-B118-009200900060}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003B00C0-0082-4796-AD80-00C500B20081}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -11357,13 +11393,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0030001F-008E-44CA-BB85-00B20018004E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00980060-004D-49FB-82DD-003100500089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003900FB-0006-4BF5-8F35-0040004500BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009C0094-00DB-4488-A55D-00E200A60065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
UPDATED: Exposes "saveTest" to external plugins, in order to create Tests from MVP-template
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="16"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="825">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -2253,9 +2253,6 @@
     <t>elementary</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t xml:space="preserve">¿En qué continente vive más gente?</t>
   </si>
   <si>
@@ -2382,9 +2379,6 @@
     <t xml:space="preserve">¿Las mujeres pueden quedarse embarazadas a cualquier edad?</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Indica cuál de los siguientes países tiene una TASA DE NATALIDAD muy BAJA.</t>
   </si>
   <si>
@@ -2416,6 +2410,9 @@
   </si>
   <si>
     <t xml:space="preserve">upper intermediate</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t xml:space="preserve">¿Qué es el CRECIMIENTO NATURAL O VEGETATIVO?</t>
@@ -2584,18 +2581,18 @@
 |Cuenca.</t>
   </si>
   <si>
+    <t>useAllQuestions</t>
+  </si>
+  <si>
+    <t>questions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feature image</t>
   </si>
   <si>
     <t xml:space="preserve">Use all questions</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of questions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select by tag</t>
-  </si>
-  <si>
     <t>Questions</t>
   </si>
   <si>
@@ -2620,10 +2617,10 @@
     <t>learn</t>
   </si>
   <si>
-    <t xml:space="preserve">map | monoresponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q001 |Q008 |Q009 |Q020</t>
+    <t>q01|q08|q09|q20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Cuánto sabes de este tema?</t>
   </si>
   <si>
     <t>test02</t>
@@ -2644,7 +2641,7 @@
     <t>#d9b68c</t>
   </si>
   <si>
-    <t xml:space="preserve">Q002 |Q004 |Q006 |Q007 |Q010 |Q011 |Q012 |Q017 |Q018</t>
+    <t>q02|q04|q06|q07|q10|q11|q12|q17|q18</t>
   </si>
 </sst>
 </file>
@@ -4929,13 +4926,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00B600B8-0048-420D-85A4-001B00FD0029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A300A0-0093-421F-9BC1-00E2001C0032}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E4002B-00CC-41A4-8D02-00C7006E004D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0075000B-0012-4567-BA6A-003500B40094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5080,7 +5077,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0083006D-0022-40BF-AE4A-00A200190014}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004600BF-0077-4DF4-AC73-00D600B4002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7233,26 +7230,26 @@
       <c r="E3" s="79" t="s">
         <v>726</v>
       </c>
-      <c r="F3" s="79" t="s">
-        <v>727</v>
+      <c r="F3" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G3" s="180"/>
       <c r="H3" s="181" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I3" s="79"/>
       <c r="J3" s="181" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="K3" s="182"/>
       <c r="L3" s="79">
         <v>1</v>
       </c>
       <c r="M3" s="181" t="s">
+        <v>729</v>
+      </c>
+      <c r="N3" s="181" t="s">
         <v>730</v>
-      </c>
-      <c r="N3" s="181" t="s">
-        <v>731</v>
       </c>
       <c r="O3" s="79"/>
       <c r="P3" s="183">
@@ -7272,31 +7269,31 @@
         <v>724</v>
       </c>
       <c r="D4" s="79" t="s">
+        <v>731</v>
+      </c>
+      <c r="E4" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E4" s="79" t="s">
-        <v>733</v>
-      </c>
-      <c r="F4" s="79" t="s">
-        <v>727</v>
+      <c r="F4" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G4" s="180"/>
       <c r="H4" s="181" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I4" s="79"/>
       <c r="J4" s="181" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K4" s="79"/>
       <c r="L4" s="79">
         <v>4</v>
       </c>
       <c r="M4" s="181" t="s">
+        <v>735</v>
+      </c>
+      <c r="N4" s="181" t="s">
         <v>736</v>
-      </c>
-      <c r="N4" s="181" t="s">
-        <v>737</v>
       </c>
       <c r="O4" s="79"/>
       <c r="P4" s="183">
@@ -7320,28 +7317,28 @@
         <v>725</v>
       </c>
       <c r="E5" s="79" t="s">
-        <v>733</v>
-      </c>
-      <c r="F5" s="79" t="s">
-        <v>727</v>
+        <v>732</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G5" s="180"/>
       <c r="H5" s="181" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="181" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="K5" s="79"/>
       <c r="L5" s="79">
         <v>3</v>
       </c>
       <c r="M5" s="181" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N5" s="181" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="O5" s="79"/>
       <c r="P5" s="183">
@@ -7362,31 +7359,31 @@
         <v>724</v>
       </c>
       <c r="D6" s="79" t="s">
+        <v>731</v>
+      </c>
+      <c r="E6" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E6" s="79" t="s">
-        <v>733</v>
-      </c>
-      <c r="F6" s="79" t="s">
-        <v>727</v>
+      <c r="F6" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G6" s="180"/>
       <c r="H6" s="181" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I6" s="79"/>
       <c r="J6" s="181" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="K6" s="79"/>
       <c r="L6" s="79">
         <v>2</v>
       </c>
       <c r="M6" s="181" t="s">
+        <v>742</v>
+      </c>
+      <c r="N6" s="181" t="s">
         <v>743</v>
-      </c>
-      <c r="N6" s="181" t="s">
-        <v>744</v>
       </c>
       <c r="O6" s="79"/>
       <c r="P6" s="183">
@@ -7410,28 +7407,28 @@
         <v>725</v>
       </c>
       <c r="E7" s="79" t="s">
-        <v>733</v>
-      </c>
-      <c r="F7" s="79" t="s">
-        <v>727</v>
+        <v>732</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G7" s="180"/>
       <c r="H7" s="181" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="I7" s="79"/>
       <c r="J7" s="181" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="K7" s="79"/>
       <c r="L7" s="79">
         <v>1</v>
       </c>
       <c r="M7" s="181" t="s">
+        <v>746</v>
+      </c>
+      <c r="N7" s="181" t="s">
         <v>747</v>
-      </c>
-      <c r="N7" s="181" t="s">
-        <v>748</v>
       </c>
       <c r="O7" s="79"/>
       <c r="P7" s="183">
@@ -7452,31 +7449,31 @@
         <v>724</v>
       </c>
       <c r="D8" s="79" t="s">
+        <v>731</v>
+      </c>
+      <c r="E8" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E8" s="79" t="s">
-        <v>733</v>
-      </c>
-      <c r="F8" s="79" t="s">
-        <v>727</v>
+      <c r="F8" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G8" s="180"/>
       <c r="H8" s="181" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="I8" s="182"/>
       <c r="J8" s="181" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="K8" s="79"/>
       <c r="L8" s="79">
         <v>2</v>
       </c>
       <c r="M8" s="181" t="s">
+        <v>750</v>
+      </c>
+      <c r="N8" s="181" t="s">
         <v>751</v>
-      </c>
-      <c r="N8" s="181" t="s">
-        <v>752</v>
       </c>
       <c r="O8" s="184"/>
       <c r="P8" s="183">
@@ -7497,31 +7494,31 @@
         <v>724</v>
       </c>
       <c r="D9" s="79" t="s">
+        <v>731</v>
+      </c>
+      <c r="E9" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E9" s="79" t="s">
-        <v>733</v>
-      </c>
-      <c r="F9" s="79" t="s">
-        <v>727</v>
+      <c r="F9" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G9" s="180"/>
       <c r="H9" s="181" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="I9" s="182"/>
       <c r="J9" s="181" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="K9" s="79"/>
       <c r="L9" s="79">
         <v>3</v>
       </c>
       <c r="M9" s="181" t="s">
+        <v>754</v>
+      </c>
+      <c r="N9" s="181" t="s">
         <v>755</v>
-      </c>
-      <c r="N9" s="181" t="s">
-        <v>756</v>
       </c>
       <c r="O9" s="79"/>
       <c r="P9" s="183">
@@ -7547,23 +7544,23 @@
       <c r="E10" s="79" t="s">
         <v>726</v>
       </c>
-      <c r="F10" s="79" t="s">
-        <v>757</v>
+      <c r="F10" s="67" t="s">
+        <v>9</v>
       </c>
       <c r="G10" s="180"/>
       <c r="H10" s="181" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="I10" s="79"/>
       <c r="J10" s="79"/>
       <c r="K10" s="81" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="L10" s="79">
         <v>2</v>
       </c>
       <c r="M10" s="181" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="N10" s="181"/>
       <c r="O10" s="79"/>
@@ -7590,28 +7587,28 @@
       <c r="E11" s="79" t="s">
         <v>726</v>
       </c>
-      <c r="F11" s="79" t="s">
-        <v>727</v>
+      <c r="F11" s="67" t="s">
+        <v>10</v>
       </c>
       <c r="G11" s="180"/>
       <c r="H11" s="181" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I11" s="81" t="s">
         <v>312</v>
       </c>
       <c r="J11" s="181" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="K11" s="79"/>
       <c r="L11" s="79">
         <v>1</v>
       </c>
       <c r="M11" s="181" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="N11" s="181" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="O11" s="79"/>
       <c r="P11" s="183">
@@ -7632,31 +7629,31 @@
         <v>724</v>
       </c>
       <c r="D12" s="79" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E12" s="79" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F12" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G12" s="180"/>
       <c r="H12" s="181" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="101" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="K12" s="79"/>
       <c r="L12" s="79">
         <v>4</v>
       </c>
       <c r="M12" s="181" t="s">
+        <v>767</v>
+      </c>
+      <c r="N12" s="181" t="s">
         <v>768</v>
-      </c>
-      <c r="N12" s="181" t="s">
-        <v>769</v>
       </c>
       <c r="O12" s="79"/>
       <c r="P12" s="183">
@@ -7677,31 +7674,31 @@
         <v>724</v>
       </c>
       <c r="D13" s="79" t="s">
+        <v>731</v>
+      </c>
+      <c r="E13" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E13" s="79" t="s">
-        <v>733</v>
-      </c>
       <c r="F13" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G13" s="180"/>
       <c r="H13" s="181" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="181" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="K13" s="79"/>
       <c r="L13" s="79">
         <v>3</v>
       </c>
       <c r="M13" s="181" t="s">
+        <v>771</v>
+      </c>
+      <c r="N13" s="181" t="s">
         <v>772</v>
-      </c>
-      <c r="N13" s="181" t="s">
-        <v>773</v>
       </c>
       <c r="O13" s="79"/>
       <c r="P13" s="183">
@@ -7722,28 +7719,28 @@
         <v>724</v>
       </c>
       <c r="D14" s="79" t="s">
+        <v>731</v>
+      </c>
+      <c r="E14" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E14" s="79" t="s">
-        <v>733</v>
-      </c>
       <c r="F14" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G14" s="180"/>
       <c r="H14" s="181" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I14" s="79"/>
       <c r="J14" s="181" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="K14" s="79"/>
       <c r="L14" s="79">
         <v>1</v>
       </c>
       <c r="M14" s="181" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="N14" s="181"/>
       <c r="O14" s="79"/>
@@ -7768,27 +7765,27 @@
         <v>725</v>
       </c>
       <c r="E15" s="79" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F15" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G15" s="180"/>
       <c r="H15" s="181" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I15" s="79" t="s">
         <v>338</v>
       </c>
       <c r="J15" s="181" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="K15" s="182"/>
       <c r="L15" s="79">
         <v>2</v>
       </c>
       <c r="M15" s="181" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="N15" s="181"/>
       <c r="O15" s="79"/>
@@ -7813,27 +7810,27 @@
         <v>725</v>
       </c>
       <c r="E16" s="79" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F16" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G16" s="180"/>
       <c r="H16" s="181" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I16" s="79" t="s">
         <v>338</v>
       </c>
       <c r="J16" s="181" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="K16" s="182"/>
       <c r="L16" s="79">
         <v>1</v>
       </c>
       <c r="M16" s="181" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="N16" s="181"/>
       <c r="O16" s="184"/>
@@ -7858,25 +7855,25 @@
         <v>725</v>
       </c>
       <c r="E17" s="79" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F17" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G17" s="180"/>
       <c r="H17" s="181" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I17" s="182"/>
       <c r="J17" s="181" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="K17" s="182"/>
       <c r="L17" s="79">
         <v>2</v>
       </c>
       <c r="M17" s="181" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="N17" s="181"/>
       <c r="O17" s="184"/>
@@ -7901,25 +7898,25 @@
         <v>725</v>
       </c>
       <c r="E18" s="79" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F18" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G18" s="180"/>
       <c r="H18" s="181" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="I18" s="182"/>
       <c r="J18" s="181" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="K18" s="182"/>
       <c r="L18" s="79">
         <v>1</v>
       </c>
       <c r="M18" s="181" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="N18" s="181"/>
       <c r="O18" s="184"/>
@@ -7941,31 +7938,31 @@
         <v>724</v>
       </c>
       <c r="D19" s="185" t="s">
+        <v>731</v>
+      </c>
+      <c r="E19" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E19" s="79" t="s">
-        <v>733</v>
-      </c>
       <c r="F19" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G19" s="180"/>
       <c r="H19" s="181" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="I19" s="182"/>
       <c r="J19" s="181" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="K19" s="182"/>
       <c r="L19" s="79">
         <v>3</v>
       </c>
       <c r="M19" s="181" t="s">
+        <v>790</v>
+      </c>
+      <c r="N19" s="181" t="s">
         <v>791</v>
-      </c>
-      <c r="N19" s="181" t="s">
-        <v>792</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="183">
@@ -7986,31 +7983,31 @@
         <v>724</v>
       </c>
       <c r="D20" s="185" t="s">
+        <v>731</v>
+      </c>
+      <c r="E20" s="79" t="s">
         <v>732</v>
       </c>
-      <c r="E20" s="79" t="s">
-        <v>733</v>
-      </c>
       <c r="F20" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G20" s="180"/>
       <c r="H20" s="181" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="I20" s="182"/>
       <c r="J20" s="181" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="K20" s="182"/>
       <c r="L20" s="79">
         <v>4</v>
       </c>
       <c r="M20" s="181" t="s">
+        <v>794</v>
+      </c>
+      <c r="N20" s="181" t="s">
         <v>795</v>
-      </c>
-      <c r="N20" s="181" t="s">
-        <v>796</v>
       </c>
       <c r="O20" s="184"/>
       <c r="P20" s="183">
@@ -8031,31 +8028,31 @@
         <v>724</v>
       </c>
       <c r="D21" s="185" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E21" s="79" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F21" s="79" t="s">
-        <v>727</v>
+        <v>764</v>
       </c>
       <c r="G21" s="180"/>
       <c r="H21" s="181" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="I21" s="79"/>
       <c r="J21" s="181" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K21" s="79"/>
       <c r="L21" s="79">
         <v>4</v>
       </c>
       <c r="M21" s="181" t="s">
+        <v>799</v>
+      </c>
+      <c r="N21" s="181" t="s">
         <v>800</v>
-      </c>
-      <c r="N21" s="181" t="s">
-        <v>801</v>
       </c>
       <c r="O21" s="79"/>
       <c r="P21" s="183">
@@ -8073,10 +8070,10 @@
         <v>qbank01</v>
       </c>
       <c r="C22" s="79" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D22" s="185" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E22" s="79" t="s">
         <v>726</v>
@@ -8084,13 +8081,13 @@
       <c r="F22" s="76"/>
       <c r="G22" s="101"/>
       <c r="H22" s="181" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I22" s="81" t="s">
         <v>315</v>
       </c>
       <c r="J22" s="181" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K22" s="182"/>
       <c r="L22" s="186"/>
@@ -8116,6 +8113,66 @@
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9" disablePrompts="0">
+        <x14:dataValidation xr:uid="{00660009-00C9-4C7F-A133-000D002A0012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000B0052-0029-4AD1-ACF5-00BA00130017}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00B50090-00A2-4FDE-9033-004C00440082}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003800F9-0044-4008-A070-0016000900E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{006A0002-0024-4732-B4F4-00450032002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00510047-0023-4790-9EB8-00AC008C007D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{006D0088-00B3-4300-885F-006A005E0096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008E0088-0038-4924-B341-009100140039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{009900B0-00C8-4BB3-AD8C-002400940065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8127,13 +8184,14 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.140625"/>
+    <col customWidth="1" min="2" max="2" width="14.57421875"/>
     <col customWidth="1" min="3" max="3" width="24.8515625"/>
     <col customWidth="1" min="4" max="4" width="32.8515625"/>
     <col customWidth="1" min="5" max="5" width="41.7109375"/>
@@ -8143,10 +8201,8 @@
     <col customWidth="1" min="10" max="10" width="13.8515625"/>
     <col min="11" max="12" style="90" width="9.140625"/>
     <col customWidth="1" min="13" max="13" style="90" width="13.57421875"/>
-    <col customWidth="1" min="14" max="14" style="90" width="12.7109375"/>
-    <col customWidth="1" min="15" max="15" width="20.8515625"/>
-    <col customWidth="1" min="17" max="17" width="17.8515625"/>
-    <col customWidth="1" min="18" max="18" style="153" width="19.140625"/>
+    <col customWidth="1" min="14" max="14" style="153" width="37.421875"/>
+    <col customWidth="1" min="15" max="15" width="43.7109375"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -8186,6 +8242,18 @@
       <c r="L1" s="5" t="s">
         <v>580</v>
       </c>
+      <c r="M1" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="2" s="153" customFormat="1" ht="28.5">
       <c r="A2" s="133" t="s">
@@ -8211,7 +8279,7 @@
         <v>260</v>
       </c>
       <c r="H2" s="113" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="I2" s="188" t="str">
         <f>PROPER(I1)</f>
@@ -8228,46 +8296,44 @@
         <v>599</v>
       </c>
       <c r="M2" s="132" t="s">
-        <v>806</v>
-      </c>
-      <c r="N2" s="132" t="s">
         <v>807</v>
       </c>
-      <c r="O2" s="113" t="s">
-        <v>430</v>
-      </c>
-      <c r="P2" s="113" t="s">
-        <v>703</v>
-      </c>
-      <c r="Q2" s="113" t="s">
+      <c r="N2" s="189" t="s">
         <v>808</v>
       </c>
-      <c r="R2" s="189" t="s">
+      <c r="O2" s="189" t="str">
+        <f>PROPER(O1)</f>
+        <v>Statement</v>
+      </c>
+      <c r="P2" s="188" t="str">
+        <f>PROPER(P1)</f>
+        <v>Creator</v>
+      </c>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+    </row>
+    <row r="3" s="74" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A3" s="179" t="s">
         <v>809</v>
-      </c>
-    </row>
-    <row r="3" s="74" customFormat="1" ht="27">
-      <c r="A3" s="179" t="s">
-        <v>810</v>
       </c>
       <c r="B3" s="165" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
       <c r="C3" s="74" t="s">
+        <v>810</v>
+      </c>
+      <c r="D3" s="74" t="s">
         <v>811</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="E3" s="162" t="s">
         <v>812</v>
       </c>
-      <c r="E3" s="162" t="s">
+      <c r="F3" s="74" t="s">
         <v>813</v>
       </c>
-      <c r="F3" s="74" t="s">
+      <c r="G3" s="74" t="s">
         <v>814</v>
-      </c>
-      <c r="G3" s="74" t="s">
-        <v>815</v>
       </c>
       <c r="H3" s="74" t="s">
         <v>272</v>
@@ -8280,48 +8346,48 @@
         <v>700</v>
       </c>
       <c r="K3" s="190" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="L3" s="67" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="190">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="N3" s="173" t="s">
+        <v>816</v>
       </c>
       <c r="O3" s="74" t="s">
         <v>817</v>
       </c>
-      <c r="P3" s="74"/>
+      <c r="P3" s="171" t="s">
+        <v>163</v>
+      </c>
       <c r="Q3" s="74"/>
-      <c r="R3" s="173" t="s">
+      <c r="R3" s="74"/>
+    </row>
+    <row r="4" s="74" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A4" s="179" t="s">
         <v>818</v>
-      </c>
-    </row>
-    <row r="4" s="74" customFormat="1" ht="40.5">
-      <c r="A4" s="179" t="s">
-        <v>819</v>
       </c>
       <c r="B4" s="165" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
       <c r="C4" s="74" t="s">
+        <v>819</v>
+      </c>
+      <c r="D4" s="74" t="s">
         <v>820</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="E4" s="162" t="s">
         <v>821</v>
       </c>
-      <c r="E4" s="162" t="s">
+      <c r="F4" s="74" t="s">
         <v>822</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="G4" s="74" t="s">
         <v>823</v>
-      </c>
-      <c r="G4" s="74" t="s">
-        <v>824</v>
       </c>
       <c r="H4" s="74" t="s">
         <v>412</v>
@@ -8334,25 +8400,25 @@
         <v>700</v>
       </c>
       <c r="K4" s="190" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="L4" s="67" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="190">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="N4" s="173" t="s">
+        <v>824</v>
       </c>
       <c r="O4" s="74" t="s">
         <v>817</v>
       </c>
-      <c r="P4" s="74"/>
+      <c r="P4" s="171" t="s">
+        <v>163</v>
+      </c>
       <c r="Q4" s="74"/>
-      <c r="R4" s="173" t="s">
-        <v>825</v>
-      </c>
+      <c r="R4" s="74"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -8362,25 +8428,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0062005C-0068-4500-BEFB-00E70021005D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C8008B-00E4-4C2E-AD55-00D200490074}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CE005D-00F0-4C9C-9336-00B300DC00FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001A0025-005E-4EA9-B683-007A008D004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C900C6-0002-43AB-8E6A-00F800FF003E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008D001C-0093-4D36-A344-00F200370079}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>M3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F000E3-0018-441F-99FD-002E006400A5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00580070-00DC-4FE6-88DE-0099006000A6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -10227,37 +10293,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00B30098-0007-435E-A3CC-003500C700D9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AD0073-0039-46E6-AFD4-005700F90010}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C2000A-001C-4C5C-B2E1-008800340044}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C9001D-0055-4388-A9F4-002B006E001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EF00C5-00D3-40D7-BCAF-008D006D0004}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009100B6-000C-4275-BF33-00A2001800D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005F006C-00C5-4219-AB75-002B00B50060}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00530072-0054-498B-830F-00D5007C00EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009F00A7-00B4-4049-9FCC-00EE00B30099}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005800CD-00C9-47AA-9C72-001A002C0012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE0096-002D-49B6-8037-00B6002400F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001C00F0-003E-4C0A-B154-0066002C0071}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -11465,31 +11531,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00F2007E-00C2-486E-8127-00E5002D00A7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008A00CC-005A-4752-8B01-0068003B0091}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D4007B-007E-4E2B-850D-0047009800DD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00480088-0037-4575-AD10-002D00190059}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00270048-0025-41EF-8CC6-00DF00F500AD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D500BC-00D0-4047-89A0-008C004E0067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E100CE-009F-4269-BC7A-0016004E008D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000E0099-0007-460D-BBD9-00B200C40039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001B0073-00F5-4E66-8B1C-000E009E0094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00810037-006A-42B9-8F8A-008A008D0070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -11640,7 +11706,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00F000A2-005C-49F7-9082-00D600000018}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005600D4-0047-4CF8-A003-00EB00B500AF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -11774,13 +11840,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00DA003D-00C5-4161-9154-00E800D000CD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EE0047-0029-4909-AD29-00EB0038002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E30054-0004-454D-BAE1-00C300E70005}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002B00DA-0057-4F5D-829B-005900290071}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
FINISH: MVP-template Tests bulk loading FIXED: several plugins menu item icons
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="17"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="883">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -2160,21 +2160,102 @@
     <t xml:space="preserve">Asegúrate de comprender bien estos conceptos porque vas a necesitar manejarlos bien en un debate próximo.</t>
   </si>
   <si>
+    <t>published</t>
+  </si>
+  <si>
     <t>qbank01</t>
   </si>
   <si>
-    <t xml:space="preserve">Demografía 2ºESO</t>
-  </si>
-  <si>
-    <t>#fabada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demografía, preguntas, eso</t>
+    <t>Demografía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2º ESO</t>
+  </si>
+  <si>
+    <t>#e6e0b3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">población, demografía</t>
   </si>
   <si>
     <t>asignatura02</t>
   </si>
   <si>
+    <t>qbank02</t>
+  </si>
+  <si>
+    <t>Románico</t>
+  </si>
+  <si>
+    <t>#8cbdd9</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/romanico_42b518af26.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arte, Edad Media, románico, Europa</t>
+  </si>
+  <si>
+    <t>qbank03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulaire français 2ESO</t>
+  </si>
+  <si>
+    <t>#669ecc</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/vocabulaire_184e02ab44.png</t>
+  </si>
+  <si>
+    <t>asignatura09</t>
+  </si>
+  <si>
+    <t>qbank04</t>
+  </si>
+  <si>
+    <t>Feudalismo</t>
+  </si>
+  <si>
+    <t>#995c33</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/castillo_medieval_87dd37d23f.gif</t>
+  </si>
+  <si>
+    <t>qbank05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grammaire 1ESO</t>
+  </si>
+  <si>
+    <t>#4091bf</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/grammaire_a8b0d428c5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verbes, grammaire</t>
+  </si>
+  <si>
+    <t>qbank06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barroco italiano</t>
+  </si>
+  <si>
+    <t>Bachillerato</t>
+  </si>
+  <si>
+    <t>#bf40b0</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/barroco_italia_f8a7412e68.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arte, Edad Moderna, Barroco, Italia</t>
+  </si>
+  <si>
     <t>qbank</t>
   </si>
   <si>
@@ -2251,6 +2332,9 @@
   </si>
   <si>
     <t>elementary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, continentes</t>
   </si>
   <si>
     <t xml:space="preserve">¿En qué continente vive más gente?</t>
@@ -2274,6 +2358,9 @@
     <t>intermediate</t>
   </si>
   <si>
+    <t xml:space="preserve">demografía, vocabulario</t>
+  </si>
+  <si>
     <t xml:space="preserve">¿Qué es la POBLACIÓN?</t>
   </si>
   <si>
@@ -2292,6 +2379,9 @@
     <t xml:space="preserve">Aunque la inmigración es importante en estudios de demografía, NO DEFINE qué es la población.</t>
   </si>
   <si>
+    <t xml:space="preserve">demografía, países</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cita los tres países que más población tienen.</t>
   </si>
   <si>
@@ -2325,6 +2415,9 @@
     <t xml:space="preserve">No confundas la densidad de población (población relativa) con la población absoluta. </t>
   </si>
   <si>
+    <t xml:space="preserve">demografía, España</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cita las dos provincias españolas con MAYOR DENSIDAD DE POBLACIÓN.</t>
   </si>
   <si>
@@ -2462,6 +2555,9 @@
 |2@Esa tesis pertenece a los poblacionistas, no a los neomalthusianos.</t>
   </si>
   <si>
+    <t xml:space="preserve">demografía, análisis de datos</t>
+  </si>
+  <si>
     <t xml:space="preserve">Observa la siguiente pirámide de población y responde: ¿La TASA DE NATALIDAD es alta o baja?</t>
   </si>
   <si>
@@ -2480,6 +2576,9 @@
   </si>
   <si>
     <t xml:space="preserve">1@Se observa que en las barras superiores (que indican las personas vivas en esos rangos de edad, las barras de la derecha (que hacen referencia a las mujeres) son más largas, lo que quiere decir que hay más mujeres vivas en esa edad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demografía, inmigración</t>
   </si>
   <si>
     <t xml:space="preserve">¿Cómo se calcula el CRECIMIENTO REAL de la población en un país?</t>
@@ -2581,6 +2680,9 @@
 |Cuenca.</t>
   </si>
   <si>
+    <t>questionBank</t>
+  </si>
+  <si>
     <t>useAllQuestions</t>
   </si>
   <si>
@@ -2599,16 +2701,10 @@
     <t>test01</t>
   </si>
   <si>
-    <t xml:space="preserve">Repaso población elemental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vocabulario 2º Gª Hª</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preguntas para repasar demografía con ACNEAE.</t>
-  </si>
-  <si>
-    <t>ACNEAE</t>
+    <t xml:space="preserve">Conceptos básicos de demografía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concdeptos básicos de demografía, 2º ESO</t>
   </si>
   <si>
     <t>#4057bf</t>
@@ -2626,22 +2722,100 @@
     <t>test02</t>
   </si>
   <si>
-    <t xml:space="preserve">Repaso vocabulario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repaso vocabulario 2º Geografía e Historia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repaso de todo el vocabulario de Gª e Hª 2º ESO.</t>
-  </si>
-  <si>
-    <t>vocabulario</t>
+    <t xml:space="preserve">Demografía: vocavulario básico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repaso de vocabulario de demografía de 2º ESO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vocabulario, demografía</t>
   </si>
   <si>
     <t>#d9b68c</t>
   </si>
   <si>
     <t>q02|q04|q06|q07|q10|q11|q12|q17|q18</t>
+  </si>
+  <si>
+    <t>test03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arquitectura románica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arte, románico, arquitectura</t>
+  </si>
+  <si>
+    <t>#d98c8c</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/alzado_romanico_dc8dae7e3b.png</t>
+  </si>
+  <si>
+    <t>test04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulaire: Mon école</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vocabulaire, école, lycée</t>
+  </si>
+  <si>
+    <t>#4d1a1a</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/mon_ecole_230b74a701.png</t>
+  </si>
+  <si>
+    <t>test05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Camino de Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edad Media, Camino nde Sanbtiago, Románico, arquitectura</t>
+  </si>
+  <si>
+    <t>#a8bf40</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/santiago_4f314525c3.jpeg</t>
+  </si>
+  <si>
+    <t>test06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grammaire: Le présent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1º ESO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grammaire, verbes, présent</t>
+  </si>
+  <si>
+    <t>#cc6666</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/verbe_aimer_76039c54a5.png</t>
+  </si>
+  <si>
+    <t>test07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arquitectura barroca italiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2º Bachillerato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arte, barroco, Italia</t>
+  </si>
+  <si>
+    <t>#40b7bf</t>
+  </si>
+  <si>
+    <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/cupula_borromini_51bd61a526.png</t>
   </si>
 </sst>
 </file>
@@ -2925,7 +3099,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -3262,12 +3436,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="192">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3775,15 +3962,18 @@
     <xf fontId="11" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="11" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="11" fillId="4" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3793,9 +3983,6 @@
     </xf>
     <xf fontId="11" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3807,7 +3994,6 @@
     <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="11" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -3821,8 +4007,14 @@
     <xf fontId="5" fillId="16" borderId="27" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="11" fillId="4" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="11" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="11" fillId="4" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4926,13 +5118,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00A300A0-0093-421F-9BC1-00E2001C0032}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00990062-00AA-432B-AF7F-003000D800F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0075000B-0012-4567-BA6A-003500B40094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00150011-00EA-4365-A2E1-009D004A00A3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5077,7 +5269,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{004600BF-0077-4DF4-AC73-00D600B4002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CB00FA-00B1-4C68-9554-009E00190082}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -6954,7 +7146,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6964,7 +7156,8 @@
     <col customWidth="1" min="3" max="3" width="16.00390625"/>
     <col customWidth="1" min="4" max="4" width="22.28125"/>
     <col customWidth="1" min="6" max="6" width="21.00390625"/>
-    <col customWidth="1" min="7" max="8" width="14.140625"/>
+    <col customWidth="1" min="7" max="7" width="23.28125"/>
+    <col customWidth="1" min="8" max="8" width="14.140625"/>
     <col customWidth="1" min="9" max="9" width="12.7109375"/>
     <col customWidth="1" min="10" max="10" width="25.57421875"/>
   </cols>
@@ -7000,6 +7193,9 @@
       <c r="J1" s="5" t="s">
         <v>87</v>
       </c>
+      <c r="K1" s="5" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="2" ht="24" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -7040,40 +7236,205 @@
         <f>PROPER(J1)</f>
         <v>Subjects</v>
       </c>
+      <c r="K2" s="136" t="str">
+        <f>PROPER(K1)</f>
+        <v>Published</v>
+      </c>
     </row>
     <row r="3" s="88" customFormat="1" ht="34.5" customHeight="1">
       <c r="A3" s="167" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B3" s="168" t="s">
-        <v>697</v>
-      </c>
-      <c r="C3" s="168"/>
+        <v>698</v>
+      </c>
+      <c r="C3" s="168" t="s">
+        <v>699</v>
+      </c>
       <c r="D3" s="169"/>
       <c r="E3" s="168" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="F3" s="170" t="s">
         <v>373</v>
       </c>
       <c r="G3" s="169" t="s">
+        <v>701</v>
+      </c>
+      <c r="H3" s="171" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" s="172" t="s">
+        <v>486</v>
+      </c>
+      <c r="J3" s="173" t="s">
+        <v>702</v>
+      </c>
+      <c r="K3" s="79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="27">
+      <c r="A4" s="167" t="s">
+        <v>703</v>
+      </c>
+      <c r="B4" s="168" t="s">
+        <v>704</v>
+      </c>
+      <c r="C4" s="168" t="s">
         <v>699</v>
       </c>
-      <c r="H3" s="171" t="str">
-        <f>users!A4</f>
-        <v>teacher01</v>
-      </c>
-      <c r="I3" s="172" t="str">
-        <f>ap_programs!A5</f>
-        <v>programB</v>
-      </c>
-      <c r="J3" s="173" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="168" t="s">
+        <v>705</v>
+      </c>
+      <c r="F4" s="170" t="s">
+        <v>706</v>
+      </c>
+      <c r="G4" s="169" t="s">
+        <v>707</v>
+      </c>
+      <c r="H4" s="171" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" s="172" t="s">
+        <v>486</v>
+      </c>
+      <c r="J4" s="173" t="s">
+        <v>702</v>
+      </c>
+      <c r="K4" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="27">
+      <c r="A5" s="167" t="s">
+        <v>708</v>
+      </c>
+      <c r="B5" s="168" t="s">
+        <v>709</v>
+      </c>
+      <c r="C5" s="168"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="168" t="s">
+        <v>710</v>
+      </c>
+      <c r="F5" s="170" t="s">
+        <v>711</v>
+      </c>
+      <c r="G5" s="169" t="s">
+        <v>650</v>
+      </c>
+      <c r="H5" s="171" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="172" t="s">
+        <v>486</v>
+      </c>
+      <c r="J5" s="173" t="s">
+        <v>712</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="40.5">
+      <c r="A6" s="167" t="s">
+        <v>713</v>
+      </c>
+      <c r="B6" s="168" t="s">
+        <v>714</v>
+      </c>
+      <c r="C6" s="168" t="s">
+        <v>699</v>
+      </c>
+      <c r="D6" s="169"/>
+      <c r="E6" s="168" t="s">
+        <v>715</v>
+      </c>
+      <c r="F6" s="170" t="s">
+        <v>716</v>
+      </c>
+      <c r="G6" s="169" t="s">
+        <v>664</v>
+      </c>
+      <c r="H6" s="171" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="172" t="s">
+        <v>486</v>
+      </c>
+      <c r="J6" s="173" t="s">
+        <v>702</v>
+      </c>
+      <c r="K6" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="167" t="s">
+        <v>717</v>
+      </c>
+      <c r="B7" s="168" t="s">
+        <v>718</v>
+      </c>
+      <c r="C7" s="168"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="168" t="s">
+        <v>719</v>
+      </c>
+      <c r="F7" s="170" t="s">
+        <v>720</v>
+      </c>
+      <c r="G7" s="169" t="s">
+        <v>721</v>
+      </c>
+      <c r="H7" s="171" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="172" t="s">
+        <v>486</v>
+      </c>
+      <c r="J7" s="173" t="s">
+        <v>712</v>
+      </c>
+      <c r="K7" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="27">
+      <c r="A8" s="167" t="s">
+        <v>722</v>
+      </c>
+      <c r="B8" s="168" t="s">
+        <v>723</v>
+      </c>
+      <c r="C8" s="168" t="s">
+        <v>724</v>
+      </c>
+      <c r="D8" s="169"/>
+      <c r="E8" s="168" t="s">
+        <v>725</v>
+      </c>
+      <c r="F8" s="170" t="s">
+        <v>726</v>
+      </c>
+      <c r="G8" s="169" t="s">
+        <v>727</v>
+      </c>
+      <c r="H8" s="171" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="172" t="s">
+        <v>486</v>
+      </c>
+      <c r="J8" s="173" t="s">
+        <v>702</v>
+      </c>
+      <c r="K8" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F3"/>
@@ -7082,6 +7443,48 @@
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
+        <x14:dataValidation xr:uid="{008A0051-00C6-4204-9261-006E0050000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008800A6-00F8-451F-B279-00C800D000C0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00EE00E9-0085-4669-8CD4-00B900E200DB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003D0054-009F-4080-ABC9-008900420073}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00ED0029-0001-48DE-9E2F-000800E30080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00220041-00C3-4EBA-B3CD-005600D200F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7103,18 +7506,18 @@
     <col customWidth="1" min="1" max="1" width="11.8515625"/>
     <col customWidth="1" min="2" max="2" width="15.8515625"/>
     <col customWidth="1" min="3" max="3" width="14.00390625"/>
-    <col customWidth="1" min="4" max="4" width="13.421875"/>
+    <col customWidth="1" min="4" max="4" style="174" width="13.421875"/>
     <col bestFit="1" min="5" max="5" style="174" width="17.3515625"/>
     <col bestFit="1" min="6" max="6" width="11.28125"/>
-    <col customWidth="1" min="7" max="7" width="15.57421875"/>
+    <col customWidth="1" min="7" max="7" style="175" width="14.7109375"/>
     <col customWidth="1" min="8" max="8" width="69.57421875"/>
-    <col bestFit="1" min="9" max="9" style="175" width="13.8515625"/>
+    <col bestFit="1" min="9" max="9" style="176" width="13.8515625"/>
     <col customWidth="1" min="10" max="10" width="73.140625"/>
-    <col bestFit="1" min="11" max="11" style="175" width="15.2109375"/>
+    <col bestFit="1" min="11" max="11" style="176" width="15.2109375"/>
     <col bestFit="1" min="12" max="12" width="9.921875"/>
     <col customWidth="1" min="13" max="13" width="114.28125"/>
     <col customWidth="1" min="14" max="14" width="35.7109375"/>
-    <col customWidth="1" min="15" max="15" style="175" width="23.8515625"/>
+    <col customWidth="1" min="15" max="15" style="176" width="23.8515625"/>
     <col bestFit="1" min="16" max="16" width="2.78125"/>
   </cols>
   <sheetData>
@@ -7123,46 +7526,46 @@
         <v>35</v>
       </c>
       <c r="B1" s="91" t="s">
-        <v>701</v>
+        <v>728</v>
       </c>
       <c r="C1" s="91" t="s">
         <v>426</v>
       </c>
       <c r="D1" s="91" t="s">
-        <v>702</v>
+        <v>729</v>
       </c>
       <c r="E1" s="91" t="s">
-        <v>703</v>
+        <v>730</v>
       </c>
       <c r="F1" s="91" t="s">
-        <v>704</v>
-      </c>
-      <c r="G1" s="176" t="s">
+        <v>731</v>
+      </c>
+      <c r="G1" s="177" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="177" t="s">
-        <v>705</v>
+      <c r="H1" s="178" t="s">
+        <v>732</v>
       </c>
       <c r="I1" s="91" t="s">
-        <v>706</v>
+        <v>733</v>
       </c>
       <c r="J1" s="91" t="s">
-        <v>707</v>
+        <v>734</v>
       </c>
       <c r="K1" s="91" t="s">
-        <v>708</v>
+        <v>735</v>
       </c>
       <c r="L1" s="91" t="s">
-        <v>709</v>
+        <v>736</v>
       </c>
       <c r="M1" s="91" t="s">
-        <v>710</v>
+        <v>737</v>
       </c>
       <c r="N1" s="91" t="s">
-        <v>711</v>
+        <v>738</v>
       </c>
       <c r="O1" s="91" t="s">
-        <v>712</v>
+        <v>739</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -7170,50 +7573,50 @@
         <v>39</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>713</v>
+        <v>740</v>
       </c>
       <c r="C2" s="113" t="s">
         <v>430</v>
       </c>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="132" t="s">
         <v>256</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>714</v>
+        <v>741</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>715</v>
-      </c>
-      <c r="G2" s="132" t="s">
+        <v>742</v>
+      </c>
+      <c r="G2" s="179" t="s">
         <v>155</v>
       </c>
-      <c r="H2" s="178" t="s">
-        <v>716</v>
+      <c r="H2" s="179" t="s">
+        <v>743</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>717</v>
+        <v>744</v>
       </c>
       <c r="J2" s="132" t="s">
-        <v>718</v>
+        <v>745</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>719</v>
+        <v>746</v>
       </c>
       <c r="L2" s="113" t="s">
-        <v>720</v>
+        <v>747</v>
       </c>
       <c r="M2" s="132" t="s">
-        <v>721</v>
+        <v>748</v>
       </c>
       <c r="N2" s="132" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>723</v>
+        <v>750</v>
       </c>
     </row>
     <row r="3" ht="114">
-      <c r="A3" s="179" t="str">
+      <c r="A3" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P3&lt;10,"0",""),P3)</f>
         <v>q01</v>
       </c>
@@ -7222,34 +7625,36 @@
         <v>qbank01</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>725</v>
+        <v>752</v>
       </c>
       <c r="E3" s="79" t="s">
-        <v>726</v>
+        <v>753</v>
       </c>
       <c r="F3" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="180"/>
+      <c r="G3" s="181" t="s">
+        <v>754</v>
+      </c>
       <c r="H3" s="181" t="s">
-        <v>727</v>
+        <v>755</v>
       </c>
       <c r="I3" s="79"/>
       <c r="J3" s="181" t="s">
-        <v>728</v>
+        <v>756</v>
       </c>
       <c r="K3" s="182"/>
       <c r="L3" s="79">
         <v>1</v>
       </c>
       <c r="M3" s="181" t="s">
-        <v>729</v>
+        <v>757</v>
       </c>
       <c r="N3" s="181" t="s">
-        <v>730</v>
+        <v>758</v>
       </c>
       <c r="O3" s="79"/>
       <c r="P3" s="183">
@@ -7257,7 +7662,7 @@
       </c>
     </row>
     <row r="4" ht="199.5">
-      <c r="A4" s="179" t="str">
+      <c r="A4" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P4&lt;10,"0",""),P4)</f>
         <v>q02</v>
       </c>
@@ -7266,34 +7671,36 @@
         <v>qbank01</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D4" s="79" t="s">
-        <v>731</v>
+        <v>759</v>
       </c>
       <c r="E4" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="180"/>
+      <c r="G4" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H4" s="181" t="s">
-        <v>733</v>
+        <v>762</v>
       </c>
       <c r="I4" s="79"/>
       <c r="J4" s="181" t="s">
-        <v>734</v>
+        <v>763</v>
       </c>
       <c r="K4" s="79"/>
       <c r="L4" s="79">
         <v>4</v>
       </c>
       <c r="M4" s="181" t="s">
-        <v>735</v>
+        <v>764</v>
       </c>
       <c r="N4" s="181" t="s">
-        <v>736</v>
+        <v>765</v>
       </c>
       <c r="O4" s="79"/>
       <c r="P4" s="183">
@@ -7302,7 +7709,7 @@
       </c>
     </row>
     <row r="5" ht="114">
-      <c r="A5" s="179" t="str">
+      <c r="A5" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P5&lt;10,"0",""),P5)</f>
         <v>q03</v>
       </c>
@@ -7311,34 +7718,36 @@
         <v>qbank01</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>725</v>
+        <v>752</v>
       </c>
       <c r="E5" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F5" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="180"/>
+      <c r="G5" s="181" t="s">
+        <v>766</v>
+      </c>
       <c r="H5" s="181" t="s">
-        <v>737</v>
+        <v>767</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="181" t="s">
-        <v>738</v>
+        <v>768</v>
       </c>
       <c r="K5" s="79"/>
       <c r="L5" s="79">
         <v>3</v>
       </c>
       <c r="M5" s="181" t="s">
-        <v>739</v>
+        <v>769</v>
       </c>
       <c r="N5" s="181" t="s">
-        <v>730</v>
+        <v>758</v>
       </c>
       <c r="O5" s="79"/>
       <c r="P5" s="183">
@@ -7347,7 +7756,7 @@
       </c>
     </row>
     <row r="6" ht="156.75">
-      <c r="A6" s="179" t="str">
+      <c r="A6" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P6&lt;10,"0",""),P6)</f>
         <v>q04</v>
       </c>
@@ -7356,34 +7765,36 @@
         <v>qbank01</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>731</v>
+        <v>759</v>
       </c>
       <c r="E6" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F6" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="180"/>
+      <c r="G6" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H6" s="181" t="s">
-        <v>740</v>
+        <v>770</v>
       </c>
       <c r="I6" s="79"/>
       <c r="J6" s="181" t="s">
-        <v>741</v>
+        <v>771</v>
       </c>
       <c r="K6" s="79"/>
       <c r="L6" s="79">
         <v>2</v>
       </c>
       <c r="M6" s="181" t="s">
-        <v>742</v>
+        <v>772</v>
       </c>
       <c r="N6" s="181" t="s">
-        <v>743</v>
+        <v>773</v>
       </c>
       <c r="O6" s="79"/>
       <c r="P6" s="183">
@@ -7392,7 +7803,7 @@
       </c>
     </row>
     <row r="7" ht="71.25">
-      <c r="A7" s="179" t="str">
+      <c r="A7" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P7&lt;10,"0",""),P7)</f>
         <v>q05</v>
       </c>
@@ -7401,34 +7812,36 @@
         <v>qbank01</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D7" s="79" t="s">
-        <v>725</v>
+        <v>752</v>
       </c>
       <c r="E7" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F7" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="180"/>
+      <c r="G7" s="181" t="s">
+        <v>774</v>
+      </c>
       <c r="H7" s="181" t="s">
-        <v>744</v>
+        <v>775</v>
       </c>
       <c r="I7" s="79"/>
       <c r="J7" s="181" t="s">
-        <v>745</v>
+        <v>776</v>
       </c>
       <c r="K7" s="79"/>
       <c r="L7" s="79">
         <v>1</v>
       </c>
       <c r="M7" s="181" t="s">
-        <v>746</v>
+        <v>777</v>
       </c>
       <c r="N7" s="181" t="s">
-        <v>747</v>
+        <v>778</v>
       </c>
       <c r="O7" s="79"/>
       <c r="P7" s="183">
@@ -7437,7 +7850,7 @@
       </c>
     </row>
     <row r="8" ht="242.25">
-      <c r="A8" s="179" t="str">
+      <c r="A8" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P8&lt;10,"0",""),P8)</f>
         <v>q06</v>
       </c>
@@ -7446,34 +7859,36 @@
         <v>qbank01</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>731</v>
+        <v>759</v>
       </c>
       <c r="E8" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F8" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="180"/>
+      <c r="G8" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H8" s="181" t="s">
-        <v>748</v>
+        <v>779</v>
       </c>
       <c r="I8" s="182"/>
       <c r="J8" s="181" t="s">
-        <v>749</v>
+        <v>780</v>
       </c>
       <c r="K8" s="79"/>
       <c r="L8" s="79">
         <v>2</v>
       </c>
       <c r="M8" s="181" t="s">
-        <v>750</v>
+        <v>781</v>
       </c>
       <c r="N8" s="181" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="O8" s="184"/>
       <c r="P8" s="183">
@@ -7482,7 +7897,7 @@
       </c>
     </row>
     <row r="9" ht="242.25">
-      <c r="A9" s="179" t="str">
+      <c r="A9" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P9&lt;10,"0",""),P9)</f>
         <v>q07</v>
       </c>
@@ -7491,34 +7906,36 @@
         <v>qbank01</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>731</v>
+        <v>759</v>
       </c>
       <c r="E9" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F9" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="180"/>
+      <c r="G9" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H9" s="181" t="s">
-        <v>752</v>
+        <v>783</v>
       </c>
       <c r="I9" s="182"/>
       <c r="J9" s="181" t="s">
-        <v>753</v>
+        <v>784</v>
       </c>
       <c r="K9" s="79"/>
       <c r="L9" s="79">
         <v>3</v>
       </c>
       <c r="M9" s="181" t="s">
-        <v>754</v>
+        <v>785</v>
       </c>
       <c r="N9" s="181" t="s">
-        <v>755</v>
+        <v>786</v>
       </c>
       <c r="O9" s="79"/>
       <c r="P9" s="183">
@@ -7527,7 +7944,7 @@
       </c>
     </row>
     <row r="10" ht="356.25">
-      <c r="A10" s="179" t="str">
+      <c r="A10" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P10&lt;10,"0",""),P10)</f>
         <v>q08</v>
       </c>
@@ -7536,31 +7953,33 @@
         <v>qbank01</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>725</v>
+        <v>752</v>
       </c>
       <c r="E10" s="79" t="s">
-        <v>726</v>
+        <v>753</v>
       </c>
       <c r="F10" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="180"/>
+      <c r="G10" s="181" t="s">
+        <v>766</v>
+      </c>
       <c r="H10" s="181" t="s">
-        <v>756</v>
+        <v>787</v>
       </c>
       <c r="I10" s="79"/>
       <c r="J10" s="79"/>
       <c r="K10" s="81" t="s">
-        <v>757</v>
+        <v>788</v>
       </c>
       <c r="L10" s="79">
         <v>2</v>
       </c>
       <c r="M10" s="181" t="s">
-        <v>758</v>
+        <v>789</v>
       </c>
       <c r="N10" s="181"/>
       <c r="O10" s="79"/>
@@ -7570,7 +7989,7 @@
       </c>
     </row>
     <row r="11" ht="185.25">
-      <c r="A11" s="179" t="str">
+      <c r="A11" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P11&lt;10,"0",""),P11)</f>
         <v>q09</v>
       </c>
@@ -7579,36 +7998,38 @@
         <v>qbank01</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D11" s="79" t="s">
-        <v>725</v>
+        <v>752</v>
       </c>
       <c r="E11" s="79" t="s">
-        <v>726</v>
+        <v>753</v>
       </c>
       <c r="F11" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="180"/>
+      <c r="G11" s="181" t="s">
+        <v>766</v>
+      </c>
       <c r="H11" s="181" t="s">
-        <v>759</v>
+        <v>790</v>
       </c>
       <c r="I11" s="81" t="s">
         <v>312</v>
       </c>
       <c r="J11" s="181" t="s">
-        <v>760</v>
+        <v>791</v>
       </c>
       <c r="K11" s="79"/>
       <c r="L11" s="79">
         <v>1</v>
       </c>
       <c r="M11" s="181" t="s">
-        <v>761</v>
+        <v>792</v>
       </c>
       <c r="N11" s="181" t="s">
-        <v>762</v>
+        <v>793</v>
       </c>
       <c r="O11" s="79"/>
       <c r="P11" s="183">
@@ -7617,7 +8038,7 @@
       </c>
     </row>
     <row r="12" ht="185.25">
-      <c r="A12" s="179" t="str">
+      <c r="A12" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P12&lt;10,"0",""),P12)</f>
         <v>q10</v>
       </c>
@@ -7626,34 +8047,36 @@
         <v>qbank01</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D12" s="79" t="s">
-        <v>731</v>
+        <v>759</v>
       </c>
       <c r="E12" s="79" t="s">
-        <v>763</v>
+        <v>794</v>
       </c>
       <c r="F12" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G12" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G12" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H12" s="181" t="s">
-        <v>765</v>
+        <v>796</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="101" t="s">
-        <v>766</v>
+        <v>797</v>
       </c>
       <c r="K12" s="79"/>
       <c r="L12" s="79">
         <v>4</v>
       </c>
       <c r="M12" s="181" t="s">
-        <v>767</v>
+        <v>798</v>
       </c>
       <c r="N12" s="181" t="s">
-        <v>768</v>
+        <v>799</v>
       </c>
       <c r="O12" s="79"/>
       <c r="P12" s="183">
@@ -7662,7 +8085,7 @@
       </c>
     </row>
     <row r="13" ht="185.25">
-      <c r="A13" s="179" t="str">
+      <c r="A13" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P13&lt;10,"0",""),P13)</f>
         <v>q11</v>
       </c>
@@ -7671,34 +8094,36 @@
         <v>qbank01</v>
       </c>
       <c r="C13" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D13" s="79" t="s">
-        <v>731</v>
+        <v>759</v>
       </c>
       <c r="E13" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F13" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G13" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G13" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H13" s="181" t="s">
-        <v>769</v>
+        <v>800</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="181" t="s">
-        <v>770</v>
+        <v>801</v>
       </c>
       <c r="K13" s="79"/>
       <c r="L13" s="79">
         <v>3</v>
       </c>
       <c r="M13" s="181" t="s">
-        <v>771</v>
+        <v>802</v>
       </c>
       <c r="N13" s="181" t="s">
-        <v>772</v>
+        <v>803</v>
       </c>
       <c r="O13" s="79"/>
       <c r="P13" s="183">
@@ -7707,7 +8132,7 @@
       </c>
     </row>
     <row r="14" ht="185.25">
-      <c r="A14" s="179" t="str">
+      <c r="A14" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P14&lt;10,"0",""),P14)</f>
         <v>q12</v>
       </c>
@@ -7716,31 +8141,33 @@
         <v>qbank01</v>
       </c>
       <c r="C14" s="79" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D14" s="79" t="s">
-        <v>731</v>
+        <v>759</v>
       </c>
       <c r="E14" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F14" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G14" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G14" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H14" s="181" t="s">
-        <v>773</v>
+        <v>804</v>
       </c>
       <c r="I14" s="79"/>
       <c r="J14" s="181" t="s">
-        <v>774</v>
+        <v>805</v>
       </c>
       <c r="K14" s="79"/>
       <c r="L14" s="79">
         <v>1</v>
       </c>
       <c r="M14" s="181" t="s">
-        <v>775</v>
+        <v>806</v>
       </c>
       <c r="N14" s="181"/>
       <c r="O14" s="79"/>
@@ -7750,7 +8177,7 @@
       </c>
     </row>
     <row r="15" ht="114">
-      <c r="A15" s="179" t="str">
+      <c r="A15" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P15&lt;10,"0",""),P15)</f>
         <v>q13</v>
       </c>
@@ -7759,33 +8186,35 @@
         <v>qbank01</v>
       </c>
       <c r="C15" s="79" t="s">
-        <v>724</v>
-      </c>
-      <c r="D15" s="185" t="s">
-        <v>725</v>
+        <v>751</v>
+      </c>
+      <c r="D15" s="79" t="s">
+        <v>752</v>
       </c>
       <c r="E15" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F15" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G15" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G15" s="181" t="s">
+        <v>807</v>
+      </c>
       <c r="H15" s="181" t="s">
-        <v>776</v>
+        <v>808</v>
       </c>
       <c r="I15" s="79" t="s">
         <v>338</v>
       </c>
       <c r="J15" s="181" t="s">
-        <v>777</v>
+        <v>809</v>
       </c>
       <c r="K15" s="182"/>
       <c r="L15" s="79">
         <v>2</v>
       </c>
       <c r="M15" s="181" t="s">
-        <v>778</v>
+        <v>810</v>
       </c>
       <c r="N15" s="181"/>
       <c r="O15" s="79"/>
@@ -7795,7 +8224,7 @@
       </c>
     </row>
     <row r="16" ht="114">
-      <c r="A16" s="179" t="str">
+      <c r="A16" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P16&lt;10,"0",""),P16)</f>
         <v>q14</v>
       </c>
@@ -7804,33 +8233,35 @@
         <v>qbank01</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>724</v>
-      </c>
-      <c r="D16" s="185" t="s">
-        <v>725</v>
+        <v>751</v>
+      </c>
+      <c r="D16" s="79" t="s">
+        <v>752</v>
       </c>
       <c r="E16" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F16" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G16" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G16" s="181" t="s">
+        <v>807</v>
+      </c>
       <c r="H16" s="181" t="s">
-        <v>779</v>
+        <v>811</v>
       </c>
       <c r="I16" s="79" t="s">
         <v>338</v>
       </c>
       <c r="J16" s="181" t="s">
-        <v>780</v>
+        <v>812</v>
       </c>
       <c r="K16" s="182"/>
       <c r="L16" s="79">
         <v>1</v>
       </c>
       <c r="M16" s="181" t="s">
-        <v>781</v>
+        <v>813</v>
       </c>
       <c r="N16" s="181"/>
       <c r="O16" s="184"/>
@@ -7840,7 +8271,7 @@
       </c>
     </row>
     <row r="17" ht="142.5">
-      <c r="A17" s="179" t="str">
+      <c r="A17" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P17&lt;10,"0",""),P17)</f>
         <v>q15</v>
       </c>
@@ -7849,31 +8280,33 @@
         <v>qbank01</v>
       </c>
       <c r="C17" s="79" t="s">
-        <v>724</v>
-      </c>
-      <c r="D17" s="185" t="s">
-        <v>725</v>
+        <v>751</v>
+      </c>
+      <c r="D17" s="79" t="s">
+        <v>752</v>
       </c>
       <c r="E17" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F17" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G17" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G17" s="181" t="s">
+        <v>814</v>
+      </c>
       <c r="H17" s="181" t="s">
-        <v>782</v>
+        <v>815</v>
       </c>
       <c r="I17" s="182"/>
       <c r="J17" s="181" t="s">
-        <v>783</v>
+        <v>816</v>
       </c>
       <c r="K17" s="182"/>
       <c r="L17" s="79">
         <v>2</v>
       </c>
       <c r="M17" s="181" t="s">
-        <v>784</v>
+        <v>817</v>
       </c>
       <c r="N17" s="181"/>
       <c r="O17" s="184"/>
@@ -7883,7 +8316,7 @@
       </c>
     </row>
     <row r="18" ht="242.25">
-      <c r="A18" s="179" t="str">
+      <c r="A18" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P18&lt;10,"0",""),P18)</f>
         <v>q16</v>
       </c>
@@ -7892,31 +8325,33 @@
         <v>qbank01</v>
       </c>
       <c r="C18" s="79" t="s">
-        <v>724</v>
-      </c>
-      <c r="D18" s="185" t="s">
-        <v>725</v>
+        <v>751</v>
+      </c>
+      <c r="D18" s="79" t="s">
+        <v>752</v>
       </c>
       <c r="E18" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F18" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G18" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G18" s="181" t="s">
+        <v>807</v>
+      </c>
       <c r="H18" s="181" t="s">
-        <v>785</v>
+        <v>818</v>
       </c>
       <c r="I18" s="182"/>
       <c r="J18" s="181" t="s">
-        <v>786</v>
+        <v>819</v>
       </c>
       <c r="K18" s="182"/>
       <c r="L18" s="79">
         <v>1</v>
       </c>
       <c r="M18" s="181" t="s">
-        <v>787</v>
+        <v>820</v>
       </c>
       <c r="N18" s="181"/>
       <c r="O18" s="184"/>
@@ -7926,7 +8361,7 @@
       </c>
     </row>
     <row r="19" ht="213.75">
-      <c r="A19" s="179" t="str">
+      <c r="A19" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P19&lt;10,"0",""),P19)</f>
         <v>q17</v>
       </c>
@@ -7935,34 +8370,36 @@
         <v>qbank01</v>
       </c>
       <c r="C19" s="79" t="s">
-        <v>724</v>
-      </c>
-      <c r="D19" s="185" t="s">
-        <v>731</v>
+        <v>751</v>
+      </c>
+      <c r="D19" s="79" t="s">
+        <v>759</v>
       </c>
       <c r="E19" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F19" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G19" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G19" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H19" s="181" t="s">
-        <v>788</v>
+        <v>821</v>
       </c>
       <c r="I19" s="182"/>
       <c r="J19" s="181" t="s">
-        <v>789</v>
+        <v>822</v>
       </c>
       <c r="K19" s="182"/>
       <c r="L19" s="79">
         <v>3</v>
       </c>
       <c r="M19" s="181" t="s">
-        <v>790</v>
+        <v>823</v>
       </c>
       <c r="N19" s="181" t="s">
-        <v>791</v>
+        <v>824</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="183">
@@ -7971,7 +8408,7 @@
       </c>
     </row>
     <row r="20" ht="242.25">
-      <c r="A20" s="179" t="str">
+      <c r="A20" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P20&lt;10,"0",""),P20)</f>
         <v>q18</v>
       </c>
@@ -7980,34 +8417,36 @@
         <v>qbank01</v>
       </c>
       <c r="C20" s="79" t="s">
-        <v>724</v>
-      </c>
-      <c r="D20" s="185" t="s">
-        <v>731</v>
+        <v>751</v>
+      </c>
+      <c r="D20" s="79" t="s">
+        <v>759</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="F20" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G20" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G20" s="181" t="s">
+        <v>761</v>
+      </c>
       <c r="H20" s="181" t="s">
-        <v>792</v>
+        <v>825</v>
       </c>
       <c r="I20" s="182"/>
       <c r="J20" s="181" t="s">
-        <v>793</v>
+        <v>826</v>
       </c>
       <c r="K20" s="182"/>
       <c r="L20" s="79">
         <v>4</v>
       </c>
       <c r="M20" s="181" t="s">
-        <v>794</v>
+        <v>827</v>
       </c>
       <c r="N20" s="181" t="s">
-        <v>795</v>
+        <v>828</v>
       </c>
       <c r="O20" s="184"/>
       <c r="P20" s="183">
@@ -8016,7 +8455,7 @@
       </c>
     </row>
     <row r="21" ht="409.5">
-      <c r="A21" s="179" t="str">
+      <c r="A21" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P21&lt;10,"0",""),P21)</f>
         <v>q19</v>
       </c>
@@ -8025,34 +8464,36 @@
         <v>qbank01</v>
       </c>
       <c r="C21" s="79" t="s">
-        <v>724</v>
-      </c>
-      <c r="D21" s="185" t="s">
-        <v>796</v>
+        <v>751</v>
+      </c>
+      <c r="D21" s="79" t="s">
+        <v>829</v>
       </c>
       <c r="E21" s="79" t="s">
-        <v>763</v>
+        <v>794</v>
       </c>
       <c r="F21" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="G21" s="180"/>
+        <v>795</v>
+      </c>
+      <c r="G21" s="181" t="s">
+        <v>814</v>
+      </c>
       <c r="H21" s="181" t="s">
-        <v>797</v>
+        <v>830</v>
       </c>
       <c r="I21" s="79"/>
       <c r="J21" s="181" t="s">
-        <v>798</v>
+        <v>831</v>
       </c>
       <c r="K21" s="79"/>
       <c r="L21" s="79">
         <v>4</v>
       </c>
       <c r="M21" s="181" t="s">
-        <v>799</v>
+        <v>832</v>
       </c>
       <c r="N21" s="181" t="s">
-        <v>800</v>
+        <v>833</v>
       </c>
       <c r="O21" s="79"/>
       <c r="P21" s="183">
@@ -8061,7 +8502,7 @@
       </c>
     </row>
     <row r="22" ht="114">
-      <c r="A22" s="179" t="str">
+      <c r="A22" s="180" t="str">
         <f>_xlfn.CONCAT("q",IF(P22&lt;10,"0",""),P22)</f>
         <v>q20</v>
       </c>
@@ -8070,33 +8511,35 @@
         <v>qbank01</v>
       </c>
       <c r="C22" s="79" t="s">
-        <v>801</v>
-      </c>
-      <c r="D22" s="185" t="s">
-        <v>796</v>
+        <v>834</v>
+      </c>
+      <c r="D22" s="79" t="s">
+        <v>829</v>
       </c>
       <c r="E22" s="79" t="s">
-        <v>726</v>
+        <v>753</v>
       </c>
       <c r="F22" s="76"/>
-      <c r="G22" s="101"/>
+      <c r="G22" s="181" t="s">
+        <v>774</v>
+      </c>
       <c r="H22" s="181" t="s">
-        <v>802</v>
+        <v>835</v>
       </c>
       <c r="I22" s="81" t="s">
         <v>315</v>
       </c>
       <c r="J22" s="181" t="s">
-        <v>803</v>
+        <v>836</v>
       </c>
       <c r="K22" s="182"/>
-      <c r="L22" s="186"/>
+      <c r="L22" s="185"/>
       <c r="M22" s="146"/>
       <c r="N22" s="146"/>
       <c r="O22" s="76" t="s">
         <v>392</v>
       </c>
-      <c r="P22" s="187">
+      <c r="P22" s="186">
         <f>P21+1</f>
         <v>20</v>
       </c>
@@ -8116,55 +8559,55 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00660009-00C9-4C7F-A133-000D002A0012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00400012-000B-4512-BA72-00C0003B003B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000B0052-0029-4AD1-ACF5-00BA00130017}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007A00AB-0046-46D7-86E6-0029001F0040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B50090-00A2-4FDE-9033-004C00440082}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001800ED-006B-450E-B54C-00DE0005007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003800F9-0044-4008-A070-0016000900E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003D0008-0008-4C7E-BE42-00BB006D0055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006A0002-0024-4732-B4F4-00450032002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002D007A-0018-4996-94AE-002300C800D4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00510047-0023-4790-9EB8-00AC008C007D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007A0052-00D7-4696-8A08-00E30054006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006D0088-00B3-4300-885F-006A005E0096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0043003C-004A-4BA0-8076-008C0059002F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008E0088-0038-4924-B341-009100140039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F8002F-00A7-4CBB-ABFF-006E00BB0073}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009900B0-00C8-4BB3-AD8C-002400940065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A000E7-009B-435B-ACCD-001300050037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -8193,9 +8636,9 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="14.57421875"/>
     <col customWidth="1" min="3" max="3" width="24.8515625"/>
-    <col customWidth="1" min="4" max="4" width="32.8515625"/>
-    <col customWidth="1" min="5" max="5" width="41.7109375"/>
-    <col customWidth="1" min="6" max="6" width="11.28125"/>
+    <col customWidth="1" min="4" max="4" width="41.421875"/>
+    <col customWidth="1" min="5" max="5" width="25.00390625"/>
+    <col customWidth="1" min="6" max="6" style="153" width="18.8515625"/>
     <col customWidth="1" min="8" max="8" width="14.7109375"/>
     <col customWidth="1" min="9" max="9" width="11.28125"/>
     <col customWidth="1" min="10" max="10" width="13.8515625"/>
@@ -8210,7 +8653,7 @@
         <v>35</v>
       </c>
       <c r="B1" s="91" t="s">
-        <v>701</v>
+        <v>837</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>36</v>
@@ -8221,7 +8664,7 @@
       <c r="E1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="135" t="s">
         <v>148</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -8243,16 +8686,19 @@
         <v>580</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>804</v>
+        <v>838</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>805</v>
+        <v>839</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>578</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>440</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="2" s="153" customFormat="1" ht="28.5">
@@ -8260,7 +8706,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="136" t="s">
-        <v>713</v>
+        <v>740</v>
       </c>
       <c r="C2" s="113" t="s">
         <v>40</v>
@@ -8279,13 +8725,13 @@
         <v>260</v>
       </c>
       <c r="H2" s="113" t="s">
-        <v>806</v>
-      </c>
-      <c r="I2" s="188" t="str">
+        <v>840</v>
+      </c>
+      <c r="I2" s="187" t="str">
         <f>PROPER(I1)</f>
         <v>Program</v>
       </c>
-      <c r="J2" s="189" t="str">
+      <c r="J2" s="188" t="str">
         <f>PROPER(J1)</f>
         <v>Subjects</v>
       </c>
@@ -8296,44 +8742,45 @@
         <v>599</v>
       </c>
       <c r="M2" s="132" t="s">
-        <v>807</v>
-      </c>
-      <c r="N2" s="189" t="s">
-        <v>808</v>
-      </c>
-      <c r="O2" s="189" t="str">
+        <v>841</v>
+      </c>
+      <c r="N2" s="188" t="s">
+        <v>842</v>
+      </c>
+      <c r="O2" s="188" t="str">
         <f>PROPER(O1)</f>
         <v>Statement</v>
       </c>
-      <c r="P2" s="188" t="str">
+      <c r="P2" s="187" t="str">
         <f>PROPER(P1)</f>
         <v>Creator</v>
       </c>
-      <c r="Q2" s="153"/>
+      <c r="Q2" s="115" t="str">
+        <f>PROPER(Q1)</f>
+        <v>Published</v>
+      </c>
       <c r="R2" s="153"/>
     </row>
     <row r="3" s="74" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="179" t="s">
-        <v>809</v>
+      <c r="A3" s="180" t="s">
+        <v>843</v>
       </c>
       <c r="B3" s="165" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>810</v>
-      </c>
-      <c r="D3" s="74" t="s">
-        <v>811</v>
-      </c>
-      <c r="E3" s="162" t="s">
-        <v>812</v>
-      </c>
-      <c r="F3" s="74" t="s">
-        <v>813</v>
+        <v>844</v>
+      </c>
+      <c r="D3" s="162" t="s">
+        <v>845</v>
+      </c>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162" t="s">
+        <v>326</v>
       </c>
       <c r="G3" s="74" t="s">
-        <v>814</v>
+        <v>846</v>
       </c>
       <c r="H3" s="74" t="s">
         <v>272</v>
@@ -8342,52 +8789,52 @@
         <f>ap_programs!A5</f>
         <v>programB</v>
       </c>
-      <c r="J3" s="173" t="s">
-        <v>700</v>
+      <c r="J3" s="189" t="s">
+        <v>702</v>
       </c>
       <c r="K3" s="190" t="s">
-        <v>815</v>
-      </c>
-      <c r="L3" s="67" t="s">
+        <v>847</v>
+      </c>
+      <c r="L3" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="67" t="s">
+      <c r="M3" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="173" t="s">
-        <v>816</v>
+      <c r="N3" s="189" t="s">
+        <v>848</v>
       </c>
       <c r="O3" s="74" t="s">
-        <v>817</v>
-      </c>
-      <c r="P3" s="171" t="s">
+        <v>849</v>
+      </c>
+      <c r="P3" s="191" t="s">
         <v>163</v>
       </c>
-      <c r="Q3" s="74"/>
+      <c r="Q3" s="79" t="s">
+        <v>9</v>
+      </c>
       <c r="R3" s="74"/>
     </row>
-    <row r="4" s="74" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A4" s="179" t="s">
-        <v>818</v>
+    <row r="4" s="74" customFormat="1" ht="27">
+      <c r="A4" s="180" t="s">
+        <v>850</v>
       </c>
       <c r="B4" s="165" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>819</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>820</v>
-      </c>
-      <c r="E4" s="162" t="s">
-        <v>821</v>
-      </c>
-      <c r="F4" s="74" t="s">
-        <v>822</v>
+        <v>851</v>
+      </c>
+      <c r="D4" s="162" t="s">
+        <v>852</v>
+      </c>
+      <c r="E4" s="162"/>
+      <c r="F4" s="162" t="s">
+        <v>853</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>823</v>
+        <v>854</v>
       </c>
       <c r="H4" s="74" t="s">
         <v>412</v>
@@ -8396,29 +8843,212 @@
         <f>I3</f>
         <v>programB</v>
       </c>
-      <c r="J4" s="173" t="s">
-        <v>700</v>
+      <c r="J4" s="189" t="s">
+        <v>702</v>
       </c>
       <c r="K4" s="190" t="s">
-        <v>815</v>
-      </c>
-      <c r="L4" s="67" t="s">
+        <v>847</v>
+      </c>
+      <c r="L4" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="173" t="s">
-        <v>824</v>
+      <c r="N4" s="189" t="s">
+        <v>855</v>
       </c>
       <c r="O4" s="74" t="s">
-        <v>817</v>
-      </c>
-      <c r="P4" s="171" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q4" s="74"/>
+        <v>849</v>
+      </c>
+      <c r="P4" s="191" t="str">
+        <f>P3</f>
+        <v>teacher01</v>
+      </c>
+      <c r="Q4" s="79" t="s">
+        <v>9</v>
+      </c>
       <c r="R4" s="74"/>
+    </row>
+    <row r="5" ht="27">
+      <c r="A5" s="180" t="s">
+        <v>856</v>
+      </c>
+      <c r="B5" s="165"/>
+      <c r="C5" s="74" t="s">
+        <v>857</v>
+      </c>
+      <c r="D5" s="162" t="s">
+        <v>699</v>
+      </c>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162" t="s">
+        <v>858</v>
+      </c>
+      <c r="G5" s="74" t="s">
+        <v>859</v>
+      </c>
+      <c r="H5" s="74" t="s">
+        <v>860</v>
+      </c>
+      <c r="I5" s="172"/>
+      <c r="J5" s="189"/>
+      <c r="K5" s="190"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="189"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="191" t="str">
+        <f>P4</f>
+        <v>teacher01</v>
+      </c>
+      <c r="Q5" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="27">
+      <c r="A6" s="180" t="s">
+        <v>861</v>
+      </c>
+      <c r="B6" s="165"/>
+      <c r="C6" s="74" t="s">
+        <v>862</v>
+      </c>
+      <c r="D6" s="162" t="s">
+        <v>699</v>
+      </c>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162" t="s">
+        <v>863</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>864</v>
+      </c>
+      <c r="H6" s="74" t="s">
+        <v>865</v>
+      </c>
+      <c r="I6" s="172"/>
+      <c r="J6" s="189"/>
+      <c r="K6" s="190"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="189"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="191" t="str">
+        <f>P5</f>
+        <v>teacher01</v>
+      </c>
+      <c r="Q6" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="40.5">
+      <c r="A7" s="180" t="s">
+        <v>866</v>
+      </c>
+      <c r="B7" s="165"/>
+      <c r="C7" s="74" t="s">
+        <v>867</v>
+      </c>
+      <c r="D7" s="162" t="s">
+        <v>699</v>
+      </c>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162" t="s">
+        <v>868</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>869</v>
+      </c>
+      <c r="H7" s="74" t="s">
+        <v>870</v>
+      </c>
+      <c r="I7" s="172"/>
+      <c r="J7" s="189"/>
+      <c r="K7" s="190"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="189"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="191" t="str">
+        <f>P6</f>
+        <v>teacher01</v>
+      </c>
+      <c r="Q7" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="27">
+      <c r="A8" s="180" t="s">
+        <v>871</v>
+      </c>
+      <c r="B8" s="165"/>
+      <c r="C8" s="74" t="s">
+        <v>872</v>
+      </c>
+      <c r="D8" s="162" t="s">
+        <v>873</v>
+      </c>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162" t="s">
+        <v>874</v>
+      </c>
+      <c r="G8" s="74" t="s">
+        <v>875</v>
+      </c>
+      <c r="H8" s="74" t="s">
+        <v>876</v>
+      </c>
+      <c r="I8" s="172"/>
+      <c r="J8" s="189"/>
+      <c r="K8" s="190"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="189"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="191" t="str">
+        <f>P7</f>
+        <v>teacher01</v>
+      </c>
+      <c r="Q8" s="79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="180" t="s">
+        <v>877</v>
+      </c>
+      <c r="B9" s="165"/>
+      <c r="C9" s="74" t="s">
+        <v>878</v>
+      </c>
+      <c r="D9" s="162" t="s">
+        <v>879</v>
+      </c>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162" t="s">
+        <v>880</v>
+      </c>
+      <c r="G9" s="74" t="s">
+        <v>881</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>882</v>
+      </c>
+      <c r="I9" s="172"/>
+      <c r="J9" s="189"/>
+      <c r="K9" s="190"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="189"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="191" t="str">
+        <f>P8</f>
+        <v>teacher01</v>
+      </c>
+      <c r="Q9" s="79" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -8427,30 +9057,72 @@
   <headerFooter/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00C8008B-00E4-4C2E-AD55-00D200490074}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11" disablePrompts="0">
+        <x14:dataValidation xr:uid="{001C0036-00FF-4423-A8AB-0039001C00B7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001A0025-005E-4EA9-B683-007A008D004A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004B007D-0047-4788-8759-00D8005600DA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008D001C-0093-4D36-A344-00F200370079}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006900CB-0001-4927-85D7-000E00EB002D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>M3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00580070-00DC-4FE6-88DE-0099006000A6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008D0011-0028-4848-A559-00A700000072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>M4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{004B0026-003F-4CB2-B17D-005900DD00C4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00A900A1-0093-4302-A00D-00A7004000D7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00AA009F-0010-4D88-A20C-0005008B0076}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003000D8-005E-4EF7-A637-0070005C0009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0090001D-008A-4849-92E1-0033009A0028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00FF00EE-0031-4840-839D-009600350051}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00B10015-0038-4808-B57F-0096002A00B5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10293,37 +10965,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00AD0073-0039-46E6-AFD4-005700F90010}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008000C6-0006-45EB-9BE1-00DE00020021}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C9001D-0055-4388-A9F4-002B006E001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E600F0-0086-4666-B54B-006C003C00E2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009100B6-000C-4275-BF33-00A2001800D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00580032-003D-4DB8-97C7-001A00A000A4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00530072-0054-498B-830F-00D5007C00EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003300A6-004E-4BA1-A93D-0023005C00F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005800CD-00C9-47AA-9C72-001A002C0012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009600F0-0027-4E0C-8A5C-00B100600072}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001C00F0-003E-4C0A-B154-0066002C0071}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EF0058-0077-4682-B499-0043005100F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -11531,31 +12203,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5" disablePrompts="0">
-        <x14:dataValidation xr:uid="{008A00CC-005A-4752-8B01-0068003B0091}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001400B9-0055-4B23-B0CD-0030006A0043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00480088-0037-4575-AD10-002D00190059}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002E00E5-00C4-40BA-ACE2-009A00B1002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D500BC-00D0-4047-89A0-008C004E0067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00680015-00E6-4541-A5DB-00B40060004D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000E0099-0007-460D-BBD9-00B200C40039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002400D6-0063-4977-B272-00210023008A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00810037-006A-42B9-8F8A-008A008D0070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009500CE-00AC-4BE1-998F-00B200D000EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -11706,7 +12378,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{005600D4-0047-4CF8-A003-00EB00B500AF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005E00ED-0028-4228-B602-008F00DC00DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -11840,13 +12512,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00EE0047-0029-4909-AD29-00EB0038002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EF0022-006E-4C1E-BB93-00D5004A00EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002B00DA-0057-4F5D-829B-005900290071}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008C008B-00B3-436A-B6AC-00D900DC0080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
FIXED: duplicated categories in Qbank bulk loading
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="16"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -2221,7 +2221,7 @@
     <t>qbank03</t>
   </si>
   <si>
-    <t xml:space="preserve">Vocabulaire français 2ESO</t>
+    <t xml:space="preserve">Vocabulaire français</t>
   </si>
   <si>
     <t>#669ecc</t>
@@ -2248,7 +2248,10 @@
     <t>qbank05</t>
   </si>
   <si>
-    <t xml:space="preserve">grammaire 1ESO</t>
+    <t>Grammaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1º ESO</t>
   </si>
   <si>
     <t>#4091bf</t>
@@ -2799,9 +2802,6 @@
   </si>
   <si>
     <t xml:space="preserve">Grammaire: Le présent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1º ESO</t>
   </si>
   <si>
     <t xml:space="preserve">grammaire, verbes, présent</t>
@@ -5166,13 +5166,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007B0044-0080-41E4-AF1A-002B000000F9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B70096-000B-479F-B4C9-00CA00840003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007A00DD-00EE-4F74-A5B6-00CC009800F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00490028-0023-4587-9B54-00FB002C0007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5317,7 +5317,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{003D00E1-00CE-49B1-91D3-002F002000B0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00280012-0072-42EF-9091-006600610089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7194,7 +7194,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -7362,7 +7362,9 @@
       <c r="B5" s="168" t="s">
         <v>716</v>
       </c>
-      <c r="C5" s="168"/>
+      <c r="C5" s="168" t="s">
+        <v>706</v>
+      </c>
       <c r="D5" s="169"/>
       <c r="E5" s="168" t="s">
         <v>717</v>
@@ -7426,16 +7428,18 @@
       <c r="B7" s="168" t="s">
         <v>725</v>
       </c>
-      <c r="C7" s="168"/>
+      <c r="C7" s="168" t="s">
+        <v>726</v>
+      </c>
       <c r="D7" s="169"/>
       <c r="E7" s="168" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F7" s="170" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G7" s="169" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="H7" s="171" t="s">
         <v>170</v>
@@ -7452,23 +7456,23 @@
     </row>
     <row r="8" ht="27">
       <c r="A8" s="167" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B8" s="168" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C8" s="168" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D8" s="169"/>
       <c r="E8" s="168" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="F8" s="170" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="G8" s="169" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="H8" s="171" t="s">
         <v>170</v>
@@ -7494,37 +7498,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00870067-001F-4B56-9D09-00C4009C0057}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00ED00FC-0055-4E63-846B-00FC00BA001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B20024-00D1-4B63-BE18-00E900BC003A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002200AB-00C0-4D55-9397-008C00460005}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00120030-00CD-4B5E-A379-00C40073006F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CD002F-0080-48C5-ACF4-00F1001C00F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0088005E-0005-446F-9067-0013003900E4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00940052-0035-4D66-BED5-00F40089001C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B700FF-0005-4E0C-9930-007F002000CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001200AA-0094-405D-9548-005200E90067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005E0094-0031-4236-9E71-00BE00790039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006800EE-0048-4D02-BD5D-00AC00E1002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7574,46 +7578,46 @@
         <v>42</v>
       </c>
       <c r="B1" s="91" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C1" s="91" t="s">
         <v>433</v>
       </c>
       <c r="D1" s="91" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="E1" s="91" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="F1" s="91" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="G1" s="177" t="s">
         <v>155</v>
       </c>
       <c r="H1" s="178" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="I1" s="91" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="J1" s="91" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="K1" s="91" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="L1" s="91" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="M1" s="91" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="N1" s="91" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="O1" s="91" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="2" ht="28.5">
@@ -7621,7 +7625,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C2" s="113" t="s">
         <v>437</v>
@@ -7630,37 +7634,37 @@
         <v>263</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="G2" s="179" t="s">
         <v>162</v>
       </c>
       <c r="H2" s="179" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="J2" s="132" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="L2" s="113" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="M2" s="132" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="N2" s="132" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="3" ht="114">
@@ -7673,10 +7677,10 @@
         <v>qbank01</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E3" s="79" t="s">
         <v>37</v>
@@ -7685,24 +7689,24 @@
         <v>10</v>
       </c>
       <c r="G3" s="181" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="H3" s="181" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="I3" s="79"/>
       <c r="J3" s="181" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="K3" s="182"/>
       <c r="L3" s="79">
         <v>1</v>
       </c>
       <c r="M3" s="181" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="N3" s="181" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="O3" s="79"/>
       <c r="P3" s="183">
@@ -7719,10 +7723,10 @@
         <v>qbank01</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D4" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E4" s="79" t="s">
         <v>39</v>
@@ -7731,24 +7735,24 @@
         <v>10</v>
       </c>
       <c r="G4" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H4" s="181" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="I4" s="79"/>
       <c r="J4" s="181" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="K4" s="79"/>
       <c r="L4" s="79">
         <v>4</v>
       </c>
       <c r="M4" s="181" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="N4" s="181" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="O4" s="79"/>
       <c r="P4" s="183">
@@ -7766,10 +7770,10 @@
         <v>qbank01</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E5" s="79" t="s">
         <v>39</v>
@@ -7778,24 +7782,24 @@
         <v>10</v>
       </c>
       <c r="G5" s="181" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H5" s="181" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="I5" s="79"/>
       <c r="J5" s="181" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="K5" s="79"/>
       <c r="L5" s="79">
         <v>3</v>
       </c>
       <c r="M5" s="181" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="N5" s="181" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="O5" s="79"/>
       <c r="P5" s="183">
@@ -7813,10 +7817,10 @@
         <v>qbank01</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E6" s="79" t="s">
         <v>39</v>
@@ -7825,24 +7829,24 @@
         <v>10</v>
       </c>
       <c r="G6" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H6" s="181" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="I6" s="79"/>
       <c r="J6" s="181" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="K6" s="79"/>
       <c r="L6" s="79">
         <v>2</v>
       </c>
       <c r="M6" s="181" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="N6" s="181" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="O6" s="79"/>
       <c r="P6" s="183">
@@ -7860,10 +7864,10 @@
         <v>qbank01</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D7" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E7" s="79" t="s">
         <v>39</v>
@@ -7872,24 +7876,24 @@
         <v>10</v>
       </c>
       <c r="G7" s="181" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="H7" s="181" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="I7" s="79"/>
       <c r="J7" s="181" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="K7" s="79"/>
       <c r="L7" s="79">
         <v>1</v>
       </c>
       <c r="M7" s="181" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="N7" s="181" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="O7" s="79"/>
       <c r="P7" s="183">
@@ -7907,10 +7911,10 @@
         <v>qbank01</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E8" s="79" t="s">
         <v>39</v>
@@ -7919,24 +7923,24 @@
         <v>10</v>
       </c>
       <c r="G8" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H8" s="181" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="I8" s="182"/>
       <c r="J8" s="181" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="K8" s="79"/>
       <c r="L8" s="79">
         <v>2</v>
       </c>
       <c r="M8" s="181" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="N8" s="181" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="O8" s="184"/>
       <c r="P8" s="183">
@@ -7954,10 +7958,10 @@
         <v>qbank01</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E9" s="79" t="s">
         <v>39</v>
@@ -7966,24 +7970,24 @@
         <v>10</v>
       </c>
       <c r="G9" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H9" s="181" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="I9" s="182"/>
       <c r="J9" s="181" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="K9" s="79"/>
       <c r="L9" s="79">
         <v>3</v>
       </c>
       <c r="M9" s="181" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="N9" s="181" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="O9" s="79"/>
       <c r="P9" s="183">
@@ -8001,10 +8005,10 @@
         <v>qbank01</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E10" s="79" t="s">
         <v>37</v>
@@ -8013,21 +8017,21 @@
         <v>9</v>
       </c>
       <c r="G10" s="181" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H10" s="181" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="I10" s="79"/>
       <c r="J10" s="79"/>
       <c r="K10" s="81" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="L10" s="79">
         <v>2</v>
       </c>
       <c r="M10" s="181" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="N10" s="181"/>
       <c r="O10" s="79"/>
@@ -8046,10 +8050,10 @@
         <v>qbank01</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D11" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E11" s="79" t="s">
         <v>37</v>
@@ -8058,26 +8062,26 @@
         <v>10</v>
       </c>
       <c r="G11" s="181" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H11" s="181" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="I11" s="81" t="s">
         <v>319</v>
       </c>
       <c r="J11" s="181" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="K11" s="79"/>
       <c r="L11" s="79">
         <v>1</v>
       </c>
       <c r="M11" s="181" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="N11" s="181" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="O11" s="79"/>
       <c r="P11" s="183">
@@ -8095,36 +8099,36 @@
         <v>qbank01</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D12" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E12" s="79" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G12" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H12" s="181" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="I12" s="79"/>
       <c r="J12" s="101" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="K12" s="79"/>
       <c r="L12" s="79">
         <v>4</v>
       </c>
       <c r="M12" s="181" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="N12" s="181" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="O12" s="79"/>
       <c r="P12" s="183">
@@ -8142,36 +8146,36 @@
         <v>qbank01</v>
       </c>
       <c r="C13" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D13" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E13" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G13" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H13" s="181" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="181" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="K13" s="79"/>
       <c r="L13" s="79">
         <v>3</v>
       </c>
       <c r="M13" s="181" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="N13" s="181" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="O13" s="79"/>
       <c r="P13" s="183">
@@ -8189,33 +8193,33 @@
         <v>qbank01</v>
       </c>
       <c r="C14" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D14" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E14" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G14" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H14" s="181" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="I14" s="79"/>
       <c r="J14" s="181" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="K14" s="79"/>
       <c r="L14" s="79">
         <v>1</v>
       </c>
       <c r="M14" s="181" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="N14" s="181"/>
       <c r="O14" s="79"/>
@@ -8234,35 +8238,35 @@
         <v>qbank01</v>
       </c>
       <c r="C15" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D15" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E15" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G15" s="181" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H15" s="181" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="I15" s="79" t="s">
         <v>345</v>
       </c>
       <c r="J15" s="181" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="K15" s="182"/>
       <c r="L15" s="79">
         <v>2</v>
       </c>
       <c r="M15" s="181" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="N15" s="181"/>
       <c r="O15" s="79"/>
@@ -8281,35 +8285,35 @@
         <v>qbank01</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D16" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E16" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G16" s="181" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H16" s="181" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="I16" s="79" t="s">
         <v>345</v>
       </c>
       <c r="J16" s="181" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="K16" s="182"/>
       <c r="L16" s="79">
         <v>1</v>
       </c>
       <c r="M16" s="181" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="N16" s="181"/>
       <c r="O16" s="184"/>
@@ -8328,33 +8332,33 @@
         <v>qbank01</v>
       </c>
       <c r="C17" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D17" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E17" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G17" s="181" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="H17" s="181" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="I17" s="182"/>
       <c r="J17" s="181" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="K17" s="182"/>
       <c r="L17" s="79">
         <v>2</v>
       </c>
       <c r="M17" s="181" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="N17" s="181"/>
       <c r="O17" s="184"/>
@@ -8373,33 +8377,33 @@
         <v>qbank01</v>
       </c>
       <c r="C18" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D18" s="79" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E18" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G18" s="181" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="H18" s="181" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="I18" s="182"/>
       <c r="J18" s="181" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="K18" s="182"/>
       <c r="L18" s="79">
         <v>1</v>
       </c>
       <c r="M18" s="181" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="N18" s="181"/>
       <c r="O18" s="184"/>
@@ -8418,36 +8422,36 @@
         <v>qbank01</v>
       </c>
       <c r="C19" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D19" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E19" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G19" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H19" s="181" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="I19" s="182"/>
       <c r="J19" s="181" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="K19" s="182"/>
       <c r="L19" s="79">
         <v>3</v>
       </c>
       <c r="M19" s="181" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="N19" s="181" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="O19" s="184"/>
       <c r="P19" s="183">
@@ -8465,36 +8469,36 @@
         <v>qbank01</v>
       </c>
       <c r="C20" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D20" s="79" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="E20" s="79" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G20" s="181" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H20" s="181" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="I20" s="182"/>
       <c r="J20" s="181" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="K20" s="182"/>
       <c r="L20" s="79">
         <v>4</v>
       </c>
       <c r="M20" s="181" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="N20" s="181" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="O20" s="184"/>
       <c r="P20" s="183">
@@ -8512,36 +8516,36 @@
         <v>qbank01</v>
       </c>
       <c r="C21" s="79" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D21" s="79" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="E21" s="79" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="79" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G21" s="181" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="H21" s="181" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="I21" s="79"/>
       <c r="J21" s="181" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="K21" s="79"/>
       <c r="L21" s="79">
         <v>4</v>
       </c>
       <c r="M21" s="181" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="N21" s="181" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="O21" s="79"/>
       <c r="P21" s="183">
@@ -8559,26 +8563,26 @@
         <v>qbank01</v>
       </c>
       <c r="C22" s="79" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D22" s="79" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="E22" s="79" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="76"/>
       <c r="G22" s="181" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="H22" s="181" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="I22" s="81" t="s">
         <v>322</v>
       </c>
       <c r="J22" s="181" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="K22" s="182"/>
       <c r="L22" s="185"/>
@@ -8607,175 +8611,175 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="29" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00BB009E-00EB-4900-BFCB-00CF00C5009B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000300BC-00D5-4C9E-B2B6-0071006B002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B80085-0078-4F2D-9C4F-0079004F0059}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009200AF-0022-4B0F-AFC4-0023003500BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D10072-00EE-4F99-A0B2-00BB0049000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00500086-000D-4777-BD13-007F00BA0029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0036004F-00FE-405E-8B57-002600BC0088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CA00B3-00F4-4ED5-B3F9-00AE00A60083}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007900BA-00A0-43DD-916A-00FF005E00DB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FE008A-000E-4216-86D9-00FA00E100C9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FA00D7-006D-4F79-9C65-000900A6004B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000B0018-0091-4F0D-9157-001C00980007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A600A7-003C-46C4-88F4-00900035001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0088000A-0048-478E-8BE4-00BD006500BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000C0072-006B-4A2A-8181-000100200022}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003B0097-00E6-49BB-8BCF-00D10044000D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F00041-00C7-418C-A8B2-00B80066004B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00120088-000E-4A8F-B1C9-000F00A70097}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C10011-009B-4947-9D84-0006003F00EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CF004C-00AE-4A47-A4C7-0056005C0012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E80094-00D5-4EB1-8775-00C300C700F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0019005E-0009-45B9-8A51-00EA008C0003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00380030-00AB-42A4-A6C6-00F100310032}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003700B1-0019-4D64-9720-00E0002A00FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B80015-000B-4E4C-A6FD-00B000C400CE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F200ED-00CF-4929-A0BD-005600470041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0003006D-00BE-4A80-9D58-003500460098}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D90002-005B-404B-B184-00DD00C2009A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0073003A-003B-401E-998E-000800670030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AE0065-0027-4818-8EAB-000F008D0043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0003009C-004C-4BEB-90F1-00420064009A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A6003D-0056-42BE-867C-00DB000A000E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005600E7-0054-4F96-9289-00DF009C00F9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DE0099-00E2-46BF-BE8F-005400F8004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0044003B-00EB-4DA2-8873-007E008B0041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00460075-00BB-4979-864A-0014008A00E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005D003C-00DA-468A-9ABA-003000B30065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008B00AF-0070-4539-AB45-000C00740034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00370070-00D3-43B4-9EE2-005800BA008A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C00093-00D8-48CA-B736-00FC006400E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00790042-006D-444C-A62D-00B800F40043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00150001-00CC-4660-96C5-00E4002C003E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E9002B-0078-4948-B69C-00F600C500A8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001900CC-0041-45E9-8DC4-009C00C000A8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0086003A-006D-4AB0-AE68-006F009F004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003200E5-00C2-46C6-9BE1-005C00F30062}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0043007C-0095-4F54-8796-00A6004C009C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F4003D-00B2-4FD7-BD35-00A200F0008F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004A0077-00C7-4592-B8B8-00FA00A90000}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A8006A-00DD-4734-B0FA-00BC00660036}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C200B0-0066-4E64-B291-00E000A500D3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BA00D9-00B0-4A91-8FCF-00CD0001007E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00450038-0065-449F-A4FF-008900030060}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002100B7-00A6-402F-A7F6-000C009A0022}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0031009E-00C7-4B59-8342-007D00AB0010}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000500C8-008C-4D7A-9076-009600B00052}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A10080-0066-45E0-8780-00CD00900074}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008000FF-00AE-412F-8322-00DC00A80051}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
@@ -8821,7 +8825,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="91" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>43</v>
@@ -8854,10 +8858,10 @@
         <v>587</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>585</v>
@@ -8874,7 +8878,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="136" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C2" s="113" t="s">
         <v>47</v>
@@ -8893,7 +8897,7 @@
         <v>267</v>
       </c>
       <c r="H2" s="113" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="I2" s="187" t="str">
         <f>PROPER(I1)</f>
@@ -8910,10 +8914,10 @@
         <v>606</v>
       </c>
       <c r="M2" s="132" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="N2" s="188" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="O2" s="188" t="str">
         <f>PROPER(O1)</f>
@@ -8931,24 +8935,24 @@
     </row>
     <row r="3" s="74" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="180" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B3" s="165" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D3" s="162" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="E3" s="162"/>
       <c r="F3" s="162" t="s">
         <v>333</v>
       </c>
       <c r="G3" s="74" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="H3" s="74" t="s">
         <v>279</v>
@@ -8961,7 +8965,7 @@
         <v>709</v>
       </c>
       <c r="K3" s="190" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="L3" s="79" t="s">
         <v>10</v>
@@ -8970,10 +8974,10 @@
         <v>9</v>
       </c>
       <c r="N3" s="189" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="O3" s="74" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="P3" s="191" t="s">
         <v>170</v>
@@ -8985,24 +8989,24 @@
     </row>
     <row r="4" s="74" customFormat="1" ht="27">
       <c r="A4" s="180" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B4" s="165" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D4" s="162" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="E4" s="162"/>
       <c r="F4" s="162" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H4" s="74" t="s">
         <v>419</v>
@@ -9015,7 +9019,7 @@
         <v>709</v>
       </c>
       <c r="K4" s="190" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="L4" s="79" t="s">
         <v>10</v>
@@ -9024,10 +9028,10 @@
         <v>9</v>
       </c>
       <c r="N4" s="189" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="O4" s="74" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="P4" s="191" t="str">
         <f>P3</f>
@@ -9040,24 +9044,24 @@
     </row>
     <row r="5" ht="27">
       <c r="A5" s="180" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B5" s="165"/>
       <c r="C5" s="74" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D5" s="162" t="s">
         <v>706</v>
       </c>
       <c r="E5" s="162"/>
       <c r="F5" s="162" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="I5" s="172"/>
       <c r="J5" s="189"/>
@@ -9076,24 +9080,24 @@
     </row>
     <row r="6" ht="27">
       <c r="A6" s="180" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B6" s="165"/>
       <c r="C6" s="74" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D6" s="162" t="s">
         <v>706</v>
       </c>
       <c r="E6" s="162"/>
       <c r="F6" s="162" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="G6" s="74" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="H6" s="74" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="I6" s="172"/>
       <c r="J6" s="189"/>
@@ -9112,24 +9116,24 @@
     </row>
     <row r="7" ht="40.5">
       <c r="A7" s="180" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B7" s="165"/>
       <c r="C7" s="74" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D7" s="162" t="s">
         <v>706</v>
       </c>
       <c r="E7" s="162"/>
       <c r="F7" s="162" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G7" s="74" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H7" s="74" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I7" s="172"/>
       <c r="J7" s="189"/>
@@ -9148,14 +9152,14 @@
     </row>
     <row r="8" ht="27">
       <c r="A8" s="180" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B8" s="165"/>
       <c r="C8" s="74" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D8" s="162" t="s">
-        <v>877</v>
+        <v>726</v>
       </c>
       <c r="E8" s="162"/>
       <c r="F8" s="162" t="s">
@@ -9226,67 +9230,67 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11" disablePrompts="0">
-        <x14:dataValidation xr:uid="{006700C2-0050-4797-A9B4-005B00A40062}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00780020-00C9-46E1-9884-00CD00000086}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FC00CA-00BD-4199-8A89-009500E700EC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D20004-0043-47EA-B4E1-004800F200E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007D00B2-00D8-4EDC-B36B-00F000BD004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0010001F-0091-4771-BA17-00EB000D00D1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>M3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C200B7-0050-4035-A5AC-008200820020}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007F00C7-00A7-456F-B219-00FE00FC00C5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>M4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0022007C-009C-40D9-829A-00C9008D00A3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000900B2-0095-408D-B639-0009004200D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DB0083-00D6-4166-9AD7-003C00970024}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DE0070-000E-4DF9-902B-009000AF002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0066003E-005B-41F4-B79A-006E007900C8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D30010-00E5-46B4-97F8-0051007400E9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B80001-00A6-4026-9AE3-007B00DD008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A7000A-0066-4B2C-85BD-0052001B00FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004B0009-006F-4394-8094-003A006C0051}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A7003C-0066-4429-82CB-009400320084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009C006C-0094-4B9F-99CE-007A000A008A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B000C5-00CE-4C6A-BB15-00DC002B0075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001D004D-00A6-4FFF-8E65-00DC001E0089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0031009D-003E-4D1F-ADD0-00B00089009B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -11133,37 +11137,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{004E00DA-00B7-44A7-8D28-00EC00A90009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C10091-0012-439D-9BC6-006B005B00C5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DA0035-0093-4837-8445-00E6003A00CC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009A00DE-0087-46A2-B5CA-0001002300F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C900FC-004A-4BBF-9A80-00D2008F0043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0006006D-0038-483B-B9A4-00B600ED0006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003E00DF-0086-47B6-831B-001200B900BD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E6002B-0083-4E59-A3CA-000100EF000F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008800CF-0003-41C9-9B2F-00CE0079003A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AD00D1-004E-40F4-B313-009E00560081}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003E00DE-006B-4785-9A41-0003005D002F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006D0011-006E-4FB5-A064-002E00BB0084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -12371,31 +12375,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00AF0096-00FF-4A71-B265-004300F000F1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FB0003-00C5-4DBE-A397-008000680095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006000B6-001D-4646-9043-008700920047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B200ED-0025-4F9A-909C-0052001200A0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F60040-00BD-447D-9F26-00E200B90078}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008A00EC-00DB-4E19-89F6-0010005F0023}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008800AE-0033-41E9-A74B-00F8008300E0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A60078-00BB-4EF6-9350-00AF00A70040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B5005C-005A-4BCA-83D4-0002001B0094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EC00F3-00BE-4136-8D2C-009500F1008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -12546,7 +12550,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0013001A-00C9-4176-8553-00D9003B0091}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007F0071-000E-45AF-B35B-00A700C800BC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -12680,13 +12684,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007B00A6-0000-4DD3-B307-00AF00AC00FC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009E00B5-00D5-4737-B823-0012005B00DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00750080-00D9-4C92-823A-00B200C600C6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C800D9-0060-4F49-AE8E-0092000D0023}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
ADDED: Create calendar events in MVP-Template. WIP multi-subjects events
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="15"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="te_qbanks" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="te_questions" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="te_tests" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="calendar" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="BOOLEAN_ANSWER">DB!$A$11:$A$12</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="977">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -2830,15 +2831,287 @@
   <si>
     <t>https://s3.eu-west-1.amazonaws.com/global-assets.leemons.io/cupula_borromini_51bd61a526.png</t>
   </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>repeat</t>
+  </si>
+  <si>
+    <t>isAllDay</t>
+  </si>
+  <si>
+    <t>subtask</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>hideInCalendar</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All day</t>
+  </si>
+  <si>
+    <t>Subtasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status in kanban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide in calendar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calendar to show</t>
+  </si>
+  <si>
+    <t>event01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio de curso</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>dont_repeat</t>
+  </si>
+  <si>
+    <t>event02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio de la primera evaluación</t>
+  </si>
+  <si>
+    <t>event03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Día no lectivo</t>
+  </si>
+  <si>
+    <t>event04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiesta Nacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nª Sª del Pilar</t>
+  </si>
+  <si>
+    <t>event05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiesta de Todos los Santos</t>
+  </si>
+  <si>
+    <t>event06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiesta local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nª Sª de la Almudena</t>
+  </si>
+  <si>
+    <t>event07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Día de la Constitución</t>
+  </si>
+  <si>
+    <t>event08</t>
+  </si>
+  <si>
+    <t>event09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nª Sª de la Inmaculada</t>
+  </si>
+  <si>
+    <t>event10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final de la primera evaluación</t>
+  </si>
+  <si>
+    <t>event11</t>
+  </si>
+  <si>
+    <t>event12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio de la segunda evaluación</t>
+  </si>
+  <si>
+    <t>event13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiesta del colegio</t>
+  </si>
+  <si>
+    <t>event14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semana cultural</t>
+  </si>
+  <si>
+    <t>event15</t>
+  </si>
+  <si>
+    <t>event16</t>
+  </si>
+  <si>
+    <t>event17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final de la segunda evaluación</t>
+  </si>
+  <si>
+    <t>event18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semana Santa</t>
+  </si>
+  <si>
+    <t>event19</t>
+  </si>
+  <si>
+    <t>event20</t>
+  </si>
+  <si>
+    <t>event21</t>
+  </si>
+  <si>
+    <t>event22</t>
+  </si>
+  <si>
+    <t>event23</t>
+  </si>
+  <si>
+    <t>event24</t>
+  </si>
+  <si>
+    <t>event25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio de la tercera evaluación</t>
+  </si>
+  <si>
+    <t>event26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final de la tercera evaluación</t>
+  </si>
+  <si>
+    <t>event27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Último día lectivo</t>
+  </si>
+  <si>
+    <t>event28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluación extraordinaria</t>
+  </si>
+  <si>
+    <t>event29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proyecto Socio-lingüístico</t>
+  </si>
+  <si>
+    <t>asignatura02|asignatura03</t>
+  </si>
+  <si>
+    <t>event31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examen de matemáticas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operaciones combinadas</t>
+  </si>
+  <si>
+    <t>asignatura04</t>
+  </si>
+  <si>
+    <t>event32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test de Cooper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¡Desayuno saludable!</t>
+  </si>
+  <si>
+    <t>asignatura06</t>
+  </si>
+  <si>
+    <t>event33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrega trabajo Música</t>
+  </si>
+  <si>
+    <t>asignatura08</t>
+  </si>
+  <si>
+    <t>event34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examen de Français</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unité 5: On part en vacances!</t>
+  </si>
+  <si>
+    <t>event35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corregir exámenes FR 2ºA</t>
+  </si>
+  <si>
+    <t>event36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparar examen final de Geografía e Historia de 1º ESO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparar preguntas
+|Resolver para validar</t>
+  </si>
+  <si>
+    <t>event37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corregir exámenes de francés de 2ºB.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="160" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="161" formatCode="dd/mm/yy h:mm;@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -2970,6 +3243,18 @@
       <color theme="0" tint="-0.34998626667073579"/>
       <sz val="10.000000"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
+      <color theme="0"/>
+      <sz val="10.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Menlo"/>
+      <color rgb="FFCDCDCD"/>
+      <sz val="8.500000"/>
     </font>
   </fonts>
   <fills count="24">
@@ -3112,7 +3397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -3462,12 +3747,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="200">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4028,6 +4326,30 @@
     </xf>
     <xf fontId="11" fillId="4" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="20" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="14" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="14" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="14" fillId="16" borderId="27" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="11" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="11" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="21" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="11" fillId="4" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5166,13 +5488,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00B70096-000B-479F-B4C9-00CA00840003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002900CD-0043-46F1-9BCA-00D1003E00A1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00490028-0023-4587-9B54-00FB002C0007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002700B2-0066-4D7C-8418-007800130057}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5317,7 +5639,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00280012-0072-42EF-9091-006600610089}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004400C7-0069-4EC0-9812-00F600C6005D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7194,7 +7516,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -7498,37 +7820,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00ED00FC-0055-4E63-846B-00FC00BA001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008C0079-006B-4E0F-B786-00F900A200E2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002200AB-00C0-4D55-9397-008C00460005}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C800DD-0018-40AB-ABAC-00CF0089008E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CD002F-0080-48C5-ACF4-00F1001C00F7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006F003F-0007-48E4-9C13-00ED00A50000}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00940052-0035-4D66-BED5-00F40089001C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00130010-00BA-4B98-9D81-002700AD0055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001200AA-0094-405D-9548-005200E90067}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00900026-0018-4C7B-A5F7-00EC00440030}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006800EE-0048-4D02-BD5D-00AC00E1002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A600BE-0029-41C4-AC9B-005A007300AB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -8611,175 +8933,175 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="29" disablePrompts="0">
-        <x14:dataValidation xr:uid="{000300BC-00D5-4C9E-B2B6-0071006B002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A400F1-007A-4172-8931-0089007E004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009200AF-0022-4B0F-AFC4-0023003500BF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003B001F-002F-4D4C-9659-00A800BD0065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00500086-000D-4777-BD13-007F00BA0029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EA0023-00B0-43DC-8905-002400A6005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CA00B3-00F4-4ED5-B3F9-00AE00A60083}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E900A5-0007-4D7F-AF93-003100E70008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE008A-000E-4216-86D9-00FA00E100C9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009F0068-000E-49EA-9C6D-0062002A0048}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000B0018-0091-4F0D-9157-001C00980007}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004800EC-00AE-48E1-8B50-00DA00B10006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0088000A-0048-478E-8BE4-00BD006500BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0043006F-006E-4651-AEBA-0080005200F9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003B0097-00E6-49BB-8BCF-00D10044000D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005F003F-00BB-43C0-BF9B-00A50033006F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00120088-000E-4A8F-B1C9-000F00A70097}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EB00F7-008F-40FC-B9D5-00F700B100CD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CF004C-00AE-4A47-A4C7-0056005C0012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BE00F4-00F1-4B0E-B4B9-00EF00EC009F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0019005E-0009-45B9-8A51-00EA008C0003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DA0059-00E5-4BC3-961C-00F400B20043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003700B1-0019-4D64-9720-00E0002A00FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001800FA-0098-4EE7-A823-005C00B000AF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F200ED-00CF-4929-A0BD-005600470041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C80008-0067-4213-8079-00D000C900EB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D90002-005B-404B-B184-00DD00C2009A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BC0012-0050-44B3-84FC-009D00460061}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AE0065-0027-4818-8EAB-000F008D0043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00350061-00D1-4D34-9A49-00B600070062}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A6003D-0056-42BE-867C-00DB000A000E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B900AF-00E1-4C2B-ABC9-00FF009C00F5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DE0099-00E2-46BF-BE8F-005400F8004F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0070009C-00BE-4DD9-AFEE-0079002600FA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00460075-00BB-4979-864A-0014008A00E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0080001F-005D-4469-B4D0-007800F300C4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008B00AF-0070-4539-AB45-000C00740034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AB0084-00F7-434F-9F7A-002400DD008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C00093-00D8-48CA-B736-00FC006400E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007D0038-004F-4859-A8DB-00DD00E50033}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00150001-00CC-4660-96C5-00E4002C003E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008900E6-00E4-4CF4-AAC4-003000F200FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001900CC-0041-45E9-8DC4-009C00C000A8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006D0065-0002-4A4E-8CA6-000F00830075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003200E5-00C2-46C6-9BE1-005C00F30062}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EE0034-0040-42F4-9CEA-0014009B00F6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F4003D-00B2-4FD7-BD35-00A200F0008F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E300A8-009A-486B-8573-00F300350034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A8006A-00DD-4734-B0FA-00BC00660036}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007D00BF-00D8-4C6A-91DF-005800AD0008}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00BA00D9-00B0-4A91-8FCF-00CD0001007E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C6005C-00F4-4CE2-99F3-00FE007E00C6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002100B7-00A6-402F-A7F6-000C009A0022}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00650083-00DD-4306-88AB-00C000A3003E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000500C8-008C-4D7A-9076-009600B00052}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002E00F5-006C-4A40-8C6E-00F7008E00C6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008000FF-00AE-412F-8322-00DC00A80051}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002A0019-00A6-4884-B6EC-002300C30006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
@@ -9230,71 +9552,2130 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00780020-00C9-46E1-9884-00CD00000086}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002100C3-00DD-47FF-8EE5-003900EC00EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D20004-0043-47EA-B4E1-004800F200E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BE00B4-0022-4CA2-AE6D-004E00AB006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0010001F-0091-4771-BA17-00EB000D00D1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C6006A-0039-4504-B3C9-00D4009300C9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>M3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007F00C7-00A7-456F-B219-00FE00FC00C5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000100C5-004F-43AC-9138-004D00BB0029}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>M4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000900B2-0095-408D-B639-0009004200D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006A0007-0060-42A9-B3A3-000200130055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DE0070-000E-4DF9-902B-009000AF002E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BB0064-0018-4FB0-967E-00C000C900D7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D30010-00E5-46B4-97F8-0051007400E9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C0007F-007F-4102-8ADC-00B7007500EF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A7000A-0066-4B2C-85BD-0052001B00FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003E008A-0045-425B-9F13-004800840042}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A7003C-0066-4429-82CB-009400320084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C400CE-00A0-4B8F-A31E-0028002C00C2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B000C5-00CE-4C6A-BB15-00DC002B0075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EF008F-0036-4566-B9D7-005D000100A6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0031009D-003E-4D1F-ADD0-00B00089009B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009B0029-00B1-44E2-AFAB-004700500051}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>Q9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" style="9" width="9.140625"/>
+    <col customWidth="1" min="2" max="2" style="9" width="37.140625"/>
+    <col min="3" max="3" style="174" width="9.140625"/>
+    <col customWidth="1" min="4" max="4" style="9" width="15.28125"/>
+    <col customWidth="1" min="5" max="5" style="9" width="16.28125"/>
+    <col customWidth="1" min="6" max="6" style="9" width="14.57421875"/>
+    <col min="7" max="7" style="9" width="9.140625"/>
+    <col customWidth="1" min="8" max="8" style="9" width="42.421875"/>
+    <col customWidth="1" min="9" max="9" style="152" width="22.8515625"/>
+    <col bestFit="1" min="10" max="10" style="9" width="14.61328125"/>
+    <col min="11" max="11" width="14.61328125"/>
+    <col customWidth="1" min="12" max="12" width="24.140625"/>
+    <col customWidth="1" min="13" max="13" style="174" width="11.8515625"/>
+    <col min="14" max="16384" style="9" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>433</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>888</v>
+      </c>
+      <c r="E1" s="91" t="s">
+        <v>889</v>
+      </c>
+      <c r="F1" s="91" t="s">
+        <v>890</v>
+      </c>
+      <c r="G1" s="91" t="s">
+        <v>891</v>
+      </c>
+      <c r="H1" s="178" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="178" t="s">
+        <v>892</v>
+      </c>
+      <c r="J1" s="178" t="s">
+        <v>893</v>
+      </c>
+      <c r="K1" s="91" t="s">
+        <v>894</v>
+      </c>
+      <c r="L1" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="91" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" s="74" customFormat="1" ht="35.25" customHeight="1">
+      <c r="A2" s="192" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="193" t="str">
+        <f>PROPER(B1)</f>
+        <v>Title</v>
+      </c>
+      <c r="C2" s="194" t="str">
+        <f>PROPER(C1)</f>
+        <v>Type</v>
+      </c>
+      <c r="D2" s="194" t="s">
+        <v>895</v>
+      </c>
+      <c r="E2" s="194" t="s">
+        <v>896</v>
+      </c>
+      <c r="F2" s="193" t="s">
+        <v>890</v>
+      </c>
+      <c r="G2" s="193" t="s">
+        <v>897</v>
+      </c>
+      <c r="H2" s="193" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="193" t="s">
+        <v>898</v>
+      </c>
+      <c r="J2" s="193" t="s">
+        <v>899</v>
+      </c>
+      <c r="K2" s="194" t="s">
+        <v>900</v>
+      </c>
+      <c r="L2" s="195" t="s">
+        <v>901</v>
+      </c>
+      <c r="M2" s="195" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="180" t="s">
+        <v>902</v>
+      </c>
+      <c r="B3" s="196" t="s">
+        <v>903</v>
+      </c>
+      <c r="C3" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D3" s="197">
+        <v>44447</v>
+      </c>
+      <c r="E3" s="197">
+        <v>44447</v>
+      </c>
+      <c r="F3" s="198" t="s">
+        <v>905</v>
+      </c>
+      <c r="G3" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="74"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="172" t="str">
+        <f>ap_programs!A5</f>
+        <v>programB</v>
+      </c>
+      <c r="M3" s="172" t="str">
+        <f>users!A3</f>
+        <v>admin01</v>
+      </c>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="180" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>907</v>
+      </c>
+      <c r="C4" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D4" s="197">
+        <v>44447</v>
+      </c>
+      <c r="E4" s="197">
+        <v>44447</v>
+      </c>
+      <c r="F4" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G4" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="74"/>
+      <c r="I4" s="162"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="199" t="str">
+        <f>L3</f>
+        <v>programB</v>
+      </c>
+      <c r="M4" s="172" t="str">
+        <f>M3</f>
+        <v>admin01</v>
+      </c>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="180" t="s">
+        <v>908</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C5" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D5" s="197">
+        <v>44480</v>
+      </c>
+      <c r="E5" s="197">
+        <v>44480</v>
+      </c>
+      <c r="F5" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G5" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="74"/>
+      <c r="I5" s="162"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="199" t="str">
+        <f>L4</f>
+        <v>programB</v>
+      </c>
+      <c r="M5" s="172" t="str">
+        <f>M4</f>
+        <v>admin01</v>
+      </c>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="180" t="s">
+        <v>910</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>911</v>
+      </c>
+      <c r="C6" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D6" s="197">
+        <v>44481</v>
+      </c>
+      <c r="E6" s="197">
+        <v>44481</v>
+      </c>
+      <c r="F6" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G6" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="74" t="s">
+        <v>912</v>
+      </c>
+      <c r="I6" s="162"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="199" t="str">
+        <f>L5</f>
+        <v>programB</v>
+      </c>
+      <c r="M6" s="172" t="str">
+        <f>M5</f>
+        <v>admin01</v>
+      </c>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" s="180" t="s">
+        <v>913</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>911</v>
+      </c>
+      <c r="C7" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D7" s="197">
+        <v>44501</v>
+      </c>
+      <c r="E7" s="197">
+        <v>44501</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G7" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="74" t="s">
+        <v>914</v>
+      </c>
+      <c r="I7" s="162"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="199" t="str">
+        <f>L6</f>
+        <v>programB</v>
+      </c>
+      <c r="M7" s="172" t="str">
+        <f>M6</f>
+        <v>admin01</v>
+      </c>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" ht="19.5" customHeight="1">
+      <c r="A8" s="180" t="s">
+        <v>915</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>916</v>
+      </c>
+      <c r="C8" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D8" s="197">
+        <v>44509</v>
+      </c>
+      <c r="E8" s="197">
+        <v>44509</v>
+      </c>
+      <c r="F8" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G8" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="74" t="s">
+        <v>917</v>
+      </c>
+      <c r="I8" s="162"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="172" t="str">
+        <f>L7</f>
+        <v>programB</v>
+      </c>
+      <c r="M8" s="172" t="str">
+        <f>M7</f>
+        <v>admin01</v>
+      </c>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" ht="19.5" customHeight="1">
+      <c r="A9" s="180" t="s">
+        <v>918</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>911</v>
+      </c>
+      <c r="C9" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D9" s="197">
+        <v>44536</v>
+      </c>
+      <c r="E9" s="197">
+        <v>44536</v>
+      </c>
+      <c r="F9" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G9" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>919</v>
+      </c>
+      <c r="I9" s="162"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="172" t="str">
+        <f>L8</f>
+        <v>programB</v>
+      </c>
+      <c r="M9" s="172" t="str">
+        <f>M8</f>
+        <v>admin01</v>
+      </c>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" ht="19.5" customHeight="1">
+      <c r="A10" s="180" t="s">
+        <v>920</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C10" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D10" s="197">
+        <v>44537</v>
+      </c>
+      <c r="E10" s="197">
+        <v>44537</v>
+      </c>
+      <c r="F10" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G10" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="74"/>
+      <c r="I10" s="162"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="172" t="str">
+        <f>L9</f>
+        <v>programB</v>
+      </c>
+      <c r="M10" s="172" t="str">
+        <f>M9</f>
+        <v>admin01</v>
+      </c>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" ht="19.5" customHeight="1">
+      <c r="A11" s="180" t="s">
+        <v>921</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>911</v>
+      </c>
+      <c r="C11" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D11" s="197">
+        <v>44538</v>
+      </c>
+      <c r="E11" s="197">
+        <v>44538</v>
+      </c>
+      <c r="F11" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G11" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="74" t="s">
+        <v>922</v>
+      </c>
+      <c r="I11" s="162"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="172" t="str">
+        <f>L10</f>
+        <v>programB</v>
+      </c>
+      <c r="M11" s="172" t="str">
+        <f>M10</f>
+        <v>admin01</v>
+      </c>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" ht="19.5" customHeight="1">
+      <c r="A12" s="180" t="s">
+        <v>923</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>924</v>
+      </c>
+      <c r="C12" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D12" s="197">
+        <v>44552</v>
+      </c>
+      <c r="E12" s="197">
+        <v>44552</v>
+      </c>
+      <c r="F12" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G12" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="74"/>
+      <c r="I12" s="162"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="172" t="str">
+        <f>L11</f>
+        <v>programB</v>
+      </c>
+      <c r="M12" s="172" t="str">
+        <f>M11</f>
+        <v>admin01</v>
+      </c>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" ht="19.5" customHeight="1">
+      <c r="A13" s="180" t="s">
+        <v>925</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C13" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D13" s="197">
+        <v>44568</v>
+      </c>
+      <c r="E13" s="197">
+        <v>44568</v>
+      </c>
+      <c r="F13" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G13" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="74"/>
+      <c r="I13" s="162"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="172" t="str">
+        <f>L12</f>
+        <v>programB</v>
+      </c>
+      <c r="M13" s="172" t="str">
+        <f>M12</f>
+        <v>admin01</v>
+      </c>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" ht="19.5" customHeight="1">
+      <c r="A14" s="180" t="s">
+        <v>926</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>927</v>
+      </c>
+      <c r="C14" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D14" s="197">
+        <v>44571</v>
+      </c>
+      <c r="E14" s="197">
+        <v>44571</v>
+      </c>
+      <c r="F14" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G14" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="74"/>
+      <c r="I14" s="162"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="172" t="str">
+        <f>L13</f>
+        <v>programB</v>
+      </c>
+      <c r="M14" s="172" t="str">
+        <f>M13</f>
+        <v>admin01</v>
+      </c>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1">
+      <c r="A15" s="180" t="s">
+        <v>928</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>929</v>
+      </c>
+      <c r="C15" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D15" s="197">
+        <v>44596</v>
+      </c>
+      <c r="E15" s="197">
+        <v>44596</v>
+      </c>
+      <c r="F15" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G15" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="74"/>
+      <c r="I15" s="162"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="172" t="str">
+        <f>L14</f>
+        <v>programB</v>
+      </c>
+      <c r="M15" s="172" t="str">
+        <f>M14</f>
+        <v>admin01</v>
+      </c>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" ht="19.5" customHeight="1">
+      <c r="A16" s="180" t="s">
+        <v>930</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>931</v>
+      </c>
+      <c r="C16" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D16" s="197">
+        <v>44606</v>
+      </c>
+      <c r="E16" s="197">
+        <v>44610</v>
+      </c>
+      <c r="F16" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G16" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="74"/>
+      <c r="I16" s="162"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="172" t="str">
+        <f>L15</f>
+        <v>programB</v>
+      </c>
+      <c r="M16" s="172" t="str">
+        <f>M15</f>
+        <v>admin01</v>
+      </c>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" ht="19.5" customHeight="1">
+      <c r="A17" s="180" t="s">
+        <v>932</v>
+      </c>
+      <c r="B17" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C17" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D17" s="197">
+        <v>44617</v>
+      </c>
+      <c r="E17" s="197">
+        <v>44617</v>
+      </c>
+      <c r="F17" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G17" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="74"/>
+      <c r="I17" s="162"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="172" t="str">
+        <f>L16</f>
+        <v>programB</v>
+      </c>
+      <c r="M17" s="172" t="str">
+        <f>M16</f>
+        <v>admin01</v>
+      </c>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" ht="19.5" customHeight="1">
+      <c r="A18" s="180" t="s">
+        <v>933</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C18" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D18" s="197">
+        <v>44620</v>
+      </c>
+      <c r="E18" s="197">
+        <v>44617</v>
+      </c>
+      <c r="F18" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G18" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="74"/>
+      <c r="I18" s="162"/>
+      <c r="J18" s="74"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="172" t="str">
+        <f>L17</f>
+        <v>programB</v>
+      </c>
+      <c r="M18" s="172" t="str">
+        <f>M17</f>
+        <v>admin01</v>
+      </c>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" ht="19.5" customHeight="1">
+      <c r="A19" s="180" t="s">
+        <v>934</v>
+      </c>
+      <c r="B19" s="74" t="s">
+        <v>935</v>
+      </c>
+      <c r="C19" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D19" s="197">
+        <v>44658</v>
+      </c>
+      <c r="E19" s="197">
+        <v>44658</v>
+      </c>
+      <c r="F19" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G19" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="74"/>
+      <c r="I19" s="162"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="172" t="str">
+        <f>L18</f>
+        <v>programB</v>
+      </c>
+      <c r="M19" s="172" t="str">
+        <f>M18</f>
+        <v>admin01</v>
+      </c>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" ht="19.5" customHeight="1">
+      <c r="A20" s="180" t="s">
+        <v>936</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C20" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D20" s="197">
+        <v>44659</v>
+      </c>
+      <c r="E20" s="197">
+        <v>44659</v>
+      </c>
+      <c r="F20" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G20" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="74" t="s">
+        <v>937</v>
+      </c>
+      <c r="I20" s="162"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="172" t="str">
+        <f>L19</f>
+        <v>programB</v>
+      </c>
+      <c r="M20" s="172" t="str">
+        <f>M19</f>
+        <v>admin01</v>
+      </c>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" ht="19.5" customHeight="1">
+      <c r="A21" s="180" t="s">
+        <v>938</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C21" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D21" s="197">
+        <v>44662</v>
+      </c>
+      <c r="E21" s="197">
+        <v>44662</v>
+      </c>
+      <c r="F21" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G21" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="74" t="s">
+        <v>937</v>
+      </c>
+      <c r="I21" s="162"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="172" t="str">
+        <f>L20</f>
+        <v>programB</v>
+      </c>
+      <c r="M21" s="172" t="str">
+        <f>M20</f>
+        <v>admin01</v>
+      </c>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1">
+      <c r="A22" s="180" t="s">
+        <v>939</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C22" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D22" s="197">
+        <v>44663</v>
+      </c>
+      <c r="E22" s="197">
+        <v>44663</v>
+      </c>
+      <c r="F22" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G22" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="74" t="s">
+        <v>937</v>
+      </c>
+      <c r="I22" s="162"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="172" t="str">
+        <f>L21</f>
+        <v>programB</v>
+      </c>
+      <c r="M22" s="172" t="str">
+        <f>M21</f>
+        <v>admin01</v>
+      </c>
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" ht="19.5" customHeight="1">
+      <c r="A23" s="180" t="s">
+        <v>940</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C23" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D23" s="197">
+        <v>44664</v>
+      </c>
+      <c r="E23" s="197">
+        <v>44664</v>
+      </c>
+      <c r="F23" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G23" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="74" t="s">
+        <v>937</v>
+      </c>
+      <c r="I23" s="162"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="172" t="str">
+        <f>L22</f>
+        <v>programB</v>
+      </c>
+      <c r="M23" s="172" t="str">
+        <f>M22</f>
+        <v>admin01</v>
+      </c>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" ht="19.5" customHeight="1">
+      <c r="A24" s="180" t="s">
+        <v>941</v>
+      </c>
+      <c r="B24" s="74" t="s">
+        <v>911</v>
+      </c>
+      <c r="C24" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D24" s="197">
+        <v>44665</v>
+      </c>
+      <c r="E24" s="197">
+        <v>44665</v>
+      </c>
+      <c r="F24" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G24" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="74" t="s">
+        <v>937</v>
+      </c>
+      <c r="I24" s="162"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="172" t="str">
+        <f>L23</f>
+        <v>programB</v>
+      </c>
+      <c r="M24" s="172" t="str">
+        <f>M23</f>
+        <v>admin01</v>
+      </c>
+      <c r="N24" s="9"/>
+    </row>
+    <row r="25" ht="19.5" customHeight="1">
+      <c r="A25" s="180" t="s">
+        <v>942</v>
+      </c>
+      <c r="B25" s="74" t="s">
+        <v>911</v>
+      </c>
+      <c r="C25" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D25" s="197">
+        <v>44666</v>
+      </c>
+      <c r="E25" s="197">
+        <v>44666</v>
+      </c>
+      <c r="F25" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G25" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="74" t="s">
+        <v>937</v>
+      </c>
+      <c r="I25" s="162"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="172" t="str">
+        <f>L24</f>
+        <v>programB</v>
+      </c>
+      <c r="M25" s="172" t="str">
+        <f>M24</f>
+        <v>admin01</v>
+      </c>
+      <c r="N25" s="9"/>
+    </row>
+    <row r="26" ht="19.5" customHeight="1">
+      <c r="A26" s="180" t="s">
+        <v>943</v>
+      </c>
+      <c r="B26" s="74" t="s">
+        <v>909</v>
+      </c>
+      <c r="C26" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D26" s="197">
+        <v>44669</v>
+      </c>
+      <c r="E26" s="197">
+        <v>44667</v>
+      </c>
+      <c r="F26" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G26" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="74" t="s">
+        <v>937</v>
+      </c>
+      <c r="I26" s="162"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="172" t="str">
+        <f>L25</f>
+        <v>programB</v>
+      </c>
+      <c r="M26" s="172" t="str">
+        <f>M25</f>
+        <v>admin01</v>
+      </c>
+      <c r="N26" s="9"/>
+    </row>
+    <row r="27" ht="19.5" customHeight="1">
+      <c r="A27" s="180" t="s">
+        <v>944</v>
+      </c>
+      <c r="B27" s="74" t="s">
+        <v>945</v>
+      </c>
+      <c r="C27" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D27" s="197">
+        <v>44670</v>
+      </c>
+      <c r="E27" s="197">
+        <v>44670</v>
+      </c>
+      <c r="F27" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G27" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="74"/>
+      <c r="I27" s="162"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="172" t="str">
+        <f>L26</f>
+        <v>programB</v>
+      </c>
+      <c r="M27" s="172" t="str">
+        <f>M26</f>
+        <v>admin01</v>
+      </c>
+      <c r="N27" s="9"/>
+    </row>
+    <row r="28" ht="19.5" customHeight="1">
+      <c r="A28" s="180" t="s">
+        <v>946</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>947</v>
+      </c>
+      <c r="C28" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D28" s="197">
+        <v>44715</v>
+      </c>
+      <c r="E28" s="197">
+        <v>44715</v>
+      </c>
+      <c r="F28" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G28" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="74"/>
+      <c r="I28" s="162"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="172" t="str">
+        <f>L27</f>
+        <v>programB</v>
+      </c>
+      <c r="M28" s="172" t="str">
+        <f>M27</f>
+        <v>admin01</v>
+      </c>
+      <c r="N28" s="9"/>
+    </row>
+    <row r="29" ht="19.5" customHeight="1">
+      <c r="A29" s="180" t="s">
+        <v>948</v>
+      </c>
+      <c r="B29" s="74" t="s">
+        <v>949</v>
+      </c>
+      <c r="C29" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D29" s="197">
+        <v>44736</v>
+      </c>
+      <c r="E29" s="197">
+        <v>44736</v>
+      </c>
+      <c r="F29" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G29" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="74"/>
+      <c r="I29" s="162"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="172" t="str">
+        <f>L28</f>
+        <v>programB</v>
+      </c>
+      <c r="M29" s="172" t="str">
+        <f>M28</f>
+        <v>admin01</v>
+      </c>
+      <c r="N29" s="9"/>
+    </row>
+    <row r="30" ht="19.5" customHeight="1">
+      <c r="A30" s="180" t="s">
+        <v>950</v>
+      </c>
+      <c r="B30" s="74" t="s">
+        <v>951</v>
+      </c>
+      <c r="C30" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D30" s="197">
+        <v>44739</v>
+      </c>
+      <c r="E30" s="197">
+        <v>44739</v>
+      </c>
+      <c r="F30" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G30" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="74"/>
+      <c r="I30" s="162"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="172" t="str">
+        <f>L29</f>
+        <v>programB</v>
+      </c>
+      <c r="M30" s="172" t="str">
+        <f>M29</f>
+        <v>admin01</v>
+      </c>
+      <c r="N30" s="9"/>
+    </row>
+    <row r="31" ht="19.5" customHeight="1">
+      <c r="A31" s="180" t="s">
+        <v>952</v>
+      </c>
+      <c r="B31" s="74" t="s">
+        <v>953</v>
+      </c>
+      <c r="C31" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D31" s="197">
+        <v>44684</v>
+      </c>
+      <c r="E31" s="197">
+        <v>44697</v>
+      </c>
+      <c r="F31" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G31" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="74" t="s">
+        <v>636</v>
+      </c>
+      <c r="I31" s="162"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="172" t="s">
+        <v>954</v>
+      </c>
+      <c r="M31" s="172" t="str">
+        <f>users!A4</f>
+        <v>teacher01</v>
+      </c>
+      <c r="N31" s="9"/>
+    </row>
+    <row r="32" ht="19.5" customHeight="1">
+      <c r="A32" s="180" t="s">
+        <v>955</v>
+      </c>
+      <c r="B32" s="74" t="s">
+        <v>956</v>
+      </c>
+      <c r="C32" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D32" s="197">
+        <v>44698.489583333336</v>
+      </c>
+      <c r="E32" s="197">
+        <v>44698.527777777781</v>
+      </c>
+      <c r="F32" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G32" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="74" t="s">
+        <v>957</v>
+      </c>
+      <c r="I32" s="162"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="172" t="s">
+        <v>958</v>
+      </c>
+      <c r="M32" s="172" t="str">
+        <f>users!A5</f>
+        <v>teacher02</v>
+      </c>
+      <c r="N32" s="9"/>
+    </row>
+    <row r="33" ht="19.5" customHeight="1">
+      <c r="A33" s="180" t="s">
+        <v>959</v>
+      </c>
+      <c r="B33" s="74" t="s">
+        <v>960</v>
+      </c>
+      <c r="C33" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D33" s="197">
+        <v>44711.430555555555</v>
+      </c>
+      <c r="E33" s="197">
+        <v>44711.46875</v>
+      </c>
+      <c r="F33" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G33" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="74" t="s">
+        <v>961</v>
+      </c>
+      <c r="I33" s="162"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="172" t="s">
+        <v>962</v>
+      </c>
+      <c r="M33" s="172" t="str">
+        <f>M32</f>
+        <v>teacher02</v>
+      </c>
+      <c r="N33" s="9"/>
+    </row>
+    <row r="34" ht="19.5" customHeight="1">
+      <c r="A34" s="180" t="s">
+        <v>963</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>964</v>
+      </c>
+      <c r="C34" s="190" t="s">
+        <v>904</v>
+      </c>
+      <c r="D34" s="197">
+        <v>44700.354166666664</v>
+      </c>
+      <c r="E34" s="197">
+        <v>44700.392361111109</v>
+      </c>
+      <c r="F34" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G34" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="74"/>
+      <c r="I34" s="162"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="172" t="s">
+        <v>965</v>
+      </c>
+      <c r="M34" s="172" t="str">
+        <f>M33</f>
+        <v>teacher02</v>
+      </c>
+      <c r="N34" s="9"/>
+    </row>
+    <row r="35" ht="19.5" customHeight="1">
+      <c r="A35" s="180" t="s">
+        <v>966</v>
+      </c>
+      <c r="B35" s="74" t="s">
+        <v>967</v>
+      </c>
+      <c r="C35" s="190" t="s">
+        <v>968</v>
+      </c>
+      <c r="D35" s="197">
+        <v>44706.565972222219</v>
+      </c>
+      <c r="E35" s="197">
+        <v>44706.604166666664</v>
+      </c>
+      <c r="F35" s="79" t="s">
+        <v>905</v>
+      </c>
+      <c r="G35" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="74" t="s">
+        <v>969</v>
+      </c>
+      <c r="I35" s="162"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="172" t="s">
+        <v>719</v>
+      </c>
+      <c r="M35" s="172" t="str">
+        <f>M31</f>
+        <v>teacher01</v>
+      </c>
+      <c r="N35" s="9"/>
+    </row>
+    <row r="36" ht="19.5" customHeight="1">
+      <c r="A36" s="180" t="s">
+        <v>970</v>
+      </c>
+      <c r="B36" s="74" t="s">
+        <v>971</v>
+      </c>
+      <c r="C36" s="190" t="s">
+        <v>968</v>
+      </c>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="162"/>
+      <c r="J36" s="74">
+        <v>2</v>
+      </c>
+      <c r="K36" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" s="172" t="s">
+        <v>170</v>
+      </c>
+      <c r="M36" s="172" t="str">
+        <f>M35</f>
+        <v>teacher01</v>
+      </c>
+      <c r="N36" s="9"/>
+    </row>
+    <row r="37" ht="31.850000000000001" customHeight="1">
+      <c r="A37" s="180" t="s">
+        <v>972</v>
+      </c>
+      <c r="B37" s="74" t="s">
+        <v>973</v>
+      </c>
+      <c r="C37" s="190" t="s">
+        <v>968</v>
+      </c>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="162" t="s">
+        <v>974</v>
+      </c>
+      <c r="J37" s="74">
+        <v>3</v>
+      </c>
+      <c r="K37" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="199" t="s">
+        <v>170</v>
+      </c>
+      <c r="M37" s="172" t="str">
+        <f>M36</f>
+        <v>teacher01</v>
+      </c>
+      <c r="N37" s="9"/>
+    </row>
+    <row r="38" ht="19.5" customHeight="1">
+      <c r="A38" s="180" t="s">
+        <v>975</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>976</v>
+      </c>
+      <c r="C38" s="190" t="s">
+        <v>968</v>
+      </c>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="162"/>
+      <c r="J38" s="74">
+        <v>5</v>
+      </c>
+      <c r="K38" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="L38" s="199" t="s">
+        <v>170</v>
+      </c>
+      <c r="M38" s="172" t="str">
+        <f>M37</f>
+        <v>teacher01</v>
+      </c>
+      <c r="N38" s="9"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="174"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="152"/>
+      <c r="J39" s="9"/>
+      <c r="M39" s="174"/>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="102" disablePrompts="0">
+        <x14:dataValidation xr:uid="{006E0072-004F-48FE-8B1B-0011008100CC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F36</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003F00B2-007B-404F-8B98-00D900E4001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G32</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E20007-0080-46F3-85C3-005C00DE00E2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00400082-0010-4807-86FB-0035002900D3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00DA0025-000C-4A87-A0E1-009E005A001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0050008A-0039-43EB-8B13-00F100EA003A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{005F0038-0085-4314-AA3B-00CE004C005D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003800C1-0022-4283-98C7-009D00B1006E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{001100FF-0097-4A2A-AFC0-0079008700D9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003B002E-0002-4E8F-A069-00F800F200AA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0067006C-0099-47A3-AF63-000600400010}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00DF001B-0050-46BD-8B68-00A6009400B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0088003E-0040-44FF-AF59-000400660094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{005B002F-00AD-4575-9EAE-00D1000100BD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{009D0086-00C5-44E4-92CF-00F00004003A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0065005C-0061-44CE-934C-006800C30016}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00B000A5-00E1-449C-B6F6-00C000020078}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00550028-003B-4198-98D6-00CB00970086}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00AE00CB-00DE-4501-9575-009400300024}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E3009F-003C-416D-BDF6-00F2004800D7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000B00A8-009A-4017-BAC0-002500FD00E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{009800D1-0074-4655-84E9-004E00F30012}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008E00A3-0010-4861-A472-002E00F700C7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00F70036-005F-4278-AE20-0072006400E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000B00B5-0072-42F3-A67F-003400850021}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00BB00B3-00D1-495C-A0AD-00500034003E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00AC0053-00A7-4E7E-91FB-00B30053001B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0091001D-000D-4DD1-AA85-008F009C001B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E5004A-0096-46B9-9B77-0061002700BD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E6001B-0045-41BF-8AEE-0090003A0013}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{006C00F8-00FB-4E83-8F55-0053005A0088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0026002A-007D-42A5-9B49-009200260092}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00FE0087-0092-4734-A448-00E700C5000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003C00C8-0075-42FE-B338-000F0097008E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>G12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D100D0-00C8-4438-8C31-006600E000B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{001300E7-007D-4B7A-B719-00D8002000E7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008F00D1-0093-42FB-B57E-0060001100B3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00560075-0024-4F40-AD3D-0031007A00B2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00BC0064-006C-4181-8EA6-009A005500A4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D900DA-00DB-4272-B41D-000800700027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00F200BA-002C-4BE7-95BA-0079007400D5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D40030-0061-4E5D-86B0-00A0008B00BE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{009600C6-00A1-4F22-8ED8-00AE0025002D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000B00FC-0097-449C-827B-004B00DC0038}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00A00003-0014-4C2B-9C5E-008F007A00FE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008D0029-0064-42BF-9DA5-00CC00B6005E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000500A7-00EC-4ED1-A911-004C000D0094}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000E0015-00C2-4D60-AFA0-004A00D900D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00A800FB-0042-4BF3-97F9-0035001D008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D100FB-00C7-4A10-9C22-006400E90066}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{007F00C7-00C7-46C0-AAF7-001E004E0025}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00F600D3-00B9-45E3-9F4F-000900370077}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{005900B5-00BF-442D-B49F-00A3005A00DF}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00EB002B-00E6-44C0-A027-006600AB00B8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00F600E2-00CD-42C0-9FC4-0011006C007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00AF00C5-0032-4088-9C4D-00640094002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0010005E-00DA-4FC8-8C32-0019007000DB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003B00CD-009F-461C-8F33-0090007400E9}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00540086-00BF-43AD-A47B-0005007600E4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{002E00D3-00F3-410C-A80D-0046009600D0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K32</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00160091-0011-49B2-BC59-007000B6002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00CE0037-005F-470A-9D3D-0086006D005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0050006E-0075-45F5-958A-0037002B009D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00BA005B-00C4-44AF-AF01-008600D400DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K36</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000200E2-000A-4402-B58E-002600810024}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{003E001E-0099-459D-B69F-00E100D50046}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{006300CA-0019-4767-88C2-00ED00740050}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008300D8-00A9-48D2-A5EA-0082000C006C}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{002400F3-0062-4865-B81B-000C00490009}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E90094-0078-41E9-BCB1-000E0042007B}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00BF00BA-00A9-4AF9-90A5-006000DB00C5}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00AF009B-000F-4FD0-9068-00BB00300055}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00BB0061-0029-4850-A9CC-00F700B0002F}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00B000B6-00B1-4FCB-9625-005700A7008B}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00950060-0066-4149-9398-003F003B007D}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00140003-0099-49CB-B23A-009B00C800B3}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008A00BC-00D9-46AB-8BE0-0097004900A2}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00C2001D-00DE-4498-B4CF-00F000C8003A}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0033007A-00A1-4F6A-AD23-008200DC001C}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D8003D-0099-401D-BD8C-0044005400DF}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0076005D-0093-41F4-83D9-00B2008F00B3}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00F7003A-0028-4A4A-B4A8-00E4006B0093}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00120009-0070-47FF-AD39-00E800C10027}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{006D0072-0088-4E04-9B5C-000C00B800E3}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E40038-0084-40C7-9362-006F00F10025}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000E00BC-0053-4CE4-9870-0004003B0011}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00EC00BB-0047-4D6A-935C-005700CF00DA}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0028000B-00E6-498B-9F5D-000800210080}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{004500F7-00AC-4C97-8D9C-00A9000A00FB}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00980089-00A3-48F6-BBFE-00FD002200D2}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D30028-00CB-47DF-9A41-0076009B00B8}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00670076-00AE-4FAC-9EB9-00F4001C005E}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E00022-002D-41F5-A396-007F006B0020}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F32</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00F0002A-0055-4975-8A94-004B00910044}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F33</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00D70088-00FA-4F2E-B8EB-005800C300EA}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{0093009A-0056-4150-B31A-0095003C0093}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>F35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00B900F0-00E8-4D3C-975B-00E400400095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00FE00A6-0025-4EEC-A4ED-009F008C0044}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00E900B7-0058-43D2-8E16-006600D9007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{000B0004-0020-462F-8B2B-00DD002C0065}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{008D00CB-008D-4C05-A57A-0086005A0006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K37</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{00DA00BB-00A3-497D-B179-001400A300FC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>BOOLEAN_ANSWER</xm:f>
+          </x14:formula1>
+          <xm:sqref>K38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10368,6 +12749,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="180" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -11137,37 +13519,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00C10091-0012-439D-9BC6-006B005B00C5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00F900D1-006E-461B-AC5D-00E5007F00F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009A00DE-0087-46A2-B5CA-0001002300F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E100A4-0042-4FCC-8434-00CC00D90058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0006006D-0038-483B-B9A4-00B600ED0006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006400FE-00E2-46A0-A20F-0052000A001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E6002B-0083-4E59-A3CA-000100EF000F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00070086-005C-4FBC-B23F-00810026002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AD00D1-004E-40F4-B313-009E00560081}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008D00C9-00E3-49E4-8AC8-00E500E70071}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006D0011-006E-4FB5-A064-002E00BB0084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B200FE-00ED-49D0-B904-0043007A000E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -12375,31 +14757,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00FB0003-00C5-4DBE-A397-008000680095}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005B0048-007E-4B69-BC3B-009900900037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B200ED-0025-4F9A-909C-0052001200A0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004D001F-00D5-4536-96C1-00560064003F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008A00EC-00DB-4E19-89F6-0010005F0023}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003D0057-0090-4FBB-9B1B-004500E000F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A60078-00BB-4EF6-9350-00AF00A70040}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C600BB-0039-45C1-949A-00DB000000A0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EC00F3-00BE-4136-8D2C-009500F1008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00480064-001D-4E2F-970F-006300F90064}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -12550,7 +14932,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007F0071-000E-45AF-B35B-00A700C800BC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00690010-0072-41FE-AE9D-0007008400F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -12684,13 +15066,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{009E00B5-00D5-4737-B823-0012005B00DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BB00D2-00EF-4D2B-95E0-00BA00A6002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C800D9-0060-4F49-AE8E-0092000D0023}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0074007D-0040-42DF-95EC-00EB000400C3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Finished react-query integration with NYA
* Added react-query to full NYA integration
* Fixed error in students that made them impossible to load NYA
* Added assignable related icons to NYA cards
* Added assignable name to student NYA cards
* Willy changes in excel
</commit_message>
<xml_diff>
--- a/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
+++ b/packages/leemons-plugin-mvp-template/src/bulk/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" state="visible" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="990">
   <si>
     <t xml:space="preserve">Substages frecuency</t>
   </si>
@@ -2667,9 +2667,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cuando entras a ver tu cuenta del banco y miras tu SALDO estás revisando LO QUE TE QUEDA en la cuenta.</t>
-  </si>
-  <si>
-    <t>otros</t>
   </si>
   <si>
     <t xml:space="preserve">¿Qué dice la Declaración Universal de los Derechos Humanos sobre la inmigración?</t>
@@ -5644,13 +5641,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00A30038-002C-4CD8-888B-0077009000EE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00220059-0095-4C32-887F-009400BD001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>T4 X4:Y5 V4:V5 G4:G5 K4:K5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00580088-00D3-418B-A9A8-007600270019}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00300014-00DF-4B89-BA3B-003100C20033}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>SUBSTAGES_FRECUENCY</xm:f>
           </x14:formula1>
@@ -5795,7 +5792,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{003300FD-00F4-4DAB-8FD6-00E3003E0010}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C500C9-0059-441F-9D15-003A000A00DC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -7977,7 +7974,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{000C0091-00AF-42E4-9A7F-008900D5004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005D007F-00F8-4C45-80E5-00AD00260046}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -8019,7 +8016,7 @@
     <col customWidth="1" min="13" max="13" width="114.28125"/>
     <col customWidth="1" min="14" max="14" width="35.7109375"/>
     <col customWidth="1" min="15" max="15" style="17" width="23.8515625"/>
-    <col bestFit="1" min="16" max="16" width="2.78125"/>
+    <col bestFit="1" min="16" max="16" width="2.8515625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -8968,7 +8965,7 @@
         <v>761</v>
       </c>
       <c r="D21" s="80" t="s">
-        <v>836</v>
+        <v>762</v>
       </c>
       <c r="E21" s="80" t="s">
         <v>40</v>
@@ -8980,21 +8977,21 @@
         <v>821</v>
       </c>
       <c r="H21" s="188" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="I21" s="80"/>
       <c r="J21" s="188" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="K21" s="80"/>
       <c r="L21" s="80">
         <v>4</v>
       </c>
       <c r="M21" s="188" t="s">
+        <v>838</v>
+      </c>
+      <c r="N21" s="188" t="s">
         <v>839</v>
-      </c>
-      <c r="N21" s="188" t="s">
-        <v>840</v>
       </c>
       <c r="O21" s="80"/>
       <c r="P21" s="190">
@@ -9012,10 +9009,10 @@
         <v>qbank01</v>
       </c>
       <c r="C22" s="80" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D22" s="80" t="s">
-        <v>836</v>
+        <v>762</v>
       </c>
       <c r="E22" s="80" t="s">
         <v>37</v>
@@ -9025,13 +9022,13 @@
         <v>782</v>
       </c>
       <c r="H22" s="188" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I22" s="82" t="s">
         <v>325</v>
       </c>
       <c r="J22" s="188" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="K22" s="189"/>
       <c r="L22" s="191"/>
@@ -9060,175 +9057,175 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="29" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00CC00EF-0047-4A1D-9E43-009A0067006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001C00C3-00C7-4818-B024-0036006F0026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000F0007-000C-4577-9349-005B00980017}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CB008C-0051-4388-BFC6-002400A0000F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DB0073-0040-48CD-8538-003300E2002C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000000EA-002D-4732-A5DA-00D4004000B8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0013008F-00F8-4775-A811-00D9003900AD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0094004A-004C-4846-91D6-005E00A000A8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00230006-001B-490C-880E-005C00F700F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C40094-00C6-4B64-B0AD-00DF00A60049}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002600AD-0059-4AAF-B213-006800220036}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EE00E4-00D6-44C3-8047-00E500F7007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009C0068-00CB-4DFE-BCEB-0097001E0054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007E003F-009F-4F13-A0DB-00C300C0003B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001500A7-00B6-45F1-A508-00AE00D900DD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00220096-00B2-4489-939A-00D9001A002D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0091003B-004C-4FA6-B748-00BA000A00E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C00045-00BD-4B71-9FD8-002E009200FA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B8004A-003E-4604-8222-006D0033007F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00480062-0083-44CC-8AE6-009400D6002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002A0099-0080-49E9-AAB2-0061009A0097}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003900F7-00B2-4411-8853-00A100EA001A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008B00B3-00E1-4C17-88B0-0092003D00A6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006F001B-00AC-4247-B59C-0041003700CC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006D0030-00F8-4B37-B1AD-0036004C0091}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AF006C-0029-4D0F-B6A8-00CE00910023}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00670003-0033-4CB3-B03E-00F3007D00D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0015004B-004A-4E5D-AD02-005400BD0075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C100C6-00A5-4841-94A9-0056007700B4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A30096-00E8-4D0D-9A0D-007E00BC00AB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0068003A-00C8-4F7D-B85A-00D50086005C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003E00B7-00B8-4844-A1A9-0071001D0009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A80061-00AF-4765-AE8E-004000D90093}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00220006-006E-4F6C-B000-000000C70076}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004000D8-0010-441E-8E02-006500D600B5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BF002D-0021-48A5-BC59-007A008100B5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C800D7-0039-4BBB-B5FB-00BB00C10058}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A2009C-00F3-46DE-B589-000000BC00B4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AC008A-00A0-4C41-A092-000A008700E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BE00F4-00EB-40B2-82F9-008F00BB00AE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002D0030-0081-491F-ADCB-00CD00B10053}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A60097-0079-49A6-A07D-00CD002F00C0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DF0099-000E-4963-9A0A-000200A500B8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BB00AD-0074-48F2-8DDB-0043002600EA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003700B7-0007-4CA9-9352-009200EB0076}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00080022-0002-458E-9A07-004100E4009E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006B00E1-0031-49B3-9E4D-005E00FB00EA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0009001D-00D7-4B37-B322-002F008B008A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0006004C-00EC-4757-9033-002300E700CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001B00C4-0031-42FF-B5E5-0025008000D6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004B000D-00CD-4748-8205-00D700420028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00ED0041-0070-4630-A6E6-00C200C20004}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00900011-005F-450D-A50F-00FB00FC00AA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E9001F-00FD-4F10-BCFB-00EC0052001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AF0007-00EE-42F0-944B-004500C8001B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D400E8-00C8-4464-9355-00A800390080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
           <xm:sqref>E21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008300C1-007C-4582-843E-006300FC00F4}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00880070-002F-4BD4-A607-008B000E0033}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEVELS</xm:f>
           </x14:formula1>
@@ -9274,7 +9271,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="92" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>43</v>
@@ -9307,10 +9304,10 @@
         <v>591</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>845</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>846</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>589</v>
@@ -9346,7 +9343,7 @@
         <v>269</v>
       </c>
       <c r="H2" s="116" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="I2" s="193" t="str">
         <f>PROPER(I1)</f>
@@ -9363,10 +9360,10 @@
         <v>610</v>
       </c>
       <c r="M2" s="136" t="s">
+        <v>847</v>
+      </c>
+      <c r="N2" s="194" t="s">
         <v>848</v>
-      </c>
-      <c r="N2" s="194" t="s">
-        <v>849</v>
       </c>
       <c r="O2" s="194" t="str">
         <f>PROPER(O1)</f>
@@ -9384,27 +9381,27 @@
     </row>
     <row r="3" s="75" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="187" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B3" s="168" t="str">
         <f>te_qbanks!A3</f>
         <v>qbank01</v>
       </c>
       <c r="C3" s="195" t="s">
+        <v>850</v>
+      </c>
+      <c r="D3" s="164" t="s">
         <v>851</v>
-      </c>
-      <c r="D3" s="164" t="s">
-        <v>852</v>
       </c>
       <c r="E3" s="164"/>
       <c r="F3" s="164" t="s">
         <v>336</v>
       </c>
       <c r="G3" s="75" t="s">
+        <v>852</v>
+      </c>
+      <c r="H3" s="196" t="s">
         <v>853</v>
-      </c>
-      <c r="H3" s="196" t="s">
-        <v>854</v>
       </c>
       <c r="I3" s="179" t="str">
         <f>ap_programs!A5</f>
@@ -9414,7 +9411,7 @@
         <v>712</v>
       </c>
       <c r="K3" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="L3" s="80" t="s">
         <v>10</v>
@@ -9423,10 +9420,10 @@
         <v>9</v>
       </c>
       <c r="N3" s="197" t="s">
+        <v>855</v>
+      </c>
+      <c r="O3" s="200" t="s">
         <v>856</v>
-      </c>
-      <c r="O3" s="200" t="s">
-        <v>857</v>
       </c>
       <c r="P3" s="201" t="s">
         <v>171</v>
@@ -9438,24 +9435,24 @@
     </row>
     <row r="4" s="75" customFormat="1" ht="27">
       <c r="A4" s="187" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B4" s="168" t="str">
         <f>B3</f>
         <v>qbank01</v>
       </c>
       <c r="C4" s="195" t="s">
+        <v>858</v>
+      </c>
+      <c r="D4" s="164" t="s">
         <v>859</v>
-      </c>
-      <c r="D4" s="164" t="s">
-        <v>860</v>
       </c>
       <c r="E4" s="164"/>
       <c r="F4" s="164" t="s">
+        <v>860</v>
+      </c>
+      <c r="G4" s="75" t="s">
         <v>861</v>
-      </c>
-      <c r="G4" s="75" t="s">
-        <v>862</v>
       </c>
       <c r="H4" s="196" t="s">
         <v>423</v>
@@ -9468,7 +9465,7 @@
         <v>712</v>
       </c>
       <c r="K4" s="198" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="L4" s="80" t="s">
         <v>10</v>
@@ -9477,10 +9474,10 @@
         <v>9</v>
       </c>
       <c r="N4" s="197" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="O4" s="202" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="P4" s="201" t="str">
         <f t="shared" ref="P4:P9" si="22">P3</f>
@@ -9493,24 +9490,24 @@
     </row>
     <row r="5" ht="27">
       <c r="A5" s="187" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B5" s="168"/>
       <c r="C5" s="195" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D5" s="164" t="s">
         <v>709</v>
       </c>
       <c r="E5" s="164"/>
       <c r="F5" s="164" t="s">
+        <v>865</v>
+      </c>
+      <c r="G5" s="75" t="s">
         <v>866</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="H5" s="196" t="s">
         <v>867</v>
-      </c>
-      <c r="H5" s="196" t="s">
-        <v>868</v>
       </c>
       <c r="I5" s="179"/>
       <c r="J5" s="197"/>
@@ -9529,24 +9526,24 @@
     </row>
     <row r="6" ht="27">
       <c r="A6" s="187" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B6" s="168"/>
       <c r="C6" s="195" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D6" s="164" t="s">
         <v>709</v>
       </c>
       <c r="E6" s="164"/>
       <c r="F6" s="164" t="s">
+        <v>870</v>
+      </c>
+      <c r="G6" s="75" t="s">
         <v>871</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="H6" s="196" t="s">
         <v>872</v>
-      </c>
-      <c r="H6" s="196" t="s">
-        <v>873</v>
       </c>
       <c r="I6" s="179"/>
       <c r="J6" s="197"/>
@@ -9565,24 +9562,24 @@
     </row>
     <row r="7" ht="40.5">
       <c r="A7" s="187" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B7" s="168"/>
       <c r="C7" s="195" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D7" s="164" t="s">
         <v>709</v>
       </c>
       <c r="E7" s="164"/>
       <c r="F7" s="164" t="s">
+        <v>875</v>
+      </c>
+      <c r="G7" s="75" t="s">
         <v>876</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="H7" s="196" t="s">
         <v>877</v>
-      </c>
-      <c r="H7" s="196" t="s">
-        <v>878</v>
       </c>
       <c r="I7" s="179"/>
       <c r="J7" s="197"/>
@@ -9601,24 +9598,24 @@
     </row>
     <row r="8" ht="27">
       <c r="A8" s="187" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B8" s="168"/>
       <c r="C8" s="195" t="s">
+        <v>879</v>
+      </c>
+      <c r="D8" s="164" t="s">
         <v>880</v>
-      </c>
-      <c r="D8" s="164" t="s">
-        <v>881</v>
       </c>
       <c r="E8" s="164"/>
       <c r="F8" s="164" t="s">
+        <v>881</v>
+      </c>
+      <c r="G8" s="75" t="s">
         <v>882</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="H8" s="196" t="s">
         <v>883</v>
-      </c>
-      <c r="H8" s="196" t="s">
-        <v>884</v>
       </c>
       <c r="I8" s="179"/>
       <c r="J8" s="197"/>
@@ -9637,24 +9634,24 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="187" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B9" s="168"/>
       <c r="C9" s="195" t="s">
+        <v>885</v>
+      </c>
+      <c r="D9" s="164" t="s">
         <v>886</v>
-      </c>
-      <c r="D9" s="164" t="s">
-        <v>887</v>
       </c>
       <c r="E9" s="164"/>
       <c r="F9" s="164" t="s">
+        <v>887</v>
+      </c>
+      <c r="G9" s="75" t="s">
         <v>888</v>
       </c>
-      <c r="G9" s="75" t="s">
+      <c r="H9" s="196" t="s">
         <v>889</v>
-      </c>
-      <c r="H9" s="196" t="s">
-        <v>890</v>
       </c>
       <c r="I9" s="179"/>
       <c r="J9" s="197"/>
@@ -9682,7 +9679,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00A5007A-00A7-45DF-A2B8-00C800A100D1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001F0076-00E2-4F41-899F-00C700D500D8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -9725,34 +9722,34 @@
         <v>42</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C1" s="92" t="s">
         <v>437</v>
       </c>
       <c r="D1" s="204" t="s">
+        <v>891</v>
+      </c>
+      <c r="E1" s="92" t="s">
         <v>892</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="F1" s="92" t="s">
         <v>893</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="G1" s="92" t="s">
         <v>894</v>
-      </c>
-      <c r="G1" s="92" t="s">
-        <v>895</v>
       </c>
       <c r="H1" s="185" t="s">
         <v>44</v>
       </c>
       <c r="I1" s="185" t="s">
+        <v>895</v>
+      </c>
+      <c r="J1" s="185" t="s">
         <v>896</v>
       </c>
-      <c r="J1" s="185" t="s">
+      <c r="K1" s="92" t="s">
         <v>897</v>
-      </c>
-      <c r="K1" s="92" t="s">
-        <v>898</v>
       </c>
       <c r="L1" s="92" t="s">
         <v>93</v>
@@ -9774,31 +9771,31 @@
         <v>Type</v>
       </c>
       <c r="D2" s="208" t="s">
+        <v>898</v>
+      </c>
+      <c r="E2" s="207" t="s">
         <v>899</v>
       </c>
-      <c r="E2" s="207" t="s">
+      <c r="F2" s="206" t="s">
+        <v>893</v>
+      </c>
+      <c r="G2" s="206" t="s">
         <v>900</v>
-      </c>
-      <c r="F2" s="206" t="s">
-        <v>894</v>
-      </c>
-      <c r="G2" s="206" t="s">
-        <v>901</v>
       </c>
       <c r="H2" s="206" t="s">
         <v>49</v>
       </c>
       <c r="I2" s="206" t="s">
+        <v>901</v>
+      </c>
+      <c r="J2" s="206" t="s">
         <v>902</v>
       </c>
-      <c r="J2" s="206" t="s">
+      <c r="K2" s="207" t="s">
         <v>903</v>
       </c>
-      <c r="K2" s="207" t="s">
+      <c r="L2" s="209" t="s">
         <v>904</v>
-      </c>
-      <c r="L2" s="209" t="s">
-        <v>905</v>
       </c>
       <c r="M2" s="209" t="s">
         <v>478</v>
@@ -9806,13 +9803,13 @@
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="187" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="75" t="s">
         <v>906</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="C3" s="210" t="s">
         <v>907</v>
-      </c>
-      <c r="C3" s="210" t="s">
-        <v>908</v>
       </c>
       <c r="D3" s="211">
         <v>44447</v>
@@ -9821,7 +9818,7 @@
         <v>44447</v>
       </c>
       <c r="F3" s="212" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G3" s="80" t="s">
         <v>9</v>
@@ -9844,13 +9841,13 @@
     </row>
     <row r="4" ht="19.5" customHeight="1">
       <c r="A4" s="187" t="s">
+        <v>909</v>
+      </c>
+      <c r="B4" s="75" t="s">
         <v>910</v>
       </c>
-      <c r="B4" s="75" t="s">
-        <v>911</v>
-      </c>
       <c r="C4" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D4" s="211">
         <v>44447</v>
@@ -9859,7 +9856,7 @@
         <v>44447</v>
       </c>
       <c r="F4" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G4" s="80" t="s">
         <v>9</v>
@@ -9882,13 +9879,13 @@
     </row>
     <row r="5" ht="19.5" customHeight="1">
       <c r="A5" s="187" t="s">
+        <v>911</v>
+      </c>
+      <c r="B5" s="75" t="s">
         <v>912</v>
       </c>
-      <c r="B5" s="75" t="s">
-        <v>913</v>
-      </c>
       <c r="C5" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D5" s="211">
         <v>44480</v>
@@ -9897,7 +9894,7 @@
         <v>44480</v>
       </c>
       <c r="F5" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G5" s="80" t="s">
         <v>9</v>
@@ -9920,13 +9917,13 @@
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="187" t="s">
+        <v>913</v>
+      </c>
+      <c r="B6" s="75" t="s">
         <v>914</v>
       </c>
-      <c r="B6" s="75" t="s">
-        <v>915</v>
-      </c>
       <c r="C6" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D6" s="211">
         <v>44481</v>
@@ -9935,13 +9932,13 @@
         <v>44481</v>
       </c>
       <c r="F6" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G6" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="75" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I6" s="164"/>
       <c r="J6" s="75"/>
@@ -9960,13 +9957,13 @@
     </row>
     <row r="7" ht="19.5" customHeight="1">
       <c r="A7" s="187" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B7" s="75" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C7" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D7" s="211">
         <v>44501</v>
@@ -9975,13 +9972,13 @@
         <v>44501</v>
       </c>
       <c r="F7" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G7" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="75" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I7" s="164"/>
       <c r="J7" s="75"/>
@@ -10000,13 +9997,13 @@
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="187" t="s">
+        <v>918</v>
+      </c>
+      <c r="B8" s="75" t="s">
         <v>919</v>
       </c>
-      <c r="B8" s="75" t="s">
-        <v>920</v>
-      </c>
       <c r="C8" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D8" s="211">
         <v>44509</v>
@@ -10015,13 +10012,13 @@
         <v>44509</v>
       </c>
       <c r="F8" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G8" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="75" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="I8" s="164"/>
       <c r="J8" s="75"/>
@@ -10040,13 +10037,13 @@
     </row>
     <row r="9" ht="19.5" customHeight="1">
       <c r="A9" s="187" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C9" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D9" s="211">
         <v>44536</v>
@@ -10055,13 +10052,13 @@
         <v>44536</v>
       </c>
       <c r="F9" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G9" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="75" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="I9" s="164"/>
       <c r="J9" s="75"/>
@@ -10080,13 +10077,13 @@
     </row>
     <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="187" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C10" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D10" s="211">
         <v>44537</v>
@@ -10095,7 +10092,7 @@
         <v>44537</v>
       </c>
       <c r="F10" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G10" s="80" t="s">
         <v>9</v>
@@ -10118,13 +10115,13 @@
     </row>
     <row r="11" ht="19.5" customHeight="1">
       <c r="A11" s="187" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C11" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D11" s="211">
         <v>44538</v>
@@ -10133,13 +10130,13 @@
         <v>44538</v>
       </c>
       <c r="F11" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G11" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="75" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="I11" s="164"/>
       <c r="J11" s="75"/>
@@ -10158,13 +10155,13 @@
     </row>
     <row r="12" ht="19.5" customHeight="1">
       <c r="A12" s="187" t="s">
+        <v>926</v>
+      </c>
+      <c r="B12" s="75" t="s">
         <v>927</v>
       </c>
-      <c r="B12" s="75" t="s">
-        <v>928</v>
-      </c>
       <c r="C12" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D12" s="211">
         <v>44552</v>
@@ -10173,7 +10170,7 @@
         <v>44552</v>
       </c>
       <c r="F12" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G12" s="80" t="s">
         <v>9</v>
@@ -10196,13 +10193,13 @@
     </row>
     <row r="13" ht="19.5" customHeight="1">
       <c r="A13" s="187" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C13" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D13" s="211">
         <v>44568</v>
@@ -10211,7 +10208,7 @@
         <v>44568</v>
       </c>
       <c r="F13" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G13" s="80" t="s">
         <v>9</v>
@@ -10234,13 +10231,13 @@
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="187" t="s">
+        <v>929</v>
+      </c>
+      <c r="B14" s="75" t="s">
         <v>930</v>
       </c>
-      <c r="B14" s="75" t="s">
-        <v>931</v>
-      </c>
       <c r="C14" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D14" s="211">
         <v>44571</v>
@@ -10249,7 +10246,7 @@
         <v>44571</v>
       </c>
       <c r="F14" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G14" s="80" t="s">
         <v>9</v>
@@ -10272,13 +10269,13 @@
     </row>
     <row r="15" ht="19.5" customHeight="1">
       <c r="A15" s="187" t="s">
+        <v>931</v>
+      </c>
+      <c r="B15" s="75" t="s">
         <v>932</v>
       </c>
-      <c r="B15" s="75" t="s">
-        <v>933</v>
-      </c>
       <c r="C15" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D15" s="214">
         <v>44596</v>
@@ -10287,7 +10284,7 @@
         <v>44596</v>
       </c>
       <c r="F15" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G15" s="80" t="s">
         <v>9</v>
@@ -10310,13 +10307,13 @@
     </row>
     <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="187" t="s">
+        <v>933</v>
+      </c>
+      <c r="B16" s="75" t="s">
         <v>934</v>
       </c>
-      <c r="B16" s="75" t="s">
-        <v>935</v>
-      </c>
       <c r="C16" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D16" s="214">
         <v>44606</v>
@@ -10325,7 +10322,7 @@
         <v>44610</v>
       </c>
       <c r="F16" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G16" s="80" t="s">
         <v>9</v>
@@ -10348,13 +10345,13 @@
     </row>
     <row r="17" ht="19.5" customHeight="1">
       <c r="A17" s="187" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C17" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D17" s="211">
         <v>44617</v>
@@ -10363,7 +10360,7 @@
         <v>44617</v>
       </c>
       <c r="F17" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G17" s="80" t="s">
         <v>9</v>
@@ -10386,13 +10383,13 @@
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="187" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B18" s="215" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C18" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D18" s="211">
         <v>44620</v>
@@ -10401,7 +10398,7 @@
         <v>44617</v>
       </c>
       <c r="F18" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G18" s="80" t="s">
         <v>9</v>
@@ -10424,13 +10421,13 @@
     </row>
     <row r="19" ht="19.5" customHeight="1">
       <c r="A19" s="187" t="s">
+        <v>937</v>
+      </c>
+      <c r="B19" s="75" t="s">
         <v>938</v>
       </c>
-      <c r="B19" s="75" t="s">
-        <v>939</v>
-      </c>
       <c r="C19" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D19" s="211">
         <v>44658</v>
@@ -10439,7 +10436,7 @@
         <v>44658</v>
       </c>
       <c r="F19" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G19" s="80" t="s">
         <v>9</v>
@@ -10462,13 +10459,13 @@
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="187" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B20" s="215" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C20" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D20" s="211">
         <v>44659</v>
@@ -10477,13 +10474,13 @@
         <v>44659</v>
       </c>
       <c r="F20" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G20" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I20" s="164"/>
       <c r="J20" s="75"/>
@@ -10502,13 +10499,13 @@
     </row>
     <row r="21" ht="19.5" customHeight="1">
       <c r="A21" s="187" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B21" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C21" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D21" s="211">
         <v>44662</v>
@@ -10517,13 +10514,13 @@
         <v>44662</v>
       </c>
       <c r="F21" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G21" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I21" s="164"/>
       <c r="J21" s="75"/>
@@ -10542,13 +10539,13 @@
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="187" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C22" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D22" s="214">
         <v>44663</v>
@@ -10557,13 +10554,13 @@
         <v>44663</v>
       </c>
       <c r="F22" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G22" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H22" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I22" s="164"/>
       <c r="J22" s="75"/>
@@ -10582,13 +10579,13 @@
     </row>
     <row r="23" ht="19.5" customHeight="1">
       <c r="A23" s="187" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C23" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D23" s="214">
         <v>44664</v>
@@ -10597,13 +10594,13 @@
         <v>44664</v>
       </c>
       <c r="F23" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G23" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H23" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I23" s="164"/>
       <c r="J23" s="75"/>
@@ -10622,13 +10619,13 @@
     </row>
     <row r="24" ht="19.5" customHeight="1">
       <c r="A24" s="187" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B24" s="89" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C24" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D24" s="214">
         <v>44665</v>
@@ -10637,13 +10634,13 @@
         <v>44665</v>
       </c>
       <c r="F24" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G24" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H24" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I24" s="164"/>
       <c r="J24" s="75"/>
@@ -10662,13 +10659,13 @@
     </row>
     <row r="25" ht="19.5" customHeight="1">
       <c r="A25" s="187" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C25" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D25" s="214">
         <v>44666</v>
@@ -10677,13 +10674,13 @@
         <v>44666</v>
       </c>
       <c r="F25" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G25" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H25" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I25" s="164"/>
       <c r="J25" s="75"/>
@@ -10702,13 +10699,13 @@
     </row>
     <row r="26" ht="19.5" customHeight="1">
       <c r="A26" s="187" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C26" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D26" s="214">
         <v>44669</v>
@@ -10717,13 +10714,13 @@
         <v>44667</v>
       </c>
       <c r="F26" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G26" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H26" s="75" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I26" s="164"/>
       <c r="J26" s="75"/>
@@ -10742,13 +10739,13 @@
     </row>
     <row r="27" ht="19.5" customHeight="1">
       <c r="A27" s="187" t="s">
+        <v>947</v>
+      </c>
+      <c r="B27" s="75" t="s">
         <v>948</v>
       </c>
-      <c r="B27" s="75" t="s">
-        <v>949</v>
-      </c>
       <c r="C27" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D27" s="211">
         <v>44670</v>
@@ -10757,7 +10754,7 @@
         <v>44670</v>
       </c>
       <c r="F27" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G27" s="80" t="s">
         <v>9</v>
@@ -10780,13 +10777,13 @@
     </row>
     <row r="28" ht="19.5" customHeight="1">
       <c r="A28" s="187" t="s">
+        <v>949</v>
+      </c>
+      <c r="B28" s="75" t="s">
         <v>950</v>
       </c>
-      <c r="B28" s="75" t="s">
-        <v>951</v>
-      </c>
       <c r="C28" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D28" s="211">
         <v>44715</v>
@@ -10795,7 +10792,7 @@
         <v>44715</v>
       </c>
       <c r="F28" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G28" s="80" t="s">
         <v>9</v>
@@ -10818,13 +10815,13 @@
     </row>
     <row r="29" ht="19.5" customHeight="1">
       <c r="A29" s="187" t="s">
+        <v>951</v>
+      </c>
+      <c r="B29" s="75" t="s">
         <v>952</v>
       </c>
-      <c r="B29" s="75" t="s">
-        <v>953</v>
-      </c>
       <c r="C29" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D29" s="214">
         <v>44736</v>
@@ -10833,7 +10830,7 @@
         <v>44736</v>
       </c>
       <c r="F29" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G29" s="80" t="s">
         <v>9</v>
@@ -10856,13 +10853,13 @@
     </row>
     <row r="30" ht="19.5" customHeight="1">
       <c r="A30" s="187" t="s">
+        <v>953</v>
+      </c>
+      <c r="B30" s="75" t="s">
         <v>954</v>
       </c>
-      <c r="B30" s="75" t="s">
-        <v>955</v>
-      </c>
       <c r="C30" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D30" s="211">
         <v>44739</v>
@@ -10871,7 +10868,7 @@
         <v>44739</v>
       </c>
       <c r="F30" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G30" s="80" t="s">
         <v>9</v>
@@ -10894,13 +10891,13 @@
     </row>
     <row r="31" ht="19.5" customHeight="1">
       <c r="A31" s="187" t="s">
+        <v>955</v>
+      </c>
+      <c r="B31" s="75" t="s">
         <v>956</v>
       </c>
-      <c r="B31" s="75" t="s">
-        <v>957</v>
-      </c>
       <c r="C31" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D31" s="214">
         <v>44690</v>
@@ -10909,13 +10906,13 @@
         <v>44698</v>
       </c>
       <c r="F31" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G31" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H31" s="75" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I31" s="164"/>
       <c r="J31" s="75"/>
@@ -10923,7 +10920,7 @@
         <v>10</v>
       </c>
       <c r="L31" s="179" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="M31" s="179" t="str">
         <f>users!A4</f>
@@ -10933,13 +10930,13 @@
     </row>
     <row r="32" ht="19.5" customHeight="1">
       <c r="A32" s="187" t="s">
+        <v>959</v>
+      </c>
+      <c r="B32" s="75" t="s">
         <v>960</v>
       </c>
-      <c r="B32" s="75" t="s">
-        <v>961</v>
-      </c>
       <c r="C32" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D32" s="214">
         <v>44698.527777777781</v>
@@ -10948,13 +10945,13 @@
         <v>44698.565972222219</v>
       </c>
       <c r="F32" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G32" s="80" t="s">
         <v>9</v>
       </c>
       <c r="H32" s="75" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I32" s="164"/>
       <c r="J32" s="75"/>
@@ -10973,13 +10970,13 @@
     </row>
     <row r="33" ht="19.5" customHeight="1">
       <c r="A33" s="187" t="s">
+        <v>962</v>
+      </c>
+      <c r="B33" s="75" t="s">
         <v>963</v>
       </c>
-      <c r="B33" s="75" t="s">
-        <v>964</v>
-      </c>
       <c r="C33" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D33" s="214">
         <v>44711.527777777781</v>
@@ -10988,13 +10985,13 @@
         <v>44711.565972222219</v>
       </c>
       <c r="F33" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G33" s="80" t="s">
         <v>10</v>
       </c>
       <c r="H33" s="75" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I33" s="164"/>
       <c r="J33" s="75"/>
@@ -11013,13 +11010,13 @@
     </row>
     <row r="34" ht="19.5" customHeight="1">
       <c r="A34" s="187" t="s">
+        <v>965</v>
+      </c>
+      <c r="B34" s="75" t="s">
         <v>966</v>
       </c>
-      <c r="B34" s="75" t="s">
-        <v>967</v>
-      </c>
       <c r="C34" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D34" s="214">
         <v>44700.354166666664</v>
@@ -11028,7 +11025,7 @@
         <v>44700.392361111109</v>
       </c>
       <c r="F34" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G34" s="80" t="s">
         <v>10</v>
@@ -11051,13 +11048,13 @@
     </row>
     <row r="35" ht="19.5" customHeight="1">
       <c r="A35" s="187" t="s">
+        <v>967</v>
+      </c>
+      <c r="B35" s="75" t="s">
         <v>968</v>
       </c>
-      <c r="B35" s="75" t="s">
-        <v>969</v>
-      </c>
       <c r="C35" s="210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D35" s="214">
         <v>44706.430555555555</v>
@@ -11066,13 +11063,13 @@
         <v>44706.46875</v>
       </c>
       <c r="F35" s="80" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G35" s="80" t="s">
         <v>10</v>
       </c>
       <c r="H35" s="75" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I35" s="164"/>
       <c r="J35" s="75"/>
@@ -11091,13 +11088,13 @@
     </row>
     <row r="36" ht="19.5" customHeight="1">
       <c r="A36" s="187" t="s">
+        <v>970</v>
+      </c>
+      <c r="B36" s="75" t="s">
         <v>971</v>
       </c>
-      <c r="B36" s="75" t="s">
+      <c r="C36" s="210" t="s">
         <v>972</v>
-      </c>
-      <c r="C36" s="210" t="s">
-        <v>973</v>
       </c>
       <c r="D36" s="214"/>
       <c r="E36" s="214"/>
@@ -11125,13 +11122,13 @@
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="187" t="s">
+        <v>973</v>
+      </c>
+      <c r="B37" s="75" t="s">
         <v>974</v>
       </c>
-      <c r="B37" s="75" t="s">
-        <v>975</v>
-      </c>
       <c r="C37" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D37" s="214"/>
       <c r="E37" s="214"/>
@@ -11157,13 +11154,13 @@
     </row>
     <row r="38" ht="40.5">
       <c r="A38" s="187" t="s">
+        <v>975</v>
+      </c>
+      <c r="B38" s="89" t="s">
         <v>976</v>
       </c>
-      <c r="B38" s="89" t="s">
-        <v>977</v>
-      </c>
       <c r="C38" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D38" s="214"/>
       <c r="E38" s="214"/>
@@ -11171,7 +11168,7 @@
       <c r="G38" s="75"/>
       <c r="H38" s="75"/>
       <c r="I38" s="216" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="J38" s="75">
         <v>5</v>
@@ -11191,13 +11188,13 @@
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="187" t="s">
+        <v>978</v>
+      </c>
+      <c r="B39" s="75" t="s">
         <v>979</v>
       </c>
-      <c r="B39" s="75" t="s">
-        <v>980</v>
-      </c>
       <c r="C39" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D39" s="214">
         <v>44711.489583333336</v>
@@ -11227,13 +11224,13 @@
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="187" t="s">
+        <v>980</v>
+      </c>
+      <c r="B40" s="75" t="s">
         <v>981</v>
       </c>
-      <c r="B40" s="75" t="s">
-        <v>982</v>
-      </c>
       <c r="C40" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D40" s="214"/>
       <c r="E40" s="214"/>
@@ -11256,13 +11253,13 @@
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="187" t="s">
+        <v>982</v>
+      </c>
+      <c r="B41" s="75" t="s">
         <v>983</v>
       </c>
-      <c r="B41" s="75" t="s">
-        <v>984</v>
-      </c>
       <c r="C41" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D41" s="214"/>
       <c r="E41" s="214"/>
@@ -11285,13 +11282,13 @@
     </row>
     <row r="42" ht="14.25">
       <c r="A42" s="187" t="s">
+        <v>984</v>
+      </c>
+      <c r="B42" s="75" t="s">
         <v>985</v>
       </c>
-      <c r="B42" s="75" t="s">
-        <v>986</v>
-      </c>
       <c r="C42" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D42" s="214">
         <v>44721.430555555555</v>
@@ -11318,13 +11315,13 @@
     </row>
     <row r="43" ht="14.25">
       <c r="A43" s="187" t="s">
+        <v>986</v>
+      </c>
+      <c r="B43" s="89" t="s">
         <v>987</v>
       </c>
-      <c r="B43" s="89" t="s">
-        <v>988</v>
-      </c>
       <c r="C43" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D43" s="214">
         <v>44720.354166666664</v>
@@ -11351,13 +11348,13 @@
     </row>
     <row r="44" ht="14.25">
       <c r="A44" s="187" t="s">
+        <v>988</v>
+      </c>
+      <c r="B44" s="89" t="s">
         <v>989</v>
       </c>
-      <c r="B44" s="89" t="s">
-        <v>990</v>
-      </c>
       <c r="C44" s="210" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="D44" s="214"/>
       <c r="E44" s="214"/>
@@ -11542,391 +11539,391 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="65" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00000063-00E1-40D6-BFEE-00AC003B0052}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007D00E0-005A-4D7E-8CC7-002E002C0069}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007D00EF-0092-4B24-AFD2-00F600BA00AE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003800E9-0013-4743-919C-00C9001B007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006B005C-002C-457C-B311-00AE00E9005F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001900E7-0084-416C-9425-0008002400F3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G34</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006E000E-008D-498C-801B-00A800000062}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B400C9-00CA-47AB-AE74-00D800A10005}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G35 G36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00480059-00F9-4594-81DA-003400D20048}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DB0026-00D1-43DD-ABD9-00C30012006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G31 G32</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000F009B-005F-41DB-9B76-00C500CF0001}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00060062-004A-4D64-A70C-001B00720018}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F80079-003A-4858-AA09-00CE00BA007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008A00D3-0099-44CE-BD03-00A40012002B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C0004A-0014-409C-B503-00C000F5008B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00E100AF-0029-4FFA-ADCD-000B00AE0039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G28</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00730073-00E5-4FD4-A228-005C00950026}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005C00B1-001A-4E1C-B8F1-009E00810003}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00ED004D-004E-4BBF-990E-001D000C00A0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AE00F2-0047-4E61-90BD-00D500B300BB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005E007F-00C5-46D5-B59A-000E00A300D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A400A7-00D1-4E0D-8182-0023008200C3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G25</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B5008E-00BC-475E-A504-00DE0029009A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007D00DA-006A-4BF7-9473-00A700470070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001C007D-003B-4F96-85F9-00EC00680057}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C90012-0009-43B3-B084-00A200F200C1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002F00C5-00F4-498C-9AA1-00BE005200C5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0073000F-0080-4E98-8D03-0040007B0090}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000700B3-0032-4D13-8FF9-0025003600D1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00FE00A4-0013-4548-B7CB-00C100EE005B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00390094-00E4-4928-BD12-005900200041}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D2003D-00E4-4C19-B89E-000B003B0071}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00AF001C-0056-42D8-8958-001100980069}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B1001C-0094-405A-A573-000900000055}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00210052-0066-42C9-BC04-00C100AF00E1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000B0080-00C3-464E-978F-000C006B00B7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002A00FB-00F1-4881-AF3F-0024001A009D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005F0094-00FB-48C9-824A-0032009B0047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00300080-0039-4959-96AA-002000D20070}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D300D7-00FD-447B-A1CE-0073007800A3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E2001C-0070-4526-B998-002900640073}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002300A4-00D0-40F9-AA2C-009A00F80039}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0060001E-0020-4990-840E-005E00660038}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AE001B-001D-4652-890D-008C0014006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008A00B2-000B-4543-9690-00480038001D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AB0033-00EB-4605-83D2-00F00013005E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00380052-00EE-40B4-846E-003E006E00C1}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006C004B-0067-4670-8EEA-007A00520080}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00040065-0028-4A9D-8A1E-00610094007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{005400AC-0062-4846-AB7E-00E9008900D6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0074000B-00B5-4E9B-AB6B-00BB009000D2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008900A8-00DC-4895-B7F5-002500D20032}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008B0085-00A6-4F2B-972A-00C800EE000C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0001005F-00F4-4A6B-83BD-00D2007D0038}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003400E8-008E-4AA5-A113-00FD00A10092}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007A0034-007C-482E-8595-009A000C0052}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D9002F-00CE-483E-976F-006C008D0045}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003700B8-0078-4DAC-9240-0013005E007B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009900F5-007D-4549-82BA-0089005D00F8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00700016-0096-41E4-B44C-004E001F0096}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CB000C-001A-46BE-AB57-00A5008E0079}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C10031-00B5-4237-8C34-00410066001E}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00CF00B1-003A-4672-8CD9-007200910009}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EC0042-003B-48E4-B9D6-000900F6005A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00850068-003D-4F14-BC37-00E500410079}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006800FE-0007-426F-BDA7-002D004B00BA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>G12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004C005D-003E-460C-AE42-0077008A00CA}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00ED0085-0073-437C-BF7C-007B006D0043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>K3 K4 K5 K6 K7 K8 K9 K10 K11 K12 K13 K14 K15 K16 K17 K18 K19 K20 K21 K22 K23 K24 K25 K26 K27 K28 K29 K30 K31 K32 K33 K34 K35 K36 K37 K38 K39 K40 K41 K42 K43 K44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004D0065-004A-461F-A4C4-008600DA00CA}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00BE008B-0041-4434-9160-00EB001800AF}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003C00C6-009A-46D4-AA0D-005E00E60060}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A700F5-002B-419F-8E70-00A100CD0093}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00170019-00B9-4179-8980-000D00550088}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003B0072-006F-432E-AF76-00AD000100E3}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E9007D-0023-4826-9B06-00BD00B9002F}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004A00C3-00D3-4819-B283-00BF00C200D0}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FA00B3-00F5-473E-811C-00DE00BE008A}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DD0010-00C9-46B2-BBE9-00D400310059}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002C00B4-00E1-4486-9970-00E80065009D}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{008E0013-007A-4938-8451-003200A00069}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00300019-00D0-4D7F-AA1D-003F00700053}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B100FB-00B5-4C46-A2C2-004400C300E5}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B800C4-007E-4F37-9F37-00F500EC0010}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00AB0031-009F-4E6A-B1CD-0088002000D4}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F11</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004C000B-0049-4642-AB42-003300F60078}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00130013-0032-4745-A0BA-008300CF0097}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002200D8-0043-49F9-B67A-007900EC00F4}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B80010-0016-480C-A15F-003A00250097}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009C000E-009E-4A68-9E01-001B00E300F0}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{002C0092-0021-4FE6-B0DE-00CE008B0036}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{007900AA-007D-47E9-9A7A-00B500AE00E8}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003C00A1-0009-45B9-96FA-001800DF00D9}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F28</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0094005F-00F3-4750-95ED-00ED00500065}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00750045-00A3-4E84-88E9-00D600C7009A}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C60058-00CB-47D5-9581-0067002A000F}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00800076-0020-4B7D-9A69-005000750029}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F26</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{009600A0-00E2-4782-9FAE-007000300056}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009B003B-002C-4544-A7ED-004D00B70012}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F25</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00EA0048-00A0-4B53-8AA3-006100DE00CE}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00EB008C-002C-468B-B7AB-001600D20018}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00D00012-009A-4A9F-9194-00DA003E009A}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00970050-00C4-4655-8BFA-00BF00090007}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B200CF-00D0-4691-850D-006C004900B9}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004700D6-00AB-4321-9E66-0034009D0097}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008F002A-00C0-49BB-9A21-00320045005C}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CC0026-0034-48F5-A768-007C005F0070}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00C0006B-00B5-4ECC-A1D0-006100120079}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C30044-0010-492D-A2CD-00E6006100DF}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00610030-0044-454C-ADC8-003B00E60083}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006300C4-00FF-480E-9B12-00D900EB0037}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F40047-00BB-440F-AD87-008400990073}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0063004E-0072-40E8-A91B-00CA00800008}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{001500D1-0037-484E-8994-00D1008000ED}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0031004B-0002-4981-A38E-0070003D005A}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00DE0037-00A9-431C-B26B-0030008C00D2}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004E002F-00B1-4B7A-B92D-00D9001100CD}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00BA007A-0063-4DC3-9EC5-00750067009C}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00DD0084-00A7-4C42-80E6-00F300A800E0}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008E0013-00FE-40A5-8B24-005600C1005E}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007B00DD-00BC-4D07-9E56-006800DC0063}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008400D6-0064-4CD7-84CE-00B5009F0048}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D2005E-008C-477B-9679-0056000E00A7}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000E0033-00A0-4226-81DB-00FB000C0052}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C10041-0069-4256-A5D1-008E000E00F5}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000600B6-0035-432D-8A04-006F008E000B}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{007600C2-009E-4427-BFB9-0064002C00C1}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F32</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0084004E-00F2-4E33-9455-006600E300C9}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004B00D2-0007-4BDE-99B6-006E00F400E2}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>F33</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008C007C-0087-442E-BAE6-003000BB0065}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006500A0-00A1-42B7-AA51-00E3001D00A4}" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -13819,37 +13816,37 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6" disablePrompts="0">
-        <x14:dataValidation xr:uid="{003B00DE-0070-471F-B013-001D008700E5}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006A0086-00F9-4AC5-967E-009200A20075}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4 D18</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FD0012-0005-40E1-9ACC-0067002300CD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0003006D-007E-4F1E-972A-003E00C00043}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D18:D20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00440033-0071-4AA1-9C6A-00EE00EA00FB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00D500C3-00DA-49D9-B22B-007700C600D7}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00490015-0049-4C00-B979-001800FB0084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001800BF-00E0-4B0F-8CCD-003C00A2002A}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00320085-00F8-4D55-8D53-00C6003200A2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00A00001-003E-4129-A5F8-00C500CD00D0}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D17</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{004500A5-00E2-4962-9508-003500770062}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00210020-00A7-4F1B-91B7-002E00570006}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GENRE_ANSWER</xm:f>
           </x14:formula1>
@@ -15059,7 +15056,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00680078-0025-4FF2-92C9-003E001A0042}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009B0041-00EE-4B4C-B57E-002100570085}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>
@@ -15210,7 +15207,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{0066003F-00CA-4BA2-9B5D-00BB0056007C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{006400C2-004E-4E0C-A010-003E008C00E8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GUARDIANS_RELATIONSHIPS</xm:f>
           </x14:formula1>
@@ -15344,13 +15341,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{005E009E-0010-4EEC-A352-003000930034}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003D0033-007A-48D3-9349-00CD00F50057}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>GRADES_TYPES</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{0095003E-000F-4D5E-BD52-00B200F300FC}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001D0036-00B2-4E1B-B5F2-0006001E006C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>BOOLEAN_ANSWER</xm:f>
           </x14:formula1>

</xml_diff>